<commit_message>
Added exemplar docs probs in jsonfy, test with cums for BERTopic
</commit_message>
<xml_diff>
--- a/data/top_docs/ctm/elbow_top_docs.xlsx
+++ b/data/top_docs/ctm/elbow_top_docs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,32 +476,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['credits', 'composition', 'allmusic', 'listing', 'charts', 'piano', 'drums', 'beats', 'liner', 'label', 'recording', 'download', 'ballad', 'songwriter', 'vocals']</t>
+          <t>['album', 'song', 'chart', 'music', 'video', 'band', 'songs', 'madonna', 'track', 'pop', 'single', 'recording', 'lyrics', 'vocals', 'billboard']</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dancehall Queen ( Robyn song ) = " Dancehall Queen " is a song by Swedish recording artist Robyn , taken from her fifth studio album , Body Talk Pt . 1 ( 2010 ) . The song was written by Klas Åhlund , who produced it with disc jockey Diplo . The initial writing and production of the song arose from a discussion by Robyn , Diplo and Åhlund about Ace of Base . The song features a dancehall and reggae-infused sound with 1980s synths and subwoofers . It was released as a promotional single before the album was launched in April 2010 . The song received mixed to positive reviews from critics . Some praised its hook and chorus , while others dismissed its overall sound . " Dancehall Queen " charted at number fifty-six on the Sverigetopplistan chart and was listed there for only a week . The accompanying music video , released in November 2010 , was directed by Diplo , Red Foxx and Pomp &amp; Clout . It resembles a karaoke tape with sing-along lyrics on the bottom of the screen . Robyn herself do</t>
+          <t>Lo Mejor de Mí ( song ) = " Lo Mejor de Mí " ( " All My Best " ) is a song written and produced by Rudy Pérez and first recorded by Spanish singer Juan Ramon for his second studio album Por Haberte Amado Tanto ( 1990 ) . In the song , the protagonist tells his lover how he gave his best despite not meeting his lover 's expectation . In 1997 , Mexican recording artist Cristian Castro covered the song for his fifth studio album Lo Mejor de Mí which Pérez also produced and arranged . Castro 's version peaked at number-one on the Billboard Hot Latin Songs and the Billboard Latin Pop Songs charts in the United States . The song received a Billboard Latin Music Awards and a Lo Nuestro nomination for Pop Song of the Year . Pérez earned the American Society of Composers , Authors and Publishers award in the Pop / Ballad field . = = Background = = In 1990 , Spanish recording artist Juan Ramon released his second studio album Por Haberte Amado Tanto which was arranged and produced by Cuban-Ameri</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Harder to Breathe = " Harder to Breathe " is a song by American band Maroon 5 . The song was written by frontman Adam Levine for the band 's debut album , Songs About Jane ( 2002 ) . The song expresses tension , having been written quickly under trying circumstances . It tells the story about a former relationship Levine was involved in . " Harder to Breathe " was met with positive reception by music critics , who praised the track 's sound . It was released in 2002 as the lead single of Songs About Jane . The song peaked at number six on Airplay Monitor . It also appeared on the Hot Modern Rock Tracks chart at number 31 and the Billboard Hot 100 at number 18 . Internationally , the single charted at # 13 in the United Kingdom . " Harder to Breathe " also appeared in the Netherlands , Sweden , Australia , and New Zealand charts , respectively . The song also appears in Maroon 5 's 2004 EP 1.22.03.Acoustic in an acoustic version and the live album Live – Friday the 13th ( 2005 ) . " Har</t>
+          <t>Hot Tottie = " Hot Tottie " is a song by recording artist Usher . It was written by Usher , Ester Dean , Jay-Z and Polow da Don , with the latter producing it . The song features guest vocals from rapper Jay-Z and background vocals by Ester Dean . It is the second single in the United States and Canada from his EP , Versus , which is an extension of his sixth studio album , Raymond v. Raymond . The song was sent to rhythmic and urban airplay on August 9 , 2010 . " Hot Tottie " samples Big Tymers 's " Big Ballin ' " off their 1998 album How You Luv That Vol . 2 . " Hot Tottie " is an R &amp; B song with hip hop tones , accompanied by strobing , electronic beats . It received positive reviews , with many critics noting it as a standout from the EP . It peaked at number twenty-one on the US Billboard Hot 100 , and was a top ten hit on the US Hot R &amp; B / Hip-Hop Songs chart . Usher performed the song on The Early Show and on his OMG Tour . = = Background and composition = = The song was leaked</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Running ( No Doubt song ) = " Running " is a song written by Tony Kanal and Gwen Stefani for No Doubt 's fifth studio album Rock Steady ( 2001 ) and was released worldwide as the album 's fourth and final single on July 1 , 2003 . The song was also used on the last episode of the TV series Sabrina , the Teenage Witch in 2003 . The song received mixed reviews from music critics and was compared to Depeche Mode-style songs . The song only charted on the official charts of the United States , where it became the band 's lowest charting single , and in Germany , where it had longest charting period . The song was accompanied by a music video which was directed by Chris Hafner , which featured many old and new pictures as well as clippings of the band members . = = Background = = The song was written by Stefani and bassist Tony Kanal in Kanal 's living room . They used an old Yamaha keyboard that Kanal 's father had purchased for him when he was in eighth grade and developed the song 's har</t>
+          <t>A + No Poder = A + No Poder ( English : " To the Max " ) is the fourteenth studio album by Mexican recording artist Alejandra Guzmán . It was released on September 11 , 2015 , by Sony Music Latin . After the success of her previous live album , Primera Fila ( 2013 ) and its promotional tour , Guzmán recorded the album with original songs , composed and produced by her and Argentinian musician José Luis Pagán . After its release , A + No Poder received favorable reviews from music critics , with one expressing appreciation for the balance between ballads and rock songs . The record peaked at number twelve on the US Billboard Latin Pop Albums and number six in Mexico . To promote the album , three singles were released : " Adiós " featuring reggaeton performer Farruko , which peaked at number 26 on the Billboard Latin Pop Songs chart , " Qué Ironía " and " Esta Noche " . = = Background = = In 2013 , Alejandra Guzmán released her fourth live album titled Primera Fila , selling 90,000 unit</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>La Llamada = " La Llamada " ( English : " The Phone Call " ) is a song recorded by American recording artist Selena for her first live album Live ! ( 1993 ) . It was composed by Selena y Los Dinos backup singer Pete Astudillo and Selena 's brother and principal record producer A.B. Quintanilla III . The song was produced by Quintanilla III and Argentine music producer Bebu Silvetti . " La Llamada " was released as the second single from Live ! . It peaked at number 5 on the US Hot Latin Tracks on the week ending 23 October 1993 . On the week ending 9 April 2011 , " La Llamada " entered the Regional Mexican Digital Songs chart . The lyrical content of the song describes a girlfriend 's feelings after witnessing her boyfriend kissing another girl , telling him to never call her again and ending the relationship . The central theme explored on " La Llamada " suggests women empowerment . " La Llamada " is an uptempo Mexican cumbia song . The song received generally positive reviews from mu</t>
+          <t>Pero Me Acuerdo de Ti = " Pero Me Acuerdo de Ti " ( English : " But I Remember You " ) is a song written and produced by Rudy Pérez . It was first recorded by Puerto Rican singer Lourdes Robles on her album Definitivamente ( 1991 ) . In the ballad , the singer remembers her lover even when she tries to forget . Nine years later , American recording artist Christina Aguilera performed a cover version on her second studio album Mi Reflejo which Pérez also produced . It was released as the second single from the album in December 2000 . The music video for Aguilera 's version was directed by Kevin Bray . Aguilera performed the song live at the 2001 Grammy Awards . Her version peaked at number eight on the Billboard Hot Latin Songs chart in the United States and number three in Spain . It received a Latin Grammy nomination for Record of the Year . It has been covered by Mexican singer Edith Márquez and Jencarlos Canela . = = Background = = In 1991 , Puerto Rican recording artist Lourdes Ro</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Quiero ( Ricardo Arjona song ) = " Quiero " ( English : " I Want " ) is a latin pop song by Guatemalan recording artist Ricardo Arjona . It was released as the second single from his compilation album Quién Dijo Ayer ( 2007 ) . Written by Arjona , the song was produced by Dan Warner , Lee Levin and Puerto Rican singer-songwriter Tommy Torres , who also worked with Arjona on Adentro . " Quiero " was recorded between several studios in Miami and Mexico City , and mixed and mastered in New York City . The song was called " bohemian " and " hippie " by website ADN Mundo , stating that it was " a love story that doesn 't speak about love " . " Quiero " became a moderate commercial success , reaching number 12 on the US Billboard Top Latin Songs chart , and number eight at the Latin Pop Songs chart . It also managed to appear at number 11 on the Latin Tropical Airplay chart , and received an American Society of Composers , Authors and Publishers for Pop / Ballad Song of the year in 2009 . It</t>
+          <t xml:space="preserve">Rated R : Remixed = Rated R : Remixed ( stylized as Rated R / / / Remixed ) is the second remix album by Barbadian singer Rihanna . It was released on May 8 , 2010 , in Brazil and Europe and on May 24 , 2010 , in the United States by Def Jam Recordings . It contains remixes from her fourth studio album , Rated R ( 2009 ) . The songs were solely remixed by Chew Fu . The majority of the remixes were remastered to incorporate influences from the genre of house music , and incorporate heavy usage of synthesizers as part of their instrumentation . Rated R : Remixed received a mixed review from Jean Goon for MSN Entertainment . She praised Fu for remixing some of the dark and sombre songs into upbeat dance songs , but criticized the album as it did not provide memorability . The album peaked at number four in Greece and number six on the US Dance / Electronic Albums chart ; it peaked at number 33 on the US Top R &amp; B / Hip-Hop Albums chart and number 158 on the US Billboard 200 chart . As of </t>
         </is>
       </c>
     </row>
@@ -511,32 +511,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['film', 'release', 'released', 'million', 'story', 'scene', 'scenes', 'script', 'effects', 'production', 'opening', 'plot', 'filming', 'original', 'director']</t>
+          <t>['tropical', 'storm', 'hurricane', 'winds', 'depression', 'cyclone', 'mph', 'damage', 'rainfall', 'landfall', 'utc', 'wind', 'weakened', 'flooding', 'intensity']</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>The Killer ( 1989 film ) = The Killer ( simplified Chinese : 喋血双雄 ; traditional Chinese : 喋血雙雄 ; Jyutping : dip6 hyut3 soeng1 hung4 ; pinyin : Diéxuè shuāngxióng ) † is a 1989 Hong Kong action film written and directed by John Woo , and starring Chow Yun-fat , Danny Lee and Sally Yeh . Chow plays the assassin Ah Jong , who accidentally damages the eyes of the singer Jennie ( Sally Yeh ) during a shootout . He later discovers that if Jennie does not have an expensive operation she will go blind . To get the money for Jennie , Ah Jong decides to perform one last hit . After the financial backing from Tsui Hark became problematic following the release of Woo 's film A Better Tomorrow 2 , Woo had to find backing through Chow Yun Fat and Danny Lee 's financing companies . Woo went into filming The Killer with a rough draft whose plot was influenced by the films Le Samouraï , Mean Streets , and Narazumono . Woo desired to make a film about honour , friendship and the relationship of two seem</t>
+          <t xml:space="preserve">1949 Pacific hurricane season = The 1949 Pacific hurricane season was the first hurricane season in the Eastern Pacific hurricane database . Six tropical cyclones were known to have existed during the season , of which the first formed on June 11 and the final dissipated on September 30 . Another tropical cyclone had formed within the basin in 1949 , but was included in the Atlantic hurricane database , had it been classified operationally in the Eastern Pacific basin , would have tallied the overall season to seven tropical cyclones . In addition , there were two tropical cyclones that attained hurricane status , but none of them reached major hurricane intensity ( Category 3 or higher on the Saffir-Simpson Hurricane Scale ) . Tropical Storm Three threatened the Baja California Peninsula , while an unnumbered hurricane crossed into the Atlantic , later becoming the 1949 Texas hurricane . = = Season summary = = Tropical cyclones were recorded in the Eastern Pacific best track database </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Transformers : Dark of the Moon = Transformers : Dark of the Moon is a 2011 American science fiction action film directed by Michael Bay and based on the Transformers toy line . First released on June 23 , 2011 , it is the third installment of the live-action Transformers film series and the sequel to 2009 's Revenge of the Fallen . The film 's story is set three years after the events of the 2009 film , and follows the warring Autobots and Decepticons as they battle to possess powerful technology from their homeworld that had crashed on Earth 's moon . The film stars Shia LaBeouf , Josh Duhamel , John Turturro , Tyrese Gibson , Rosie Huntington-Whiteley , Patrick Dempsey , Kevin Dunn , Julie White , John Malkovich and Frances McDormand . The script was written by Ehren Kruger , who also collaborated on the narrative of Revenge of the Fallen . Dark of the Moon employed both regular 35mm film cameras and specially-developed 3-D cameras , with filming locations in Chicago , Florida , Ind</t>
+          <t>1852 Atlantic hurricane season = The 1852 Atlantic hurricane season was one of only three Atlantic hurricane seasons in which every known tropical cyclone attained hurricane status . Five tropical cyclones were reported during the season , which lasted from late August through the middle of October ; these dates fall within the range of most Atlantic tropical cyclone activity , and none of the cyclones coexisted with another . Though there were officially five tropical cyclones in the season , hurricane scholar Michael Chenoweth assessed two of the cyclones as being the same storm . There may have been other unconfirmed tropical cyclones during the season , as meteorologist Christopher Landsea estimated that up to six storms were missed each year from the official database ; this estimate was due to small tropical cyclone size , sparse ship reports , and relatively unpopulated coastlines . = = Season summary = = Every tropical cyclone in the season was of hurricane status , or with win</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Escape from Tomorrow = Escape from Tomorrow is a 2013 American black-and-white independent fantasy horror film , the debut of writer and director Randy Moore . It follows an unemployed father having increasingly bizarre experiences and disturbing visions on the last day of a family vacation at the Walt Disney World Resort . It premiered in January at the 2013 Sundance Film Festival and was later a personal selection of Roger Ebert , shown at his 15th annual film festival in Champaign , Illinois . The film was a 2012 official selection of the PollyGrind Film Festival , but at the time filmmakers were still working on some legal issues and asked that it not be screened . It drew attention because Moore had shot most of it on location at both Walt Disney World and Disneyland without permission from The Walt Disney Company , owner and operator of both parks . Due to Disney 's reputation of being protective of its intellectual property , the cast and crew used guerrilla filmmaking technique</t>
+          <t xml:space="preserve">1930 Atlantic hurricane season = The 1930 Atlantic hurricane season was the second least active Atlantic hurricane season on record – behind only 1914 – with only three systems reaching tropical storm intensity . Of those three , two reached hurricane status , both of which also became major hurricanes , Category 3 or higher storms on the Saffir – Simpson hurricane wind scale . The first system developed in the central Atlantic Ocean on August 21 . Later that month , a second storm , the Dominican Republic hurricane , formed on August 29 . It peaked as a Category 4 hurricane with winds of 155 mph ( 250 km / h ) . The third and final storm dissipated on October 21 . Due to the lack of systems that developed , only one tropical cyclone , the second hurricane , managed to make landfall during the season . It severely impacted areas of the Greater Antilles , particularly the Dominican Republic , before making subsequent landfalls on Cuba and the U.S. states of Florida and North Carolina , </t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Batman Returns = Batman Returns is a 1992 American superhero film , directed and produced by Tim Burton , based on the DC Comics character Batman . It is the second installment of Warner Bros. ' initial Batman film series , with Michael Keaton reprising the title role of Bruce Wayne / Batman . The film introduces the characters of Max Shreck ( Christopher Walken ) , a business tycoon who teams up with the Penguin ( Danny DeVito ) to take over Gotham City , as well as the character of Catwoman ( Michelle Pfeiffer ) . Burton originally did not want to direct another Batman film because of his mixed emotions toward the previous film in 1989 . Warner Bros. developed a script with writer Sam Hamm which had the Penguin and Catwoman going after hidden treasure . Burton agreed to return after they granted him more creative control and replaced Hamm with Daniel Waters . Wesley Strick did an uncredited rewrite , removing the characters of Harvey Dent and Robin and rewriting the climax . Annette </t>
+          <t>1929 Atlantic hurricane season = The 1929 Atlantic hurricane season was among the least active hurricane seasons in the Atlantic on record – featuring only five tropical cyclones . Of these five tropical systems , three of them intensified into a hurricane , with one strengthening further into a major hurricane ( Category 3 or higher on the Saffir – Simpson hurricane wind scale ) . The first tropical cyclone of the season developed in the Gulf of Mexico on June 27 . Becoming a hurricane on June 28 , the storm struck Texas , bringing strong winds to a large area . Three fatalities were reported , while damage was conservatively estimated at $ 675,000 ( 1929 USD ) . The second storm , nicknamed the Bahamas hurricane , developed north of the Lesser Antilles . It was the most intense tropical cyclone of the season , peaking as a Category 4 hurricane on the Saffir – Simpson hurricane wind scale with maximum sustained winds of 155 mph ( 250 km / h ) and a minimum barometric pressure of 924 m</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Guardians of the Galaxy ( film ) = Guardians of the Galaxy is a 2014 American superhero film based on the Marvel Comics superhero team of the same name , produced by Marvel Studios and distributed by Walt Disney Studios Motion Pictures . It is the tenth film in the Marvel Cinematic Universe . The film was directed by James Gunn , who wrote the screenplay with Nicole Perlman , and features an ensemble cast including Chris Pratt , Zoe Saldana , Dave Bautista , Vin Diesel , Bradley Cooper , Lee Pace , Michael Rooker , Karen Gillan , Djimon Hounsou , John C. Reilly , Glenn Close , and Benicio del Toro . In Guardians of the Galaxy , Peter Quill forms an uneasy alliance with a group of extraterrestrial misfits who are fleeing after stealing a powerful artifact . Perlman began working on the screenplay in 2009 . Producer Kevin Feige first publicly mentioned Guardians of the Galaxy as a potential film in 2010 and Marvel Studios announced it was in active development at the San Diego Comic-Con </t>
+          <t xml:space="preserve">1939 Pacific hurricane season = The 1939 Pacific hurricane season ran through the summer and fall of 1939 . Before the satellite age started in the 1960s , data on east Pacific hurricanes are extremely unreliable . Most east Pacific storms are of no threat to land . However , 1939 saw a large number of storms threaten California . = = Storms = = = = = Hurricane One = = = On June 12 , a hurricane was detected . The lowest pressure reported by a ship was 985 mbar ( 29.1 inHg ) . The hurricane was last seen June 13 . = = = Possible Tropical Cyclone Two = = = A possible tropical cyclone was located off the coast of Mexico on June 27 . A ship reported a gale and a pressure of 1,006 mbar ( 29.7 inHg ) . The system was last seen on June 28 . = = = Tropical Cyclone Three = = = On July 19 , a tropical cyclone was detected . A ship reported a pressure of 1,000.7 millibars ( 29.55 inHg ) . = = = Tropical Cyclone Four = = = On July 29 , a tropical cyclone was located midway between Manzanillo and </t>
         </is>
       </c>
     </row>
@@ -546,32 +546,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>['career', 'hit', 'games', 'season', 'league', 'baseball', 'major_league_baseball', 'signed', 'home', 'played', 'manager', 'professional', 'minor', 'earned', 'hits']</t>
+          <t>['episode', 'mulder', 'scully', 'doctor', 'episodes', 'trek', 'files', 'series', 'character', 'enterprise', 'viewers', 'television', 'season', 'broadcast', 'star']</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jason Kipnis = Jason Michael Kipnis ( born April 3 , 1987 ; nicknamed " Kip " ) is an American professional baseball second baseman for the Cleveland Indians of Major League Baseball ( MLB ) . He attended Glenbrook North High School in the suburbs of Chicago , where he earned three letters playing baseball for the Glenbrook North Spartans . He attended the University of Kentucky , but transferred to Arizona State University after two years . In college , Kipnis was an All American and the 2009 Pacific-10 Conference Player of the Year for the Sun Devils . The Indians selected Kipnis in the second round of the 2009 Major League Baseball draft . In 2010 , he was named the Indians ' Minor League Player of the Year , and a Baseball America Minor League All Star . Prior to the 2011 season , Baseball Prospectus ranked him as the top Indians prospect and the 28th-highest prospect in baseball . At mid-season , Baseball America rated him as baseball 's 31st-best prospect . He was called up from </t>
+          <t>This Is Not Happening = " This Is Not Happening " is the fourteenth episode of the eighth season and the 175th episode overall of the science fiction television series The X-Files . The episode first aired in the United States on February 25 , 2001 on the Fox Network , and subsequently aired in the United Kingdom . It was written by executive producers Chris Carter and Frank Spotnitz , and directed by Kim Manners . The episode received a Nielsen household rating of 9.7 and was watched by 16.9 million viewers , making it the highest-rated episode of the season . " This Is Not Happening " was received positively by television critics . The series centers on FBI special agents Dana Scully ( Gillian Anderson ) and her new partner John Doggett ( Robert Patrick ) — following the alien abduction of her former partner , Fox Mulder ( David Duchovny ) — who work on cases linked to the paranormal , called X-Files . In this episode , Scully , Doggett , and Walter Skinner ( Mitch Pileggi ) discover</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Bobby Lowe = Robert Lincoln " Bobby " Lowe ( July 10 , 1865 – December 8 , 1951 ) , nicknamed " Link " , was an American Major League Baseball ( MLB ) player , coach and scout . He played for the Boston Beaneaters ( 1890 – 1901 ) , Chicago Cubs ( 1902 – 1903 ) , Pittsburgh Pirates ( 1904 ) , and Detroit Tigers ( 1904 – 1907 ) . Lowe was the first player in Major League history to hit four home runs in a game , a feat which he accomplished in May 1894 . He also tied or set Major League records with 17 total bases in a single game and six hits in a single game . Lowe was a versatile player who played at every position but was principally known as a second baseman . When he retired in 1907 , his career fielding average of .953 at second base was the highest in Major League history . Lowe also worked as a baseball manager , coach and scout . He was the player-manager of the Detroit Tigers during the last half of the 1904 season . He was also a player-manager for the Grand Rapids Wolverines</t>
+          <t>The X-Files ( season 2 ) = The second season of the science fiction television series The X-Files commenced airing on the Fox network in the United States on September 16 , 1994 , concluded on the same channel on May 19 , 1995 , after airing all 25 episodes . The series follows Federal Bureau of Investigation special agents Fox Mulder and Dana Scully , portrayed by David Duchovny and Gillian Anderson respectively , who investigate paranormal or supernatural cases , known as X-Files by the FBI . The second season of The X-Files takes place after the closure of the department following the events of the first season finale . In addition to stand-alone " Monster-of-the-Week " episodes , several episodes also furthered the alien conspiracy mythology that had begun to form . Season two introduced several recurring characters — X ( Steven Williams ) , an informant to Mulder ; Alex Krycek ( Nicholas Lea ) , Mulder 's partner-turned-enemy ; and the Alien Bounty Hunter ( Brian Thompson ) , a sh</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Tyler Clippard = Tyler Lee Clippard ( born February 14 , 1985 ) is an American professional baseball pitcher for the Arizona Diamondbacks of Major League Baseball ( MLB ) . He previously played for New York Yankees , Washington Nationals , Oakland Athletics , and New York Mets . After playing baseball at J. W. Mitchell High School in New Port Richey , Florida , the Yankees drafted Clippard in the ninth round of the 2003 MLB draft . He debuted with the Yankees as a starting pitcher in 2007 . The Yankees traded him to the Nationals before the 2008 season , and the Nationals converted him into a relief pitcher in 2009 . The Nationals traded Clippard to the Athletics before the 2015 season , who traded him to the Mets during the 2015 season . He signed as a free agent with the Diamondbacks before the 2016 season . Clippard led the major leagues in holds in 2014 . He was named to the MLB All-Star Game in 2011 and 2014 , and won the MLB Delivery Man of the Month Award in June 2012 . = = Amat</t>
+          <t>Wetwired = " Wetwired " is the twenty-third episode of the third season and the 72nd episode overall of the science fiction television series The X-Files . The episode first aired in the United States on May 10 , 1996 on Fox . It was written by the show 's visual effect designer Mat Beck , and directed by Rob Bowman . The episode earned a Nielsen rating of 9.7 and was viewed by 14.48 million people . The episode received mostly positive reviews from television critics . The show centers on FBI special agents Fox Mulder ( David Duchovny ) and Dana Scully ( Gillian Anderson ) who work on cases linked to the paranormal , called X-Files . Mulder is a believer in the paranormal , while the skeptical Scully has been assigned to debunk his work . In this episode , Mulder and Scully investigate a series of murders committed by ordinary citizens angered after seeing illusory images . Scully 's trust in Mulder is put to the ultimate test . " Wetwired " was written by Mat Beck , the show 's visua</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Ed Blake = Edward James Blake ( December 23 , 1925 – April 15 , 2009 ) was an American right-handed pitcher in Major League Baseball who played four seasons with the Cincinnati Reds and the Kansas City Athletics . In eight career games , Blake pitched 8 ⅔ innings and had an 8.31 earned run average ( ERA ) . After graduating high school in East St. Louis , Blake played in the farm system of the nearby St. Louis Cardinals before enlisting in the army . He returned to baseball after being wounded in the military service , pitching in the minors for five years before making his major league debut for the Cincinnati Reds . He pitched for them on and off for three years , then spent the next six years pitching for the Toronto Maple Leafs . His last major league appearance was a stint with the Athletics in 1957 , and two years later his professional baseball career ended . After retirement he became a plumber , and died in 2009 . = = Early life = = Born in St. Louis , Missouri to Edward and K</t>
+          <t>The X-Files ( season 8 ) = The eighth season of the American science fiction television series The X-Files commenced airing in the United States on November 5 , 2000 , concluded on May 20 , 2001 , and consisted of twenty-one episodes . Season eight takes place after Fox Mulder 's ( David Duchovny ) alien abduction in the seventh season . The story arc for the search of Mulder continues until the second half of the season , while a new arc about Dana Scully 's ( Gillian Anderson ) pregnancy is formed . This arc would continue , and end , with the next season . The season explores various themes such as life , death , and belief . For this season , Duchovny elected to return only as an intermittent main character , appearing in only half of the episodes . Actor Robert Patrick was hired as a replacement for Mulder , playing John Doggett . The season also marked the first appearance of Annabeth Gish as Monica Reyes , who would become a main character in the ninth season . In addition to th</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Guillermo Mota = Guillermo Reynoso Mota ( born July 25 , 1973 ) is a former Dominican professional baseball relief pitcher in Major League Baseball . In his career , he pitched for the Montreal Expos , Los Angeles Dodgers , Florida Marlins , Cleveland Indians , New York Mets , Milwaukee Brewers and San Francisco Giants . Mota stands 6 feet 6 inches ( 1.98 m ) tall and weighs 240 pounds ( 110 kg ) . He throws and bats right-handed . He throws three pitches : a fastball , a slider , and a circle changeup . Mota was originally signed by the New York Mets in 1990 as an infielder . After several years in their organization , he was drafted by the Montreal Expos in the Rule 5 draft in 1996 and converted into a pitcher in 1997 . Mota had a 2.96 ERA in 1999 , his rookie season , but he struggled in his next two seasons and was traded to the Los Angeles Dodgers prior to 2002 . His struggles continued in his first year with the Dodgers , but Mota had a career year in 2003 , as he had a 6 – 3 rec</t>
+          <t>Ascension ( The X-Files ) = " Ascension " is the sixth episode of the second season of the American science fiction television series The X-Files . It premiered on the Fox network on October 21 , 1994 . It was written by Paul Brown , directed by Michael Lange , and featured guest appearances by Steve Railsback , Nicholas Lea , Steven Williams and Sheila Larken . The episode helped explore the series ' overarching mythology . The show centers on FBI special agents Fox Mulder ( David Duchovny ) and Dana Scully ( Gillian Anderson ) who work on cases linked to the paranormal , called X-Files . However , the events of " Ascension " are a continuation of the plot of the preceding episode , " Duane Barry " . Following the kidnapping of Scully by an unhinged alien abductee Duane Barry ( Steve Railsback ) , Mulder races to track her down . The decision to have the character of Scully abducted was driven by necessity , as Anderson had become pregnant and required time off from production . " Asc</t>
         </is>
       </c>
     </row>
@@ -581,32 +581,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['work', 'life', 'wrote', 'writing', 'published', 'book', 'written', 'women', 'works', 'history', 'world', 'writer', 'woman', 'early', 'books']</t>
+          <t>['ship', 'guns', 'ships', 'tons', 'torpedo', 'knots', 'cruiser', 'inch', 'fleet', 'cruisers', 'deck', 'gun', 'turrets', 'admiral', 'steam']</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Alfred Döblin = Bruno Alfred Döblin ( August 10 , 1878 – June 26 , 1957 ) was a German novelist , essayist , and doctor , best known for his novel Berlin Alexanderplatz ( 1929 ) . A prolific writer whose œuvre spans more than half a century and a wide variety of literary movements and styles , Döblin is one of the most important figures of German literary modernism . His complete works comprise over a dozen novels ranging in genre from historical novels to science fiction to novels about the modern metropolis ; several dramas , radio plays , and screenplays ; a true crime story ; a travel account ; two book-length philosophical treatises ; scores of essays on politics , religion , art , and society ; and numerous letters — his complete works , republished by Deutscher Taschenbuch Verlag and Fischer Verlag , span more than thirty volumes . His first published novel , Die drei Sprünge des Wang-lung ( The Three Leaps of Wang Lun ) , appeared in 1915 and his final novel , Hamlet oder Die l</t>
+          <t>German aircraft carrier I ( 1915 ) = The aircraft carrier I was the first planned aircraft carrier conversion project of the German Imperial Navy ( Kaiserliche Marine ) during World War I. The Imperial Navy had experimented previously with seaplane carriers , though these earlier conversions were too slow to operate with the High Seas Fleet and carried an insufficient number of aircraft . I was intended to carry between 23 and 30 aircraft , including fighters , bombers , and torpedo-bombers . The ship was based on the incomplete hull of the Italian passenger ship Ausonia , which was being built in Hamburg . The conversion was proposed by the Air Department of the Reichs Navy Office , but it was abandoned after negotiations within the German Navy over a proposed moratorium on new ships at the end of the war . After World War I ended , high inflation in Germany added to the cost of the ship , and as a result , the Italian shipping company for whom the ship was originally built , declined</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Elias Abu Shabaki = Elias Abu Shabaki ( also spelled Ilyas Abu Shabaka ; Arabic : الياس أبو شبكة , May 3 , 1903 – January 27 , 1947 ) was a Lebanese writer , poet , editor , translator and literary critic , he was one of the founders of the literary League of Ten and is considered as one of the leading figures of the Arabic Nahda Movement . Born into a well-to-do Lebanese family , Abu Shabaki became interested in poetry at a young age . The son of a merchant , he was left fatherless in his youth , an experience that would mark his earlier works . Elias worked as a teacher , translator and _ in addition to publishing several volumes of poetry _ as a journalist writing for many Arabic newspapers and literary magazines . Being an adherent to the Romantic school , Abu Shabki believed in inspiration and denounced conscious control in poetry . His poems were gloomy , deeply personal and often contained biblical overtones centering on his internal moral conflicts . Some of Abu Shabaki 's work</t>
+          <t xml:space="preserve">French battlecruiser proposals = In the years before the outbreak of World War I in 1914 , the French Navy considered several proposals for battlecruisers . The Navy issued specifications for a battlecruiser design to complete part of the 28 capital ships to be built by 1920 . Three designs , one by P. Gille and two by Lieutenant Durand-Viel , were completed in 1913 . All three designs were similar to contemporary battleship designs , specifically the Normandie class , which introduced a quadruple gun turret for the main battery , which was adopted for all three proposals . The first two called for the same 340 mm ( 13 in ) gun used on all French dreadnoughts , though the third proposed a much more powerful 370 mm ( 15 in ) gun . Though the design studies were complete , the French Navy did not authorize or begin construction of any battlecruisers before the start of the war . = = Background = = In the Naval Law of 30 March 1912 , the French Navy called for a total force of 20 capital </t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ayn Rand = Ayn Rand ( / ˈaɪn ˈrænd / ; born Alisa Zinov 'yevna Rosenbaum , Russian : Али ́ са Зино ́ вьевна Розенба ́ ум ; February 2 [ O.S. January 20 ] 1905 – March 6 , 1982 ) was a Russian-born American novelist , philosopher , playwright , and screenwriter . She is known for her two best-selling novels , The Fountainhead and Atlas Shrugged , and for developing a philosophical system she called Objectivism . Educated in Russia , she moved to the United States in 1926 . She had a play produced on Broadway in 1935 – 1936 . After two early novels that were initially unsuccessful in America , she achieved fame with her 1943 novel , The Fountainhead . In 1957 , Rand published her best-known work , the novel Atlas Shrugged . Afterward , she turned to non-fiction to promote her philosophy , publishing her own magazines and releasing several collections of essays until her death in 1982 . Rand advocated reason as the only means of acquiring knowledge , and rejected faith and religion . She </t>
+          <t>SMS Frithjof = SMS Frithjof was the third vessel of the six-member Siegfried class of coastal defense ships ( Küstenpanzerschiffe ) built for the German Imperial Navy . Her sister ships were Siegfried , Beowulf , Heimdall , Hildebrand , and Hagen . Frithjof was built by the AG Weser shipyard between 1890 and 1893 , and was armed with a main battery of three 24-centimeter ( 9.4 in ) guns . She served in the German fleet throughout the 1890s and was rebuilt in 1900 - 1902 . She served in the VI Battle Squadron after the outbreak of World War I in August 1914 , but saw no action . Frithjof was demobilized in 1915 and used as a barracks ship thereafter . She was rebuilt as a merchant ship in 1923 and served in this capacity until she was broken up for scrap in 1930 . = = Design = = Frithjof was 79 meters ( 259 ft ) long overall and had a beam of 14.90 m ( 48.9 ft ) and a maximum draft of 5.74 m ( 18.8 ft ) . She displaced 3,741 long tons ( 3,801 t ) at full combat load . Her propulsion sys</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Andrea Dworkin = Andrea Rita Dworkin ( September 26 , 1946 – April 9 , 2005 ) was an American radical feminist and writer best known for her criticism of pornography , which she argued was linked to rape and other forms of violence against women . Although a radical , she said there was a need for liberals , but was widely criticized by liberal feminists . At the same time , she maintained a dialogue with political conservatives and wrote a topically-related book , Right-Wing Women . After suffering abuse from her first husband , she was introduced to radical feminist literature and began writing Woman Hating . Coming to New York , she became an activist on several issues and a writer , eventually publishing 10 books on feminism . During the late 1970s and 1980s , Dworkin became known as a spokeswoman for the feminist anti-pornography movement and for her writing on pornography and sexuality , particularly Pornography : Men Possessing Women ( 1981 ) and Intercourse ( 1987 ) , which rem</t>
+          <t>SMS Medusa = SMS Medusa was the seventh member of the ten-ship Gazelle class , built by the Imperial German Navy . She was built by the AG Weser dockyard in Bremen , laid down in early 1900 , launched in December 1900 , and commissioned into the High Seas Fleet in July 1901 . Armed with a main battery of ten 10.5 cm ( 4.1 in ) guns and two 45 cm ( 18 in ) torpedo tubes , Medusa was capable of a top speed of 21.5 knots ( 39.8 km / h ; 24.7 mph ) . Medusa served in all three German navies over the span of over forty years . She served as a fleet scout in the period before World War I , and during the first two years of the conflict , she was used as a coastal defense ship . She was one of six cruisers Germany was allowed to keep by the Treaty of Versailles , and she served in the early 1920s in the Reichsmarine . She was withdrawn from service in 1924 and used in secondary duties , but in 1940 , the Kriegsmarine converted Medusa into a floating anti-aircraft battery . She defended the po</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Assemblies of God USA = The Assemblies of God USA ( AG ) , officially the General Council of the Assemblies of God , is a Pentecostal Christian denomination in the United States founded in 1914 during a meeting of Pentecostal ministers at Hot Springs , Arkansas . It is the U.S. branch of the World Assemblies of God Fellowship , the world 's largest Pentecostal body . With a constituency of over 3 million , the Assemblies of God was the ninth largest denomination in the United States in 2011 . The Assemblies of God holds to a conservative , evangelical and Arminian theology as expressed in the Statement of Fundamental Truths and position papers , which emphasize such core Pentecostal doctrines as the baptism in the Holy Spirit , speaking in tongues , divine healing and the Second Coming of Christ . It defines for itself a fourfold mission to evangelize , worship God , disciple believers , and show compassion . The fellowship 's polity is a hybrid of presbyterian and congregational model</t>
+          <t>SMS Undine = SMS Undine was the last member of the ten-ship Gazelle class , built by the Imperial German Navy . She was built by the Howaldtswerke shipyard in Kiel , laid down in 1901 , launched in December 1902 , and commissioned into the High Seas Fleet in January 1904 . Armed with a main battery of ten 10.5 cm ( 4.1 in ) guns and two 45 cm ( 18 in ) torpedo tubes , Undine was capable of a top speed of 21.5 knots ( 39.8 km / h ; 24.7 mph ) . Undine was initially used as a artillery training ship for the gunners of the German fleet . In November 1904 , she accidentally rammed and sank the torpedo boat SMS S26 while on maneuvers off Kiel ; thirty-three men were killed in the incident . After the outbreak of World War in August 1914 , Undine was deployed to the Baltic Sea for use as a coastal defense ship . She was attacked by the British submarine HMS E19 on 7 November 1915 and was hit by two torpedoes , the second of which detonated the ship 's ammunition magazines . Undine exploded a</t>
         </is>
       </c>
     </row>
@@ -616,32 +616,32 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['tons', 'beam', 'deck', 'consisted', 'guns', 'laid', 'horsepower', 'armor', 'hull', 'boilers', 'displaced', 'steam', 'mounted', 'armament', 'battery']</t>
+          <t>['species', 'genus', 'shark', 'females', 'prey', 'eggs', 'males', 'cap', 'sharks', 'fruit', 'stem', 'brown', 'habitat', 'birds', 'specimens']</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Italian cruiser Varese = Varese was a Giuseppe Garibaldi-class armored cruiser built for the Royal Italian Navy ( Regia Marina ) in the 1890s . The ship made several deployments to the Eastern Mediterranean and the Levant before the start of the Italo-Turkish War of 1911 – 12 . She supported ground forces in the occupations of Tripoli and Homs in Libya . Varese may have bombarded Beirut and did bombard the defenses of the Dardanelles during the war . She also provided naval gunfire support for the Italian Army in Libya . During World War I , the ship 's activities were limited by the threat of Austro-Hungarian submarines and Varese became a training ship in 1920 . She was struck from the naval register in 1923 and subsequently scrapped . = = Design and description = = Varese had an overall length of 111.8 meters ( 366 ft 10 in ) , a beam of 18.2 meters ( 59 ft 9 in ) and a deep draft ( ship ) of 7.3 meters ( 23 ft 11 in ) . She displaced 7,350 metric tons ( 7,230 long tons ) at normal </t>
+          <t>Myco-heterotrophy = Myco-heterotrophy ( Greek : μυκός mykós , " fungus " , ἕτερος heteros = " another " , " different " and τροφή trophe = " nutrition " ) is a symbiotic relationship between certain kinds of plants and fungi , in which the plant gets all or part of its food from parasitism upon fungi rather than from photosynthesis . A myco-heterotroph is the parasitic plant partner in this relationship . Myco-heterotrophy is considered a kind of cheating relationship and myco-heterotrophs are sometimes informally referred to as " mycorrhizal cheaters " . This relationship is sometimes referred to as mycotrophy , though this term is also used for plants that engage in mutualistic mycorrhizal relationships . = = Relationship between myco-heterotrophs and host fungi = = Full ( or obligate ) myco-heterotrophy exists when a non-photosynthetic plant ( a plant largely lacking in chlorophyll or otherwise lacking a functional photosystem ) gets all of its food from the fungi that it parasitize</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Pisa-class cruiser = The Pisa class consisted of three armored cruisers built in Italy in the first decade of the 20th century . Two of these were for the Royal Italian Navy ( Regia Marina ) and the third was sold to the Royal Hellenic Navy and named Georgios Averof . This ship served as the Greek flagship for the bulk of her active career and participated in the Balkan Wars of 1912 – 13 , fighting in two battles against the Ottoman Navy . She played a minor role in World War II after escaping from Greece during the German invasion in early 1941 . Influenced by communist agitators , her crew mutinied in 1944 , but it was suppressed without any bloodshed . Georgios Averof returned to Greece after the German evacuation in late 1944 and became a museum ship in 1952 . She is the only surviving armored cruiser in the world . The two Italian ships participated in the Italo-Turkish War of 1911 – 12 during which they supported ground forces in Libya with naval gunfire and helped to occupy town</t>
+          <t>Cortinarius iodes = Cortinarius iodes , commonly known as the spotted cort or the viscid violet cort , is a species of agaric fungus in the family Cortinariaceae . The fruit bodies have small , slimy , purple caps up to 6 cm ( 2.4 in ) in diameter that develop yellowish spots and streaks in maturity . The gill color changes from violet to rusty or grayish brown as the mushroom matures . The species range includes the eastern North America , Central America , northern South America , and northern Asia , where it grows on the ground in a mycorrhizal association with deciduous trees . Although edible , the mushroom is not recommended for consumption . Cortinarius iodeoides , one of several potential lookalike species , can be distinguished from C. iodes by its bitter-tasting cap cuticle . = = Taxonomy = = The species was first described scientifically by Miles Joseph Berkeley and Moses Ashley Curtis in 1853 . The type collection was made by American botanist Henry William Ravenel in South</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Italian cruiser Minerva = Minerva was a torpedo cruiser of the Partenope class built for the Italian Regia Marina ( Royal Navy ) in the 1880s . The second of eight ships , Minerva was built by Gio . Ansaldo &amp; C. ; her keel was laid down in February 1889 , she was launched in February 1892 , and she was commissioned in August that year . Her main armament were her five torpedo tubes , which were supported by a battery of ten small-caliber guns . Minerva spent most of her career in the main Italian fleet , where she was primarily occupied with training exercises . She was converted into a minelayer in 1909 – 10 . She did not see significant action during the Italo-Turkish War in 1911 or World War I in 1915 – 18 , though she was used to lay defensive minefields during the latter conflict . The ship was sold for scrap in 1921 . = = Design = = Minerva was 73.1 meters ( 240 ft ) long overall and had a beam of 8.22 m ( 27.0 ft ) and an average draft of 3.48 m ( 11.4 ft ) . She displaced 833 m</t>
+          <t xml:space="preserve">Hygrophoropsis = Hygrophoropsis is a genus of gilled fungi in the family Hygrophoropsidaceae . It was circumscribed in 1888 to contain the type species , H. aurantiaca , a widespread fungus that , based on its appearance , has been affiliated with Cantharellus , Clitocybe , and Paxillus . Modern molecular phylogenetic analysis shows that the genus belongs to the suborder Coniophorineae of the order Boletales . There are 16 accepted species of Hygrophoropsis , found in both the Northern and Southern Hemispheres . Hygrophoropsis is a saprophytic genus that causes brown rot in the wood it colonises . The fruit bodies grow on the ground in woodlands , on moss , peat , and on woodchips . They are convex to infundibuliform ( funnel-shaped ) and have decurrent , forked brightly colored gills . The spores are dextrinoid , meaning that they stain reddish-brown in Melzer 's reagent . Because H. aurantiaca has orange gills , it has been mistaken for a chanterelle , and hence it has been called a </t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Soviet cruiser Chervona Ukraina = Chervona Ukraina ( Ukrainian : " Червона Україна " – " Red Ukraine " ) was an Admiral Nakhimov-class light cruiser of the Soviet Navy assigned to the Black Sea Fleet . During World War II , she supported Soviet forces during the Sieges of Odessa and Sevastopol before being sunk at Sevastopol on 12 November 1941 by German aircraft . She was raised in 1947 and was used as a training hulk before becoming a target ship in 1950 . = = Description = = Chervona Ukraina displaced 8,400 long tons ( 8,500 t ) at deep load . The ship had an overall length of 163.2 metres ( 535 ft 5 in ) , a beam of 15.7 metres ( 51 ft 6 in ) and a mean draught of about 5.6 metres ( 18 ft 4 in ) . She was powered by four Curtiss-AEG steam turbines , each driving one shaft , which developed a total of 55,000 shaft horsepower ( 41,000 kW ) and gave a maximum speed of 29.5 knots ( 54.6 km / h ; 33.9 mph ) . The engines were powered by 14 Yarrow water-tube boilers . Four were coal-fire</t>
+          <t>Lactarius deterrimus = Lactarius deterrimus , also known as false saffron milkcap or orange milkcap , is a species of fungus in the family Russulaceae . The fungus produces medium-sized fruit bodies ( mushrooms ) with orangish caps up to 12 cm ( 4.7 in ) wide that develop green spots in old age or if injured . Its orange-coloured latex stains maroon within 30 minutes . Lactarius deterrimus is a mycorrhizal fungus that associates with Norway spruce and bearberry . The species is distributed in Europe , but has also found in parts of Asia . A visually similar species in the United States and Mexico is not closely related to the European species . Fruit bodies appear between late June and November , usually in spruce forests . Although the fungus is edible — like all Lactarius mushrooms from the section Deliciosi — its taste is often bitter , and it is not highly valued . The fruit bodies are used as source of food for the larvae of several insect species . Lactarius deterrimus can be dis</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Océan-class ironclad = The Océan class ironclads were a group of three wooden-hulled armored frigates built for the French Navy in the mid to late 1860s . Océan attempted to blockade Prussian ports in the Baltic Sea in 1870 during the Franco-Prussian War . Marengo participated in the French conquest of Tunisia in 1881 . Suffren was often used as the flagship for the squadron she was assigned to . She was flagship of the Cherbourg Division , the Channel Division , Mediterranean Squadron and the Northern Squadron during her career . The ships were discarded during the 1890s . = = Design and description = = The Océan-class ironclads were designed by Henri Dupuy de Lôme as an improved version of the Provence-class ironclads . The ships were central battery ironclads with the armament concentrated amidships . For the first time in a French ironclad three watertight iron bulkheads were fitted in the hull . Like most ironclads of their era they were equipped with a metal-reinforced ram . The </t>
+          <t>Guepinia = Guepinia is a genus of fungus in the Auriculariales order . It is a monotypic genus , containing the single species Guepinia helvelloides , commonly known as the apricot jelly . The fungus produces salmon-pink , ear-shaped , gelatinous fruit bodies that grow solitarily or in small tufted groups on soil , usually associated with buried rotting wood . The fruit bodies are 4 – 10 cm ( 1.6 – 3.9 in ) tall and up to 17 cm ( 6.7 in ) wide ; the stalks are not well-differentiated from the cap . The fungus , although rubbery , is edible , and may be eaten raw with salads , pickled , or candied . It has a white spore deposit , and the oblong to ellipsoid spores measure 9 – 11 by 5 – 6 micrometers . The fungus is widely distributed in the Northern Hemisphere , and has also been collected from South America . = = Taxonomy = = The species was first described and illustrated as Tremella rufa by Nicolaus Joseph von Jacquin in 1778 . Elias Magnus Fries later ( 1828 ) called it Guepinia hel</t>
         </is>
       </c>
     </row>
@@ -651,32 +651,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['different', 'called', 'given', 'form', 'example', 'point', 'elements', 'real', 'use', 'possible', 'formula', 'sequence', 'particular', 'result', 'simple']</t>
+          <t>['highway', 'route', 'road', 'interchange', 'freeway', 'intersection', 'east', 'north', 'terminus', 'lane', 'continues', 'passes', 'avenue', 'state', 'highways']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Mobility analogy = The mobility analogy , also called admittance analogy or Firestone analogy , is a method of representing a mechanical system by an analogous electrical system . The advantage of doing this is that there is a large body of theory and analysis techniques concerning complex electrical systems , especially in the field of filters . By converting to an electrical representation , these tools in the electrical domain can be directly applied to a mechanical system without modification . A further advantage occurs in electromechanical systems : Converting the mechanical part of such a system into the electrical domain allows the entire system to be analysed as a unified whole . The mathematical behaviour of the simulated electrical system is identical to the mathematical behaviour of the represented mechanical system . Each element in the electrical domain has a corresponding element in the mechanical domain with an analogous constitutive equation . All laws of circuit analy</t>
+          <t xml:space="preserve">New Brunswick Route 95 = Route 95 is a 14.5-kilometre-long ( 9.0 mi ) provincial highway in New Brunswick , which serves a connector route between Interstate 95 ( I-95 ) and U.S. Route 2 ( US 2 ) at the Houlton – Woodstock Border Crossing near Houlton , Maine , United States to Route 2 , which is part of the Trans-Canada Highway , in Woodstock , New Brunswick , Canada . Prior to the construction of Route 95 , the connection between the two cities was served by Route 5 . In 2007 the New Brunswick government completed a roadworks project to turn Route 95 into a full freeway for its entire length . = = Route description = = Route 95 begins at the Houlton – Woodstock Border Crossing on the Maine – New Brunswick border as an extension of I-95 and US 2 . The border between the two countries also marks the border between the Eastern Time Zone and the Atlantic Time Zone . The highway travels northeast through woodlands as it approaches its first interchange with Route 540 via a hybrid diamond </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Liquid crystal = Liquid crystals ( LCs ) are matter in a state which has properties between those of conventional liquids and those of solid crystals . For instance , a liquid crystal may flow like a liquid , but its molecules may be oriented in a crystal-like way . There are many different types of liquid-crystal phases , which can be distinguished by their different optical properties ( such as birefringence ) . When viewed under a microscope using a polarized light source , different liquid crystal phases will appear to have distinct textures . The contrasting areas in the textures correspond to domains where the liquid-crystal molecules are oriented in different directions . Within a domain , however , the molecules are well ordered . LC materials may not always be in a liquid-crystal phase ( just as water may turn into ice or steam ) . Liquid crystals can be divided into thermotropic , lyotropic and metallotropic phases . Thermotropic and lyotropic liquid crystals consist mostly o</t>
+          <t>Missouri Route 108 = Route 108 is a short highway in the Bootheel of southeastern Missouri . Its eastern terminus is the Arkansas state line at Arkansas Highway 77 , about six miles ( 10 km ) south of Arbyrd , the only town on the route . Its western terminus is at U.S. Route 412 ( US 412 ) about two miles ( 3 km ) north of Arbyrd . Although signed as an east – west route , the route follows mostly north – south roadways . The route was designated in 1930 , and was extended east in 1972 . = = Route description = = Route 108 begins at the Arkansas state line in Arkmo , Dunklin County , where the road continues south into that state as Highway 77 . From the Arkansas-Missouri state line , the route heads north as a two-lane undivided road , passing a few homes and businesses in Arkmo before running through farmland . The road continues through rural areas to the southern edge of Arbyrd , where it reaches an intersection with Route 164 . At this point , Route 108 turns east to form a concu</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Taylor series = In mathematics , a Taylor series is a representation of a function as an infinite sum of terms that are calculated from the values of the function 's derivatives at a single point . The concept of a Taylor series was formulated by the Scottish mathematician James Gregory and formally introduced by the English mathematician Brook Taylor in 1715 . If the Taylor series is centered at zero , then that series is also called a Maclaurin series , named after the Scottish mathematician Colin Maclaurin , who made extensive use of this special case of Taylor series in the 18th century . A function can be approximated by using a finite number of terms of its Taylor series . Taylor 's theorem gives quantitative estimates on the error introduced by the use of such an approximation . The polynomial formed by taking some initial terms of the Taylor series is called a Taylor polynomial . The Taylor series of a function is the limit of that function 's Taylor polynomials as the degree i</t>
+          <t>Ontario Highway 400A = King 's Highway 400A , once known as the Highway 400 Extension , is an unsigned 400-series highway in the Canadian province of Ontario . The short 1.1-kilometre ( 0.7 mi ) freeway stub connects Highway 400 with Highway 11 and Simcoe County Road 93 , formerly Highway 93 . The highway was created in late 1959 by the opening of Highway 400 to Coldwater , although it has always featured Highway 400 signage along the southbound lanes and Highway 11 signage northbound . = = Route description = = Highway 400A is a 1.1-kilometre ( 0.7 mi ) 400-series highway located in the Canadian province of Ontario . The unisigned freeway includes a narrow grass median for the majority of its length , and features a speed limit of 100 kilometres per hour ( 62 mph ) . On average , the highway is used by approximately 11 , 900 vehicles daily . The route begins as Highway 400 exits on the right , with the northbound lanes rising up on an embankment and crossing Highway 400A . After the b</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Finite subdivision rule = In mathematics , a finite subdivision rule is a recursive way of dividing a polygon or other two-dimensional shape into smaller and smaller pieces . Subdivision rules in a sense are generalizations of fractals . Instead of repeating exactly the same design over and over , they have slight variations in each stage , allowing a richer structure while maintaining the elegant style of fractals . Subdivision rules have been used in architecture , biology , and computer science , as well as in the study of hyperbolic manifolds . Substitution tilings are a well-studied type of subdivision rule . = = Definition = = A subdivision rule takes a tiling of the plane by polygons and turns it into a new tiling by subdividing each polygon into smaller polygons . It is finite if there are only finitely many ways that every polygon can subdivide . Each way of subdividing a tile is called a tile type . Each tile type is represented by a label ( usually a letter ) . Every tile ty</t>
+          <t xml:space="preserve">Delaware Route 44 = Delaware Route 44 ( DE 44 ) is a state highway in Kent County , Delaware . It runs from DE 300 in Everetts Corner southeast to DE 8 in Pearsons Corner . The route passes through rural areas of western Kent County as well as the town of Hartly . In Hartly , it intersects DE 11 . The route was built as a state highway east of Hartly by 1924 and west of Hartly by 1932 , receiving the DE 44 designation by 1936 . = = Route description = = Delaware Route 44 heads to the southeast of DE 300 on Everetts Corner Road . It passes through a mix of woodland and farmland before reaching the town of Hartly . In Hartly , the route intersects DE 11 , where it becomes Main Street , and passes by homes . It then heads to the east out of Hartly on Hartly Road , passing through more rural areas . The route continues to its eastern terminus at DE 8 near Pearsons Corner . DE 44 has an annual average daily traffic count ranging from a high of 4,478 vehicles at the eastern terminus at DE 8 </t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Hilbert space = The mathematical concept of a Hilbert space , named after David Hilbert , generalizes the notion of Euclidean space . It extends the methods of vector algebra and calculus from the two-dimensional Euclidean plane and three-dimensional space to spaces with any finite or infinite number of dimensions . A Hilbert space is an abstract vector space possessing the structure of an inner product that allows length and angle to be measured . Furthermore , Hilbert spaces are complete : there are enough limits in the space to allow the techniques of calculus to be used . Hilbert spaces arise naturally and frequently in mathematics and physics , typically as infinite-dimensional function spaces . The earliest Hilbert spaces were studied from this point of view in the first decade of the 20th century by David Hilbert , Erhard Schmidt , and Frigyes Riesz . They are indispensable tools in the theories of partial differential equations , quantum mechanics , Fourier analysis ( which inc</t>
+          <t>Ontario Highway 23 = King 's Highway 23 , commonly referred to as Highway 23 , is a provincially maintained highway in the Canadian province of Ontario . The route travels from Highway 7 east of Elginfield north to Highway 9 and Highway 89 in Harriston . The total length of Highway 23 is 97.7 kilometres ( 60.7 miles ) . The highway was first established in 1927 between Highway 8 in Mitchell and Highway 9 in Teviotdale , via Monkton , Listowel and Palmerston . As part of a depression relief program , it was extended south to Highway 7 in 1934 . It remained relatively unchanged until 2003 , when it was rerouted northward from Palmerston to Harriston . = = Route description = = Highway 23 begins at Highway 7 , east of Elginfield , a community straddling the boundary between the municipalities of Middlesex Centre and Lucan Biddulph . The route travels north through the latter , surrounded on both sides by farmland . At Whalen Corners , the highway curves northeast as it exits Middlesex Cou</t>
         </is>
       </c>
     </row>
@@ -686,32 +686,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>['war', 'american', 'later', 'wrote', 'years', 'began', 'men', 'time', 'british', 'land', 'united_states', 'known', 'general', 'early', 'received']</t>
+          <t>['game', 'player', 'gameplay', 'games', 'players', 'playstation', 'nintendo', 'released', 'xbox', 'characters', 'graphics', 'soundtrack', 'mode', 'version', 'mario']</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Joseph Dudley = Joseph Dudley ( 23 September 1647 – 2 April 1720 ) was an English colonial administrator . A native of Roxbury , Massachusetts , and the son of one of its founders , Dudley had a leading role in the administration of the Dominion of New England ( 1686 – 1689 ) , overthrown in the 1689 Boston revolt , and served briefly on the council of the Province of New York . In New York , he oversaw the trial that convicted Jacob Leisler , the ringleader of Leisler 's Rebellion . He then spent eight years in England in the 1690s as Lieutenant-Governor of the Isle of Wight , including one year as a Member of Parliament for Newtown , ( Isle of Wight ) . In 1702 he returned to New England after being appointed governor of the provinces of Massachusetts Bay and New Hampshire , posts he held until 1715 . His rule of Massachusetts was characterized by hostility and tension , with political enemies opposing his attempts to gain a regular salary , and regularly making complaints about his </t>
+          <t>Dr. Mario = Dr. Mario ( Japanese : ドクターマリオ , Hepburn : Dokutā Mario , often stylized as D ℞ . Mario ) is a 1990 Mario arcade-style action puzzle video game designed by Gunpei Yokoi and produced by Takahiro Harada . Nintendo developed and published the game for the Nintendo Entertainment System and Game Boy consoles . The game 's soundtrack was composed by Hirokazu Tanaka . The game focuses on the player character Mario , who assumes the role of a doctor and is tasked with eradicating deadly viruses . In this falling block puzzle game , the player 's objective is to destroy the viruses populating the on-screen playing field by using colored capsules that are dropped into the field . The player manipulates the capsules as they fall so that they are aligned with viruses of matching colors , which removes them from play . The player progresses through the game by eliminating all the viruses on the screen in each level . Dr. Mario received positive reception , appearing on several " Best Ni</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Troy H. Middleton = Lieutenant General Troy Houston Middleton ( 12 October 1889 – 9 October 1976 ) was a distinguished educator and senior officer of the United States Army who served as a corps commander in the European Theatre during World War II and later as President of Louisiana State University ( LSU ) . He is best known for his decision to hold Bastogne during the Battle of the Bulge , contrary to the recommendation of General George Patton , Commanding General ( CG ) of the United States Third Army . Enlisting in the U.S. Army in 1910 , Middleton was first assigned to the 29th Infantry Regiment where he worked as a clerk . Here he did not become an infantryman as he had hoped , but he was pressed into service playing football , a sport strongly endorsed by the Army . Following two years of enlisted service , Middleton was transferred to Fort Leavenworth , Kansas , where he was given the opportunity to compete for an officer 's commission . Of the 300 individuals who were vying </t>
+          <t>Rhythm game = Rhythm game or rhythm action is a genre of music-themed action video game that challenges a player 's sense of rhythm . Games in the genre typically focus on dance or the simulated performance of musical instruments , and require players to press buttons in a sequence dictated on the screen . Doing so causes the game 's protagonist or avatar to dance or to play their instrument correctly , which increases the player 's score . Many rhythm games include multiplayer modes in which players compete for the highest score or cooperate as a simulated musical ensemble . While conventional control pads may be used as input devices , rhythm games often feature novel game controllers that emulate musical instruments . Certain dance-based games require the player to physically dance on a mat , with pressure-sensitive pads acting as the input device . The 1996 title PaRappa the Rapper has been deemed the first influential rhythm game , whose basic template formed the core of subsequen</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Saratoga campaign = The Saratoga Campaign in 1777 was an attempt by the British high command for North America to gain military control of the strategically important Hudson River valley during the American Revolutionary War . It ended in the surrender of the British army , which historian Edmund Morgan argues , " was a great turning point of the war , because it won for Americans the foreign assistance which was the last element needed for victory . The primary thrust of the campaign was planned and initiated by General John Burgoyne . Commanding a main force of some 8,000 men , he moved south in June from Quebec , boated up Lake Champlain to middle New York , then marched over the divide and down the Hudson Valley to Saratoga . He initially skirmished there with the Patriot defenders with mixed results . Then , after losses in the Battles of Saratoga in September and October , his deteriorating position and ever increasing size of the American army forced him to surrender his forces </t>
+          <t>Super Mario Bros. : The Lost Levels = Super Mario Bros. : The Lost Levels is a 1986 side-scrolling , platformer action game developed and published by Nintendo as the sequel to the 1985 Super Mario Bros. The games are similar in style and gameplay apart from a large increase in difficulty . Like the original , Mario or Luigi venture to rescue the princess from Bowser . Unlike the original , the game has no two-player option and Luigi is differentiated from his twin plumber brother by having less ground friction and higher jump height . The Lost Levels also introduces setbacks like poison mushroom power-ups , counterproductive level warps , and mid-air wind gusts . The main game has 32 levels across eight worlds , followed by five bonus worlds . The Lost Levels was first released in Japan for the Family Computer Disk System as Super Mario Bros. 2 ( Japanese : スーパーマリオブラザーズ 2 ) on June 3 , 1986 , following the success of its predecessor . It was developed by Nintendo R &amp; D4 , the team led</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Spanish conquest of Yucatán = The Spanish conquest of Yucatán was the campaign undertaken by the Spanish conquistadores against the Late Postclassic Maya states and polities in the Yucatán Peninsula , a vast limestone plain covering south-eastern Mexico , northern Guatemala , and all of Belize . The Spanish conquest of the Yucatán Peninsula was hindered by its politically fragmented state . The Spanish engaged in a strategy of concentrating native populations in newly founded colonial towns . Native resistance to the new nucleated settlements took the form of the flight into inaccessible regions such as the forest or joining neighbouring Maya groups that had not yet submitted to the Spanish . Among the Maya , ambush was a favoured tactic . Spanish weaponry included broadswords , rapiers , lances , pikes , halberds , crossbows , matchlocks and light artillery . Maya warriors fought with flint-tipped spears , bows and arrows and stones , and wore padded cotton armour to protect themselve</t>
+          <t>Super Mario Land = Super Mario Land is a 1989 side-scrolling platform video game , the first in the Super Mario Land series , developed and published by Nintendo as a launch title for their Game Boy handheld game console . In gameplay similar to that of the 1985 Super Mario Bros. , but resized for the smaller device 's screen , the player advances Mario to the end of 12 levels by moving to the right and jumping across platforms to avoid enemies and pitfalls . Unlike other Mario games , Super Mario Land is set in Sarasaland , a new environment depicted in line art , and Mario pursues Princess Daisy . The game introduces two Gradius-style shooter levels . At Nintendo CEO Hiroshi Yamauchi 's request , Game Boy creator Gunpei Yokoi 's Nintendo R &amp; D1 developed a Mario game to sell the new console . It was the first portable version of Mario and the first to be made without Mario creator and Yokoi protégé Shigeru Miyamoto . Accordingly , the development team shrunk Mario gameplay elements f</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Frederick Russell Burnham = Frederick Russell Burnham DSO ( May 11 , 1861 – September 1 , 1947 ) was an American scout and world-traveling adventurer . He is known for his service to the British South Africa Company and to the British Army in colonial Africa , and for teaching woodcraft to Robert Baden-Powell in Rhodesia . He helped inspire the founding of the international Scouting Movement . Burnham was born on a Lakota Sioux Indian reservation in Minnesota where he learned the ways of American Indians as a boy . By the age of 14 , he was supporting himself in California , while also learning scouting from some of the last of the cowboys and frontiersmen of the American Southwest . Burnham had little formal education , never finishing high school . After moving to the Arizona Territory in the early 1880s , he was drawn into the Pleasant Valley War , a feud between families of ranchers and sheepherders . He escaped and later worked as a civilian tracker for the United States Army in t</t>
+          <t>Music of the Final Fantasy series = Final Fantasy is a media franchise created by Hironobu Sakaguchi and owned by Square Enix that includes video games , motion pictures , and other merchandise . The series began in 1987 as an eponymous role-playing video game developed by Square , spawning a video game series that became the central focus of the franchise . The music of the Final Fantasy series refers to the soundtracks of the Final Fantasy series of video games , as well as the surrounding medley of soundtrack , arranged , and compilation albums . The series ' music ranges from very light background music to emotionally intense interweavings of character and situation leitmotifs . The franchise includes a main series of numbered games as well as several spin-off series such as Crystal Chronicles and the Final Fantasy Tactics series . The primary composer of music for the main series was Nobuo Uematsu , who single-handedly composed the soundtracks for the first nine games , as well as</t>
         </is>
       </c>
     </row>
@@ -721,32 +721,32 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>['game', 'released', 'games', 'player', 'music', 'version', 'original', 'series', 'release', 'story', 'characters', 'players', 'main', 'character', 'japan']</t>
+          <t>['film', 'films', 'bond', 'disney', 'movie', 'role', 'actor', 'director', 'cast', 'filming', 'script', 'production', 'starred', 'grossing', 'batman']</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Key ( company ) = Key is a Japanese visual novel studio which formed on July 21 , 1998 as a brand under the publisher VisualArt 's and is located in Kita , Osaka , Japan . Key released their debut visual novel Kanon in June 1999 , which combined an elaborate storyline , an up-to-date anime-style drawing style , and a musical score which helped to set the mood for the game . Key 's second game Air released in September 2000 had a similar if not more complex storyline to Kanon and a more thorough gameplay . Both Kanon and Air were originally produced as adult games , but Key broke this trend with their third title Clannad which was released in April 2004 for all ages . Key has worked in the past with Interchannel and Prototype for the consumer port releases of the brand 's games . Key collaborated with P.A. Works and Aniplex to produce the anime series Angel Beats ! ( 2010 ) and Charlotte ( 2015 ) . The brand 's ninth game Rewrite was released in June 2011 , and a fan disc for the game t</t>
+          <t>Paresh Mokashi = Paresh Mokashi ( born 6 February 1969 ) is an Indian filmmaker , producer , actor and Theatre director-producer ; working predominantly in Marathi cinema and Marathi theatre . He started working as a backstage worker for theatre and did few minor roles for plays as well as films . Mokashi made his directorial debut for theatre with the Marathi play , Sangeet Debuchya Mulee in 1999 . He continued to work for theatre and made his directorial debut for cinema with the 2009 Marathi feature film , Harishchandrachi Factory . The film depicts the making of India 's first full-length feature film , Raja Harishchandra ( 1913 ) , made by Dadasaheb Phalke . The film was acclaimed critically and won several awards . It was also selected as India 's official entry to 82nd Academy Awards in the Best Foreign Language Film category . = = Personal life = = Paresh Mokashi was born to a Maharashtrian family in Pune and was brought up in Lonavla . He is a grandson of a noted Marathi write</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Guitar Hero III : Legends of Rock = Guitar Hero III : Legends of Rock is a music rhythm game , the third main installment in the Guitar Hero series , and the fourth title overall . The game was published by Activision and distributed by RedOctane . It is the first game in the series to be developed by Neversoft after Activision 's acquisition of RedOctane and MTV Games ' purchase of Harmonix , the previous development studio for the series . The game was released worldwide for the PlayStation 2 , PlayStation 3 , Wii and Xbox 360 in October 2007 , with Budcat Creations assisting Neversoft on developing the PlayStation 2 port and Vicarious Visions solely developing on the Wii port respectively . Aspyr Media published the Microsoft Windows and Mac OS X versions of the game , releasing them later in 2007 . Guitar Hero III : Legends of Rock retains the basic gameplay from previous games in the Guitar Hero series , where the player uses a guitar-shaped controller to simulate the playing of l</t>
+          <t>Mani Ratnam = Gopala Ratnam Subramaniam ( born 2 June 1955 ) , commonly known by his screen name Mani Ratnam , is an Indian film director , screenwriter , and producer who predominantly works in Tamil cinema . Cited by the media as one of India 's most acclaimed and influential filmmakers , Mani Ratnam is widely credited with revolutionising the Tamil film industry and altering the profile of Indian cinema . Although working in the mainstream medium , his films are noted for their realism , technical finesse , and craft . The Government of India honoured him with the Padma Shri , acknowledging his contributions to film in 2002 . Despite being born into a film family , Mani Ratnam did not develop any interest towards films when he was young . Upon completion of his post graduation in management , he started his career as a consultant . He entered the film industry through the 1983 Kannada film Pallavi Anu Pallavi . The failure of his subsequent films would mean that he was left with lit</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Final Fantasy III = Final Fantasy III ( ファイナルファンタジーIII , Fainaru Fantajī Surī ) is a role-playing video game developed and published by Square in 1990 for the Family Computer as the third installment in the Final Fantasy series and the last main series game for the console . It is the first numbered Final Fantasy game to feature the job-change system . The story revolves around four orphaned youths drawn to a crystal of light . The crystal grants them some of its power , and instructs them to go forth and restore balance to the world . Not knowing what to make of the crystal 's pronouncements , but nonetheless recognizing the importance of its words , the four inform their adoptive families of their mission and set out to explore and bring back balance to the world . The game was originally released in Japan on April 27 , 1990 . It had not been released outside Japan until a remake was developed by Matrix Software for the Nintendo DS on August 24 , 2006 . At that time , it was the only</t>
+          <t>Balu Mahendra = Balanathan Benjamin Mahendran ( 20 May 1939 – 13 February 2014 ) , commonly known as Balu Mahendra , was a Sri Lankan cinematographer , director , screenwriter and film editor , who worked in various Indian film industries , primarily in Tamil cinema . Born into a Sri Lankan Tamil household , Mahendra developed a passion towards photography and literature at a young age . He was drawn towards film-making after witnessing the shoot of David Lean 's The Bridge on the River Kwai ( 1957 ) in Sri Lanka . A graduate of the London University , he started his career as a draughtsman before gaining an admission to the Film and Television Institute of India ( FTII ) to pursue a course in cinematography . Mahendra entered films as a cinematographer in the early 1970s and gradually rose to becoming a film-maker by the end of the decade . Making his directorial debut through the Kannada film Kokila ( 1977 ) , Mahendra made over 20 films in all South Indian languages and two in Hindi</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Pokémon Ruby and Sapphire = Pokémon Ruby Version and Sapphire Version ( ポケットモンスター ルビー &amp; サファイア , Poketto Monsutā Rubī &amp; Safaia , " Pocket Monsters : Ruby &amp; Sapphire " ) are the third installments of the Pokémon series of role-playing video games , developed by Game Freak and published by Nintendo for the Game Boy Advance . The games were first released in Japan in late 2002 and internationally in 2003 . Pokémon Emerald , a special edition version , was released two years later in each region . These three games ( Pokémon Ruby , Sapphire , and Emerald ) are part of the third generation of the Pokémon video game series , also known as the " advanced generation " . Remakes of the two games , titled Omega Ruby and Alpha Sapphire , were released for the Nintendo 3DS onward worldwide on November 21 , 2014 , exactly twelve years to the date of the original Ruby and Sapphire release date , with the exception of Europe , where it was released on November 28 , 2014 . The gameplay is mostly unchan</t>
+          <t xml:space="preserve">Vishal Bhardwaj = Vishal Bhardwaj ( born 4 August 1965 ) is an Indian film director , screenwriter , producer , music composer and playback singer . He is known for his work in Hindi cinema , and is the recipient of a Filmfare Award and seven National Film Awards in four categories . Bhardwaj made his debut as a music composer with the children 's film Abhay ( The Fearless ) ( 1995 ) , and received wider recognition with his compositions in Gulzar 's Maachis ( 1996 ) . He received the Filmfare RD Burman Award for New Music Talent for the latter . He went on to compose music for the films Satya ( 1998 ) and Godmother ( 1999 ) . For the latter , he garnered the National Film Award for Best Music Direction . Bhardwaj made his directorial debut with the children 's film Makdee ( 2002 ) , for which he also composed the music . He garnered critical acclaim and several accolades for writing and directing the Indian adaptations of three tragedies by William Shakespeare : Maqbool ( 2003 ) from </t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Blue Dragon = Blue Dragon ( Japanese : ブルードラゴン , Hepburn : Burū Doragon ) is a role-playing video game developed by Mistwalker and Artoon and published by Microsoft Game Studios exclusively for the Xbox 360 . Blue Dragon is based on a design by Final Fantasy series creator Hironobu Sakaguchi , who also supervised development and wrote the plot . It is both Mistwalker 's debut title and the first title to be helmed by Sakaguchi outside of Square Enix . The game was released in Japan on December 7 , 2006 , where it was sold both as a standalone title and as part of a bundle with the Xbox 360 ( including the game , the Xbox 360 system itself , and a Blue Dragon console skin ) . Other regions received only the game itself , with a release in Europe on August 24 , 2007 , and in North America on August 28 , 2007 . Taking place in a fictional open-world environment , the story of Blue Dragon focuses on five friends ( Shu , Jiro , Kluke , Zola , and Marumaro ) as they travel across the world t</t>
+          <t>Amanda Seyfried = Amanda Michelle Seyfried ( / ˈsaɪfrɛd / SY-fred ; born December 3 , 1985 ) is an American actress , model , and singer . She began her career as a model when she was 11 , then her acting career at 15 began an acting career with recurring parts on the soap operas As the World Turns and All My Children . In 2004 , Seyfried made her film debut in the teen comedy Mean Girls . Her subsequent supporting roles were in independent films , such as the drama Nine Lives ( 2005 ) and the crime drama Alpha Dog ( 2006 ) , she also had a recurring role in the UPN drama show Veronica Mars ( 2004 – 06 ) . Between 2006 and 2011 , she starred on the HBO drama series Big Love and appeared in the 2008 musical feature film Mamma Mia ! . Her other appearances include leading roles in the black comedy horror film Jennifer 's Body ( 2009 ) , as a call girl in the erotic thriller Chloe ( 2009 ) , the romantic drama-war film Dear John ( 2010 ) , and the romantic drama Letters to Juliet ( 2010 )</t>
         </is>
       </c>
     </row>
@@ -756,32 +756,32 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>['tropical', 'storm', 'cyclone', 'area', 'cyclones', 'near', 'level', 'wind', 'low', 'formed', 'depression', 'miles', 'winds', 'water', 'west']</t>
+          <t>['army', 'persian', 'byzantine', 'arab', 'syria', 'emperor', 'polish', 'muslim', 'byzantines', 'constantine', 'battle', 'hungary', 'ottoman', 'king', 'forces']</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1984 Pacific typhoon season = The 1984 Pacific typhoon season has no official bounds , but most tropical cyclones tend to form in the northwestern Pacific Ocean between May and November . These dates conventionally delimit the period of each year when most tropical cyclones form in the northwestern Pacific Ocean . Tropical Storms formed in the entire west pacific basin were assigned a name by the Joint Typhoon Warning Center . Tropical depressions that enter or form in the Philippine area of responsibility are assigned a name by the Philippine Atmospheric , Geophysical and Astronomical Services Administration or PAGASA . This can often result in the same storm having two names . A total of 30 tropical depressions formed in 1984 in the Western Pacific , of which 27 became tropical storms , 16 reached typhoon intensity , and two reached super typhoon strength . Eight tropical cyclones moved into mainland China , four struck Vietnam , four moved through the Philippines , and one cyclone m</t>
+          <t>Siege of Klis = The Siege of Klis or Battle of Klis ( Croatian : Opsada Klisa or Bitka kod Klisa , Turkish : Klise Kuşatması ) was a siege of Klis Fortress in the Kingdom of Croatia within Habsburg Monarchy . The siege of the fortress , which lasted for more than two decades , and the final battle near Klis in 1537 , were fought as a part of the Ottoman – Habsburg wars between the defending Croatian-Habsburg forces under the leadership of Croatian feudal lord Petar Kružić , and the attacking Ottoman army under the leadership of the Ottoman general Murat-beg Tardić . After decisive Ottoman victory at the Battle of Krbava field in 1493 , and especially after the Battle of Mohács in 1526 , the Croats continued defending themselves against the Ottoman attacks . The Ottoman conquest during the early years of the 16th century prompted the formation of the Uskoks , which were led by Croatian captain Petar Kružić , also called ( Prince of Klis ) . As a part of the Habsburg defensive system , U</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Mount Garibaldi = Mount Garibaldi is a potentially active stratovolcano in the Sea to Sky Country of British Columbia , 80 km ( 50 mi ) north of Vancouver , British Columbia , Canada . Located in the southernmost Coast Mountains , it is one of the most recognized peaks in the South Coast region , as well as British Columbia 's best known volcano . It lies within the Garibaldi Ranges of the Pacific Ranges . This heavily eroded dome complex occupies the southwest corner of Garibaldi Provincial Park overlooking the town of Squamish . It is the only major Pleistocene age volcano in North America known to have formed upon a glacier . Although part of the Garibaldi Volcanic Belt within the Cascade Volcanic Arc , it is not considered part of the Cascade Range . = = Human history = = = = = Indigenous people = = = To Squamish people , the local indigenous people of this territory , the mountain is called Nch 'kay . In their language it means " Dirty Place " or " Grimy One " . This name of the m</t>
+          <t>Cutzinas = Cutzinas or Koutzinas ( Greek : Κουτζίνας ) was a Berber tribal leader who played a major role in the wars of the East Roman or Byzantine Empire against the Berber tribes in Africa in the middle of the 6th century , fighting both against and for the Byzantines . A staunch Byzantine ally during the latter stages of the Berber rebellion , he remained an imperial vassal until his murder in 563 by the new Byzantine governor . = = Life = = Cutzinas was of mixed stock : his father was a Berber , while his mother came from the Romanized population of North Africa . Following the reconquest of North Africa by the East Roman ( Byzantine ) Empire in the Vandalic War ( 533 – 534 ) , several uprisings by the native Berber tribes occurred in the North African provinces . Cutzinas is mentioned by the eyewitness historian Procopius of Caesarea as one of the leaders of the rebellion in the province of Byzacena , alongside Esdilasas , Medisinissas and Iourphouthes . In spring 535 , however ,</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1986 Pacific typhoon season = The 1986 Pacific typhoon season has no official bounds ; it ran year-round in 1986 , but most tropical cyclones tend to form in the northwestern Pacific Ocean between May and December . These dates conventionally delimit the period of each year when most tropical cyclones form in the northwestern Pacific Ocean . Tropical Storms formed in the entire west pacific basin were assigned a name by the Joint Typhoon Warning Center . Tropical depressions that enter or form in the Philippine area of responsibility are assigned a name by the Philippine Atmospheric , Geophysical and Astronomical Services Administration or PAGASA . This can often result in the same storm having two names . A total of 32 tropical depressions formed in 1986 in the Western Pacific over an eleven-month time span . Of the 32 , 30 became tropical storms , 19 storms reached typhoon intensity , and 3 reached super typhoon strength . The Joint Typhoon Warning Center considered Vera as two tropi</t>
+          <t xml:space="preserve">Siege of Güns = The Siege of Güns or Siege of Kőszeg ( Turkish : Güns Kuşatması ) was a siege of Kőszeg ( German : Güns ) in the Kingdom of Hungary within the Habsburg Empire , that took place in 1532 . In the siege , the defending forces of the Austrian Habsburg Monarchy under the leadership of Croatian Captain Nikola Jurišić ( Hungarian : Miklós Jurisics ) , defended the small border fort of Kőszeg with only 700 – 800 Croatian soldiers , with no cannons and few guns . The defenders prevented the advance of the Ottoman army of 120,000 – 200,000 toward Vienna , under the leadership of Sultan Suleiman the Magnificent ( Ottoman Turkish : سليمان Süleymān ) and Pargalı Ibrahim Pasha . The exact outcome is unknown , since it has two versions which differ depending on the source . In the first version Nikola Jurišić rejected the offer to surrender on favourable terms , and in the second version , the city was offered terms for a nominal surrender . Suleiman , having been delayed nearly four </t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve">1988 Pacific hurricane season = The 1988 Pacific hurricane season was a Pacific hurricane season that saw a below-average amount of tropical cyclones form , the first time since 1981 . It officially began May 15 , 1988 in the eastern Pacific , and June 1 , 1988 in the central Pacific and lasted until November 30 , 1988 . These dates conventionally delimit the period of each year when most tropical cyclones form in the northeastern Pacific Ocean . The first named storm , Tropical Storm Aletta , formed on June 16 , and the last-named storm , Tropical Storm Miriam , was previously named Hurricane Joan in the Atlantic Ocean before crossing Central America and re-emerging in the eastern Pacific ; Miriam continued westward and dissipated on November 2 . The season produced 23 tropical depressions , of which 15 attained tropical storm status . Seven storms reached hurricane status , three of which became major hurricanes . The strongest storm of the season , Hurricane Hector , formed on July </t>
+          <t xml:space="preserve">Siege of Tyana = A Siege of Tyana was carried out by the Umayyad Caliphate in 707 – 708 / 708 – 709 in retaliation for a heavy defeat of an Umayyad army under Maimun the Mardaite by the Byzantine Empire in c . 706 . The Arab army invaded Byzantine territory and laid siege to the city in summer 707 or 708 . In fact virtually each of the extant Greek , Arabic and Syriac parallel sources has in this respect a different date . Tyana initially withstood the siege with success , and the Arab army faced great hardship during the ensuing winter . Emperor Justinian II sent a relief army in the next spring , but the Umayyads defeated them , whereupon the inhabitants of the city were forced to surrender . Despite the agreement of terms , the city was plundered and largely destroyed , and according to Byzantine sources its people were made captive and deported , leaving the city deserted . = = Background = = In 692 / 693 , the Byzantine emperor Justinian II ( reigned 685 – 695 and 705 – 711 ) and </t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>1997 Pacific hurricane season = The 1997 Pacific hurricane season was a very active hurricane season . With hundreds of deaths and hundreds of millions of dollars in damage , this season was the costliest and one of the deadliest Pacific hurricane seasons . This was due to the exceptionally strong 1997 – 98 El Niño event . The 1997 Pacific hurricane season officially started on May 15 , 1997 in the eastern Pacific , and on June 1 , 1997 in the central Pacific , and lasted until November 30 , 1997 . These dates conventionally delimit the period of each year when almost all tropical cyclones form in the northeastern Pacific Ocean . Several storms impacted land . The first was Tropical Storm Andres which killed four people and left another two missing . In August , Tropical Storm Ignacio took an unusual path , and its extratropical remnants caused minor damage in the Pacific Northwest and California . Linda became the most intense east Pacific hurricane in recorded history . Although it n</t>
+          <t>Michael Shishman of Bulgaria = Michael Asen III ( Bulgarian : Михаил Асен III , Mihail Asen III , commonly called Michael Shishman ( Михаил Шишман , Mihail Šišman ) ) , ruled as emperor ( tsar ) of Bulgaria from 1323 to 1330 . The exact year of his birth is unknown but it was between 1280 and 1292 . He was the founder of the last ruling dynasty of the Second Bulgarian Empire , the Shishman dynasty . After he was crowned , however , Michael used the name Asen to emphasize his connection with the Asen dynasty , the first one to rule over the Second Empire . An energetic and ambitious ruler , Michael Shishman led an aggressive but opportunistic and inconsistent foreign policy against the Byzantine Empire and the Kingdom of Serbia , which ended in the disastrous battle of Velbazhd which claimed his own life . He was the last medieval Bulgarian ruler who aimed at military and political hegemony of the Bulgarian Empire over the Balkans and the last one who attempted to seize Constantinople .</t>
         </is>
       </c>
     </row>
@@ -791,32 +791,32 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>['court', 'act', 'public', 'law', 'state', 'rights', 'case', 'government', 'right', 'cases', 'united_states', 'courts', 'decision', 'singapore', 'person']</t>
+          <t>['trains', 'station', 'railway', 'building', 'line', 'tunnel', 'bridge', 'rail', 'services', 'train', 'oslo', 'passenger', 'stations', 'river', 'built']</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Article 14 of the Constitution of Singapore = Article 14 of the Constitution of the Republic of Singapore , specifically Article 14 ( 1 ) , guarantees to Singapore citizens the rights to freedom of speech and expression , peaceful assembly without arms , and association . However , the enjoyment of these rights may be restricted by laws imposed by the Parliament of Singapore on the grounds stated in Article 14 ( 2 ) of the Constitution . There are two types of grounds . For the first type , it must be shown that restricting the rights is " necessary or expedient in the interest " of the grounds . The grounds are the security of Singapore and public order ( applicable to all three rights protected by Article 14 ( 1 ) ) , morality ( freedom of speech and freedom of association ) , and friendly relations with other countries ( freedom of speech only ) . In a 2005 judgment , the High Court expressed the view that the phrase necessary or expedient confers upon Parliament " an extremely wide</t>
+          <t>Upminster Bridge tube station = Upminster Bridge is a London Underground station on Upminster Road in the Upminster Bridge neighbourhood of the London Borough of Havering in northeast London , England . The station is on the District line and is the penultimate station on the eastern extremity of that line . The station was opened on 17 December 1934 by the London , Midland and Scottish Railway on the local electrified tracks between Upminster and Barking that were constructed in 1932 . The main station building is of a distinctive polygonal design . It has relatively low usage for a suburban station with approximately 1 million entries and exits during 2011 . = = History = = The London , Tilbury and Southend Railway from Fenchurch Street and Barking was constructed through the Upminster Bridge area in 1885 , with stations at Hornchurch and Upminster . The Whitechapel and Bow Railway opened in 1902 and allowed through services of the District Railway to operate to Upminster . The Metro</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Legitimate expectation in Singapore law = The doctrine of legitimate expectation in Singapore protects both procedural and substantive rights . In administrative law , a legitimate expectation generally arises when there has been a representation of a certain outcome by the public authorities to an individual . To derogate from the representation may amount to an abuse of power or unfairness . The doctrine of legitimate expectation as a ground to quash decisions of public authorities has been firmly established by the English courts . Thus , where a public authority has made a representation to an individual who would be affected by a decision by the authority , the individual has a legitimate expectation to have his or her views heard before the decision is taken . Alternatively , an individual may also have a legitimate expectation to a substantive right . The recognition of substantive legitimate expectations is somewhat controversial as it requires a balancing of the requirements o</t>
+          <t xml:space="preserve">Winschoten railway station = Winschoten ( Dutch pronunciation : [ ˈʋɪnsxoːtən ] ; abbreviation : Ws ) is an unstaffed railway station in Winschoten in the Netherlands . It is located on the Harlingen – Nieuweschans railway between Scheemda and Bad Nieuweschans in the province of Groningen . The station building , designed by Karel Hendrik van Brederode , was completed in 1865 and expanded in 1904 . Train services started on 1 May 1868 and have since been provided by Maatschappij tot Exploitatie van Staatsspoorwegen ( 1868 – 1937 ) , Nederlandse Spoorwegen ( 1938 – 2000 ) , NoordNed ( 2000 – 2005 ) , and Arriva ( 2005 – present ) . During World War II , 500 Jews were transported from the station via the Westerbork transit camp to Nazi concentration camps , where most of them were killed . The station has three tracks and two platforms . As of 2016 there are two local train services with trains every half an hour to and from Groningen , and trains every hour to and from Bad Nieuweschans </t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>United States v. More = United States v. More , 7 U.S. 159 ( 1805 ) , was a United States Supreme Court case in which the Court held that it had no jurisdiction to hear appeals from criminal cases in the circuit courts by writs of error . Relying on the Exceptions Clause , More held that Congress 's enumerated grants of appellate jurisdiction to the Court operated as an exercise of Congress 's power to eliminate all other forms of appellate jurisdiction . The second of forty-one criminal cases heard by the Marshall Court , More ensured that the Court 's criminal jurisprudence would be limited to writs of error from the state ( and later , territorial ) courts , original habeas petitions and writs of error from habeas petitions in the circuit courts , and certificates of division and mandamus from the circuit courts . Congress did not grant the Court jurisdiction to hear writs of error from the circuit courts in criminal cases until 1889 , for capital crimes , and 1891 , for other " inf</t>
+          <t>Trondheim Airport Station = Trondheim Airport Station ( IATA code : TRD ) , also known as Værnes Station ( Norwegian : Værnes holdeplass ) , is a railway station located within the terminal complex of Trondheim Airport , Værnes in Stjørdal , Norway . Situated on the Nordland Line , it serves both express trains and the Trøndelag Commuter Rail both operated by Norges Statsbaner . The station was opened on 15 November 1994 along with a new terminal at the airport , making it the first airport rail link in the Nordic Countries . The station cost NOK 24 million , and was built along the existing railway line . In each direction , the station handles one to two hourly commuter rail services , and three daily express services . Travel time to Trondheim is 38 minutes , while it is 9 hours and 5 minutes to Bodø . Access to the airport terminal is outdoors , but sheltered . = = Facilities = = The station is located at the terminal of Trondheim Airport , Værnes . The connection between the stati</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Article 15 of the Constitution of Singapore = Article 15 of the Constitution of the Republic of Singapore guarantees freedom of religion in Singapore . Specifically , Article 15 ( 1 ) states : " Every person has the right to profess and practise his religion and to propagate it . " The terms profess , practise and propagate are not defined in the Constitution , but cases from Singapore and other jurisdictions may shed light on their meaning . The word profess in relation to a religion was defined in a 1964 Singapore case not involving the Constitution as meaning " to affirm , or declare one 's faith in or allegiance to " . A 2001 Malaysian decision suggested that the profession of religion does not encompass the renunciation of a religion or the profession of an irreligious viewpoint . As regards the word propagate , in 1977 the Supreme Court of India held that it confers on an individual the right to transmit or spread his or her religion by an exposition of its tenets , but not the r</t>
+          <t>East Finchley tube station = East Finchley is a London Underground station in East Finchley in the London Borough of Barnet , north London . The station is on the High Barnet branch of the Northern line , between Highgate and Finchley Central stations and is in Travelcard Zone 3 . The station was opened in 1867 as part of the Great Northern Railway 's line between Finsbury Park and Edgware stations . As part of London Underground 's only partially completed Northern Heights plan , the station was completely rebuilt with additional tracks in the late 1930s . Northern line trains started serving the station in 1939 and main line passenger services ended in 1941 . = = History = = = = = Original station = = = East Finchley station was built by the Edgware , Highgate and London Railway ( EH &amp; LR ) on its line from Finsbury Park station to Edgware station . Before the line was opened it was purchased in July 1867 by the larger Great Northern Railway ( GNR ) , whose main line from King 's Cro</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Crimes Act of 1790 = The Crimes Act of 1790 ( or the Federal Criminal Code of 1790 ) , formally titled An Act for the Punishment of Certain Crimes Against the United States , defined some of the first federal crimes in the United States and expanded on the criminal procedure provisions of the Judiciary Act of 1789 . The Crimes Act was a " comprehensive statute defining an impressive variety of federal crimes . " As an enactment of the First Congress , the Crimes Act is often regarded as a quasi-constitutional text . The punishment of treason , piracy , counterfeiting , as well as crimes committed on the high seas or against the law of nations , followed from relatively explicit constitutional authority . The creation of crimes within areas under exclusive federal jurisdiction followed from the plenary power of Congress over the " Seat of the Government , " federal enclaves , and federal territories . The creation of crimes involving the integrity of the judicial process derived from Co</t>
+          <t>Oslo Tunnel = The Oslo Tunnel ( Norwegian : Oslotunnelen ) is a 3,632-meter ( 11,916 ft ) , double-track , railway tunnel which runs between Olav Kyrres plass and Oslo Central Station ( Oslo S ) in Oslo , Norway . The tunnel constitutes the eastern-most section of the Drammen Line and runs below the central business district of Oslo . It features the four-track Nationaltheatret Station , Norway 's second-busiest railway station , where the Oslo Tunnels lies directly beneath the Common Tunnel of the Oslo Metro . At Frogner , the Elisenberg Station was built , but has never been used . The tunnel is the busiest section of railway line in Norway and serves all west-bound trains from Oslo , including many services of the Oslo Commuter Rail and the Airport Express Train . Traditionally , Oslo had two stations , the larger Oslo East Station ( or Oslo Ø , located at the spot of the current Oslo S ) and Oslo West Station ( Oslo V ) , which served the Drammen Line . This caused a physical barri</t>
         </is>
       </c>
     </row>
@@ -826,32 +826,32 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>['bridge', 'miles', 'area', 'road', 'construction', 'river', 'route', 'line', 'traffic', 'dam', 'water', 'station', 'feet', 'tunnel', 'built']</t>
+          <t>['battalion', 'brigade', 'aircraft', 'division', 'regiment', 'squadron', 'wing', 'infantry', 'training', 'battalions', 'unit', 'units', 'flight', 'air', 'australian']</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Bergen Line = The Bergen Line ( Norwegian : Bergensbanen or Bergensbana ) , also called the Bergen Railway , is a 371-kilometre ( 231 mi ) long standard gauge railway line between Bergen and Hønefoss , Norway . The name is often applied for the entire route from Bergen via Drammen to Oslo , where the passenger trains go , a distance of 496 kilometres ( 308 mi ) . It is the highest mainline railway line in Northern Europe , crossing the Hardangervidda plateau at 1,237 metres ( 4,058 ft ) above sea level . The railway opened from Bergen to Voss in 1883 as the narrow gauge Voss Line . In 1909 the route was continued over the mountain to Oslo and the whole route converted to standard gauge , and the Voss Line became part of the Bergen Line . The line is single track , and was electrified in 1954-64 . The Bergen Line is owned and maintained by the Norwegian National Rail Administration , and served with passenger trains by Norwegian State Railways ( NSB ) and freight trains by CargoNet . Th</t>
+          <t>No. 77 Wing RAAF = No. 77 Wing was a Royal Australian Air Force ( RAAF ) wing of World War II . It formed part of No. 10 Operational Group ( later the Australian First Tactical Air Force ) at its establishment in November 1943 , when it comprised three squadrons equipped with Vultee Vengeance dive bombers . No. 77 Wing commenced operations in early 1944 , flying out of Nadzab , Papua New Guinea . Soon afterwards , however , the Vengeance units were withdrawn from combat and replaced with squadrons flying Douglas Bostons , Bristol Beaufighters and Bristol Beauforts . The wing saw action in the assaults on Noemfoor , Tarakan , and North Borneo , by which time it was an all-Beaufighter formation made up of Nos. 22 , 30 and 31 Squadrons . It was to have taken part in the Battle of Balikpapan in June 1945 , but unsuitable landing grounds meant that the Beaufighter units were withdrawn to Morotai , sitting out the remainder of the war before returning to Australia , where they disbanded , al</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Laguna Canyon = Laguna Canyon ( also called Cañada de las Lagunas , Spanish : Lagoon Canyon ) is the name of a canyon that cuts through the San Joaquin Hills in southern Orange County , California , in the United States , directly west of the city of Irvine . The canyon runs from northeast to southwest , drained on the east side by tributaries of San Diego Creek and on the west by Laguna Canyon Creek . It is deeper and more rugged on the southwestern end near Laguna Beach . Geologically , the canyon likely originated millions of years ago as the result of San Diego Creek cutting through the San Joaquin Hills . Uplift diverted that stream to its present course , leaving Laguna Canyon as a wind gap . California State Route 133 runs the entire length of the canyon connecting Laguna Beach and Irvine , while California State Route 73 crosses it , running southeast-northwest . A majority of the canyon is located within the Laguna Coast Wilderness Park ; small portions are part of Aliso and W</t>
+          <t>10th Combat Aviation Brigade ( United States ) = The Combat Aviation Brigade , 10th Mountain Division is a combat aviation brigade of the United States Army based at Fort Drum , New York . It is a subordinate unit of the 10th Mountain Division . Reactivated in 1988 , the 10th Mountain Division 's Combat Aviation Brigade supported the division as it undertook numerous operations and overseas contingencies in the 1990s , including Operation Restore Hope , Operation Uphold Democracy , and Task Force Eagle , as well as disaster relief following Hurricane Andrew . The brigade has since become involved in the War on Terrorism , seeing four deployments to Afghanistan to support Operation Enduring Freedom and a deployment to Iraq to support Operation Iraqi Freedom . The brigade is currently on its fourth deployment to Afghanistan and is serving in Regional Command - East under Combined Joint Task Force 101 in support of Operation Enduring Freedom . = = Organization = = The Combat Aviation Brig</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Oroville Dam = Oroville Dam is an earthfill embankment dam on the Feather River east of the city of Oroville , California in the United States . At 770 feet ( 230 m ) high , it is the tallest dam in the U.S. and serves mainly for water supply , hydroelectricity generation and flood control . The dam impounds Lake Oroville , the second largest man-made lake in the state of California , capable of storing more than 3.5 million acre-feet ( 4.4 km3 ) , and is located in the Sierra Nevada foothills east of the Sacramento Valley . Built by the California Department of Water Resources ( DWR ) , Oroville Dam is one of the key features of the California State Water Project ( SWP ) , one of two major projects passed that set up California 's statewide water system . Construction was initiated in 1961 , and despite numerous difficulties encountered during its construction , including multiple floods and a major train wreck on the rail line used to transport materials to the dam site , the embankm</t>
+          <t>166th Aviation Brigade ( United States ) = The 166th Aviation Brigade was an aviation training brigade of the United States Army headquartered at Fort Hood , Texas . It was a subordinate unit of First Army - Division West . An " AC / RC " ( Active Component / Reserve Component ) formation , the 166th Aviation Brigade was the sole organization responsible for the post-mobilization training of United States Army Reserve &amp; National Guard aviation units . The unit was formerly designated as 3rd Brigade , 75th Division . From 1997 , the 166th Aviation Brigade has trained other aviation units for front-line service . As such , it has never seen combat , and has thus never earned any campaign streamers or unit awards . As the only brigade in the First Army responsible for training aviation units , the 166th Aviation Brigade is the principal unit for training Army Reserve and Army National Guard assets preparing to deploy to contingencies around the world , which means it is responsible for 47</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Solomon Creek = Solomon Creek is a tributary of the Susquehanna River in Luzerne County , Pennsylvania , in the United States . It is approximately 8.8 miles ( 14.2 km ) long and flows through Fairview Township , Hanover Township , and Wilkes-Barre . The creek is affected by acid mine drainage and has significant loads of iron , aluminum , and manganese . The creek 's named tributaries are Spring Run , Sugar Notch Run , and Pine Creek . The Solomon Creek watershed is located in the Anthracite Valley section of the ridge-and-valley geographical province . Major rock formations in the watershed include the Mauch Chunk Formation , the Spechty Kopf Formation , and the Catskill Formation . Solomon Creek was first settled by Native Americans around 8000 to 6000 B.C.E. A settler arrived at the confluence of the creek with the Susquehanna River by 1774 . In the 1800s , more people began arriving in the watershed to exploit its natural resources . Anthracite mining was especially prevalent in t</t>
+          <t>18th Military Police Brigade ( United States ) = The 18th Military Police Brigade is a military police brigade of the United States Army based in Grafenwoehr , Germany , with subordinate battalions and companies stationed throughout Germany . It provides law enforcement and force protection duties to United States Army Europe . Activated during the Vietnam War , the Brigade oversaw all Military Police operations in the country for a large portion of the conflict , undertaking a wide variety of missions throughout the country and providing command and control for other military police groups in the region . After Vietnam , the Brigade deployed units to several other operations , namely Operation Desert Storm and Operation Provide Comfort . The brigade itself also deployed to Kosovo , supporting many of the units operating there attempting to settle unrest in the area due to the 1999 Bosnian War . The brigade has also seen multiple deployments in the Global War on Terrorism to the Iraq W</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Filton Abbey Wood railway station = Filton Abbey Wood railway station serves the town of Filton in South Gloucestershire , England , inside the Bristol conurbation . It is 4.4 miles ( 7.1 km ) from Bristol Temple Meads . Its three letter station code is FIT . There are three platforms but minimal facilities . The station is managed by Great Western Railway , the seventh company to be responsible for the station , and the third franchise since privatisation in 1997 . They provide most train services at the station , with two trains per day operated by CrossCountry . The general service level is eight trains per hour - two to South Wales , two to Bristol Parkway , two toward Weston-super-Mare and two toward Westbury . Filton Abbey Wood is the third station on the site . The first station , Filton , was opened in 1863 by the Bristol and South Wales Union Railway . The station had a single platform , with a second added in 1886 to cope with traffic from the Severn Tunnel . The station was </t>
+          <t>Special Troops Battalion , 173rd Airborne Brigade Combat Team ( United States ) = The Special Troops Battalion , 173rd Airborne Brigade Combat Team is a special troops battalion of the United States Army headquartered at Caserma Del Din in Vicenza , Italy . It is the organization for the command elements of the 173rd Airborne Brigade Combat Team . The battalion contains the brigade 's senior command structure , including its Headquarters and Headquarters Company , as well as communication and support elements . Activated in 2000 from inactivating support units , the Special Troops Battalion deployed with the 173rd Airborne Brigade Combat Team to Afghanistan in 2007 until 2008 and again in early 2010 . = = Organization = = The Special Troops Battalion is subordinate to the 173rd Airborne Brigade Combat Team and is a permanent formation of the brigade , as the 173rd 's command elements are all contained in the STB . The battalion consists of three companies and the brigade 's Headquarter</t>
         </is>
       </c>
     </row>
@@ -861,32 +861,32 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>['century', 'known', 'breed', 'horses', 'horse', 'found', 'popular', 'island', 'today', 'breeds', 'including', 'period', 'dog', 'large', 'early']</t>
+          <t>['election', 'governor', 'bush', 'republican', 'senate', 'president', 'democratic', 'massachusetts', 'campaign', 'presidential', 'elected', 'kentucky', 'lincoln', 'senator', 'vote']</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Maine Coon = The Maine Coon is the largest domesticated breed of cat . It has a distinctive physical appearance and valuable hunting skills . It is one of the oldest natural breeds in North America , specifically " native " to the state of Maine ( though the feline was simply introduced there ) , where it is the official state cat . No records of the Maine Coon 's exact origins and date of introduction to the United States exist , so several competing hypotheses have been suggested . The breed was popular in cat shows in the late 19th century , but its existence became threatened when long-haired breeds from overseas were introduced in the early 20th century . The Maine Coon has since made a comeback and is now one of the more popular cat breeds in the world . The Maine Coon is a large and sociable cat , hence its nickname , " the gentle giant " . It is characterized by a robust bone structure , rectangular body shape , a silky flowing coat and a long , bushy tail . The breed 's colors</t>
+          <t>James Fisher Robinson = James Fisher Robinson ( October 4 , 1800 – October 31 , 1882 ) was the 22nd Governor of Kentucky , serving the remainder of the unfinished term of Governor Beriah Magoffin . Magoffin , a Confederate sympathizer , became increasingly ineffective after the elections of 1861 yielded a supermajority to pro-Union forces in both houses of the Kentucky General Assembly . Magoffin agreed to resign the governorship , provided he could select his successor . He selected Robinson . Politically , Robinson opposed both secession and abolition . Though he had Union sympathies , he was considered a moderate , opposing both fugitive slave laws and the enlistment of black soldiers . As a state senator , he supported the Crittenden Compromise and opposed the Civil War . As governor , he drew criticism from the administration of President Abraham Lincoln for opposing the Emancipation Proclamation . = = Early life = = Robinson was born to Jonathan and Jane Black Robinson in Scott C</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Northern Isles = The Northern Isles ( Scots : Northren Isles ; Scottish Gaelic : Na h-Eileanan a Tuath ; Old Norse : Norðreyjar ) is an archipelago comprising a chain of islands off the north coast of mainland Scotland . The climate is cool and temperate and much influenced by the surrounding seas . There are two main island groups : Shetland and Orkney . There are a total of 26 inhabited islands with landscapes of the fertile agricultural islands of Orkney contrasting with the more rugged Shetland islands to the north , where the economy is more dependent on fishing and the oil wealth of the surrounding seas . Both have a developing renewable energy industry . They also share a common Pictish and Norse history . Both island groups were absorbed into the Kingdom of Scotland in the 15th century and remained part of the country following the formation of the Kingdom of Great Britain in 1707 , and later the United Kingdom after 1801 . The islands played a significant naval role during the</t>
+          <t xml:space="preserve">Christopher Greenup = Christopher Greenup ( c . 1750 – April 27 , 1818 ) was an American politician who served as a U.S. Representative and the third Governor of Kentucky . Little is known about his early life ; the first reliable records about him are documents recording his service in the Revolutionary War where he served as a lieutenant in the Continental Army and a colonel in the Virginia militia . After his service in the war , Greenup helped settle the trans-Appalachian regions of Virginia . He became involved in politics , and played an active role in three of the ten statehood conventions that secured the separation of Kentucky from Virginia in 1792 . He became one of the state 's first representatives , and served in the Kentucky General Assembly before being elected governor in a race where , due to his immense popularity , he ran unopposed . Greenup 's term in office was marred by accusations that he had participated in the Burr Conspiracy to align Kentucky with Spain prior </t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Narcissus ( plant ) = Narcissus / nɑːrˈsɪsəs / is a genus of predominantly spring perennial plants in the Amaryllidaceae ( amaryllis ) family . Various common names including daffodil , daffadowndilly , narcissus , and jonquil are used to describe all or some members of the genus . Narcissus has conspicuous flowers with six petal-like tepals surmounted by a cup- or trumpet-shaped corona . The flowers are generally white or yellow ( orange or pink in garden varieties ) , with either uniform or contrasting coloured tepals and corona . Narcissus were well known in ancient civilisation , both medicinally and botanically , but formally described by Linnaeus in his Species Plantarum ( 1753 ) . The genus is generally considered to have about ten sections with approximately 50 species . The number of species has varied , depending on how they are classified , due to similarity between species and hybridization . The genus arose some time in the Late Oligocene to Early Miocene epochs , in the I</t>
+          <t>John Breathitt = John Breathitt ( September 9 , 1786 – February 21 , 1834 ) was the 11th Governor of Kentucky . He was the first Democrat to hold this office and was the second Kentucky governor to die in office . Shortly after his death , Breathitt County , Kentucky was created and named in his honor . Early in life , Breathitt was appointed a deputy surveyor in Illinois Territory . On his return to Kentucky , he taught at a country school , and through wise investments , amassed enough wealth to sustain him while he studied law with Judge Caleb Wallace . In 1811 , he was elected to the first of several terms in the Kentucky House of Representatives . He was the Democratic nominee for lieutenant governor in 1828 . Although his running mate William T. Barry lost the office of governor to Thomas Metcalfe , Breathitt defeated his opponent for lieutenant governor . During his term as lieutenant governor , Breathitt was one of several proposed candidates to succeed John Rowan in the United</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Cuisine of the Thirteen Colonies = The cuisine of the Thirteen Colonies includes the foods , eating habits , and cooking methods of the Thirteen British colonies in North America before the American revolution . It was derived from familiar traditions from the colonists ’ home countries in the British Isles and particularly England . Many agricultural items came through trade with England and the West Indies . Certain familiar items grew better in the Old World than others , and this led to a dependence on imports which drove the daily lives of the colonists . However , the colonial diet was increasingly supplemented by new animal and plant foods indigenous to the New World . In the years leading up to 1776 , a number of events led to a drastic change in the diet of the American colonists . As they could no longer depend on British and West Indian imports , agricultural practices of the colonists began to focus on becoming completely self-sufficient . = = Regional cuisines = = The majo</t>
+          <t xml:space="preserve">Lazarus W. Powell = Lazarus Whitehead Powell ( October 6 , 1812 – July 3 , 1867 ) was the 19th Governor of Kentucky , serving from 1851 to 1855 . He was later elected to represent Kentucky in the U.S. Senate from 1859 to 1865 . The reforms enacted during Powell 's term as governor gave Kentucky one of the top educational systems in the antebellum South . He also improved Kentucky 's transportation system and vetoed legislation that he felt would have created an overabundance of banks in the Commonwealth . Powell 's election as governor marked the end of Whig dominance in Kentucky . Powell 's predecessor , John J. Crittenden , was the last governor elected from the party of the Commonwealth 's favorite son , Henry Clay . Following his term as governor , Powell was elected to the U.S. Senate . Before he could assume office , President James Buchanan dispatched Powell and Major Benjamin McCulloch to Utah to ease tensions with Brigham Young and the Mormons . Powell assumed his Senate seat </t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Salt = Common salt is a mineral composed primarily of sodium chloride ( NaCl ) , a chemical compound belonging to the larger class of salts ; salt in its natural form as a crystalline mineral is known as rock salt or halite . Salt is present in vast quantities in seawater , where it is the main mineral constituent . The open ocean has about 35 grams ( 1.2 oz ) of solids per litre , a salinity of 3.5 % . Salt is essential for human life , and saltiness is one of the basic human tastes . The tissues of animals contain larger quantities of salt than do plant tissues . Salt is one of the oldest and most ubiquitous food seasonings , and salting is an important method of food preservation . Some of the earliest evidence of salt processing dates to around 8,000 years ago , when people living in an area in what is now known as the country of Romania were boiling spring water to extract the salts ; a salt-works in China dates to approximately the same period . Salt was prized by the ancient Heb</t>
+          <t xml:space="preserve">Thomas E. Bramlette = Thomas Elliott Bramlette ( January 3 , 1817 – January 12 , 1875 ) was the 23rd Governor of Kentucky . He was elected in 1863 and guided the state through the latter part of the Civil War and the beginning of Reconstruction . At the outbreak of the war , Bramlette put his promising political career on hold and enlisted in the Union Army , raising and commanding the 3rd Kentucky Infantry . In 1862 , President Abraham Lincoln appointed him district attorney for Kentucky . A year later , he was the Union Democrats ' nominee for governor . Election interference by the Union Army gave him a landslide victory over his opponent , Charles A. Wickliffe . Within a year , however , federal policies such as recruiting Kentucky Negroes for the Union Army and suspending the writ of habeas corpus for Kentucky citizens caused Bramlette to abandon his support of the Lincoln administration and declare that he would " bloodily baptize the state into the Confederacy " . After the war </t>
         </is>
       </c>
     </row>
@@ -896,32 +896,32 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>['september', 'storm', 'mph', 'august', 'hurricane', 'october', 'day', 'damage', 'near', 'early', 'developed', 'later', 'tropical', 'began', 'caused']</t>
+          <t>['castle', 'church', 'century', 'castles', 'king', 'cathedral', 'tower', 'medieval', 'earl', 'england', 'nave', 'bishop', 'edward', 'chancel', 'built']</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1997 Pacific hurricane season = The 1997 Pacific hurricane season was a very active hurricane season . With hundreds of deaths and hundreds of millions of dollars in damage , this season was the costliest and one of the deadliest Pacific hurricane seasons . This was due to the exceptionally strong 1997 – 98 El Niño event . The 1997 Pacific hurricane season officially started on May 15 , 1997 in the eastern Pacific , and on June 1 , 1997 in the central Pacific , and lasted until November 30 , 1997 . These dates conventionally delimit the period of each year when almost all tropical cyclones form in the northeastern Pacific Ocean . Several storms impacted land . The first was Tropical Storm Andres which killed four people and left another two missing . In August , Tropical Storm Ignacio took an unusual path , and its extratropical remnants caused minor damage in the Pacific Northwest and California . Linda became the most intense east Pacific hurricane in recorded history . Although it n</t>
+          <t>Nidan = Nidan ( sometimes known as Midan or Idan ) was a Welsh priest and , according to some sources , a bishop , in the 6th and 7th centuries . He is now commemorated as a saint . He was the confessor for the monastery headed by St Seiriol at Penmon , and established a church at what is now known as Llanidan , which are both places on the Welsh island of Anglesey . He is the patron saint of two churches in Anglesey : St Nidan 's Church , Llanidan , built in the 19th century , and its medieval predecessor , the Old Church of St Nidan , Llanidan . Midmar Old Kirk in Aberdeenshire , Scotland , is also dedicated to him : Nidan is said to have helped to establish Christianity in that area as a companion of St Kentigern . St Nidan 's , Llanidan , has a reliquary dating from the 14th or 16th century , which is said to house his relics . = = Life = = Little is known in detail about Nidan 's life , and his year and place of birth are unknown . He is sometimes referred to as " Midan " or " Ida</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1975 Pacific hurricane season = The 1975 Pacific hurricane season officially started May 15 , 1975 in the eastern Pacific , and June 1 , 1975 in the central Pacific , and lasted until November 30 , 1975 . These dates conventionally delimit the period of each year when most tropical cyclones form in the northeast Pacific Ocean . The 1975 Pacific hurricane season was near average , with 17 tropical storms forming . Of these , 9 became hurricanes , and 4 became major hurricanes by reaching Category 3 or higher on the Saffir-Simpson Hurricane Scale . The only notable storms are Hurricane Olivia , which killed 30 people , caused $ 30 million ( 1975 USD ) in damage , and left thousands homeless when it made landfall in October ; and an unnamed hurricane that developed at very high latitude , but had no effect on land . Hurricane Denise was the strongest storm of the year . Hurricanes Lily and Katrina passed close to Socorro Island and Tropical Storm Eleanor made landfall in Mexico . Hurrican</t>
+          <t>Cynfarwy = Cynfarwy was a Christian in the 7th century about whom little is known . He was venerated by the early church in Wales as a saint , although he was never formally canonised . St Cynfarwy 's Church in Anglesey is dedicated to him , and his name is also preserved in the name of the settlement around the church , Llechgynfarwy ( or sometimes " Llechcynfarwy " ) . His feast day is in November , although the date varies between sources . = = Life and commemoration = = Little is known for certain about Cynfarwy ; his dates of birth and death are not given in the Bonedd y Saint ( a Welsh genealogical tract compiled in the late 18th century using material from older manuscripts ) . According to the 19th-century Celtic scholar Robert Williams , Cynfarwy was active in the 7th century . According to the Bonedd y Saint , he was the son of the otherwise unknown " Awy ab Llehenog , Lord of Cornwall " . Cynfarwy is venerated as a saint , although he was never canonized by a pope : as the h</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hurricane Charley = Hurricane Charley was the third named storm , the second hurricane , and the second major hurricane of the 2004 Atlantic hurricane season . Charley lasted from August 9 to August 15 , and at its peak intensity it attained 150 mph ( 240 km / h ) winds , making it a strong Category 4 hurricane on the Saffir-Simpson Hurricane Scale . It made landfall in southwestern Florida at maximum strength , making it the strongest hurricane to hit the United States since Hurricane Andrew struck Florida in 1992 . After moving slowly through the Caribbean Sea , Charley crossed Cuba on Friday , August 13 as a Category 3 hurricane , causing heavy damage and four deaths . That same day , it crossed over the Dry Tortugas , just 22 hours after Tropical Storm Bonnie had struck northwestern Florida . It was the first time in history that two tropical cyclones struck the same state in a 24-hour period . At its peak intensity of 150 mph ( 240 km / h ) , Hurricane Charley struck the northern </t>
+          <t>Æthelric II = Æthelric ( called Æthelric II to distinguish him from an earlier Æthelric who was also bishop of Selsey and also spelled Ethelric ; died c . 1076 ) was the second to last medieval Bishop of Selsey in England before the see was moved to Chichester . Consecrated a bishop in 1058 , he was deposed in 1070 for unknown reasons and then imprisoned by King William I of England . He was considered one of the best legal experts of his time , and was even brought from his prison to attend the trial on Penenden Heath where he gave testimony about English law before the Norman Conquest of England . = = Early life = = Æthelric was a monk at Christ Church Priory at Canterbury prior to his becoming a bishop . Several historians opine that he might have been the same as the Æthelric who was a monk of Canterbury and a relative of Godwin , Earl of Wessex . That Æthelric was elected by the monks of Canterbury to be Archbishop of Canterbury in 1050 , but was not confirmed by King Edward the C</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t xml:space="preserve">1997 Atlantic hurricane season = The 1997 Atlantic hurricane season was a below average season and is the most recent season to feature no tropical cyclones in August – typically one of the most active months . The season officially began on June 1 , and lasted until November 30 . These dates conventionally delimit the period of each year when most tropical cyclones form in the Atlantic basin . The 1997 season was inactive , with only seven named storms forming , with an additional tropical depression and an unnumbered subtropical storm . It was the first time since the 1961 season that there were no active tropical cyclones in the Atlantic basin during the entire month of August . A strong El Niño is credited with reducing the number of storms in the Atlantic , while increasing the number of storms in the Eastern and Western Pacific basin to 19 and 29 storms , respectively . As is common in El Niño years , tropical cyclogenesis was suppressed in the tropical latitudes , with only two </t>
+          <t>St Mary 's Church , Llanfair Mathafarn Eithaf = St Mary 's Church , Llanfair Mathafarn Eithaf is a small medieval church in Anglesey , north Wales . The earliest parts of the building , including the nave and the north doorway , date from the 14th century . Other parts , including the chancel and the east window , date from the 15th century . It is associated with the Welsh poet and clergyman Goronwy Owen , who was born nearby and served as curate here . He later travelled to America to teach at The College of William &amp; Mary , Virginia . The church is still in use for worship , as part of the Church in Wales , as one of three churches in the combined parish of Llanfair Mathafarn Eithaf with Llanbedrgoch with Pentraeth . It is a Grade II * listed building , a national designation given to " particularly important buildings of more than special interest " , because it is a " good rural church retaining substantial medieval fabric . " = = History and location = = St Mary 's Church is situ</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>1983 Pacific hurricane season = The 1983 Pacific hurricane season was the longest season ever recorded at that time . The 1983 Pacific hurricane season started on May 15 , 1983 in the eastern Pacific , and on June 1 , 1983 in the central Pacific , and lasted until November 30 , 1983 . These dates conventionally delimit the period of each year when most tropical cyclones form in the northeastern Pacific Ocean . During the 1983 season , there were 21 named storms , which was slightly less than the previous season . Furthermore , eight storms reached major hurricane status , or Category 3 or higher on the Saffir – Simpson hurricane wind scale ( SSHWS ) . The decaying 1982-83 El Niño event likely contributed to this level of activity . That same El Niño influenced a very quiet Atlantic hurricane season . The first storm of the season , Hurricane Adolph became the southernmost-forming east Pacific tropical cyclone on record after forming at a latitude of 7.1 ° N. After a slow start , activi</t>
+          <t>Hugh Nonant = Hugh Nonant ( sometimes Hugh de Nonant ; died 27 March 1198 ) was a medieval Bishop of Coventry in England . A great-nephew and nephew of two Bishops of Lisieux , he held the office of archdeacon in that diocese before serving successively Thomas Becket , the Archbishop of Canterbury and King Henry II of England . Diplomatic successes earned him the nomination to Coventry , but diplomatic missions after his elevation led to a long delay before he was consecrated . After King Henry 's death , Nonant served Henry 's son , King Richard I , who rewarded him with the office of sheriff in three counties . Nonant replaced his monastic cathedral chapter with secular clergy , and attempted to persuade his fellow bishops to do the same , but was unsuccessful . When King Richard was captured and held for ransom , Nonant supported Prince John 's efforts to seize power in England , but had to purchase Richard 's favour when the king returned . = = Early life = = Nonant was a great-nep</t>
         </is>
       </c>
     </row>
@@ -931,32 +931,32 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>['said', 'told', 'death', 'police', 'murder', 'family', 'life', 'found', 'asked', 'relationship', 'killed', 'later', 'mother', 'character', 'man']</t>
+          <t>['yard', 'yards', 'touchdown', 'season', 'michigan', 'team', 'nba', 'league', 'coach', 'tech', 'alabama', 'football', 'points', 'quarter', 'games']</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Wyatt Earp = Wyatt Berry Stapp Earp ( March 19 , 1848 – January 13 , 1929 ) was an American Old West gambler , a deputy sheriff in Pima County , and deputy town marshal in Tombstone , Arizona Territory , who took part in the Gunfight at the O.K. Corral , during which lawmen killed three outlaw Cowboys . He is often regarded as the central figure in the shootout in Tombstone , although his brother Virgil was Tombstone city marshal and Deputy U.S. Marshal that day , and had far more experience as a sheriff , constable , marshal , and soldier in combat . Earp lived a restless life . He was at different times a constable , city policeman , county sheriff , Deputy U.S. Marshal , teamster , buffalo hunter , bouncer , saloon-keeper , gambler , Brothel keeper , miner , and boxing referee . Earp spent his early life in Iowa . In 1870 , Earp married his first wife , Urilla Sutherland Earp , who contracted typhoid fever and died shortly before their first child was to be born . Within the next tw</t>
+          <t>Chad Mottola = Charles Edward " Chad " Mottola ( born October 15 , 1971 ) is an American retired professional baseball player who played five seasons in Major League Baseball ( MLB ) as an outfielder . Considered a journeyman , Mottola played professionally from 1992 through 2007 , appearing in 59 MLB games and 1,801 minor league games . He was the hitting coach for the Toronto Blue Jays during the 2013 season , but his contract was not renewed for 2014 . Mottola is an alumnus of the University of Central Florida ( UCF ) , where he played college baseball for the UCF Knights baseball team . A highly regarded prospect , Mottola was selected by the Cincinnati Reds with the fifth overall selection of the 1992 MLB Draft . Mottola played in minor league baseball for different organizations , receiving major league playing time with the Cincinnati Reds in 1996 , the Toronto Blue Jays in 2000 and 2006 , the Florida Marlins in 2001 and the Baltimore Orioles in 2004 . As he received less playin</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Chris Pappas ( Neighbours ) = Christos " Chris " Pappas is a fictional character from the Australian soap opera Neighbours , played by James Mason . Mason was told the character was gay when he successfully auditioned for the role in 2009 . He began filming his first scenes in October of that year and he made his first screen appearance during the episode broadcast on 25 February 2010 . Executive producer Susan Bower said the character 's storyline was created because of requests from young viewers in the Neighbours website 's online forums . The storyline has also been based on the real life experiences of the show 's writers . Chris was the first prominent , ongoing male homosexual character in the show 's twenty-five-year history . He was the second ongoing homosexual character overall , following Lana Crawford 's ( Bridget Neval ) introduction in 2004 . Chris departed on 27 March 2015 , but made a cameo appearance on 6 November . Chris was a high school student who befriended the s</t>
+          <t>Mickey Micelotta = Robert Peter " Mickey " Micelotta ( born October 20 , 1928 ) is a former American shortstop in Major League Baseball ( MLB ) . He played 13 total seasons of professional baseball , two of which were spent in the National League with the Philadelphia Phillies . In 17 career MLB games , Micelotta posted a batting average of .000 and had two runs in nine plate appearances . Born and raised in Wisconsin , Micelotta first played professionally with the Dayton Indians and Carbondale Pioneers in 1947 . Over the next three seasons , he played for various minor league teams in the Phillies organization before missing the 1951 and 1952 seasons , serving in the Korean War . He returned and played for the Terre Haute Phillies in 1953 and the Syracuse Chiefs from 1954 to 1955 , splitting time between the Chiefs and the Phillies ' major league squad . Micelotta spent the next three seasons with the Miami Marlins and three seasons after that with the Birmingham Barons before retiri</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Case of the Hooded Man = R v Williams ( 1913 ) 8 Cr App R 133 ( known as the Case of the Hooded Man and the Eastbourne Murder ) was a 1912 murder in England that took its name from the hood the defendant , John Williams , wore when travelling to and from court . After the murder of a police inspector in Eastbourne , with no witnesses and little forensic evidence , Edgar Power , a former medical student , told the police that his friend John Williams had committed the murder . Power helped the police conduct a sting operation to catch Williams ; police also interrogated Williams 's girlfriend Florence Seymour , who then confessed to having helped Williams hide the murder weapon . However , Seymour later recanted her story , and another man came forth claiming to know the identity of the real killer . This new evidence , along with the behaviour of the judge in both the initial case and the appeal , made the case controversial enough that Members of Parliament from the three major politi</t>
+          <t xml:space="preserve">J. T. White = John T. " J.T. " White ( July 10 , 1920 – November 21 , 2005 ) was a college football assistant coach , and a second-team 1947 College Football All-American center who played for national championship teams at both the University of Michigan and Ohio State University . White also played basketball for the Ohio State Buckeyes men 's basketball team . Although White was drafted to play professional football , he chose to pursue a career as an assistant football coach for both the Michigan Wolverines and Penn State Nittany Lions football teams . He served as an assistant coach for a national champion at Michigan and three undefeated and untied seasons at Penn State . White served in the United States Army during World War II causing a break in his collegiate education . = = Personal = = White was born in Wadley , Georgia and raised in River Rouge , Michigan . White earned his bachelor 's degree in education from Michigan in 1948 . He earned his master 's degree in education </t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Maurice Clemmons = Maurice Clemmons ( February 6 , 1972 – December 1 , 2009 ) was an American who was responsible for the November 29 , 2009 , murder of four police officers in Parkland , Washington . After evading police for two days following the shooting , Clemmons was shot and killed by a police officer in Seattle . Prior to his involvement in the shooting , Clemmons had at least five felony convictions in Arkansas and at least eight felony charges in Washington . His first incarceration began in 1989 , at age 17 . Facing sentences totaling 108 years in prison , the burglary sentences were reduced in 2000 by Governor of Arkansas Mike Huckabee to 47 years , which made him immediately eligible for parole . The Arkansas Parole Board unanimously moved to release him in 2000 . Clemmons was subsequently arrested on other charges and was jailed several times . In the months prior to the Parkland shooting , he was in jail on charges of assaulting a police officer and raping a child . One w</t>
+          <t>Eduardo Núñez = Eduardo Michelle Núñez Méndez ( born June 15 , 1987 ) is a Dominican professional baseball infielder for the Minnesota Twins of Major League Baseball ( MLB ) . He played in MLB for the New York Yankees from 2010 through 2013 . Although shortstop is his primary position , Núñez serves as a utility infielder , and played in the outfield for the Yankees as well . The Yankees signed Núñez as an international free agent in 2004 . He played minor league baseball in their organization from 2005 through 2010 , until he made his MLB debut with the Yankees on August 19 , 2010 . He has served to allow Derek Jeter and Alex Rodriguez the ability to take days off in the field . Due to struggles and inconsistency , the Yankees designated Núñez for assignment at the start of the 2014 season . He was traded to the Twins , and enjoyed a breakout season in 2016 , when he was named to appear in the MLB All-Star Game . = = Professional career = = = = = Minor leagues = = = The New York Yanke</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Joran van der Sloot = Joran Andreas Petrus van der Sloot ( Dutch pronunciation : [ ˈjoːrɑn vɑn dεr ˈsloːt ] ; born 6 August 1987 ) is a Dutch citizen , the murderer of Stephany Flores Ramírez in Lima , in 2010 , and the primary suspect in the 2005 disappearance of Natalee Holloway , in Aruba . After Flores Ramírez 's murder on 30 May 2010 van der Sloot fled to Chile , where he was arrested and extradited back to Peru for questioning regarding the murder . On 7 June 2010 , he confessed to bludgeoning Flores . He later tried to formally retract his confession , claiming that he had been intimidated by the National Police of Peru and framed by the FBI . A Peruvian judge ruled on 25 June 2010 that the confession was valid and on 13 January 2012 , Van der Sloot was sentenced to 28 years imprisonment for Flores ' murder . Five years earlier , while living in Aruba , van der Sloot had been the primary suspect in the disappearance of American teenager Natalee Holloway , who disappeared in Arub</t>
+          <t>Orator Shafer = George W. Shafer [ sometimes spelled Shaffer or Schaefer ] ( October 1851 – January 21 , 1922 ) was an outfielder in Major League Baseball . Nicknamed " Orator " , because he was an avid speaker , Shafer played for 10 teams in four different major leagues between 1874 and 1890 . Though he was a good hitter who batted over .300 three times , Shafer was best known for his defensive abilities . He led the National League 's outfielders in assists four times . In 1879 , he set an MLB single-season record with 50 outfield assists , which is a mark that has stood for over 130 years . He was considered by some to be the greatest right fielder of his era . Shafer was 5 feet 9 inches ( 1.75 m ) tall and weighed 165 pounds ( 75 kg ) . = = Background = = Shafer was born in Philadelphia , Pennsylvania , in 1851 . He was a " promising young Philadelphia amateur " before starting his professional baseball career in 1874 in the National Association . That year , he played in nine game</t>
         </is>
       </c>
     </row>
@@ -966,32 +966,32 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>['city', 'million', 'school', 'company', 'building', 'stadium', 'students', 'center', 'schools', 'year', 'sports', 'largest', 'located', 'community', 'years']</t>
+          <t>['olympics', 'olympic', 'athletes', 'medal', 'championships', 'murray', 'meter', 'freestyle', 'round', 'beijing', 'medals', 'games', 'gold', 'seconds', 'relay']</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blackford County , Indiana = Blackford County is located in the east central portion of the U.S. state of Indiana . The county is named for Judge Isaac Blackford , who was the first speaker of the Indiana General Assembly and a long-time chief justice of the Indiana Supreme Court . Created in 1838 , Blackford County is divided into four townships , and its county seat is Hartford City . Two incorporated cities and one incorporated town are located within the county . The county is also the site of numerous unincorporated communities and ghost towns . Occupying only 165.58 square miles ( 428.9 km2 ) , Blackford County is the fourth smallest county in Indiana . As of the 2010 census , the county 's population is 12,766 people in 5,236 households . Based on population , the county is the 8th smallest county of the 92 in Indiana . Although no interstate highways are located in Blackford County , three Indiana state roads cross the county , and an additional state road is located along the </t>
+          <t>Belize at the 2008 Summer Olympics = Belize competed in the 2008 Summer Olympics , held in Beijing , People 's Republic of China from 8 to 24 August 2008 . Its participation in Beijing marked its eighth Olympic appearance under the name " Belize " and its tenth overall , as its first two appearances ( 1968 in Mexico City and 1972 in Munich ) were under the name " British Honduras " . The Belizean delegation in 2008 included four athletes : three participated in track and field events ( Jonathan Williams , Tricia Flores , and Jayson Jones ) and one in taekwondo ( Alfonso Martínez ) . Belize did not medal in Beijing , and had not medaled before Beijing , but Jonathan Williams became the first Belizean athlete to advance past the first round of any Olympic event . = = Background = = Belize first participated in the Olympic games at the 1968 Summer Olympics in Mexico City and has appeared in every Summer Olympics since with the exception of the 1980 Summer Olympics in the Soviet Union , re</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>River Oaks , Houston = River Oaks is a residential community located in the center of Houston , Texas , United States . Located within the 610 Loop and between Downtown and Uptown , the community spans 1,100 acres ( 450 ha ) . Established in the 1920s by brothers William and Michael Hogg , the community became a well-publicized national model for community planning . River Oaks is the wealthiest and most expensive community in Texas and among the top ten in the United States . Real estate values in the community range from $ 1 million to over $ 20 million . River Oaks was also named the most expensive neighborhood in Houston in 2013 . The community is home to River Oaks Country Club , which includes a golf course designed by architect Donald Ross . = = History = = William and Michael Hogg , the sons of former Texas Governor Jim Hogg , and attorney Hugh Potter established River Oaks in the 1920s . Potter obtained an option to purchase 200 acres ( 81 ha ) around the River Oaks Country Cl</t>
+          <t>Mauritania at the 2008 Summer Olympics = Mauritania competed at the 2008 Summer Olympics which was held in Beijing , China . The country 's participation at Beijing marked its seventh appearance in the Summer Olympics since its debut in the 1984 Summer Olympics . The delegation included two track and field athletes , Souleymane Ould Chebal and Bounkou Camara , who were both selected by wildcards after both failed to meet either the " A " or " B " qualifying standards . Chebal was selected as the flag bearer for the opening ceremony . Neither of the Mauritanians progressed beyond the heats . = = Background = = Mauritania participated in seven Summer Olympic games between its debut in the 1984 Summer Olympics in Los Angeles , United States and the 2008 Summer Olympics in Beijing . Two athletes from Mauritania were selected to compete in the Beijing games ; Souleymane Ould Chebal in the track and field 800 meters and Bounkou Camara in the track and field 100 meters . Both were selected by</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Briarcliff Farms = Briarcliff Farms was a farm established in 1890 by Walter William Law in Briarcliff Manor , a village in Westchester County , New York . One of several enterprises established by Law at the turn of the 20th century , the farm was known for its milk , butter , and cream and also produced other dairy products , American Beauty roses , bottled water , and print media . At its height , the farm was one of the largest dairy operations in the Northeastern United States , operating about 8,000 acres ( 10 sq mi ) with over 1,000 Jersey cattle . In 1907 , the farm moved to Pine Plains in New York 's Dutchess County , and it was purchased by New York banker Oakleigh Thorne in 1918 , who developed it into an Angus cattle farm . After Thorne 's death in 1948 , the farm changed hands several times ; in 1968 it became Stockbriar Farm , a beef feeding operation . Stockbriar sold the farmland to its current owners in 1979 . The farm combined a practical American business model with </t>
+          <t>Great Britain at the 2010 Winter Paralympics = Great Britain competed at the 2010 Winter Paralympics held in Vancouver , Canada . The team was made up of athletes from the whole United Kingdom ; athletes from Northern Ireland , who may elect to hold Irish citizenship under the pre-1999 article 2 of the Irish constitution , are able to be selected to represent either Great Britain or Ireland at the Paralympics . Kelly Gallagher became the first Northern Irish athlete to compete in the Winter Paralympics by taking part in the alpine skiing discipline . Additionally some British overseas territories compete separately from Britain in Paralympic competition . In order to be eligible to take part in the Games athletes had to have a disability that fell into one of the five Paralympics disability categories . Great Britain fielded twelve athletes in total ; a team of five in wheelchair curling , and seven athletes in alpine skiing . The team failed to win a medal for the first time since the</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>International Finance Corporation = The International Finance Corporation ( IFC ) is an international financial institution that offers investment , advisory , and asset management services to encourage private sector development in developing countries . The IFC is a member of the World Bank Group and is headquartered in Washington , D.C. , United States . It was established in 1956 as the private sector arm of the World Bank Group to advance economic development by investing in strictly for-profit and commercial projects that purport to reduce poverty and promote development . The IFC 's stated aim is to create opportunities for people to escape poverty and achieve better living standards by mobilizing financial resources for private enterprise , promoting accessible and competitive markets , supporting businesses and other private sector entities , and creating jobs and delivering necessary services to those who are poverty-stricken or otherwise vulnerable . Since 2009 , the IFC has</t>
+          <t>Glencora Ralph = Glencora Ralph ( born 8 August 1988 ) is an Australian water polo centre back / driver . She attended the Curtin University of Technology and is a dental therapist . She competes for the Fremantle Marlins in the National Water Polo League , and was on sides that won the league championship in 2003 , 2004 , 2006 and 2007 . She has been a member of the Australia women 's national water polo team on the junior and senior level . She has won gold medals at the 2011 Canada Cup and at the 2007 FINA Junior World Championships . She won silver medals at the 2010 FINA World League Super Finals and at the 2010 FINA Women 's Water Polo World Cup . She won a bronze medal at the 2009 FINA World League Super Finals . She is one of seventeen players vying for thirteen spots on the national team to represent Australia in water polo at the 2012 Summer Olympics . = = Personal = = Ralph was born on 8 August 1988 in Geraldton , Western Australia . She has three siblings , one of whom , Me</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Amarillo , Texas = Amarillo ( / ˌæməˈrɪloʊ / am-ə-RIL-o ) is the fourteenth most populous city in the state of Texas , in the United States . It is also the largest city in the Texas Panhandle , and the seat of Potter County . A portion of the city extends into Randall County . The population was 190,695 at the 2010 census ( 105,486 in Potter County , and 85,209 in Randall ) . The Amarillo metropolitan area has an estimated population of 236,113 in four counties . Amarillo , originally named Oneida , is situated in the Llano Estacado region . The availability of the railroad and freight service provided by the Fort Worth and Denver City Railroad contributed to the city 's growth as a cattle marketing center in the late 19th century . The city was once the self-proclaimed " Helium Capital of the World " for having one of the country 's most productive helium fields . The city is also known as " The Yellow Rose of Texas " ( as the city takes its name from the Spanish word for yellow ) , </t>
+          <t xml:space="preserve">Great Britain at the 2008 Summer Olympics = The United Kingdom of Great Britain and Northern Ireland competed as Great Britain at the 2008 Summer Olympics in Beijing , China . The United Kingdom was represented by the British Olympic Association ( BOA ) , and the team of selected athletes was officially known as Team GB . Britain is one of only five NOCs to have competed in every modern Summer Olympic Games since 1896 . The delegation of 547 people included 311 competitors – 168 men , 143 women – and 236 officials . The team was made up of athletes from the whole United Kingdom including Northern Ireland ( whose people may elect to hold Irish citizenship and are able to be selected to represent either Great Britain or Ireland at the Olympics ) . Additionally some British overseas territories compete separately from Britain in Olympic competition . Great Britain 's medal performance at the 2008 Summer Olympics was its best in a century ; only its performance at the 1908 Summer Olympics </t>
         </is>
       </c>
     </row>
@@ -1001,32 +1001,32 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>['film', 'role', 'appeared', 'award', 'acting', 'director', 'roles', 'success', 'actor', 'performance', 'directed', 'comedy', 'drama', 'actors', 'films']</t>
+          <t>['match', 'tag', 'wrestling', 'championship', 'wwe', 'ring', 'raw', 'event', 'michaels', 'defeated', 'heavyweight', 'smackdown', 'feud', 'wwf', 'angle']</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Jonathan Pryce = Jonathan Pryce , CBE ( born John Price ; 1 June 1947 ) is a Welsh actor and singer . After studying at the Royal Academy of Dramatic Art and meeting his longtime girlfriend , English actress Kate Fahy , in 1974 , he began his career as a stage actor in the 1970s . His work in theatre , including an award-winning performance in the title role of the Royal Court Theatre 's Hamlet , led to several supporting roles in film and television . He made his breakthrough screen performance in Terry Gilliam 's 1985 cult film Brazil . Critically lauded for his versatility , Pryce has participated in big-budget films including Evita , Tomorrow Never Dies , Pirates of the Caribbean , The New World , GI Joe : The Rise of Cobra , GI Joe : Retaliation as well as independent films including Glengarry Glen Ross and Carrington . His career in theatre has also been prolific , and he has won two Tony Awards — the first in 1977 for his Broadway debut in Comedians , the second for his 1991 rol</t>
+          <t>Backlash ( 2007 ) = Backlash ( 2007 ) was a professional wrestling pay-per-view event produced by World Wrestling Entertainment ( WWE ) , which took place on April 29 , 2007 , at the Philips Arena in Atlanta , Georgia . Following WrestleMania , all pay-per-views became tri-branded . It was the ninth annual event under the Backlash name and starred talent from Raw , SmackDown ! , and ECW . The main match on the Raw brand was a Fatal Four-Way match for the WWE Championship involving champion John Cena , Randy Orton , Edge , and Shawn Michaels . Cena won the match and retained the championship after pinning Orton . The primary match on the SmackDown ! brand was a Last Man Standing match for the World Heavyweight Championship between The Undertaker and Batista , which ended in a no-contest after both men failed get to their feet before the referee counted to ten . The featured match on the ECW brand was Bobby Lashley versus Team McMahon ( Umaga , Vince and Shane McMahon ) in a Handicap mat</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Anurag Kashyap = Anurag Singh Kashyap ( born 10 September 1972 ) is an Indian film director , screenwriter , producer and actor . He is often regarded as the face of an emerging new wave cinema for producing numerous independent films with newcomers . For his contributions to film , the Government of France awarded him the Ordre des Arts et des Lettres ( Knight of the Order of Arts and Letters ) in 2013 . After writing a television serial , Kashyap got his major break as a co-writer in Ram Gopal Varma 's crime drama Satya ( 1998 ) , and made his directorial debut with Paanch , which never had a theatrical release due to censorship issues . He then went on to direct Black Friday ( 2007 ) , a film based on the book by Hussain Zaidi about the 1993 Bombay bombings . Its release was held up for two years by the Central Board of Film Certification because of the pending verdict of the case at that time , but was released in 2007 to widespread critical appreciation . Kashyap 's followup , No </t>
+          <t xml:space="preserve">World Heavyweight Championship ( WWE ) = The World Heavyweight Championship was a professional wrestling world heavyweight championship owned by WWE . It was one of two top championships in WWE , complementing the WWE World Championship . It was established under the Raw brand in 2002 , after Raw and SmackDown ! became distinct brands under WWE , and moved between both brands on different occasions ( mainly as a result of the WWE draft ) until August 29 , 2011 when all programming became full roster " supershows " . The World Heavyweight Championship was retired at the WWE PPV TLC : Tables , Ladders , and Chairs on December 15 , 2013 when it was unified with the WWE Championship . The title was one of six to be represented by the historic Big Gold Belt , first introduced in 1986 . Its heritage can be traced back to the first world heavyweight championship , thereby giving the belt a legacy over 100 years old , the oldest in the world . = = History = = = = = Origin = = = WWE introduced </t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ranveer Singh = Ranveer Singh Bhavnani ( born 6 July 1985 ) is an Indian film actor who appears in Hindi films . After completing a bachelor 's degree from Indiana University , Bloomington , Singh returned to India to pursue a career in film . He made his acting debut in 2010 with a leading role in Yash Raj Films ' romantic comedy Band Baaja Baaraat . The film emerged as a critical and commercial success , earning Singh a Filmfare Award in the Best Male Debut category . Singh went on to star in the romantic drama Lootera ( 2013 ) , Sanjay Leela Bhansali 's tragic romance Goliyon Ki Raasleela Ram-Leela ( 2013 ) , his biggest commercial successes to that point , and in the action-drama Gunday ( 2014 ) . In 2015 , he starred in the ensemble comedy-drama Dil Dhadakne Do ( 2015 ) , and portrayed Bajirao I in the historical romance Bajirao Mastani , one of the highest-grossing Bollywood films , for which he garnered critical acclaim and won the Filmfare Award for Best Actor . = = Early life </t>
+          <t>Cyber Sunday ( 2007 ) = Cyber Sunday ( 2007 ) was the fourth annual Cyber Sunday professional wrestling pay-per-view event produced by World Wrestling Entertainment ( WWE ) . It was presented by Fathead and took place on October 28 , 2007 , at the Verizon Center in Washington , D.C. The most important feature of Cyber Sunday is the ability for fans to vote online through WWE.com on certain aspects of every match . The main match on the SmackDown ! brand was Batista versus The Undertaker for the World Heavyweight Championship , which Batista won by pinfall after executing a Batista Bomb . The Special Guest Referee , which was either Stone Cold Steve Austin , John " Bradshaw " Layfield or Mick Foley . The predominant match on the Raw brand was for the WWE Championship between Randy Orton and the fans ' choice of either Shawn Michaels , Jeff Hardy or Mr. Kennedy . The voting for the event started on October 9 , 2007 , and ended during the event . Most of the existing feuds continued after</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Michael Sheen = Michael Sheen , OBE ( born 5 February 1969 ) is a Welsh actor . After training at London 's Royal Academy of Dramatic Art ( RADA ) , he worked mainly in theatre throughout the 1990s and made notable stage appearances in Romeo and Juliet ( 1992 ) , Don 't Fool With Love ( 1993 ) , Peer Gynt ( 1994 ) , The Seagull ( 1995 ) , The Homecoming ( 1997 ) , and Henry V ( 1997 ) . His performances in Amadeus at the Old Vic and Look Back in Anger at the National Theatre were nominated for Olivier Awards in 1998 and 1999 , respectively . In 2003 , he was nominated for a third Olivier Award for his performance in Caligula at the Donmar Warehouse . Sheen has become better known as a screen actor since the 2000s , in particular through his roles in various biopics . With writer Peter Morgan , he has starred in a trilogy of films as British politician Tony Blair : the television film The Deal in 2003 , followed by The Queen ( 2006 ) and The Special Relationship ( 2010 ) . For playing B</t>
+          <t>Judgment Day ( 2007 ) = Judgment Day ( 2007 ) was the ninth annual Judgment Day professional wrestling pay-per-view event produced by World Wrestling Entertainment ( WWE ) . It took place on May 20 , 2007 from the Scottrade Center in St. Louis , Missouri . This was the first Judgment Day event since 2003 to be an inter-brand pay-per-view , as it featured talent from the Raw , SmackDown ! , and ECW brands . The main match on the Raw brand was John Cena versus The Great Khali for the WWE Championship , which Cena won after forcing Khali to submit to the STFU . The featured match on the SmackDown ! brand was Edge versus Batista for the World Heavyweight Championship , which Edge won via pinfall with a school boy pin . The primary match on the ECW brand was a Handicap match for the ECW World Championship between Team McMahon ( champion Vince McMahon , Shane McMahon and Umaga ) and Bobby Lashley . Lashley won the match by pinning Shane McMahon ; however , he did not win the title since he d</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Deborah Kerr = Deborah Kerr CBE ( / kɑːr / ; born Deborah Jane Kerr-Trimmer ; 30 September 1921 – 16 October 2007 ) was a Scottish-born film , theatre and television actress . During her career , she won a Golden Globe for her performance as Anna Leonowens in the motion picture The King and I ( 1956 ) and the Sarah Siddons Award for her performance as " Laura Reynolds " in the play Tea and Sympathy ( a role she originated on Broadway ) . She was also a three-time winner of the New York Film Critics Circle Award for Best Actress . Kerr was nominated six times for the Academy Award for Best Actress , more than any other actress without ever winning . In 1994 , however , having already received honorary awards from the Cannes Film Festival and BAFTA , she received an Academy Honorary Award with a citation recognising her as " an artist of impeccable grace and beauty , a dedicated actress whose motion picture career has always stood for perfection , discipline and elegance " . As well as T</t>
+          <t xml:space="preserve">Survivor Series ( 2005 ) = Survivor Series ( 2005 ) was the 19th annual Survivor Series professional wrestling pay-per-view event produced by World Wrestling Entertainment ( WWE ) . It took place on November 27 , 2005 , at the Joe Louis Arena in Detroit , Michigan and consisted of six professional wrestling matches involving wrestlers from the Raw and SmackDown brands . In the first of two main event matches , WWE Champion John Cena defeated Kurt Angle to retain his title . The second main event was an interpromotional 5-on-5 Survivor Series match , in which Team SmackDown ( Batista , Rey Mysterio , John " Bradshaw " Layfield ( JBL ) , Bobby Lashley , and Randy Orton ) defeated Team Raw ( Shawn Michaels , Kane , The Big Show , Carlito , and Chris Masters ) after Orton last eliminated Michaels . In another match , Triple H defeated Ric Flair in a Last Man Standing match . = = Background = = The event 's card consisted of six professional wrestling involving wrestlers from either Raw or </t>
         </is>
       </c>
     </row>
@@ -1036,32 +1036,32 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>['cambridge', 'oxford', 'boat', 'competition', 'silver', 'summer', 'competed', 'referred', 'medal', 'seconds', 'olympics', 'compete', 'athletes', 'champions', 'heat']</t>
+          <t>['watershed', 'creek', 'dam', 'island', 'population', 'city', 'area', 'river', 'volcano', 'volcanic', 'flows', 'lighthouse', 'lava', 'bay', 'water']</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>The Boat Race 1873 = The 30th Boat Race took place on the 29 March 1873 . The Boat Race is an annual side-by-side rowing race between crews from the Universities of Oxford and Cambridge along the River Thames . In a race umpired by former Oxford rower Joseph William Chitty , Cambridge won by three lengths in a time of 19 minutes and 35 seconds , the fastest time in the history of the event . It was the first time that rowers raced on sliding seats . = = Background = = The Boat Race is a side-by-side rowing competition between the University of Oxford ( sometimes referred to as the " Dark Blues " ) and the University of Cambridge ( sometimes referred to as the " Light Blues " ) . The race was first held in 1829 , and since 1845 has taken place on the 4.2-mile ( 6.8 km ) Championship Course on the River Thames in southwest London . Cambridge went into the race as reigning champions , having defeated Oxford by two lengths in the previous year 's race , while Oxford led overall with sixtee</t>
+          <t>Little Catawissa Creek = Little Catawissa Creek is a tributary of Catawissa Creek in Columbia County and Schuylkill County , in Pennsylvania , in the United States . It is approximately 10.8 miles ( 17.4 km ) long and flows through Conyngham Township in Columbia County and Union Township and North Union Township in Schuylkill County . The named tributaries of the creek include Stony Run and Trexler Run . The creek has some alkalinity and is slightly acidic . The main rock formations in the watershed of it are the Mauch Chunk Formation , the Pocono Formation , and the Pottsville Formation . A number of other rock formations occur in small areas of the watershed as well . The main soils in the watershed are the Leck Kill soil and the Hazleton soil . The watershed of Little Catawissa Creek has an area of 16.70 square miles ( 43.3 km2 ) . A number of bridges cross the creek . There are a number of major roads in the watershed of the creek and most of the creek is within several hundred met</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>The Boat Race 1956 = The 102nd Boat Race took place on 24 March 1956 . Held annually , the Boat Race is a side-by-side rowing race between crews from the Universities of Oxford and Cambridge along the River Thames . In a race umpired by former rower Kenneth Payne , Cambridge won by one-and-a-quarter lengths in a time of 18 minutes 36 seconds , the fourth quickest time in the history of the event . The victory took the overall record to 56 – 45 in their favour . = = Background = = The Boat Race is a side-by-side rowing competition between the University of Oxford ( sometimes referred to as the " Dark Blues " ) and the University of Cambridge ( sometimes referred to as the " Light Blues " ) . First held in 1829 , the race takes place on the 4.2-mile ( 6.8 km ) Championship Course on the River Thames in southwest London . The rivalry is a major point of honour between the two universities ; it is followed throughout the United Kingdom and , as of 2014 , broadcast worldwide . Cambridge wen</t>
+          <t xml:space="preserve">Muncy Creek = Muncy Creek ( also known as Big Muncy Creek ) is a tributary of the West Branch Susquehanna River in Sullivan County and Lycoming County , in Pennsylvania , in the United States . It is approximately 34.5 miles ( 55.5 km ) long . The watershed of the creek has an area of 216 square miles ( 560 km2 ) . The creek 's discharge averages 49 cubic feet per second ( 1.4 m3 / s ) at Sonestown , but can be up to a thousand times higher at Muncy . The headwaters of the creek are on the Allegheny Plateau . Rock formations in the watershed include the Chemung Formation and the Catskill Formation . There are a number of lakes in the watershed of Muncy Creek , including Eagles Mere Lake , Highland Lake , and Beaver Lake . The creek was known as Occohpocheny to Native Americans . The area in its vicinity was settled in 1783 . Various other industries and mills were constructed in the creek 's vicinity from the late 18th century to the early 20th century . Wild trout naturally reproduce </t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve">The Boat Race 2006 = The 152nd Boat Race took place on 2 April 2006 . Held annually , the Boat Race is a side-by-side rowing race between crews from the Universities of Oxford and Cambridge along the River Thames . Oxford , whose crew contained the first French rower in the history of the event , won the race by five lengths which was umpired by former Oxford rower Simon Harris . In the reserve race Goldie beat Isis and Oxford won the Women 's Boat Race . = = Background = = The Boat Race is a side-by-side rowing competition between the University of Oxford ( sometimes referred to as the " Dark Blues " ) and the University of Cambridge ( sometimes referred to as the " Light Blues " ) . First held in 1829 , the race takes place on the 4.2-mile ( 6.8 km ) Championship Course on the River Thames in southwest London . The rivalry is a major point of honour between the two universities and followed throughout the United Kingdom and broadcast worldwide . Oxford went into the race as reigning </t>
+          <t xml:space="preserve">West Branch Fishing Creek = West Branch Fishing Creek is one of the northernmost major tributaries of Fishing Creek in Sullivan County , Pennsylvania and Columbia County , Pennsylvania , in the United States . It is 11.1 miles ( 17.9 km ) long and flows through Davidson Township , Sullivan County and Sugarloaf Township , Columbia County . The creek 's watershed has an area of 33.5 square miles , nearly all of which is forested land . Rock formations in the watershed of West Branch Fishing Creek include the Catskill Formation , the Huntley Mountain Formation , and the Burgoon Sandstone . North Mountain , Huckleberry Mountain , and Central Mountain are all in the creek 's vicinity . The temperature of the creek 's waters ranges from − 2 ° C ( 28 ° F ) to 23 ° C ( 73 ° F ) and its pH ranges from approximately 5.5 to just under 7.0 . The creek 's discharge ranges from nearly 0 cubic meters per second to approximately 25 cubic meters per second . Communities in the watershed of West Branch </t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>The Boat Race 1861 = The 18th Boat Race took place on the River Thames on 16 March 1861 . Held annually , The Boat Race is a side-by-side rowing race between crews from the Universities of Oxford and Cambridge . The 1861 event , which featured the first ever non-British competitor , suffered numerous interruptions from river traffic . Oxford won by 16 lengths . = = Background = = The Boat Race is a side-by-side rowing competition between the University of Oxford ( sometimes referred to as the " Dark Blues " ) and the University of Cambridge ( sometimes referred to as the " Light Blues " ) . The race was first held in 1829 , and since 1845 has taken place on the 4.2-mile ( 6.8 km ) Championship Course on the River Thames in southwest London . Cambridge went into the race as reigning champions , having defeated Oxford by one length in the previous year 's race and led overall with ten wins to Oxford 's seven . The challenge to race was sent from Oxford in the October term which was accep</t>
+          <t>Sulphur Creek ( California ) = Sulphur Creek is a 4.5-mile ( 7.2 km ) tributary of Aliso Creek in Orange County in the U.S. state of California . Draining about 6 square miles ( 16 km2 ) of mostly residential land in the southern San Joaquin Hills , it is Aliso Creek 's largest tributary . Geologically the Sulphur Creek watershed was once part of a large and shallow sea that covered most of southern California . As the San Joaquin Hills rose and river sediments were deposited , land gradually emerged to form the present-day Orange County coast . Sulphur Creek is located in a crumpled , hilly area in the southern part of this range , formed differently from the continuous mountain chain to the north . Historically , being south of Aliso Creek , the Sulphur Creek watershed was part of the territory of the semi-nomadic Acjachemen Indian group , conquered by Spanish conquistadors in the 17th and 18th centuries and renamed the Juaneño by them . During the 19th century , the watershed became</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>The Boat Race 1937 = The 89th Boat Race took place on 24 March 1937 . Held annually , the Boat Race is a side-by-side rowing race between crews from the Universities of Oxford and Cambridge along the River Thames . In a race umpired by the former Cambridge rower and coach Harold Rickett , Oxford won by three lengths in a time of 22 minutes 39 seconds . It was their first success since the 1923 race and ended Cambridge 's record streak of 13 wins . The victory took the overall record in the event to 47 – 41 in Cambridge 's favour . = = Background = = The Boat Race is a side-by-side rowing competition between the University of Oxford ( sometimes referred to as the " Dark Blues " ) and the University of Cambridge ( sometimes referred to as the " Light Blues " ) . The race was first held in 1829 , and since 1845 has taken place on the 4.2-mile ( 6.8 km ) Championship Course on the River Thames in southwest London . The rivalry is a major point of honour between the two universities ; it is</t>
+          <t>Shickshinny Creek = Shickshinny Creek ( historically known as Shickohinna ) is a tributary of the Susquehanna River in the Wyoming Valley in Luzerne County , Pennsylvania , in the United States . It is approximately 10.1 miles ( 16.3 km ) long and flows through Ross Township , Union Township , and Shickshinny . Its watershed has an area of 35.0 square miles ( 91 km2 ) and its tributaries include Culver Creek , Reyburn Creek , and Little Shickshinny Creek . The creek is designated as a Coldwater Fishery and a Migratory Fishery . A sawmill and a gristmill were built on the creek in 1802 and 1804 , respectively . Several bridges have also been constructed over it . The creek was historically polluted by culm near its mouth , but agriculture was the main industry in the watershed in the early 1900s . It was historically used as a water supply . The surficial geology near Shickshinny Creek mainly consists of urban land , fill , alluvium , alluvial terrace , alluvial fan , Wisconsinan Ice-Co</t>
         </is>
       </c>
     </row>
@@ -1071,32 +1071,32 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>['album', 'music', 'songs', 'rock', 'recorded', 'recording', 'band', 'beatles', 'lyrics', 'musicians', 'george_harrison', 'sound', 'harrison', 'song', 'bands']</t>
+          <t>['liz', 'dwight', 'jim', 'pam', 'michael', 'episode', 'nbc', 'jack', 'fey', 'jenna', 'andy', 'office', 'tracy', 'kenneth', 'tgs']</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Alternative rock = Alternative rock ( also called alternative music , alt-rock or simply alternative ) is a genre of rock music that emerged from the independent music underground of the 1980s and became widely popular in the 1990s and 2000s . In this instance , the word " alternative " refers to the genre 's distinction from mainstream rock music . The term 's original meaning was broader , referring to a generation of musicians unified by their collective debt to either the musical style or simply the independent , D.I.Y. ethos of punk rock , which in the late 1970s laid the groundwork for alternative music . At times , " alternative " has been used as a catch-all description for music from underground rock artists that receives mainstream recognition , or for any music , whether rock or not , that is seen to be descended from punk rock ( including some examples of punk itself , as well as new wave , and post-punk ) . Alternative rock is a broad umbrella term consisting of music that</t>
+          <t>Tracy Does Conan = " Tracy Does Conan " is the seventh episode of NBC 's first season of 30 Rock . It was written by the series ' creator and executive producer , Tina Fey and it was directed by one of the season 's supervising producers , Adam Bernstein . It first aired on December 7 , 2006 in the United States and November 29 , 2007 in the United Kingdom . Guest stars in the episode included Katrina Bowden , Kevin Brown , Grizz Chapman , Rachel Dratch , Dave Finkel , Steve Hollander , Johnnie May , Maulik Pancholy , Chris Parnell , Aubrey Plaza , Keith Powell , R. N. Rao and Dean Winters . Conan O 'Brien appeared as himself in this episode . The episode marks the first appearance of Chris Parnell as recurring character , Dr. Leo Spaceman . This episode revolves around Liz Lemon ( played by Tina Fey ) and Pete Hornberger ( Scott Adsit ) trying to get Tracy Jordan ( Tracy Morgan ) to make a successful appearance on Late Night with Conan O 'Brien , a late night talk show . These attempt</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t xml:space="preserve">This Guitar ( Can 't Keep from Crying ) = " This Guitar ( Can 't Keep from Crying ) " is a song by English musician George Harrison , released on his 1975 studio album Extra Texture ( Read All About It ) . Harrison wrote the song as a sequel to his popular Beatles composition " While My Guitar Gently Weeps " , in response to the personal criticism he had received during and after his 1974 North American tour with Ravi Shankar , particularly from Rolling Stone magazine . " This Guitar " was issued as a single in December 1975 – the final release for Apple Records in its original incarnation – but it failed to chart in either the United States or Britain . The song follows in a tradition established by singers such as Woody Guthrie and Pete Seeger , of attributing emotions and actions to a musical instrument . The lyrics also serve as an example of a dialogue that was commonplace during the 1970s between songwriters and music critics . Contributing to Harrison 's sense of injustice in " </t>
+          <t>Sandwich Day = " Sandwich Day " is the fourteenth episode of the second season of 30 Rock and the thirty-fifth episode overall . It was written by one of the season 's executive producers , Robert Carlock , and one of the season 's co-executive producers , Jack Burditt . The episode was directed by one of the season 's producers , Don Scardino . The episode first aired on May 1 , 2008 on the NBC network in the United States . Guest stars in this episode included Bill Cwikowski , Brian Dennehy , Marceline Hugot , Johnnie May , Jason Sudeikis , Miriam Tolan and Rip Torn . The episode earned Tina Fey the Primetime Emmy Award for Outstanding Lead Actress in a Comedy Series . Unusually this episode begins on the 30 Rock title sequence - there is no cold open as is normally the case . This episode begins on the annual TGS with Tracy Jordan ( a fictional sketch comedy series ) Sandwich Day . Liz Lemon ( Tina Fey ) receives a phone call from her ex-boyfriend , Floyd ( Jason Sudeikis ) , asking</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ding Dong , Ding Dong = " Ding Dong , Ding Dong " is a song by English musician George Harrison , written as a New Year 's Eve singalong and released in December 1974 on his album Dark Horse . It was the album 's lead single in Britain and some other European countries , and the second single , after " Dark Horse " , in North America . A large-scale production , the song incorporates aspects of Phil Spector 's Wall of Sound technique , particularly his Christmas recordings from 1963 . In addition , some Harrison biographers view " Ding Dong " as an attempt to emulate the success of two glam rock anthems from the 1973 – 74 holiday season : " Merry Xmas Everybody " by Slade , and Wizzard 's " I Wish It Could Be Christmas Everyday " . The song became only a minor hit in Britain and the United States , although it was a top-twenty hit elsewhere in the world . Harrison took the lyrics to " Ding Dong " from engravings he found at his nineteenth-century home , Friar Park , in Oxfordshire – a </t>
+          <t>A Benihana Christmas = " A Benihana Christmas " is the tenth and eleventh episode of the third season of the American comedy television series The Office , and the thirty-eighth and thirty-ninth episode overall . It was written by Jennifer Celotta and directed by Harold Ramis . The episode originally aired in the United States on December 14 , 2006 , on NBC . In the episode , Christmas time at the office leads to depression for Michael , when his girlfriend Carol ( Steve Carell 's wife , Nancy Walls ) breaks up with him . Michael , Andy , Dwight , and Jim then go to a local Benihana restaurant , where Michael and Andy find dates with two of the restaurant 's waitresses . Back at the office , after a conflict with a bossy Angela , Karen and Pam decide to create their own Christmas party . When the majority of the office decide to go to Karen and Pam 's party , Angela becomes upset , and seeing this , Karen and Pam decide to combine the parties . Soon after , Michael and Andy 's dates le</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t xml:space="preserve">You ( George Harrison song ) = " You " is a song by English musician George Harrison , released as the opening track of his 1975 album Extra Texture ( Read All About It ) . It was also the album 's lead single , becoming a top 20 hit in America and reaching number 9 in Canada . A 45-second instrumental portion of the song , titled " A Bit More of You " , appears on Extra Texture also , opening side two of the original LP format . Harrison wrote " You " in 1970 as a song for Ronnie Spector , formerly of the Ronettes , and wife of Harrison 's All Things Must Pass co-producer Phil Spector . The composition reflects Harrison 's admiration for 1960s American soul / R &amp; B , particularly Motown . In February 1971 , Ronnie Spector recorded " You " in London for a proposed solo album on the Beatles ' Apple record label , but the recording remained unissued . Four years later , Harrison returned to this backing track while making his final album for Apple Records , in Los Angeles . The released </t>
+          <t>Ben Franklin ( The Office ) = " Ben Franklin " is the fifteenth episode of the third season of the American comedy television series The Office , and the show 's forty-third episode overall . Written by Mindy Kaling , who also acts in the show as Kelly Kapoor , and directed by Randall Einhorn , the episode first aired in the United States on February 1 , 2007 on NBC . " Ben Franklin " received 5.0 / 13 in the ages 18 – 49 demographic of the Nielsen ratings , and was watched by an estimated audience of 10.1 million viewers , and the episode received mixed reviews among critics . In the episode , the employees from the office prepare for Phyllis 's wedding . Michael , acting under advice from Todd , instructs Dwight to hire a stripper for the men and delegates Jim to hire one for the women . While Dwight hires a stripper , Jim ends up hiring a Ben Franklin impersonator instead . = = Plot = = The office plays host to a bridal shower for Phyllis Lapin ( Phyllis Smith ) while Bob Vance 's (</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Ballad of Sir Frankie Crisp ( Let It Roll ) = " Ballad of Sir Frankie Crisp ( Let It Roll ) " is a song by English musician George Harrison , released on his 1970 triple album All Things Must Pass . Harrison wrote the song as a tribute to Frank Crisp , a nineteenth-century lawyer and the original owner of Friar Park – the Victorian Gothic residence in Henley-on-Thames , Oxfordshire , that Harrison purchased in early 1970 . Commentators have likened the song to a cinematic journey through the grand house and the grounds of the estate . The recording features backing from musicians such as Pete Drake , Billy Preston , Gary Wright , Klaus Voormann and Alan White . It was co-produced by Phil Spector , whose heavy use of reverb adds to the ethereal quality of the song . AllMusic critic Scott Janovitz describes " Ballad of Sir Frankie Crisp ( Let It Roll ) " as offering " a glimpse of the true George Harrison – at once mystical , humorous , solitary , playful , and serious " . Crisp 's eccen</t>
+          <t>The Aftermath ( 30 Rock ) = " The Aftermath " is the second episode of the first season of the American situation comedy 30 Rock , which first aired on October 17 , 2006 on CTV in Canada . It aired on October 18 , 2006 on the NBC network in the United States , its country of origin , and October 18 , 2007 in the United Kingdom . The episode was written by Tina Fey and was directed by Adam Bernstein . Guest stars in this episode include Katrina Bowden , Tom Broecker , Teddy Coluca , Rachel Dratch , Adrienne Frost , Maulik Pancholy , Keith Powell , Lonny Ross , Kevin Scanlon and Sorab Wadia . The episode focuses on the reaction of the crew to the casting of Tracy Jordan ( Tracy Morgan ) , and the subsequent changes made to The Girlie Show . This becomes evident when Jack Donaghy ( Alec Baldwin ) changes the title of the show to TGS with Tracy Jordan , much to Jenna Maroney 's ( Jane Krakowski ) dismay . Liz Lemon ( Tina Fey ) struggles to keep the cast and crew happy , so together with T</t>
         </is>
       </c>
     </row>
@@ -1106,32 +1106,32 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>['song', 'video', 'number', 'like', 'performance', 'tour', 'music', 'madonna', 'performed', 'best', 'songs', 'stage', 'beyoncé', 'week', 'gaga']</t>
+          <t>['oxford', 'cambridge', 'race', 'boat', 'blues', 'rowed', 'rowing', 'lengths', 'crews', 'rower', 'thames', 'races', 'crew', 'universities', 'university_of_cambridge']</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Sticky &amp; Sweet Tour = Sticky &amp; Sweet Tour was the eighth concert tour by American singer Madonna to promote her eleventh studio album , Hard Candy . It began in August 2008 and was Madonna 's first tour from her new recording and business deal with Live Nation . The tour was announced in February 2008 , with dates for European and North American venues revealed . Though initially planned , the tour did not visit Australia due to financial problems and the financial recession . Costume designer Arianne Phillips designed the costumes , supported by a number of famous designers and brands . The stage for the main show was planned similarly to that of her previous 2006 Confessions Tour . After the tour concluded in 2008 , Madonna announced plans of playing a second European leg in 2009 to play in territories she either had never been to or had not played for a long time . The tour was described as a " rock driven dancetastic journey " . It was divided into four acts : Pimp , where S &amp; M wa</t>
+          <t>The Boat Race 1873 = The 30th Boat Race took place on the 29 March 1873 . The Boat Race is an annual side-by-side rowing race between crews from the Universities of Oxford and Cambridge along the River Thames . In a race umpired by former Oxford rower Joseph William Chitty , Cambridge won by three lengths in a time of 19 minutes and 35 seconds , the fastest time in the history of the event . It was the first time that rowers raced on sliding seats . = = Background = = The Boat Race is a side-by-side rowing competition between the University of Oxford ( sometimes referred to as the " Dark Blues " ) and the University of Cambridge ( sometimes referred to as the " Light Blues " ) . The race was first held in 1829 , and since 1845 has taken place on the 4.2-mile ( 6.8 km ) Championship Course on the River Thames in southwest London . Cambridge went into the race as reigning champions , having defeated Oxford by two lengths in the previous year 's race , while Oxford led overall with sixtee</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Till the World Ends = " Till the World Ends " is a song recorded by American singer Britney Spears for her seventh studio album , Femme Fatale ( 2011 ) . It was written by Kesha Sebert , Lukasz " Dr. Luke " Gottwald , Alexander Kronlund , and Max Martin . Gottwald , Martin and Billboard produced the song , while vocal production was handled by Emily Wright . " Till the World Ends " is an uptempo dance-pop and electropop song with an electro beat . It opens with sirens , and has elements of trance and Eurodance . The song features a chant-like chorus , and lyrics in which Spears sings about dancing until the end of the world . " Till the World Ends " received comparisons to past hits by artists like Kesha and Enrique Iglesias . Some music critics deemed it a catchy dance track and complimenting its anthemic nature . " Till the World Ends " was treated with different remixes , most notably the Femme Fatale Remix , featuring rapper Nicki Minaj and Kesha , which was released on April 25 , </t>
+          <t xml:space="preserve">The Boat Race 1879 = The 36th Boat Race took place on 5 April 1879 . The Boat Race is an annual side-by-side rowing race between crews from the Universities of Oxford and Cambridge along the River Thames . Each crew contained four Blues . In a race umpired by former Oxford rower Joseph William Chitty , Cambridge led all the way , and won by a margin of three lengths in a time of 21 minutes 18 seconds . The victory took the overall record to 18 – 17 in Oxford 's favour . = = Background = = The Boat Race is a side-by-side rowing competition between the University of Oxford ( sometimes referred to as the " Dark Blues " ) and the University of Cambridge ( sometimes referred to as the " Light Blues " ) . The race was first held in 1829 , and since 1845 has taken place on the 4.2-mile ( 6.8 km ) Championship Course on the River Thames in southwest London . Cambridge went into the race as reigning champions having won the previous year 's race by ten lengths . However Oxford held the overall </t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Drowned World Tour = Drowned World Tour was the fifth concert tour by American singer-songwriter Madonna in support of her seventh and eighth studio albums Ray of Light and Music . It was also her first tour in eight years , following The Girlie Show World Tour in 1993 . The tour was supposed to start in 1999 , but was delayed until 2001 as Madonna gave birth to her son , got married to Guy Ritchie , was working on Music , and was busy filming The Next Best Thing . When the tour was decided , Madonna appointed Jamie King as choreographer and the tour was planned in a short timespan of three months , including signing up the dancers , musicians and technicians . Designer Jean-Paul Gaultier was the costume designer who designed the costumes in such way that they indicated different phases of Madonna 's career . The poster and logo for the tour included references to Kabbalah , which Madonna studied . The show was divided into five segments , namely Cyber-Punk , Geisha , Cowgirl , Spanish</t>
+          <t>The Boat Race 1882 = The 39th Boat Race took place on 1 April 1882 . The Boat Race is an annual side-by-side rowing race between crews from the Universities of Oxford and Cambridge along the River Thames . In the race , umpired by former Cambridge rower Robert Lewis-Lloyd , Oxford won by a margin of seven lengths in a time of 20 minutes 12 seconds , taking the overall record to 21 – 17 in their favour . = = Background = = The Boat Race is an annual rowing eight competition between the University of Oxford and the University of Cambridge . First held in 1829 , the competition is a 4.2-mile ( 6.8 km ) race along The Championship Course on the River Thames in southwest London . The rivalry is a major point of honour between the two universities and followed throughout the United Kingdom and worldwide . Oxford went into the race as reigning champions having won the previous year 's race by three lengths , and held the overall lead , with 20 victories to Cambridge 's 17 ( excluding the " de</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Born This Way ( song ) = " Born This Way " is a song by American singer Lady Gaga , and the lead single from her second studio album of the same name . Written by Gaga and Jeppe Laursen , who produced along with Fernando Garibay and DJ White Shadow , it was developed while Gaga was on the road with The Monster Ball Tour . Inspired by the 1990s empowering music for women and the gay community , Gaga explained that " Born This Way " was her freedom song . She sang part of the chorus at the 2010 MTV Video Music Awards in 2010 and announced the song as the lead single from the album . The single was released on February 11 , 2011 . The song is backed by rumbling synth sounds , a humming bass and additional chorus percussion , with sole organ toward the end . The lyrics discuss the self-empowerment of minorities including the LGBT community as well as racial minorities , referring to " cholas " and " orients " , which drew criticism from Latino and Asian communities . Critics positively rev</t>
+          <t xml:space="preserve">The Boat Race 1889 = The 46th Boat Race took place on 30 March 1889 . The Boat Race is an annual side-by-side rowing race between crews from the Universities of Oxford and Cambridge along the River Thames . For the first time in the history of the event , all eight rowers in the Cambridge crew had rowed the previous year . Cambridge won by three lengths in a time of 20 minutes 14 seconds , their fourth consecutive victory which took the overall record in the event to 23 – 22 in Oxford 's favour . = = Background = = The Boat Race is a side-by-side rowing competition between the University of Oxford ( sometimes referred to as the " Dark Blues " ) and the University of Cambridge ( sometimes referred to as the " Light Blues " ) . First held in 1829 , the race takes place on the 4.2 miles ( 6.8 km ) Championship Course on the River Thames in southwest London . The rivalry is a major point of honour between the two universities ; it is followed throughout the United Kingdom and as of 2014 , </t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Secret ( Madonna song ) = " Secret " is a song recorded by American singer and songwriter Madonna from her sixth studio album Bedtime Stories ( 1994 ) . It was released on September 27 , 1994 , as the lead single from the album by Warner Bros. Records as well as Maverick and Sire . The song was later included on her greatest hits compilations GHV2 ( 2001 ) and Celebration ( 2009 ) . " Secret " was developed based on a demo version created by producer Shep Pettibone , which was reworked by Dallas Austin , with whom Madonna was working on Bedtime Stories . Written and produced by the singer with Austin , an additional writer on the track was Pettibone . The song was a departure from the style of music that Madonna had previously released ; up to that point in her career her music had mostly been big-sounding dance tracks or melodic ballads . " Secret " combined pop and R &amp; B genres with instrumentation from acoustic guitar , drums and strings , while lyrically talking about a lover havin</t>
+          <t>The Boat Race 1872 = The 29th Boat Race took place on the 27 March 1872 . The Boat Race is an annual side-by-side rowing race between crews from the Universities of Oxford and Cambridge along the River Thames . In a race umpired by Robert Lewis-Lloyd , Cambridge won by two lengths in a time of 21 minutes 15 seconds taking the overall record to 16 – 13 in Oxford 's favour . = = Background = = The Boat Race is a side-by-side rowing competition between the University of Oxford ( sometimes referred to as the " Dark Blues " ) and the University of Cambridge ( sometimes referred to as the " Light Blues " ) . The race was first held in 1829 , and since 1845 has taken place on the 4.2-mile ( 6.8 km ) Championship Course on the River Thames in southwest London . Cambridge went into the race as reigning champions , having defeated Oxford by one length in the previous year 's race , while Oxford led overall with sixteen wins to Cambridge 's twelve . During the build-up to the race , Oxford 's boa</t>
         </is>
       </c>
     </row>
@@ -1141,32 +1141,32 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>['class', 'built', 'main', 'guns', 'line', 'castle', 'new', 'service', 'use', 'long', 'locomotives', 'london', 'speed', 'intended', 'locomotive']</t>
+          <t>['women', 'party', 'police', 'labour', 'book', 'rights', 'suffrage', 'government', 'feminist', 'political', 'feminism', 'murder', 'case', 'minister', 'trial']</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Motte-and-bailey castle = A motte-and-bailey castle is a fortification with a wooden or stone keep situated on a raised earthwork called a motte , accompanied by an enclosed courtyard , or bailey , surrounded by a protective ditch and palisade . Relatively easy to build with unskilled , often forced , labour , but still militarily formidable , these castles were built across northern Europe from the 10th century onwards , spreading from Normandy and Anjou in France , into the Holy Roman Empire in the 11th century . The Normans introduced the design into England and Wales following their invasion in 1066 . Motte-and-bailey castles were adopted in Scotland , Ireland , the Low Countries and Denmark in the 12th and 13th centuries . By the end of the 13th century , the design was largely superseded by alternative forms of fortification , but the earthworks remain a prominent feature in many countries . = = Architecture = = = = = Structures = = = A motte-and-bailey castle was made up of two </t>
+          <t xml:space="preserve">Free Expression Policy Project = The Free Expression Policy Project ( FEPP ) is an organization devoted to assisting researchers with assembling information related to freedom of speech , media democracy , and copyright , and advocating for these issues . Civil liberties lawyer Marjorie Heins founded the nonprofit organization in 2000 . Based in Manhattan , New York , it was initially associated with the National Coalition Against Censorship , and subsequently operated as part of the Democracy Program of the Brennan Center for Justice at New York University Law School . The FEPP conducted a survey in 2001 which revealed that online monitoring software , including Net Nanny , SurfWatch , and Cybersitter , cast too broad a net and often blocked legitimate educational websites in their attempts to censor material from youths . In 2003 , the organization assisted 33 academics in filing a friend-of-the-court brief challenging a law which restricted the sale of violent video games to minors </t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Heinkel He 111 = The Heinkel He 111 was a German aircraft designed by Siegfried and Walter Günter at Heinkel Flugzeugwerke in 1934 . Through development it was described as a " wolf in sheep 's clothing " because the project masqueraded the machine as civilian transport , though from conception the Heinkel was intended to provide the nascent Luftwaffe with a fast medium bomber . Perhaps the best-recognised German bomber due to the distinctive , extensively glazed " greenhouse " nose of later versions , the Heinkel He 111 was the most numerous Luftwaffe bomber during the early stages of World War II . The bomber fared well until the Battle of Britain , when its weak defensive armament was exposed . Nevertheless , it proved capable of sustaining heavy damage and remaining airborne . As the war progressed , the He 111 was used in a variety of roles on every front in the European theatre . It was used as a strategic bomber during the Battle of Britain , a torpedo bomber in the Atlantic and</t>
+          <t>Weiquan movement = The Weiquan movement is a non-centralized group of lawyers , legal experts , and intellectuals in China who seek to protect and defend the civil rights of the citizenry through litigation and legal activism . The movement , which began in the early 2000s , has organized demonstrations , sought reform via the legal system and media , defended victims of human rights abuses , and written appeal letters , despite opposition from Communist Party authorities . Among the issues adopted by Weiquan lawyers are property and housing rights , protection for AIDS victims , environmental damage , religious freedom , freedom of speech and the press , and defending the rights of other lawyers facing disbarment or imprisonment . Individuals involved in the Weiquan movement have met with occasionally harsh reprisals from Chinese officials , including disbarment , detention , harassment , and , in extreme instances , torture . Authorities have also responded to the movement with the l</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>York Castle = York Castle in the city of York , England , is a fortified complex comprising , over the last nine centuries , a sequence of castles , prisons , law courts and other buildings on the south side of the River Foss . The now-ruinous keep of the medieval Norman castle is commonly referred to as Clifford 's Tower . Built originally on the orders of William I to dominate the former Viking city of York , the castle suffered a tumultuous early history before developing into a major fortification with extensive water defences . After a major explosion in 1684 rendered the remaining military defences uninhabitable , York Castle continued to be used as a jail and prison until 1929 . The first motte and bailey castle on the site was built in 1068 following the Norman conquest of York . After the destruction of the castle by rebels and a Viking army in 1069 , York Castle was rebuilt and reinforced with extensive water defences , including a moat and an artificial lake . York Castle fo</t>
+          <t>Azimzhan Askarov = Azimzhan Askarov ( Uzbek : Azimjon Asqarov , Азимжон Асқаров ; born 1951 ) is an ethnically Uzbek Kyrgyzstani political activist who founded the group Vozduh in 2002 to investigate police brutality . During the 2010 South Kyrgyzstan ethnic clashes , which primarily targeted people of the Uzbek nationality , Askarov worked to document the violence . He was subsequently arrested and prosecuted on charges of creating mass disturbances , incitement of ethnic hatred , and complicity in murder . Following a trial protested by several international human rights groups for irregularities — including alleged torture and the courtroom intimidation of witnesses by police — Askarov was given a life sentence , which he is currently serving . In November 2010 , Askarov 's health was reported to be rapidly deteriorating as a result of his confinement . Numerous groups have advocated on his behalf , including Human Rights Watch , Reporters Without Borders , People In Need , the Comm</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>SR V Schools class = The SR V class , more commonly known as the Schools class , is a class of steam locomotive designed by Richard Maunsell for the Southern Railway . The class was a cut down version of his Lord Nelson class but also incorporated components from Urie and Maunsell 's LSWR / SR King Arthur class . It was the last locomotive in Britain to be designed with a 4-4-0 wheel arrangement , and was the most powerful class of 4-4-0 ever produced in Europe . All 40 of the class were named after English public schools , and were designed to provide a powerful class of intermediate express passenger locomotive on semi-fast services for lines which could cope with high axle loads but some of which had short turntables . Because of the use of a ‘ ’ King Arthur ’ ’ firebox , rather than the square-topped Belpaire firebox used on the Lord Nelsons , the class could be used on lines with a restricted loading gauge and some of the best performance by the class was on the heavily restricted</t>
+          <t>New Labour = New Labour refers to a period in the history of the British Labour Party from the mid-1990s to the early 2010s , under leaders Tony Blair and Gordon Brown . The name dates from a conference slogan first used by the party in 1994 which was later seen in a draft manifesto published in 1996 , called New Labour , New Life For Britain . It was presented as the brand of a newly reformed party that had altered Clause IV and endorsed market economics . The branding was extensively used while the party was in government , between 1997 and 2010 . New Labour won landslide election victories in 1997 and 2001 , and won again in 2005 . In 2007 , Blair resigned as the party 's leader and was succeeded by Gordon Brown . Labour lost the 2010 general election , which resulted in a hung parliament and led to the creation of a Conservative – Liberal Democrat coalition government ; Gordon Brown resigned as Prime Minister , and as Labour leader shortly thereafter . He was succeeded by Ed Miliba</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Lion-class battleship = The Lion-class battleships were a class of six fast battleships designed for the Royal Navy in the late 1930s . They were a larger , improved version of the King George V class with 16-inch ( 406 mm ) guns . Only two ships were laid down before World War II began in September 1939 and a third was ordered during the war , but their construction was suspended shortly afterwards . Their design changed several times in response to the removal of treaty restrictions on size and in light of war experience . None of the other ships planned were laid down , although there was a proposal to modify one of the suspended ships into a hybrid battleship / aircraft carrier with two 16-inch gun turrets and a flight deck . The two ships already begun were scrapped after the end of the war . = = Design and description = = The choice of 14-inch ( 356 mm ) gun and the mix of quadruple and twin turrets for the main battery of the King George Vs had been dictated by the Second London</t>
+          <t xml:space="preserve">Feminism in India = Feminism in India is a set of movements aimed at defining , establishing , and defending equal political , economic , and social rights and equal opportunities for Indian women . It is the pursuit of women 's rights within the society of India . Like their feminist counterparts all over the world , feminists in India seek gender equality : the right to work for equal wages , the right to equal access to health and education , and equal political rights . Indian feminists also have fought against culture-specific issues within India 's patriarchal society , such as inheritance laws and the practice of widow immolation known as Sati . The history of feminism in India can be divided into three phases : the first phase , beginning in the mid-nineteenth century , initiated when male European colonists began to speak out against the social evils of Sati ; the second phase , from 1915 to Indian independence , when Gandhi incorporated women 's movements into the Quit India </t>
         </is>
       </c>
     </row>
@@ -1176,32 +1176,32 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>['cap', 'fruit', 'color', 'shaped', 'spores', 'bodies', 'fungus', 'stem', 'mushroom', 'spore', 'taxonomy', 'yellow', 'diameter', 'collected', 'gill']</t>
+          <t>['officer', 'commander', 'lieutenant', 'command', 'fighter', 'promoted', 'victories', 'war', 'aircraft', 'flying', 'squadron', 'enemy', 'rank', 'medal', 'training']</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Amanita gemmata = Amanita gemmata , commonly known as the gemmed Amanita or the jonquil Amanita , is an agaric mushroom of the family Amanitaceae and genus Amanita . The fruit body has a cap that is a dull to golden shade of yellow , and typically 2.5 – 12 cm ( 1.0 – 4.7 in ) in diameter . The cap surface is sticky when moist , and characterized by white warts , which are easily detached . It is initially convex , and flattens out when mature . The flesh is white and does not change colour when cut . Gills are white and closely spaced . The stem is pale yellow , and measures 4 – 12 cm ( 1.6 – 4.7 in ) long by 0.5 – 1.9 cm ( 0.2 – 0.7 in ) thick . The partial veil that covers the young fruit body turns into the ring on the stem at maturity . The spore print is white , while the spores are roughly elliptical , and measure 8 – 10 by 6.5 – 7.5 µm . This species is a mycorrhizal fungus , widespread in the Americas and Europe . It can grow either singly , scattered , or in groups . It prefer</t>
+          <t>Neville McNamara = Air Chief Marshal Sir Neville Patrick McNamara , KBE , AO , AFC , AE ( 17 April 1923 – 7 May 2014 ) was a senior commander of the Royal Australian Air Force ( RAAF ) . He served as Chief of the Air Staff ( CAS ) , the RAAF 's highest-ranking position , from 1979 until 1982 , and as Chief of the Defence Force Staff ( CDFS ) , Australia 's top military role at the time , from 1982 until 1984 . He was the second RAAF officer to hold the rank of air chief marshal . Born in Queensland , McNamara joined the RAAF during World War II and saw action in the South West Pacific , flying P-40 Kittyhawks . He also flew combat missions in Gloster Meteors during the Korean War . In 1961 , he was awarded the Air Force Cross for his leadership of No. 2 Operational Conversion Unit . He gained further operational experience heading the RAAF presence in Ubon , Thailand , in the late 1960s . Promoted to air commodore , McNamara was Commander RAAF Forces Vietnam , and Deputy Commander Aust</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Boletus subluridellus = Boletus subluridellus is a species of bolete fungus in the family Boletaceae . Described as new to science in 1971 by American mycologists , the bolete is found in the eastern United States and Canada . It grows on the ground in coniferous and mixed forests in a mycorrhizal association with deciduous trees , especially oak . The fruit bodies ( mushrooms ) have orangish-red , broadly convex caps that are up to 10 cm ( 3.9 in ) in diameter , with small , dark reddish pores on the underside . The pale yellow stipe measures 4 – 9 cm ( 1.6 – 3.5 in ) long by 1.5 – 2.3 cm ( 0.6 – 0.9 in ) thick . All parts of the fruit body will quickly stain blue when injured or touched . = = Taxonomy = = The species was described by American mycologists Alexander H. Smith and Harry D. Thiers in their 1971 monograph on the bolete fungi of Michigan . The type collection was made by Smith on a golf course near Ypsilanti , Michigan in September 1961 ; it is kept at the University of Mic</t>
+          <t>Richard Barrons = General Sir Richard Lawson Barrons KCB , CBE , ADC Gen ( born 17 May 1959 ) is a retired British Army officer . He was Commander Joint Forces Command from April 2013 until his retirement in April 2016 . Barrons ' early career was spent in various staff and field posts in the UK , across Europe , and in the Far East . He also spent time working at the Ministry of Defence and in education . Sent to Germany in 1991 , Barrons then served his first tour of duty in the Balkans in 1993 . Returning to the UK , Barrons took up a staff position and went on to do a tour in Northern Ireland and then to become a Military Assistant , first to the High Representative for Bosnia and Herzegovina and then to the Chief of the General Staff . Between 2000 and 2003 , Barrons served again in the Balkans , in Afghanistan during the early days of International Security Assistance Force , and then in a staff position in Basra , Iraq . As a brigadier in 2003 , Barrons served his second tour in</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hydnellum ferrugineum = Hydnellum ferrugineum , commonly known as the mealy tooth or the reddish-brown corky spine fungus , is a species of tooth fungus in the family Bankeraceae . A widely distributed species , it is found in north Africa , Asia , Europe , and North America . The fungus fruits on the ground singly or in clusters in conifer forest , usually in poor ( low nutrient ) or sandy soil . Fruit bodies are somewhat top-shaped , measuring 3 – 10 cm ( 1 – 4 in ) in diameter . Their velvety surfaces , initially white to pink , sometimes exude drops of red liquid . The lower surface of the fruit body features white to reddish-brown spines up to 6 mm long . Mature fruit bodies become dark reddish brown in color , and are then difficult to distinguish from other similar Hydnellum species . H. ferrugineum forms a mat of mycelia in the humus and upper soil where it grows . The presence of the fungus changes the characteristics of the soil , making it more podzolized . = = Taxonomy = = </t>
+          <t>John Emilius Fauquier = Air Commodore John Emilius " Johnny " Fauquier DSO &amp; Two Bars , DFC ( March 19 , 1909 – April 3 , 1981 ) was a Canadian aviator and Second World War Bomber Command leader . He commanded No. 405 Squadron RCAF and later No. 617 Squadron RAF ( the Dambusters ) over the course of the war . A bush pilot , prior to the war , he joined the Royal Canadian Air Force as a flight instructor in 1939 . He then joined 405 Squadron in 1941 and would fly operationally for the rest of the war , taking a drop in rank on one occasion to return to active command . During his three tours of operation he participated in Operation Hydra and dozens of other sorties over Europe . = = Early years = = John Emilius " Johnny " Fauquier was born at Ottawa , Ontario on March 19 , 1909 , educated at Ashbury College and then entered the investment business at Montreal , Quebec where he joined a flying club . After earning his commercial pilot 's licence he formed Commercial Airways at Noranda ,</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Phallus ravenelii = Phallus ravenelii , commonly known as Ravenel 's stinkhorn , is a fungus found in eastern North America . Its mushrooms commonly grow in large clusters and are noted for their foul odor and phallic shape when mature . It is saprobic , and as such it is encountered in a wide variety of habitats rich in wood debris , from forests to mulched gardens or sawdust piles in urban areas . It appears from August to October . The fruit body emerges from a pink or lavender-colored egg to form a tall , cylindrical , hollow and spongy white stalk with a bell-shaped cap . The remains of the egg persist as a white to pink or lilac volva at the base of the stalk . The cap is covered in a foul-smelling olive-green spore slime , which attracts insects that help to spread the spores . Sometimes , the cap has a " veil " attached — a thin membrane that hangs underneath . The lack of a roughly ridged and pitted cap differentiates it from the closely related Phallus impudicus . The fungus </t>
+          <t>Jean-Marie Defrance = Jean-Marie Defrance ( 1771 – 1855 ) was a French General of the French Revolutionary Wars and the Napoleonic Wars . He was also a member of the Council of Five Hundred ( the lower house of the legislative branch of the French government under The Directory ) , and a teacher at the military school of Rebais , Champagne . Defrance had an extensive and successful military career in the French Revolutionary Wars and the Napoleonic Wars . After the First Battle of Zurich , he refused a battlefield promotion to brigadier general , asking instead for a cavalry regiment ; he received command of the 12th Regiment of Chasseurs-a-Cheval ( light cavalry ) as Chef-de-Brigade , a rank equivalent to colonel . He led this brigade in the campaigns of 1799 – 1800 in southwestern Germany and northern Italy . By 1805 , he had been promoted to brigadier general . At the Battle of Austerlitz and the Battle of Jena-Auerstadt , he commanded a cavalry brigade of carabiniers in Étienne Mar</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Bisporella citrina = Bisporella citrina , commonly known as yellow fairy cups or lemon discos , is a species of fungus in the family Helotiaceae . The fungus produces tiny yellow cups up to 3 mm ( 0.12 in ) in diameter , often without stalks , that fruit in groups or dense clusters on decaying deciduous wood that has lost its bark . The widely distributed species is found in North Africa , Asia , Europe , North America , and Central and South America . Found in late summer and autumn , the fungus is fairly common , but is easily overlooked owing to its small size . There are several similar species that can in most cases be distinguished by differences in color , morphology , or substrate . Microscopically , B. citrina can be distinguished from these lookalikes by its elliptical spores , which have a central partition , and an oil drop at each end . = = Taxonomy = = The species was originally described from Europe in 1789 by German naturalist August Batsch as Peziza citrina . Elias Fri</t>
+          <t>Humfrey Gale = Lieutenant General Sir Humfrey Myddelton Gale KBE , CB , CVO , MC ( 4 October 1890 – 8 April 1971 ) was an officer in the British Army who served in the First and Second World War , during which he was Chief Administrative Officer at Allied Forces Headquarters and later SHAEF under General of the Army Dwight Eisenhower . After the Second World War he was European Director of the United Nations Relief and Rehabilitation Administration , worked for the Anglo-Iranian Oil Company , and was chairman of the Basildon , Essex New Town Development Corporation = = Early life = = Humfrey Myddelton Gale was born in London , England on 4 October 1890 , the eldest of five children of Ernest Sewell Gale , an architect , and his wife Charlotte Sarah née Goddard . He was educated at St Paul 's School , London and studied at the Architectural School , Westminster from 1908 to 1910 . While there he served with the Artists Rifles . He decided to pursue a career in the British Indian Army an</t>
         </is>
       </c>
     </row>
@@ -1211,32 +1211,32 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>['episode', 'mulder', 'plot', 'find', 'scully', 'nielsen', 'doctor', 'files', 'scene', 'david_duchovny', 'finds', 'x-files', 'filmed', 'dana_scully', 'enterprise']</t>
+          <t>['breed', 'horses', 'horse', 'breeds', 'dog', 'dogs', 'arabian', 'bred', 'breeding', 'stud', 'stallion', 'breeders', 'pony', 'registered', 'hair']</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Three Words ( The X-Files ) = " Three Words " is the sixteenth episode of the eighth season ( and the 177th episode overall ) of the science fiction television series The X-Files and first aired in the United States and Canada on April 8 , 2001 , on Fox . It was written by executive producers Chris Carter and Frank Spotnitz , and directed by Tony Wharmby . The episode explores the series ' overarching mythology and earned a Nielsen rating of 7.6 and was viewed by 7.77 million households , receiving mixed to positive reviews from television critics . The show centers on FBI special agents Fox Mulder ( David Duchovny ) , Dana Scully ( Gillian Anderson ) and John Doggett ( Robert Patrick ) who work on cases linked to the paranormal , called X-Files . In this episode , Mulder secretly conducts his own investigation after a man is gunned down on the White House lawn attempting to inform the President of a planned alien invasion . However , he is soon in over his head as he tries to expose f</t>
+          <t>Heck horse = The Heck horse is a horse breed that is claimed to resemble the tarpan ( Equus ferus ferus ) , an extinct wild equine . The breed was created by the German zoologist brothers Heinz Heck and Lutz Heck in an attempt to breed back the tarpan . Although unsuccessful at creating a genetic copy of the extinct species , they developed a breed with grullo coloration and primitive markings . After the Nazi invasion of Poland , they were introduced to the Białowieża Forest , where a small herd still survives . Heck horses were subsequently exported to the United States , where a breed association was created in the 1960s . = = Breed characteristics = = Heck horses are dun or grullo ( a dun variant ) in color , with no white markings . The breed has primitive markings , including a dorsal stripe and horizontal striping on the legs . Heck horses generally stand between 12.2 and 13.2 hands ( 50 and 54 inches , 127 and 137 cm ) tall . The head is large , the withers low , and the legs a</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Never Again ( The X-Files ) = " Never Again " is the thirteenth episode of the fourth season of the American science fiction television series The X-Files . It was written by producers Glen Morgan and James Wong , and directed by Rob Bowman . The episode aired in the United States on February 2 , 1997 on the Fox network and in the United Kingdom on BBC One on December 3 , 1997 . The episode is a " Monster-of-the-Week " story , a stand-alone plot which is unconnected to the series ' wider mythology . The episode received a Nielsen rating of 13 and was viewed by 21.36 million viewers . It received mostly positive reviews from television critics . The show centers on FBI special agents Fox Mulder ( David Duchovny ) and Dana Scully ( Gillian Anderson ) who work on cases linked to the paranormal , called X-Files . Mulder is a believer in the paranormal , while the skeptical Scully has been assigned to debunk his work . In this episode , Scully leaves town — and Mulder — for a solo assignmen</t>
+          <t>Florida Cracker Horse = The Florida Cracker Horse is a breed of horse from Florida in the United States . It is genetically and physically similar to many other Spanish-style horses , especially those from the Spanish Colonial Horse group . The Florida Cracker is a gaited breed known for its agility and speed . The Spanish first brought horses to Florida with their expeditions in the early 16th century ; as colonial settlement progressed , they used the horses for herding cattle . These horses developed into the Florida Cracker type seen today , and continued to be used by Florida cowboys ( known as " crackers " ) until the 1930s . At this point they were superseded by American Quarter Horses needed to work larger cattle brought to Florida during the Dust Bowl , and population numbers declined precipitously . Through the efforts of several private families and the Florida government , the breed was saved from extinction , but there is still concern about its low numbers . Both The Live</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hellbound ( The X-Files ) = " Hellbound " is the eighth episode of the ninth season of the American science fiction television series The X-Files . It originally aired on the Fox network on January 27 , 2002 . It was written by David Amann and directed by Kim Manners . The episode is a " monster-of-the-week " episode , a stand-alone plot which is unconnected to the series ' wider mythology , or the overarching fictional history . The episode earned a Nielsen household rating of 5.1 and was viewed by 7.8 million viewers in its initial broadcast . It received positive reviews from television critics . The show centers on FBI special agents who work on cases linked to the paranormal , called X-Files ; this season focuses on the investigations of John Doggett ( Robert Patrick ) , Monica Reyes ( Annabeth Gish ) , and Dana Scully ( Gillian Anderson ) . In this episode , Reyes takes the lead while investigating an X-File case surrounding a man found skinned alive . When she discovers that he </t>
+          <t xml:space="preserve">Colorado Ranger = The Colorado Ranger is a horse breed from the Colorado High Plains in the United States . The breed is descended from two stallions imported from Turkey to the US state of Virginia in the late 1800s . These stallions were then bred to ranch horses in Nebraska and Colorado , and in the early 1900s the two stallions who every registered Colorado Ranger traces to , Patches # 1 and Max # 2 , were foaled . The breed was championed by rancher Mike Ruby , who founded the Colorado Ranger Horse Association in 1935 . Original registry membership limits resulted in many Colorado Ranger horses being registered instead as Appaloosas , but pedigree research is ongoing to discover additional horses who trace their ancestry back to the original stallions . By 2005 , more than 6,000 Colorado Ranger horses had been registered . Colorado Rangers may be any solid color or carry leopard spotting patterns . Pinto coloration and American Paint Horse breeding are not allowed , nor are draft </t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Fight Club ( The X-Files ) = " Fight Club " is the twentieth episode of the seventh season of the science fiction television series The X-Files . It premiered on the Fox network in the United States on May 7 , 2000 . It was written by series creator Chris Carter , directed by Paul Shapiro , and featured a guest appearance by Kathy Griffin . The episode plot serves as a " Monster-of-the-Week " story , which is unconnected to the series ' wider mythology . " Fight Club " earned a Nielsen household rating of 6.9 , being watched by 11.70 million people in its initial broadcast . The episode received mostly negative reviews from television critics . The show centers on FBI special agents Fox Mulder ( David Duchovny ) and Dana Scully ( Gillian Anderson ) who work on cases linked to the paranormal , called X-Files . Mulder is a believer in the paranormal , while the skeptical Scully has been assigned to debunk his work . In this episode , Mulder and Scully cross paths with a pair of doppelgan</t>
+          <t>Kentucky Mountain Saddle Horse = The Kentucky Mountain Saddle Horse is a horse breed from the US state of Kentucky . Developed as an all-around farm and riding horse in eastern Kentucky , they are related to the Tennessee Walking Horse and other gaited breeds . In 1989 the Kentucky Mountain Saddle Horse Association ( KMSHA ) was formed , and in 2002 , the subsidiary Spotted Mountain Horse Association ( SMHA ) was developed to registered Kentucky Mountain Saddle Horses with excessive white markings and pinto patterns . Conformation standards are the same for the two groups of horses , with the main difference being the color requirements . The KMSHA studbook is now closed to horses from unregistered parents , although it cross-registers with several other registries , while the SMHA studbook remains open . = = Characteristics = = Kentucky Mountain Saddle Horses must stand above 11 hands ( 44 inches , 112 cm ) high to be registered . Horses above this height are divided into two categori</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t xml:space="preserve">The End ( The X-Files ) = " The End " is the 20th and final episode of the fifth season , and 117th overall of the science fiction television series The X-Files . The episode first aired in the United States and Canada on May 17 , 1998 . " The End " subsequently aired in the United Kingdom on March 17 , 1999 on BBC One . The episode was written by executive producer Chris Carter , and directed by R. W. Goodwin . " The End " earned a Nielsen household rating of 11.9 , being watched by 18.76 million people in its initial broadcast . The episode received mixed to positive reviews from television critics . The show centers on FBI special agents Fox Mulder ( David Duchovny ) and Dana Scully ( Gillian Anderson ) who work on cases linked to the paranormal , called X-Files . Mulder is a believer in the paranormal , while the skeptical Scully has been assigned to debunk his work . In this episode , the assassination of a chess grandmaster leads Mulder and Scully into an investigation that they </t>
+          <t>Azteca horse = The Azteca is a horse breed from Mexico , with a subtype , called the " American Azteca " , found in the United States . They are well-muscled horses that may be of any solid color , and the American Azteca may also have pinto coloration . Aztecas are known to compete in many western riding and some English riding disciplines . The Mexican registry for the original Azteca and the United States registries for the American Azteca have registration rules that vary in several key aspects , including ancestral bloodlines and requirements for physical inspections . The Azteca was first developed in Mexico in 1972 , from a blend of Andalusian , American Quarter Horse and Mexican Criollo bloodlines . From there , they spread to the United States , where American Paint Horse blood was added . = = Breed characteristics = = The three foundation breeds of the Azteca are the Andalusian ( defined by the Mexican registry as either Pura Raza Española or Lusitano ) , American Quarter Hor</t>
         </is>
       </c>
     </row>
@@ -1246,32 +1246,32 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>['son', 'king', 'died', 'brother', 'death', 'daughter', 'father', 'reign', 'royal', 'kings', 'younger', 'succeeded', 'sons', 'kingdom', 'probably']</t>
+          <t>['british', 'french', 'militia', 'troops', 'fort', 'howe', 'battle', 'frigate', 'spanish', 'men', 'washington', 'fleet', 'expedition', 'continental_army', 'wounded']</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Sitric Cáech = Sitric Cáech , also known as Sitric Gále , ( Old Norse : Sigtryggr , died 927 ) was a Viking leader who ruled Dublin and then Viking Northumbria in the early 10th century . He was a grandson of Ímar and a member of the Uí Ímair . Sitric was most probably among those Vikings expelled from Dublin in 902 , whereafter he may have ruled territory in the eastern Danelaw in England . In 917 , he and his kinsman Ragnall ua Ímair sailed separate fleets to Ireland where they won several battles against local kings . Sitric successfully recaptured Dublin and established himself as king , while Ragnall returned to England to become King of Northumbria . In 919 , Sitric won a victory at the Battle of Islandbridge over a coalition of local Irish kings who aimed to expel the Uí Ímair from Ireland . Six Irish kings were killed in the battle , including Niall Glúndub , overking of the Northern Uí Néill and High King of Ireland . In 920 Sitric left Dublin for Northumbria , with his kinsma</t>
+          <t xml:space="preserve">Battle of Bonchurch = The Battle of Bonchurch took place sometime in late July 1545 at Bonchurch on the Isle of Wight . No source of information states a specific date , although it could have happened on 21 July . The battle was a part of the wider Italian War of 1542 – 1546 , and took place during the 1545 French invasion of the Isle of Wight . Several landings were made by the French during the invasion of the Isle of Wight , including the one at Bonchurch . The two combatants were the Kingdom of England and the Kingdom of France . England won the battle , and the French advance across the Isle of Wight was halted . The battle was fought between French regular soldiers , and English militiamen . The number of French soldiers involved is believed to be around 500 . The number of English militiamen is uncertain , with one source of information stating 300 , and another stating 2800 . English forces at the battle are understood to have been commanded by Captain Robert Fyssher , whilst </t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Stephen V of Hungary = Stephen V ( Hungarian : V. István , Croatian : Stjepan V. , Slovak : Štefan V ; before 18 October 1239 – 6 August 1272 , Csepel Island ) was King of Hungary and Croatia between 1270 and 1272 , and Duke of Styria from 1258 to 1260 . He was the oldest son of King Béla IV and Maria Laskarina . King Béla had his son crowned king at the age of six and appointed him Duke of Slavonia . Still a child , Stephen married Elizabeth , a daughter of a chieftain of the Cumans whom his father settled in the Great Hungarian Plain . King Béla appointed Stephen Duke of Transylvania in 1257 and Duke of Styria in 1258 . The local noblemen in Styria , which had been annexed four years before , opposed his rule . Assisted by King Ottokar II of Bohemia , they rebelled and expelled Stephen 's troops from most parts of Styria . After Ottokar II routed the united army of Stephen and his father in the Battle of Kressenbrunn on 12 July 1260 , Stephen left Styria and returned to Transylvania </t>
+          <t>Boston campaign = The Boston campaign was the opening campaign of the American Revolutionary War , taking place primarily in the Province of Massachusetts Bay . The campaign began with the Battles of Lexington and Concord on April 19 , 1775 , in which the local colonial militias interdicted a British government attempt to seize military stores and leaders in Concord , Massachusetts . The entire British expedition suffered significant casualties during a running battle back to Charlestown against an ever-growing number of militia . Subsequently , accumulated militia forces surrounded the city of Boston , beginning the Siege of Boston . The main action during the siege , the Battle of Bunker Hill on June 17 , 1775 , was one of the bloodiest encounters of the war , an resulted in a Pyrrhic British victory . There were also numerous skirmishes near Boston and the coastal areas of Boston , resulting in loss of life , military supplies , or both . In July 1775 , George Washington took comman</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Géza II of Hungary = Géza II ( Hungarian : II . Géza ; Croatian : Gejza II ; Slovak : Gejza II ; 1130 – 31 May 1162 ) was King of Hungary and Croatia from 1141 to 1162 . He was the oldest son of Béla the Blind and his wife , Helena of Rascia . When his father died , Géza was still a child and he started ruling under the guardianship of his mother and her brother , Beloš . A pretender to the throne , Boris Kalamanos , who had already claimed Hungary during Béla the Blind 's reign , temporarily captured Pressburg ( now Bratislava in Slovakia ) with the assistance of German mercenaries in early 1146 . In retaliation , Géza , who came of age in the same year , invaded Austria and routed Henry Jasomirgott , Margrave of Austria , in the Battle of the Fischa . Although the German – Hungarian relations remained tense , no major confrontations occurred when the German crusaders marched through Hungary in June 1147 . Two months later , Louis VII of France and his crusaders arrived , along with B</t>
+          <t>Meigs Raid = The Meigs Raid ( also known as the Battle of Sag Harbor ) was a military raid by American Continental Army forces , under the command of Connecticut Colonel Return Jonathan Meigs , on a British Loyalist foraging party at Sag Harbor , New York on May 24 , 1777 during the American Revolutionary War . Six Loyalists were killed and 90 captured while the Americans suffered no casualties . The raid was made in response to a successful British raid on Danbury , Connecticut in late April that was opposed by American forces in the Battle of Ridgefield . Organized in New Haven , Connecticut by Brigadier General Samuel Holden Parsons , the expedition crossed Long Island Sound from Guilford on May 23 , dragged whaleboats across the North Fork of Long Island , and raided Sag Harbor early the next morning , destroying boats and supplies . The battle marked the first American victory in the state of New York after New York City and Long Island had fallen in the British campaign for the c</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Andrew I of Hungary = Andrew I the White or the Catholic ( Hungarian : I. Fehér or Katolikus András or Endre ; c . 1015 – Zirc , before 6 December 1060 ) was King of Hungary from 1046 to 1060 . He descended from a younger branch of the Árpád dynasty . After spending fifteen years in exile , he ascended the throne during an extensive revolt of the pagan Hungarians . He strengthened the position of Christianity in the Kingdom of Hungary and successfully defended its independence against the Holy Roman Empire . His efforts to ensure the succession of his son , Solomon , resulted in the open revolt of his brother , Béla . Béla dethroned Andrew by force in 1060 . Andrew suffered severe injuries during the fighting and died before his brother was crowned king . = = Early life = = = = = Childhood ( c . 1015 – 1031 ) = = = Medieval sources provide two contradictory reports of the parents of Andrew , and his two brothers , Levente and Béla . For instance , the Chronicle of Zagreb and Saint Gera</t>
+          <t>Battle of Kemp 's Landing = The Battle of Kemp 's Landing , also known as the Skirmish of Kempsville , was a skirmish in the American Revolutionary War that occurred on November 15 , 1775 . Militia companies from Princess Anne County in the Province of Virginia assembled at Kemp 's Landing to counter British troops under the command of Virginia 's last colonial governor , John Murray , Lord Dunmore , that had landed at nearby Great Bridge . Dunmore was investigating rumors of Patriot troop arrivals from North Carolina that turned out to be false ; he instead moved against the Princess Anne militia , defeating their attempt at an ambush and routing them . Dunmore followed up the victory with a reading of his proclamation declaring martial law and promising freedom to slaves belonging to Patriot owners if they served in the British military . This increased opposition to his activities , and he was eventually forced to leave Virginia . = = Background = = Tensions in the British Colony of</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Robert Bloet = Robert Bloet ( sometimes Robert Bloett ; died 1123 ) was Bishop of Lincoln 1093-1123 and Chancellor of England . Born into a noble Norman family , he became a royal clerk under King William I. Under William I 's son and successor King William II , Bloet was first named chancellor then appointed to the See of Lincoln . Continuing to serve the king while bishop , Bloet remained a close royal councillor to William II 's successor , King Henry I. He did much to embellish Lincoln Cathedral , and gave generously to his cathedral and other religious houses . He educated a number of noblemen , including illegitimate children of Henry I. He also was the patron of the medieval chronicler Henry of Huntingdon , and was an early patron of Gilbert of Sempringham , the founder of the Gilbertine monastic order . = = Early life = = Bloet was a member of the Norman noble family that held Ivry in Normandy . Bloet was related in some manner to Hugh , the Bishop of Bayeux from 1015 to 1049 ,</t>
+          <t>Mount Hope Bay raids = The Mount Hope Bay raids were a series of military raids conducted by British troops during the American Revolutionary War against communities on the shores of Mount Hope Bay on May 25 and 30 , 1778 . The towns of Bristol and Warren , Rhode Island were significantly damaged , and Freetown , Massachusetts ( present-day Fall River ) was also attacked , although its militia resisted British activities . The British destroyed military defenses in the area , including supplies that had been cached by the Continental Army in anticipation of an assault on British-occupied Newport , Rhode Island . Homes as well as municipal and religious buildings were also destroyed in the raids . On May 25 , 500 British and Hessian soldiers , under orders from General Sir Robert Pigot , the commander of the British garrison at Newport , Rhode Island , landed between Bristol and Warren , destroyed boats and other supplies , and plundered Bristol . Local resistance was minimal and ineffe</t>
         </is>
       </c>
     </row>
@@ -1281,32 +1281,32 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>['text', 'notes', 'book', 'bach', 'sunday', 'published', 'setting', 'edition', 'movements', 'describes', 'publication', 'bass', 'read', 'author', 'magazine']</t>
+          <t>['lap', 'race', 'drivers', 'laps', 'pit', 'car', 'ferrari', 'prix', 'driver', 'qualifying', 'session', 'fastest', 'ahead', 'hamilton', 'points']</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Gleichwie der Regen und Schnee vom Himmel fällt , BWV 18 = Gleichwie der Regen und Schnee vom Himmel fällt ( Just as the rain and snow fall from heaven ) , BWV 18 , is an early church cantata by Johann Sebastian Bach . He composed it in Weimar for the Sunday Sexagesimae , the second Sunday before Lent , likely by 1713 . The cantata is based on a text by Erdmann Neumeister published in 1711 . It is one of Bach cantata texts of the Weimar period not written by the court poet Salomon Franck . The text cites Isaiah , related to the gospel , the parable of the Sower . The third movement is in the style of a sermon , combined with a litany by Martin Luther . The closing chorale is the eighth stanza of Lazarus Spengler 's hymn " Durch Adams Fall ist ganz verderbt " . The cantata falls relatively early in Bach 's chronology of cantata compositions . It was possibly composed for 24 February 1715 , but more likely a year or even two earlier . Bach structured the work in five movements , a sinfon</t>
+          <t>2010 Showtime Southern 500 = The 2010 Showtime Southern 500 , 61st running of the event , was a NASCAR Sprint Cup Series motor race that was held on May 8 , 2010 at Darlington Raceway in Darlington , South Carolina . It was the eleventh race of the 2010 NASCAR Sprint Cup Series season . The event began at 7 : 30 p.m. EDT . It was televised live in the United States on Fox and its U.S. radio coverage was broadcast on Motor Racing Network starting at 6 p.m. EDT . The 367-lap race was won by Denny Hamlin for Joe Gibbs Racing after starting seven positions behind polesitter Jamie McMurray . McMurray finished second in a Chevrolet , and Kurt Busch finished third in a Dodge . The race had a total of 11 cautions and 22 lead changes among 11 different drivers . Kevin Harvick remained the point leader after finishing the race in the sixth position . = = Background = = Coming into the race , Richard Childress Racing driver Kevin Harvick led the Drivers ' Championship with 1,467 points , with Hen</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Schwingt freudig euch empor , BWV 36 = Schwingt freudig euch empor ( Soar joyfully upwards ) , BWV 36 , is a church cantata by Johann Sebastian Bach . He composed it in Leipzig in 1731 for the first Sunday in Advent , drawing on material from previous congratulatory cantatas , beginning with Schwingt freudig euch empor , BWV 36c ( 1725 ) . The Gospel for the Sunday was the Entry into Jerusalem , thus the mood of the secular work matched " the people 's jubilant shouts of Hosanna " . In a unique structure in Bach 's cantatas , he interpolated four movements derived from the former works with four stanzas from two important hymns for Advent , to add liturgical focus , three from Luther 's " Nun komm , der Heiden Heiland " and one from Nicolai 's " Wie schön leuchtet der Morgenstern " . He first performed the cantata in its final form of two parts , eight movements , on 2 December 1731 . = = History and words = = Bach composed the cantata in 1731 in Leipzig , for the first Sunday of Adven</t>
+          <t>2013 Mudsummer Classic = The 2013 Mudsummer Classic ( formally the CarCash Mudsummer Classic presented by CNBC Prime 's The Profit ) was a NASCAR Camping World Truck Series stock car race held on July 24 , 2013 at Eldora Speedway in New Weston , Ohio . The race was the first dirt track race held by a NASCAR national touring series ( Cup , Xfinity , Trucks ) since 1970 . Contested over 150 laps , the race was the tenth of the 2013 NASCAR Camping World Truck Series season . Ken Schrader of self-owned Ken Schrader Racing won the pole position , and became the oldest pole sitter in NASCAR history at 58 years of age . Austin Dillon of Richard Childress Racing won the race , while Kyle Larson and Ryan Newman finished second and third , respectively . The qualifying procedure was unique for the race ; drivers ' qualifying times set the starting grids for five heat races to determine the feature race 's starting lineup , while the top five of a last chance qualifier ( LCQ ) advance to the feat</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Aus der Tiefen rufe ich , Herr , zu dir , BWV 131 = Aus der Tiefen rufe ich , Herr , zu dir ( Out of the depths I call , Lord , to You ) , BWV 131 , is a church cantata by the German composer Johann Sebastian Bach . It was composed in either 1707 or 1708 , which makes it one of Bach 's earliest cantatas . Some sources suggest that it could be his earliest surviving work in this form , but current thinking is that there are one or two earlier examples . The cantata was commissioned by the minister of one of the churches in Mühlhausen , the city where Bach worked at the time . It was possibly written for a special occasion . The text is based on Luther 's German version of Psalm 130 and also incorporates the words of a chorale . Bach 's music integrates melodies from the chorale into larger structures . Bach also shows his interest in counterpoint , something which was characteristic of him throughout his career . = = History and words = = A note on the autograph score of the cantata ind</t>
+          <t>2009 Ford 400 = The 2009 Ford 400 was the thirty-six and final stock car race of the 2009 NASCAR Sprint Cup Series as well as the tenth and final race of the season-ending Chase for the Sprint Cup . It was held on November 22 , 2009 at Homestead-Miami Speedway , in Homestead , Florida before a crowd of 70,000 people . The 267-lap race was won by Denny Hamlin of the Joe Gibbs Racing team after starting from thirty-eighth position . Jeff Burton finished second and his teammate Kevin Harvick came in third . Jimmie Johnson won the pole position and maintained his lead on the first lap of the race . Many Chase for the Sprint Cup participants , including Johnson , Kurt Busch and Mark Martin , were in the top ten for most of the race , although some encountered problems in the closing laps . Kyle Busch was leading the race with forty-four laps remaining , giving the lead to Hamlin who maintained it to win the race . There were seven cautions in the race , as well as eighteen lead changes amon</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Geist und Seele wird verwirret , BWV 35 = Geist und Seele wird verwirret ( Spirit and soul become confused ) , BWV 35 , is a church cantata by Johann Sebastian Bach . He composed the solo cantata for alto voice in Leipzig for the twelfth Sunday after Trinity and first performed it on 8 September 1726 . Bach composed the cantata in his fourth year as Thomaskantor ( musical director ) in Leipzig . The text is based on the day 's prescribed reading from the Gospel of Mark , the healing of a deaf mute man . The librettist is Georg Christian Lehms , whose poetry Bach had used already in Weimar as the basis for solo cantatas . The text quotes ideas from the gospel and derives from these the analogy that as the tongue of the deaf mute man was opened , the believer should be open to admire God 's miraculous deeds . The cantatas for this Sunday have a positive character , which Bach stressed in earlier works for the occasion by including trumpets in the score . In this work , he uses instead an</t>
+          <t>2010 Price Chopper 400 = The 2010 Price Chopper 400 was a NASCAR Sprint Cup Series stock car race that was held on October 3 , 2010 at Kansas Speedway in Kansas City , Kansas . The 300 lap race was the twenty-ninth in the 2010 NASCAR Sprint Cup Series . The race was also the third event in the ten round Chase for the Sprint Cup competition , which would conclude the 2010 season . Greg Biffle , of the Roush Fenway Racing team , won the race , with Jimmie Johnson finishing second and Kevin Harvick third . Pole position driver Kasey Kahne maintained his lead on the first lap to begin the race , as Jeff Gordon , who started in the third position on the grid , remained behind him . Twenty-three laps later Jeff Gordon became the leader of the race . After the final pit stops , Paul Menard became the leader of the race , but with less than fifty laps remaining , Biffle passed him . He maintained the first position to lead a total of sixty laps , and to win his second race of the season . Ther</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Preise , Jerusalem , den Herrn , BWV 119 = Preise , Jerusalem , den Herrn ( Praise the Lord , Jerusalem ) , BWV 119 , is a sacred cantata by Johann Sebastian Bach . He composed it in Leipzig for Ratswechsel , the inauguration of a new town council , and first performed it on 30 August 1723 . Bach composed the cantata in his first year as Thomaskantor in Leipzig , about three months after taking office at the end of May 1723 . A festive service at the Nikolaikirche was an annual event , celebrating the inauguration of a new town council , always held on the Monday after St. Bartholomew ( August 24 ) . The text by an anonymous poet includes psalm verses and an excerpt from Martin Luther 's German Te Deum . It is focused on acknowledgement of authority as a gift of God , thanks for past blessings , and prayer for future help . The cantata is structured in nine movements , three of them choral ( 1 , 7 , 9 ) , the others alternating arias and recitatives . The orchestra is large and represe</t>
+          <t>2011 Coca-Cola 600 = The 2011 Coca-Cola 600 , the 52nd running of the event , was a NASCAR Sprint Cup Series motor race held on May 29 , 2011 , at Charlotte Motor Speedway in Concord , North Carolina . Contested over 400 laps on the 1.5-mile ( 2.4 km ) asphalt quad-oval , it was the twelfth race of the 2011 Sprint Cup Series season . The race was won by Kevin Harvick for the Richard Childress Racing team . David Ragan finished second , and Joey Logano clinched third . There were 14 cautions and 38 lead changes among 19 different drivers throughout the course of the race . The result moved Harvick to the second position in the Drivers ' Championship . He remained 36 points behind first place driver Carl Edwards and one ahead of Jimmie Johnson in third . In the Manufacturers ' Championship , Chevrolet was first with 83 points , six ahead of Ford . Toyota was third with 64 points , 24 points ahead of Dodge . The race was extended to 402 laps and 603 miles ( 970 km ) , making it the longes</t>
         </is>
       </c>
     </row>
@@ -1316,32 +1316,32 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>['raaf', 'flying', 'wing', 'combat', 'unit', 'training', 'operational', 'pilot', 'officer', 'aircraft', 'flight', 'pilots', 'disbanded', 'commanding', 'squadron']</t>
+          <t>['temple', 'mosque', 'han', 'dynasty', 'sanskrit', 'buddhist', 'hindu', 'chinese', 'bce', 'texts', 'monastery', 'buddhism', 'temples', 'wall', 'text']</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">No. 84 Wing RAAF = No. 84 Wing is a Royal Australian Air Force ( RAAF ) transport wing . Coming under the control of Air Mobility Group ( AMG ) , it is headquartered at RAAF Base Richmond , New South Wales . The wing comprises No. 34 Squadron , operating Boeing 737 and Bombardier Challenger 604 VIP jets ; No. 37 Squadron , operating Lockheed Martin C-130J Super Hercules medium transports ; and a technical training unit , No. 285 Squadron . Formed in 1944 for army co-operation duties in the South West Pacific theatre of World War II , No. 84 Wing operated a mix of aircraft including CAC Boomerangs , CAC Wirraways , Auster AOPs and Bristol Beauforts , before disbanding in 1946 . It was re-formed in 1991 as a tactical transport wing headquartered at RAAF Base Townsville , Queensland , comprising Nos. 35 and 38 Squadrons operating de Havilland Canada DHC-4 Caribous . By 1996 , it had been augmented by No. 32 Squadron , operating Hawker Siddeley HS 748 trainer-transports . In 1998 , No. 84 </t>
+          <t>Pundarikakshan Perumal Temple = Pundarikakshan Perumal Temple or Thiruvellarai a in Thiruvellarai , a village in the outskirts of Tiruchirappalli in the South Indian state of Tamil Nadu , is dedicated to the Hindu god Vishnu . Constructed in the Dravidian style of architecture , the temple is glorified in the Divya Prabandha , the early medieval Tamil canon of the Azhwar saints from the 6th – 9th centuries AD . It is one of the 108 Divyadesam dedicated to Vishnu , who is worshipped as Pundarikakshan and his consort Lakshmi as Pankajavalli . The temple was built by Shivi Chakravarthy , king of Ayodhya in Treta Yuga 15 lakh years ago . This temple is older than Srirangam temple.The temple has three inscriptions in its two rock-cut caves , two dating from the period of Nandivarman II ( 732 – 796 AD ) and the other to that of Dantivarman ( 796 – 847 ) . It also has Pallava sculptural depictions of Narasimha and Varaha , two of the ten avatars of Vishnu . A granite wall surrounds the temple</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Lockheed YF-22 = The Lockheed / Boeing / General Dynamics YF-22 was an American single-seat , twin-engine fighter aircraft technology demonstrator designed for the United States Air Force ( USAF ) . The design was a finalist in the USAF 's Advanced Tactical Fighter competition , and two prototypes were built for the demonstration / validation phase of the competition . The YF-22 won the contest against the Northrop YF-23 , and entered production as the Lockheed Martin F-22 Raptor . The YF-22 has similar aerodynamic layout and configuration as the F-22 , but with differences in the position and design of the cockpit , tail fins and wings , and in internal structural layout . In the 1980s , the USAF began looking for a replacement for its fighter aircraft , especially to counter the advanced Su-27 and MiG-29 . A number of companies , divided into two teams , submitted their proposals . Northrop and McDonnell Douglas submitted the YF-23 . Lockheed , Boeing and General Dynamics proposed an</t>
+          <t xml:space="preserve">Kandariya Mahadeva Temple = The Kandariya Mahadeva Temple ( Devanagari : कंदारिया महादेव मंदिर , Kaṇḍāriyā Mahādeva Mandir ) , meaning " the Great God of the Cave " , is the largest and most ornate Hindu temple in the medieval temple group found at Khajuraho in Madhya Pradesh , India . It is considered one of the best examples of temples preserved from the medieval period in India . = = Location = = Kaṇḍāriyā Mahādeva Temple is located in the Chhatarpur district of Madhya Pradesh in Central India . It is in the Khajuraho village , and the temple complex is spread over an area of 6 square kilometres ( 2.3 sq mi ) . It is in the western part of the village to the west of the Vishnu temple . The temple complex , in the Khajuraho village at an elevation of 282 metres ( 925 ft ) , is well connected by road , rail and air services . Khajuraho is 34 miles ( 55 km ) to the south of Mahoba , 29 miles ( 47 km ) away from the Chhatarpur city to its east , 27 miles ( 43 km ) away from Panna , 400 </t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>No. 3 Elementary Flying Training School RAAF = No. 3 Elementary Flying Training School ( No. 3 EFTS ) was a Royal Australian Air Force ( RAAF ) pilot training unit that operated during World War II . It was one of twelve elementary flying training schools employed by the RAAF to provide introductory flight instruction to new pilots as part of Australia 's contribution to the Empire Air Training Scheme . No. 3 EFTS was established in January 1940 at Essendon , Victoria , and initially included a significant proportion of civilian staff and private aircraft ; by mid-year these had been largely integrated into the military . The school was disbanded in May 1942 , its aircraft and instructional staff having been transferred to No. 11 Elementary Flying School at Benalla . = = History = = Flying instruction in the Royal Australian Air Force ( RAAF ) underwent major changes following the outbreak of World War II , in response to a vast increase in the number of aircrew volunteers and the comm</t>
+          <t>Raghunath Temple = Raghunath Temple consists of a complex of seven Hindu shrines , each with its own Shikhara . It is one of the largest temple complexes of north India . It is located in Jammu in the Indian state of Jammu and Kashmir . The temple was built during the period 1822 – 1860 by order of Maharaja Ranjit Singh , while Jammu was under his administration by Maharaja Gulab Singh . The temple has many gods in its complex of shrines , but the presiding deity is Rama , an Avatar of Vishnu . The Mughal architectural influence is seen in all the spiral shaped towers which have gold plated spires , except the tower over the main shrine which is said to be in Sikh architectural style . The niches in the walls of the shrines are decorated with 300 well crafted images of deities . The paintings in the 15 panels of the main shrine are based on themes from Ramayana , Mahabharata , and Bhagavad Gita . The temple was also in the news during 2002 when suicide bombers Fidayeen of the Lashkar-e</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>No. 486 Squadron RAAF = No. 486 Squadron was a maintenance unit of the Royal Australian Air Force ( RAAF ) . It was formed in August 1946 as part of No. 86 ( Transport ) Wing , which operated Douglas C-47 Dakotas out of RAAF Station Schofields , New South Wales . The squadron transferred to RAAF Station Richmond in June 1949 . It relocated again to RAAF Base Canberra in April 1954 , before returning to Richmond in August 1958 to commence maintenance of No. 86 Wing 's newly delivered Lockheed C-130 Hercules . The squadron was disbanded between August 1964 and March 1966 . In the 1980s and 1990s , it was responsible for servicing the RAAF 's Boeing 707 tanker / transports , as well as the Hercules . No. 486 Squadron was again disbanded at Richmond in October 1998 , and its functions handed over to No. 86 Wing 's Hercules squadrons . = = History = = No. 486 ( Maintenance ) Squadron was established at RAAF Station Schofields , New South Wales , on 26 August 1946 . Commanded by Wing Command</t>
+          <t>Zhenguo Temple = Zhenguo Temple ( Chinese : 镇国寺 ) is a Buddhist temple located 10 km from Pingyao in the village of Hadongcun , in Shanxi Province , China . The temple 's oldest hall , the Wanfo Hall , was built in 963 during the Northern Han dynasty , and is notable for featuring very large brackets that hold up the roof and flying eaves . The sculptures inside the hall are among the only examples of 10th century Buddhist sculpture in China . = = History = = The history of the temple begins in 963 , when it was recorded that Ten-Thousand Buddha Hall ( Wànfó diàn 万佛殿 ) was built . The date is written on a beam in the hall , and is also the date given by a local history of Pingyao county written in the 19th century . A stela written in 1819 also confirms this date . Wanfo Hall is the oldest building at Zhenguo temple , and is the only surviving building that dates from the short-lived Northern Han dynasty . Although little is known of the temple 's history , stelae record that it was re</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>10th Combat Aviation Brigade ( United States ) = The Combat Aviation Brigade , 10th Mountain Division is a combat aviation brigade of the United States Army based at Fort Drum , New York . It is a subordinate unit of the 10th Mountain Division . Reactivated in 1988 , the 10th Mountain Division 's Combat Aviation Brigade supported the division as it undertook numerous operations and overseas contingencies in the 1990s , including Operation Restore Hope , Operation Uphold Democracy , and Task Force Eagle , as well as disaster relief following Hurricane Andrew . The brigade has since become involved in the War on Terrorism , seeing four deployments to Afghanistan to support Operation Enduring Freedom and a deployment to Iraq to support Operation Iraqi Freedom . The brigade is currently on its fourth deployment to Afghanistan and is serving in Regional Command - East under Combined Joint Task Force 101 in support of Operation Enduring Freedom . = = Organization = = The Combat Aviation Brig</t>
+          <t>Jokhang = The Jokhang ( Tibetan : ཇོ ་ ཁང ། , Chinese : 大昭寺 ) , also known as the Qoikang Monastery , Jokang , Jokhang Temple , Jokhang Monastery and Zuglagkang ( Tibetan : གཙུག ་ ལག ་ ཁང ༌ ། , Wylie : gtsug-lag-khang , ZYPY : Zuglagkang or Tsuklakang ) , is a Buddhist temple in Barkhor Square in Lhasa , the capital city of Tibet . Tibetans , in general , consider this temple as the most sacred and important temple in Tibet . The temple is currently maintained by the Gelug school , but they accept worshipers from all sects of Buddhism . The temple 's architectural style is a mixture of Indian vihara design , Tibetan and Nepalese design . The Jokhang was founded during the reign of King Songtsen Gampo . According to tradition , the temple was built for the king 's two brides : Princess Wencheng of the Chinese Tang dynasty and Princess Bhrikuti of Nepal . Both are said to have brought important Buddhist statues and images from China and Nepal to Tibet , which were housed here , as part o</t>
         </is>
       </c>
     </row>
@@ -1351,32 +1351,32 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>['took', 'second', 'played', 'runs', 'team', 'tour', 'england', 'australia', 'playing', 'class', 'run', 'came', 'score', 'match', 'taking']</t>
+          <t>['simpsons', 'south_park', 'homer', 'lisa', 'episode', 'episodes', 'kenny', 'jake', 'stan', 'kyle', 'finn', 'animated', 'parker', 'voice', 'voiced']</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Ray Lindwall = Raymond Russell Lindwall MBE ( 3 October 1921 – 23 June 1996 ) was a cricketer who represented Australia in 61 Tests from 1946 to 1960 . He is widely regarded as one of the greatest fast bowlers of all time . He also played top-flight rugby league football with St. George , appearing in two grand finals for the club before retiring to fully concentrate on Test cricket . A right-arm fast bowler of express pace , Lindwall was widely regarded as the greatest pace bowler of his era and one of the finest of all time . Together with Keith Miller , Lindwall formed a new-ball pairing regarded as one of the greatest to have played cricket . Lindwall was known for his classical style , with a smooth and rhythmic run-up and textbook side-on bowling action , from which he generated his trademark outswinger which moved away late at high pace . Lindwall mixed his outswinger with a searing yorker , subtle changes of pace and an intimidating bouncer that skidded at the heads of opposing</t>
+          <t>SpongeBob SquarePants ( season 7 ) = The seventh season of the American animated television series SpongeBob SquarePants , created by marine biologist and animator Stephen Hillenburg , originally aired on Nickelodeon in the United States from July 19 , 2009 to June 11 , 2011 . It contained 26 episodes , beginning with the episodes " Tentacle Vision " and " I Heart Dancing " . The series chronicles the exploits and adventures of the title character and his various friends in the fictional underwater city of Bikini Bottom . The season was executive produced by series creator Hillenburg and writer Paul Tibbitt , who also acted as the showrunner . In 2011 , Legends of Bikini Bottom , an anthology series consists of five episodes from the season , was launched . A number of guest stars appeared on the season 's episodes . Several compilation DVDs that contained episodes from the season were released . The SpongeBob SquarePants : Complete Seventh Season DVD was released in Region 1 on Decemb</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Military career of Keith Miller = The military career of Keith Miller , an Australian Test cricketer and Australian rules footballer , lasted from August 1940 until June 1946 , when World War II interrupted his sporting career . Miller enlisted in the Militia , before switching to the Royal Australian Air Force , where he served from November 1941 until 1946 when he was discharged with the rank of flying officer . Miller trained as a fighter pilot , and in the last month of the European theatre of war , he flew combat missions over German installations . However , Miller was more notable for his efforts as a cricketer , representing the Royal Australian Air Force cricket team and after VE Day , the Australian Services in the Victory Tests of 1945 , followed by a tour of the Indian subcontinent and Australia before being demobilised . While serving in the Militia , Miller continued playing football for St Kilda Saints and interstate cricket for Victoria when he was off duty . Miller str</t>
+          <t>Cartman 's Mom Is a Dirty Slut = " Cartman 's Mom Is a Dirty Slut " is the first season finale of the American animated television series South Park . It originally aired on Comedy Central in the United States on February 25 , 1998 . The episode is the highest viewed episode in the entire South Park series , with 6.4 million views . It is part one of a two-episode story arc , which concluded with " Cartman 's Mom Is Still a Dirty Slut " . The episode follows Eric Cartman , one of the show 's child protagonists , becoming curious about the identity of his father . He discovers that his father is most likely a man his mother had sexual intercourse with during an annual party called " The Drunken Barn Dance " . Meanwhile , his friends Stan , Kyle and Kenny participate on America 's Stupidest Home Videos , after filming Cartman playing in his yard with plush toys . The episode was written by Trey Parker and staff writer David A. Goodman , and directed by Parker . It featured a guest appear</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Port Phillip v Van Diemen 's Land , 1851 = On 11 and 12 February 1851 , teams from Port Phillip , Victoria and Van Diemen 's Land ( now Tasmania ) played a timeless cricket match at the Launceston Racecourse , known now as the NTCA Ground , in Tasmania . The match was held under the aegis of the Launceston Cricket Club , which represented the Van Diemen 's Land cricket team as the home team , and the Melbourne Cricket Club , which represented the Port Phillip team as the visiting team . The match was organised in celebration of the separation of Victoria from New South Wales . William Philpott was the captain of the Port Phillip team , while John Marshall led the Van Diemen 's Land team . All overs bowled in the first first-class cricket match had only four deliveries each . The first ball bowled during the match was an underarm delivery by William Henty of Van Diemen 's Land . Port Phillip 's Thomas Ferrier Hamilton scored the most runs during the match , while Thomas Antill , again f</t>
+          <t>An Elephant Makes Love to a Pig = " An Elephant Makes Love to a Pig " is the fifth episode in the first season of the American animated television series South Park . It originally aired on Comedy Central in the United States on September 10 , 1997 . In the episode , the boys of South Park try to force Kyle 's pet elephant to crossbreed with Cartman 's pet pig for a class project on genetic engineering . Meanwhile , Stan tries to deal with his sister Shelley , who keeps beating him up . The episode was written by series co-creators Trey Parker and Matt Stone along with Dan Sterling . The episode served as both a parody of genetic engineering and a statement against its potential evils . The scenes of Stan getting beat up by his sister were inspired by Parker 's real-life childhood experiences with his own sister , who is also named Shelley . " An Elephant Makes Love to a Pig " was met with generally positive reviews , and has been described as one of the most popular early South Park e</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Queen 's Park Oval = The Queen 's Park Oval is a sports stadium in Port of Spain , Trinidad and Tobago . Privately owned by the Queen 's Park Cricket Club , it is currently the largest capacity cricket ground in the West Indies with seating for about 18,000 . It has hosted more Test matches than any other ground in the Caribbean , and also hosted a number of One-Day International ( ODI ) matches , including many World Series Cricket games in 1979 and matches of the 2007 Cricket World Cup . The Trinidad and Tobago cricket team play most of their home matches at the ground , and it is the home ground of the Caribbean Premier League team Trinidad and Tobago Red Steel . Considered by many players , journalists and critics as one of the most picturesque cricket venues , the ground first hosted a Test match in February 1930 when England toured the Caribbean , though it had previously hosted many first class tours as early as the 1897 tour under Lord Hawke . The pavilion dates back to 1896 , </t>
+          <t>Julie Kavner = Julie Deborah Kavner ( born September 7 , 1950 ) is an American film and television actress , voice actress and comedian . She first attracted notice for her role as Valerie Harper 's character 's younger sister Brenda in the sitcom Rhoda for which she won a Primetime Emmy Award for Outstanding Supporting Actress in a Comedy Series . She is best known for her voice role as Marge Simpson on the animated television series The Simpsons . She also voices other characters for the show , including Jacqueline Bouvier , and Patty and Selma Bouvier . Known for her improvisation and distinctive " honeyed gravel voice , " Kavner was cast in her first professional acting role as Brenda Morgenstern in Rhoda in 1974 . She received the Primetime Emmy Award in 1978 and three more nominations for playing the character . Following Rhoda , Kavner was cast in The Tracey Ullman Show , which debuted in 1987 . The Tracey Ullman Show included a series of animated shorts about a dysfunctional fa</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Charles Ollivierre = Charles Augustus Ollivierre ( 20 July 1876 – 25 March 1949 ) was a Vincentian cricketer who represented the West Indies in matches before they attained Test match status . Born in St Vincent , Ollivierre initially played first-class cricket for Trinidad ; he was selected to tour England with the West Indies team in 1900 . He later qualified to play first-class cricket for Derbyshire between 1901 and 1907 , becoming the first black West Indian to play for an English county . Ollivierre was reasonably successful in county cricket and had a reputation as a stylish batsman . However , he dropped out of first-class cricket after 1907 owing to eye trouble . = = Early life and career = = Ollivierre was born in St Vincent on 20 July 1876 . His family were enthusiastic cricketers , although the region had little history within the sport , and his two younger brothers Richard and Helon went on to represent the West Indies in first-class cricket . Initially , Ollivierre playe</t>
+          <t>Reptar on Ice = " Reptar on Ice " is the tenth episode of the second season of the animated television series Rugrats . It is the first segment of the twenty-third episode for the entire series . The episode was written by Peter Gaffney and directed by Howard E. Baker . It was originally broadcast on November 8 , 1992 . " Reptar on Ice " followed the infant main characters , Tommy , Chuckie , Phil , and Lil going to an ice show with their parents that follows the love story of the babies ' favorite monster , Reptar . There , the babies attempt to return a lizard to the actor , assuming it is his child . " Reptar on Ice " continued Rugrats ' employment of the character Reptar , a satirical parody of Godzilla . The episode included several other cultural references ; the basic theme lampoons the commercialization of children 's media products and its plethora of merchandise tie-ins . The ice show the children see is referent to real-life ice shows , such as " Disney on Ice , " and its pl</t>
         </is>
       </c>
     </row>
@@ -1386,32 +1386,32 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>['highway', 'north', 'road', 'east', 'route', 'lane', 'south', 'intersection', 'west', 'continues', 'interchange', 'designated', 'completed', 'state', 'passes']</t>
+          <t>['formula', 'matrix', 'function', 'newton', 'linear', 'plants', 'constant', 'language', 'defined', 'theory', 'functions', 'example', 'consciousness', 'space', 'derivative']</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Maryland Route 23 = Maryland Route 23 ( MD 23 ) is a state highway in the U.S. state of Maryland . The state highway runs 20.58 miles ( 33.12 km ) from U.S. Route 1 ( US 1 ) in Hickory north and west to the Pennsylvania state line near Norrisville , where the highway continues as Pennsylvania Route 24 ( PA 24 ) . MD 23 is an L-shaped highway in northwestern Harford County that consists of two major sections . Between US 1 and MD 165 in Jarrettsville , MD 23 is marked east – west along a two-lane controlled access road named East – West Highway . From MD 165 to the state line , the state highway is marked north – south along Norrisville Road , a rural two-lane highway that passes through the villages of Madonna and Shawsville . The two sections of MD 23 are connected by a short concurrency with MD 165 . MD 23 from Hickory to Jarrettsville was one of the original state highways marked for improvement by the Maryland State Roads Commission in 1909 and one of the original state-numbered hi</t>
+          <t>Biology = Biology is a natural science concerned with the study of life and living organisms , including their structure , function , growth , evolution , distribution , identification and taxonomy . Modern biology is a vast and eclectic field , composed of many branches and subdisciplines . However , despite the broad scope of biology , there are certain general and unifying concepts within it that govern all study and research , consolidating it into single , coherent field . In general , biology recognizes the cell as the basic unit of life , genes as the basic unit of heredity , and evolution as the engine that propels the synthesis and creation of new species . It is also understood today that all the organisms survive by consuming and transforming energy and by regulating their internal environment to maintain a stable and vital condition known as homeostasis . Sub-disciplines of biology are defined by the scale at which organisms are studied , the kinds of organisms studied , an</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Business routes of Interstate 96 = There have been six business routes of Interstate 96 ( I-96 ) in the US state of Michigan . There are two business loops designated Business Loop Interstate 96 ( BL I-96 ) : one through Lansing and one through Howell . Both follow the old route of US Highway 16 ( US 16 ) , with appropriate connections to I-96 . There are three former business spurs that were designated Business Spur Interstate 96 ( BS I-96 ) . One connected to the carferry docks in Muskegon , running concurrently with part of Business US 31 ( Bus . US 31 ) along former US 16 , but it has been eliminated . The second spur ran into downtown Portland until it was decommissioned in 2007 . Two routes in the Detroit area — a loop through Farmington and a spur into Detroit — both using Grand River Avenue , and meeting at the temporary end of I-96 near Purdue Avenue , were eliminated when I-96 was moved to the completed Jeffries Freeway in 1977 . These Detroit-area business routes are still s</t>
+          <t>Myco-heterotrophy = Myco-heterotrophy ( Greek : μυκός mykós , " fungus " , ἕτερος heteros = " another " , " different " and τροφή trophe = " nutrition " ) is a symbiotic relationship between certain kinds of plants and fungi , in which the plant gets all or part of its food from parasitism upon fungi rather than from photosynthesis . A myco-heterotroph is the parasitic plant partner in this relationship . Myco-heterotrophy is considered a kind of cheating relationship and myco-heterotrophs are sometimes informally referred to as " mycorrhizal cheaters " . This relationship is sometimes referred to as mycotrophy , though this term is also used for plants that engage in mutualistic mycorrhizal relationships . = = Relationship between myco-heterotrophs and host fungi = = Full ( or obligate ) myco-heterotrophy exists when a non-photosynthetic plant ( a plant largely lacking in chlorophyll or otherwise lacking a functional photosystem ) gets all of its food from the fungi that it parasitize</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Interstate 70 in Maryland = Interstate 70 ( I-70 ) is a part of the Interstate Highway System that runs from Cove Fort , Utah to Baltimore , Maryland . In Maryland , the Interstate Highway runs 93.62 miles ( 150.67 km ) from the Pennsylvania state line in Hancock east to the Interstate 's eastern terminus near its junction with I-695 at a park and ride in Baltimore . I-70 is the primary east – west Interstate in Maryland ; the Interstate Highway connects Baltimore — and Washington via I-270 — with Western Maryland . The Interstate serves Frederick and Hagerstown directly and provides access to Cumberland via its junction with I-68 at Hancock . I-70 runs concurrently with its predecessor highway , U.S. Route 40 ( US 40 ) , from Hancock to Indian Springs in Washington County and from Frederick to West Friendship in Howard County . I-70 's route from Frederick to West Friendship was constructed as a divided highway relocation of US 40 in the early to mid-1950s and a freeway bypass of Fred</t>
+          <t>Philosophy of science = Philosophy of science is a branch of philosophy concerned with the foundations , methods , and implications of science . The central questions of this study concern what qualifies as science , the reliability of scientific theories , and the ultimate purpose of science . This discipline overlaps with metaphysics , ontology , and epistemology , for example , when it explores the relationship between science and truth . There is no consensus among philosophers about many of the central problems concerned with the philosophy of science , including whether science can reveal the truth about unobservable things and whether scientific reasoning can be justified at all . In addition to these general questions about science as a whole , philosophers of science consider problems that apply to particular sciences ( such as biology or physics ) . Some philosophers of science also use contemporary results in science to reach conclusions about philosophy itself . While philo</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Maryland Route 404 = Maryland Route 404 ( MD 404 ) is a major highway on Maryland 's Eastern Shore in the United States . It runs 24.61 miles ( 39.61 km ) from MD 662 in Wye Mills on the border of Queen Anne 's and Talbot counties , southeast to the Delaware state line in Caroline County , where the road continues as Delaware Route 404 ( DE 404 ) to Nassau ( near Rehoboth Beach ) . The Maryland and Delaware state highways together cross the width of the Delmarva Peninsula and serve to connect the cities west of the Chesapeake Bay by way of the Chesapeake Bay Bridge and U.S. Route 50 ( US 50 ) with the Delaware Beaches . Along the way , MD 404 passes through mostly farmland and woodland as well as the towns of Queen Anne , Hillsboro , and Denton . The road is a two-lane undivided highway for most of its length with the exception of the bypass around Denton and a section near Hillsboro , which is a four-lane divided highway . MD 404 was designated by 1933 to run from Matapeake ( where th</t>
+          <t>Ecology = Ecology ( from Greek : οἶκος , " house " , or " environment " ; -λογία , " study of " ) is the scientific analysis and study of interactions among organisms and their environment . It is an interdisciplinary field that includes biology , geography , and Earth science . Ecology includes the study of interactions organisms have with each other , other organisms , and with abiotic components of their environment . Topics of interest to ecologists include the diversity , distribution , amount ( biomass ) , and number ( population ) of particular organisms , as well as cooperation and competition between organisms , both within and among ecosystems . Ecosystems are composed of dynamically interacting parts including organisms , the communities they make up , and the non-living components of their environment . Ecosystem processes , such as primary production , pedogenesis , nutrient cycling , and various niche construction activities , regulate the flux of energy and matter throug</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Business routes of Interstate 69 in Michigan = There are currently four business routes of Interstate 69 ( I-69 ) in the US state of Michigan . Designated Business Loop Interstate 69 ( BL I-69 ) , they are all former routings of I-69 's predecessor highways , US Highway 27 ( US 27 ) , M-78 or M-21 , in whole or in part . The BL I-69 in Coldwater and the one in Charlotte were both parts of US 27 before the freeway bypassed those two cities in 1967 and the early 1970s , respectively . The BL I-69 through Lansing and East Lansing was previously part of M-78 and Temporary I-69 until it was redesignated in 1987 . Before 1984 , the loop in Port Huron was originally part of M-21 and was initially a business spur numbered Business Spur Interstate 69 ( BS I-69 ) . It was later redesignated when it was extended to run concurrently with that city 's BL I-94 which was originally part of I-94 's predecessor , US 25 . Each business loop follows streets through each city 's downtown areas and connect</t>
+          <t xml:space="preserve">Force = In physics , a force is any interaction that , when unopposed , will change the motion of an object . In other words , a force can cause an object with mass to change its velocity ( which includes to begin moving from a state of rest ) , i.e. , to accelerate . Force can also be described by intuitive concepts such as a push or a pull . A force has both magnitude and direction , making it a vector quantity . It is measured in the SI unit of newtons and represented by the symbol F. The original form of Newton 's second law states that the net force acting upon an object is equal to the rate at which its momentum changes with time . If the mass of the object is constant , this law implies that the acceleration of an object is directly proportional to the net force acting on the object , is in the direction of the net force , and is inversely proportional to the mass of the object Related concepts to force include : thrust , which increases the velocity of an object ; drag , which </t>
         </is>
       </c>
     </row>
@@ -1421,32 +1421,32 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>['game', 'team', 'play', 'season', 'second', 'defense', 'kick', 'led', 'lead', 'week', 'half', 'record', 'end', 'football', 'field']</t>
+          <t>['glee', 'kurt', 'rachel', 'meredith', 'finn', 'episode', 'grey', 'quinn', 'anatomy', 'viewers', 'sue', 'watched', 'yang', 'club', 'grace']</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2012 Alabama Crimson Tide football team = The 2012 Alabama Crimson Tide football team ( variously " Alabama " , " UA " , " Bama " or " The Tide " ) represented the University of Alabama in the 2012 National Collegiate Athletic Association ( NCAA ) Division I Football Bowl Subdivision ( FBS ) football season . It marked the Crimson Tide 's 118th overall season of playing college football , 79th as a member of the Southeastern Conference ( SEC ) and 21st within the SEC Western Division . The team was led by head coach Nick Saban , in his sixth year , and played its home games at Bryant – Denny Stadium in Tuscaloosa , Alabama . They finished the season with a record of 13 wins and 1 loss ( 13 – 1 overall , 7 – 1 in the SEC ) , as SEC champions and as consensus national champions after they defeated Notre Dame in the Bowl Championship Series ( BCS ) National Championship Game . After they captured the 2011 national championship , the Crimson Tide signed a highly rated recruiting class in F</t>
+          <t xml:space="preserve">Ballad ( Glee ) = " Ballad " is the tenth episode of the American television series Glee . The episode premiered on the Fox network on November 18 , 2009 , and was written and directed by series creator Brad Falchuk . " Ballad " sees the glee club split into pairs to sing ballads to one another . Rachel ( Lea Michele ) is paired with club director Will ( Matthew Morrison ) and develops a crush on him . Quinn 's ( Dianna Agron ) parents learn that Quinn is pregnant , and she moves in with Finn ( Cory Monteith ) and his mother when her own parents evict her . Gregg Henry and Charlotte Ross guest-star as Quinn 's parents Russell and Judy Fabray , and Sarah Drew appears as Suzy Pepper , a student with a former crush on Will . Romy Rosemont returns as Finn 's mother , Carole Hudson . The episode features covers of seven songs , including a mash-up of " Don 't Stand So Close to Me " by The Police and " Young Girl " by Gary Puckett and The Union Gap . Studio recordings of all songs performed </t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2010 Alabama Crimson Tide football team = The 2010 Alabama Crimson Tide football team ( variously " Alabama " , " UA " , " Bama " or " The Tide " ) represented the University of Alabama in the 2010 NCAA Division I FBS football season . It was the Crimson Tide 's 116th overall season , 77th as a member of the Southeastern Conference ( SEC ) and its 19th within the SEC Western Division . The team was led by head coach Nick Saban , in his fourth year , and played their home games at Bryant – Denny Stadium in Tuscaloosa , Alabama . They finished the season with a record of ten wins and three losses ( 10 – 3 , 5 – 3 in the SEC ) and defeated Michigan State 49 – 7 in the Capital One Bowl . Alabama entered the season as defending national champions , and began the 2010 season as the preseason number one team in both the AP and Coaches ' Polls . Favored to win a second consecutive SEC championship and be in contention for the national championship , the Crimson Tide opened the season with five</t>
+          <t>The Rhodes Not Taken = " The Rhodes Not Taken " is the fifth episode of the American television series Glee . It premiered on the Fox network on September 30 , 2009 and was written by series co-creator Ian Brennan and directed by John Scott . The episode features glee club director Will Schuester ( Matthew Morrison ) recruiting former star April Rhodes ( Kristin Chenoweth ) , hoping to improve the club 's chances in the wake of Rachel 's ( Lea Michele ) defection to the school musical . Finn ( Cory Monteith ) flirts with Rachel in an attempt to convince her to return , and although Rachel is angry when she discovers Finn 's girlfriend is pregnant , she ultimately rejoins the club . Special guest star Kristin Chenoweth played April , and performed on three of the episode 's six musical tracks . Studio recordings of four of the songs performed in the episode were released as singles , available for digital download , and two appear on the album Glee : The Music , Volume 1 . The episode w</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1995 Sugar Bowl ( December ) = The 1995 Sugar Bowl was the 62nd edition of the post-season American college football Sugar Bowl bowl game . It featured the Virginia Tech Hokies and the Texas Longhorns and was held at the Louisiana Superdome in New Orleans , Louisiana on December 31 , 1995 . The game was the final contest of the 1995 NCAA Division I-A football season for both teams , and ended in a 28 – 10 victory for Virginia Tech . In 1995 , the Sugar Bowl was held under the rules of the Bowl Alliance . The Alliance , predecessor to the modern Bowl Championship Series , was intended to match the champions of the Southeastern Conference , Big East Conference , Atlantic Coast Conference , Big 12 , Southwest Conference , and one at-large team against each other in the Sugar Bowl , Orange Bowl , and Fiesta Bowl . Each year , the two highest-ranked teams would play in a National Championship Game held in place of one of the bowl games . The site of the national championship game rotated am</t>
+          <t>Get It Right ( Glee cast song ) = " Get It Right " is a song performed by the cast of American television series Glee , taken from their sixth soundtrack album , Glee : The Music , Volume 5 . It is sung by Lea Michele who portrays the series ' lead character , Rachel Berry . The song was written by the series ' music producer Adam Anders , who created the song with his wife Nikki Hassman , and writing partner Peer Åström . Anders and company wrote the song specifically for Michele , and based the lyrics on the storyline of Rachel . The song was released with a number of Glee songs on the iTunes Store on March 15 , 2011 . Musically , " Get It Right " is a piano-driven pop ballad , with mild country influences . According to MTV 's Aly Semigran , the song has similarities to Britney Spears ' Everytime " ( 2004 ) . While critics praised Michele 's vocals in the song , they were not as receptive to the song itself with it being coined as " dull " and " boring . " The lyrics of the song rev</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t xml:space="preserve">2009 Alabama Crimson Tide football team = The 2009 Alabama Crimson Tide football team ( variously " Alabama " , " UA " , " Bama " or " The Tide " ) represented the University of Alabama in the 2009 NCAA Division I FBS football season . It was the Crimson Tide 's 115th overall season , 76th season as a member of the Southeastern Conference ( SEC ) and its 18th within the SEC Western Division . The team was led by head coach Nick Saban , in his third year , and played their home games at Bryant – Denny Stadium in Tuscaloosa , Alabama . They finished the season undefeated with a record of 14 – 0 ( 8 – 0 in the SEC ) and as national champions . Looking to build on the successes of the 2008 campaign , Alabama entered the 2009 season as the favorite to win the Western Division and meet the Florida Gators in the 2009 SEC Championship Game . Alabama closed the regular season with a 12 – 0 record including four wins against Top 25-ranked teams — and met the Gators for the SEC Championship in a </t>
+          <t xml:space="preserve">Journey to Regionals = " Journey to Regionals " is the twenty-second episode and first season finale of the American television series Glee . The episode was written and directed by series creator Brad Falchuk , and premiered on the Fox network on June 8 , 2010 . In " Journey to Regionals " , New Directions performs at Regionals in front of celebrity judges Josh Groban , Olivia Newton-John , Rod Remington ( Bill A. Jones ) and Sue Sylvester ( Jane Lynch ) . Club member Quinn ( Dianna Agron ) gives birth to her daughter , Beth , whom rival glee club coach Shelby Corcoran ( Idina Menzel ) adopts . Co-captains Finn ( Cory Monteith ) and Rachel ( Lea Michele ) reunite , and director Will Schuester ( Matthew Morrison ) professes his love for guidance counselor Emma Pillsbury ( Jayma Mays ) . Although New Directions comes in last in the competition , Sue persuades Principal Figgins ( Iqbal Theba ) not to disband the club for another year . The episode features cover versions of nine songs , </t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2011 Alabama Crimson Tide football team = The 2011 Alabama Crimson Tide football team ( variously " Alabama " , " UA " , " Bama " or " The Tide " ) represented the University of Alabama in the 2011 NCAA Division I FBS football season . It was the Crimson Tide 's 117th overall and 78th season as a member of the Southeastern Conference ( SEC ) and its 20th within the SEC Western Division . The team was led by head coach Nick Saban , in his fifth year , and played their home games at Bryant – Denny Stadium in Tuscaloosa , Alabama . They finished the season with a record of twelve wins and one loss ( 12 – 1 overall , 7 – 1 in the SEC ) and as consensus national champions . After the completion of the 2010 season , the Crimson Tide signed a highly rated recruiting class in February 2011 and completed spring practice the following April . With seventeen returning starters from the previous season , Alabama entered their 2011 campaign ranked as the number two team in the nation and as a favor</t>
+          <t>Throwdown ( Glee ) = " Throwdown " is the seventh episode of the American television series Glee . The episode premiered on the Fox network on October 14 , 2009 . It was directed by series creator Ryan Murphy and written by Brad Falchuk . The episode includes a clash between glee club director Will Schuester ( Matthew Morrison ) and cheerleading coach Sue Sylvester ( Jane Lynch ) when she is named co-director of the glee club . As Sue tries to divide the club by turning the students against Will , his wife Terri ( Jessalyn Gilsig ) blackmails her OB / GYN into colluding with her over her fake pregnancy . The episode features covers of five songs . Studio recordings of four of the songs performed were released as singles , available for digital download , and were also included on the album Glee : The Music , Volume 1 . " Throwdown " was watched by 7.65 million US viewers and received mixed reviews from critics . The pregnancy storyline was criticized by both Ken Tucker of Entertainment</t>
         </is>
       </c>
     </row>
@@ -1456,32 +1456,32 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>['second', 'place', 'position', 'race', 'track', 'car', 'lead', 'fifth', 'fourth', 'sixth', 'pole', 'passed', 'championship', 'ferrari', 'stop']</t>
+          <t>['bach', 'poem', 'poems', 'shakespeare', 'poet', 'poetry', 'movement', 'ode', 'movements', 'soprano', 'text', 'alto', 'aria', 'stanza', 'narrator']</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2015 Italian Grand Prix = The 2015 Italian Grand Prix ( formally known as the Formula 1 Gran Premio d 'Italia 2015 ) was a Formula One motor race held on 6 September 2015 at the Autodromo Nazionale Monza in Monza , Italy . The race was the twelfth round of the 2015 season , and marked the eighty-fifth running of the Italian Grand Prix . Lewis Hamilton of Mercedes was the defending race winner , and entered with a 28-point lead over teammate Nico Rosberg in the Drivers ' Championship , with Sebastian Vettel a further 39 points behind . Mercedes lead the Constructors ' Championship by 184 points over Ferrari , with Williams a further 81 points behind in third . Hamilton completed the second Grand Slam of his career by winning the race , taking pole position , setting the fastest lap and leading every lap of the race . He finished 25 seconds ahead of Vettel , while Felipe Massa finished third for Williams . Rosberg retired with three laps to go due to an engine failure , resulting in Hami</t>
+          <t xml:space="preserve">Der Herr ist mein getreuer Hirt , BWV 112 = Der Herr ist mein getreuer Hirt ( The Lord is my faithful Shepherd ) , BWV 112 , is a cantata by Johann Sebastian Bach , a church cantata for the second Sunday after Easter . Bach composed the chorale cantata in Leipzig and first performed it on 8 April 1731 . It is based on the hymn by Wolfgang Meuslin , a paraphrase of Psalm 23 written in 1530 , sung to a melody by Nikolaus Decius . Bach , the Thomaskantor in Leipzig from May 1723 , composed this cantata to complete his second cantata cycle of chorale cantatas , begun in 1724 . He used the lyrics of the hymn unchanged , which reflect the psalm and Jesus as the Good Shepherd . Bach structured the work in five movements . The outer choral movements are a chorale fantasia and a four-part closing chorale , both on the hymn tune . Bach set the inner stanzas as aria – recitative – aria , with music unrelated to the hymn tune . He scored the cantata for four vocal soloists , a four-part choir and </t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t xml:space="preserve">2011 Canadian Grand Prix = The 2011 Canadian Grand Prix ( formally the Formula 1 Grand Prix du Canada ) was a Formula One motor race held on 12 June 2011 at the Circuit Gilles Villeneuve , in Montreal , Canada . It was the seventh race of the 2011 Formula One season and the 48th Canadian Grand Prix . The 70-lap race was won by McLaren driver Jenson Button after starting from seventh position . Sebastian Vettel , who started from pole position , finished second in a Red Bull with teammate Mark Webber finishing third . The race began behind the safety car , and once it returned to the pits Vettel built a lead over Fernando Alonso . A second safety car deployment caused by the collision of Button and teammate Lewis Hamilton closed the time gaps between cars , but Vettel retained the lead . By lap 26 , increasingly heavy rain led to the race 's suspension , before it was restarted over two hours later . Button was involved in another collision on lap 37 , which led to Alonso 's retirement </t>
+          <t>Lobe den Herrn , meine Seele , BWV 143 = Lobe den Herrn , meine Seele ( Praise the Lord , my soul ) , BWV 143 , is an early cantata by Johann Sebastian Bach . It is not known if he composed the cantata for New Year 's Day in Mühlhausen or Weimar , as the date of composition is unclear . An unknown librettist drew mainly from Psalm 146 and from Jakob Ebert 's hymn " Du Friedefürst , Herr Jesu Christ " to develop seven movements , supplying only two of the movements himself . The text assembly is similar to Bach 's early cantatas . Bach 's authorship is doubted because the cantata has several features unusual for Bach 's later cantatas : it is the only Bach cantata to combine three corni da caccia with timpani . The cantata is in seven movements which combine the three major text sources : psalm , hymn and contemporary poetry . The opening chorus is based on a psalm verse , followed by the first hymn stanza and another psalm verse as a recitative . An aria on poetry is followed by a thir</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2015 Spanish Grand Prix = The 2015 Spanish Grand Prix , formally titled the Formula 1 Gran Premio de España Pirelli 2015 , was a Formula One motor race held on 10 May 2015 at the Circuit de Barcelona-Catalunya in Montmeló , Spain . The race was the fifth round of the 2015 season and marked the forty-fifth running of the Spanish Grand Prix as a round of the Formula One World Championship and the twenty-fifth running at Catalunya . Mercedes driver Nico Rosberg took his first win of the season , his first in Spain and the ninth of his career . His team-mate Lewis Hamilton finished second after a bad start , followed by Sebastian Vettel in third . = = Report = = = = = Background = = = Mercedes were expected to be dominant in Barcelona , since it was at the circuit that their advantage per lap had been biggest in 2014 and they had shown strong form at the two pre-season tests at the circuit . After problems with their engine in the first races , which saw Daniel Ricciardo down to his last p</t>
+          <t>Unser Mund sei voll Lachens , BWV 110 = Unser Mund sei voll Lachens ( May our mouth be full of laughter ) , BWV 110 , is a church cantata by Johann Sebastian Bach . He composed the Christmas cantata in Leipzig for Christmas Day and first performed it on 25 December 1725 . Bach composed the cantata in his third year as Thomaskantor in Leipzig . He used a text by Georg Christian Lehms , which was published already in 1711 . The text has no recitatives alternating with arias , but instead three biblical quotations , opening with verses from Psalm 26 , then a verse from the Book of Jeremiah about God 's greatness , and finally the angels ' song from the Nativity according to the Gospel of Luke . The closing chorale is taken from Caspar Füger 's " Wir Christenleut " . Bach scored the work festively for four vocal soloists , a four-part choir and a Baroque instrumental ensemble of trumpets and timpani , transverse flutes , different kinds of oboe , strings and basso continuo including bassoo</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2012 Formula One season = The 2012 Formula One season was the 63rd season of FIA Formula One motor racing . It featured the 2012 FIA Formula One World Championship , a motor racing series for Formula One cars , recognised by the Fédération Internationale de l 'Automobile ( FIA ) — the governing body of motorsport — as the highest class of competition for open-wheel racing cars . The championship was contested over twenty rounds , which started in Australia on 18 March and ended in Brazil on 25 November . The 2012 season saw the return of the United States Grand Prix , which was held at the Circuit of the Americas , a purpose-built circuit in Austin , Texas . After being cancelled in 2011 due to civil protests , the Bahrain Grand Prix also returned to the calendar . The early season was tumultuous , with seven different drivers winning the first seven races of the championship ; a record for the series . It was not until the European Grand Prix in June that a driver , Ferrari 's Fernand</t>
+          <t>Du Friedefürst , Herr Jesu Christ , BWV 116 = Du Friedefürst , Herr Jesu Christ ( You Prince of Peace , Lord Jesus Christ ) , BWV 116 , is a church cantata written by Johann Sebastian Bach in 1724 in Leipzig for the 25th Sunday after Trinity . He led the first performance it on 26 November 1724 , concluding the liturgical year of 1724 . The cantata is based upon Jakob Ebert 's hymn " Du Friedefürst , Herr Jesu Christ " . It matches the Sunday 's prescribed gospel reading , the Tribulation from the Gospel of Matthew , in a general way . The hymn 's first and last stanza are used unchanged in both text and tune : the former is set as a chorale fantasia , the latter as a four-part closing chorale . An unknown librettist paraphrased the inner stanzas as alternating arias and recitatives . Bach scored the cantata for four vocal soloists ( soprano , alto , tenor , bass ) , a four-part choir and a Baroque instrumental ensemble of natural horn , enforcing the soprano in the hymn tune , two obo</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2015 Bahrain Grand Prix = The 2015 Bahrain Grand Prix ( formally known as the 2015 Formula 1 Gulf Air Bahrain Grand Prix ) was a Formula One motor race that was held on 19 April 2015 at the Bahrain International Circuit in Sakhir , Bahrain . The race was the fourth round of the 2015 season and marked the eleventh time that the Bahrain Grand Prix has been run as a round of the Formula One World Championship . Lewis Hamilton , who was the defending race winner , came into the race with a 13-point lead over Sebastian Vettel after his victory a week prior in China . He took the 42nd pole position of his career during Saturday 's qualifying , and his fourth in a row . In the race , Hamilton managed to win from Kimi Räikkönen and Nico Rosberg , taking his 36th race victory . = = Report = = = = = Background = = = There were tensions in the Mercedes team prior to the Grand Prix . After the Chinese Grand Prix the week before , Nico Rosberg had accused his teammate Lewis Hamilton of deliberately</t>
+          <t>Es ist das Heil uns kommen her , BWV 9 = Es ist das Heil uns kommen her ( It is our salvation come here to us ) , BWV 9 , is a church cantata by Johann Sebastian Bach . He composed the chorale cantata in Leipzig for the sixth Sunday after Trinity between 1732 and 1735 , based on the hymn " Es ist das Heil uns kommen her " by Paul Speratus . Bach composed the cantata to fill a gap in his cycle of chorale cantatas written for performances in Leipzig from 1724 . The cantata is structured in seven movements , framed as the earlier chorale cantatas by a chorale fantasia and a chorale four-part setting of the first and the twelfth stanza in the original words by the reformer Speratus , published in the First Lutheran Hymnal . The theme is salvation from sin by God 's grace alone . An anonymous librettist paraphrased the content of ten inner stanzas to alternating recitatives and arias . Bach scored the cantata for a chamber ensemble of four vocal parts , flauto traverso , oboe d 'amore , str</t>
         </is>
       </c>
     </row>
@@ -1491,32 +1491,32 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>['episode', 'viewers', 'glee', 'club', 'watched', 'relationship', 'finn', 'rating', 'rachel', 'character', 'tells', 'kurt', 'storyline', 'share', 'demographic']</t>
+          <t>['wickets', 'innings', 'test', 'cricket', 'wicket', 'runs', 'matches', 'australia', 'england', 'scored', 'bowling', 'match', 'bowled', 'overs', 'miller']</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>St. Valentine 's Day ( 30 Rock ) = " St. Valentine 's Day " is the eleventh episode of the third season , and forty-seventh episode overall , of the American television comedy series 30 Rock . It was written by co-executive producer Jack Burditt and series ' creator , executive producer and lead actress Tina Fey . The director of this episode was series producer Don Scardino . The episode originally aired on the National Broadcasting Company ( NBC ) in the United States on February 12 , 2009 . Guest stars in " St. Valentine 's Day " include Marylouise Burke , Jon Hamm , Salma Hayek , Zak Orth , Laila Robins , Maria Thayer , and Allie Trimm . In the episode , Liz Lemon ( Fey ) insists that she and Dr. Drew Baird ( Hamm ) have their first official date on Valentine 's Day , while Jack Donaghy ( Alec Baldwin ) prepares himself for an unconventional Valentine 's Day spent at church with his girlfriend Elisa ( Hayek ) . Finally , Tracy Jordan ( Tracy Morgan ) tries to help Kenneth Parcell (</t>
+          <t xml:space="preserve">Munir Malik = Munir Malik ( Urdu : منيرملک ; 10 July 1934 – 30 November 2012 ) was a Pakistani cricketer who played three Tests for Pakistan between 1959 and 1962 . A right-arm fast-medium bowler , he took nine wickets in Test cricket at an average of 39.77 , including a five-wicket haul against England . During his first-class career , he took 197 wickets at the average of 21.75 . = = First-class career = = Malik played 49 first-class matches for Karachi , Punjab , Rawalpindi and Services teams during 1956 – 66 . During his first-class career , he achieved five or more wickets in an innings on fourteen occasions , and ten or more wickets in a match four times . Malik made his first-class debut for Punjab B during the Quaid-e-Azam Trophy , against Bahawalpur in 1956 – 57 . He finished the season taking 13 wickets at an average of 8.30 . His 5 wickets for 19 runs for Punjab B , against Punjab , was his best performance in the season . Malik played three matches during 1957 – 58 and his </t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Grilled Cheesus = " Grilled Cheesus " is the third episode of the second season of the American television series Glee , and the twenty-fifth episode overall . It was written by Brad Falchuk , directed by Alfonso Gomez-Rejon , and premiered on the Fox network on October 5 , 2010 . Prior to its broadcast , series co-creator Ryan Murphy predicted the episode would be Glee 's most controversial , as it focuses on religion and what God means to the members of the glee club . When Burt Hummel ( Mike O 'Malley ) has a heart attack , the glee club rally around his son Kurt ( Chris Colfer ) , attempting to support the Hummels through their various faiths . Meanwhile , club co-captain Finn Hudson ( Cory Monteith ) believes he has found the face of Jesus in a grilled cheese sandwich . Murphy hoped to produce a balanced depiction of religion , and he , Falchuk and series co-creator Ian Brennan worked to ensure that there was an equality between pro and anti-religious sentiments expressed . The ep</t>
+          <t>1889 – 90 Currie Cup = The 1889 – 90 Currie Cup was the inaugural edition of the Currie Cup , the premier first-class cricket tournament in South Africa . The 1889 – 90 competition involved just two teams , Transvaal and Kimberley . The two sides played a single , three-day match , which was won by Transvaal by six wickets . Both sides made low scores in their first innings ; Kimberley , who had opted to bat first , were dismissed for 98 runs , and in their reply Transvaal reached 117 , a lead of just 19 runs . In the second innings , they both fared better ; a century from Bernard Tancred helped Kimberley to a total of 235 , but Transvaal reached their total in 38 five-ball overs , helped by a century from Monty Bowden . = = Background = = First-class cricket was first played in South Africa in the previous 1888 – 89 season , when Robert Warton managed a side which toured the country , playing against representative teams from each of the provinces , and two matches against South Afri</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Hell-O ( Glee ) = " Hell-O " is the fourteenth episode of the American television series Glee . The episode premiered on the Fox network on April 13 , 2010 . It was written by series creator Ian Brennan and directed by Brad Falchuk . In " Hell-O " , cheer-leading coach Sue Sylvester ( Jane Lynch ) attempts to sabotage the relationship between glee club members Finn Hudson ( Cory Monteith ) and Rachel Berry ( Lea Michele ) . Glee club director Will Schuester ( Matthew Morrison ) attempts to begin a relationship with school guidance counsellor Emma Pillsbury ( Jayma Mays ) , but several obstacles come between them , including the coach of rival glee club Vocal Adrenaline . " Hell-O " introduces special guest stars Idina Menzel as Shelby Corcoran , the coach of Vocal Adrenaline , and Jonathan Groff as Jesse St. James , the group 's lead singer . Glee fans had previously lobbied for Menzel to be cast as Rachel 's biological mother . The episode features cover versions of six songs , five o</t>
+          <t>Maurice Fernandes = Maurius Pacheco " Maurice " Fernandes , ( 12 August 1897 – 8 May 1981 ) was a West Indian Test cricketer who played first-class cricket for British Guiana between 1922 and 1932 . He made two Test appearances for the West Indies , in 1928 and 1930 . Fernandes played as a right-handed top-order batsman and occasional wicket-keeper . He scored 2,087 first-class runs in 46 appearances at an average of 28.20 . Graduating from playing at the Demerara Cricket Club as a teenager , to play for British Guiana in 1922 , Fernandes took part in tours of England in 1923 and 1928 . He made his debut Test appearance during the 1928 tour , playing in the first of the three Tests . His next , and final Test match came during the English tour of the West Indies in 1930 . At the time , the West Indies had a practice of picking their captain from the colony that the match was being played in , and Fernandes was granted the honour for the match in British Guiana . The West Indies won the</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Lovely ( Desperate Housewives ) = " Lovely " is the fifteenth episode of the sixth season of the American comedy-drama series , Desperate Housewives , and the 126th overall episode of the series . It originally aired on ABC in the United States on February 21 , 2010 . In the episode , former stripper Robin Gallagher ( Julie Benz ) interacts with each of the women of Wisteria Lane , drastically affecting their lives . She grows particularly close to Katherine Mayfair ( Dana Delany ) , with whom she shares a kiss during a bar outing . The episode was written by David Schladweiler and directed by David Warren . It included the second in a string of guest appearances by Benz , who had recently departed as a regular from the Showtime drama series , Dexter . " Lovely " introduced an ongoing storyline of Katherine exploring her sexuality , a subplot which was met with enthusiasm by actress Delany . The pairing between Robin and Katherine was the first lesbian relationship in Desperate Housewi</t>
+          <t>Haseeb Ahsan = Haseeb Ahsan ( Urdu : حسيب احسن ; 15 July 1939 – 8 March 2013 ) was a Pakistani cricketer who played 12 Tests for Pakistan between 1958 and 1962 . He was born in Peshawar , Khyber Pakhtunkhwa . A right-arm off spinner , he took 27 wickets in Test cricket at an average of 49.25 , including two five-wicket hauls . During his first-class career , he played 49 matches and took 142 wickets at an average of 27.71 . Former Pakistan cricketer Waqar Hasan said about him that he " was a fighter to the core and served Pakistan cricket with honour and dignity . " Ahsan had conflicts with former Pakistan captain Javed Burki . A controversy regarding his bowling action resulted in the premature end of his international career when he was only 23 . He worked as chief selector , team manager of Pakistan , and member of the 1987 Cricket World Cup organising committee . He died in Karachi on 8 March 2013 , aged 73 . = = Cricketing career = = Ahsan played 49 first-class matches for Pakista</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Don Geiss , America and Hope = " Don Geiss , America , and Hope " is the fifteenth episode of the fourth season of the American television comedy series 30 Rock , and the 73rd overall episode of the series . It was directed by Stephen Lee Davis , and written by Jack Burditt and Tracey Wigfield . The episode originally aired on the National Broadcasting Company ( NBC ) network in the United States on March 18 , 2010 . Guest stars in " Don Geiss , America and Hope " include John Anderson , Scott Bryce , Marceline Hugot , James Rebhorn , and Michael Sheen . In the episode , Liz Lemon ( Tina Fey ) attempts to avoid running into Wesley Snipes ( Sheen ) after they fail to hit it off in their first encounter , but fate seems to want them together . At the same time , Jack Donaghy ( Alec Baldwin ) deals with the impending purchase of NBC . Finally , Tracy Jordan ( Tracy Morgan ) does damage control after his former nanny publishes a tell-all book . The episode continued a story arc involving W</t>
+          <t>Steph Davies = Stephanie Ann Davies , commonly known as Steph Davies , ( born 21 October 1987 ) is an international cricketer who has represented the England women 's cricket team in four One Day Internationals ( ODIs ) . A right-arm medium-fast bowler and right-handed attacking batsman , she has played for Somerset women since 2001 . After making her county debut for Somerset at the age of 13 , Davies quickly progressed into the England development and youth sides . She toured Australia with England Under-19s aged 15 and after two successful European tournaments , she captained the England Under-21s to victory in the 2006 Under-21 European Championships . After more matches for the development squad , and a number of tour matches for England , she made her ODI debut during the 2007 – 08 tour of Australia and New Zealand , playing the fifth and final one-day match against Australia , and three of the five matches against New Zealand . Following this , she continued to be involved in th</t>
         </is>
       </c>
     </row>
@@ -1526,32 +1526,32 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>['time', 'year', 'world', 'won', 'games', 'record', 'team', 'years', 'title', 'season', 'final', 'second', 'player', 'win', 'best']</t>
+          <t>['hitler', 'holocaust', 'physics', 'jews', 'nazi', 'nuclear', 'germany', 'manhattan_project', 'atomic', 'berlin', 'jewish', 'nobel', 'german', 'munich', 'research']</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Big Four ( tennis ) = In tennis , the term Big Four refers to the quartet of men 's singles players Roger Federer , Rafael Nadal , Novak Djokovic , and Andy Murray . They reigned as the four best players in the world every season from 2008 – 2016 . These players were considered dominant in terms of ranking and tournament victories , including Grand Slam tournaments and ATP Masters 1000 events , as well as the ATP World Tour Finals and Olympic Games . Federer was the first to come to prominence after winning Wimbledon in 2003 and established himself as the world No. 1 by the beginning of 2004 . Nadal followed in 2005 after a French Open triumph including a win over Federer , and they occupied the top two places in the ATP rankings for 211 consecutive weeks from July 2005 to August 2009 . Djokovic , from 2007 , and later Murray , from 2009 , increasingly challenged Federer 's and Nadal 's dominance with seasonal consistency : Djokovic captured three of the four major tournaments in 2011 </t>
+          <t>Henry DeWolf Smyth = Henry DeWolf " Harry " Smyth ( / ˈhɛnri dəˈwʊlf ˈsmaɪθ / ; May 1 , 1898 – September 11 , 1986 ) was an American physicist , diplomat , and bureaucrat . He played a number of key roles in the early development of nuclear energy , as a participant in the Manhattan Project , a member of the U.S. Atomic Energy Commission ( AEC ) , and U.S. ambassador to the International Atomic Energy Agency ( IAEA ) . Educated at Princeton University and the University of Cambridge , he was a faculty member in Princeton 's Department of Physics from 1924 to 1966 . He chaired the department from 1935 to 1949 . His early research was on the ionization of gases , but his interests shifted toward nuclear physics beginning in the mid-1930s . During World War II he was a member of the National Defense Research Committee 's Uranium Section and a consultant on the Manhattan Project . He wrote the Manhattan Project 's first public official history , which came to be known as the Smyth Report .</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Egypt at the 2012 Summer Olympics = Egypt competed at the 2012 Summer Olympics in London , from 27 July to 12 August 2012 , sending one of its largest delegations ever . A total of 110 Egyptian athletes participated in 83 events across 20 sports , with more women taking part than ever before . The nation 's flagbearer in the opening ceremonies was Hesham Mesbah , a judoka who was its only medalist from the 2008 Summer Olympics . Egypt won two medals in London : Alaaeldin Abouelkassem earned silver in the men 's foil , becoming the first competitor from an African nation to win a fencing medal , while Karam Gaber captured silver in the men 's 84 kg Greco-Roman wrestling event . Among other achievements , Mostafa Mansour was the nation 's first competitor in sprint canoeing while fencer Shaimaa El-Gammal became the first Egyptian female to appear in four editions of the Olympics . Prior to 2012 , Egypt had sent athletes to nineteen editions of the Summer Olympic Games , the 1906 Intercal</t>
+          <t xml:space="preserve">Julius Schreck = Julius Schreck ( 13 July 1898 – 16 May 1936 ) was a senior Nazi official and close confidant of Adolf Hitler . Born on 13 July 1898 in Munich , Schreck served in World War I and shortly afterwards joined right-wing paramilitary units . He joined the Nazi Party in 1920 and developed a close friendship with Adolf Hitler . Schreck was a founding member of the Sturmabteilung ( " Storm Department " ; SA ) and was active in its development . Later in 1925 , he became the first leader of the Schutzstaffel ( " Protection Squadron " ; SS ) . He then served for a time as a chauffeur for Hitler . Schreck developed meningitis in 1936 and died on 16 May . Hitler gave him a state funeral which was attended by several members of the Nazi elite with Hitler delivering the eulogy . = = Early life = = Julius Schreck was born on 13 July 1898 in Munich , a largely Catholic city in Bavaria . He served in the German Army during World War I. After the war ended in November 1918 , he became a </t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Roger Federer = Roger Federer ( German : [ ˈfeːdərər ] born 8 August 1981 ) is a Swiss professional tennis player who is currently ranked world No. 3 by the Association of Tennis Professionals ( ATP ) . His accomplishments in professional tennis have led to him being regarded by many as the greatest tennis player of all time . Federer turned professional in 1998 and has been continuously ranked in the top 10 since October 2002 . Federer holds several records of the Open Era : holding the world No. 1 position for 302 weeks ( including 237 consecutive weeks ) ; winning 17 Grand Slam singles titles ; reaching each Grand Slam final at least five times ( an all-time record ) ; and reaching the Wimbledon final ten times . He is among the eight men ( and among the five in Open Era ) to capture a career Grand Slam . Federer shares an Open Era record for most titles at Wimbledon with Pete Sampras ( seven ) and at the US Open with Jimmy Connors and Sampras ( five ) . He is the only male player t</t>
+          <t>Robert Brode = Robert Bigham Brode ( June 12 , 1900 – February 19 , 1986 ) was an American physicist , who during World War II led the group at the Manhattan Project 's Los Alamos laboratory that developed the fuses used in the atomic bombing of Hiroshima and Nagasaki . A graduate of the California Institute of Technology , where he earned his doctorate in 1924 , Brode attended Oxford University on a Rhodes Scholarship and the University of Göttingen on a National Research Council Fellowship . During World War II , Brode worked at Applied Physics Laboratory at Johns Hopkins University , where he helped develop the proximity fuse , and then as a group leader at the Los Alamos Laboratory . In 1950 he was one of a dozen prominent scientists who petitioned President Harry S. Truman to declare that the United States would never be the first to use the hydrogen bomb . After the war , Brode returned to teaching at Berkeley . Between 1930 and 1957 he supervised 37 graduate students . In additi</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Svetlana Kuznetsova = Svetlana Aleksandrovna Kuznetsova ( Russian : Светла ́ на Алекса ́ ндровна Кузнецо ́ ва ; IPA : [ svʲɪtˈlanə ɐlʲɪkˈsandrəvnə kʊznʲɪˈtsovə ] ; born 27 June 1985 ) is a Russian professional tennis player . Kuznetsova has appeared in four Grand Slam singles finals , winning two , and has also appeared in seven doubles finals , winning twice . As a doubles player , Kuznetsova has reached the finals of each Grand Slam at least once , winning the Australian Open twice . She has qualified five times for the round-robin stage of the WTA Tour Championships but has never reached the semifinals . Born to an athletic family , Kuznetsova moved at the age of seven to Spain to attend the Sanchez-Casal Academy . In 2001 she first took part on a WTA tournament , the Madrid Open , and a year later won her first WTA title at the Nordea Nordic Light Open in Helsinki , Finland . Her first appearance in a Grand Slam was at the 2002 Australian Open and her first Grand Slam title came at</t>
+          <t>Adolf Hitler = Adolf Hitler ( German : [ ˈadɔlf ˈhɪtlɐ ] ; 20 April 1889 – 30 April 1945 ) was a German politician who was the leader of the Nazi Party ( Nationalsozialistische Deutsche Arbeiterpartei ; NSDAP ) , Chancellor of Germany from 1933 to 1945 , and Führer ( " leader " ) of Nazi Germany from 1934 to 1945 . As dictator of Nazi Germany , he initiated World War II in Europe with the invasion of Poland in September 1939 and was a central figure of the Holocaust . Hitler was born in Austria , then part of Austria-Hungary , and raised near Linz . He moved to Germany in 1913 and was decorated during his service in the German Army in World War I. He joined the German Workers ' Party , the precursor of the NSDAP , in 1919 and became leader of the NSDAP in 1921 . In 1923 , he attempted a coup in Munich to seize power . The failed coup resulted in Hitler 's imprisonment , during which time he dictated the first volume of his autobiography and political manifesto Mein Kampf ( " My Struggl</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Federer – Nadal rivalry = The Federer – Nadal rivalry ( known by many as Fedal ) is between two professional tennis players , Roger Federer of Switzerland and Rafael Nadal of Spain . They are currently engaged in a storied rivalry , which many consider to be the greatest in tennis history . They have played 34 times , most recently in the 2015 Swiss Indoors final , and Nadal leads their twelve-year-old rivalry with an overall record of 23 – 11 . Federer and Nadal are the only pair of men to have finished six consecutive calendar years as the top two ranked players on the ATP Tour , which they did from 2005 – 10 . This included a record 211 consecutive weeks sharing the top two rankings from July 2005 to August 2009 . Of their 34 matches , 15 have been on clay , 16 have been on hard court , and three have been on grass . Federer has a winning record on grass ( 2 – 1 ) , while Nadal leads on clay ( 13 – 2 ) and hard court ( 9 – 7 ) . Nadal leads the head-to-head of their 11 Grand Slam ma</t>
+          <t>Mujaddid Ahmed Ijaz = Mujaddid Ahmed Ijaz , Ph.D. ( Urdu : مجدد احمد اعجا ز ; June 12 , 1937 — July 9 , 1992 ) , was a Pakistani-American experimental physicist noted for his role in discovering new isotopes that expanded the neutron-deficient side of the atomic chart . Some of the isotopes he discovered enabled significant advances in medical research , particularly in the treatment of cancer , and further advanced the experimental understanding of nuclear structures . Ijaz conducted his research work at Oak Ridge National Laboratories ( ORNL ) . He and his ORNL colleagues published more than 60 papers in physics journals announcing isotope discoveries and other results of their accelerator experiments from 1968 until 1983 . Ijaz participated in the U.S. Atoms for Peace initiative during the 1970s . The program provided a number of third-world countries , including Pakistan , with civilian nuclear reactor technology to develop energy for peaceful purposes . As a tenured professor of P</t>
         </is>
       </c>
     </row>
@@ -1561,32 +1561,32 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>['game', 'player', 'mario', 'mega', 'gameplay', 'graphics', 'praised', 'enemies', 'players', 'ign', 'controls', 'gaming', 'sonic', 'arcade', 'console']</t>
+          <t>['ride', 'coaster', 'roller', 'riders', 'train', 'flags', 'coasters', 'park', 'cedar', 'lift', 'attraction', 'drop', 'queue', 'trains', 'rides']</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Mario Kart DS = Mario Kart DS ( マリオカートDS , Mario Kāto Dī Esu ) is a 2005 go-kart racing game developed and published by Nintendo . It was released for the Nintendo DS handheld game console on November 14 , 2005 in North America , on November 17 , 2005 in Australia , on November 25 , 2005 in Europe , on December 8 , 2005 in Japan , and on April 5 , 2007 in South Korea . The game is the fifth installment in the Mario Kart series of video games , and the first to be playable via the Nintendo Wi-Fi Connection online service ; the service has since been terminated , along with other games playable via the service . Like other games in the series , Mario Kart DS features characters from the Mario series , and pits them against each other as they race in karts on tracks based on locations in the Mario series . The game was very well received , receiving an aggregated score of 91 % from Metacritic . Praise focused on the game 's graphics and gameplay , while criticism targeted its repetitive s</t>
+          <t>Dive Coaster = The Dive Coaster is a steel roller coaster manufactured by Bolliger &amp; Mabillard where riders experience a moment of free-falling with at least one 90-degree drop . Unlike other roller coasters where the lift hill takes the train directly to the first drop , a Dive Coaster lift hill leads to a flat section of track followed by a holding brake which stops the train just as it enters the vertical drop . After a few seconds , the train is released into the drop . Development of the Dive Coaster began between 1994 and 1995 with Oblivion at Alton Towers opening on March 14 , 1998 , making it the world 's first Dive Coaster . The trains for this type of coaster are relatively short consisting of two to three cars . Bolliger &amp; Mabillard have recently begun to also use floorless trains on this model to enhance the experience . As of May 2016 , ten Dive Coasters have been built , with the newest being Valravn at Cedar Point . = = History = = According to Walter Bolliger , developm</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Mario &amp; Luigi : Superstar Saga = Mario &amp; Luigi : Superstar Saga , known in Japan as Mario &amp; Luigi RPG ( マリオ ＆ ルイージRPG , Mario ando Ruīji Aru Pī Jī ) , is a role-playing video game developed by AlphaDream and published by Nintendo for the Game Boy Advance in 2003 . The first game in the Mario &amp; Luigi RPG series , Superstar Saga was followed by four sequels : Mario &amp; Luigi : Partners in Time and Mario &amp; Luigi : Bowser 's Inside Story for the Nintendo DS , Mario &amp; Luigi : Dream Team for the Nintendo 3DS and Mario &amp; Luigi : Paper Jam also for the Nintendo 3DS . The game was later re-released for the Wii U Virtual Console on the Nintendo eShop in 2014 . The setting of the game begins in the Mushroom Kingdom , but progresses to the Beanbean Kingdom for the majority of the game . In the game , Mario and Luigi combat Cackletta , the primary antagonist . The quest begins when Cackletta , with the aid of her assistant Fawful , steals Princess Peach 's voice after adopting the guise of an ambassa</t>
+          <t xml:space="preserve">Bolliger &amp; Mabillard = Bolliger &amp; Mabillard , abbreviated B &amp; M and formally known as Bolliger &amp; Mabillard Consulting Engineers Inc . , is a roller coaster design consultancy based in Monthey , Switzerland . The company was founded in 1988 by Walter Bolliger and Claude Mabillard , with Bolliger as president and Mabillard as vice-president . Since 1988 , B &amp; M has built 100 roller coasters around the world and have pioneered several new ride technologies , most notably the inverted roller coaster . Since 1990 , all coasters designed by B &amp; M that have been built within North America have been manufactured by Clermont Steel Fabricators which is located in Batavia , Ohio , United States . B &amp; M started with four employees and has since grown ; as of 2012 it employs 37 people , mostly engineers and draftsmen . In 2016 the company completed its 100th coaster . = = History = = Walter Bolliger and Claude Mabillard starting working for Giovanola , a manufacturing company who supplied rides to </t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Castle Crashers = Castle Crashers is a 2D beat ' em up video game developed by The Behemoth . It features music created by members of Newgrounds . The Xbox 360 version was released on August 27 , 2008 via Xbox Live Arcade as part of the Xbox Live Summer of Arcade . The PlayStation 3 version was released in North America on August 31 , 2010 and November 3 , 2010 in Europe via the PlayStation Network . A Microsoft Windows version , exclusive to Steam , was announced on August 16 , 2012 . The game is set in a fictional medieval universe in which a dark wizard steals a mystical gem and captures four princesses . Four knights are charged by the king to rescue the princesses , recover the jewel , and bring the wizard to justice . On June 15 , 2015 , The Behemoth announced a remastered version of the game for Xbox One . Castle Crashers was well received by critics on all platforms on which it was released . The Xbox 360 version holds a score of 82.73 % at GameRankings and 82 / 100 at Metacrit</t>
+          <t xml:space="preserve">Tatsu = Tatsu is a steel flying roller coaster designed by Bolliger &amp; Mabillard at the Six Flags Magic Mountain amusement park located in Valencia , California . Announced on November 17 , 2005 , the roller coaster opened to the public on May 13 , 2006 as the park 's seventeenth roller coaster . Tatsu reaches a height of 170 feet ( 52 m ) and speeds up to 62 miles per hour ( 100 km / h ) . The ride 's name comes from Japanese mythology and means Flying Beast in Japanese . The roller coaster is also the world 's tallest and fastest flying coaster ; is the only flying roller coaster to feature a zero-gravity roll ; and has the world 's highest pretzel loop . It was the world 's longest flying coaster until The Flying Dinosaur surpassed it . In the roller coaster 's opening year , it was named the 40th best roller coaster in the world in Amusement Today 's Golden Ticket Awards ; in Mitch Hawker 's Best Steel Roller Coaster Poll , the roller coaster placed at the 34 position . = = History </t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>MediEvil 2 = MediEvil 2 ( stylised as MediEvil II in North America ) is an action-adventure hack and slash video game developed by SCE Cambridge Studio and published by Sony Computer Entertainment for the PlayStation . It is the second instalment in the MediEvil series and a sequel to MediEvil . It was first released on 19 April 2000 in Europe and 30 April 2000 in North America . Taking place 500 years after the events of the first game , it follows series ' protagonist Sir Daniel Fortesque 's revival in Victorian era London as he attempts to stop sorcerer Lord Palethorn and Jack the Ripper 's plans to terrorise the city by raising the dead . Following the positive reception of the first game , Sony Computer Entertainment commissioned SCE Cambridge Studio to make a sequel to MediEvil before the end of the PlayStation 's lifespan . The original concepts for MediEvil 2 went through many transformations during development before the Cambridge team finally settled on making a sequel set du</t>
+          <t>Batman : The Dark Knight ( roller coaster ) = Batman : The Dark Knight ( formerly known as Batman : The Ride ) is a steel floorless roller coaster designed by Bolliger &amp; Mabillard located in the south end of Six Flags New England . The roller coaster has 2,600 feet ( 790 m ) of track , reaches a maximum height of 117.8 feet ( 35.9 m ) , and features five inversions . The coaster was announced on February 6 , 2002 and opened to the public on April 20 , 2002 . In 2008 , the ride 's name was changed to Batman : The Ride to avoid confusion with The Dark Knight Coaster that was planned to be built at the park ; after the project was cancelled , the ride 's name reverted to its original . = = History = = Batman : The Dark Knight was announced to the public on February 6 , 2002 though construction had started in September 2001 . After construction and testing was completed by Martin &amp; Vleminckx , the ride officially opened on April 20 , 2002 . In 2007 , Six Flags announced three The Dark Knig</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>SSX 3 = SSX 3 is a snowboard racing game developed by EA Canada and published by EA Sports Big . The game was initially released on October 20 , 2003 for the GameCube , PlayStation 2 , and Xbox . It was later ported to the Game Boy Advance by Visual Impact on November 11 , 2003 and to the Gizmondo by Exient Entertainment on August 31 , 2005 as a launch title . It is the third installment in the SSX series . Set on a fictional mountain , the single-player mode follows snowboarders competing in the SSX Championship . Players choose from a variety of characters and take part in various events in different locations , earning points and money by performing tricks , winning races , completing goals and finding collectables . Money can be used to upgrade character attributes , buy new clothes and boards , and unlock music and extras . Multiple players can play against each other in local multiplayer modes , and an online multiplayer mode also allowed players to connect to games and play agai</t>
+          <t>Kumba ( roller coaster ) = Kumba is a Bolliger &amp; Mabillard sit down roller coaster located at Busch Gardens Tampa Bay , in Tampa , Florida . Opened in 1993 , it stands 143 feet ( 44 m ) tall and has a top speed of 60 miles per hour ( 97 km / h ) . Kumba features a total of seven inversions across the 3-minute ride . = = History = = Kumba was officially announced in November 1992 as a record-breaking Bolliger &amp; Mabillard roller coaster set to become the park 's signature attraction . The ride officially opened to the public on April 20 , 1993 . When Kumba opened , it featured the world 's tallest vertical loop , and was also the tallest , fastest and longest roller coaster in Florida . In 1995 , Kumba conceded the title of ride with the world 's tallest vertical loop to Dragon Khan at PortAventura which features a 118-foot-tall ( 36 m ) vertical loop . In 1996 , it conceded Florida 's titles of tallest and longest roller coaster to Montu , a Bolliger &amp; Mabillard roller coaster in the Eg</t>
         </is>
       </c>
     </row>
@@ -1596,32 +1596,32 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>['series', 'character', 'television', 'season', 'episodes', 'episode', 'characters', 'story', 'cast', 'dvd', 'aired', 'doctor', 'viewers', 'producer', 'seasons']</t>
+          <t>['chicken', 'cheese', 'fried', 'sandwich', 'wine', 'dishes', 'recipes', 'dish', 'cream', 'cuisine', 'cooking', 'food', 'ingredients', 'bacon', 'meat']</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Star Cops = Star Cops is a British science fiction television series first broadcast on BBC2 in 1987 . It was devised by Chris Boucher , a writer who had previously worked on the science fiction television series Doctor Who and Blake 's 7 as well as crime dramas such as Juliet Bravo and Bergerac . Set in the year 2027 , a time where Interplanetary travel has become commonplace , it starred David Calder as Nathan Spring , commander of the International Space Police Force — nicknamed the “ Star Cops " — who provide law enforcement for the newly developing colonies of the Solar System . The series follows Nathan Spring and the rest of his multinational team as they work to establish the Star Cops and solve whatever crimes come their way . Operating in a relatively accurately realised hard SF , near-future , space environment , many of the cases that the Star Cops investigate arise from opportunities for new crimes presented by the technologically advanced future society the series depicts</t>
+          <t>Beurre Maître d 'Hôtel = Beurre Maître d 'Hôtel , also referred to as Maître d 'Hôtel butter , is a type of compound butter ( French : " Beurre composé " ) of French origin , prepared with butter , parsley , lemon juice , salt and pepper . It is a savory butter that is used on meats such as steak ( including the chateaubriand sauce for chateaubriand steak ) , fish , vegetables and other foods . It may be used in place of a sauce , and can significantly enhance a dish 's flavor . Some variations with a sweet flavor exist . It is usually served cold as sliced disks on foods , and is sometimes served as a side condiment . = = Etymology = = The name of Beurre Maître d 'Hôtel is derived from the manner in which it was commonly prepared from scratch by a restaurant 's maître d 'hôtel at diners ' tables . It is also referred to as Maître d 'Hôtel butter . = = Preparation = = Beurre Maître d 'Hôtel is a savory butter prepared by mixing softened butter with very finely minced parsley , lemon ju</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Cardcaptor Sakura = Cardcaptor Sakura ( カードキャプターさくら , Kādokyaputā Sakura ) , abbreviated as CCS and also known as Cardcaptors , is a Japanese shōjo manga series written and illustrated by the manga group Clamp . The manga was originally serialized in Nakayoshi from May 1996 to June 2000 , and published in 12 tankōbon volumes by Kodansha from November 1996 to July 2000 . The story focuses on Sakura Kinomoto , an elementary school student who discovers that she possesses magical powers after accidentally freeing a set of magical cards from the book they had been sealed in for years . She is then tasked with retrieving those cards in order to avoid an unknown catastrophe from befalling the world . A sequel by Clamp focusing on Sakura in junior high school began serialization in Nakayoshi with the July 2016 issue . The series was adapted into a 70-episode anime TV series by Madhouse that aired on Japan 's satellite television channel NHK BS2 from April 1998 to March 2000 . Additional media</t>
+          <t>Applesauce cake = Applesauce cake is a dessert cake prepared using apple sauce , flour and sugar as primary ingredients . Various spices are typically used , and it tends to be a moist cake . Applesauce cake prepared with chunky-style apple sauce may be less moist . Several additional ingredients may also be used in its preparation , and it is sometimes prepared and served as a coffee cake . The cake dates back to early colonial times in the United States . National Applesauce Cake Day occurs annually on June 6 in the U.S. = = History = = The preparation of applesauce cake dates back to early colonial times in the New England Colonies of the northeastern United States . From 1900 to the 1950s , recipes for applesauce cake frequently appeared in American cookbooks . In the United States , National Applesauce Cake Day occurs annually on June 6 . = = Ingredients and preparation = = Applesauce cake is a dessert cake prepared using apple sauce , flour and sugar as main ingredients . Store-b</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Encounter at Farpoint = " Encounter at Farpoint " is the first episode and series premiere of the American science fiction television series Star Trek : The Next Generation , which premiered in syndication on September 28 , 1987 . It was written by D. C. Fontana and Gene Roddenberry and directed by Corey Allen . Roddenberry was the creator of Star Trek , and Fontana was a writer on the original series . The series follows the adventures of the crew of the Starfleet starship Enterprise . In this episode , the crew of the newly built Enterprise examine the mysterious Farpoint Station which the Bandi people are offering to the Federation , while under the gaze of a powerful alien entity that calls itself " Q " ( John de Lancie ) . The episode was made as a pilot for the new Star Trek series , and was a double length episode at Paramount Television Group 's insistence . After the show was initially announced on October 10 , 1986 , Roddenberry put together a production team which included s</t>
+          <t>Avocado cake = Avocado cake is a cake prepared using avocado as a primary ingredient , together with other typical cake ingredients . The avocados may be mashed , and may be used as an ingredient in cake batter , in cake toppings and alone atop a cake . Cake variations include raw avocado cake , avocado brownies and avocado cheesecake . Raw , uncooked versions of avocado cake can be high in vitamin E and essential fatty acids , which are derived from avocado . Avocado-based cake toppings include avocado fool and avocado crazy . = = Overview = = Avocado is a main ingredient in avocado cake , along with other typical cake ingredients . Various varieties of avocados may be used . Avocado cake may have a subtle avocado flavor imbued in the dish . Mashed avocado may be used as an ingredient in the batter and in cake frostings and toppings . Sliced avocado may be used to top or garnish it , as may other ingredients such as the zest of citrus fruits . Additional ingredients used may include y</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Rhys Williams ( Torchwood ) = Rhys Alun Williams , portrayed by Kai Owen , is a fictional character in the BBC television programme Torchwood , a spin-off from the long-running series Doctor Who . The character is introduced in the premiere episode as the co-habiting boyfriend of principal character Gwen Cooper . Initially a recurring character , Rhys ' role is increased after the second series ; actor Kai Owen is given star billing from the show 's third series — a five-part serial subtitled Torchwood : Children of Earth — onwards . The character has gone on to appear in expanded universe material such as the Torchwood novels and audiobooks , comic books and radio plays . Throughout the first series ( 2006 ) , Rhys is initially unaware of Gwen 's vocation as a Torchwood agent , believing her to work in generic special forces . Gwen 's relationship with Rhys languishes while she is unable to communicate fully with him , but in the early part of series two ( 2008 ) he discovers the trut</t>
+          <t>Carrot soup = Carrot soup ( referred to in French as Potage de Crécy , Potage Crécy , Potage à la Crécy , Purée à la Crécy and Crème à la Crécy ) is a soup prepared with carrot as a primary ingredient . It may be prepared as a cream- or broth-style soup . Additional vegetables , root vegetables and various other ingredients may be used in its preparation . It may be served hot or cold , and several recipes exist . Carrot soup has been described as a " classic " dish in French cuisine . The soup was eaten by King Edward VII every year on 26 August to commemorate the 1346 Battle of Crécy . = = Overview = = Carrot soup may be prepared as a cream-style soup and as a broth-style soup . Vegetable stock or chicken stock may be used as ingredients in both styles of soup . Other vegetables may be used in the dish , including root vegetables , the latter of which may include garlic onion , shallot , potato , turnip and others . Carrot juice and orange juice may be used in its preparation , and s</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Veronica Mars = Veronica Mars is an American teen noir mystery drama television series created by screenwriter Rob Thomas . The series is set in the fictional town of Neptune , California , and stars Kristen Bell as the eponymous character . The series premiered on September 22 , 2004 , during television network UPN 's final two years , and ended on May 22 , 2007 , after a season on UPN 's successor , The CW , airing for three seasons total . Veronica Mars was produced by Warner Bros. Television , Silver Pictures Television , Stu Segall Productions , and Rob Thomas Productions . Joel Silver and Rob Thomas were executive producers for the entire run of the series , while Diane Ruggiero was promoted in the third season . Veronica Mars is a student who progresses from high school to college while moonlighting as a private investigator under the tutelage of her detective father . In each episode , Veronica solves a different stand-alone case while working to solve a more complex mystery . </t>
+          <t>Israeli cuisine = Israeli cuisine ( Hebrew : המטבח הישראלי ha-mitbach ha-yisra ’ eli ) comprises local dishes by people native to Israel and dishes brought to Israel by Jews from the Diaspora . Since before the establishment of the State of Israel in 1948 , and particularly since the late 1970s , an Israeli Jewish fusion cuisine has developed . Israeli cuisine has adopted , and continues to adapt , elements of various styles of Jewish cuisine , particularly the Mizrahi , Sephardic and Ashkenazi styles of cooking . It incorporates many foods traditionally eaten in Levantine , Middle Eastern and Mediterranean cuisines , and foods such as falafel , hummus , msabbha , shakshouka , couscous , and za 'atar are now widely popular in Israel . Other influences on the cuisine are the availability of foods common to the Mediterranean region , especially certain kinds of fruits and vegetables , dairy products and fish ; the distinctive traditional dishes prepared at holiday times ; the tradition o</t>
         </is>
       </c>
     </row>
@@ -1631,32 +1631,32 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>['campaign', 'said', 'announced', 'stated', 'saying', 'support', 'election', 'media', 'party', 'political', 'criticized', 'government', 'president', 'leader', 'presidential']</t>
+          <t>['buenos_aires', 'soviet', 'argentina', 'argentine', 'revolution', 'cuban', 'dictator', 'drug', 'government', 'soviet_union', 'mafia', 'cuba', 'spanish', 'political', 'spain']</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve">South African general election , 2014 = The 2014 South African general election was held on 7 May 2014 , to elect a new National Assembly and new provincial legislatures in each province . It was the fifth election held in South Africa under conditions of universal adult suffrage since the end of the apartheid era in 1994 , and also the first held since the death of Nelson Mandela . It was also the first time that South African expatriates were allowed to vote in a South African national election . The National Assembly election was won by the African National Congress ( ANC ) , but with a reduced majority of 62.1 % , down from 65.9 % in the 2009 election . The official opposition Democratic Alliance ( DA ) increased its share of the vote from 16.7 % to 22.2 % , while the newly formed Economic Freedom Fighters ( EFF ) obtained 6.4 % of the vote . Eight of the nine provincial legislatures were won by the ANC . The EFF obtained over 10 % of the vote in Gauteng , Limpopo and North West , </t>
+          <t>Last use of capital punishment in Spain = The last use of capital punishment in Spain took place on 27 September 1975 when two members of the armed Basque nationalist and separatist group ETA political-military and three members of the Revolutionary Antifascist Patriotic Front ( FRAP ) were shot dead by firing squads after having been convicted and sentenced to death by military tribunals for the murder of policemen and civil guards . Spain was Western Europe 's last dictatorship at this time and had been unpopular and internationally isolated in the post-war period due to its relations with Nazi Germany in the 1930s and the fact that the authoritarian Spanish leader , Francisco Franco , had come to power by overthrowing a democratically elected government . As a result , the executions resulted in substantial criticism of the Spanish government , both domestically and abroad . Reactions included street protests , attacks on Spanish embassies , international criticism of the Spanish go</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Jon Huntsman presidential campaign , 2012 = The Jon Huntsman presidential campaign of 2012 began in mid-2011 when Ambassador and former Governor of Utah Jon Huntsman , Jr. announced his candidacy for the Republican Party ( GOP ) nomination for President of the United States in the 2012 election . On May 3 , 2011 , Huntsman announced his intentions to file a political action committee with the Federal Election Commission ( named " H-PAC " ) . Subsequently , Huntsman announced on June 14 , 2011 , he was running for president and made an official announcement in Liberty State Park one week later on June 21 . Huntsman sought to establish himself as an anti-negative candidate and take the " high road " . In his announcement , he also stated " I don 't think you need to run down someone 's reputation in order to run for the office of president . " Huntsman aggressively touted himself as a fiscal conservative , pledging considerable business and personal tax cuts as well as a foreign policy m</t>
+          <t xml:space="preserve">Ricardo Arias Calderón = Ricardo Arias Calderón ( born 4 May 1933 ) is a Panamanian politician who served as First Vice President from 1989 to 1992 . A Roman Catholic who studied at Yale and the Sorbonne , Arias returned to Panama in the 1960s to work for political reform . He went on to become the president of the Christian Democratic Party of Panama and a leading opponent of the military government of Manuel Noriega . In 1984 , he ran as a candidate for Second Vice President on the ticket of three-time former president Arnulfo Arias , but they were defeated by pro-Noriega candidate Nicolás Ardito Barletta . Following an annulled 1989 election and the US invasion of Panama later in the same year , Arias Calderón was sworn in as First Vice President of Panama under President Guillermo Endara . After growing tensions in the ruling coalition , Arias resigned his position on December 17 , 1992 , stating that the government had not done enough to help Panama 's people . He continued to be </t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Premiership of Gordon Brown = The premiership of Gordon Brown began on 27 June 2007 when Brown accepted the Queen 's invitation to form a government , replacing Tony Blair as the Prime Minister of the United Kingdom . It ended with his resignation as Prime Minister on 11 May 2010 . While serving as Prime Minister , Brown also served as the First Lord of the Treasury , the Minister for the Civil Service and the Leader of the Labour Party . He was succeeded as Prime Minister by David Cameron Brown 's style of government differed from that of Tony Blair , who had been seen as presidential . Brown rescinded some of the policies which had been introduced or were planned by Blair 's administration . He remained committed to close ties with the United States and to the war in Iraq , although he established an inquiry into the reasons for Britain 's participation in the conflict . He proposed a " government of all the talents " which would involve co-opting leading personalities from industry </t>
+          <t>Adolfo Rodríguez Saá = Adolfo Rodríguez Saá ( born July 25 , 1947 ) is an Argentine Peronist politician . Born in a family that was highly influential in the history of the San Luis Province , he became governor in 1983 , after the end of the National Reorganization Process military dictatorship . He remained governor up to 2001 , being re-elected in successive elections . President Fernando de la Rúa resigned in that year , amid the December 2001 riots , and the Congress appointed Rodríguez Saá as president of Argentina . In response to the 1998 – 2002 Argentine great depression , he declared the highest sovereign default in history and resigned days later amid civil unrest . The Congress appointed a new president , Eduardo Duhalde , who completed the term of office of De la Rúa . Rodríguez Saá ran for the 2003 and 2015 presidential elections but did not win . = = Early life = = Rodríguez Saá was born to an important political family in San Luis . The Rodriguez Saá family is well know</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Laura Bush = Laura Lane Welch Bush ( born November 4 , 1946 ) is the wife of the 43rd President of the United States , George W. Bush , and was the First Lady from 2001 to 2009 . Bush graduated from Southern Methodist University in 1968 with a Bachelor 's Degree in Education , and took a job as a second grade teacher . After attaining her Master 's Degree in Library Science at the University of Texas at Austin , she was employed as a librarian . Bush is an avid proponent of the Dewey Decimal System . Bush met her future husband , George W. Bush , in 1977 , and they were married later that year . The couple had twin daughters in 1981 . Bush 's political involvement began during her marriage . She campaigned with her husband during his unsuccessful 1978 run for the United States Congress , and later for his successful Texas gubernatorial campaign . As First Lady of Texas , Bush implemented many initiatives focused on health , education , and literacy . In 1999 , she aided her husband in </t>
+          <t>Fidel Castro = Fidel Alejandro Castro Ruz ( American Spanish : [ fiˈðel aleˈxandɾo ˈkastɾo ˈrus ] audio ; born August 13 , 1926 ) , commonly known as Fidel Castro , is a Cuban politician and revolutionary who governed the Republic of Cuba as Prime Minister from 1959 to 1976 and then as President from 1976 to 2008 . Politically a Marxist – Leninist and Cuban nationalist , he also served as the First Secretary of the Communist Party of Cuba from 1961 until 2011 . Under his administration Cuba became a one-party communist state ; industry and business were nationalized , and state socialist reforms implemented throughout society . Born in Birán as the son of a wealthy farmer , Castro adopted leftist anti-imperialist politics while studying law at the University of Havana . After participating in rebellions against right-wing governments in the Dominican Republic and Colombia , he planned the overthrow of Cuban President Fulgencio Batista , launching a failed attack on the Moncada Barracks</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Scott Brown = Scott Philip Brown ( born September 12 , 1959 ) is an American attorney and politician . He was a United States Senator from Massachusetts , 2010 to 2013 . Prior to his term in the Senate , Brown served as a member of the Massachusetts General Court , first in the State House of Representatives ( 1998 – 2004 ) and then in the State Senate ( 2004 – 2010 ) . Brown served 35 years in the Army National Guard , retiring in 2014 with the rank of colonel . Brown is currently working as a political contributor for Fox News Channel and as an on-call host for select Fox News Channel shows , including Fox &amp; Friends . Brown is a member of the Republican Party , and faced the Democratic candidate , Massachusetts Attorney General Martha Coakley , in the 2010 special election to succeed U.S. Senator Ted Kennedy for the remainder of the term ending January 3 , 2013 . While initially trailing Coakley in polling by a large margin , Brown saw a sudden late surge in the polls and posted a su</t>
+          <t>Regina Martínez Pérez = Regina Martínez Pérez ( 7 September 1963 – 28 April 2012 ) was a Mexican journalist and veteran crime reporter for Proceso , a center-left Mexican news magazine known for its critical reporting of the social and political establishment . Born in a small town in the state of Veracruz , Martínez Pérez left her hometown to study journalism at Universidad Veracruzana . After graduating from university , she went to work at a state-owned television company in Chiapas in the early 1980s , but she encountered various forms of censorship that convinced her to pursue a career in print media . After five years in Chiapas , Martínez Pérez relocated to Veracruz and worked for several local newspapers . In Veracruz , Martínez Pérez faced several challenges of censorship by the political establishment for her direct reporting , and particularly for being an outspoken critic of human rights violations , government corruption , abuse of authority , and for her in-depth coverage</t>
         </is>
       </c>
     </row>
@@ -1666,32 +1666,32 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>['member', 'served', 'elected', 'governor', 'committee', 'serving', 'worked', 'election', 'appointed', 'kentucky', 'married', 'resigned', 'attended', 'born', 'fellow']</t>
+          <t>['twitter', 'cylinder', 'cylinders', 'vehicle', 'watson', 'vehicles', 'toyota', 'users', 'model', 'models', 'gas', 'car', 'electric', 'engine', 'valve']</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Joseph Tydings = Joseph Davies Tydings ( born May 4 , 1928 ) is a former Democratic member of the United States Senate , representing the state of Maryland from 1965 to 1971 . Born in North Carolina , Tydings moved to Maryland as a youth after he was adopted by Millard Tydings , U.S. Senator from Maryland . After serving in the military , he obtained his law degree and entered into practice . He served in the Maryland House of Delegates from 1955 to 1961 , and as United States Attorney from 1961 until his resignation in 1963 to run for Senate . Tydings won election to the Senate in 1964 . However , his controversial stances on gun control and crime in the District of Columbia cost him re-election in 1970 . He made another attempt at his old seat in 1976 , but was defeated in the Democratic primary election by Paul Sarbanes . He later served as a member of the Board of Regents of the University of Maryland , College Park and the University System of Maryland , and continues to practice </t>
+          <t>Saviem = The Société Anonyme de Véhicules Industriels et d 'Equipements Mécaniques ( French pronunciation : ​ [ sɔsjete də vɛikyl ɛ ̃ dystʁijɛl e dəkipəmɑ ̃ mekanik ] ) , commonly known by the acronym Saviem ( French pronunciation : ​ [ savjɛ ̃ ] ) , was a French manufacturer of trucks and buses / coaches part of the Renault group , headquartered in Suresnes . The company was established in 1955 by merging Renault heavy vehicle operations with Somua and Latil and disappeared in 1978 when was merged with former rival Berliet to form Renault Véhicules Industriels . The company initially had various factories for vehicle production around France ( mainly at the Paris area ) which came from its predecessors and Chausson , but it soon centred assembly on Blainville-sur-Orne ( trucks ) and Annonay ( buses and coaches ) . Saviem formed partnerships with other manufacturers , leading to technology-sharing agreements . = = History = = = = = Early years = = = At the end of 1946 , Renault abandon</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>William B. Washburn = William Barrett Washburn ( January 31 , 1820 – October 5 , 1887 ) was an American businessman and politician from Massachusetts . Washburn served several terms in the United States House of Representatives ( 1863 – 71 ) and as the 28th Governor of Massachusetts from 1872 to 1874 , when he won election to the United States Senate in a special election to succeed the recently deceased Charles Sumner . A moderate Republican , Washburn only partially supported the Radical Republican agenda during the American Civil War and the Reconstruction Era that followed . A Yale graduate , Washburn parlayed early business success in furniture manufacture into banking and railroads , based in the Connecticut River valley town of Greenfield . He was a major proponent of a railroads in northern and western Massachusetts , sitting on the board of the Connecticut River Railroad for many years , and playing an oversight role in the construction of the Hoosac Tunnel . He has been descr</t>
+          <t>Renault Agriculture = Renault Agriculture S.A.S. ( French pronunciation : ​ [ ʁəno aɡʁikyltyʁ ( ə ) ] ) was the agricultural machinery division of the French car manufacturer Renault established in 1918 from its armored military vehicles division . While in operation , Renault Agriculture had various partnerships with major manufacturers and focussed production on tractors . The company was sold between 2003 and 2008 to German rival Claas . Renault Agriculture was dissolved in 2008 and its facilities became part of Claas ' tractor division . Claas ' tractor division and Renault 's Auto Châssis International are Renault Agriculture successors . = = History = = After the end of World War I , the Renault company used its experience in armored tanks to devise agricultural vehicles . The Renault 's Department 14 ( responsible for the FT tank ) developed the first tractor of the company , the Type GP , which was powered by an engine similar to that of the FT ( a four-cylinder ) and had track</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Herbert Charles Wilson = Herbert Charles Wilson ( December 7 , 1859 – December 17 , 1909 ) was a Canadian politician and physician . He served as mayor of the Town of Edmonton and Speaker of the Legislative Assembly of the North-West Territories . Wilson was born in 1859 in what would become the province of Ontario . The son of a manufacturer , Wilson 's family had extensive business interests in the area of Picton , Ontario . Wilson studied medicine and moved to Edmonton in 1882 , one of the first physicians to settle there . He was appointed to official medical positions and , for several years , owned a drugstore in town . He served as a consultant to First Nations reserves near Edmonton and also became a director of many local corporations . He was elected to the Territorial council in 1885 , and soon became its speaker . During his speakership , he helped to change the council 's rules and procedures . He left territorial politics after six years , citing health reasons . He maint</t>
+          <t>Renault Samsung Motors = Renault Samsung Motors ( Korean : 르노삼성자동차 , IPA : [ ɾɯnoː sʰamsʰʌŋ dʑadoŋtɕʰa ] ) , also known by the acronym RSM , is a South Korean car manufacturer headquartered in Busan where its single assembly site is also located , with additional facilities at Seoul ( administration ) and Giheung ( research and development ) . It was first established as Samsung Motors in 1994 by the chaebol Samsung , with technical assistance from Nissan . The company started selling cars in 1998 , just before South Korea was hit by the Asian financial crisis . In September 2000 , it became a subsidiary of Renault and adopted its present name , although Samsung maintained a minority ownership . RSM markets a range of cars , including electric models and crossovers . = = History = = = = = Beginnings : Samsung Group era ( 1994 – 2000 ) = = = In the early 1990s , Samsung 's Chairman Kun Hee Lee recognised the automotive industry as the culmination of several others . For the Samsung Grou</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Andrew Wodrow = Andrew Wodrow ( 1752 – 1814 ) was a prominent Scottish American merchant , militia officer , clerk of court , lawyer , and landowner in the colony ( and later U.S. state ) of Virginia . Wodrow was born in Scotland in 1752 and immigrated to Virginia in 1768 . In Fredericksburg , he engaged in a thriving import business . Following the outbreak of the American Revolutionary War , Wodrow placed his entire inventory up for public auction and contributed the profits to the American Revolutionary patriot cause . During the war , Wodrow served as a lieutenant colonel in command of cavalry in the Continental Army . Wodrow was the first resident clerk of court for Hampshire County , Virginia ( now West Virginia ) , a position in which he served for a tenure lasting 32 years ( 1782 – 1814 ) . There , Wodrow served in the position of major in the Hampshire County militia . In addition , he represented Hampshire County at the Virginia Ratifying Convention , held to ratify the Unite</t>
+          <t>NextWorth = NextWorth is an electronics trade-in and recycling service . Users of the service exchange used electronics for cash or discounts on newer models . NextWorth was founded by business students at Babson College in 2005 . It started as a commission-based service to help businesses setup online auctions for their used items , then changed its business model to focus on electronics trade-ins in 2006 . As of late 2012 , NextWorth was one of the best-known and largest electronics trade-in and recycling services in the United States , although it handles only a small percentage of total trade-in traffic . = = History = = NextWorth was founded by David Chen , Andrew Walsh and Scott Richardson while they were students at Babson College . The company was selected for Babson College 's 2005 Business Hatcheries program , which provides free resources to student-led startups . NextWorth Inc. began operations the following year . It was originally a service that helped businesses and non-</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Robert Q. Marston = Robert Quarles Marston ( February 12 , 1923 – March 14 , 1999 ) was an American physician , research scientist , governmental appointee and university administrator . Marston was a native of Virginia , and , after earning his bachelor 's , medical and research degrees , he became a research scientist and medical professor . He served as the dean of the University of Mississippi School of Medicine , the director of the National Institutes of Health , and the president of the University of Florida . = = Early life and education = = He was born in Toano , Virginia , a small unincorporated community near Williamsburg , in 1923 . He graduated from the Virginia Military Institute ( VMI ) in Lexington , Virginia with a bachelor of science degree in 1944 . While attending the Medical College of Virginia ( MCV ) in Richmond , Virginia , he married Ann Carter Garnett in 1946 . Following his graduation from MCV with a doctor of medicine degree ( M.D. ) in 1947 , he received a </t>
+          <t>Lexus = Lexus ( レクサス , Rekusasu ) is the luxury vehicle division of Japanese automaker Toyota . The Lexus marque is marketed in over 70 countries and territories worldwide , has become Japan 's largest-selling make of premium cars , and has ranked among the ten largest Japanese global brands in market value . Lexus is headquartered in Nagoya , Japan . Operational centers are located in Brussels , Belgium , and the U.S. in Torrance , California . Lexus originated from a corporate project to develop a new premium sedan , code-named F1 , which began in 1983 and culminated in the launch of the Lexus LS in 1989 . Subsequently , the division added sedan , coupé , convertible , and SUV models . Until 2005 Lexus did not exist as a brand in its home market and all vehicles marketed internationally as Lexus from 1989-2005 were released in Japan under the Toyota marque and an equivalent model name . In 2005 , a hybrid version of the RX crossover debuted , and additional hybrid models later joined</t>
         </is>
       </c>
     </row>
@@ -1701,32 +1701,32 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>['daily', 'trunkline', 'roadway', 'national_highway_system', 'travels', 'designated', 'surveys', 'entire', 'paved', 'intersections', 'designation', 'traveling', 'terminus', 'rural', 'mdot']</t>
+          <t>['fiction', 'gay', 'stories', 'pulp', 'lgbt', 'science', 'magazine', 'lesbian', 'comics', 'fantasy', 'issue', 'magazines', 'comic', 'hugo', 'published']</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Route 261 ( Delaware – Pennsylvania ) = Delaware Route 261 ( DE 261 ) and Pennsylvania Route 261 ( PA 261 ) , also known as Foulk Road , is a 6.88-mile ( 11.07 km ) state highway running through Delaware and Pennsylvania . DE 261 runs 4.62 miles ( 7.44 km ) through New Castle County , Delaware from an interchange with U.S. Route 202 ( US 202 ) and DE 141 north of Interstate 95 ( I-95 ) near Fairfax , Delaware , a community north of Wilmington , northeast to the Pennsylvania state line . The road runs through suburban areas of Brandywine Hundred as a four-lane road south of DE 92 and a two-lane road north of DE 92 . At the Pennsylvania state line , Foulk Road becomes PA 261 and continues 2.26 miles ( 3.64 km ) through Bethel Township in Delaware County , intersecting PA 491 in Booths Corner before ending at an interchange with US 322 . DE 261 was originally designated along Foulk Road in the 1930s . In the 1960s , most of the route was widened into a four-lane road . The southern termin</t>
+          <t>Uncanny Stories ( magazine ) = Uncanny Stories was a pulp magazine which published a single issue , dated April 1941 . It was published by Abraham and Martin Goodman , who were better known for " weird-menace " pulp magazines that included much more sex in the fiction than was usual in science fiction of that era . The Goodmans published Marvel Science Stories from 1938 to 1941 , and Uncanny Stories appeared just as Marvel Science Stories ceased publication , perhaps in order to use up the material in inventory acquired by Marvel Science Stories . The fiction was poor quality ; the lead story , Ray Cummings ' " Coming of the Giant Germs " , has been described as " one of his most appalling stories " . = = Publication history = = Although science fiction had been published before the 1920s , it did not begin to coalesce into a separately marketed genre until the appearance in 1926 of Amazing Stories , a pulp magazine published by Hugo Gernsback . After 1931 , when Miracle Science and Fa</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Arizona State Route 88 = State Route 88 ( SR 88 ) is a 45.67 mi ( 73.50 km ) long state highway in the U.S. state of Arizona . It runs from U.S. Route 60 ( US 60 ) in Apache Junction through desert terrain to SR 188 near Roosevelt Dam . Following the Salt River for much of its length , the section east of Tortilla Flat is known as the Apache Trail and is part of the National Forest Scenic Byway system . The Apache Trail was built in the mid-1920s and the number 88 was assigned in 1927 . An eastern extension of SR 88 to Globe was redesignated as SR 188 in the late 1990s . = = Route description = = SR 88 begins at a diamond interchange with US 60 , the Superstition Freeway , in southern Apache Junction . The route follows Idaho Road northward through a residential area with four lanes . Following a junction with Old West Highway , SR 88 turns northeast onto Apache Trail and narrows to two lanes . The route exits the city limits of Apache Junction , entering desert terrain . Passing a gho</t>
+          <t>Dynamic Science Stories = Dynamic Science Stories was a pulp magazine which published two issues , dated February and April 1939 . A companion to Marvel Science Stories , it was edited by Robert O. Erisman and published by Western Fiction Publishing . Among the better known authors who appeared in its pages were L. Sprague de Camp and Manly Wade Wellman . = = Publication history and contents = = Although science fiction had been published before the 1920s , it did not begin to coalesce into a separately marketed genre until the appearance in 1926 of Amazing Stories , a pulp magazine published by Hugo Gernsback . By the end of the 1930s the field was booming . In 1938 Abraham and Martin Goodman , two brothers who owned a publishing company with multiple imprints , launched Marvel Science Stories , edited by Robert O. Erisman . In February of the following year they added Dynamic Science Stories as a companion magazine intended to run longer stories . The contents were typical pulp scien</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Ontario Highway 148 = King 's Highway 148 , commonly referred to as Highway 148 , is a provincially maintained highway in Ontario , Canada . The highway acts as an extension of Route 148 in Quebec , once connecting it with Highway 17 , the Trans-Canada Highway , near Pembroke . It was shortened to its present terminus in 1997 , and now connects downtown Pembroke to the provincial border . Highway 148 follows a route that was once part of Highway 17 and Highway 62 until the Pembroke Bypass opened in 1982 . The 7.0-kilometre ( 4.3 mi ) route of Highway 148 takes it along the Ontario shoreline of the Ottawa River from the outskirts of Pembroke to the opposite shore as L 'Isle-aux-Allumettes , where it crosses the river into Quebec . The section of the highway within Pembroke is locally maintained under a Connecting Link agreement . = = Route description = = Highway 148 connects Pembroke to the Quebec border at L 'Isle-aux-Allumettes , a distance of 5 km ( 3.1 mi ) . It originally connecte</t>
+          <t>Fantastic Story Quarterly = Fantastic Story Quarterly was a pulp science fiction magazine , published from 1950 to 1955 by Best Books , a subsidiary imprint of Standard Magazines . The name was changed with the Summer 1951 issue to Fantastic Story Magazine . It was launched to reprint stories from the early years of the science fiction pulp magazines , and was initially intended to carry no new fiction , though in the end every issue contained at least one new story . It was sufficiently successful for Standard to launch Wonder Story Annual as a vehicle for more science fiction reprints , but the success did not last . In 1955 it was merged with Standard 's Startling Stories . Original fiction in Fantastic Story included Gordon R. Dickson 's first sale , " Trespass " , and stories by Walter M. Miller and Richard Matheson . = = Publication history and contents = = The first science fiction ( sf ) magazine , Amazing Stories , was launched in 1926 by Hugo Gernsback at the height of the pu</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Delaware Route 42 = Delaware Route 42 ( DE 42 ) is a state highway in Kent County , Delaware . It runs from DE 6 in Blackiston east to DE 9 in Leipsic . DE 42 passes through rural areas along with the towns of Kenton and Cheswold . The route intersects DE 300 in Kenton , DE 15 between Seven Hickories and Moores Corner , and U.S. Route 13 ( US 13 ) in Cheswold . The road was built as a state highway during the 1920s and 1930s . DE 42 was designated by 1936 between Kenton and Leipsic and extended to Blackiston by 1966 . = = Route description = = DE 42 begins at an intersection with DE 6 in Blackiston . Northwest of DE 6 , the road becomes Longridge Road , which changes names to Delaney Maryland Line Road and Clayton Delaney Road before it reaches the Maryland border and becomes Maryland Route 330 ( MD 330 ) . MD 330 heads west into Kent County , Maryland and , by way of MD 313 , provides access to US 301 . From the western terminus , DE 42 heads southeast on two-lane undivided Blackiston</t>
+          <t xml:space="preserve">Ghost Stories ( magazine ) = Ghost Stories was a pulp magazine which published 64 issues between 1926 and 1932 . It was one of the earliest competitors to Weird Tales , the first magazine to specialize in the fantasy and occult fiction genre . It was a companion magazine to True Story and True Detective Stories , and focused almost entirely on stories about ghosts , with many of the stories written by staff writers but presented under pseudonyms in a " true confession " style . These were often accompanied by faked photographs to make the stories appear more believable . Ghost Stories also ran original and reprinted contributions , including works by Robert E. Howard , Carl Jacobi , and Frank Belknap Long . Among the reprints were Agatha Christie 's " The Last Seance " ( under the title " The Woman Who Stole a Ghost " ) , several stories by H.G. Wells , and Charles Dickens ' " The Signalman " . The magazine was initially successful , but began to lose readers , and in 1930 was sold to </t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Washington State Route 542 = State Route 542 ( SR 542 ) is a 57.24-mile-long ( 92.12 km ) state highway in the U.S. state of Washington , serving Mount Baker in Whatcom County . SR 542 travels east as the Mount Baker Highway from an interchange with Interstate 5 ( I-5 ) in Bellingham through the Nooksack River valley to the Mt . Baker Ski Area at Austin Pass . It serves as the main highway to Mount Baker and the communities of Deming , Kendall , and Maple Falls along the Nooksack River . The highway was constructed in 1893 by Whatcom County as a wagon road between Bellingham and Maple Falls and was added to the state highway system as a branch of State Road 1 in 1925 . The branch was transferred to Primary State Highway 1 ( PSH 1 ) during its creation in 1937 and became SR 542 during the 1964 highway renumbering . = = Route description = = SR 542 begins as Sunset Drive and the Mount Baker Highway at a partial cloverleaf interchange with I-5 to the northeast of downtown Bellingham . The</t>
+          <t>Miracle Science and Fantasy Stories = Miracle Science and Fantasy Stories was a pulp science fiction magazine which published two issues in 1931 . The fiction was unremarkable , but the cover art and illustrations , by Elliott Dold , were high quality , and have made the magazine a collector 's item . The magazine ceased publication when Dold became ill and was unable to continue his duties both as editor and artist . = = Publication history = = In 1931 , Harold Hersey , who had been working in the pulp magazine field for over a decade , decided to launch a new science fiction ( sf ) and fantasy magazine . Hersey had been the editor for the first half of The Thrill Book 's run of 16 issues in 1919 , and had also worked for Clayton Magazines , where in 1928 he had proposed a sf magazine to William Clayton . Clayton turned down the idea , but the following year changed his mind and launched Astounding Stories of Super Science , with Harry Bates as editor . After Hersey left Clayton and s</t>
         </is>
       </c>
     </row>
@@ -1736,32 +1736,32 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>['song', 'video', 'number', 'single', 'chart', 'performed', 'peaked', 'weeks', 'carey', 'debuted', 'rihanna', 'hot', 'background', 'week', 'girl']</t>
+          <t>['nickelodeon', 'patrick', 'dvd', 'bikini', 'episodes', 'animation', 'kenny', 'voice', 'kids', 'storyboard', 'episode', 'animated', 'lawrence', 'character', 'television']</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>The Beyoncé Experience Live = The Beyoncé Experience Live is a live DVD by American recording artist Beyoncé , released by Columbia Records on November 20 , 2007 . It was shot at the Staples Center , Los Angeles , California , on September 2 , 2007 during her worldwide tour The Beyoncé Experience . It features guest appearances from rapper Jay-Z on " Upgrade U " and former Destiny 's Child mates Michelle Williams and Kelly Rowland on " Survivor " . The show featured on the album was broadcast on different channels ; for one night only on November 19 , 2007 , the show was shown in ninety-six theaters across the US , Black Entertainment Television ( BET ) aired an edited version of the concert on Thanksgiving day and AEG Network and 3sat also aired the concert . The album features performances of songs from Beyoncé 's two studio albums Dangerously in Love ( 2003 ) and B 'Day ( 2006 ) as well as songs which she recorded with Destiny 's Child . Upon its release , The Beyoncé Experience Liv</t>
+          <t>Crab dip = Crab dip , sometimes referred to as Maryland crab dip , is a thick , creamy dip that is typically prepared from cream cheese and lump crab meat . Other primary ingredients such as mayonnaise may be used . Various types of crab preparations , species and superfamilies are used , as are a variety of added ingredients . It is typically served hot , although cold versions also exist . Hot versions are typically baked or broiled . It is sometimes served as an appetizer . Accompaniments may include crackers and various breads . Some U.S. restaurants offer crab dip , commercially produced varieties exist , and some stadiums offer it as a part of their concessions . = = Ingredients = = Fresh , frozen or canned crab meat may be used in the preparation of crab dip . Different types of crab meat may be used , such as jumbo lump , lump backfin , leg and claw , among others . Various types of crab species and superfamilies are also used , such as blue crab , Dungeness crab and Alaska kin</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Birthday Cake ( song ) = " Birthday Cake " is a song by Barbadian recording artist Rihanna , from her sixth studio album , Talk That Talk ( 2011 ) . After it leaked onto the internet , fans expressed interest in the track being included on Talk That Talk , but it was later revealed that the 1 : 18 ( one minute , 18 seconds ) length that leaked was in fact the final cut and was not being considered for inclusion on the album . Due to a high level of fan interest , the song was included on the album as an interlude . The full length version , also known as the official remix of the track , featuring Rihanna 's ex-boyfriend Chris Brown , was premiered online on February 20 , 2012 , to coincide with Rihanna 's 24th birthday . The song peaked in the top fifty . The lyrics to " Birthday Cake " express the desire to have spontaneous sex . Music critics were divided on " Birthday Cake " , with the majority both praising and criticising the song 's sexual lyrical content . Several critics compa</t>
+          <t>SpongeBob SquarePants ( season 7 ) = The seventh season of the American animated television series SpongeBob SquarePants , created by marine biologist and animator Stephen Hillenburg , originally aired on Nickelodeon in the United States from July 19 , 2009 to June 11 , 2011 . It contained 26 episodes , beginning with the episodes " Tentacle Vision " and " I Heart Dancing " . The series chronicles the exploits and adventures of the title character and his various friends in the fictional underwater city of Bikini Bottom . The season was executive produced by series creator Hillenburg and writer Paul Tibbitt , who also acted as the showrunner . In 2011 , Legends of Bikini Bottom , an anthology series consists of five episodes from the season , was launched . A number of guest stars appeared on the season 's episodes . Several compilation DVDs that contained episodes from the season were released . The SpongeBob SquarePants : Complete Seventh Season DVD was released in Region 1 on Decemb</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t xml:space="preserve">How Will I Know = " How Will I Know " is a song recorded by American recording artist Whitney Houston for her debut album , titled Whitney Houston , which was released in February 1985 . It was released by Arista Records in November that year , as the album 's third single . Composed by George Merrill and Shannon Rubicam , the song was originally intended for Janet Jackson , but she passed on it . Houston then recorded the song with altered lyrics and production from Narada Michael Walden . The lyrics speak about the protagonist trying to discern if a boy she likes will ever like her back . " How Will I Know " received mainly positive reviews . The song became Houston 's second number one single on the United States Billboard Hot 100 . It spent two weeks atop the chart and also became Houston 's first chart topper on the Canadian RPM Singles Chart . Success was worldwide : it reached the top 10 in Sweden , Ireland , Norway , and the United Kingdom , and the top 20 in the Netherlands , </t>
+          <t>SpongeBob SquarePants ( season 6 ) = The sixth season of the American animated television series SpongeBob SquarePants , created by former marine biologist and animator Stephen Hillenburg , aired on Nickelodeon from March 3 , 2008 to July 5 , 2010 , and contained 26 episodes , beginning with the episode " Krabby Road " . The series chronicles the exploits and adventures of the title character and his various friends in the fictional underwater city of Bikini Bottom . The season was executive produced by series creator Hillenburg , who also acted as the showrunner . In 2009 , the show celebrated its tenth anniversary on television . The documentary film titled Square Roots : The Story of SpongeBob SquarePants premiered on July 17 , 2009 , and marked the anniversary . SpongeBob 's Truth or Square , a television film , and the special episode " To SquarePants or Not to SquarePants " were broadcast on Nickelodeon , as part of the celebration . The show itself received several recognition ,</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Crawl ( Chris Brown song ) = " Crawl " is a song by American recording artist Chris Brown . It is the second single from his third studio album Graffiti , released as a digital download on November 24 , 2009 . The song was produced by The Messengers and was written by Nasri Atweh , Adam Messinger , Luke Boyd , and Brown . The song is about yearning to rebuild a failed relationship and was interpreted by critics as being about Brown 's former relationship with Barbadian singer Rihanna . However , Brown has stated the song is not about any of his previous relationships . The song received positive to mixed reviews . It charted in the top twenty in Japan and New Zealand , and the top forty in the United Kingdom and Ireland . It peaked in the United States at number fifty-three . The accompanying music video features Brown and American R &amp; B singer Cassie as his love interest . In the video , he yearns for their relationship on a winter night in a city and in a desert scene . Brown perform</t>
+          <t>SpongeBob SquarePants ( season 4 ) = The fourth season of the American animated television series SpongeBob SquarePants , created by former marine biologist and animator Stephen Hillenburg , aired on Nickelodeon from May 6 , 2005 to July 24 , 2007 , and contained 20 episodes , beginning with the episodes " Fear of a Krabby Patty " and " Shell of a Man " . The series chronicles the exploits and adventures of the title character and his various friends in the fictional underwater city of Bikini Bottom . The season was executive produced by series creator Hillenburg , while writer Paul Tibbitt acted as the showrunner . The show underwent a hiatus on television as Hillenburg halted the production in 2002 to work on the film adaptation of the series , The SpongeBob SquarePants Movie . Once the film was finalized and the previous season had completed broadcast on television , Hillenburg wanted to end the show , but the success of the series led to more episodes , so Tibbitt took over Hillenb</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Miles Away ( Madonna song ) = " Miles Away " is a song by American singer and songwriter Madonna from her eleventh studio album , Hard Candy . It was first released as a promotional single in Japan , during June 2008 , as the theme for the Fuji Television Japanese drama , Change . The song was released by Warner Bros. Records , as the third and final single from the album on October 17 , 2008 , and was subsequently included on her compilation album , Celebration ( 2009 ) . Written by Madonna , Justin Timberlake , Timbaland and Nate " Danja " Hills , " Miles Away " is a melancholy electronic ballad , which according to Madonna is autobiographical , and is inspired by her then husband Guy Ritchie . Lyrically , the song deals with long-distance relationships . " Miles Away " has received positive appreciation from music critics for being a harmonious and meaningful ballad . It reached the top forty in most countries , while peaking inside the top ten in Czech Republic , Netherlands , Hung</t>
+          <t>Pizza Delivery ( SpongeBob SquarePants ) = " Pizza Delivery " is the first segment of the fifth episode of the American animated television series SpongeBob SquarePants . The episode was written by Sherm Cohen , Aaron Springer , and Peter Burns , and was directed by Sean Dempsey . Cohen also functioned as storyboard director , and Springer worked as storyboard artist . It originally aired on Nickelodeon in the United States on August 14 , 1999 . In the episode , the Krusty Krab receives a call from a customer ordering a pizza , and Mr. Krabs sends SpongeBob and Squidward to deliver it . When the two employees become stranded in the middle of a desert , they get into numerous predicaments . Along the way , SpongeBob tries to show Squidward the way of the pioneers . In pitching the show to Nickelodeon , creator Stephen Hillenburg originally wanted the idea of having the characters on a road trip , inspired by the 1989 film Powwow Highway . However , he eventually gave up the idea , and r</t>
         </is>
       </c>
     </row>
@@ -1771,32 +1771,32 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>['war', 'following', 'german', 'april', 'training', 'japanese', 'division', 'attack', 'march', 'assigned', 'transferred', 'november', 'december', 'command', 'commander']</t>
+          <t>['scottish', 'scotland', 'painting', 'edinburgh', 'architecture', 'houses', 'century', 'churches', 'scots', 'bricks', 'portrait', 'highlands', 'glasgow', 'brick', 'portraits']</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Gordon Gollob = Gordon Mac Gollob ( 16 June 1912 – 7 September 1987 ) was a German Luftwaffe military aviator during World War II , a fighter ace credited with 150 enemy aircraft shot down in over 340 combat missions . Originally from Austria , he claimed the majority of his victories over the Eastern Front , and six over the Western Front , five of which he claimed as a Messerschmitt Bf 110 fighter pilot . Gollob volunteered for military service in the Austrian Austrian Armed Forces in 1933 . In March 1938 , following the Anschluss , the annexation of Austria into Nazi Germany , Gollob was transferred to the Luftwaffe . In 1939 , Gollob was posted to Zerstörergeschwader 76 ( ZG 76 — 76th Destroyer Wing ) , a twin-engined heavy fighter wing . Following the outbreak of World War II , he claimed his first aerial victory on 5 September 1939 during the invasion of Poland . Gollob claimed one victory during the Battle of the Heligoland Bight and two victories during the Norwegian Campaign .</t>
+          <t>Architecture of Scotland in the Middle Ages = The architecture of Scotland in the Middle Ages includes all building within the modern borders of Scotland , between the departure of the Romans from Northern Britain in the early fifth century and the adoption of the Renaissance in the early sixteenth century , and includes vernacular , ecclesiastical , royal , aristocratic and military constructions . The first surviving houses in Scotland go back 9500 years . There is evidence of different forms of stone and wooden houses exist and earthwork hill forts from the Iron Age . The arrival of the Romans from about led to the abandonment of many of these forts . After the departure of the Romans in the fifth century , there evidence their reoccupation and of the building of a series of smaller " nucleated " constructions sometimes utilising major geographical features , as at Dunadd and Dumbarton . In the following centuries new forms of construction emerged throughout Scotland that would come</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>173rd Airborne Brigade Combat Team = The 173rd Airborne Brigade Combat Team ( " Sky Soldiers " ) is an airborne infantry brigade combat team of the United States Army based in Vicenza , Italy . It is the United States European Command 's conventional airborne strategic response force for Europe . Activated in 1915 , as the 173rd Infantry Brigade , the unit saw service in World War I , but is best known for its actions during the Vietnam War . The brigade was the first major United States Army ground formation deployed in Vietnam , serving there from 1965 to 1971 and losing almost 1,800 soldiers . Noted for its roles in Operation Hump and Operation Junction City , the 173rd is best known for the Battle of Dak To , where it suffered heavy casualties in close combat with North Vietnamese forces . Brigade members received over 7,700 decorations , including more than 6,000 Purple Hearts . The brigade returned to the United States in 1972 , where the 1st and 2nd battalions of the 503rd Airbo</t>
+          <t>Architecture of Scotland = The architecture of Scotland includes all human building within the modern borders of Scotland , from the Neolithic era to the present day . The earliest surviving houses go back around 9500 years , and the first villages 6000 years : Skara Brae on the Mainland of Orkney being the earliest preserved example in Europe . Crannogs , roundhouses , each built on an artificial island , date from the Bronze Age and stone buildings called Atlantic roundhouses and larger earthwork hill forts from the Iron Age . The arrival of the Romans from about 71 AD led to the creation of forts like that at Trimontium , and a continuous fortification between the Firth of Forth and the Firth of Clyde known as the Antonine Wall , built in the second century AD . Beyond Roman influence , there is evidence of wheelhouses and underground souterrains . After the departure of the Romans there were a series of nucleated hill forts , often utilising major geographical features , as at Duna</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Australian Army during World War I = The Australian Army was the largest service in the Australian military during World War I. The First Australian Imperial Force ( AIF ) was the Army 's main expeditionary force and was formed from 15 August 1914 with an initial strength of 20,000 men , following Britain 's declaration of war on Germany . Meanwhile , the separate , hastily raised 2,000-man Australian Naval and Military Expeditionary Force ( AN &amp; MEF ) , landed near Rabaul in German New Guinea on 11 September 1914 and obtained the surrender of the German garrison after ten days ; it later provided occupation forces for the duration of the war . In addition , small military forces based on the pre-war Permanent Forces and part-time Citizen Forces were maintained in Australia to defend the country from attack . The AIF initially consisted of one infantry division and one light horse brigade . The first contingent departed Australia by ship for Egypt on 1 November 1914 , where it formed p</t>
+          <t>Scottish art in the eighteenth century = Scottish art in the eighteenth century is the body of visual art made in Scotland , by Scots , or about Scottish subjects , in the eighteenth century . This period saw development of professionalisation , with art academies were established in Edinburgh and Glasgow . Art was increasingly influenced by Neoclassicism , the Enlightenment and towards the end of the century by Romanticism , with Italy becoming a major centre of Scottish art . The origins of the tradition of Scottish landscape painting are in the capriccios of Italian and Dutch landscapes undertaken by James Norie and his sons . These were further developed by Jacob More , who added a romantic sensibility to the Scottish landscape . Alexander Nasmyth helped found the Scottish landscape tradition and was highly influential as a teacher in Edinburgh on the subsequent generation of artists . John Knox linked it with the Romantic works of Walter Scott and was one of the first artists to t</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>North Staffordshire Regiment = The North Staffordshire Regiment ( Prince of Wales 's ) was a line infantry regiment of the British Army , which was in existence between 1881 and 1959 . The 64th ( 2nd Staffordshire ) Regiment of Foot was created on 21 April 1758 from the 2nd Battalion of the 11th Regiment of Foot . In 1881 , under the Childers Reforms , the 64th Regiment of Foot was merged with the 98th ( Prince of Wales 's ) Regiment of Foot ( originally raised in 1824 ) to form the Prince of Wales 's ( North Staffordshire Regiment ) . In 1921 the regimental title was altered to the North Staffordshire Regiment ( Prince of Wales 's ) . Formed at a time when the British Empire was reaching its peak , the regiment served all over the Empire , in times of both peace and war , and in many theatres of war outside the Empire . It fought with distinction in World War I and World War II , as well as in other smaller conflicts around the world . These other wars included the Second Sudanese War</t>
+          <t>Art in early modern Scotland = Art in early modern Scotland includes all forms of artistic production within the modern borders of Scotland , between the adoption of the Renaissance in the early sixteenth century to the beginnings of the Enlightenment in the mid-eighteenth century . Devotional art before the Reformation included books and images commissioned in the Netherlands . Before the Reformation in the mid-sixteenth century the interiors of Scottish churches were often elaborate and colourful , with sacrament houses and monumental effigies . Scotland 's ecclesiastical art paid a heavy toll as a result of Reformation iconoclasm , with the almost total loss of medieval stained glass , religious sculpture and paintings . In about 1500 the Scottish monarchy turned to the recording of royal likenesses in panel portraits . More impressive are the works or artists imported from the continent , particularly the Netherlands . The tradition of royal portrait painting in Scotland was probab</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Herbert Ernest Hart = Brigadier General Sir Herbert Ernest Hart KBE , CB , CMG , DSO , VD ( 13 October 1882 – 5 March 1968 ) was an officer in the New Zealand Military Forces who served during the Second Boer War and the First World War . He later served as the Administrator of Western Samoa and worked for the Imperial War Graves Commission . Hart volunteered for the Ninth New Zealand South African Contingent , which was raised for service in South Africa during the Second Boer War . By the time the contingent arrived in South Africa , the war was largely over . He saw extensive action during the First World War as a volunteer with the New Zealand Expeditionary Force , first at Gallipoli and then on the Western Front . By the end of the war , he had advanced in rank to brigadier general , commanding a number of brigades in the New Zealand Division . Trained as a lawyer before the war , Hart returned to New Zealand to resume his legal practice after his discharge from the New Zealand Ex</t>
+          <t>Church architecture in Scotland = Church architecture in Scotland incorporates all church building within the modern borders of Scotland , from the earliest Christian structures in the sixth century until the present day . The early Christian churches for which there is evidence are basic masonry-built constructions on the west coast and islands . As Christianity spread , local churches tended to remain much simpler than their English counterparts . By the eighth century more sophisticated ashlar block-built buildings began to be constructed . From the eleventh century , there were larger and more ornate Romanesque buildings , as with Dunfermline Abbey and St Magnus Cathedral in Orkney . From the twelfth century the introduction of new monastic orders led to a boom in ecclesiastical building , often using English and Continental forms . From the thirteenth century elements of the European Gothic style began to appear in Scotland , cumulating in buildings such as Glasgow Cathedral and t</t>
         </is>
       </c>
     </row>
@@ -1806,32 +1806,32 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>['rainfall', 'meteorological', 'preparations', 'watch', 'florida', 'flooding', 'damage', 'winds', 'hurricane', 'issued', 'reported', 'rain', 'landfall', 'mexico', 'usd']</t>
+          <t>['hebrew', 'text', 'manuscripts', 'gospel', 'jesus', 'manuscript', 'matthew', 'john', 'biblical', 'luke', 'greek', 'printing', 'readings', 'scholars', 'letters']</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Hurricane Odile ( 1984 ) = Hurricane Odile was the second of three tropical storms to make landfall in Mexico during the 1984 Pacific hurricane season . The fifteenth named storm and twelfth hurricane of the active season , it developed from a tropical disturbance about 185 miles ( 300 km ) south of Acapulco on September 17 . Curving towards the northwest , Odile became a Category 1 hurricane on September 19 . The tropical cyclone reached its peak intensity with winds of 105 mph ( 165 km / h ) two days later ; however , Hurricane Odile began to weaken as moved erratically it encountered less favorable conditions and was downgraded to a tropical storm shortly before making landfall northwest of Zihuatanejo . Over land , the storm rapidly weakened , and dissipated on September 23 . The storm caused significant rainfall accumulations of 24.73 inches ( 628.1 mm ) in Southern Mexico , resulting in severe damage to tourism resorts . Flooding from Odile resulted in the evacuation of 7,000 peo</t>
+          <t>Codex Boreelianus = Codex Boreelianus , Codex Boreelianus Rheno-Trajectinus ( full name ) , designated by Fe or 09 in the Gregory-Aland numbering and ε 86 in von Soden numbering , is a 9th ( or 10th ) century uncial manuscript of the four Gospels in Greek . The manuscript , written on parchment , is full of lacunae ( or gaps ) , many of which arose between 1751 and 1830 . The codex was named Boreelianus after Johannes Boreel ( 1577 – 1629 ) , who brought it from the East . The text of the codex represents the majority of the text ( Byzantine text-type ) , but with numerous alien readings ( non-Byzantine ) . Some of its readings do not occur in any other manuscript ( so called singular readings ) . According to the present textual critics its text is not a very important manuscript , but it is quoted in all modern editions of the Greek New Testament . The manuscript was brought from the East at the beginning of the 17th century . It was in private hands for over 100 years . Since 1830 i</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hurricane Able ( 1951 ) = Hurricane Able was a rare hurricane that formed outside of the typical North Atlantic hurricane season . The first tropical cyclone in 1951 , Able developed from a trough of low pressure on May 15 about 300 miles ( 480 km ) south of Bermuda . Initially subtropical in nature , Able acquired tropical characteristics as it moved over the warm waters of the Gulf Stream and attained hurricane status on May 17 off the coast of Florida . This made Able one of only four May Atlantic hurricanes on record . On May 22 Able reached peak winds of 90 mph ( 150 km / h ) about 70 miles ( 115 km ) off of Cape Hatteras , North Carolina . The hurricane weakened as it turned eastward , and became an extratropical cyclone on May 23 . Hurricane Able did not affect land significantly . In Florida , the storm dropped light precipitation , while in the Bahamas it produced winds of up to 95 mph ( 152 km / h ) . From North Carolina through New England , Able produced higher than normal </t>
+          <t>Novum Instrumentum omne = Novum Instrumentum omne was the first published New Testament in Greek ( 1516 ) . It was prepared by Desiderius Erasmus ( 1469 – 1536 ) and printed by Johann Froben ( 1460 – 1527 ) of Basel . Although the first printed Greek New Testament was the Complutensian Polyglot ( 1514 ) , it was the second to be published ( 1522 ) . Erasmus used several Greek manuscripts housed in Basel , but some a few verses in Revelation he translated from the Latin Vulgate . Five editions of Novum Instrumentum omne were published , though its title was changed to Novum Testamentum omne with the second edition , and the name continued . Erasmus issued editions in 1516 , 1519 , 1522 , 1527 , and 1536 . Notable amongst these are the second edition ( 1519 ) , used by Martin Luther for his translation of the New Testament into German , the so-called " September Testament , " and the third edition ( 1522 ) , which was used by Tyndale for the first English New Testament ( 1526 ) and later</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Hurricane Madeline ( 1976 ) = Hurricane Madeline was a Category 4 hurricane that made landfall in Mexico in October 1976 . Madeline formed on September 29 , not far from Central America . The next day , the circulation dissipated , and as a result weakened to a remnant low . Four days later , on October 3 , the low regenerated into a tropical depression . The system remained weak for three days as it drifted west-northwest . When it began to recurve towards Mexico on October 6 , the cyclone rapidly intensified , eventually making landfall at peak intensity as a Category 4 . Shortly after landfall , the cyclone rapidly dissipated . Prior to the arrival of Madeline , 15,000 people evacuated form the coast , which had already been impacted by Hurricane Liza . Heavy damage was reported , along with seven fatalities . Two dams were flooded ; extensive crop damage was reported . = = Meteorological history = = Early on September 27 , 1976 , the Eastern Pacific Hurricane Center ( EPHC ) report</t>
+          <t>Codex Zacynthius = Codex Zacynthius ( designated by siglum Ξ or 040 in the Gregory-Aland numbering ; A1 in von Soden ) is a Greek New Testament codex , dated paleographically to the 6th century . First thought to have been written in the 8th century , it is a palimpsest — the original ( lower ) text was washed off its vellum pages and overwritten in the 12th or 13th century . The upper text of the palimpsest contains weekday Gospel lessons ; the lower text contains portions of the Gospel of Luke , deciphered by biblical scholar and palaeographer Tregelles in 1861 . The lower text is of most interest to scholars . The manuscript came from Zakynthos , a Greek island , and has survived in a fragmentary condition . It was brought to England in 1821 and transferred to Cambridge University in 1985 . It is often cited in critical editions of the Greek New Testament . = = Description = = The lower text of the manuscript contains fragments of the chapters 1 : 1-11 : 33 of the Gospel of Luke . T</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Hurricane Diana ( 1984 ) = Hurricane Diana was the fourth tropical storm , the first hurricane , the first major hurricane , and the strongest storm of the 1984 Atlantic hurricane season . Diana was the first major hurricane to hit the U.S. East Coast in nearly 20 years . Watches and warnings were issued for the storm along the East coast between eastern Florida and Virginia . It caused moderate damage in North Carolina while it looped offshore and after it made landfall as a Category 2 hurricane . Forming on September 8 , Diana moved northward and wandered across North Carolina for a couple of days during mid-September , dropping heavy rainfall . Once it left the state and accelerated east-northeast , Diana quickly evolved into an extratropical cyclone . Damages to the United States totaled $ 65.5 million ( 1984 USD ) . Three indirect fatalities were caused by the cyclone . = = Meteorological history = = The origins of Hurricane Diana can be traced back to a stalled out area of low pr</t>
+          <t>Codex Alexandrinus = The Codex Alexandrinus ( London , British Library , MS Royal 1 . D. V-VIII ; Gregory-Aland no . A or 02 , Soden δ 4 ) is a fifth-century manuscript of the Greek Bible , containing the majority of the Septuagint and the New Testament . It is one of the four Great uncial codices . Along with the Codex Sinaiticus and the Vaticanus , it is one of the earliest and most complete manuscripts of the Bible . Brian Walton assigned Alexandrinus the capital Latin letter A in the Polyglot Bible of 1657 . This designation was maintained when the system was standardized by Wettstein in 1751 . Thus , Alexandrinus held the first position in the manuscript list . It derives its name from Alexandria where it resided for a number of years before it was brought by the Eastern Orthodox Patriarch Cyril Lucaris from Alexandria to Constantinople . Then it was given to Charles I of England in the 17th century . Until the later purchase of Codex Sinaiticus , it was the best manuscript of the</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tropical Storm Elena ( 1979 ) = Tropical Storm Elena was a weak tropical storm that moved ashore along Texas in the 1979 Atlantic hurricane season . The sixth tropical storm of the season , Elena developed from a tropical wave to the south of Louisiana on August 29 . It tracked generally west-northwest , strengthening little before making landfall on Matagorda Island on September 1 as a minimal tropical storm ; the storm quickly dissipated over land . Elena dropped moderate rainfall along its path , causing two direct deaths in Houston from drowning ; storm damage was minor , amounting to less than $ 10 million ( 1979 USD , $ 28 million 2007 USD ) . Lightning from the storm set fire to an oil supertanker in Houston , causing three indirect deaths and 13 injuries . = = Meteorological history = = A tropical wave moved off the coast of Africa on August 17 . It tracked westward , passing through the Lesser Antilles on August 22 , and on August 27 the weak wave axis crossed through Florida </t>
+          <t>Gospel of John = The Gospel According to John ( Greek : Τὸ κατὰ Ἰωάννην εὐαγγέλιον , translit . To kata Iōánnēn euangélion ; also called the Gospel of John , the Fourth Gospel , or simply John ) is one of the four canonical gospels in the New Testament . It traditionally appears fourth , after the synoptic gospels of Matthew , Mark , and Luke . John begins with the witness and affirmation of John the Baptist and concludes with the death , burial , resurrection , and post-resurrection appearances of Jesus . The author is identified as " the Disciple whom Jesus loved " , whom early Christian tradition identified as John the Apostle , one of Jesus ' Twelve Apostles . The gospel is so closely related in style and content to the three surviving Johannine epistles that commentators treat the four books , along with the Book of Revelation , as a single corpus of Johannine literature , but there are some arguments made by modern scholars who believe John the Apostle was not the author of any o</t>
         </is>
       </c>
     </row>
@@ -1841,32 +1841,32 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>['rating', 'office', 'jim', 'dwight', 'episode', 'aired', 'nbc', 'watching', 'nielsen', 'michael', 'pam', 'share', 'rated', 'viewed', 'ratings']</t>
+          <t>['comics', 'story', 'belgian', 'adventures', 'snowy', 'moon', 'brussels', 'cartoonist', 'comic', 'depiction', 'belgium', 'adventure', 'sun', 'explorers', 'book']</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t xml:space="preserve">The Inner Circle ( The Office ) = " The Inner Circle " is the twenty-third episode of the seventh season of the American comedy television series The Office and the show 's 149th episode overall . The episode originally aired on May 5 , 2011 , on NBC . The episode also marked Will Ferrell 's final appearance as Deangelo , having signed up for four episodes . Cody Horn also makes her first guest appearance for the series as Jordan Garfield . The series depicts the everyday lives of office employees in the Scranton , Pennsylvania branch of the fictional Dunder Mifflin Paper Company . In this episode , new office manager Deangelo begins picking favorites among the staff , revealing his true management style . After he only picks men to join his " inner circle " , many of the female staffers begin to believe he is sexist . The episode was written by Charlie Grandy and directed by Matt Sohn . The episode marks the first episode since Steve Carell left the series as a series regular . " The </t>
+          <t>Comics = Comics is a medium used to express ideas by images , often combined with text or other visual information . Comics frequently takes the form of juxtaposed sequences of panels of images . Often textual devices such as speech balloons , captions , and onomatopoeia indicate dialogue , narration , sound effects , or other information . Size and arrangement of panels contribute to narrative pacing . Cartooning and similar forms of illustration are the most common image-making means in comics ; fumetti is a form which uses photographic images . Common forms of comics include comic strips , editorial and gag cartoons , and comic books . Since the late 20th century , bound volumes such as graphic novels , comic albums , and tankōbon have become increasingly common , and online webcomics have proliferated in the 21st century . The history of comics has followed different paths in different cultures . Scholars have posited a pre-history as far back as the Lascaux cave paintings . By the</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Get the Girl = " Get the Girl " is the nineteenth episode of the eighth season of the American comedy television series The Office , and the show 's 171st episode overall . The episode originally aired on NBC in the United States on March 15 , 2012 . " Get the Girl " was written by Charlie Grandy and directed by series regular Rainn Wilson , who portrays Dwight Schrute . The series — presented as if it were a real documentary — depicts the everyday lives of office employees in the Scranton , Pennsylvania , branch of the fictional Dunder Mifflin Paper Company . In the episode , Andy Bernard ( Ed Helms ) drives across the country to get Erin Hannon ( Ellie Kemper ) , who has taken up caring for an elderly woman . Meanwhile , in the Scranton branch , Nellie ( Catherine Tate ) shows up and tries to claim the manager position . " Get the Girl " received mixed reviews by television commentators , with multiple critics criticizing Andy and Erin 's romance . According to Nielsen ratings , " Ge</t>
+          <t>Flash Gordon Strange Adventure Magazine = Flash Gordon Strange Adventure Magazine was a pulp magazine which was launched in December 1936 . It was published by Harold Hersey , and was an attempt to cash in on the growing comics boom , and the popularity of the Flash Gordon comic strip in particular . The magazine contained a novel about Flash Gordon and three unrelated stories ; there were also eight full-page color illustrations . The quality of both the artwork and the fiction was low , and the magazine only saw a single issue . It is now extremely rare . = = Publication history and contents = = Although science fiction ( sf ) had been published before the 1920s , it did not begin to coalesce into a separately marketed genre until the appearance in 1926 of Amazing Stories , a pulp magazine published by Hugo Gernsback . After 1931 , when Miracle Science and Fantasy Stories was launched , no new science fiction magazines appeared for several years . In 1934 a science fiction comic stri</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Cutbacks ( 30 Rock ) = " Cutbacks " is the seventeenth episode of the third season of the American television comedy series 30 Rock , and the 53rd episode of the series overall . It was written by supervising producer Matt Hubbard and directed by Gail Mancuso . The episode originally aired on the National Broadcasting Company ( NBC ) network in the United States on April 9 , 2009 . Guest stars in this episode include Roger Bart , Todd Buonopane , and Don Pardo . In the episode , joy about the fiftieth episode for the fictitious show The Girlie Show with Tracy Jordan ( TGS ) turns to worry when word spreads about imminent budget cuts at the 30 Rock workplace . Before long , Jack Donaghy ( Alec Baldwin ) must fire several employees to save money , NBC page Kenneth Parcell ( Jack McBrayer ) takes on new responsibilities , and Liz Lemon ( Tina Fey ) wheels and deals to spare her staffers from layoffs . Meanwhile , Jenna Maroney ( Jane Krakowski ) and Tracy Jordan ( Tracy Morgan ) suspect t</t>
+          <t>Canadian comics = Canadian comics refers to comics and cartooning by citizens of Canada or permanent residents of Canada regardless of residence . Canada has two official languages , and distinct comics cultures have developed in English and French Canada . The English tends to follow American trends , and the French Franco-Belgian ones , with little crossover between the two cultures . Canadian comics run the gamut of comics forms , including editorial cartooning , comic strips , comic books , graphic novels , and webcomics , and are published in newspapers , magazines , books , and online . They have received attention in international comics communities and have received support from the federal and provincial governments , including grants from the Canada Council for the Arts . There are a comics publishers throughout the country , as well as large small press , self-publishing , and minicomics communities . In English Canada many cartoonists , from Hal Foster to Todd McFarlane , h</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Broke ( The Office ) = " Broke " is the 25th episode of the fifth season of the television series The Office , and the 97th overall episode of the series . It originally aired on NBC in the United States on April 23 , 2009 . In this episode , Michael learns his paper company is broke , and tries to keep this fact a secret when Dunder Mifflin offers to buy out the Michael Scott Paper Company since the company has stolen most of Dunder Mifflin Scranton 's clients . The episode was written by Charlie Grandy and directed by Steve Carell , marking his directorial debut . " Broke " was the last of a six-episode arc involving Michael quitting to start the Michael Scott Paper Company ; it was also the last of six episodes to prominently feature Idris Elba as Dunder Mifflin V.P. Charles Miner . According to Nielsen ratings , it was watched by 7.21 million viewers , and received the season 's lowest rating in the 18 – 49 age group during its regular timeslot to that point in the season . = = Plo</t>
+          <t>10 Story Fantasy = 10 Story Fantasy ( occasionally referred to as Ten Story Fantasy ) was a science fiction and fantasy pulp magazine which was launched in 1951 . The market for pulp magazines was already declining by that time , and the magazine only lasted a single issue . The stories were of generally good quality , and included work by many well-known writers , such as John Wyndham , A.E. van Vogt and Fritz Leiber . The most famous story it published was Arthur C. Clarke 's " Sentinel from Eternity " , which later became part of the basis of the movie 2001 : A Space Odyssey . = = Publication history = = The early 1950s saw dramatic changes in the world of U.S. science fiction ( sf ) publishing . At the start of 1949 , all but one of the major magazines in the field were in pulp format ; by the end of 1955 , almost all had either ceased publication or switched to digest format . Despite the rapid decline of the pulp market , several new science fiction magazines were launched in pul</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Survivor Man = " Survivor Man " is the eleventh episode of the fourth season of the American comedy television series The Office — the show 's sixty-fourth episode overall . Written by Steve Carell , who also acts on the show as Regional Manager Michael Scott , and directed by Paul Feig , it originally aired on NBC on November 8 , 2007 . The episode aired during NBC 's week of " green episodes " , which lasted from November 4 through November 10 , 2007 . In the episode , Ryan excludes Michael from a company nature excursion , prompting Michael to try to prove to himself and his peers that he can survive in the wild . Dwight drops Michael off in the middle of a local wooded area and contrary to Michael 's wishes , stays behind to monitor Michael . Meanwhile , Jim spends the day as boss , but his plan to incorporate multiple birthdays into one combined event ends up alienating the entire office against him . = = Plot = = Ryan Howard ( B. J. Novak ) invites the regional branch managers an</t>
+          <t>Wonder Story Annual = Wonder Story Annual was a science fiction pulp magazine which was launched in 1950 by Standard Magazines . It was created as a vehicle to reprint stories from early issues of Wonder Stories , Startling Stories , and Wonder Stories Quarterly , which were owned by the same publisher . It lasted for four issues , succumbing in 1953 to competition from the growing market for paperback science fiction . Reprinted stories included Twice in Time , by Manly Wade Wellman , and " The Brain-Stealers of Mars " , by John W. Campbell . = = Publication history and contents = = The first science fiction ( sf ) magazine , Amazing Stories , was launched in 1926 by Hugo Gernsback at the height of the pulp magazine era . It helped to form science fiction as a separately marketed genre , and by the mid-1930s several more sf magazines had appeared , including Wonder Stories , also published by Gernsback . In 1936 , Ned Pines of Beacon Publications bought Wonder Stories from Gernsback ,</t>
         </is>
       </c>
     </row>
@@ -1876,32 +1876,32 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>['species', 'small', 'female', 'large', 'male', 'found', 'larger', 'size', 'long', 'shark', 'dorsal', 'head', 'adult', 'waters', 'body']</t>
+          <t>['spacecraft', 'apollo', 'nasa', 'lunar', 'mission', 'orbit', 'launch', 'moon', 'saturn', 'module', 'manned', 'docking', 'landing', 'flight', 'space']</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Coral catshark = The coral catshark ( Atelomycterus marmoratus ) is a species of catshark , and part of the family Scyliorhinidae . It is common on shallow coral reefs across the Indo-West Pacific , from Pakistan to New Guinea . Reaching up to 70 cm ( 28 in ) in length , the coral catshark has an extremely slender body , a short head and tail , and two dorsal fins that are angled backwards . It can be identified by the numerous black and white spots on its back , sides , and fins , which often merge to form horizontal bars . Furthermore , adult males have distinctively long and thin claspers . Reclusive and inactive during the day , at dusk and at night the coral catshark actively forages for small , bottom-living invertebrates and bony fishes . Its slender form allows it to access tight spaces on the reef . It is oviparous : females lay purse-shaped egg capsules two at a time on the bottom , and the young hatch after 4 – 6 months . This small , harmless shark adapts well to captivity </t>
+          <t>Advanced Gemini = Advanced Gemini is a number of proposals that would have extended the Gemini program by the addition of various missions , including manned low Earth orbit , circumlunar and lunar landing missions . Gemini was the second manned spaceflight program operated by NASA , and consisted of a two-seat spacecraft capable of maneuvering in orbit , docking with unmanned spacecraft such as Agena Target Vehicles , and allowing the crew to perform tethered extra-vehicular activities . A range of applications were considered for Advanced Gemini missions , including military flights , space station crew and logistics delivery , and lunar flights . The Lunar proposals ranged from reusing the docking systems developed for the Agena target vehicle on more powerful upper stages such as the Centaur , which could propel the spacecraft to the Moon , to complete modifications of the Gemini to enable it to land on the Lunar surface . Its applications would have ranged from manned lunar flybys</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Bigeye sand tiger = The bigeye sand tiger ( Odontaspis noronhai ) is an extremely rare species of mackerel shark in the family Odontaspididae , with a possible worldwide distribution . A large , bulky species reaching at least 3.6 m ( 12 ft ) in length , the bigeye sand tiger has a long bulbous snout , large orange eyes without nictitating membranes , and a capacious mouth with the narrow teeth prominently exposed . It can be distinguished from the similar smalltooth sand tiger ( O. ferox ) by its teeth , which have only one lateral cusplet on each side , and by its uniformly dark brown color . Inhabiting continental margins and oceanic waters at depths of 60 – 1,000 m ( 200 – 3,280 ft ) , the bigeye sand tiger may make vertical and horizontal migratory movements . It feeds on bony fishes and squid , and its sizable eyes and dark coloration suggest that it may spend most of its time in the mesopelagic zone . Reproduction is probably viviparous with oophagous embryos like in other macke</t>
+          <t>Soyuz TM-30 = Soyuz TM-30 ( Russian : Союз ТМ-30 , Union TM-30 ) , also known as Mir EO-28 , was a Soyuz mission , the 39th and final human spaceflight to the Mir space station . The crew of the mission was sent by MirCorp , a privately funded company , to reactivate and repair the station . The crew also resupplied the station and boosted the station to an orbit with a low point ( perigee ) of 360 and a high point ( apogee ) of 378 kilometers ( 223 and 235 miles , respectively ) . The boost in the station 's orbit , which was done by utilizing the engines of the Progress M1-1 and M1-2 spacecraft , made transit between Mir and the International Space Station impossible , as desired by NASA . The mission was the first privately funded mission to a space station . The mission was part of an effort by MirCorp to refurbish and privatize the aging Mir space station , which was nearing the end of its operational life . Further commercially funded missions beyond Soyuz TM-30 were originally p</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Blacknose shark = The blacknose shark ( Carcharhinus acronotus ) is a species of requiem shark , belonging to the family Carcharhinidae , common in the tropical and subtropical waters of the western Atlantic Ocean . This species generally inhabits coastal seagrass , sand , or rubble habitats , with adults preferring deeper water than juveniles . A small shark typically measuring 1.3 m ( 4.3 ft ) long , the blacknose has a typical streamlined " requiem shark " shape with a long , rounded snout , large eyes , and a small first dorsal fin . Its common name comes from a characteristic black blotch on the tip of its snout , though this may be indistinct in older individuals . Blacknose sharks feed primarily on small bony fishes and cephalopods , and in turn fall prey to larger sharks . Like other members of their family , they exhibit a viviparous mode of reproduction in which the developing embryos are sustained by a placental connection . The females give birth to three to six young in la</t>
+          <t xml:space="preserve">Apollo program = The Apollo program , also known as Project Apollo , was the third United States human spaceflight program carried out by the National Aeronautics and Space Administration ( NASA ) , which accomplished landing the first humans on the Moon from 1969 to 1972 . First conceived during Dwight D. Eisenhower 's administration as a three-man spacecraft to follow the one-man Project Mercury which put the first Americans in space , Apollo was later dedicated to President John F. Kennedy 's national goal of " landing a man on the Moon and returning him safely to the Earth " by the end of the 1960s , which he proposed in an address to Congress on May 25 , 1961 . Kennedy 's goal was accomplished on the Apollo 11 mission when astronauts Neil Armstrong and Buzz Aldrin landed their Lunar Module ( LM ) on July 20 , 1969 , and walked on the lunar surface , while Michael Collins remained in lunar orbit in the Command / Service Module ( CSM ) , and all three landed safely on Earth on July </t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Leopard shark = The leopard shark ( Triakis semifasciata ) is a species of houndshark , in the family Triakidae . It is found along the Pacific coast of North America , from the U.S. state of Oregon to Mazatlán in Mexico . Typically measuring 1.2 – 1.5 m ( 3.9 – 4.9 ft ) long , this slender-bodied shark is immediately identifiable by the striking pattern of black saddle-like markings and large spots over its back , from which it derives its common name . Large schools of leopard sharks are a common sight in bays and estuaries , swimming over sandy or muddy flats or rock-strewn areas near kelp beds and reefs . They are most common near the coast , in water less than 4 m ( 13 ft ) deep . Active-swimming predators , groups of leopard sharks often follow the tide onto intertidal mudflats to forage for food , mainly clams , spoon worms , crabs , shrimp , bony fish , and fish eggs . Most leopard sharks tend to remain within a particular area rather than undertaking long movements elsewhere ,</t>
+          <t>Space Interferometry Mission = The Space Interferometry Mission , or SIM , also known as SIM Lite ( formerly known as SIM PlanetQuest ) , was a planned space telescope developed by the U.S. National Aeronautics and Space Administration ( NASA ) , in conjunction with contractor Northrop Grumman . One of the main goals of the mission was the hunt for Earth-sized planets orbiting in the habitable zones of nearby stars other than the Sun . SIM was postponed several times and finally cancelled in 2010 . In addition to hunting for extrasolar planets , SIM would have helped astronomers construct a map of the Milky Way galaxy . Other important tasks would have included collecting data to help pinpoint stellar masses for specific types of stars , assisting in the determination of the spatial distribution of dark matter in the Milky Way and in the Local Group of galaxies and using the gravitational microlensing effect to measure the mass of stars . The spacecraft would have used optical interfer</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Horn shark = The horn shark ( Heterodontus francisci ) is a species of bullhead shark , in the family Heterodontidae . It is endemic to the coastal waters off the western coast of North America , from California to the Gulf of California . Young sharks are segregated spatially from the adults , with the former preferring deeper sandy flats and the latter preferring shallower rocky reefs or algal beds . A small species typically measuring 1 m ( 3.3 ft ) in length , the horn shark can be recognized by a short , blunt head with ridges over its eyes , two high dorsal fins with large spines , and a brown or gray coloration with many small dark spots . Slow-moving , generally solitary predators , horn sharks hunt at night inside small home ranges and retreat to a favored shelter during the day . Their daily activity cycles are controlled by environmental light levels . Adult sharks prey mainly on hard-shelled molluscs , echinoderms , and crustaceans , which they crush between powerful jaws a</t>
+          <t>STS-8 = STS-8 was the eighth NASA Space Shuttle mission and the third flight of the Space Shuttle Challenger . It launched on August 30 , 1983 and landed on September 5 , conducting the first night launch and night landing of the Space Shuttle program . It also carried the first African-American astronaut , Guion Bluford . The mission successfully achieved all of its planned research objectives , but was marred by the subsequent discovery that a solid-fuel rocket booster had almost malfunctioned catastrophically during the launch . The mission 's primary payload was INSAT-1B , an Indian communications and weather observation satellite , which was released by the orbiter and boosted into a geostationary orbit . The secondary payload , replacing a delayed NASA communications satellite , was a four-metric-ton dummy payload , intended to test the use of the shuttle 's " Canadarm " remote manipulator system . Scientific experiments carried onboard Challenger included the environmental testi</t>
         </is>
       </c>
     </row>
@@ -1911,32 +1911,32 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>['ride', 'train', 'coaster', 'roller', 'riders', 'station', 'steel', 'trains', 'lift', 'operate', 'hour', 'brake', 'drop', 'themed', 'officially']</t>
+          <t>['phillies', 'inning', 'yankees', 'dodgers', 'giants', 'yankee', 'breaker', 'innings', 'tie', 'pitcher', 'run', 'braves', 'game', 'runs', 'pennant']</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Green Lantern Coaster = Green Lantern Coaster is a steel roller coaster at Warner Bros. Movie World on the Gold Coast , Queensland , Australia . The ride is themed after DC Comics ' Green Lantern and is located within the park 's DC Comics superhero hub . The ride is an El Loco roller coaster manufactured by S &amp; S Worldwide , characterised by a tight circuit featuring a beyond-vertical drop and an outward banked turn . It holds the record for the steepest drop of any roller coaster in the Southern Hemisphere , and the second steepest in the world . Green Lantern Coaster officially opened on 23 December 2011 . = = History = = In May 2011 , preliminary groundwork began on a plot of land in front of Warner Bros. Movie World . On 31 July 2011 , the firm announced a multimillion-dollar attraction coming before Christmas 2011 . In early September , pieces of S &amp; S Worldwide roller coaster track began appearing in the car park . On 13 September 2011 , Warner Bros. Movie World began releasing </t>
+          <t>2013 American League Wild Card tie-breaker game = The 2013 American League Wild Card tie-breaker game was a one-game extension to Major League Baseball 's ( MLB ) 2013 regular season , played between the Texas Rangers and Tampa Bay Rays to determine the second participant in the 2013 American League ( AL ) Wild Card Game . It was played at the Rangers Ballpark in Arlington on September 30 , 2013 . The Rays defeated the Rangers , 5 – 2 , and advanced to the AL Wild Card Game against the Cleveland Indians at Progressive Field , which they won 4 – 0 ; the Rangers failed to qualify for the postseason . The tie-breaker game was necessary after both teams finished the season with win – loss records of 91 – 71 and thus tied for the second Wild Card position in the AL . The Rangers were awarded home field for the game , as they won the regular season series against the Rays , four-games-to-three . The game was televised on TBS . It was the fourth tie-breaker in MLB history for a Wild Card spot</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Dive Coaster = The Dive Coaster is a steel roller coaster manufactured by Bolliger &amp; Mabillard where riders experience a moment of free-falling with at least one 90-degree drop . Unlike other roller coasters where the lift hill takes the train directly to the first drop , a Dive Coaster lift hill leads to a flat section of track followed by a holding brake which stops the train just as it enters the vertical drop . After a few seconds , the train is released into the drop . Development of the Dive Coaster began between 1994 and 1995 with Oblivion at Alton Towers opening on March 14 , 1998 , making it the world 's first Dive Coaster . The trains for this type of coaster are relatively short consisting of two to three cars . Bolliger &amp; Mabillard have recently begun to also use floorless trains on this model to enhance the experience . As of May 2016 , ten Dive Coasters have been built , with the newest being Valravn at Cedar Point . = = History = = According to Walter Bolliger , developm</t>
+          <t>2014 National League Wild Card Game = The 2014 National League Wild Card Game was a play-in game during Major League Baseball 's ( MLB ) 2014 postseason played between the National League 's ( NL ) two wild card teams , the San Francisco Giants and the Pittsburgh Pirates . It was held at PNC Park in Pittsburgh , Pennsylvania , on October 1 , 2014 , starting at 8 : 07 p.m. EDT . After both teams finished the regular season with identical records of 88 – 74 , the Pirates were awarded home field for the game , as they won the season series against the Giants , four games to two . Despite this advantage , the Giants won by a score of 8 – 0 and advanced to play the Washington Nationals in the NL Division Series ( NLDS ) . In addition to being the third NL Wild Card Game played , it is notable for the first postseason grand slam hit by a shortstop . The game was televised on ESPN , and was also broadcast on ESPN Radio . = = Background = = In Major League Baseball , the two teams with the bes</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Patriot ( Worlds of Fun ) = Patriot is a steel inverted roller coaster designed by Bolliger &amp; Mabillard at the Worlds of Fun amusement park in Kansas City , Missouri . Announced on September 7 , 2005 , the roller coaster opened to the public on April 8 , 2006 . The ride lasts about 2 minutes and 18 seconds and features four inversions , a maximum height of 149 feet ( 45 m ) and a length of 3,081 feet ( 939 m ) . = = History = = Patriot was announced on September 7 , 2005 and was the park 's largest investment at the time . Construction started in the transfer track and station area before progressing to the lift hill in early-October 2005 . Just over two weeks later , the roller coaster 's 149-foot ( 45 m ) lift hill was topped off . After erecting the first drop and loop , construction on the zero-gravity-roll was complete by mid-November . The third inversion , and Immelmann loop , was completed about a week later followed by the placement of the inclined loop pieces . After the cork</t>
+          <t>1951 National League tie-breaker series = The 1951 National League tie-breaker series was a best-of-three playoff series at the conclusion of Major League Baseball 's ( MLB ) 1951 regular season to decide the winner of the National League ( NL ) pennant . The games were played on October 1 , 2 , and 3 , 1951 , between the New York Giants and Brooklyn Dodgers . It was necessary after both teams finished the season with identical win – loss records of 96 – 58 . It is most famous for the walk-off home run hit by Bobby Thomson of the Giants in the deciding game , which has come to be known as baseball 's " Shot Heard ' Round the World " . This was the second three-game playoff in NL history . After no tiebreakers had been needed since the American League ( AL ) became a major league in 1901 , this was the third such tie in the previous six seasons . The Dodgers had been involved in the previous one as well , losing to the St. Louis Cardinals during the 1946 season in two straight games . I</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t xml:space="preserve">NSB Class 93 = NSB Class 93 ( Norwegian : NSB-type 93 ) is a tilting two-carriage diesel multiple unit used by Norwegian State Railways ( NSB ) for passenger trains on non-electrified stretches of the Norwegian railway network . Used on the Nordland Line , the Røros Line and the Rauma Line , they were purchased to replace the aging Di3 locomotive-hauled trains . The Class 93 was produced by Bombardier , and is part of the Talent family . Fifteen units were delivered between 2000 and 2002 . Powered by two Cummins diesel engines with a combined output of 612 kW ( 821 hp ) , the trains are capable of speeds of 140 km / h ( 87 mph ) . The trains entered service as part of the Agenda regional train concept . However , the technical problems to which the units have been prone and a cramped interior design have made them unpopular among riders . In 2007 , the units were replaced by locomotive-hauled trains on some services on the Nordland Line . = = History = = During the mid-1990s , NSB had </t>
+          <t xml:space="preserve">1999 National League Wild Card tie-breaker game = The 1999 National League wild-card tie-breaker game was a one-game extension to Major League Baseball 's ( MLB ) 1999 regular season , played between the New York Mets and Cincinnati Reds to determine the winner of the National League ( NL ) wild card . It was played at Cinergy Field in Cincinnati , on October 4 , 1999 . The Mets won the game 5 – 0 , with starting pitcher Al Leiter pitching a two-hit shutout . As a result , the Mets qualified for the postseason and the Reds did not . The game was necessary after both teams finished the season with identical win – loss records of 96 – 66 . Some described the Mets as collapsing late in the season while the race between the Reds and their division rival Houston Astros was close enough to create the possibility of a three-way tie . The Reds won a coin flip late in the season which , by rule at the time , awarded them home field for the game . Upon winning , the Mets advanced to NL Division </t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Magnum XL-200 = Magnum XL-200 , colloquially known as simply Magnum , is a steel roller coaster built by Arrow Dynamics at Cedar Point in Sandusky , Ohio . When built in 1989 , it was the tallest , fastest , and steepest complete-circuit roller coaster in the world as well as the first hypercoaster – a roller coaster that exceeds 200 feet ( 61 m ) in height . Some have credited Magnum with starting a period in the industry known as the roller coaster wars , in which amusement parks competed with one another at a rapid pace to build the next tallest and fastest roller coaster . More than 40 million people had ridden Magnum as of 2009 . Magnum XL-200 held the title of tallest roller coaster in the world until 1994 when Pepsi Max Big One opened at Blackpool Pleasure Beach in the United Kingdom . Amusement Today presented Magnum with its " Best Steel Roller Coaster " Golden Ticket Award for three consecutive years in a row from 1998 to 2000 . As of 2014 , it was ranked thirteenth in the wo</t>
+          <t xml:space="preserve">1959 National League tie-breaker series = The 1959 National League tie-breaker series was a best-of-three playoff series at the conclusion of Major League Baseball 's ( MLB ) 1959 regular season to decide the winner of the National League ( NL ) pennant . The games were played on September 28 and 29 , 1959 , between the Los Angeles Dodgers and the Milwaukee Braves . The first game was played at Milwaukee County Stadium and the second took place at Los Angeles Memorial Coliseum . The playoff series was necessary after both teams finished the season with identical win – loss records of 86 – 68 . The Dodgers won a coin flip late in the season that gave them home field advantage for the series , although the series did not reach a third game . Following a rain-delayed start , the Dodgers won Game 1 by a close 3 – 2 score , with a home run by John Roseboro providing the margin of victory . The Dodgers then won the series and the pennant with another close victory in Game 2 ; they came back </t>
         </is>
       </c>
     </row>
@@ -1946,32 +1946,32 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>['building', 'church', 'stone', 'wall', 'built', 'site', 'listed', 'roof', 'windows', 'century', 'walls', 'buildings', 'tower', '19th', 'restoration']</t>
+          <t>['amendment', 'shall', 'constitution', 'clause', 'defendant', 'states', 'rights', 'congress', 'jury', 'amendments', 'ratification', 'constitutional', 'supreme_court', 'senate', 'convention']</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Pyramid of Userkaf = The pyramid complex of Userkaf was built c . 2490 BC for the pharaoh Userkaf ( reign 2494 – 2487 BC ) , founder of the 5th dynasty of Egypt ( c . 2494 – 2345 BC ) . It is located in the pyramid field at Saqqara , on the north-east of the step pyramid of Djoser ( reigned ca . 2670 BC ) . Constructed in dressed stone with a core of rubble , the pyramid is now ruined and resembles a conical hill in the sands of Saqqara . For this reason , it is known locally as El-Haram el-Maharbish , the " Heap of Stone " and was recognized as a royal pyramid by western archaeologists in the 19th century . Userkaf 's pyramid is part of a larger mortuary complex comprising a mortuary temple , an offering chapel and a cult pyramid as well as separate pyramid and mortuary temple for Userkaf 's wife , queen Neferhetepes . Userkaf 's mortuary temple and cult pyramid are today completely ruined and difficult to recognize . The pyramid of the queen is no more than a mound of rubble , with i</t>
+          <t>Crimes Act of 1790 = The Crimes Act of 1790 ( or the Federal Criminal Code of 1790 ) , formally titled An Act for the Punishment of Certain Crimes Against the United States , defined some of the first federal crimes in the United States and expanded on the criminal procedure provisions of the Judiciary Act of 1789 . The Crimes Act was a " comprehensive statute defining an impressive variety of federal crimes . " As an enactment of the First Congress , the Crimes Act is often regarded as a quasi-constitutional text . The punishment of treason , piracy , counterfeiting , as well as crimes committed on the high seas or against the law of nations , followed from relatively explicit constitutional authority . The creation of crimes within areas under exclusive federal jurisdiction followed from the plenary power of Congress over the " Seat of the Government , " federal enclaves , and federal territories . The creation of crimes involving the integrity of the judicial process derived from Co</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>St Mary 's Church , Bodewryd = St Mary 's Church , Bodewryd is a small medieval church in the hamlet of Bodewryd , in Anglesey , north Wales . The date of construction is unknown , but there was a church on this site in 1254 and the earliest feature to which a date can be given is a doorway in a 15th-century style dating to around 1500 . When the church was restored in 1867 after being struck by lightning , stained glass with Islamic-influenced patterns was included in the windows , a requirement of Lord Stanley of Alderley , the church 's benefactor , who was a convert to Islam . The church is used for worship by the Church in Wales , and is one of five churches in a combined parish . It is a Grade II listed building , a national designation given to " buildings of special interest , which warrant every effort being made to preserve them " , in particular because it is a " simple , rural church of Medieval origins . " = = History and location = = The date of foundation of the first re</t>
+          <t xml:space="preserve">United States constitutional criminal procedure = The United States Constitution contains several provisions regarding the law of criminal procedure . Petit jury and venue provisions — both traceable to enumerated complaints in the Declaration of Independence — are included in Article Three of the United States Constitution . More criminal procedure provisions are contained in the United States Bill of Rights , specifically the Fifth , Sixth , and Eighth Amendments . With the exception of the Grand Jury Clause of the Fifth Amendment , the Vicinage Clause of the Sixth Amendment , and ( maybe ) the Excessive Bail Clause of the Eighth Amendment , all of the criminal procedure provisions of the Bill of Rights have been incorporated to apply to the state governments . Several of these rights regulate pre-trial procedure : access to a non-excessive bail , the right to indictment by a grand jury , the right to an information ( charging document ) , the right to a speedy trial , and the right </t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t xml:space="preserve">St Cwyllog 's Church , Llangwyllog = St Cwyllog 's Church , Llangwyllog is a medieval church near Llangwyllog , in Anglesey , north Wales . St Cwyllog founded a church here in the 6th century , although the exact date is unknown . The existence of a church here was recorded in 1254 and parts of the present building may date from around 1200 . Other parts are from the 15th century , with an unusual annexe ( possibly intended for use as a schoolroom ) added in the 16th century . The church contains some 18th-century fittings , including a rare Georgian three-decker pulpit and reading desk . The church is still in use for worship by the Church in Wales , as one of seven churches in a combined group of parishes . It is a Grade II * listed building , a national designation given to " particularly important buildings of more than special interest " , because it is regarded as a " good rural medieval church " with some features from the 15th century , as well as the 18th-century fittings . = </t>
+          <t>Vicinage Clause = The Vicinage Clause is a provision in the Sixth Amendment to the United States Constitution regulating the vicinity from which a jury pool may be selected . The clause says that the accused shall be entitled to a jury " of the State and district wherein the crime shall have been committed , which district shall have been previously ascertained by law " . The Vicinage Clause limits the vicinity of criminal jury selection to both the state and the federal judicial district where the crime has been committed whereas the venue provision of Article Three of the United States Constitution regulates the location of the actual trial . The Vicinage clause has its roots in medieval English criminal procedure , the perceived abuses of criminal vicinage and venue during the colonial period and Anti-federalist objections to the United States Constitution . The clause is one of the few constitutional criminal procedure provisions that has not been incorporated to apply to proceedin</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t xml:space="preserve">St Beuno 's Church , Trefdraeth = St Beuno 's Church , Trefdraeth is the medieval parish church of Trefdraeth , a hamlet in Anglesey , north Wales . Although one 19th-century historian recorded that the first church on this location was reportedly established in about 616 , no part of any 7th-century structure survives ; the oldest parts of the present building date are from the 13th century . Alterations were made in subsequent centuries , but few of them during the 19th century , a time when many other churches in Anglesey were rebuilt or were restored . St Beuno 's is part of the Church in Wales , and its parish is one in a group of four . The church remains in use but as of 2013 there is no parish priest . It is a Grade II * listed building , a national designation for " particularly important buildings of more than special interest " , in particular because it is regarded as " an important example of a late Medieval rural church " with an unaltered simple design . = = History and </t>
+          <t>Section Thirty-four of the Canadian Charter of Rights and Freedoms = Section 34 of the Canadian Charter of Rights and Freedoms is the last section of Canada 's Charter of Rights , which is entrenched in the Constitution Act , 1982 . Section 34 provides guidance for the legal citation of the Charter . The section has been interpreted by Canadian writers , who have analyzed both its intention and its meaning . Because the section affirms the name of the Charter and thus entrenches it in the Constitution Act , it came into focus in 1994 when a Member of Parliament ( MP ) proposed to change the name of the Charter . = = Text = = Under the heading " Citation , " the section reads : = = Function = = Section 34 , as part of the Constitution Act , 1982 , came into force on April 17 , 1982 . According to the government of Canada , section 34 's function " simply " relates to citation . The section clarifies that the first 34 sections of the Constitution Act , 1982 may be collectively called the</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Uppsala Cathedral = Uppsala Cathedral ( Swedish : Uppsala domkyrka ) is a cathedral located between Uppsala University and the River Fyris in the centre of Uppsala , southeastern Sweden . Controlled by the Lutheran Church of Sweden , Uppsala Cathedral is the seat of the Archbishop of Uppsala , the primate of Sweden . The archbishop is Antje Jackelén and the current bishop is Ragnar Persenius . The cathedral dates to the late 13th century and at a height of 118.7 metres ( 389 ft ) , it is the tallest church in the Nordic countries . Originally built under Roman Catholicism , it was used for coronations of Swedish monarchs for a lengthy period following the Protestant Reformation . Several of its chapels were converted to house the tombs of Swedish monarchs , including Gustav Vasa and John III . Carl Linnaeus , Olaus Rudbeck , Emanuel Swedenborg , and several archbishops are also buried here . The church was designed in the French Gothic style by French architects including Étienne de Bo</t>
+          <t>Fifteenth Amendment to the United States Constitution = The Fifteenth Amendment ( Amendment XV ) to the United States Constitution prohibits the federal and state governments from denying a citizen the right to vote based on that citizen 's " race , color , or previous condition of servitude . " It was ratified on February 3 , 1870 , as the third and last of the Reconstruction Amendments . In the final years of the American Civil War and the Reconstruction Era that followed , Congress repeatedly debated the rights of the millions of black former slaves . By 1869 , amendments had been passed to abolish slavery and provide citizenship and equal protection under the laws , but the election of Ulysses S. Grant to the presidency in 1868 convinced a majority of Republicans that protecting the franchise of black voters was important for the party 's future . After rejecting more sweeping versions of a suffrage amendment , Congress proposed a compromise amendment banning franchise restrictions</t>
         </is>
       </c>
     </row>
@@ -1981,32 +1981,32 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>['battle', 'men', 'army', 'troops', 'french', 'command', 'general', 'british', 'sent', 'attack', 'soldiers', 'forces', 'wounded', 'killed', 'commanded']</t>
+          <t>['singapore', 'law', 'judicial', 'parliament', 'constitution', 'article', 'courts', 'minister', 'court', 'constitutional', 'high_court', 'persons', 'public', 'tribunal', 'act']</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Battle of Chelsea Creek = The Battle of Chelsea Creek was the second military engagement of the Boston campaign of the American Revolutionary War . It is also known as the Battle of Noddle 's Island , Battle of Hog Island and the Battle of the Chelsea Estuary . This battle was fought on May 27 and 28 , 1775 , on Chelsea Creek and on salt marshes , mudflats , and islands of Boston Harbor , northeast of the Boston peninsula . Most of these areas have since been united with the mainland by land reclamation and are now part of East Boston , Chelsea , Winthrop , and Revere . The American colonists met their goal of strengthening the siege of Boston by removing livestock and hay on those islands from the reach of the British regulars . The British armed schooner Diana was also destroyed and its weaponry was appropriated by the Colonial side . This was the first naval capture of the war , and it was a significant boost to the morale of the Colonial forces . = = Background = = The Battle of Le</t>
+          <t>Article 14 of the Constitution of Singapore = Article 14 of the Constitution of the Republic of Singapore , specifically Article 14 ( 1 ) , guarantees to Singapore citizens the rights to freedom of speech and expression , peaceful assembly without arms , and association . However , the enjoyment of these rights may be restricted by laws imposed by the Parliament of Singapore on the grounds stated in Article 14 ( 2 ) of the Constitution . There are two types of grounds . For the first type , it must be shown that restricting the rights is " necessary or expedient in the interest " of the grounds . The grounds are the security of Singapore and public order ( applicable to all three rights protected by Article 14 ( 1 ) ) , morality ( freedom of speech and freedom of association ) , and friendly relations with other countries ( freedom of speech only ) . In a 2005 judgment , the High Court expressed the view that the phrase necessary or expedient confers upon Parliament " an extremely wide</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Battle of Machias = The Battle of Machias ( also known as the Battle of the Margaretta ) was the second naval engagement of the American Revolutionary War , the Battle off Fairhaven being the first . It took place on June 11 – 12 , 1775 , in and around the port of Machias in what is now eastern Maine , and resulted in the capture by Patriot militia of a British schooner . Following the outbreak of the war and the start of the Siege of Boston , British authorities enlisted the assistance of Loyalist merchant Ichabod Jones to assist in the acquisition of needed supplies . Two of Jones ' merchant ships arrived in Machias on June 2 , accompanied by the British armed sloop Margaretta , commanded by midshipman James Moore . The townspeople , unhappy with Jones ' business practices , decided to arrest him , and in the attempt , decided to go after Moore and his ship . Moore was able to escape out of the harbor , but the townspeople seized one of Jones ' ships , armed it and a second local shi</t>
+          <t>Rule of law doctrine in Singapore = In Singapore , the rule of law doctrine has been the topic of considerable disagreement and debate , largely through differing conceptions of the doctrine . These conceptions can generally be divided into two categories developed by legal academics , the " thin " , or formal , conception and the " thick " , or substantive , conception of the rule of law . The thin conception , often associated with the legal scholars Albert Venn Dicey and Joseph Raz , advocates the view that the rule of law is fulfilled by adhering to formal procedures and requirements , such as the stipulations that all laws be prospective , clear , stable and constitutionally enacted , and that the parties to legal disputes are treated equally and without bias on the part of judges . While people subscribing to the thin conception do not dismiss the importance of the content of the law , they take the view that this is a matter of substantive justice and should not be regarded as p</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Honoré Théodore Maxime Gazan de la Peyrière = Honoré Théodore Maxime Gazan de la Peyrière ( October 29 , 1764 – April 9 , 1845 ) was a French general who fought in the French Revolutionary Wars and the Napoleonic Wars . Gazan started his military career as a cannonier in the French Coast Guard . He was later appointed to the Royal Life Guards and , upon the beginning of the French Revolution in 1789 , he joined the French National Guard . After service in the Upper Rhine valley and the Netherlands , he joined André Masséna in Switzerland in 1799 , and fought at the battles of Winterthur and First Zurich . In August 1805 , Gazan commanded of a division of the Army that encircled the Austrians in Ulm . On November 11 , under Joseph Mortier , his division provided the advance guard in the advance on Vienna . Mortier over-extended his line of march and Gazan 's division was surrounded by Kutuzov 's Coalition army ; Gazan lost 40 percent of his force in the Battle of Dürenstein . Following </t>
+          <t xml:space="preserve">Article 9 of the Constitution of Singapore = Article 9 of the Constitution of the Republic of Singapore , specifically Article 9 ( 1 ) , guarantees the right to life and the right to personal liberty . The Court of Appeal has called the right to life the most basic of human rights , but has yet to fully define the term in the Constitution . Contrary to the broad position taken in jurisdictions such as Malaysia and the United States , the High Court of Singapore has said that personal liberty only refers to freedom from unlawful incarceration or detention . Article 9 ( 1 ) states that persons may be deprived of life or personal liberty " in accordance with law " . In Ong Ah Chuan v. Public Prosecutor ( 1980 ) , an appeal to the Judicial Committee of the Privy Council from Singapore , it was held that the term law means more than just legislation validly enacted by Parliament , and includes fundamental rules of natural justice . Subsequently , in Yong Vui Kong v. Attorney-General ( 2011 </t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Battle of Bloody Creek ( 1711 ) = The Battle of Bloody Creek was fought on 10 / 21 June 1711 during Queen Anne 's War . An Abenaki militia successfully ambushed British and New England soldiers at a place that became known as Bloody Creek after the battles fought there . The creek empties into the Annapolis River at present day Carleton Corner , Nova Scotia , and was also the location of a battle in 1757 . The battle was part of an orchestrated attempt by the leaders of New France to weaken the British hold on Annapolis Royal . The British had only captured the fort the previous year and they only had a very tenuous control of the area . The battle , in which the entire British force was captured or killed , emboldened the French and their native allies to blockade Annapolis Royal . Without heavy weapons , the force was unable to effectively attack the fort , and abandoned the siege when British reinforcements arrived by sea . = = Background = = Port Royal , the capital of the French c</t>
+          <t>Article 12 of the Constitution of Singapore = Article 12 of the Constitution of the Republic of Singapore guarantees to all persons equality before the law and equal protection of the law . The Article also identifies four forbidden classifications – religion , race , descent and place of birth – upon which Singapore citizens may not be discriminated for specific reasons . For example , discrimination on those classifications is prohibited in the appointment to any office or employment under a public authority or in the administration of any law relating to the establishing or carrying on of any trade , business , profession , vocation or employment . Persons unable to show that one of the forbidden classifications applies to them may try to argue that they are members of a group defined by a law in a way that violates the general guarantee of equality and equal protection . To succeed , they must establish that the classification used in the law fails the rational nexus test , which i</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Battle of Solachon = The Battle of Solachon was fought in 586 CE in northern Mesopotamia between the East Roman ( Byzantine ) forces , led by Philippicus , and the Sassanid Persians under Kardarigan . The engagement was part of the long and inconclusive Byzantine – Sassanid War of 572 – 591 . The Battle of Solachon ended in a major Byzantine victory which improved the Byzantine position in Mesopotamia , but it was not in the end decisive . The war dragged on until 591 , when it ended with a negotiated settlement between Maurice and the Persian shah Khosrau II ( r . 590 – 628 ) . In the days before the battle , Philippicus , newly assigned to the Persian front , moved to intercept an anticipated Persian invasion . He chose to deploy his army at Solachon , controlling the various routes of the Mesopotamian plain , and especially access to the main local watering source , the Arzamon river . Kardarigan , confident of victory , advanced against the Byzantines , but they had been warned and</t>
+          <t>Section 3 of the Human Rights Act 1998 = Section 3 of the Human Rights Act 1998 is a provision of the Human Rights Act 1998 that enables the Act to take effect in the United Kingdom . The section requires courts to interpret both primary and subordinate legislation so that their provisions are compatible with the articles of the European Convention of Human Rights , which are also part of the Human Rights Act 1998 . This interpretation goes far beyond normal statutory interpretation , and includes past and future legislation , therefore preventing the Human Rights act from being impliedly repealed by subsequent contradictory legislation . Courts have applied section 3 of the Act through three forms of interpretation : " reading in " – inserting words where there are none in a statute ; " reading out " where words are omitted from a statute ; and " reading down " where a particular meaning is chosen to be in compliance . They do not interpret statutes to conflict with legislative intent</t>
         </is>
       </c>
     </row>
@@ -2016,32 +2016,32 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>['championship', 'match', 'title', 'defeated', 'event', 'team', 'face', 'won', 'night', 'following', 'kane', 'attacked', 'main', 'wrestler', 'win']</t>
+          <t>['motorway', 'croatia', 'toll', 'croatian', 'traffic', 'interchanges', 'kilometre', 'route', 'interchange', 'section', 'rest', 'kilometres', 'areas', 'tunnels', 'construction']</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t xml:space="preserve">John Morrison ( wrestler ) = John Randall Hennigan ( born October 3 , 1979 ) is an American professional wrestler and actor , who is best known for his tenure with the WWE where he was better known by his ring names John Morrison and Johnny Nitro . He currently wrestles for Lucha Underground under the ring name Johnny Mundo . Hennigan entered Tough Enough III , a televised competition that would award the winner a WWE contract . Hennigan won the competition and was assigned to their developmental territory , Ohio Valley Wrestling ( OVW ) , to continue his wrestling training . While situated at OVW , he adopted the ring name Johnny Nitro and was placed in a tag team with Joey Mercury . The duo won the OVW Southern Tag Team Championship and alongside their manager Melina , the stable was called MNM . After signing with WWE , MNM was called up to the SmackDown ! roster and on their debut match in April 2005 , Hennigan and Mercury won the WWE Tag Team Championship . In 2005 , Hennigan won </t>
+          <t xml:space="preserve">A5 ( Croatia ) = The A5 motorway ( Croatian : Autocesta A5 ) is a motorway in Croatia spanning 55.5 kilometres ( 34.5 mi ) . It connects Osijek , the largest city in Slavonia region , to the Croatian motorway network at the Sredanci interchange of the A3 motorway . The A5 represents a significant north – south transportation corridor in Croatia and is a part of the European route E73 . The A5 motorway route also follows Pan-European corridor Vc . In addition to Osijek , the A5 motorway also passes near Đakovo . The first section of the A5 , joining the Sredanci interchange to Đakovo , was opened in 2007 ; the route to Osijek opened in 2009 . As of September 2011 , the section south of the A3 , extending to the Sava River and border of Bosnia and Herzegovina , is under construction . Once the entire Pan-European corridor Vc is completed , motorists will recognize the A5 's importance as a transit route . When completed , the corridor shall entail the A5 itself extended to the Hungarian </t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>The Great American Bash ( 2004 ) = The Great American Bash ( 2004 ) was the 15th Great American Bash professional wrestling pay-per-view event , and the first produced by World Wrestling Entertainment ( WWE ) . The event , presented by Subway , took place on June 27 , 2004 , at the Norfolk Scope in Norfolk , Virginia and was a SmackDown ! brand-exclusive event . Three of the eight matches on the card were contested for a championship ; one was lost while the other two were retained . The event grossed $ 325,000 with 6,500 ticket sales and received a 0.47 buyrate . The main event was a Handicap match between The Dudley Boyz ( Bubba Ray and D-Von ) and The Undertaker . Undertaker won the match after pinning D-Von following a Tombstone Piledriver . One of the featured matches on the undercard was a Texas Bullrope match for the WWE Championship between John " Bradshaw " Layfield ( JBL ) and champion Eddie Guerrero . JBL won the match and the WWE Championship after touching all four turnbuc</t>
+          <t>A6 ( Croatia ) = The A6 motorway ( Croatian : Autocesta A6 ) is a motorway in Croatia spanning 80.2 kilometres ( 49.8 mi ) . It connects the nation 's capital , Zagreb , via the A1 , to the seaport of Rijeka . The motorway forms a major north – south transportation corridor in Croatia and is a part of European route E65 Nagykanizsa – Zagreb – Rijeka – Zadar – Split – Dubrovnik – Podgorica . The A6 motorway route also follows Pan-European corridor Vb . The A6 motorway runs near a number of Croatian cities , provides access to Risnjak National Park and indirectly to numerous resorts , notably in the Istria and Kvarner Gulf regions . The motorway route was completed in 2008 . The motorway is nationally significant because of its positive economic impact on the cities and towns it connects , and because of its contribution to tourism in Croatia . The importance of the motorway as a transit route will be further increased upon completion of a proposed expansion of the Port of Rijeka and Rij</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Kelly Kelly = Barbara Jean " Barbie " Blank-Souray ( born January 15 , 1987 ) is an American model , former professional wrestler and professional wrestling valet , better known by her ring name Kelly Kelly . She is best known for her time with WWE . Blank has a background in gymnastics and cheerleading . She studied broadcast journalism , hoping to become a television anchor , and worked as a model for Venus Swimwear and Hawaiian Tropic . In 2006 , Blank was signed to a contract by WWE and sent to Ohio Valley Wrestling , a WWE developmental territory . She debuted on the ECW brand in June 2006 as ' Kelly Kelly ' , with the character of an exhibitionist and performing a striptease . She continued her stripteases , in a segment known as Kelly 's Exposé , weekly on ECW , and also became the valet of her on-screen boyfriend Mike Knox . The following year , she formed Extreme Exposé with Layla and Brooke Adams , and the trio performed regular dance segments on ECW . They later became invol</t>
+          <t>A3 ( Croatia ) = The A3 motorway ( Croatian : Autocesta A3 ) is a major motorway in Croatia spanning 306.5 kilometres ( 190.5 mi ) . The motorway connects Zagreb , the nation 's capital , to the Slavonia region and a number of cities along the Sava River . It represents a major east – west transportation corridor in Croatia and a significant part of the Pan-European Corridor X , serving as a transit route between the European Union states and the Balkans . Apart from Zagreb , where the A3 motorway comprises a considerable part of the Zagreb bypass , the motorway runs near a number of significant Croatian cities . The motorway has a positive economic impact on the cities and towns it connects , and is an important route within Croatia . The motorway consists of two traffic lanes and an emergency lane in each driving direction , separated by a central reservation . All intersections of the A3 motorway are grade separated , and the motorway comprises several large stack and cloverleaf int</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Taboo Tuesday ( 2005 ) = Taboo Tuesday ( 2005 ) was a professional wrestling pay-per-view event produced by World Wrestling Entertainment ( WWE ) , which took place on November 1 , 2005 , at the iPayOne Center in San Diego . It was the second annual Taboo Tuesday event in which the fans were given the chance to vote on stipulations for the matches . The voting for the event started on October 24 , 2005 , and ended during the event . Eight professional wrestling matches were featured on the event 's card . The buildup to the matches and the scenarios that took place before , during , and after the event were planned by WWE 's script writers . The event starred wrestlers from the Raw brand : a storyline expansion of the promotion where employees are assigned to a wrestling brand under the WWE banner . The main event was a Triple Threat match , a standard match involving three wrestlers , for the WWE Championship . In this match , John Cena defeated Kurt Angle and Shawn Michaels to retain</t>
+          <t>Delaware Route 37 = Delaware Route 37 ( DE 37 ) is a state highway in New Castle County , Delaware . The route runs from Delaware Route 273 near Christiana northeast to U.S. Route 202 and Delaware Route 141 near the Wilmington Airport . The road runs through suburban neighborhoods before passing along the edge of Wilmington Airport , where it provides access to business parks . The Airport Road portion of DE 37 was originally a dirt road that was paved by 1942 . DE 37 was assigned to its current alignment by 1985 . = = Route description = = DE 37 heads to the northeast from DE 273 on the two-lane , undivided Airport Road . It passes through suburban neighborhoods and then intersects DE 58 ( Churchmans Road ) in a commercial area . Past the DE 58 intersection , the route widens into a four-lane divided highway and forms the northwestern boundary of the Wilmington Airport , with residential areas on the opposite side of the road . After the boundary with the airport , Airport Road splits</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>In Your House 1 = In Your House ( retroactively titled In Your House : Premiere , and sequentially known as In Your House 1 ) was a professional wrestling pay-per-view event produced by the World Wrestling Federation ( WWF ) , which took place on May 14 , 1995 , at the Onondaga War Memorial in Syracuse , New York . It was the first pay-per-view of the In Your House series and consisted of ten professional wrestling matches . In the main event WWF World Heavyweight Champion Diesel defeated Sid to retain his title . In the undercard Bret Hart defeated Hakushi , but lost to Jerry Lawler , whereas Razor Ramon defeated Jeff Jarrett and The Roadie in a two-on-one handicap match . The pay-per-view received a 0.83 buyrate , equivalent to approximately 332,000 buys . = = Background = = The pay-per-view was the first ever under the In Your House banner , which signaled the beginning of the WWF 's monthly pay-per-views . The In Your House pay-per-views were promoted at US $ 14.95 , which was chea</t>
+          <t>A9 ( Croatia ) = The A9 motorway ( Croatian : Autocesta A9 ) is a north – south motorway in Croatia , with a length of 78.3 kilometres ( 48.7 miles ) . Beginning in Pula , the largest city on the Istrian peninsula , it runs north to the Croatian motorway and expressway network at the Kanfanar interchange . Here it meets the A8 motorway , forming the Istrian Y road system . The A9 continues north from here to the Kaštel and Plovanija border crossings into Slovenia . The motorway represents a significant north – south transportation corridor in Croatia and is a part of the European route E751 . The motorway 's national significance is reflected in the positive economic impact on the cities and towns it connects , as well as its importance to tourism in Croatia . Importance of the motorway for tourism is particularly high during summer tourist seasons , when traffic volume increases by more than 80 % . The A9 motorway construction works began in 1988 with its first section opening in 1991</t>
         </is>
       </c>
     </row>
@@ -2051,32 +2051,32 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>['entertain', 'entertained', 'buddy', 'profanity', 'flamboyant', 'racially', 'courted', 'rampant', 'subtitles', 'bishop', 'psychologically', 'app', 'oppressed', 'horrific', 'bother']</t>
+          <t>['clark', 'superman', 'oliver', 'finale', 'season', 'comic', 'character', 'relationship', 'whitney', 'metropolis', 'believes', 'discovers', 'secret', 'martha', 'series']</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Fursuit = Fursuits are animal costumes . Fursuits can be worn for personal enjoyment , work or charity . The term " fursuit " is believed to have been coined in 1993 by Robert King and is usually used to describe custom-made animal costumes owned and worn by cosplayers or members of the furry fandom . Unlike mascot suits , which are usually affiliated with a team or organization , fursuits represent a stand-alone character . Fursuiters may adopt another personality while in costume for the purpose of performance . Fursuits are typically sold online by commission or auction , but can also be sold at conventions . = = Creation and construction = = Most fursuits are created by specialized online businesses if they are not self-made . Workmanship quality varies widely depending on the cost of the suit and skill of the maker . A fursuit may cost more than a thousand dollars . Many suits include special padding or undersuits to give the character its desired shape ( this is especially presen</t>
+          <t>Batman in film = The fictional character Batman , a comic book superhero featured in DC Comics publications and created by Bob Kane and Bill Finger , has appeared in various films since his inception . The character first starred in two serial films in the 1940s , Batman and Batman and Robin . The character also appeared in the 1966 film Batman , which was a feature film adaptation of the 1960s Batman TV series starring Adam West and Burt Ward , who also starred in the film . Toward the end of the 1980s , the Warner Bros. studio began producing a series of feature films starring Batman , beginning with the 1989 film Batman , directed by Tim Burton and starring Michael Keaton . Burton and Keaton returned for the 1992 sequel Batman Returns , and in 1995 , Joel Schumacher directed Batman Forever with Val Kilmer as Batman . Schumacher also directed the 1997 sequel Batman &amp; Robin , which starred George Clooney . Batman &amp; Robin was poorly received by both critics and fans , leading to the ca</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Becket Hill State Park Reserve = Becket Hill State Park Reserve is a public recreation area lying adjacent to Nehantic State Forest in the town of Lyme , Connecticut , United States . The state park is listed by the Connecticut Department of Energy and Environmental Protection as an undeveloped , walk-in park totaling 260 acres ( 110 ha ) with no officially listed activities . The park 's name is sometimes misspelled as Beckett Hill . = = History = = Becket Hill State Park Reserve is named for an early settler of the area named Becket and the land was part of the Nehantic tribe 's territory . This state park was acquired by the State of Connecticut in order to preserve the hill , but unlike the abutting Nehantic State Forest , Becket Hill has accessibility problems and is returning to its natural state . In 1961 , the land for the Becket Hill State Park Reserve was given to the State of Connecticut by the George Dudley Seymour Trust . Beckett Hill was first listed on the Connecticut Re</t>
+          <t>Clark Kent ( Smallville ) = Clark Kent is a fictional character on the television series Smallville . The character of Clark Kent , first created for comic books by Jerry Siegel and Joe Shuster in 1938 as the alternate identity of Superman , was adapted to television in 2001 by Alfred Gough and Miles Millar . This is the fourth time the character has been adapted to a live-action television series . Clark Kent has been played continually by Tom Welling , with various other actors portraying Clark as a child . The character has also appeared in various literature based on the Smallville series , all of which are completely independent of the television episodes . As of 2011 , Smallville 's Clark Kent has appeared in eighteen young adult novels . In the series , Clark Kent attempts to live the life of a normal human being , and struggles with keeping the secret of his alien heritage from his friends . He has an on-again , off-again relationship with Lana Lang through the first seven seas</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Avocado cake = Avocado cake is a cake prepared using avocado as a primary ingredient , together with other typical cake ingredients . The avocados may be mashed , and may be used as an ingredient in cake batter , in cake toppings and alone atop a cake . Cake variations include raw avocado cake , avocado brownies and avocado cheesecake . Raw , uncooked versions of avocado cake can be high in vitamin E and essential fatty acids , which are derived from avocado . Avocado-based cake toppings include avocado fool and avocado crazy . = = Overview = = Avocado is a main ingredient in avocado cake , along with other typical cake ingredients . Various varieties of avocados may be used . Avocado cake may have a subtle avocado flavor imbued in the dish . Mashed avocado may be used as an ingredient in the batter and in cake frostings and toppings . Sliced avocado may be used to top or garnish it , as may other ingredients such as the zest of citrus fruits . Additional ingredients used may include y</t>
+          <t>Justice League ( Smallville ) = The Justice League is a fictional group of superheroes on the television series , Smallville , who were adapted for television by Alfred Gough and Miles Millar . The Justice League originally included Oliver Queen , Bart Allen , Victor Stone , and Arthur Curry ; Clark Kent did not accept a role until three seasons later . As the team continued to appear in the series , new characters were introduced and subsequently joined the team . The original Justice League first appeared in the DC comic book The Brave and the Bold # 28 ( 1960 ) , and consisted of members Superman , Batman , Wonder Woman , Flash , Green Lantern , Aquaman , and the Martian Manhunter . In Smallville , the team did not make its first official appearance until the season six episode " Justice " , although each member had been previously introduced individually on various episodes since season four . In the series , the team never formalized a name for themselves , although the cast and c</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Jænberht = Jænberht ( also Jambert , Jaenbeorht , Jænbert , Jaenberht or Jaenbert ; died 792 ) was a medieval monk , and later the abbot , of St Augustine 's Abbey , Canterbury who was named Archbishop of Canterbury in 765 . As archbishop , he had a difficult relationship with King Offa of Mercia , who at one point confiscated lands from the archbishopric . By 787 , some of the bishoprics under Canterbury 's supervision were transferred to the control of the newly created Archbishopric of Lichfield , although it is not clear if Jænberht ever recognised its legitimacy . Besides the issue with Lichfield , Jænberht also presided over church councils in England . He died in 792 and was considered a saint after his death . = = Early life = = Jænberht was a monk at St Augustine 's Abbey , Canterbury before being selected as abbot of that monastic house . He came from a prominent family in the kingdom of Kent , and a kinsman of his , Eadhun , was the reeve of King Egbert II of Kent . Jænberht</t>
+          <t>Finale ( Smallville ) = " Finale " is the title of the two-episode series finale of the superhero television series Smallville . The episodes are the 21st and 22nd of the 10th season , and the 216th and 217th episodes overall . The finale originally aired on The CW in the United States on May 13 , 2011 . The first half was written by Al Septien and Turi Meyer , and directed by Kevin G. Fair , and the second half was written by Kelly Souders and Brian Peterson , and directed by Greg Beeman . The series follows the adventures of the young Clark Kent ( Tom Welling ) in the fictional town of Smallville , Kansas , before he becomes Superman . In the series finale , Tess Mercer ( Cassidy Freeman ) learns that the planet Apokolips is coming to destroy humanity , and that Oliver Queen ( Justin Hartley ) is under the possession of Darkseid . Meanwhile , a parallel universe version of Lionel Luthor ( John Glover ) attempts to bring a clone of his son Lex ( Michael Rosenbaum ) to life . Clark fin</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Romanus ( bishop of Rochester ) = Romanus ( died before 627 ) was the second bishop of Rochester and presumably was a member of the Gregorian mission sent to Kent to Christianize the Anglo-Saxons from their native Anglo-Saxon paganism . Romanus was consecrated bishop around 624 and died before 627 by drowning . Little is known of his life beyond these facts . = = Career = = Presumably Romanus came to England with Augustine of Canterbury 's mission to Kent , He would have arrived either in 597 with the first group of missionaries , or in 601 with the second group . He was consecrated as bishop by his predecessor Justus in 624 , after Justus became Archbishop of Canterbury . He was the second bishop at Rochester . Romanus died before 627 , probably about 625 . He drowned in the Mediterranean Sea off Italy while on a mission to Rome for Justus . Presumably this happened before Justus ' death in 627 . He was certainly dead by 633 , when Paulinus of York became bishop at Rochester after fle</t>
+          <t xml:space="preserve">The X-Files ( season 9 ) = The ninth season of the American science fiction television series The X-Files commenced airing in the United States on November 11 , 2001 , concluded on May 19 , 2002 , and consists of twenty episodes . Season nine takes place after Fox Mulder ( David Duchovny ) goes into hiding , following the events of the eighth season finale , " Existence " . As such , the main storyarc for the season follows Dana Scully ( Gillian Anderson ) , John Doggett ( Robert Patrick ) , and Monica Reyes ( Annabeth Gish ) on their hunt to reveal a government conspiracy who are creating " Super Soldiers " . For this season , former series ' leads Duchovny and Anderson scaled back their involvement with the show , with the former only starring in the two episodes that formed the season finale , " The Truth " . Doggett and Reyes became the show 's central characters , and former recurring character Walter Skinner ( Mitch Pileggi ) became a main character . Series creator Chris Carter </t>
         </is>
       </c>
     </row>
@@ -2086,32 +2086,32 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>['production', 'system', 'crew', 'mission', 'use', 'development', 'based', 'high', 'million', 'aircraft', 'engine', 'control', 'announced', 'new', 'flight']</t>
+          <t>['euro', 'coins', 'currency', 'note', 'notes', 'denominations', 'dollar', 'value', 'stripe', 'tender', 'silver', 'puerto_rico', 'thread', 'ink', 'issued']</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>McDonnell Douglas F-4 Phantom II in UK service = The United Kingdom operated the McDonnell Douglas F-4 Phantom II as one of its principal combat aircraft from the 1960s to the early 1990s . The UK was the first export customer for the Phantom , which was ordered in the context of political and economic difficulties around indigenous British designs for the roles that it was eventually purchased to undertake . The Phantom was procured to serve in both the Fleet Air Arm and Royal Air Force in several roles including air defence , close air support , low-level strike and tactical reconnaissance . Although assembled in the United States , the UK 's Phantoms were a special batch built separately and containing a significant amount of British technology as a means of easing the pressure on the domestic aerospace industry in the wake of major project cancellations . Two individual variants were eventually built for the UK ; the F-4K variant was designed from the outset as an air defence inter</t>
+          <t>Euro = The euro ( sign : € ; code : EUR ) is the official currency of the eurozone , which consists of 19 of the 28 member states of the European Union : Austria , Belgium , Cyprus , Estonia , Finland , France , Germany , Greece , Ireland , Italy , Latvia , Lithuania , Luxembourg , Malta , the Netherlands , Portugal , Slovakia , Slovenia , and Spain . The currency is also officially used by the institutions of the European Union and four other European countries , as well as unilaterally by two others , and is consequently used daily by some 337 million Europeans as of 2015 . Outside of Europe , a number of overseas territories of EU members also use the euro as their currency . Additionally , 210 million people worldwide as of 2013 use currencies pegged to the euro . The euro is the second largest reserve currency as well as the second most traded currency in the world after the United States dollar . As of August 2014 , with more than € 995,000,000,000 in circulation , the euro has t</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Panavia Tornado = The Panavia Tornado is a family of twin-engine , variable-sweep wing multirole combat aircraft , which was jointly developed and manufactured by Italy , the United Kingdom , and West Germany . There are three primary Tornado variants : the Tornado IDS ( interdictor / strike ) fighter-bomber , the suppression of enemy air defences Tornado ECR ( electronic combat / reconnaissance ) and the Tornado ADV ( air defence variant ) interceptor aircraft . The Tornado was developed and built by Panavia Aircraft GmbH , a tri-national consortium consisting of British Aerospace ( previously British Aircraft Corporation ) , MBB of West Germany , and Aeritalia of Italy . It first flew on 14 August 1974 and was introduced into service in 1979 – 1980 . Due to its multirole nature , it was able to replace several different fleets of aircraft in the adopting air forces . The Royal Saudi Air Force ( RSAF ) became the only export operator of the Tornado in addition to the three original pa</t>
+          <t>500 euro note = The five hundred euro note ( € 500 ) is the highest-value euro banknote and has been used since the introduction of the euro ( in its cash form ) in 2002 . It is one of the highest value circulating banknotes in the world , worth around 551 USD , 3,677 CNY , 58,254 JPY , 543 CHF or 417 GBP . The note is used in the 23 countries which have the euro as their sole currency ( with 22 legally adopting it ) , with a population of about 338 million . It is the largest note measuring 160 × 82 mm and has a purple colour scheme . The five hundred euro banknotes depict bridges and arches / doorways in modern architecture ( around the late 20th century ) . The five hundred euro note contains several complex security features such as watermarks , invisible ink , holograms and microprinting that make counterfeiting very difficult . Initially the high denomination notes were introduced very rapidly so that in first 7 years ( by Dec 2008 ) there were 530,064,413 five hundred euro bankn</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Bicycle and motorcycle dynamics = Bicycle and motorcycle dynamics is the science of the motion of bicycles and motorcycles and their components , due to the forces acting on them . Dynamics is a branch of classical mechanics , which in turn is a branch of physics . Bike motions of interest include balancing , steering , braking , accelerating , suspension activation , and vibration . The study of these motions began in the late 19th century and continues today . Bicycles and motorcycles are both single-track vehicles and so their motions have many fundamental attributes in common and are fundamentally different from and more difficult to study than other wheeled vehicles such as dicycles , tricycles , and quadracycles . As with unicycles , bikes lack lateral stability when stationary , and under most circumstances can only remain upright when moving forward . Experimentation and mathematical analysis have shown that a bike stays upright when it is steered to keep its center of mass ove</t>
+          <t>50 euro note = The fifty euro note ( € 50 ) is one of the middle value euro banknotes and has been used since the introduction of the euro ( in its cash form ) in 2002 . The note is used daily by some 332 million Europeans and in the 23 countries which have the euro as their sole currency ( with 22 legally adopting it ) . It is the fourth smallest note , measuring 140 mm × 77 mm , and has an orange colour scheme . The note depicts bridges and arches / doorways in the Renaissance era ( 15th and 16th centuries ) . The € 50 note contains several complex security features such as watermarks , invisible ink , holograms and microprinting that document its authenticity . In January 2016 , there were about 8,170,123,315 fifty euro banknotes in circulation in the eurozone . It is by far the most widely circulated denomination , compromising over 44 % of the total banknotes . The full design of the Europa series € 50 banknote was revealed on 5 July 2016 ; it is due to be launched in April 2017 .</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Lockheed Martin F-22 Raptor = The Lockheed Martin F-22 Raptor is a fifth-generation , single-seat , twin-engine , all-weather stealth tactical fighter aircraft developed for the United States Air Force ( USAF ) . The result of the USAF 's Advanced Tactical Fighter program , the aircraft was designed primarily as an air superiority fighter , but also has ground attack , electronic warfare , and signals intelligence capabilities . The prime contractor , Lockheed Martin , built most of the F-22 's airframe and weapons systems and did its final assembly , while Boeing provided the wings , aft fuselage , avionics integration , and training systems . The aircraft was variously designated F-22 and F / A-22 before it formally entered service in December 2005 as the F-22A . After a protracted development and despite operational issues , the USAF considers the F-22 critical to its tactical air power , and says that the aircraft is unmatched by any known or projected fighter . The Raptor 's combi</t>
+          <t>10 euro note = The ten euro note ( € 10 ) is the second-lowest value euro banknote and has been used since the introduction of the euro ( in its cash form ) in 2002 . The note is used in the 23 countries which have it as their sole currency ( with 22 legally adopting it ) ; with a population of about 332 million . It is the second-smallest note measuring 127x67mm with a red colour scheme . The ten euro banknotes depict bridges and arches / doorways in Romanesque architecture ( between the 11th and 12th centuries ) . The ten euro note contains several complex security features such as watermarks , invisible ink , holograms and microprinting that document its authenticity . In September 2011 , there were approximately 2,005,149,600 ten euro banknotes in circulation around the eurozone . = = History = = The euro was founded on 1 January 1999 , when it became the currency of over 300 million people in Europe . For the first three years of its existence it was an invisible currency , only u</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Sinclair C5 = The Sinclair C5 is a small one-person battery electric vehicle , technically an " electrically assisted pedal cycle " . ( Although widely described as an " electric car " , Sinclair characterised it as a " vehicle , not a car " . ) It was the culmination of Sir Clive Sinclair 's long-running interest in electric vehicles . Sinclair had become one of the UK 's best-known millionaires and earned a knighthood on the back of the highly successful Sinclair Research range of home computers in the early 1980s . He now hoped to repeat his success in the electric vehicle market , which he saw as ripe for a new approach . The C5 emerged from an earlier project to produce a Renault Twizy-style electric car called the C1 . After a change in the law prompted by lobbying from bicycle manufacturers , Sinclair developed the C5 as an electrically powered tricycle with a polypropylene body and a chassis designed by Lotus Cars . It was intended to be the first in a series of increasingly am</t>
+          <t xml:space="preserve">Aksumite currency = Aksumite currency was coinage produced and used within the Kingdom of Aksum ( or Axum ) centered in present-day Ethiopia and Eritrea . It was issued and circulated from the reign of King Endubis around AD 270 until it began its decline in the first half of the 7th century . During the succeeding medieval period , Mogadishu currency , minted by the Sultanate of Mogadishu , was the most widely circulated currency in the Horn of Africa . Aksum 's currency served as a vessel of propaganda demonstrating the kingdom 's wealth and promoting the national religion ( first polytheistic and later Oriental Christianity ) . It also facilitated the Red Sea trade on which it thrived . The coinage has also proved invaluable in providing a reliable chronology of Aksumite kings due to the lack of extensive archaeological work in the area . = = Origins = = = = = Pre-coinage period = = = Though the issuing of minted coins didn 't begin until around 270 , metal coins may have been used </t>
         </is>
       </c>
     </row>
@@ -2121,32 +2121,32 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>['album', 'songs', 'number', 'band', 'release', 'single', 'music', 'track', 'copies', 'released', 'chart', 'billboard', 'tracks', 'sound', 'recording']</t>
+          <t>['painting', 'paintings', 'works', 'abstract', 'dots', 'art', 'canvas', 'okay', 'artist', 'breasts', 'portrait', 'mirror', 'girl', 'work', 'balloon']</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Documentaly = Documentaly ( stylized as DocumentaLy , Japanese pronunciation : [ dokjɯmentaɺi : ] ) is the fifth studio album by Japanese band Sakanaction , released on September 28 , 2011 . Written around a documentary theme , the band were inspired by personal and world events in 2011 to create material for the album . The band decided to release three singles prior to the album , as a way to alleviate the pressure that the band felt to release new music after the success of their previous album Kikuuiki ( 2010 ) , and as a way to show the album 's development process . The first single " Identity " , a song originally written during that album 's recording sessions , was released three months after Kikuuiki . The band intended to release " Endless " as the album 's second single , however as they were not fully satisfied with the song , released " Rookie " in its place in March 2011 . Just prior to the single 's physical release , Japan experienced the 2011 Tōhoku earthquake and tsu</t>
+          <t xml:space="preserve">Artist 's Studio — Look Mickey = Artist 's Studio — Look Mickey ( sometimes Artist 's Studio , Look Mickey , Artist 's Studio – Look Mickey or Artist 's Studio No. 1 ( Look Mickey ) ) is a 1973 painting by Roy Lichtenstein . It is one of five large-scale studio interior paintings in a series . The series is either referred to as the Artist 's Studio series or more colloquially as the Studios and sometimes is described as excluding the other 1973 painting , reducing the series to four . The series refers to a set of works by Henri Matisse , with this work specifically referring to L 'Atelier Rouge . The work incorporates several other Lichtenstein 's works and gets its name from the large portion of Lichtenstein 's Look Mickey that is included . Lichtenstein used a much more realistic representation of his own works than is standard for most artists . Elements of the work also refer to works from both Fernand Léger and Matisse . = = Background = = Lichtenstein 's studios reference what </t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Random Access Memories = Random Access Memories is the fourth studio album by the French electronic music duo Daft Punk , released on 17 May 2013 by the duo 's imprint Daft Life and Columbia Records . The album pays tribute to the late 1970s and early 1980s era of music in the United States , particularly the sounds of said era that emerged from Los Angeles . This theme was reflected in the promotional campaign for the album that included billboards , television advertisements and a web series , as well as in the album 's packaging . Unlike their previous albums , Daft Punk recruited session musicians to perform live instrumentation in professional recording locations , and limited the use of electronic instruments to usage of drum machines , a custom-built modular synthesizer and vintage vocoders . The album features collaborations with Giorgio Moroder , Panda Bear , Julian Casablancas , Todd Edwards , DJ Falcon , Chilly Gonzales , Nile Rodgers , Paul Williams and Pharrell Williams . </t>
+          <t>Girl with Ball = Girl with Ball is a 1961 painting by Roy Lichtenstein . It is an oil on canvas Pop art work that is now in the collection of the Museum of Modern Art , after being owned for several decades by Philip Johnson . It is one of Lichtenstein 's earliest Pop art works and is known for its source , which is a newspaper ad that ran for several decades and which was among Lichtenstein 's earliest works sourced from pop culture . Girl with Ball was exhibited at Lichtenstein 's first solo exhibition and was displayed in Newsweek 's review of the show . This work significantly alters the original source and is considered exemplary of Lichtenstein 's works that exaggerate the mechanically produced appearance although the result of his painterly work . It is an enduring depiction of the contemporary beauty figure . = = Background = = Girl with Ball was inspired by a 1961 advertisement for the Mount Airy Lodge in the Pocono Mountains . The ad , which started running in 1955 , was wide</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Drama Queen ( Ivy Queen album ) = Drama Queen is the seventh studio album by Puerto Rican reggaeton recording artist Ivy Queen . It was released on July 13 , 2010 by Machete Music . The album was written by Queen with help from Rafael Castillo , Marcos Masis and others , while production was handled by Luny Tunes , Tainy and Noriega . The album features collaborations with De La Ghetto , Frank Reyes , Wisin &amp; Yandel and Franco " El Gorila " . It features a wide variety of musical styles in common with her previous album , Sentimiento , released three years earlier on a different label . Selling 3,000 units in its first week , Drama Queen debuted and peaked at number 163 on the US Billboard 200 chart , number three on the Billboard Top Latin Albums chart , number one on the Billboard Latin Rhythm Albums chart and number 18 on the Billboard Rap Albums chart . The recording received a Latin Grammy nomination for Best Urban Music Album at the Latin Grammy Awards of 2011 and two nominations</t>
+          <t>Brushstrokes series = Brushstrokes series is the name for a series of paintings produced in 1965 – 66 by Roy Lichtenstein . It also refers to derivative sculptural representations of these paintings that were first made in the 1980s . In the series , the theme is art as a subject , but rather than reproduce masterpieces as he had starting in 1962 , Lichtenstein depicted the gestural expressions of the painting brushstroke itself . The works in this series are linked to those produced by artists who use the gestural painting style of abstract expressionism made famous by Jackson Pollock , but differ from them due to their mechanically produced appearance . The series is considered a satire or parody of gestural painting by both Lichtenstein and his critics . After 1966 , Lichtenstein incorporated this series into later motifs and themes of his work . = = Background = = In the early 1960s , Lichtenstein reproduced masterpieces by Cézanne , Mondrian and Picasso before embarking on the Bru</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Kaleidoscope Dream = Kaleidoscope Dream is the second studio album by American R &amp; B recording artist Miguel , released on September 25 , 2012 , by RCA Records . After attaining commercial standing with his 2010 debut album All I Want Is You , Miguel wanted to play a larger creative role in his music and principally produced and wrote Kaleidoscope Dream . He recorded most of the album at Platinum Sound Recording Studios in New York City and MJP Studios in Los Angeles , and worked with producers Warren " Oak " Felder , Jerry " Wonda " Duplessis and Salaam Remi , among others . The music on Kaleidoscope Dream draws on R &amp; B , pop , funk , rock and soul styles , as well as elements from electronic and psychedelic music . The album 's producers incorporated dense bass lines , buzzing synthesizers , and hazy , reverbed sounds in the songs , which deal mostly with sex , romance , and existential ideas . Miguel titled Kaleidoscope Dream as a metaphor for life and wanted the songs to reflect h</t>
+          <t>Symphony in White , No. 2 : The Little White Girl = Symphony in White , No. 2 , also known as The Little White Girl is a painting by James Abbott McNeill Whistler . The work shows a woman in three-quarter figure standing by a fireplace with a mirror over it . She is holding a fan in her hand , and wearing a white dress . The model is Joanna Hiffernan , the artist 's mistress . Though the painting was originally called The Little White Girl , Whistler later started calling it Symphony in White , No. 2 . By referring to his work in such abstract terms , he intended to emphasize his " art for art 's sake " philosophy . In this painting , Heffernan wears a ring on her ring finger , even though the two were not married . By this religious imagery , Whistler emphasizes the aesthetic philosophy behind his work . Whistler created the painting in the winter of 1864 , and it was displayed at the Royal Academy the next year . The original frame carried a poem written by Whistler 's friend Algerno</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enter the Grave = Enter the Grave is the debut album by the English thrash metal band Evile . Released on 27 August 2007 in Europe and on 25 September in North America and Japan , the album received generally favorable reviews and entered the UK Rock Chart at number 33 . It was produced by Flemming Rasmussen and recorded at Sweet Silence Studios , Copenhagen , Denmark . Rasmussen had produced three Metallica albums , which raised the profile of the album 's release . The track " Thrasher " was included on the 2008 Earache Thrash Pack , a downloadable selection of songs for the music video console game Rock Band . The album 's lyrics were inspired by films scripts , recounts of the life of Countess Bathory and witch burnings . Enter the Grave was re-released as a limited-edition " redux " version on 13 October 2008 in Europe and on 28 October in North America . According to the Huddersfield Daily Examiner , Enter the Grave had shifted 30,000 copies by September 2009 . = = Recording = = </t>
+          <t>Grrrrrrrrrrr ! ! = Grrrrrrrrrrr ! ! is a 1965 oil and Magna on canvas painting by Roy Lichtenstein . Measuring 68 in × 56.125 in ( 172.7 cm × 142.6 cm ) , it was bequeathed to the Solomon R. Guggenheim Museum collection from Lichtenstein 's estate . It depicts a head-on representation of an angry dog growling with the onomatopoeic expression " Grrrrrrrrrrr ! ! " . The work was derived from Our Fighting Forces , which also served as the source for other military dog paintwork by Lichtenstein . = = Background = = The Lichtenstein foundation notes that the inspiration for this painting is a frame of Our Fighting Forces # 66 ( February 1962 ) , which was published by National Periodical Publications ( now DC Comics ) . In that frame only a portion of the dog 's head is visible and the speech balloon says " Grrrrr ! " In addition to the painting itself , Lichtenstein produced a small 5.75 in × 4.5 in ( 14.6 cm × 11.4 cm ) graphite on paper study . The painting was bestowed to the Guggenheim</t>
         </is>
       </c>
     </row>
@@ -2156,67 +2156,32 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>['ship', 'ships', 'torpedo', 'tons', 'guns', 'admiral', 'cruiser', 'fleet', 'submarine', 'sank', 'laid', 'sinking', 'convoy', 'german', 'destroyer']</t>
+          <t>['ben', 'shannon', 'survivors', 'bernard', 'island', 'freighter', 'dave', 'frank', 'plane', 'jack', 'alex', 'miles', 'kate', 'crash', 'rose']</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>German destroyer Z8 Bruno Heinemann = Z8 Bruno Heinemann was a Type 1934A-class destroyer built for Nazi Germany 's Kriegsmarine in the mid-1930s . After the start of World War II in September 1939 , she blockaded the Polish coast and searched neutral shipping for contraband . In late 1939 and early 1940 the ship made three successful minelaying sorties off the English coast that claimed 17 merchant ships . Bruno Heinemann participated in the early stages of the Norwegian Campaign by transporting troops to the Trondheim area in early April 1940 . The ship was transferred to France a year later to escort German ships that used the French ports on the Atlantic coast . She was returning to France in early 1942 when she struck two mines and sank off the coast of Belgium . = = Design and description = = Bruno Heinemann had an overall length of 119 meters ( 390 ft 5 in ) and was 114 meters ( 374 ft 0 in ) long at the waterline . The ship had a beam of 11.30 meters ( 37 ft 1 in ) , and a maxi</t>
+          <t xml:space="preserve">Shannon Rutherford = Shannon Rutherford was a fictional character played by Maggie Grace on the ABC drama television series Lost , which chronicled the lives of the survivors of a plane crash in the South Pacific . Shannon was introduced in the pilot episode as the stepsister of fellow crash survivor Boone Carlyle ( Ian Somerhalder ) . She was a series regular until her funeral in " What Kate Did " . For most of her time on the Island , she was unhelpful and spent much of her time sunbathing . She formed a relationship with another survivor from the plane crash , Sayid Jarrah ( Naveen Andrews ) . Shannon was accidentally shot by Ana Lucia Cortez who mistakes her for an Other . During the casting process , she was compared to Paris Hilton . Naveen Andrews , who played the character Sayid on the show , had the idea of encouraging the writers to write a romantic relationship between his character and Shannon into the story . Critics found her to be a largely unsympathetic character until </t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t xml:space="preserve">HMS Hesperus ( H57 ) = HMS Hesperus was an H-class destroyer that had originally been ordered by the Brazilian Navy with the name Juruena in the late 1930s , but was bought by the Royal Navy after the beginning of World War II in September 1939 and later renamed . She was damaged by German aircraft during the Norwegian Campaign in May 1940 and was assigned to convoy escort and anti-submarine patrols after her repairs were completed . The ship was assigned to the Western Approaches Command for convoy escort duties in late 1940 . She was briefly assigned to Force H in 1941 , but her anti-aircraft armament was deemed too weak and she was transferred to the Newfoundland Escort Force the next month for escort duties in the North Atlantic . Hesperus was transferred to the Mid-Ocean Escort Force in late 1941 and continued to escort convoys in the North Atlantic for the next three years . She was converted to an escort destroyer in early 1943 after suffering damage from one of her two ramming </t>
+          <t>Danielle Rousseau = Danielle Rousseau is a fictional character on the ABC drama television series Lost , which chronicles the lives of over forty people after their plane crashes on a remote island somewhere in the South Pacific . Croatian actress Mira Furlan plays the scientist who shipwrecks on the island sixteen years prior to the crash of Oceanic Flight 815 . After Rousseau is killed in the fourth season , the American actress Melissa Farman portrayed a younger version of the character in the fifth season . Furlan later reappears for one episode in the sixth season . Rousseau is a recurring on-island character who has appeared in nineteen episodes in seasons one through four , as well as one episode where her voice alone is heard , and her final episode in the sixth season . The character , who is commonly known as " The French Woman " among the survivors on the island , is introduced early in the first season . Sixteen years prior to the plane crash , Rousseau was a member of a Fr</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>C and D-class destroyer = The C and D class was a group of 14 destroyers built for the Royal Navy in the early 1930s . As in previous years , it was originally intended to order a complete flotilla comprising eight destroyers — plus a flotilla leader as the ninth unit — in each year . However , only four ships — plus a leader — were ordered under the 1929 – 30 Programme as the C class . The other four ships planned for the C class were never ordered as an economy measure and disarmament gesture by the Labour government of Ramsay Macdonald . A complete flotilla — the ' D ' class — was ordered under the 1930 – 31 Programme . The five ships of the C class were assigned to Home Fleet upon their completion , although they reinforced the Mediterranean Fleet during the Italian invasion of Abyssinia of 1935 – 36 and enforced the Non-Intervention Agreement during the Spanish Civil War of 1936 – 39 . They were transferred to the Royal Canadian Navy ( RCN ) in 1937 – 39 and spent most of their ti</t>
+          <t>Tom Friendly = Tom Friendly , often referred to as Tom or Mr. Friendly , is a fictional character portrayed by M. C. Gainey on the American Broadcasting Company ( ABC ) television series Lost . The series follows the lives of around forty survivors from the crash of Oceanic Flight 815 . The survivors find themselves on a mysterious tropical island , and interact with a group known as the Others , who appear to have lived on the island since long before the crash . Tom is an influential member of the Others , and is introduced in 2005 in the season one finale " Exodus : Part 2 " , where he kidnaps one of the survivors . The character makes another fifteen appearances before being killed in the season three finale " Through the Looking Glass " . Tom appears twice in season four in the flashbacks of other characters . Gainey was initially credited as playing " bearded man " and then as " Mr. Friendly " throughout season two before the character was given a first name . In a montage of dec</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>HMS Hotspur ( H01 ) = HMS Hotspur was an H-class destroyer built for the Royal Navy during the 1930s . During the Spanish Civil War of 1936 – 1939 the ship spent considerable time in Spanish waters , enforcing the arms blockade imposed by Britain and France on both sides of the conflict . During the Norwegian Campaign of the Second World War , she fought in the First Battle of Narvik in April 1940 where she was badly damaged . After her repairs were completed , Hotspur was transferred to Gibraltar where she participated in the Battle of Dakar in September . A month later the ship was badly damaged when she rammed and sank an Italian submarine . She received permanent repairs in Malta and was transferred to the Mediterranean Fleet when they were finished in early 1941 . Hotspur participated in the Battle of Cape Matapan in March and evacuated British and Australian troops from both Greece and Crete in April – May . In June the ship participated in the Syria-Lebanon Campaign and was esco</t>
+          <t>Rose and Bernard Nadler = Rose and Bernard Nadler are fictional characters on the American Broadcasting Company ( ABC ) television series Lost , played by L. Scott Caldwell and Sam Anderson respectively . Rose and Bernard visit a faith healer on their honeymoon in Australia , in the hope of healing Rose 's cancer . When Bernard visits the restroom during the return flight , the plane splits in half , with the two halves crashing on different parts of an island in the South Pacific . The couple reunite midway through season two , and Rose reveals the Island has healed her . After time traveling in season five they separate from the remaining survivors and build a cabin near the ocean to live in . Originally , the story of a woman separated from her husband when the plane crashes was going to be used for Kate , but when Kate 's role in the series changed the producers kept that story for Rose . Much of the couple 's story prior to the plane crash was based on the events of Caldwell 's li</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>HMS Firedrake ( H79 ) = HMS Firedrake was an F-class destroyer built for the Royal Navy during the early 1930s . Although assigned to the Home Fleet upon completion , the ship was attached to the Mediterranean Fleet in 1935 – 36 during the Abyssinia Crisis . During the Spanish Civil War of 1936 – 39 , she spent much time in Spanish waters , enforcing the arms blockade imposed by Britain and France on both sides of the conflict . Several weeks after the start of the Second World War in September 1939 , Firedrake helped to sink a German submarine and took part in the Norwegian Campaign in early 1940 . She was sent to Gibraltar in mid-1940 and formed part of Force H where she escorted many Malta convoys in the Mediterranean and helped to sink an Italian submarine . Firedrake participated in the Battle of Cape Spartivento and screened the capital ships of Force H as they bombarded Genoa before she was damaged by an Italian bomb in mid-1941 . After her repairs were completed the ship became</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>49</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>['government', 'war', 'military', 'led', 'political', 'country', 'party', 'support', 'polish', 'foreign', 'soviet', 'revolution', 'leader', 'russian', 'members']</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Roman Dmowski = Roman Stanisław Dmowski [ ˈrɔman staˈɲiswaf ˈdmɔfski ] ( 9 August 1864 – 2 January 1939 ) was a Polish politician , statesman , and co-founder and chief ideologue of the right-wing National Democracy ( " ND " : in Polish , " Endecja " ) political movement . He saw the aggressive Germanization of Polish territories controlled by the German Empire as the major threat to Polish culture and therefore advocated a degree of accommodation with another power that had partitioned Poland , the Russian Empire . He favored the re-establishment of Polish independence by nonviolent means , and supported policies favorable to the Polish middle class . During World War I , in Paris , through his Polish National Committee he was a prominent spokesman , to the Allies , for Polish aspirations . He was a principal figure instrumental in the postwar restoration of Poland 's independent existence . Dmowski never wielded official political power , except for a brief period in 1923 as minister</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Leonid Brezhnev = Leonid Ilyich Brezhnev ( / ˈbrɛʒnɛf / ; Russian : Леони ́ д Ильи ́ ч Бре ́ жнев ; IPA : [ lʲɪɐˈnʲid ɪˈlʲjitɕ ˈbrʲɛʐnʲɪf ] ; Ukrainian : Леоні ́ д Іллі ́ ч Бре ́ жнєв , 19 December 1906 ( O.S. 6 December ) – 10 November 1982 ) was the General Secretary of the Central Committee ( CC ) of the Communist Party of the Soviet Union ( CPSU ) , presiding over the country from 1964 until his death in 1982 . His eighteen-year term as General Secretary was second only to that of Joseph Stalin in duration . During Brezhnev 's rule , the global influence of the Soviet Union grew dramatically , in part because of the expansion of the Soviet military during this time . His tenure as leader was marked by the beginning of an era of economic and social stagnation in the Soviet Union . Brezhnev was born in Kamenskoe into a Russian worker 's family . After graduating from the Dniprodzerzhynsk Metallurgical Technicum , he became a metallurgical engineer in the iron and steel industry , in </t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>Mikhail Suslov = Mikhail Andreyevich Suslov ( Russian : Михаи ́ л Андре ́ евич Су ́ слов ; 21 November [ O.S. 8 November ] 1902 – 25 January 1982 ) was a Soviet statesman during the Cold War . He served as Second Secretary of the Communist Party of the Soviet Union from 1965 , and as unofficial Chief Ideologue of the Party until his death in 1982 . Suslov was responsible for party democracy and the power separation within the Communist Party . His hardline attitude toward change made him one of the foremost anti-reformist Soviet leaders . Born in rural Russia in 1902 , Suslov became a member of the All-Union Communist Party ( Bolsheviks ) in 1921 and studied economics for much of the 1920s . He left his job as a teacher in 1931 to pursue politics full-time , becoming one of the many Soviet politicians who took part in the mass repression begun by Joseph Stalin 's regime . Suslov impressed the Soviet leadership to such an extent in the pre-Eastern Front Soviet Union that he was made Fir</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Andranik = Andranik Ozanian , commonly known as Andranik ( Armenian : Անդրանիկ ; 25 February 1865 – 31 August 1927 ) was an Armenian military commander and statesman , the best known fedayi and a key figure of the Armenian national liberation movement . He became active in an armed struggle against the Ottoman government and Kurdish irregulars in the late 1880s . He joined the Armenian Revolutionary Federation ( Dashnaktustyun ) party and , along with other fedayi ( militias ) , sought to defend the Armenian peasantry living in their ancestral homeland , an area known as Turkish ( or Western ) Armenia — at the time part of the Ottoman Empire . His revolutionary activities ceased and he left the Ottoman Empire after the unsuccessful uprising in Sasun in 1904 . In 1907 , Andranik left Dashnaktustyun because he disapproved of its cooperation with the Young Turks , a party which years later perpetrated the Armenian Genocide . Between 1912 and 1913 , together with Garegin Nzhdeh , Andranik </t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>Nikolai Ryzhkov = Nikolai Ivanovich Ryzhkov ( Russian : Николай Иванович Рыжков , Nikolaj Ivanovič Ryžkov ; born 28 September 1929 ) is a former Soviet official who became a Russian politician following the dissolution of the Soviet Union . He served as the last Chairman of the Council of Ministers ( the post was abolished and replaced by that of Prime Minister in 1991 ) . Responsible for the cultural and economic administration of the Soviet Union during the late Gorbachev Era , Ryzhkov was succeeded as premier by Valentin Pavlov in 1991 . The same year , he lost his seat on the Presidential Council , going on to become Boris Yeltsin 's leading opponent in the Russian Soviet Federative Socialist Republic ( RSFSR ) 1991 presidential election . Ryzhkov was born in the city of Dzerzhynsk , Ukrainian Soviet Socialist Republic in 1929 . After graduating in the 1950s he started work in the 1970s and began his political career in local industry , working his way up through the hierarchy of S</t>
+          <t>Ben Linus = Benjamin " Ben " Linus is a fictional character portrayed by Michael Emerson on the ABC television series Lost . Ben was the leader of a group of island natives called the Others and was initially known as Henry Gale to the survivors of Oceanic Flight 815 . He began as the main antagonist during the second and third seasons , but in subsequent seasons , becomes a morally ambiguous ally to the main characters . Other characters frequently describe him as loyal only to himself , though it is also often hinted that he may be driven by some higher purpose . As with most characters on Lost , Ben 's history is revealed through flashbacks and episodes set in other time periods which are revealed slowly as the series progresses . Sterling Beaumon first portrayed a young Ben late in season three , in the character 's first centric episode , " The Man Behind the Curtain " . Ben 's childhood is further explored in the fifth season of the series , partially set in 1977 . Fifth season e</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added first version of llm_val
</commit_message>
<xml_diff>
--- a/data/top_docs/ctm/elbow_top_docs.xlsx
+++ b/data/top_docs/ctm/elbow_top_docs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,32 +476,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['album', 'song', 'chart', 'music', 'video', 'band', 'songs', 'madonna', 'track', 'pop', 'single', 'recording', 'lyrics', 'vocals', 'billboard']</t>
+          <t>['credits', 'composition', 'allmusic', 'listing', 'charts', 'piano', 'drums', 'beats', 'liner', 'label', 'recording', 'download', 'ballad', 'songwriter', 'vocals']</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Lo Mejor de Mí ( song ) = " Lo Mejor de Mí " ( " All My Best " ) is a song written and produced by Rudy Pérez and first recorded by Spanish singer Juan Ramon for his second studio album Por Haberte Amado Tanto ( 1990 ) . In the song , the protagonist tells his lover how he gave his best despite not meeting his lover 's expectation . In 1997 , Mexican recording artist Cristian Castro covered the song for his fifth studio album Lo Mejor de Mí which Pérez also produced and arranged . Castro 's version peaked at number-one on the Billboard Hot Latin Songs and the Billboard Latin Pop Songs charts in the United States . The song received a Billboard Latin Music Awards and a Lo Nuestro nomination for Pop Song of the Year . Pérez earned the American Society of Composers , Authors and Publishers award in the Pop / Ballad field . = = Background = = In 1990 , Spanish recording artist Juan Ramon released his second studio album Por Haberte Amado Tanto which was arranged and produced by Cuban-Ameri</t>
+          <t>Playlist : The Very Best of Destiny 's Child = Playlist : The Very Best of Destiny 's Child is the third compilation album by American R &amp; B girl group Destiny 's Child . It was released on October 9 , 2012 through Columbia Records matching with the fifteenth anniversary of Destiny 's Child 's formation . The compilation contained fourteen songs from the group 's repertoire consisting of four studio albums . Upon its release , the received positive reviews from critics who praised its track list featuring the band 's most popular songs ; however some of them noted the lack of new material as a downside . It peaked at numbers 77 and 17 on the Billboard 200 and the magazine 's Top R &amp; B / Hip-Hop Albums chart respectively , becoming the highest ranking release of the playlist album series through Legacy Recordings . = = Background and release = = On July 7 , 2012 , Mathew Knowles , the music manager of the group , revealed that Destiny 's Child would reunite after a seven-year-long hiatu</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Hot Tottie = " Hot Tottie " is a song by recording artist Usher . It was written by Usher , Ester Dean , Jay-Z and Polow da Don , with the latter producing it . The song features guest vocals from rapper Jay-Z and background vocals by Ester Dean . It is the second single in the United States and Canada from his EP , Versus , which is an extension of his sixth studio album , Raymond v. Raymond . The song was sent to rhythmic and urban airplay on August 9 , 2010 . " Hot Tottie " samples Big Tymers 's " Big Ballin ' " off their 1998 album How You Luv That Vol . 2 . " Hot Tottie " is an R &amp; B song with hip hop tones , accompanied by strobing , electronic beats . It received positive reviews , with many critics noting it as a standout from the EP . It peaked at number twenty-one on the US Billboard Hot 100 , and was a top ten hit on the US Hot R &amp; B / Hip-Hop Songs chart . Usher performed the song on The Early Show and on his OMG Tour . = = Background and composition = = The song was leaked</t>
+          <t>Here I Stand ( Usher song ) = " Here I Stand " is a song by American recording artist Usher . It was sent to urban adult contemporary radio on August 18 , 2008 by LaFace Records and RCA Records as the fifth single from Usher 's fifth studio album , Here I Stand ( Usher album ) . Penned by the singer with Polow da Don , Adam Blackstone , Gerrell Gaddis , and Dre &amp; Vidal , and produced by Dre &amp; Vidal , " Here I Stand " is a slow soul ballad and contains similarities to Stevie Wonder 's music . The record received critical acclaim , and was nominated for the Best Male R &amp; B Vocal Performance award at the 51st Grammy Awards . " Here I Stand " maintained a position on the United States Hot R &amp; B / Hip-Hop Songs for several weeks in 2008 and 2009 , reaching the top twenty . It also appeared on the US Radio Songs and Bubbling Under Hot 100 Singles charts , peaking at numbers seventy-two and six , respectively . = = Background and composition = = " Here I Stand " was written by Usher , Polow d</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>A + No Poder = A + No Poder ( English : " To the Max " ) is the fourteenth studio album by Mexican recording artist Alejandra Guzmán . It was released on September 11 , 2015 , by Sony Music Latin . After the success of her previous live album , Primera Fila ( 2013 ) and its promotional tour , Guzmán recorded the album with original songs , composed and produced by her and Argentinian musician José Luis Pagán . After its release , A + No Poder received favorable reviews from music critics , with one expressing appreciation for the balance between ballads and rock songs . The record peaked at number twelve on the US Billboard Latin Pop Albums and number six in Mexico . To promote the album , three singles were released : " Adiós " featuring reggaeton performer Farruko , which peaked at number 26 on the Billboard Latin Pop Songs chart , " Qué Ironía " and " Esta Noche " . = = Background = = In 2013 , Alejandra Guzmán released her fourth live album titled Primera Fila , selling 90,000 unit</t>
+          <t>If It 's Over = " If It 's Over " is a song written by American singer-songwriters Mariah Carey and Carole King , with the former and Walter Afanasieff helming its production . It was originally released on September 17 , 1991 on Carey 's second studio effort , Emotions . Lyrically , the song tells of a romance that has withered , and finds the protagonist asking her lover " if it 's over , let me go . " Several months after the release of Emotions , Carey performed the song during her appearance on the television show MTV Unplugged , as the second number on her setlist . Following the release of the extended play ( EP ) MTV Unplugged , the song 's live version was used as the second single for the EP in the third quarter of 1992 . The live single version omits the second verse and chorus , as the songs were shortened for the show . It received a very limited release , being featured as an airplay only single in certain territories . Its only peak was in the Netherlands , where it reac</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Pero Me Acuerdo de Ti = " Pero Me Acuerdo de Ti " ( English : " But I Remember You " ) is a song written and produced by Rudy Pérez . It was first recorded by Puerto Rican singer Lourdes Robles on her album Definitivamente ( 1991 ) . In the ballad , the singer remembers her lover even when she tries to forget . Nine years later , American recording artist Christina Aguilera performed a cover version on her second studio album Mi Reflejo which Pérez also produced . It was released as the second single from the album in December 2000 . The music video for Aguilera 's version was directed by Kevin Bray . Aguilera performed the song live at the 2001 Grammy Awards . Her version peaked at number eight on the Billboard Hot Latin Songs chart in the United States and number three in Spain . It received a Latin Grammy nomination for Record of the Year . It has been covered by Mexican singer Edith Márquez and Jencarlos Canela . = = Background = = In 1991 , Puerto Rican recording artist Lourdes Ro</t>
+          <t xml:space="preserve">Made in America ( Jay-Z and Kanye West song ) = " Made in America " is a song by American hip hop artists Kanye West and Jay-Z , from their first collaborative album Watch the Throne . It is the 11th track on the album and features vocals from OFWGKTA singer Frank Ocean . Lyrically , the song explores themes of family life and the American Dream . It expresses the hardships of youth and coming of age . The track received positive reviews from music critics who praised Ocean 's vocal hook , and the subject matter of the verses . The song has been compared to " inspirational ballads of late-period Michael Jackson . " The song charted on South Korea Gaon International Chart at position 178 . Jay-Z and West performed the song at their 2011 Watch the Throne Tour . = = Background = = Jay-Z and Kanye West are both American rappers who have collaborated on several tracks together . In 2010 , they began production and recording on a collaborative record Watch the Throne . Frank Ocean is an R &amp; </t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rated R : Remixed = Rated R : Remixed ( stylized as Rated R / / / Remixed ) is the second remix album by Barbadian singer Rihanna . It was released on May 8 , 2010 , in Brazil and Europe and on May 24 , 2010 , in the United States by Def Jam Recordings . It contains remixes from her fourth studio album , Rated R ( 2009 ) . The songs were solely remixed by Chew Fu . The majority of the remixes were remastered to incorporate influences from the genre of house music , and incorporate heavy usage of synthesizers as part of their instrumentation . Rated R : Remixed received a mixed review from Jean Goon for MSN Entertainment . She praised Fu for remixing some of the dark and sombre songs into upbeat dance songs , but criticized the album as it did not provide memorability . The album peaked at number four in Greece and number six on the US Dance / Electronic Albums chart ; it peaked at number 33 on the US Top R &amp; B / Hip-Hop Albums chart and number 158 on the US Billboard 200 chart . As of </t>
+          <t xml:space="preserve">My Hands = " My Hands " is a song recorded by British singer-songwriter Leona Lewis for her second studio album Echo ( 2009 ) . It was written by Arnthor Birgisson and Ina Wroldsen and produced by the former . Alongside Birgisson , Lewis was involved with the song 's vocal production . Lyrically , it is about life after the end of a relationship . The strings were performed by Urban Soul Orchestra , who were led by Simon Fischer . " My Hands " was selected as the official theme song for the English version of the video game Final Fantasy XIII . Lewis decided to accept the offer of her track being used as she felt as though she connected with the video game 's female protagonist , Lightning . The song garnered a mixed response from music critics , who described it as forgettable , despite noting that Lewis performs the song undeniably well . In March 2010 , " My Hands " debuted on the UK Singles Chart at number 145 . = = Background and production = = " My Hands " was recorded for Lewis </t>
         </is>
       </c>
     </row>
@@ -511,32 +511,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['tropical', 'storm', 'hurricane', 'winds', 'depression', 'cyclone', 'mph', 'damage', 'rainfall', 'landfall', 'utc', 'wind', 'weakened', 'flooding', 'intensity']</t>
+          <t>['film', 'release', 'released', 'million', 'story', 'scene', 'scenes', 'script', 'effects', 'production', 'opening', 'plot', 'filming', 'original', 'director']</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">1949 Pacific hurricane season = The 1949 Pacific hurricane season was the first hurricane season in the Eastern Pacific hurricane database . Six tropical cyclones were known to have existed during the season , of which the first formed on June 11 and the final dissipated on September 30 . Another tropical cyclone had formed within the basin in 1949 , but was included in the Atlantic hurricane database , had it been classified operationally in the Eastern Pacific basin , would have tallied the overall season to seven tropical cyclones . In addition , there were two tropical cyclones that attained hurricane status , but none of them reached major hurricane intensity ( Category 3 or higher on the Saffir-Simpson Hurricane Scale ) . Tropical Storm Three threatened the Baja California Peninsula , while an unnumbered hurricane crossed into the Atlantic , later becoming the 1949 Texas hurricane . = = Season summary = = Tropical cyclones were recorded in the Eastern Pacific best track database </t>
+          <t xml:space="preserve">The Evil Dead = The Evil Dead is a 1981 American black comedy horror film written and directed by Sam Raimi and executive produced by Raimi and Bruce Campbell , who also stars alongside Ellen Sandweiss and Betsy Baker . The film focuses on five college students vacationing in an isolated cabin in a remote wooded area . After they find an audiotape that releases a legion of demons and spirits , members of the group suffer from demonic possession , leading to increasingly gory mayhem . Raimi and the cast produced the short film Within the Woods as a " prototype " to build the interest of potential investors , which secured Raimi US $ 90,000 to produce The Evil Dead . The film was shot on location in a remote cabin located in Newport , Tennessee , in a difficult filming process that proved extremely uncomfortable for the majority of the cast and crew . The low-budget horror film attracted the interest of producer Irvin Shapiro , who helped screen the film at the 1982 Cannes Film Festival </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1852 Atlantic hurricane season = The 1852 Atlantic hurricane season was one of only three Atlantic hurricane seasons in which every known tropical cyclone attained hurricane status . Five tropical cyclones were reported during the season , which lasted from late August through the middle of October ; these dates fall within the range of most Atlantic tropical cyclone activity , and none of the cyclones coexisted with another . Though there were officially five tropical cyclones in the season , hurricane scholar Michael Chenoweth assessed two of the cyclones as being the same storm . There may have been other unconfirmed tropical cyclones during the season , as meteorologist Christopher Landsea estimated that up to six storms were missed each year from the official database ; this estimate was due to small tropical cyclone size , sparse ship reports , and relatively unpopulated coastlines . = = Season summary = = Every tropical cyclone in the season was of hurricane status , or with win</t>
+          <t>Despicable Me 2 = Despicable Me 2 is a 2013 American 3D computer-animated comedy film and the sequel to the 2010 animated film Despicable Me . Produced by Illumination Entertainment for Universal Pictures , and animated by Illumination Mac Guff , the film is directed by Pierre Coffin and Chris Renaud , and written by Cinco Paul and Ken Daurio . Steve Carell , Russell Brand , Miranda Cosgrove , Elsie Fisher , and Dana Gaier reprise their roles as Gru , Dr. Nefario , Margo , Agnes , and Edith respectively . Kristen Wiig , who played Miss Hattie in the first film , voices agent Lucy Wilde , while Ken Jeong , who played the Talk Show Host , voices Floyd Eagle-san . New cast members include Benjamin Bratt as Eduardo " El Macho " Pérez and Steve Coogan as Silas Ramsbottom , head of the Anti-Villain League ( AVL ) . The film premiered on June 5 , 2013 in Australia , and was theatrically released in the United States on July 3 , 2013 . The film received mostly positive reviews from critics , a</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">1930 Atlantic hurricane season = The 1930 Atlantic hurricane season was the second least active Atlantic hurricane season on record – behind only 1914 – with only three systems reaching tropical storm intensity . Of those three , two reached hurricane status , both of which also became major hurricanes , Category 3 or higher storms on the Saffir – Simpson hurricane wind scale . The first system developed in the central Atlantic Ocean on August 21 . Later that month , a second storm , the Dominican Republic hurricane , formed on August 29 . It peaked as a Category 4 hurricane with winds of 155 mph ( 250 km / h ) . The third and final storm dissipated on October 21 . Due to the lack of systems that developed , only one tropical cyclone , the second hurricane , managed to make landfall during the season . It severely impacted areas of the Greater Antilles , particularly the Dominican Republic , before making subsequent landfalls on Cuba and the U.S. states of Florida and North Carolina , </t>
+          <t>Never Say Never Again = Never Say Never Again is a 1983 British spy film directed by Irvin Kershner , produced by Jack Schwartzman , and written by Lorenzo Semple Jr. with uncredited additional co-writers Dick Clement and Ian La Frenais , from a story by Kevin McClory , Jack Whittingham , and Ian Fleming . It is the second adaption of Fleming 's Thunderball , which was previously adapted as the 1965 film of the same name . Unlike the majority of Bond films , Never Say Never Again was not produced by Eon Productions , but by an independent production company , one of whose members was Kevin McClory . McClory , one of the original writers of the Thunderball storyline , retained the filming rights of the novel following a rights controversy . Sean Connery played the role of James Bond for the seventh time , marking his return to the character 12 years after Diamonds Are Forever . The film 's title is a reference to Connery 's reported declaration in 1971 that he would " never again " play</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1929 Atlantic hurricane season = The 1929 Atlantic hurricane season was among the least active hurricane seasons in the Atlantic on record – featuring only five tropical cyclones . Of these five tropical systems , three of them intensified into a hurricane , with one strengthening further into a major hurricane ( Category 3 or higher on the Saffir – Simpson hurricane wind scale ) . The first tropical cyclone of the season developed in the Gulf of Mexico on June 27 . Becoming a hurricane on June 28 , the storm struck Texas , bringing strong winds to a large area . Three fatalities were reported , while damage was conservatively estimated at $ 675,000 ( 1929 USD ) . The second storm , nicknamed the Bahamas hurricane , developed north of the Lesser Antilles . It was the most intense tropical cyclone of the season , peaking as a Category 4 hurricane on the Saffir – Simpson hurricane wind scale with maximum sustained winds of 155 mph ( 250 km / h ) and a minimum barometric pressure of 924 m</t>
+          <t>Speed 2 : Cruise Control = Speed 2 : Cruise Control is a 1997 American disaster thriller film , and a sequel to Speed ( 1994 ) . The film was produced and directed by Jan de Bont , and written by Randall McCormick and Jeff Nathanson , based on a story by de Bont and McCormick . Sandra Bullock stars in the film , reprising her role from Speed , while Jason Patric and Willem Dafoe co-star . The film was released by 20th Century Fox on June 13 , 1997 . The plot involves couple Annie and Alex taking a vacation in the Caribbean aboard a luxury cruise ship , which is hijacked by a villain named Geiger who hacked into the ship 's computer system . As they are trapped aboard the ship , Annie and Alex work with the ship 's first officer to try to stop the ship , which they discover is programmed to crash into an oil tanker . De Bont came up with the idea for the film after he had a recurring nightmare about a cruise ship crashing into an island . Speed star Keanu Reeves was initially supposed t</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">1939 Pacific hurricane season = The 1939 Pacific hurricane season ran through the summer and fall of 1939 . Before the satellite age started in the 1960s , data on east Pacific hurricanes are extremely unreliable . Most east Pacific storms are of no threat to land . However , 1939 saw a large number of storms threaten California . = = Storms = = = = = Hurricane One = = = On June 12 , a hurricane was detected . The lowest pressure reported by a ship was 985 mbar ( 29.1 inHg ) . The hurricane was last seen June 13 . = = = Possible Tropical Cyclone Two = = = A possible tropical cyclone was located off the coast of Mexico on June 27 . A ship reported a gale and a pressure of 1,006 mbar ( 29.7 inHg ) . The system was last seen on June 28 . = = = Tropical Cyclone Three = = = On July 19 , a tropical cyclone was detected . A ship reported a pressure of 1,000.7 millibars ( 29.55 inHg ) . = = = Tropical Cyclone Four = = = On July 29 , a tropical cyclone was located midway between Manzanillo and </t>
+          <t>Escape from Tomorrow = Escape from Tomorrow is a 2013 American black-and-white independent fantasy horror film , the debut of writer and director Randy Moore . It follows an unemployed father having increasingly bizarre experiences and disturbing visions on the last day of a family vacation at the Walt Disney World Resort . It premiered in January at the 2013 Sundance Film Festival and was later a personal selection of Roger Ebert , shown at his 15th annual film festival in Champaign , Illinois . The film was a 2012 official selection of the PollyGrind Film Festival , but at the time filmmakers were still working on some legal issues and asked that it not be screened . It drew attention because Moore had shot most of it on location at both Walt Disney World and Disneyland without permission from The Walt Disney Company , owner and operator of both parks . Due to Disney 's reputation of being protective of its intellectual property , the cast and crew used guerrilla filmmaking technique</t>
         </is>
       </c>
     </row>
@@ -546,32 +546,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>['episode', 'mulder', 'scully', 'doctor', 'episodes', 'trek', 'files', 'series', 'character', 'enterprise', 'viewers', 'television', 'season', 'broadcast', 'star']</t>
+          <t>['career', 'hit', 'games', 'season', 'league', 'baseball', 'major_league_baseball', 'signed', 'home', 'played', 'manager', 'professional', 'minor', 'earned', 'hits']</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>This Is Not Happening = " This Is Not Happening " is the fourteenth episode of the eighth season and the 175th episode overall of the science fiction television series The X-Files . The episode first aired in the United States on February 25 , 2001 on the Fox Network , and subsequently aired in the United Kingdom . It was written by executive producers Chris Carter and Frank Spotnitz , and directed by Kim Manners . The episode received a Nielsen household rating of 9.7 and was watched by 16.9 million viewers , making it the highest-rated episode of the season . " This Is Not Happening " was received positively by television critics . The series centers on FBI special agents Dana Scully ( Gillian Anderson ) and her new partner John Doggett ( Robert Patrick ) — following the alien abduction of her former partner , Fox Mulder ( David Duchovny ) — who work on cases linked to the paranormal , called X-Files . In this episode , Scully , Doggett , and Walter Skinner ( Mitch Pileggi ) discover</t>
+          <t>Ryan Garko = Ryan Francis Garko ( born January 2 , 1981 ) is a former professional baseball outfielder , first baseman , and designated hitter . In college , he was a catcher . He has played for the Cleveland Indians , the San Francisco Giants , and the Texas Rangers in Major League Baseball as well as the Samsung Lions in the Korea Baseball Organization . Garko is seen by former ESPN reporter John Sickels as a good hitter who hits to all parts of the field , but with poor defensive instincts . Through 2010 , he has a .275 career average , 427 hits , 55 home runs , and 250 RBI in 463 games . When he attended Stanford University , Garko won the Johnny Bench Award and was named the Pac-10 Co-Player of the Year his senior year . He was also voted onto the College World Series Legends Team , featuring 28 of the best College World Series players as voted upon by fans , writers , and head coaches . During his time in the Cleveland Indians ' organization , Garko was converted into a first bas</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>The X-Files ( season 2 ) = The second season of the science fiction television series The X-Files commenced airing on the Fox network in the United States on September 16 , 1994 , concluded on the same channel on May 19 , 1995 , after airing all 25 episodes . The series follows Federal Bureau of Investigation special agents Fox Mulder and Dana Scully , portrayed by David Duchovny and Gillian Anderson respectively , who investigate paranormal or supernatural cases , known as X-Files by the FBI . The second season of The X-Files takes place after the closure of the department following the events of the first season finale . In addition to stand-alone " Monster-of-the-Week " episodes , several episodes also furthered the alien conspiracy mythology that had begun to form . Season two introduced several recurring characters — X ( Steven Williams ) , an informant to Mulder ; Alex Krycek ( Nicholas Lea ) , Mulder 's partner-turned-enemy ; and the Alien Bounty Hunter ( Brian Thompson ) , a sh</t>
+          <t>Doug Fister = Douglas Wildes Fister ( born February 4 , 1984 ) is an American professional baseball pitcher for the Houston Astros of Major League Baseball ( MLB ) . He previously played in MLB for the Seattle Mariners , Detroit Tigers and Washington Nationals . Fister bats left-handed , and throws right-handed . He was born in Merced , California and attended Golden Valley High School . He then attended Merced College , and later Fresno State University . He spent four seasons ( 2006 – 2009 ) in the Seattle Mariners minor league organization before being promoted to their Major League roster in 2009 . = = Early life = = Fister was born February 4 , 1984 , to Larry and Jan Fister . Larry Fister is a fire captain who played football at Fresno State University from 1976 to 1977 . Jan is a homemaker . Fister has three siblings ; a brother and two sisters . He grew up in Merced , California where he began playing baseball at the age of six . He was a fan of both the Oakland Athletics and S</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Wetwired = " Wetwired " is the twenty-third episode of the third season and the 72nd episode overall of the science fiction television series The X-Files . The episode first aired in the United States on May 10 , 1996 on Fox . It was written by the show 's visual effect designer Mat Beck , and directed by Rob Bowman . The episode earned a Nielsen rating of 9.7 and was viewed by 14.48 million people . The episode received mostly positive reviews from television critics . The show centers on FBI special agents Fox Mulder ( David Duchovny ) and Dana Scully ( Gillian Anderson ) who work on cases linked to the paranormal , called X-Files . Mulder is a believer in the paranormal , while the skeptical Scully has been assigned to debunk his work . In this episode , Mulder and Scully investigate a series of murders committed by ordinary citizens angered after seeing illusory images . Scully 's trust in Mulder is put to the ultimate test . " Wetwired " was written by Mat Beck , the show 's visua</t>
+          <t xml:space="preserve">Dave Martinez = David Martinez ( born September 26 , 1964 ) is an American professional baseball coach and former outfielder . He is the bench coach for the Chicago Cubs of Major League Baseball ( MLB ) . He played in MLB for the Cubs , Montreal Expos , Cincinnati Reds , San Francisco Giants , Chicago White Sox , Tampa Bay Devil Rays , Texas Rangers , Toronto Blue Jays , and Atlanta Braves from 1986 to 2001 . Martinez had a .276 career batting average , 1,599 hits , 91 home runs , 795 runs scored , and 580 runs batted in . Martinez became the bench coach for the Tampa Bay Rays in 2008 , during which time he became a candidate for several managerial positions in MLB . After Rays ' manager Joe Maddon became manager of the Cubs after the 2014 season , Martinez joined the Cubs as their bench coach . = = Early life = = Martinez was born in Brooklyn , New York , to Puerto Rican parents . He lived at East 93rd Street and Lexington Avenue in Manhattan . At age 13 , his family moved to Orlando </t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>The X-Files ( season 8 ) = The eighth season of the American science fiction television series The X-Files commenced airing in the United States on November 5 , 2000 , concluded on May 20 , 2001 , and consisted of twenty-one episodes . Season eight takes place after Fox Mulder 's ( David Duchovny ) alien abduction in the seventh season . The story arc for the search of Mulder continues until the second half of the season , while a new arc about Dana Scully 's ( Gillian Anderson ) pregnancy is formed . This arc would continue , and end , with the next season . The season explores various themes such as life , death , and belief . For this season , Duchovny elected to return only as an intermittent main character , appearing in only half of the episodes . Actor Robert Patrick was hired as a replacement for Mulder , playing John Doggett . The season also marked the first appearance of Annabeth Gish as Monica Reyes , who would become a main character in the ninth season . In addition to th</t>
+          <t>Wally Pipp = Walter Clement Pipp ( February 17 , 1893 – January 11 , 1965 ) was an American professional baseball player . A first baseman , Pipp played in Major League Baseball ( MLB ) for the Detroit Tigers , New York Yankees , and Cincinnati Reds between 1913 and 1928 . After appearing in 12 games for the Tigers in 1913 and playing in the minor leagues in 1914 , he was purchased by the Yankees before the 1915 season . They made him their starting first baseman . He and Home Run Baker led an improved Yankee lineup that led the league in home runs . He led the American League in home runs in 1916 and 1917 . With Babe Ruth , Bob Meusel , Joe Dugan , and Waite Hoyt , the Yankees won three consecutive American League pennants from 1921 through 1923 , and won the 1923 World Series . In 1925 , he lost his starting role to Lou Gehrig , after which he finished his major league career with Cincinnati . Pipp is considered to be one of the best power hitters of the dead ball era . Pipp is now b</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Ascension ( The X-Files ) = " Ascension " is the sixth episode of the second season of the American science fiction television series The X-Files . It premiered on the Fox network on October 21 , 1994 . It was written by Paul Brown , directed by Michael Lange , and featured guest appearances by Steve Railsback , Nicholas Lea , Steven Williams and Sheila Larken . The episode helped explore the series ' overarching mythology . The show centers on FBI special agents Fox Mulder ( David Duchovny ) and Dana Scully ( Gillian Anderson ) who work on cases linked to the paranormal , called X-Files . However , the events of " Ascension " are a continuation of the plot of the preceding episode , " Duane Barry " . Following the kidnapping of Scully by an unhinged alien abductee Duane Barry ( Steve Railsback ) , Mulder races to track her down . The decision to have the character of Scully abducted was driven by necessity , as Anderson had become pregnant and required time off from production . " Asc</t>
+          <t>1951 National League tie-breaker series = The 1951 National League tie-breaker series was a best-of-three playoff series at the conclusion of Major League Baseball 's ( MLB ) 1951 regular season to decide the winner of the National League ( NL ) pennant . The games were played on October 1 , 2 , and 3 , 1951 , between the New York Giants and Brooklyn Dodgers . It was necessary after both teams finished the season with identical win – loss records of 96 – 58 . It is most famous for the walk-off home run hit by Bobby Thomson of the Giants in the deciding game , which has come to be known as baseball 's " Shot Heard ' Round the World " . This was the second three-game playoff in NL history . After no tiebreakers had been needed since the American League ( AL ) became a major league in 1901 , this was the third such tie in the previous six seasons . The Dodgers had been involved in the previous one as well , losing to the St. Louis Cardinals during the 1946 season in two straight games . I</t>
         </is>
       </c>
     </row>
@@ -581,32 +581,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['ship', 'guns', 'ships', 'tons', 'torpedo', 'knots', 'cruiser', 'inch', 'fleet', 'cruisers', 'deck', 'gun', 'turrets', 'admiral', 'steam']</t>
+          <t>['work', 'life', 'wrote', 'writing', 'published', 'book', 'written', 'women', 'works', 'history', 'world', 'writer', 'woman', 'early', 'books']</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>German aircraft carrier I ( 1915 ) = The aircraft carrier I was the first planned aircraft carrier conversion project of the German Imperial Navy ( Kaiserliche Marine ) during World War I. The Imperial Navy had experimented previously with seaplane carriers , though these earlier conversions were too slow to operate with the High Seas Fleet and carried an insufficient number of aircraft . I was intended to carry between 23 and 30 aircraft , including fighters , bombers , and torpedo-bombers . The ship was based on the incomplete hull of the Italian passenger ship Ausonia , which was being built in Hamburg . The conversion was proposed by the Air Department of the Reichs Navy Office , but it was abandoned after negotiations within the German Navy over a proposed moratorium on new ships at the end of the war . After World War I ended , high inflation in Germany added to the cost of the ship , and as a result , the Italian shipping company for whom the ship was originally built , declined</t>
+          <t xml:space="preserve">Feminism in India = Feminism in India is a set of movements aimed at defining , establishing , and defending equal political , economic , and social rights and equal opportunities for Indian women . It is the pursuit of women 's rights within the society of India . Like their feminist counterparts all over the world , feminists in India seek gender equality : the right to work for equal wages , the right to equal access to health and education , and equal political rights . Indian feminists also have fought against culture-specific issues within India 's patriarchal society , such as inheritance laws and the practice of widow immolation known as Sati . The history of feminism in India can be divided into three phases : the first phase , beginning in the mid-nineteenth century , initiated when male European colonists began to speak out against the social evils of Sati ; the second phase , from 1915 to Indian independence , when Gandhi incorporated women 's movements into the Quit India </t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">French battlecruiser proposals = In the years before the outbreak of World War I in 1914 , the French Navy considered several proposals for battlecruisers . The Navy issued specifications for a battlecruiser design to complete part of the 28 capital ships to be built by 1920 . Three designs , one by P. Gille and two by Lieutenant Durand-Viel , were completed in 1913 . All three designs were similar to contemporary battleship designs , specifically the Normandie class , which introduced a quadruple gun turret for the main battery , which was adopted for all three proposals . The first two called for the same 340 mm ( 13 in ) gun used on all French dreadnoughts , though the third proposed a much more powerful 370 mm ( 15 in ) gun . Though the design studies were complete , the French Navy did not authorize or begin construction of any battlecruisers before the start of the war . = = Background = = In the Naval Law of 30 March 1912 , the French Navy called for a total force of 20 capital </t>
+          <t>Tristan Tzara = Tristan Tzara ( French : [ tʁistɑ ̃ dzaʁa ] ; Romanian : [ trisˈtan ˈt ͡ sara ] ; born Samuel or Samy Rosenstock , also known as S. Samyro ; April 16 [ O.S. April 4 ] 1896 – December 25 , 1963 ) was a Romanian and French avant-garde poet , essayist and performance artist . Also active as a journalist , playwright , literary and art critic , composer and film director , he was known best for being one of the founders and central figures of the anti-establishment Dada movement . Under the influence of Adrian Maniu , the adolescent Tzara became interested in Symbolism and co-founded the magazine Simbolul with Ion Vinea ( with whom he also wrote experimental poetry ) and painter Marcel Janco . During World War I , after briefly collaborating on Vinea 's Chemarea , he joined Janco in Switzerland . There , Tzara 's shows at the Cabaret Voltaire and Zunfthaus zur Waag , as well as his poetry and art manifestos , became a main feature of early Dadaism . His work represented Dad</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>SMS Frithjof = SMS Frithjof was the third vessel of the six-member Siegfried class of coastal defense ships ( Küstenpanzerschiffe ) built for the German Imperial Navy . Her sister ships were Siegfried , Beowulf , Heimdall , Hildebrand , and Hagen . Frithjof was built by the AG Weser shipyard between 1890 and 1893 , and was armed with a main battery of three 24-centimeter ( 9.4 in ) guns . She served in the German fleet throughout the 1890s and was rebuilt in 1900 - 1902 . She served in the VI Battle Squadron after the outbreak of World War I in August 1914 , but saw no action . Frithjof was demobilized in 1915 and used as a barracks ship thereafter . She was rebuilt as a merchant ship in 1923 and served in this capacity until she was broken up for scrap in 1930 . = = Design = = Frithjof was 79 meters ( 259 ft ) long overall and had a beam of 14.90 m ( 48.9 ft ) and a maximum draft of 5.74 m ( 18.8 ft ) . She displaced 3,741 long tons ( 3,801 t ) at full combat load . Her propulsion sys</t>
+          <t>Aleister Crowley = Aleister Crowley ( / ˈkroʊli / ; born Edward Alexander Crowley ; 12 October 1875 – 1 December 1947 ) was an English occultist , ceremonial magician , poet , painter , novelist , and mountaineer . He founded the religion and philosophy of Thelema , identifying himself as the prophet entrusted with guiding humanity into the Æon of Horus in the early 20th century . Born to a wealthy Plymouth Brethren family in Royal Leamington Spa , Warwickshire , Crowley rejected this fundamentalist Christian faith to pursue an interest in Western esotericism . He was educated at the University of Cambridge , where he focused his attentions on mountaineering and poetry , resulting in several publications . Some biographers allege that here he was recruited into a British intelligence agency , further suggesting that he remained a spy throughout his life . In 1898 he joined the esoteric Hermetic Order of the Golden Dawn , where he was trained in ceremonial magic by Samuel Liddell MacGre</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>SMS Medusa = SMS Medusa was the seventh member of the ten-ship Gazelle class , built by the Imperial German Navy . She was built by the AG Weser dockyard in Bremen , laid down in early 1900 , launched in December 1900 , and commissioned into the High Seas Fleet in July 1901 . Armed with a main battery of ten 10.5 cm ( 4.1 in ) guns and two 45 cm ( 18 in ) torpedo tubes , Medusa was capable of a top speed of 21.5 knots ( 39.8 km / h ; 24.7 mph ) . Medusa served in all three German navies over the span of over forty years . She served as a fleet scout in the period before World War I , and during the first two years of the conflict , she was used as a coastal defense ship . She was one of six cruisers Germany was allowed to keep by the Treaty of Versailles , and she served in the early 1920s in the Reichsmarine . She was withdrawn from service in 1924 and used in secondary duties , but in 1940 , the Kriegsmarine converted Medusa into a floating anti-aircraft battery . She defended the po</t>
+          <t>Elizabeth Cady Stanton = Elizabeth Cady Stanton ( November 12 , 1815 – October 26 , 1902 ) was an American suffragist , social activist , abolitionist , and leading figure of the early women 's rights movement . Her Declaration of Sentiments , presented at the Seneca Falls Convention held in 1848 in Seneca Falls , New York , is often credited with initiating the first organized women 's rights and women 's suffrage movements in the United States . Stanton was president of the National Woman Suffrage Association from 1892 until 1900 . Before Stanton narrowed her political focus almost exclusively to women 's rights , she was an active abolitionist with her husband Henry Brewster Stanton ( co-founder of the Republican Party ) and cousin Gerrit Smith . Unlike many of those involved in the women 's rights movement , Stanton addressed various issues pertaining to women beyond voting rights . Her concerns included women 's parental and custody rights , property rights , employment and income</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>SMS Undine = SMS Undine was the last member of the ten-ship Gazelle class , built by the Imperial German Navy . She was built by the Howaldtswerke shipyard in Kiel , laid down in 1901 , launched in December 1902 , and commissioned into the High Seas Fleet in January 1904 . Armed with a main battery of ten 10.5 cm ( 4.1 in ) guns and two 45 cm ( 18 in ) torpedo tubes , Undine was capable of a top speed of 21.5 knots ( 39.8 km / h ; 24.7 mph ) . Undine was initially used as a artillery training ship for the gunners of the German fleet . In November 1904 , she accidentally rammed and sank the torpedo boat SMS S26 while on maneuvers off Kiel ; thirty-three men were killed in the incident . After the outbreak of World War in August 1914 , Undine was deployed to the Baltic Sea for use as a coastal defense ship . She was attacked by the British submarine HMS E19 on 7 November 1915 and was hit by two torpedoes , the second of which detonated the ship 's ammunition magazines . Undine exploded a</t>
+          <t>R. K. Narayan = R. K. Narayan ( 10 October 1906 – 13 May 2001 ) , full name Rasipuram Krishnaswami Iyer Narayanaswami , is an Indian writer , best known for his works set in the fictional South Indian town of Malgudi . He is a leading author of early Indian literature in English , along with Mulk Raj Anand and Raja Rao . Narayan 's mentor and friend , Graham Greene was instrumental in getting publishers for Narayan ’ s first four books , including the semi-autobiographical trilogy of Swami and Friends , The Bachelor of Arts and The English Teacher . The fictional town of Malgudi , was first introduced in Swami and Friends . Narayan ’ s The Financial Expert , was hailed as one of the most original works of 1951 , and Sahitya Akademi Award winner The Guide , was adapted for film and for Broadway . Narayan highlights the social context and everyday life of his characters , and he has been compared to William Faulkner , who also created a similar fictional town , and likewise explored with</t>
         </is>
       </c>
     </row>
@@ -616,32 +616,32 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['species', 'genus', 'shark', 'females', 'prey', 'eggs', 'males', 'cap', 'sharks', 'fruit', 'stem', 'brown', 'habitat', 'birds', 'specimens']</t>
+          <t>['tons', 'beam', 'deck', 'consisted', 'guns', 'laid', 'horsepower', 'armor', 'hull', 'boilers', 'displaced', 'steam', 'mounted', 'armament', 'battery']</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Myco-heterotrophy = Myco-heterotrophy ( Greek : μυκός mykós , " fungus " , ἕτερος heteros = " another " , " different " and τροφή trophe = " nutrition " ) is a symbiotic relationship between certain kinds of plants and fungi , in which the plant gets all or part of its food from parasitism upon fungi rather than from photosynthesis . A myco-heterotroph is the parasitic plant partner in this relationship . Myco-heterotrophy is considered a kind of cheating relationship and myco-heterotrophs are sometimes informally referred to as " mycorrhizal cheaters " . This relationship is sometimes referred to as mycotrophy , though this term is also used for plants that engage in mutualistic mycorrhizal relationships . = = Relationship between myco-heterotrophs and host fungi = = Full ( or obligate ) myco-heterotrophy exists when a non-photosynthetic plant ( a plant largely lacking in chlorophyll or otherwise lacking a functional photosystem ) gets all of its food from the fungi that it parasitize</t>
+          <t xml:space="preserve">Océan-class ironclad = The Océan class ironclads were a group of three wooden-hulled armored frigates built for the French Navy in the mid to late 1860s . Océan attempted to blockade Prussian ports in the Baltic Sea in 1870 during the Franco-Prussian War . Marengo participated in the French conquest of Tunisia in 1881 . Suffren was often used as the flagship for the squadron she was assigned to . She was flagship of the Cherbourg Division , the Channel Division , Mediterranean Squadron and the Northern Squadron during her career . The ships were discarded during the 1890s . = = Design and description = = The Océan-class ironclads were designed by Henri Dupuy de Lôme as an improved version of the Provence-class ironclads . The ships were central battery ironclads with the armament concentrated amidships . For the first time in a French ironclad three watertight iron bulkheads were fitted in the hull . Like most ironclads of their era they were equipped with a metal-reinforced ram . The </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Cortinarius iodes = Cortinarius iodes , commonly known as the spotted cort or the viscid violet cort , is a species of agaric fungus in the family Cortinariaceae . The fruit bodies have small , slimy , purple caps up to 6 cm ( 2.4 in ) in diameter that develop yellowish spots and streaks in maturity . The gill color changes from violet to rusty or grayish brown as the mushroom matures . The species range includes the eastern North America , Central America , northern South America , and northern Asia , where it grows on the ground in a mycorrhizal association with deciduous trees . Although edible , the mushroom is not recommended for consumption . Cortinarius iodeoides , one of several potential lookalike species , can be distinguished from C. iodes by its bitter-tasting cap cuticle . = = Taxonomy = = The species was first described scientifically by Miles Joseph Berkeley and Moses Ashley Curtis in 1853 . The type collection was made by American botanist Henry William Ravenel in South</t>
+          <t>French ironclad Victorieuse = Victorieuse ( Victorious ) was the second ship of the La Galissonnière class of wooden-hulled , armored corvettes built for the French Navy during the 1870s . Her construction was delayed for years and the navy took advantage of the extended construction time to upgrade her armament in comparison to the lead ship , La Galissonnière . Unlike her sisters , Victorieuse did not see any combat although she participated in the pacification of the Marquesas Islands in 1880 . She was condemned in 1900 . = = Design and description = = The La Galissonnière-class ironclads were designed as faster , more heavily armed versions of the Alma-class ironclads by Henri Dupuy de Lôme . They used the same central battery layout as their predecessors , although the battery was lengthened 4 meters ( 13 ft 1 in ) to provide enough room to work the larger 240-millimeter ( 9.4 in ) guns . Victorieuse and her sister ship Triomphante were modified by Sabattier who reduced the number</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hygrophoropsis = Hygrophoropsis is a genus of gilled fungi in the family Hygrophoropsidaceae . It was circumscribed in 1888 to contain the type species , H. aurantiaca , a widespread fungus that , based on its appearance , has been affiliated with Cantharellus , Clitocybe , and Paxillus . Modern molecular phylogenetic analysis shows that the genus belongs to the suborder Coniophorineae of the order Boletales . There are 16 accepted species of Hygrophoropsis , found in both the Northern and Southern Hemispheres . Hygrophoropsis is a saprophytic genus that causes brown rot in the wood it colonises . The fruit bodies grow on the ground in woodlands , on moss , peat , and on woodchips . They are convex to infundibuliform ( funnel-shaped ) and have decurrent , forked brightly colored gills . The spores are dextrinoid , meaning that they stain reddish-brown in Melzer 's reagent . Because H. aurantiaca has orange gills , it has been mistaken for a chanterelle , and hence it has been called a </t>
+          <t>Italian ironclad Principe Amedeo = Principe Amedeo was an ironclad warship built by the Italian Regia Marina in the 1860s and 1870s . She was the lead ship of the Principe Amedeo class , alongside her sister ship Palestro . Principe Amedeo was laid down in 1865 , launched in 1872 , and completed in late 1874 . She was armed with a battery of six 10 in ( 254 mm ) guns and one 11 in ( 279 mm ) gun . The last sail-rigged ironclad of the Italian fleet , she had a single steam engine that was capable of propelling the ship at a speed of slightly over 12 knots ( 22 km / h ; 14 mph ) . Principe Amedeo 's lengthy construction time rendered her obsolescent by the time she entered service . As a result , she primarily served as a station ship in Italy 's overseas empire . In November 1881 , she collided with the ironclad Roma in a storm in Naples . Principe Amadeo was withdrawn from service in 1888 and converted into a headquarters ship for the vessels defending Taranto . She was stricken from t</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Lactarius deterrimus = Lactarius deterrimus , also known as false saffron milkcap or orange milkcap , is a species of fungus in the family Russulaceae . The fungus produces medium-sized fruit bodies ( mushrooms ) with orangish caps up to 12 cm ( 4.7 in ) wide that develop green spots in old age or if injured . Its orange-coloured latex stains maroon within 30 minutes . Lactarius deterrimus is a mycorrhizal fungus that associates with Norway spruce and bearberry . The species is distributed in Europe , but has also found in parts of Asia . A visually similar species in the United States and Mexico is not closely related to the European species . Fruit bodies appear between late June and November , usually in spruce forests . Although the fungus is edible — like all Lactarius mushrooms from the section Deliciosi — its taste is often bitter , and it is not highly valued . The fruit bodies are used as source of food for the larvae of several insect species . Lactarius deterrimus can be dis</t>
+          <t>Italian cruiser Caprera = Caprera was a torpedo cruiser of the Partenope class built for the Italian Regia Marina ( Royal Navy ) in the 1880s . She was built by the Cantiere navale fratelli Orlando shipyard ; her keel was laid in July 1891 , she was launched in May 1894 , and was commissioned in December 1895 . Her main armament were her five torpedo tubes , which were supported by a battery of eleven small-caliber guns . Caprera spent most of her career in the main Italian fleet , where she was primarily occupied with training exercises . She served in the Red Sea during the Italo-Turkish War of 1911 – 12 , where she conducted shore bombardments and blockaded Ottoman ports in the area . Caprera did not remain in service long after the war , being sold for scrap in May 1913 . = = Design = = Caprera was 73.1 meters ( 239 ft 10 in ) long overall and had a beam of 8.22 m ( 27 ft 0 in ) and an average draft of 3.48 m ( 11 ft 5 in ) . She displaced 833 metric tons ( 820 long tons ; 918 shor</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Guepinia = Guepinia is a genus of fungus in the Auriculariales order . It is a monotypic genus , containing the single species Guepinia helvelloides , commonly known as the apricot jelly . The fungus produces salmon-pink , ear-shaped , gelatinous fruit bodies that grow solitarily or in small tufted groups on soil , usually associated with buried rotting wood . The fruit bodies are 4 – 10 cm ( 1.6 – 3.9 in ) tall and up to 17 cm ( 6.7 in ) wide ; the stalks are not well-differentiated from the cap . The fungus , although rubbery , is edible , and may be eaten raw with salads , pickled , or candied . It has a white spore deposit , and the oblong to ellipsoid spores measure 9 – 11 by 5 – 6 micrometers . The fungus is widely distributed in the Northern Hemisphere , and has also been collected from South America . = = Taxonomy = = The species was first described and illustrated as Tremella rufa by Nicolaus Joseph von Jacquin in 1778 . Elias Magnus Fries later ( 1828 ) called it Guepinia hel</t>
+          <t>French battleship Jauréguiberry = Jauréguiberry was a pre-dreadnought battleship of the French Navy ( French : Marine Nationale ) , launched in 1893 . She was one of the class of five roughly similar battleships built in the 1890s , including Masséna , Bouvet , Carnot , and Charles Martel ; Jauréguiberry and the latter two are sometimes erroneously referenced as a single class . She was named after Admiral Bernard Jauréguiberry . Jauréguiberry was in the Mediterranean when World War I began and she spent most of 1914 escorting troop convoys from North Africa and India to France . She supported French troops during the Gallipoli Campaign in 1915 before she became guardship at Port Said from 1916 for the rest of the war . Upon her return to France in 1919 she became an accommodation hulk until 1932 . She was sold for scrapping in 1934 . = = Design and description = = The Charles Martel group of battleships all shared the same layout for their main and secondary armament — a design that m</t>
         </is>
       </c>
     </row>
@@ -651,32 +651,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['highway', 'route', 'road', 'interchange', 'freeway', 'intersection', 'east', 'north', 'terminus', 'lane', 'continues', 'passes', 'avenue', 'state', 'highways']</t>
+          <t>['different', 'called', 'given', 'form', 'example', 'point', 'elements', 'real', 'use', 'possible', 'formula', 'sequence', 'particular', 'result', 'simple']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">New Brunswick Route 95 = Route 95 is a 14.5-kilometre-long ( 9.0 mi ) provincial highway in New Brunswick , which serves a connector route between Interstate 95 ( I-95 ) and U.S. Route 2 ( US 2 ) at the Houlton – Woodstock Border Crossing near Houlton , Maine , United States to Route 2 , which is part of the Trans-Canada Highway , in Woodstock , New Brunswick , Canada . Prior to the construction of Route 95 , the connection between the two cities was served by Route 5 . In 2007 the New Brunswick government completed a roadworks project to turn Route 95 into a full freeway for its entire length . = = Route description = = Route 95 begins at the Houlton – Woodstock Border Crossing on the Maine – New Brunswick border as an extension of I-95 and US 2 . The border between the two countries also marks the border between the Eastern Time Zone and the Atlantic Time Zone . The highway travels northeast through woodlands as it approaches its first interchange with Route 540 via a hybrid diamond </t>
+          <t>Negative resistance = In electronics , negative resistance ( NR ) is a property of some electrical circuits and devices in which an increase in voltage across the device 's terminals results in a decrease in electric current through it . This is in contrast to an ordinary resistor in which an increase of applied voltage causes a proportional increase in current due to Ohm 's law , resulting in a positive resistance . While a positive resistance consumes power from current passing through it , a negative resistance produces power . Under certain conditions it can increase the power of an electrical signal , amplifying it . Negative resistance is an uncommon property which occurs in a few nonlinear electronic components . In a nonlinear device , two types of resistance can be defined : ' static ' or ' absolute resistance ' , the ratio of voltage to current &lt;formula&gt; , and differential resistance , the ratio of a change in voltage to the resulting change in current &lt;formula&gt; . The term ne</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Missouri Route 108 = Route 108 is a short highway in the Bootheel of southeastern Missouri . Its eastern terminus is the Arkansas state line at Arkansas Highway 77 , about six miles ( 10 km ) south of Arbyrd , the only town on the route . Its western terminus is at U.S. Route 412 ( US 412 ) about two miles ( 3 km ) north of Arbyrd . Although signed as an east – west route , the route follows mostly north – south roadways . The route was designated in 1930 , and was extended east in 1972 . = = Route description = = Route 108 begins at the Arkansas state line in Arkmo , Dunklin County , where the road continues south into that state as Highway 77 . From the Arkansas-Missouri state line , the route heads north as a two-lane undivided road , passing a few homes and businesses in Arkmo before running through farmland . The road continues through rural areas to the southern edge of Arbyrd , where it reaches an intersection with Route 164 . At this point , Route 108 turns east to form a concu</t>
+          <t>Pythagorean theorem = In mathematics , the Pythagorean theorem , also known as Pythagoras ' theorem , is a fundamental relation in Euclidean geometry among the three sides of a right triangle . It states that the square of the hypotenuse ( the side opposite the right angle ) is equal to the sum of the squares of the other two sides . The theorem can be written as an equation relating the lengths of the sides a , b and c , often called the " Pythagorean equation " : &lt;formula&gt; where c represents the length of the hypotenuse and a and b the lengths of the triangle 's other two sides . Although it is often argued that knowledge of the theorem predates him , the theorem is named after the ancient Greek mathematician Pythagoras ( c . 570 – c . 495 BC ) as it is he who , by tradition , is credited with its first recorded proof . There is some evidence that Babylonian mathematicians understood the formula , although little of it indicates an application within a mathematical framework . Mesopo</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Ontario Highway 400A = King 's Highway 400A , once known as the Highway 400 Extension , is an unsigned 400-series highway in the Canadian province of Ontario . The short 1.1-kilometre ( 0.7 mi ) freeway stub connects Highway 400 with Highway 11 and Simcoe County Road 93 , formerly Highway 93 . The highway was created in late 1959 by the opening of Highway 400 to Coldwater , although it has always featured Highway 400 signage along the southbound lanes and Highway 11 signage northbound . = = Route description = = Highway 400A is a 1.1-kilometre ( 0.7 mi ) 400-series highway located in the Canadian province of Ontario . The unisigned freeway includes a narrow grass median for the majority of its length , and features a speed limit of 100 kilometres per hour ( 62 mph ) . On average , the highway is used by approximately 11 , 900 vehicles daily . The route begins as Highway 400 exits on the right , with the northbound lanes rising up on an embankment and crossing Highway 400A . After the b</t>
+          <t>Taylor series = In mathematics , a Taylor series is a representation of a function as an infinite sum of terms that are calculated from the values of the function 's derivatives at a single point . The concept of a Taylor series was formulated by the Scottish mathematician James Gregory and formally introduced by the English mathematician Brook Taylor in 1715 . If the Taylor series is centered at zero , then that series is also called a Maclaurin series , named after the Scottish mathematician Colin Maclaurin , who made extensive use of this special case of Taylor series in the 18th century . A function can be approximated by using a finite number of terms of its Taylor series . Taylor 's theorem gives quantitative estimates on the error introduced by the use of such an approximation . The polynomial formed by taking some initial terms of the Taylor series is called a Taylor polynomial . The Taylor series of a function is the limit of that function 's Taylor polynomials as the degree i</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delaware Route 44 = Delaware Route 44 ( DE 44 ) is a state highway in Kent County , Delaware . It runs from DE 300 in Everetts Corner southeast to DE 8 in Pearsons Corner . The route passes through rural areas of western Kent County as well as the town of Hartly . In Hartly , it intersects DE 11 . The route was built as a state highway east of Hartly by 1924 and west of Hartly by 1932 , receiving the DE 44 designation by 1936 . = = Route description = = Delaware Route 44 heads to the southeast of DE 300 on Everetts Corner Road . It passes through a mix of woodland and farmland before reaching the town of Hartly . In Hartly , the route intersects DE 11 , where it becomes Main Street , and passes by homes . It then heads to the east out of Hartly on Hartly Road , passing through more rural areas . The route continues to its eastern terminus at DE 8 near Pearsons Corner . DE 44 has an annual average daily traffic count ranging from a high of 4,478 vehicles at the eastern terminus at DE 8 </t>
+          <t>Book embedding = In graph theory , a book embedding is a generalization of planar embedding of a graph to embeddings into a book , a collection of half-planes all having the same line as their boundary . Usually , the vertices of the graph are required to lie on this boundary line , called the spine , and the edges are required to stay within a single half-plane . The book thickness of a graph is the smallest possible number of half-planes for any book embedding of the graph . Book thickness is also called pagenumber , stacknumber or fixed outerthickness . Book embeddings have also been used to define several other graph invariants including the pagewidth and book crossing number . Every graph with n vertices has book thickness at most &lt;formula&gt; , and this formula gives the exact book thickness for complete graphs . The graphs with book thickness one are the outerplanar graphs . The graphs with book thickness at most two are the subhamiltonian graphs , which are always planar ; more ge</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Ontario Highway 23 = King 's Highway 23 , commonly referred to as Highway 23 , is a provincially maintained highway in the Canadian province of Ontario . The route travels from Highway 7 east of Elginfield north to Highway 9 and Highway 89 in Harriston . The total length of Highway 23 is 97.7 kilometres ( 60.7 miles ) . The highway was first established in 1927 between Highway 8 in Mitchell and Highway 9 in Teviotdale , via Monkton , Listowel and Palmerston . As part of a depression relief program , it was extended south to Highway 7 in 1934 . It remained relatively unchanged until 2003 , when it was rerouted northward from Palmerston to Harriston . = = Route description = = Highway 23 begins at Highway 7 , east of Elginfield , a community straddling the boundary between the municipalities of Middlesex Centre and Lucan Biddulph . The route travels north through the latter , surrounded on both sides by farmland . At Whalen Corners , the highway curves northeast as it exits Middlesex Cou</t>
+          <t>Addition = Addition ( often signified by the plus symbol " + " ) is one of the four basic operations of arithmetic , with the others being subtraction , multiplication and division . The addition of two whole numbers is the total amount of those quantities combined . For example , in the picture on the right , there is a combination of three apples and two apples together , making a total of five apples . This observation is equivalent to the mathematical expression " 3 + 2 = 5 " i.e. , " 3 add 2 is equal to 5 " . Besides counting fruits , addition can also represent combining other physical objects . Using systematic generalizations , addition can also be defined on more abstract quantities , such as integers , rational numbers , real numbers and complex numbers and other abstract objects such as vectors and matrices . In arithmetic , rules for addition involving fractions and negative numbers have been devised amongst others . In algebra , addition is studied more abstractly . Additi</t>
         </is>
       </c>
     </row>
@@ -686,32 +686,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>['game', 'player', 'gameplay', 'games', 'players', 'playstation', 'nintendo', 'released', 'xbox', 'characters', 'graphics', 'soundtrack', 'mode', 'version', 'mario']</t>
+          <t>['war', 'american', 'later', 'wrote', 'years', 'began', 'men', 'time', 'british', 'land', 'united_states', 'known', 'general', 'early', 'received']</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Dr. Mario = Dr. Mario ( Japanese : ドクターマリオ , Hepburn : Dokutā Mario , often stylized as D ℞ . Mario ) is a 1990 Mario arcade-style action puzzle video game designed by Gunpei Yokoi and produced by Takahiro Harada . Nintendo developed and published the game for the Nintendo Entertainment System and Game Boy consoles . The game 's soundtrack was composed by Hirokazu Tanaka . The game focuses on the player character Mario , who assumes the role of a doctor and is tasked with eradicating deadly viruses . In this falling block puzzle game , the player 's objective is to destroy the viruses populating the on-screen playing field by using colored capsules that are dropped into the field . The player manipulates the capsules as they fall so that they are aligned with viruses of matching colors , which removes them from play . The player progresses through the game by eliminating all the viruses on the screen in each level . Dr. Mario received positive reception , appearing on several " Best Ni</t>
+          <t>George Washington = George Washington ( February 22 , 1732 [ O.S. February 11 , 1731 ] – December 14 , 1799 ) was the first President of the United States ( 1789 – 97 ) , the Commander-in-Chief of the Continental Army during the American Revolutionary War , and one of the Founding Fathers of the United States . He presided over the convention that drafted the current United States Constitution and during his lifetime was called the " father of his country " . Widely admired for his strong leadership qualities , Washington was unanimously elected president by the Electoral College in the first two national elections . He oversaw the creation of a strong , well-financed national government that maintained neutrality in the French Revolutionary Wars , suppressed the Whiskey Rebellion , and won acceptance among Americans of all types . Washington 's incumbency established many precedents , still in use today , such as the cabinet system , the inaugural address , and the title Mr. President</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Rhythm game = Rhythm game or rhythm action is a genre of music-themed action video game that challenges a player 's sense of rhythm . Games in the genre typically focus on dance or the simulated performance of musical instruments , and require players to press buttons in a sequence dictated on the screen . Doing so causes the game 's protagonist or avatar to dance or to play their instrument correctly , which increases the player 's score . Many rhythm games include multiplayer modes in which players compete for the highest score or cooperate as a simulated musical ensemble . While conventional control pads may be used as input devices , rhythm games often feature novel game controllers that emulate musical instruments . Certain dance-based games require the player to physically dance on a mat , with pressure-sensitive pads acting as the input device . The 1996 title PaRappa the Rapper has been deemed the first influential rhythm game , whose basic template formed the core of subsequen</t>
+          <t xml:space="preserve">Spanish conquest of the Maya = The Spanish conquest of the Maya was a protracted conflict during the Spanish colonisation of the Americas , in which the Spanish conquistadores and their allies gradually incorporated the territory of the Late Postclassic Maya states and polities into the colonial Viceroyalty of New Spain . The Maya occupied a territory that is now incorporated into the modern countries of Mexico , Guatemala , Belize , Honduras and El Salvador ; the conquest began in the early 16th century and is generally considered to have ended in 1697 . The conquest of the Maya was hindered by their politically fragmented state . Spanish and native tactics and technology differed greatly . The Spanish engaged in a strategy of concentrating native populations in newly founded colonial towns ; they viewed the taking of prisoners as a hindrance to outright victory , whereas the Maya prioritised the capture of live prisoners and of booty . Among the Maya , ambush was a favoured tactic ; </t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Super Mario Bros. : The Lost Levels = Super Mario Bros. : The Lost Levels is a 1986 side-scrolling , platformer action game developed and published by Nintendo as the sequel to the 1985 Super Mario Bros. The games are similar in style and gameplay apart from a large increase in difficulty . Like the original , Mario or Luigi venture to rescue the princess from Bowser . Unlike the original , the game has no two-player option and Luigi is differentiated from his twin plumber brother by having less ground friction and higher jump height . The Lost Levels also introduces setbacks like poison mushroom power-ups , counterproductive level warps , and mid-air wind gusts . The main game has 32 levels across eight worlds , followed by five bonus worlds . The Lost Levels was first released in Japan for the Family Computer Disk System as Super Mario Bros. 2 ( Japanese : スーパーマリオブラザーズ 2 ) on June 3 , 1986 , following the success of its predecessor . It was developed by Nintendo R &amp; D4 , the team led</t>
+          <t>History of the United States Navy = The history of the United States Navy divides into two major periods : the " Old Navy " , a small but respected force of sailing ships that was also notable for innovation in the use of ironclads during the American Civil War , and the " New Navy " , the result of a modernization effort that began in the 1880s and made it the largest in the world by the 1920s . The United States Navy claims 13 October 1775 as the date of its official establishment , when the Second Continental Congress passed a resolution creating the Continental Navy . With the end of the American Revolutionary War , the Continental Navy was disbanded . Under President George Washington threats to American merchant shipping by Barbary pirates from 4 north African Muslim States , in the Mediterranean , led to the Naval Act of 1794 , which created a permanent standing U.S. Navy . The original six frigates were authorized as part of the Act . Over the next 20 years , the Navy fought th</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Super Mario Land = Super Mario Land is a 1989 side-scrolling platform video game , the first in the Super Mario Land series , developed and published by Nintendo as a launch title for their Game Boy handheld game console . In gameplay similar to that of the 1985 Super Mario Bros. , but resized for the smaller device 's screen , the player advances Mario to the end of 12 levels by moving to the right and jumping across platforms to avoid enemies and pitfalls . Unlike other Mario games , Super Mario Land is set in Sarasaland , a new environment depicted in line art , and Mario pursues Princess Daisy . The game introduces two Gradius-style shooter levels . At Nintendo CEO Hiroshi Yamauchi 's request , Game Boy creator Gunpei Yokoi 's Nintendo R &amp; D1 developed a Mario game to sell the new console . It was the first portable version of Mario and the first to be made without Mario creator and Yokoi protégé Shigeru Miyamoto . Accordingly , the development team shrunk Mario gameplay elements f</t>
+          <t>History of slavery in Indiana = Slavery in Indiana occurred between the time of French rule during late seventeenth century and 1826 , with a few traces of slavery afterward . When the United States first forcibly removed the Native Americans from the region , slavery was accepted as a necessity to keep peace with the Indians and the French . When the Indiana Territory was established in 1800 , William Henry Harrison , a former slaveholder , was appointed governor and slavery continued to be tolerated through a series of laws enacted by the appointed legislature . Opposition against slavery began to organize in Indiana around 1805 , and in 1809 abolitionists took control of the territorial legislature and overturned many of the laws permitting retaining of slaves . By the time Indiana was granted statehood in 1816 , the abolitionists were in firm control and slavery was banned in the constitution . In 1820 , an Supreme Court of Indiana ruling in Polly v. Lasselle freed all the remainin</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Music of the Final Fantasy series = Final Fantasy is a media franchise created by Hironobu Sakaguchi and owned by Square Enix that includes video games , motion pictures , and other merchandise . The series began in 1987 as an eponymous role-playing video game developed by Square , spawning a video game series that became the central focus of the franchise . The music of the Final Fantasy series refers to the soundtracks of the Final Fantasy series of video games , as well as the surrounding medley of soundtrack , arranged , and compilation albums . The series ' music ranges from very light background music to emotionally intense interweavings of character and situation leitmotifs . The franchise includes a main series of numbered games as well as several spin-off series such as Crystal Chronicles and the Final Fantasy Tactics series . The primary composer of music for the main series was Nobuo Uematsu , who single-handedly composed the soundtracks for the first nine games , as well as</t>
+          <t>James Longstreet = James Longstreet ( January 8 , 1821 – January 2 , 1904 ) was one of the foremost Confederate generals of the American Civil War and the principal subordinate to General Robert E. Lee , who called him his " Old War Horse . " He served under Lee as a corps commander for many of the famous battles fought by the Army of Northern Virginia in the Eastern Theater , but also with Gen. Braxton Bragg in the Army of Tennessee in the Western Theater . Biographer and historian Jeffry D. Wert wrote that " Longstreet ... was the finest corps commander in the Army of Northern Virginia ; in fact , he was arguably the best corps commander in the conflict on either side . " Longstreet 's talents as a general made significant contributions to the Confederate victories at Second Bull Run ( Second Manassas ) , Fredericksburg , and Chickamauga , in both offensive and defensive roles . He also performed strongly during the Seven Days Battles , the Battle of Antietam , and until he was serio</t>
         </is>
       </c>
     </row>
@@ -721,32 +721,32 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>['film', 'films', 'bond', 'disney', 'movie', 'role', 'actor', 'director', 'cast', 'filming', 'script', 'production', 'starred', 'grossing', 'batman']</t>
+          <t>['game', 'released', 'games', 'player', 'music', 'version', 'original', 'series', 'release', 'story', 'characters', 'players', 'main', 'character', 'japan']</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Paresh Mokashi = Paresh Mokashi ( born 6 February 1969 ) is an Indian filmmaker , producer , actor and Theatre director-producer ; working predominantly in Marathi cinema and Marathi theatre . He started working as a backstage worker for theatre and did few minor roles for plays as well as films . Mokashi made his directorial debut for theatre with the Marathi play , Sangeet Debuchya Mulee in 1999 . He continued to work for theatre and made his directorial debut for cinema with the 2009 Marathi feature film , Harishchandrachi Factory . The film depicts the making of India 's first full-length feature film , Raja Harishchandra ( 1913 ) , made by Dadasaheb Phalke . The film was acclaimed critically and won several awards . It was also selected as India 's official entry to 82nd Academy Awards in the Best Foreign Language Film category . = = Personal life = = Paresh Mokashi was born to a Maharashtrian family in Pune and was brought up in Lonavla . He is a grandson of a noted Marathi write</t>
+          <t>Dragon Quest = Dragon Quest ( Japanese : ドラゴンクエスト , Hepburn : Doragon Kuesuto ) , published as Dragon Warrior in North America until 2005 , is a series of internationally best-selling console role-playing video game ( RPG ) titles created by Yuji Horii and his studio , Armor Project . The series is published by Square Enix ( formerly Enix ) , with localized versions of later installments for the Nintendo DS being published by Nintendo outside Japan . With its first title published in 1986 , there are currently ten main-series titles , along with numerous spin-off games . Nearly every game in the main series has either an anime or manga adaptation , or both . The series has had a significant impact on the development of console RPGs , and introduced a number of features to the genre . Installments of the series have appeared on MSX computers , Nintendo Entertainment System , Super Nintendo Entertainment System , Game Boy Color , Game Boy Advance , Nintendo DS , PlayStation , PlayStation</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Mani Ratnam = Gopala Ratnam Subramaniam ( born 2 June 1955 ) , commonly known by his screen name Mani Ratnam , is an Indian film director , screenwriter , and producer who predominantly works in Tamil cinema . Cited by the media as one of India 's most acclaimed and influential filmmakers , Mani Ratnam is widely credited with revolutionising the Tamil film industry and altering the profile of Indian cinema . Although working in the mainstream medium , his films are noted for their realism , technical finesse , and craft . The Government of India honoured him with the Padma Shri , acknowledging his contributions to film in 2002 . Despite being born into a film family , Mani Ratnam did not develop any interest towards films when he was young . Upon completion of his post graduation in management , he started his career as a consultant . He entered the film industry through the 1983 Kannada film Pallavi Anu Pallavi . The failure of his subsequent films would mean that he was left with lit</t>
+          <t xml:space="preserve">Little Busters ! = Little Busters ! ( リトルバスターズ ! , Ritoru Basutāzu ! ) is a Japanese visual novel developed by Key . It was released on July 27 , 2007 for Windows PCs and is rated for all ages . Little Busters ! is Key 's sixth game , along with other titles such as Kanon , Air , and Clannad . An adult version of the game titled Little Busters ! Ecstasy was released on July 25 , 2008 for Windows , unlike Kanon and Air , which were first released with adult content and then had later versions with such content removed . Ecstasy was later ported to the PlayStation 2 , PlayStation Portable , PlayStation Vita , and PlayStation 3 . The story follows the life of Riki Naoe , a high school student who has been a member of a group of friends named the Little Busters since childhood . Riki brings multiple girls at his school into the Little Busters to have enough people to play a baseball game . The gameplay in Little Busters ! follows a branching plot line which offers pre-determined scenarios </t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Balu Mahendra = Balanathan Benjamin Mahendran ( 20 May 1939 – 13 February 2014 ) , commonly known as Balu Mahendra , was a Sri Lankan cinematographer , director , screenwriter and film editor , who worked in various Indian film industries , primarily in Tamil cinema . Born into a Sri Lankan Tamil household , Mahendra developed a passion towards photography and literature at a young age . He was drawn towards film-making after witnessing the shoot of David Lean 's The Bridge on the River Kwai ( 1957 ) in Sri Lanka . A graduate of the London University , he started his career as a draughtsman before gaining an admission to the Film and Television Institute of India ( FTII ) to pursue a course in cinematography . Mahendra entered films as a cinematographer in the early 1970s and gradually rose to becoming a film-maker by the end of the decade . Making his directorial debut through the Kannada film Kokila ( 1977 ) , Mahendra made over 20 films in all South Indian languages and two in Hindi</t>
+          <t>Key ( company ) = Key is a Japanese visual novel studio which formed on July 21 , 1998 as a brand under the publisher VisualArt 's and is located in Kita , Osaka , Japan . Key released their debut visual novel Kanon in June 1999 , which combined an elaborate storyline , an up-to-date anime-style drawing style , and a musical score which helped to set the mood for the game . Key 's second game Air released in September 2000 had a similar if not more complex storyline to Kanon and a more thorough gameplay . Both Kanon and Air were originally produced as adult games , but Key broke this trend with their third title Clannad which was released in April 2004 for all ages . Key has worked in the past with Interchannel and Prototype for the consumer port releases of the brand 's games . Key collaborated with P.A. Works and Aniplex to produce the anime series Angel Beats ! ( 2010 ) and Charlotte ( 2015 ) . The brand 's ninth game Rewrite was released in June 2011 , and a fan disc for the game t</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Vishal Bhardwaj = Vishal Bhardwaj ( born 4 August 1965 ) is an Indian film director , screenwriter , producer , music composer and playback singer . He is known for his work in Hindi cinema , and is the recipient of a Filmfare Award and seven National Film Awards in four categories . Bhardwaj made his debut as a music composer with the children 's film Abhay ( The Fearless ) ( 1995 ) , and received wider recognition with his compositions in Gulzar 's Maachis ( 1996 ) . He received the Filmfare RD Burman Award for New Music Talent for the latter . He went on to compose music for the films Satya ( 1998 ) and Godmother ( 1999 ) . For the latter , he garnered the National Film Award for Best Music Direction . Bhardwaj made his directorial debut with the children 's film Makdee ( 2002 ) , for which he also composed the music . He garnered critical acclaim and several accolades for writing and directing the Indian adaptations of three tragedies by William Shakespeare : Maqbool ( 2003 ) from </t>
+          <t>Localization of Square Enix video games = The Japanese video game developer and publisher Square Enix ( formally two companies called Square and Enix prior to 2003 ) has been translating its games for North America and the PAL region since the late 1980s . It has not always released all of its games in all major regions , and continues to selectively release games even today depending on multiple factors such as the viability of platforms or the condition of the game itself . The process of localization has changed during that time from having a one-person team with a short time and tight memory capacities to having a team of translators preparing simultaneous launches in multiple languages . The companies ' first major projects were Dragon Quest and Final Fantasy , which each proved successful enough to launch video game franchises . Since then , the majority of the games produced by the companies have been localized for western audiences , although the process was not given a high pr</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Amanda Seyfried = Amanda Michelle Seyfried ( / ˈsaɪfrɛd / SY-fred ; born December 3 , 1985 ) is an American actress , model , and singer . She began her career as a model when she was 11 , then her acting career at 15 began an acting career with recurring parts on the soap operas As the World Turns and All My Children . In 2004 , Seyfried made her film debut in the teen comedy Mean Girls . Her subsequent supporting roles were in independent films , such as the drama Nine Lives ( 2005 ) and the crime drama Alpha Dog ( 2006 ) , she also had a recurring role in the UPN drama show Veronica Mars ( 2004 – 06 ) . Between 2006 and 2011 , she starred on the HBO drama series Big Love and appeared in the 2008 musical feature film Mamma Mia ! . Her other appearances include leading roles in the black comedy horror film Jennifer 's Body ( 2009 ) , as a call girl in the erotic thriller Chloe ( 2009 ) , the romantic drama-war film Dear John ( 2010 ) , and the romantic drama Letters to Juliet ( 2010 )</t>
+          <t>Insomniac Games = Insomniac Games , Inc. is an American video game developer whose corporate headquarters is located in Burbank , California . It was founded in 1994 by Ted Price as " Xtreme Software " , and was renamed " Insomniac Games " a year later . It has released titles for the PlayStation , PlayStation 2 , PlayStation 3 , Xbox 360 , PlayStation 4 and Xbox One video game consoles . The company 's first project was Disruptor , for the first PlayStation console , whose poor sales almost led to the company 's bankruptcy . Insomniac 's next project was Spyro the Dragon , a successful video game that spawned two sequels within two years . Insomniac then developed a new franchise , Ratchet &amp; Clank , for the PlayStation 2 . The company also developed the Resistance series for the PlayStation 3 , and released its first multi-platform game , Fuse in 2013 . The company also worked with Microsoft Studios on 2014 's Sunset Overdrive . The company 's current projects include an underwater Me</t>
         </is>
       </c>
     </row>
@@ -756,32 +756,32 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>['army', 'persian', 'byzantine', 'arab', 'syria', 'emperor', 'polish', 'muslim', 'byzantines', 'constantine', 'battle', 'hungary', 'ottoman', 'king', 'forces']</t>
+          <t>['tropical', 'storm', 'cyclone', 'area', 'cyclones', 'near', 'level', 'wind', 'low', 'formed', 'depression', 'miles', 'winds', 'water', 'west']</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Siege of Klis = The Siege of Klis or Battle of Klis ( Croatian : Opsada Klisa or Bitka kod Klisa , Turkish : Klise Kuşatması ) was a siege of Klis Fortress in the Kingdom of Croatia within Habsburg Monarchy . The siege of the fortress , which lasted for more than two decades , and the final battle near Klis in 1537 , were fought as a part of the Ottoman – Habsburg wars between the defending Croatian-Habsburg forces under the leadership of Croatian feudal lord Petar Kružić , and the attacking Ottoman army under the leadership of the Ottoman general Murat-beg Tardić . After decisive Ottoman victory at the Battle of Krbava field in 1493 , and especially after the Battle of Mohács in 1526 , the Croats continued defending themselves against the Ottoman attacks . The Ottoman conquest during the early years of the 16th century prompted the formation of the Uskoks , which were led by Croatian captain Petar Kružić , also called ( Prince of Klis ) . As a part of the Habsburg defensive system , U</t>
+          <t>1982 Pacific typhoon season = The 1982 Pacific typhoon season had no official bounds ; it ran year-round in 1982 . On average , most tropical cyclones tend to form in the northwestern Pacific Ocean between May and November . These dates conventionally delimit the period of each year when most tropical cyclones form in the northwestern Pacific Ocean . The scope of this article is limited to the Pacific Ocean , north of the equator and west of the International Date Line . Storms that form east of the date line and north of the equator are called hurricanes . Tropical Storms that formed in the entire west Pacific basin were assigned a name by the Joint Typhoon Warning Center . Tropical depressions that enter or form in the Philippine area of responsibility are assigned a name by the Philippine Atmospheric , Geophysical and Astronomical Services Administration or PAGASA . This can often result in the same storm having two names . During this season , the first tropical cyclone formed on M</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Cutzinas = Cutzinas or Koutzinas ( Greek : Κουτζίνας ) was a Berber tribal leader who played a major role in the wars of the East Roman or Byzantine Empire against the Berber tribes in Africa in the middle of the 6th century , fighting both against and for the Byzantines . A staunch Byzantine ally during the latter stages of the Berber rebellion , he remained an imperial vassal until his murder in 563 by the new Byzantine governor . = = Life = = Cutzinas was of mixed stock : his father was a Berber , while his mother came from the Romanized population of North Africa . Following the reconquest of North Africa by the East Roman ( Byzantine ) Empire in the Vandalic War ( 533 – 534 ) , several uprisings by the native Berber tribes occurred in the North African provinces . Cutzinas is mentioned by the eyewitness historian Procopius of Caesarea as one of the leaders of the rebellion in the province of Byzacena , alongside Esdilasas , Medisinissas and Iourphouthes . In spring 535 , however ,</t>
+          <t>1986 Pacific typhoon season = The 1986 Pacific typhoon season has no official bounds ; it ran year-round in 1986 , but most tropical cyclones tend to form in the northwestern Pacific Ocean between May and December . These dates conventionally delimit the period of each year when most tropical cyclones form in the northwestern Pacific Ocean . Tropical Storms formed in the entire west pacific basin were assigned a name by the Joint Typhoon Warning Center . Tropical depressions that enter or form in the Philippine area of responsibility are assigned a name by the Philippine Atmospheric , Geophysical and Astronomical Services Administration or PAGASA . This can often result in the same storm having two names . A total of 32 tropical depressions formed in 1986 in the Western Pacific over an eleven-month time span . Of the 32 , 30 became tropical storms , 19 storms reached typhoon intensity , and 3 reached super typhoon strength . The Joint Typhoon Warning Center considered Vera as two tropi</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Siege of Güns = The Siege of Güns or Siege of Kőszeg ( Turkish : Güns Kuşatması ) was a siege of Kőszeg ( German : Güns ) in the Kingdom of Hungary within the Habsburg Empire , that took place in 1532 . In the siege , the defending forces of the Austrian Habsburg Monarchy under the leadership of Croatian Captain Nikola Jurišić ( Hungarian : Miklós Jurisics ) , defended the small border fort of Kőszeg with only 700 – 800 Croatian soldiers , with no cannons and few guns . The defenders prevented the advance of the Ottoman army of 120,000 – 200,000 toward Vienna , under the leadership of Sultan Suleiman the Magnificent ( Ottoman Turkish : سليمان Süleymān ) and Pargalı Ibrahim Pasha . The exact outcome is unknown , since it has two versions which differ depending on the source . In the first version Nikola Jurišić rejected the offer to surrender on favourable terms , and in the second version , the city was offered terms for a nominal surrender . Suleiman , having been delayed nearly four </t>
+          <t xml:space="preserve">1939 Pacific typhoon season = The 1939 Pacific typhoon season has no official bounds ; it ran year-round in 1939 , but most tropical cyclones tend to form in the northwestern Pacific Ocean between May and November . These dates conventionally delimit the period of each year when most tropical cyclones form in the northwestern Pacific Ocean . The scope of this article is limited to the Pacific Ocean , north of the equator and west of the international date line . Storms that form east of the date line and north of the equator are called hurricanes ; see 1939 Pacific hurricane season . Storms in the season were tracked by the United States Weather Bureau and released in the Monthly Weather Review under the header " Typhoons and Depressions over the Far East " . The Monthly Weather Review only covers tropical cyclones west of 150 ° E. Due to lack of satellites and ship reports due to the Pacific Theatre of World War II , it is possible other tropical cyclones existed , especially if they </t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Siege of Tyana = A Siege of Tyana was carried out by the Umayyad Caliphate in 707 – 708 / 708 – 709 in retaliation for a heavy defeat of an Umayyad army under Maimun the Mardaite by the Byzantine Empire in c . 706 . The Arab army invaded Byzantine territory and laid siege to the city in summer 707 or 708 . In fact virtually each of the extant Greek , Arabic and Syriac parallel sources has in this respect a different date . Tyana initially withstood the siege with success , and the Arab army faced great hardship during the ensuing winter . Emperor Justinian II sent a relief army in the next spring , but the Umayyads defeated them , whereupon the inhabitants of the city were forced to surrender . Despite the agreement of terms , the city was plundered and largely destroyed , and according to Byzantine sources its people were made captive and deported , leaving the city deserted . = = Background = = In 692 / 693 , the Byzantine emperor Justinian II ( reigned 685 – 695 and 705 – 711 ) and </t>
+          <t>1981 – 82 South-West Indian Ocean cyclone season = The 1981 – 82 South-West Indian Ocean cyclone season was destructive and deadly in Madagascar , where four cyclones killed 100 people and caused $ 250 million ( USD ) in damage . The season was fairly active , lasting from October to May . There were nine named storms that attained gale-force winds , or at least 65 km / h ( 40 mph ) . Five of the storms attained tropical cyclone status , which have 10 minute sustained winds of at least 120 km / h ( 75 mph ) . The first storm was Tropical Cyclone Alex , which was named by the Australian Bureau of Meteorology ( BoM ) . this was due to the boundary of the basin at the time , which incorporated the Indian Ocean south of the equator and extended from the east coast of Africa to 80 ° E ; the eastern extent was later moved to 90 ° E. Two other storms – Armelle and Damia – also originated in the Australian basin . The latter was the strongest cyclone on record in the basin at the time by barom</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Michael Shishman of Bulgaria = Michael Asen III ( Bulgarian : Михаил Асен III , Mihail Asen III , commonly called Michael Shishman ( Михаил Шишман , Mihail Šišman ) ) , ruled as emperor ( tsar ) of Bulgaria from 1323 to 1330 . The exact year of his birth is unknown but it was between 1280 and 1292 . He was the founder of the last ruling dynasty of the Second Bulgarian Empire , the Shishman dynasty . After he was crowned , however , Michael used the name Asen to emphasize his connection with the Asen dynasty , the first one to rule over the Second Empire . An energetic and ambitious ruler , Michael Shishman led an aggressive but opportunistic and inconsistent foreign policy against the Byzantine Empire and the Kingdom of Serbia , which ended in the disastrous battle of Velbazhd which claimed his own life . He was the last medieval Bulgarian ruler who aimed at military and political hegemony of the Bulgarian Empire over the Balkans and the last one who attempted to seize Constantinople .</t>
+          <t>Nescopeck Creek = Nescopeck Creek is a 37.5-mile-long ( 60.4 km ) tributary of the Susquehanna River in Luzerne County , Pennsylvania , in the United States . The creek is in the Coal Region of Pennsylvania . The meaning of the creek 's name is " deep black waters " . The waters of Nescopeck Creek have difficulty ratings between Class I and Class III . However , during parts of the year , Nescopeck Creek is impossible to navigate due to rapids , flooding , and tight bends . Nescopeck Creek is home to a number of species of trout , although the waters are not always optimal for them . Nescopeck Creek 's water is acidic , with a pH as low as 3.6 in some studies . Much of the land in the Nescopeck Creek 's watershed is forest . Farmland is common in the lower portions of the Nescopeck Creek watershed and the Little Nescopeck Creek watershed , while coal mines are more common on Nescopeck Creek 's tributaries Black Creek , Stony Creek , and Cranberry Creek . A 6-mile ( 10 km ) portion of N</t>
         </is>
       </c>
     </row>
@@ -791,32 +791,32 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>['trains', 'station', 'railway', 'building', 'line', 'tunnel', 'bridge', 'rail', 'services', 'train', 'oslo', 'passenger', 'stations', 'river', 'built']</t>
+          <t>['court', 'act', 'public', 'law', 'state', 'rights', 'case', 'government', 'right', 'cases', 'united_states', 'courts', 'decision', 'singapore', 'person']</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Upminster Bridge tube station = Upminster Bridge is a London Underground station on Upminster Road in the Upminster Bridge neighbourhood of the London Borough of Havering in northeast London , England . The station is on the District line and is the penultimate station on the eastern extremity of that line . The station was opened on 17 December 1934 by the London , Midland and Scottish Railway on the local electrified tracks between Upminster and Barking that were constructed in 1932 . The main station building is of a distinctive polygonal design . It has relatively low usage for a suburban station with approximately 1 million entries and exits during 2011 . = = History = = The London , Tilbury and Southend Railway from Fenchurch Street and Barking was constructed through the Upminster Bridge area in 1885 , with stations at Hornchurch and Upminster . The Whitechapel and Bow Railway opened in 1902 and allowed through services of the District Railway to operate to Upminster . The Metro</t>
+          <t>Rule of law doctrine in Singapore = In Singapore , the rule of law doctrine has been the topic of considerable disagreement and debate , largely through differing conceptions of the doctrine . These conceptions can generally be divided into two categories developed by legal academics , the " thin " , or formal , conception and the " thick " , or substantive , conception of the rule of law . The thin conception , often associated with the legal scholars Albert Venn Dicey and Joseph Raz , advocates the view that the rule of law is fulfilled by adhering to formal procedures and requirements , such as the stipulations that all laws be prospective , clear , stable and constitutionally enacted , and that the parties to legal disputes are treated equally and without bias on the part of judges . While people subscribing to the thin conception do not dismiss the importance of the content of the law , they take the view that this is a matter of substantive justice and should not be regarded as p</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Winschoten railway station = Winschoten ( Dutch pronunciation : [ ˈʋɪnsxoːtən ] ; abbreviation : Ws ) is an unstaffed railway station in Winschoten in the Netherlands . It is located on the Harlingen – Nieuweschans railway between Scheemda and Bad Nieuweschans in the province of Groningen . The station building , designed by Karel Hendrik van Brederode , was completed in 1865 and expanded in 1904 . Train services started on 1 May 1868 and have since been provided by Maatschappij tot Exploitatie van Staatsspoorwegen ( 1868 – 1937 ) , Nederlandse Spoorwegen ( 1938 – 2000 ) , NoordNed ( 2000 – 2005 ) , and Arriva ( 2005 – present ) . During World War II , 500 Jews were transported from the station via the Westerbork transit camp to Nazi concentration camps , where most of them were killed . The station has three tracks and two platforms . As of 2016 there are two local train services with trains every half an hour to and from Groningen , and trains every hour to and from Bad Nieuweschans </t>
+          <t>Article 15 of the Constitution of Singapore = Article 15 of the Constitution of the Republic of Singapore guarantees freedom of religion in Singapore . Specifically , Article 15 ( 1 ) states : " Every person has the right to profess and practise his religion and to propagate it . " The terms profess , practise and propagate are not defined in the Constitution , but cases from Singapore and other jurisdictions may shed light on their meaning . The word profess in relation to a religion was defined in a 1964 Singapore case not involving the Constitution as meaning " to affirm , or declare one 's faith in or allegiance to " . A 2001 Malaysian decision suggested that the profession of religion does not encompass the renunciation of a religion or the profession of an irreligious viewpoint . As regards the word propagate , in 1977 the Supreme Court of India held that it confers on an individual the right to transmit or spread his or her religion by an exposition of its tenets , but not the r</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Trondheim Airport Station = Trondheim Airport Station ( IATA code : TRD ) , also known as Værnes Station ( Norwegian : Værnes holdeplass ) , is a railway station located within the terminal complex of Trondheim Airport , Værnes in Stjørdal , Norway . Situated on the Nordland Line , it serves both express trains and the Trøndelag Commuter Rail both operated by Norges Statsbaner . The station was opened on 15 November 1994 along with a new terminal at the airport , making it the first airport rail link in the Nordic Countries . The station cost NOK 24 million , and was built along the existing railway line . In each direction , the station handles one to two hourly commuter rail services , and three daily express services . Travel time to Trondheim is 38 minutes , while it is 9 hours and 5 minutes to Bodø . Access to the airport terminal is outdoors , but sheltered . = = Facilities = = The station is located at the terminal of Trondheim Airport , Værnes . The connection between the stati</t>
+          <t>Legitimate expectation in Singapore law = The doctrine of legitimate expectation in Singapore protects both procedural and substantive rights . In administrative law , a legitimate expectation generally arises when there has been a representation of a certain outcome by the public authorities to an individual . To derogate from the representation may amount to an abuse of power or unfairness . The doctrine of legitimate expectation as a ground to quash decisions of public authorities has been firmly established by the English courts . Thus , where a public authority has made a representation to an individual who would be affected by a decision by the authority , the individual has a legitimate expectation to have his or her views heard before the decision is taken . Alternatively , an individual may also have a legitimate expectation to a substantive right . The recognition of substantive legitimate expectations is somewhat controversial as it requires a balancing of the requirements o</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>East Finchley tube station = East Finchley is a London Underground station in East Finchley in the London Borough of Barnet , north London . The station is on the High Barnet branch of the Northern line , between Highgate and Finchley Central stations and is in Travelcard Zone 3 . The station was opened in 1867 as part of the Great Northern Railway 's line between Finsbury Park and Edgware stations . As part of London Underground 's only partially completed Northern Heights plan , the station was completely rebuilt with additional tracks in the late 1930s . Northern line trains started serving the station in 1939 and main line passenger services ended in 1941 . = = History = = = = = Original station = = = East Finchley station was built by the Edgware , Highgate and London Railway ( EH &amp; LR ) on its line from Finsbury Park station to Edgware station . Before the line was opened it was purchased in July 1867 by the larger Great Northern Railway ( GNR ) , whose main line from King 's Cro</t>
+          <t>Section 3 of the Human Rights Act 1998 = Section 3 of the Human Rights Act 1998 is a provision of the Human Rights Act 1998 that enables the Act to take effect in the United Kingdom . The section requires courts to interpret both primary and subordinate legislation so that their provisions are compatible with the articles of the European Convention of Human Rights , which are also part of the Human Rights Act 1998 . This interpretation goes far beyond normal statutory interpretation , and includes past and future legislation , therefore preventing the Human Rights act from being impliedly repealed by subsequent contradictory legislation . Courts have applied section 3 of the Act through three forms of interpretation : " reading in " – inserting words where there are none in a statute ; " reading out " where words are omitted from a statute ; and " reading down " where a particular meaning is chosen to be in compliance . They do not interpret statutes to conflict with legislative intent</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Oslo Tunnel = The Oslo Tunnel ( Norwegian : Oslotunnelen ) is a 3,632-meter ( 11,916 ft ) , double-track , railway tunnel which runs between Olav Kyrres plass and Oslo Central Station ( Oslo S ) in Oslo , Norway . The tunnel constitutes the eastern-most section of the Drammen Line and runs below the central business district of Oslo . It features the four-track Nationaltheatret Station , Norway 's second-busiest railway station , where the Oslo Tunnels lies directly beneath the Common Tunnel of the Oslo Metro . At Frogner , the Elisenberg Station was built , but has never been used . The tunnel is the busiest section of railway line in Norway and serves all west-bound trains from Oslo , including many services of the Oslo Commuter Rail and the Airport Express Train . Traditionally , Oslo had two stations , the larger Oslo East Station ( or Oslo Ø , located at the spot of the current Oslo S ) and Oslo West Station ( Oslo V ) , which served the Drammen Line . This caused a physical barri</t>
+          <t>Fourth Amendment to the United States Constitution = The Fourth Amendment ( Amendment IV ) to the United States Constitution prohibits unreasonable searches and seizures and requires any warrant to be judicially sanctioned and supported by probable cause . It is part of the Bill of Rights and was adopted in response to the abuse of the writ of assistance , a type of general search warrant issued by the British government and a major source of tension in pre-Revolutionary America . The Fourth Amendment was introduced in Congress in 1789 by James Madison , along with the other amendments in the Bill of Rights , in response to Anti-Federalist objections to the new Constitution . Congress submitted the amendment to the states on September 28 , 1789 . By December 15 , 1791 , the necessary three-quarters of the states had ratified it . On March 1 , 1792 , Secretary of State Thomas Jefferson announced the adoption of the amendment . Because the Bill of Rights did not initially apply to the st</t>
         </is>
       </c>
     </row>
@@ -826,32 +826,32 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>['battalion', 'brigade', 'aircraft', 'division', 'regiment', 'squadron', 'wing', 'infantry', 'training', 'battalions', 'unit', 'units', 'flight', 'air', 'australian']</t>
+          <t>['bridge', 'miles', 'area', 'road', 'construction', 'river', 'route', 'line', 'traffic', 'dam', 'water', 'station', 'feet', 'tunnel', 'built']</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>No. 77 Wing RAAF = No. 77 Wing was a Royal Australian Air Force ( RAAF ) wing of World War II . It formed part of No. 10 Operational Group ( later the Australian First Tactical Air Force ) at its establishment in November 1943 , when it comprised three squadrons equipped with Vultee Vengeance dive bombers . No. 77 Wing commenced operations in early 1944 , flying out of Nadzab , Papua New Guinea . Soon afterwards , however , the Vengeance units were withdrawn from combat and replaced with squadrons flying Douglas Bostons , Bristol Beaufighters and Bristol Beauforts . The wing saw action in the assaults on Noemfoor , Tarakan , and North Borneo , by which time it was an all-Beaufighter formation made up of Nos. 22 , 30 and 31 Squadrons . It was to have taken part in the Battle of Balikpapan in June 1945 , but unsuitable landing grounds meant that the Beaufighter units were withdrawn to Morotai , sitting out the remainder of the war before returning to Australia , where they disbanded , al</t>
+          <t>Big Wapwallopen Creek = Big Wapwallopen Creek ( also known as Wapwallopen Creek or Big Wap ) is a tributary of the Susquehanna River in Luzerne County , Pennsylvania , in the United States . It is approximately 23 miles ( 37 km ) long and flows through Bear Creek Township , Fairview Township , Rice Township , Wright Township , Dorrance Township , Hollenback Township , Nescopeck Township , and Conyngham Township . The watershed of the creek has an area of 53.2 square miles ( 138 km2 ) . The creek has three named tributaries : Balliet Run , Watering Run , and Bow Creek . The creek is designated as a Coldwater Fishery and a Migratory Fishery and is also Class A Wild Trout Waters for part of its length . However , it is considered to be impaired by organic enrichment and / or low levels of dissolved oxygen and its pH ranges from moderately acidic to slightly alkaline . Big Wapwallopen Creek has three large waterfalls , all of which are more than 25 feet ( 7.6 m ) high . The creek flows thr</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>10th Combat Aviation Brigade ( United States ) = The Combat Aviation Brigade , 10th Mountain Division is a combat aviation brigade of the United States Army based at Fort Drum , New York . It is a subordinate unit of the 10th Mountain Division . Reactivated in 1988 , the 10th Mountain Division 's Combat Aviation Brigade supported the division as it undertook numerous operations and overseas contingencies in the 1990s , including Operation Restore Hope , Operation Uphold Democracy , and Task Force Eagle , as well as disaster relief following Hurricane Andrew . The brigade has since become involved in the War on Terrorism , seeing four deployments to Afghanistan to support Operation Enduring Freedom and a deployment to Iraq to support Operation Iraqi Freedom . The brigade is currently on its fourth deployment to Afghanistan and is serving in Regional Command - East under Combined Joint Task Force 101 in support of Operation Enduring Freedom . = = Organization = = The Combat Aviation Brig</t>
+          <t>River Torrens = The River Torrens / ˈtɒrənz / is the most significant river of the Adelaide Plains and was one of the reasons for the siting of the city of Adelaide , capital of South Australia . It flows 85 kilometres ( 53 mi ) from its source in the Adelaide Hills near Mount Pleasant , across the Adelaide Plains , past the city centre and empties into Gulf St Vincent between Henley Beach South and West Beach . The upper stretches of the river and the reservoirs in its watershed supply a significant part of the city 's water supply . The river 's long linear parks and a constructed lake in the lower stretch are iconic of the city . At its 1836 discovery an inland bend was chosen as the site of the Adelaide city centre and North Adelaide . The river is named after Colonel Robert Torrens , chairman of the colonial commissioners and a significant figure in the city 's founding . The river is also known by its native Kaurna name Karra wirra-parri . The river and its tributaries are highly</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>166th Aviation Brigade ( United States ) = The 166th Aviation Brigade was an aviation training brigade of the United States Army headquartered at Fort Hood , Texas . It was a subordinate unit of First Army - Division West . An " AC / RC " ( Active Component / Reserve Component ) formation , the 166th Aviation Brigade was the sole organization responsible for the post-mobilization training of United States Army Reserve &amp; National Guard aviation units . The unit was formerly designated as 3rd Brigade , 75th Division . From 1997 , the 166th Aviation Brigade has trained other aviation units for front-line service . As such , it has never seen combat , and has thus never earned any campaign streamers or unit awards . As the only brigade in the First Army responsible for training aviation units , the 166th Aviation Brigade is the principal unit for training Army Reserve and Army National Guard assets preparing to deploy to contingencies around the world , which means it is responsible for 47</t>
+          <t>Solomon Creek = Solomon Creek is a tributary of the Susquehanna River in Luzerne County , Pennsylvania , in the United States . It is approximately 8.8 miles ( 14.2 km ) long and flows through Fairview Township , Hanover Township , and Wilkes-Barre . The creek is affected by acid mine drainage and has significant loads of iron , aluminum , and manganese . The creek 's named tributaries are Spring Run , Sugar Notch Run , and Pine Creek . The Solomon Creek watershed is located in the Anthracite Valley section of the ridge-and-valley geographical province . Major rock formations in the watershed include the Mauch Chunk Formation , the Spechty Kopf Formation , and the Catskill Formation . Solomon Creek was first settled by Native Americans around 8000 to 6000 B.C.E. A settler arrived at the confluence of the creek with the Susquehanna River by 1774 . In the 1800s , more people began arriving in the watershed to exploit its natural resources . Anthracite mining was especially prevalent in t</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>18th Military Police Brigade ( United States ) = The 18th Military Police Brigade is a military police brigade of the United States Army based in Grafenwoehr , Germany , with subordinate battalions and companies stationed throughout Germany . It provides law enforcement and force protection duties to United States Army Europe . Activated during the Vietnam War , the Brigade oversaw all Military Police operations in the country for a large portion of the conflict , undertaking a wide variety of missions throughout the country and providing command and control for other military police groups in the region . After Vietnam , the Brigade deployed units to several other operations , namely Operation Desert Storm and Operation Provide Comfort . The brigade itself also deployed to Kosovo , supporting many of the units operating there attempting to settle unrest in the area due to the 1999 Bosnian War . The brigade has also seen multiple deployments in the Global War on Terrorism to the Iraq W</t>
+          <t xml:space="preserve">Rail transport in Victoria = Rail transport in Victoria , Australia , is provided by a number of railway operators who operate over the government-owned railway lines . Victorian lines use 5 ft 3 in ( 1,600 mm ) broad gauge , with the exception of a number of standard gauge 4 ft 8 1 ⁄ 2 in ( 1,435 mm ) freight and interstate lines , a few experimental 2 ft 6 in ( 762 mm ) narrow gauge lines , and various private logging , mining and industrial railways . Railways were privately owned and operated , until the State Government established the vertically integrated Victorian Railways in 1883 . This remained until corporatisation occurred in the 1980s , followed by privatisation in the 1990s . Passenger services today are operated by Metro Trains Melbourne in suburban Melbourne with electric multiple units , and V / Line in regional Victoria with diesel trains . Freight services are operated by Aurizon ( interstate ) , Pacific National and SCT Logistics ( interstate and intrastate ) , and </t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Special Troops Battalion , 173rd Airborne Brigade Combat Team ( United States ) = The Special Troops Battalion , 173rd Airborne Brigade Combat Team is a special troops battalion of the United States Army headquartered at Caserma Del Din in Vicenza , Italy . It is the organization for the command elements of the 173rd Airborne Brigade Combat Team . The battalion contains the brigade 's senior command structure , including its Headquarters and Headquarters Company , as well as communication and support elements . Activated in 2000 from inactivating support units , the Special Troops Battalion deployed with the 173rd Airborne Brigade Combat Team to Afghanistan in 2007 until 2008 and again in early 2010 . = = Organization = = The Special Troops Battalion is subordinate to the 173rd Airborne Brigade Combat Team and is a permanent formation of the brigade , as the 173rd 's command elements are all contained in the STB . The battalion consists of three companies and the brigade 's Headquarter</t>
+          <t>Mitchell Freeway = Mitchell Freeway is a 30-kilometre-long ( 19 mi ) freeway in the northern suburbs of Perth , Western Australia , linking central Perth with the satellite city of Joondalup . It is the northern section of State Route 2 , which continues south as Kwinana Freeway and Forrest Highway . Along its length are interchanges with several major roads , including Graham Farmer Freeway and Reid Highway . The southern terminus of the Mitchell Freeway is at the Narrows Bridge , which crosses the Swan River , and the northern terminus is at Burns Beach Road , which is the northern border of the suburb of Joondalup . Planning for the route began in the 1950s , and the first segment in central Perth was constructed between 1967 and 1973 . The Mitchell Freeway has been progressively extended north since then . In the 1970s , the first two extensions were completed , up to Hutton Street in Osborne Park . By the end of the 1980s , the freeway had reached Ocean Reef Road in Edgewater . Th</t>
         </is>
       </c>
     </row>
@@ -861,32 +861,32 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>['election', 'governor', 'bush', 'republican', 'senate', 'president', 'democratic', 'massachusetts', 'campaign', 'presidential', 'elected', 'kentucky', 'lincoln', 'senator', 'vote']</t>
+          <t>['century', 'known', 'breed', 'horses', 'horse', 'found', 'popular', 'island', 'today', 'breeds', 'including', 'period', 'dog', 'large', 'early']</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>James Fisher Robinson = James Fisher Robinson ( October 4 , 1800 – October 31 , 1882 ) was the 22nd Governor of Kentucky , serving the remainder of the unfinished term of Governor Beriah Magoffin . Magoffin , a Confederate sympathizer , became increasingly ineffective after the elections of 1861 yielded a supermajority to pro-Union forces in both houses of the Kentucky General Assembly . Magoffin agreed to resign the governorship , provided he could select his successor . He selected Robinson . Politically , Robinson opposed both secession and abolition . Though he had Union sympathies , he was considered a moderate , opposing both fugitive slave laws and the enlistment of black soldiers . As a state senator , he supported the Crittenden Compromise and opposed the Civil War . As governor , he drew criticism from the administration of President Abraham Lincoln for opposing the Emancipation Proclamation . = = Early life = = Robinson was born to Jonathan and Jane Black Robinson in Scott C</t>
+          <t>Fried chicken = Fried chicken ( also referred to as Southern fried chicken for the variant in the United States ) is a dish consisting of chicken pieces usually from broiler chickens which have been floured or battered and then pan-fried , deep fried , or pressure fried . The breading adds a crisp coating or crust to the exterior . What separates fried chicken from other fried forms of chicken is that generally the chicken is cut at the joints , and the bones and skin are left intact . Crisp well-seasoned skin , rendered of excess fat , is a hallmark of well made fried chicken . The first dish known to have been deep fried was fritters , which were popular in the Middle Ages . However , it was the Scottish who were the first to deep fry their chicken . The dish was first brought to the United States by Scottish immigrants . Prior to the Second World War , fried chicken was often very expensive and was only enjoyed on special occasions . In the late 1900s and early 2000s , however , fri</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Christopher Greenup = Christopher Greenup ( c . 1750 – April 27 , 1818 ) was an American politician who served as a U.S. Representative and the third Governor of Kentucky . Little is known about his early life ; the first reliable records about him are documents recording his service in the Revolutionary War where he served as a lieutenant in the Continental Army and a colonel in the Virginia militia . After his service in the war , Greenup helped settle the trans-Appalachian regions of Virginia . He became involved in politics , and played an active role in three of the ten statehood conventions that secured the separation of Kentucky from Virginia in 1792 . He became one of the state 's first representatives , and served in the Kentucky General Assembly before being elected governor in a race where , due to his immense popularity , he ran unopposed . Greenup 's term in office was marred by accusations that he had participated in the Burr Conspiracy to align Kentucky with Spain prior </t>
+          <t>History of the horse in Britain = The known history of the horse in Britain starts with horse remains found in Pakefield , Suffolk , dating from 700,000 BC , and in Boxgrove , West Sussex , dating from 500,000 BC . Early humans were active hunters of horses , and finds from the Ice Age have been recovered from many sites . At that time , land which now forms the British Isles was part of a peninsula attached to continental Europe by a low-lying area now known as " Doggerland , " and land animals could migrate freely between what is now island Britain and continental Europe . The domestication of horses , and their use to pull vehicles , had begun in Britain by 2500 BC ; by the time of the Roman conquest of Britain , British tribes could assemble armies which included thousands of chariots . Horse improvement as a goal , and horse breeding as an enterprise , date to medieval times ; King John imported a hundred Flemish stallions , Edward III imported fifty Spanish stallions , and variou</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>John Breathitt = John Breathitt ( September 9 , 1786 – February 21 , 1834 ) was the 11th Governor of Kentucky . He was the first Democrat to hold this office and was the second Kentucky governor to die in office . Shortly after his death , Breathitt County , Kentucky was created and named in his honor . Early in life , Breathitt was appointed a deputy surveyor in Illinois Territory . On his return to Kentucky , he taught at a country school , and through wise investments , amassed enough wealth to sustain him while he studied law with Judge Caleb Wallace . In 1811 , he was elected to the first of several terms in the Kentucky House of Representatives . He was the Democratic nominee for lieutenant governor in 1828 . Although his running mate William T. Barry lost the office of governor to Thomas Metcalfe , Breathitt defeated his opponent for lieutenant governor . During his term as lieutenant governor , Breathitt was one of several proposed candidates to succeed John Rowan in the United</t>
+          <t xml:space="preserve">Beer = Beer is the world 's most widely consumed and probably the oldest alcoholic beverage ; it is the third most popular drink overall , after water and tea . The production of beer is called brewing , which involves the fermentation of starches , mainly derived from cereal grains — most commonly malted barley , although wheat , maize ( corn ) , and rice are widely used . Most beer is flavoured with hops , which add bitterness and act as a natural preservative , though other flavourings such as herbs or fruit may occasionally be included . The fermentation process causes a natural carbonation effect , although this is often removed during processing , and replaced with forced carbonation . Some of humanity 's earliest known writings refer to the production and distribution of beer : the Code of Hammurabi included laws regulating beer and beer parlours , and " The Hymn to Ninkasi " , a prayer to the Mesopotamian goddess of beer , served as both a prayer and as a method of remembering </t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lazarus W. Powell = Lazarus Whitehead Powell ( October 6 , 1812 – July 3 , 1867 ) was the 19th Governor of Kentucky , serving from 1851 to 1855 . He was later elected to represent Kentucky in the U.S. Senate from 1859 to 1865 . The reforms enacted during Powell 's term as governor gave Kentucky one of the top educational systems in the antebellum South . He also improved Kentucky 's transportation system and vetoed legislation that he felt would have created an overabundance of banks in the Commonwealth . Powell 's election as governor marked the end of Whig dominance in Kentucky . Powell 's predecessor , John J. Crittenden , was the last governor elected from the party of the Commonwealth 's favorite son , Henry Clay . Following his term as governor , Powell was elected to the U.S. Senate . Before he could assume office , President James Buchanan dispatched Powell and Major Benjamin McCulloch to Utah to ease tensions with Brigham Young and the Mormons . Powell assumed his Senate seat </t>
+          <t>Maine Coon = The Maine Coon is the largest domesticated breed of cat . It has a distinctive physical appearance and valuable hunting skills . It is one of the oldest natural breeds in North America , specifically " native " to the state of Maine ( though the feline was simply introduced there ) , where it is the official state cat . No records of the Maine Coon 's exact origins and date of introduction to the United States exist , so several competing hypotheses have been suggested . The breed was popular in cat shows in the late 19th century , but its existence became threatened when long-haired breeds from overseas were introduced in the early 20th century . The Maine Coon has since made a comeback and is now one of the more popular cat breeds in the world . The Maine Coon is a large and sociable cat , hence its nickname , " the gentle giant " . It is characterized by a robust bone structure , rectangular body shape , a silky flowing coat and a long , bushy tail . The breed 's colors</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Thomas E. Bramlette = Thomas Elliott Bramlette ( January 3 , 1817 – January 12 , 1875 ) was the 23rd Governor of Kentucky . He was elected in 1863 and guided the state through the latter part of the Civil War and the beginning of Reconstruction . At the outbreak of the war , Bramlette put his promising political career on hold and enlisted in the Union Army , raising and commanding the 3rd Kentucky Infantry . In 1862 , President Abraham Lincoln appointed him district attorney for Kentucky . A year later , he was the Union Democrats ' nominee for governor . Election interference by the Union Army gave him a landslide victory over his opponent , Charles A. Wickliffe . Within a year , however , federal policies such as recruiting Kentucky Negroes for the Union Army and suspending the writ of habeas corpus for Kentucky citizens caused Bramlette to abandon his support of the Lincoln administration and declare that he would " bloodily baptize the state into the Confederacy " . After the war </t>
+          <t>Meat ant = The meat ant ( Iridomyrmex purpureus ) , also known as the gravel ant or southern meat ant , is a species of ant endemic to Australia . A member of the genus Iridomyrmex in the subfamily Dolichoderinae , it was described by British entomologist Frederick Smith in 1858 . The meat ant is associated with many common names due to its appearance , nest-building behaviour and abundance , of which its specific name , purpureus , refers to its coloured appearance . It is among the best-known species of ant found throughout Australia ; it occurs in almost all states and territories except for Tasmania . Its enormous distribution , aggression and ecological importance have made this ant a dominant species . The meat ant is monomorphic ( occurs in a particular form ) , although there is evidence that certain populations can be polymorphic . It is characterised by its dark-bluish body and red head . It is a medium to large species , measuring 6 – 12 mm ( 0.24 – 0.47 in ) . The workers a</t>
         </is>
       </c>
     </row>
@@ -896,32 +896,32 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>['castle', 'church', 'century', 'castles', 'king', 'cathedral', 'tower', 'medieval', 'earl', 'england', 'nave', 'bishop', 'edward', 'chancel', 'built']</t>
+          <t>['september', 'storm', 'mph', 'august', 'hurricane', 'october', 'day', 'damage', 'near', 'early', 'developed', 'later', 'tropical', 'began', 'caused']</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Nidan = Nidan ( sometimes known as Midan or Idan ) was a Welsh priest and , according to some sources , a bishop , in the 6th and 7th centuries . He is now commemorated as a saint . He was the confessor for the monastery headed by St Seiriol at Penmon , and established a church at what is now known as Llanidan , which are both places on the Welsh island of Anglesey . He is the patron saint of two churches in Anglesey : St Nidan 's Church , Llanidan , built in the 19th century , and its medieval predecessor , the Old Church of St Nidan , Llanidan . Midmar Old Kirk in Aberdeenshire , Scotland , is also dedicated to him : Nidan is said to have helped to establish Christianity in that area as a companion of St Kentigern . St Nidan 's , Llanidan , has a reliquary dating from the 14th or 16th century , which is said to house his relics . = = Life = = Little is known in detail about Nidan 's life , and his year and place of birth are unknown . He is sometimes referred to as " Midan " or " Ida</t>
+          <t>1996 Atlantic hurricane season = The 1996 Atlantic hurricane season had the most major hurricanes since 1964 , which are Category 3 or higher on the Saffir-Simpson hurricane wind scale . Featuring a total of thirteen named storms , nine hurricanes , and six major hurricanes , the season officially began on June 1 , 1996 , and ended on November 30 , 1996 , dates which conventionally delimit the period of each year when most tropical cyclones form in the Atlantic basin . The season 's first tropical cyclone , Tropical Storm Arthur , developed on June 17 , while the final cyclone , Hurricane Marco dissipated on November 26 . The most intense hurricane , Edouard , was a powerful Cape Verde-type hurricane that affected portions of the Mid-Atlantic states and New England . The season featured nine tropical cyclone landfalls , including six hurricanes , one of which was a major hurricane . In total , six major hurricanes formed during the 1996 Atlantic hurricane season — the highest number pr</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Cynfarwy = Cynfarwy was a Christian in the 7th century about whom little is known . He was venerated by the early church in Wales as a saint , although he was never formally canonised . St Cynfarwy 's Church in Anglesey is dedicated to him , and his name is also preserved in the name of the settlement around the church , Llechgynfarwy ( or sometimes " Llechcynfarwy " ) . His feast day is in November , although the date varies between sources . = = Life and commemoration = = Little is known for certain about Cynfarwy ; his dates of birth and death are not given in the Bonedd y Saint ( a Welsh genealogical tract compiled in the late 18th century using material from older manuscripts ) . According to the 19th-century Celtic scholar Robert Williams , Cynfarwy was active in the 7th century . According to the Bonedd y Saint , he was the son of the otherwise unknown " Awy ab Llehenog , Lord of Cornwall " . Cynfarwy is venerated as a saint , although he was never canonized by a pope : as the h</t>
+          <t xml:space="preserve">1989 Atlantic hurricane season = The 1989 Atlantic hurricane season featured the costliest tropical cyclone in the Atlantic basin at the time , Hurricane Hugo . The season officially began on June 1 , and ended on November 30 . It was a near average season with 11 named storms . The first storm , Tropical Depression One , developed on June 15 , and dissipated two days later without effects on land . Later that month , Tropical Storm Allison caused severe flooding , especially in Texas and Louisiana . Tropical Storm Barry , Tropical Depressions Six , Nine , and Thirteen , and Hurricanes Erin and Felix caused negligible impact . Hurricane Gabrielle and Tropical Storm Iris caused light effects on land , with the former resulting in nine fatalities from rip currents offshore the East Coast of the United States and Atlantic Canada , while the latter produced minor flooding in the United States Virgin Islands . The most notable storm of the season was Hurricane Hugo , a Category 5 hurricane </t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Æthelric II = Æthelric ( called Æthelric II to distinguish him from an earlier Æthelric who was also bishop of Selsey and also spelled Ethelric ; died c . 1076 ) was the second to last medieval Bishop of Selsey in England before the see was moved to Chichester . Consecrated a bishop in 1058 , he was deposed in 1070 for unknown reasons and then imprisoned by King William I of England . He was considered one of the best legal experts of his time , and was even brought from his prison to attend the trial on Penenden Heath where he gave testimony about English law before the Norman Conquest of England . = = Early life = = Æthelric was a monk at Christ Church Priory at Canterbury prior to his becoming a bishop . Several historians opine that he might have been the same as the Æthelric who was a monk of Canterbury and a relative of Godwin , Earl of Wessex . That Æthelric was elected by the monks of Canterbury to be Archbishop of Canterbury in 1050 , but was not confirmed by King Edward the C</t>
+          <t>1954 Atlantic hurricane season = The 1954 Atlantic hurricane season resulted in over $ 750 million in damage , the most of any season at the time . The season officially began on June 15 , and nine days later the first named storm developed . Hurricane Alice developed in the Gulf of Mexico and moved inland along the Rio Grande , producing significant precipitation and record flooding that killed 55 people . Activity was slow until late August ; only Barbara , a minimal tropical storm , developed in July . In the span of two weeks , hurricanes Carol and Edna followed similar paths before both striking New England as major hurricanes . The latter became the costliest hurricane in Maine 's history . In late September , Tropical Storm Gilda killed 29 people after drenching northern Honduras . A tropical depression in early October was captured by a high-altitude photograph on a rocket , thus producing the first large-scale image of a tropical cyclone . The strongest and deadliest hurricane</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>St Mary 's Church , Llanfair Mathafarn Eithaf = St Mary 's Church , Llanfair Mathafarn Eithaf is a small medieval church in Anglesey , north Wales . The earliest parts of the building , including the nave and the north doorway , date from the 14th century . Other parts , including the chancel and the east window , date from the 15th century . It is associated with the Welsh poet and clergyman Goronwy Owen , who was born nearby and served as curate here . He later travelled to America to teach at The College of William &amp; Mary , Virginia . The church is still in use for worship , as part of the Church in Wales , as one of three churches in the combined parish of Llanfair Mathafarn Eithaf with Llanbedrgoch with Pentraeth . It is a Grade II * listed building , a national designation given to " particularly important buildings of more than special interest " , because it is a " good rural church retaining substantial medieval fabric . " = = History and location = = St Mary 's Church is situ</t>
+          <t xml:space="preserve">1899 Atlantic hurricane season = The 1899 Atlantic hurricane season featured the longest-lasting tropical cyclone in the Atlantic basin on record . There were nine tropical storms , of which five became hurricanes . Two of those strengthened into major hurricanes , which are Category 3 or higher on the modern day Saffir – Simpson hurricane wind scale . The first system was initially observed in the northeastern Gulf of Mexico on June 26 . The tenth and final system dissipated near Bermuda on November 10 . These dates fall within the period with the most tropical cyclone activity in the Atlantic . In post-season analysis , two tropical cyclones that existed in October were added to HURDAT – the official Atlantic hurricane database . At one point during the season , September 3 through the following day , a set of three tropical cyclones existed simultaneously . The most significant storm of the season was Hurricane Three , nicknamed the San Ciriaco hurricane . A post-season analysis of </t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Hugh Nonant = Hugh Nonant ( sometimes Hugh de Nonant ; died 27 March 1198 ) was a medieval Bishop of Coventry in England . A great-nephew and nephew of two Bishops of Lisieux , he held the office of archdeacon in that diocese before serving successively Thomas Becket , the Archbishop of Canterbury and King Henry II of England . Diplomatic successes earned him the nomination to Coventry , but diplomatic missions after his elevation led to a long delay before he was consecrated . After King Henry 's death , Nonant served Henry 's son , King Richard I , who rewarded him with the office of sheriff in three counties . Nonant replaced his monastic cathedral chapter with secular clergy , and attempted to persuade his fellow bishops to do the same , but was unsuccessful . When King Richard was captured and held for ransom , Nonant supported Prince John 's efforts to seize power in England , but had to purchase Richard 's favour when the king returned . = = Early life = = Nonant was a great-nep</t>
+          <t xml:space="preserve">Hurricane Charley = Hurricane Charley was the third named storm , the second hurricane , and the second major hurricane of the 2004 Atlantic hurricane season . Charley lasted from August 9 to August 15 , and at its peak intensity it attained 150 mph ( 240 km / h ) winds , making it a strong Category 4 hurricane on the Saffir-Simpson Hurricane Scale . It made landfall in southwestern Florida at maximum strength , making it the strongest hurricane to hit the United States since Hurricane Andrew struck Florida in 1992 . After moving slowly through the Caribbean Sea , Charley crossed Cuba on Friday , August 13 as a Category 3 hurricane , causing heavy damage and four deaths . That same day , it crossed over the Dry Tortugas , just 22 hours after Tropical Storm Bonnie had struck northwestern Florida . It was the first time in history that two tropical cyclones struck the same state in a 24-hour period . At its peak intensity of 150 mph ( 240 km / h ) , Hurricane Charley struck the northern </t>
         </is>
       </c>
     </row>
@@ -931,32 +931,32 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>['yard', 'yards', 'touchdown', 'season', 'michigan', 'team', 'nba', 'league', 'coach', 'tech', 'alabama', 'football', 'points', 'quarter', 'games']</t>
+          <t>['said', 'told', 'death', 'police', 'murder', 'family', 'life', 'found', 'asked', 'relationship', 'killed', 'later', 'mother', 'character', 'man']</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Chad Mottola = Charles Edward " Chad " Mottola ( born October 15 , 1971 ) is an American retired professional baseball player who played five seasons in Major League Baseball ( MLB ) as an outfielder . Considered a journeyman , Mottola played professionally from 1992 through 2007 , appearing in 59 MLB games and 1,801 minor league games . He was the hitting coach for the Toronto Blue Jays during the 2013 season , but his contract was not renewed for 2014 . Mottola is an alumnus of the University of Central Florida ( UCF ) , where he played college baseball for the UCF Knights baseball team . A highly regarded prospect , Mottola was selected by the Cincinnati Reds with the fifth overall selection of the 1992 MLB Draft . Mottola played in minor league baseball for different organizations , receiving major league playing time with the Cincinnati Reds in 1996 , the Toronto Blue Jays in 2000 and 2006 , the Florida Marlins in 2001 and the Baltimore Orioles in 2004 . As he received less playin</t>
+          <t>Mercedes McQueen = Mercedes Maria Theresa Immaculata McQueen ( previously Owen , Fisher and Browning ) is a fictional character from the British Channel 4 soap opera Hollyoaks , played by Jennifer Metcalfe . She debuted on-screen during the episode airing on 19 June 2006 as the first character to be introduced to the series by series producer , Bryan Kirkwood . In 2008 Metcalfe feared that the character was to be axed but was later reassured by the series producer that she would not be . Metcalfe later stated her intention to stay with the series . Mercedes is part of the McQueen family and is the longest serving McQueen on the series . On 26 August 2014 , it was revealed that Metcalfe had decided to quit the soap . In November 2014 , Mercedes was presumably stabbed to death , with her body discarded . However , Metcalfe returned to screens on 17 February 2015 in a surprise , unannounced twist which saw Mercedes revealed as alive and well , living in Nice , France . It was announced th</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Mickey Micelotta = Robert Peter " Mickey " Micelotta ( born October 20 , 1928 ) is a former American shortstop in Major League Baseball ( MLB ) . He played 13 total seasons of professional baseball , two of which were spent in the National League with the Philadelphia Phillies . In 17 career MLB games , Micelotta posted a batting average of .000 and had two runs in nine plate appearances . Born and raised in Wisconsin , Micelotta first played professionally with the Dayton Indians and Carbondale Pioneers in 1947 . Over the next three seasons , he played for various minor league teams in the Phillies organization before missing the 1951 and 1952 seasons , serving in the Korean War . He returned and played for the Terre Haute Phillies in 1953 and the Syracuse Chiefs from 1954 to 1955 , splitting time between the Chiefs and the Phillies ' major league squad . Micelotta spent the next three seasons with the Miami Marlins and three seasons after that with the Birmingham Barons before retiri</t>
+          <t>Lewis Archer = Lewis Archer is a fictional character from the British soap opera Coronation Street , played by Nigel Havers . The character was created and introduced as a love interest for Audrey Roberts ( Sue Nicholls ) . Executive producer Kim Crowther revealed the team wanted an actor who was slightly younger than Audrey and who was very charming . Various actors were considered for the part , but the casting director suggested Havers as she knew he was a big fan of the show . The actor said he could not turn down a chance to appear in Coronation Street as his character had an interesting story arc . Havers was contracted until July 2010 and he made his debut as Lewis in the episode broadcast on 18 December 2009 . Lewis is a gentleman escort , who is described as being suave , charming and charismatic . He is first seen accompanying Claudia Colby ( Rula Lenska ) to a Christmas ball . He is introduced to Audrey , who falls for his charm and later hires him to be her companion to ano</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve">J. T. White = John T. " J.T. " White ( July 10 , 1920 – November 21 , 2005 ) was a college football assistant coach , and a second-team 1947 College Football All-American center who played for national championship teams at both the University of Michigan and Ohio State University . White also played basketball for the Ohio State Buckeyes men 's basketball team . Although White was drafted to play professional football , he chose to pursue a career as an assistant football coach for both the Michigan Wolverines and Penn State Nittany Lions football teams . He served as an assistant coach for a national champion at Michigan and three undefeated and untied seasons at Penn State . White served in the United States Army during World War II causing a break in his collegiate education . = = Personal = = White was born in Wadley , Georgia and raised in River Rouge , Michigan . White earned his bachelor 's degree in education from Michigan in 1948 . He earned his master 's degree in education </t>
+          <t>Wyatt Earp = Wyatt Berry Stapp Earp ( March 19 , 1848 – January 13 , 1929 ) was an American Old West gambler , a deputy sheriff in Pima County , and deputy town marshal in Tombstone , Arizona Territory , who took part in the Gunfight at the O.K. Corral , during which lawmen killed three outlaw Cowboys . He is often regarded as the central figure in the shootout in Tombstone , although his brother Virgil was Tombstone city marshal and Deputy U.S. Marshal that day , and had far more experience as a sheriff , constable , marshal , and soldier in combat . Earp lived a restless life . He was at different times a constable , city policeman , county sheriff , Deputy U.S. Marshal , teamster , buffalo hunter , bouncer , saloon-keeper , gambler , Brothel keeper , miner , and boxing referee . Earp spent his early life in Iowa . In 1870 , Earp married his first wife , Urilla Sutherland Earp , who contracted typhoid fever and died shortly before their first child was to be born . Within the next tw</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Eduardo Núñez = Eduardo Michelle Núñez Méndez ( born June 15 , 1987 ) is a Dominican professional baseball infielder for the Minnesota Twins of Major League Baseball ( MLB ) . He played in MLB for the New York Yankees from 2010 through 2013 . Although shortstop is his primary position , Núñez serves as a utility infielder , and played in the outfield for the Yankees as well . The Yankees signed Núñez as an international free agent in 2004 . He played minor league baseball in their organization from 2005 through 2010 , until he made his MLB debut with the Yankees on August 19 , 2010 . He has served to allow Derek Jeter and Alex Rodriguez the ability to take days off in the field . Due to struggles and inconsistency , the Yankees designated Núñez for assignment at the start of the 2014 season . He was traded to the Twins , and enjoyed a breakout season in 2016 , when he was named to appear in the MLB All-Star Game . = = Professional career = = = = = Minor leagues = = = The New York Yanke</t>
+          <t>Bali Nine = The Bali Nine is the name given to a group of nine Australians arrested 17 April 2005 , and convicted for smuggling 8.3 kg ( 18 lb ) of heroin valued at around A $ 4 million ( US $ 3.1 million ) from Indonesia to Australia . Ringleaders Andrew Chan and Myuran Sukumaran were sentenced to death and were executed on 29 April 2015 . Other members Si Yi Chen , Michael Czugaj , Renae Lawrence , Tan Duc Thanh Nguyen , Matthew Norman , Scott Rush , and Martin Stephens were sent to prison . Australian authorities contacted their Indonesian counterparts with the tip-off that precipitated these arrests . On 13 February 2006 , Lawrence and Rush , the first of the nine to face sentencing , were sentenced to life imprisonment . The next day , Czugaj and Stephens were sentenced to life imprisonment , and the group ringleaders , Chan and Sukumaran , were sentenced to death by firing squad , the first ever death sentences imposed by the Denpasar District Court . The other three , Norman , C</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Orator Shafer = George W. Shafer [ sometimes spelled Shaffer or Schaefer ] ( October 1851 – January 21 , 1922 ) was an outfielder in Major League Baseball . Nicknamed " Orator " , because he was an avid speaker , Shafer played for 10 teams in four different major leagues between 1874 and 1890 . Though he was a good hitter who batted over .300 three times , Shafer was best known for his defensive abilities . He led the National League 's outfielders in assists four times . In 1879 , he set an MLB single-season record with 50 outfield assists , which is a mark that has stood for over 130 years . He was considered by some to be the greatest right fielder of his era . Shafer was 5 feet 9 inches ( 1.75 m ) tall and weighed 165 pounds ( 75 kg ) . = = Background = = Shafer was born in Philadelphia , Pennsylvania , in 1851 . He was a " promising young Philadelphia amateur " before starting his professional baseball career in 1874 in the National Association . That year , he played in nine game</t>
+          <t xml:space="preserve">Death of Keith Blakelock = Keith Henry Blakelock , a London Metropolitan Police constable , was killed on 6 October 1985 during rioting on the Broadwater Farm housing estate in Tottenham , north London . The trouble broke out after a local black woman died of heart failure during a police search of her home . It took place against a backdrop of unrest in several English cities and a breakdown of relations between the police and black communities . PC Blakelock had been assigned on the night of his death to Serial 502 , a unit of 10 constables and one sergeant dispatched to protect firefighters . When the rioters forced the officers back , Blakelock stumbled and fell . Surrounded by a mob of 30 to 50 people , he received more than 40 injuries inflicted by machetes or similar , and was found with a six-inch-long knife in his neck , buried up to the hilt . He was the first constable to be killed in a riot in Britain since 1833 , when PC Robert Culley was stabbed to death in Clerkenwell , </t>
         </is>
       </c>
     </row>
@@ -966,32 +966,32 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>['olympics', 'olympic', 'athletes', 'medal', 'championships', 'murray', 'meter', 'freestyle', 'round', 'beijing', 'medals', 'games', 'gold', 'seconds', 'relay']</t>
+          <t>['city', 'million', 'school', 'company', 'building', 'stadium', 'students', 'center', 'schools', 'year', 'sports', 'largest', 'located', 'community', 'years']</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Belize at the 2008 Summer Olympics = Belize competed in the 2008 Summer Olympics , held in Beijing , People 's Republic of China from 8 to 24 August 2008 . Its participation in Beijing marked its eighth Olympic appearance under the name " Belize " and its tenth overall , as its first two appearances ( 1968 in Mexico City and 1972 in Munich ) were under the name " British Honduras " . The Belizean delegation in 2008 included four athletes : three participated in track and field events ( Jonathan Williams , Tricia Flores , and Jayson Jones ) and one in taekwondo ( Alfonso Martínez ) . Belize did not medal in Beijing , and had not medaled before Beijing , but Jonathan Williams became the first Belizean athlete to advance past the first round of any Olympic event . = = Background = = Belize first participated in the Olympic games at the 1968 Summer Olympics in Mexico City and has appeared in every Summer Olympics since with the exception of the 1980 Summer Olympics in the Soviet Union , re</t>
+          <t>Apogee Stadium = Apogee Stadium is a college football stadium located at the junction of Interstate 35 East and West in Denton , Texas . Opened in 2011 , it is home to the University of North Texas ( UNT ) Mean Green football team , which competes in Conference USA . The facility replaced Fouts Field , where the school 's football program had been based since 1952 . The stadium was proposed by the University of North Texas System Board of Regents after the 2002 New Orleans Bowl . Designed by HKS , Inc . , it was constructed at a cost of $ 78 million after a contentious student body election in 2008 . It was originally named " Mean Green Stadium " , but was renamed when ResNet provider Apogee purchased the naming rights in 2011 . The stadium hosted its first major event on September 10 , 2011 when the Mean Green lost 48 – 23 against the University of Houston Cougars . That game 's attendance of 28,075 holds the record for the stadium ; the Mean Green have never sold out a home game in t</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Mauritania at the 2008 Summer Olympics = Mauritania competed at the 2008 Summer Olympics which was held in Beijing , China . The country 's participation at Beijing marked its seventh appearance in the Summer Olympics since its debut in the 1984 Summer Olympics . The delegation included two track and field athletes , Souleymane Ould Chebal and Bounkou Camara , who were both selected by wildcards after both failed to meet either the " A " or " B " qualifying standards . Chebal was selected as the flag bearer for the opening ceremony . Neither of the Mauritanians progressed beyond the heats . = = Background = = Mauritania participated in seven Summer Olympic games between its debut in the 1984 Summer Olympics in Los Angeles , United States and the 2008 Summer Olympics in Beijing . Two athletes from Mauritania were selected to compete in the Beijing games ; Souleymane Ould Chebal in the track and field 800 meters and Bounkou Camara in the track and field 100 meters . Both were selected by</t>
+          <t>Davenport , Iowa = Davenport is the county seat of Scott County in Iowa and is the largest of the Quad Cities , a metropolitan area with a population estimate of 382,630 and a CSA population of 474,226 , making it the 90th largest CSA in the nation . Davenport was founded on May 14 , 1836 by Antoine LeClaire and was named for his friend , George Davenport , a colonel during the Black Hawk War stationed at nearby Fort Armstrong . According to the 2010 census , the city had a population of 99,685 ( making it Iowa 's third-largest city ) . However , the city is currently appealing this figure , arguing that the Census Bureau missed a section of residents that would place the total population over 100,000 , and indeed , even the Census Bureau 's own estimate for Davenport 's 2011 population is 100,802 . Located approximately halfway between Chicago and Des Moines , Davenport is on the border of Iowa and Illinois . The city is prone to frequent flooding due to its location on the Mississipp</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Great Britain at the 2010 Winter Paralympics = Great Britain competed at the 2010 Winter Paralympics held in Vancouver , Canada . The team was made up of athletes from the whole United Kingdom ; athletes from Northern Ireland , who may elect to hold Irish citizenship under the pre-1999 article 2 of the Irish constitution , are able to be selected to represent either Great Britain or Ireland at the Paralympics . Kelly Gallagher became the first Northern Irish athlete to compete in the Winter Paralympics by taking part in the alpine skiing discipline . Additionally some British overseas territories compete separately from Britain in Paralympic competition . In order to be eligible to take part in the Games athletes had to have a disability that fell into one of the five Paralympics disability categories . Great Britain fielded twelve athletes in total ; a team of five in wheelchair curling , and seven athletes in alpine skiing . The team failed to win a medal for the first time since the</t>
+          <t>Virginia Beach , Virginia = Virginia Beach is an independent city located in the U.S. state of Virginia . As of the 2010 census , the population was 437,994 . In 2015 , the population was estimated to be 452,745 . Although mostly suburban in character , it is the most populous city in Virginia and the 41st most populous city in the nation . Located on the Atlantic Ocean at the mouth of the Chesapeake Bay , Virginia Beach is included in the Hampton Roads metropolitan area . This area , known as " America 's First Region " , also includes the independent cities of Chesapeake , Hampton , Newport News , Norfolk , Portsmouth , and Suffolk , as well as other smaller cities , counties , and towns of Hampton Roads . Virginia Beach is a resort city with miles of beaches and hundreds of hotels , motels , and restaurants along its oceanfront . Every year the city hosts the East Coast Surfing Championships as well as the North American Sand Soccer Championship , a beach soccer tournament . It is a</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Glencora Ralph = Glencora Ralph ( born 8 August 1988 ) is an Australian water polo centre back / driver . She attended the Curtin University of Technology and is a dental therapist . She competes for the Fremantle Marlins in the National Water Polo League , and was on sides that won the league championship in 2003 , 2004 , 2006 and 2007 . She has been a member of the Australia women 's national water polo team on the junior and senior level . She has won gold medals at the 2011 Canada Cup and at the 2007 FINA Junior World Championships . She won silver medals at the 2010 FINA World League Super Finals and at the 2010 FINA Women 's Water Polo World Cup . She won a bronze medal at the 2009 FINA World League Super Finals . She is one of seventeen players vying for thirteen spots on the national team to represent Australia in water polo at the 2012 Summer Olympics . = = Personal = = Ralph was born on 8 August 1988 in Geraldton , Western Australia . She has three siblings , one of whom , Me</t>
+          <t>Saint Paul , Minnesota = Saint Paul ( / ˌseɪnt ˈpɔːl / ; abbreviated St. Paul ) is the capital and second-most populous city of the U.S. state of Minnesota . As of 2015 , the city 's estimated population was 300,851 . Saint Paul is the county seat of Ramsey County , the smallest and most densely populated county in Minnesota . The city lies mostly on the east bank of the Mississippi River in the area surrounding its point of confluence with the Minnesota River , and adjoins Minneapolis , the state 's largest city . Known as the " Twin Cities " , the two form the core of Minneapolis – Saint Paul , the 16th-largest metropolitan area in the United States , with about 3.52 million residents . Founded near historic Native American settlements as a trading and transportation center , the city rose to prominence when it was named the capital of the Minnesota Territory in 1849 . Though Minneapolis is better-known nationally , Saint Paul contains the state government and other important institu</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Great Britain at the 2008 Summer Olympics = The United Kingdom of Great Britain and Northern Ireland competed as Great Britain at the 2008 Summer Olympics in Beijing , China . The United Kingdom was represented by the British Olympic Association ( BOA ) , and the team of selected athletes was officially known as Team GB . Britain is one of only five NOCs to have competed in every modern Summer Olympic Games since 1896 . The delegation of 547 people included 311 competitors – 168 men , 143 women – and 236 officials . The team was made up of athletes from the whole United Kingdom including Northern Ireland ( whose people may elect to hold Irish citizenship and are able to be selected to represent either Great Britain or Ireland at the Olympics ) . Additionally some British overseas territories compete separately from Britain in Olympic competition . Great Britain 's medal performance at the 2008 Summer Olympics was its best in a century ; only its performance at the 1908 Summer Olympics </t>
+          <t>Bellaire , Texas = Bellaire is a city in southwest Harris County , Texas , United States , within the Houston – Sugar Land – Baytown metropolitan area . As of the 2010 U.S. Census , the city population was 16,855 and is surrounded by the cities of Houston and West University Place . Bellaire is known as the " City of Homes , " owing to its mostly residential character ; however , there are offices along the 610 Loop within the city limits . = = History = = Bellaire was founded in 1908 by William Wright Baldwin , who was the president of the South End Land Company . Baldwin , a native of Iowa , was well known as the vice president of the Burlington Railroad . Bellaire was founded on what was part of William Marsh Rice 's 9,449 acres ( 38.24 km2 ) ranch . Baldwin surveyed the eastern 1,000 acres ( 4.0 km2 ) of the ranch into small truck farms . He named those farms " Westmoreland Farms " . Baldwin started Bellaire in the middle of " Westmoreland Farms " to serve as a residential neighbor</t>
         </is>
       </c>
     </row>
@@ -1001,32 +1001,32 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>['match', 'tag', 'wrestling', 'championship', 'wwe', 'ring', 'raw', 'event', 'michaels', 'defeated', 'heavyweight', 'smackdown', 'feud', 'wwf', 'angle']</t>
+          <t>['film', 'role', 'appeared', 'award', 'acting', 'director', 'roles', 'success', 'actor', 'performance', 'directed', 'comedy', 'drama', 'actors', 'films']</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Backlash ( 2007 ) = Backlash ( 2007 ) was a professional wrestling pay-per-view event produced by World Wrestling Entertainment ( WWE ) , which took place on April 29 , 2007 , at the Philips Arena in Atlanta , Georgia . Following WrestleMania , all pay-per-views became tri-branded . It was the ninth annual event under the Backlash name and starred talent from Raw , SmackDown ! , and ECW . The main match on the Raw brand was a Fatal Four-Way match for the WWE Championship involving champion John Cena , Randy Orton , Edge , and Shawn Michaels . Cena won the match and retained the championship after pinning Orton . The primary match on the SmackDown ! brand was a Last Man Standing match for the World Heavyweight Championship between The Undertaker and Batista , which ended in a no-contest after both men failed get to their feet before the referee counted to ten . The featured match on the ECW brand was Bobby Lashley versus Team McMahon ( Umaga , Vince and Shane McMahon ) in a Handicap mat</t>
+          <t>Deborah Kerr = Deborah Kerr CBE ( / kɑːr / ; born Deborah Jane Kerr-Trimmer ; 30 September 1921 – 16 October 2007 ) was a Scottish-born film , theatre and television actress . During her career , she won a Golden Globe for her performance as Anna Leonowens in the motion picture The King and I ( 1956 ) and the Sarah Siddons Award for her performance as " Laura Reynolds " in the play Tea and Sympathy ( a role she originated on Broadway ) . She was also a three-time winner of the New York Film Critics Circle Award for Best Actress . Kerr was nominated six times for the Academy Award for Best Actress , more than any other actress without ever winning . In 1994 , however , having already received honorary awards from the Cannes Film Festival and BAFTA , she received an Academy Honorary Award with a citation recognising her as " an artist of impeccable grace and beauty , a dedicated actress whose motion picture career has always stood for perfection , discipline and elegance " . As well as T</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve">World Heavyweight Championship ( WWE ) = The World Heavyweight Championship was a professional wrestling world heavyweight championship owned by WWE . It was one of two top championships in WWE , complementing the WWE World Championship . It was established under the Raw brand in 2002 , after Raw and SmackDown ! became distinct brands under WWE , and moved between both brands on different occasions ( mainly as a result of the WWE draft ) until August 29 , 2011 when all programming became full roster " supershows " . The World Heavyweight Championship was retired at the WWE PPV TLC : Tables , Ladders , and Chairs on December 15 , 2013 when it was unified with the WWE Championship . The title was one of six to be represented by the historic Big Gold Belt , first introduced in 1986 . Its heritage can be traced back to the first world heavyweight championship , thereby giving the belt a legacy over 100 years old , the oldest in the world . = = History = = = = = Origin = = = WWE introduced </t>
+          <t xml:space="preserve">Kadhalikka Neramillai = Kadhalikka Neramillai ( English : No Time for Love ) is a 1964 Indian Tamil-language romantic comedy film produced and directed by C. V. Sridhar , who also conceived and co-wrote its script with Chitralaya Gopu . The film features an ensemble cast consisting of T. S. Balaiah , R. Muthuraman , Nagesh , Rajasree , Sachu , Ravichandran and Kanchana . The latter two made their debut in Tamil cinema with this film . The plot of Kadhalikka Neramillai revolves around Viswanathan , an estate owner who hopes to get his daughters Nirmala and Kanchana married to wealthy grooms . However , Nirmala falls in love with Ashok , a poor man who was once employed by Vishwanathan . To earn Viswanathan 's approval , Ashok pretends to be the only heir of a rich businessman ; he is supported by his friend Vasu , who poses as Ashok 's fictional millionaire father Chidambaram . A comedy of errors ensues when Vasu discovers his lover Kanchana is Viswanathan 's other daughter . Principal </t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Cyber Sunday ( 2007 ) = Cyber Sunday ( 2007 ) was the fourth annual Cyber Sunday professional wrestling pay-per-view event produced by World Wrestling Entertainment ( WWE ) . It was presented by Fathead and took place on October 28 , 2007 , at the Verizon Center in Washington , D.C. The most important feature of Cyber Sunday is the ability for fans to vote online through WWE.com on certain aspects of every match . The main match on the SmackDown ! brand was Batista versus The Undertaker for the World Heavyweight Championship , which Batista won by pinfall after executing a Batista Bomb . The Special Guest Referee , which was either Stone Cold Steve Austin , John " Bradshaw " Layfield or Mick Foley . The predominant match on the Raw brand was for the WWE Championship between Randy Orton and the fans ' choice of either Shawn Michaels , Jeff Hardy or Mr. Kennedy . The voting for the event started on October 9 , 2007 , and ended during the event . Most of the existing feuds continued after</t>
+          <t>Jessie Bond = Jessie Bond ( 10 January 1853 – 17 June 1942 ) was an English singer and actress best known for creating the mezzo-soprano soubrette roles in the Gilbert and Sullivan comic operas . She spent twenty years on the stage , the bulk of them with the D 'Oyly Carte Opera Company . Musical from an early age , Bond began a concert singing career in Liverpool by 1870 . At the age of 17 , she entered into a brief , unhappy marriage . After leaving her abusive husband , she continued her concert career and studied at the Royal Academy of Music in London with such famous singing teachers as Manuel García . At the age of 25 , in 1878 , Bond began her theatrical career , creating the role of Cousin Hebe in Gilbert and Sullivan 's H.M.S. Pinafore , which became an international success . After this , she created roles of increasing importance with the D 'Oyly Carte Opera Company in a series of successful comic operas , including the title role in Iolanthe ( 1882 ) , Pitti Sing in The Mi</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Judgment Day ( 2007 ) = Judgment Day ( 2007 ) was the ninth annual Judgment Day professional wrestling pay-per-view event produced by World Wrestling Entertainment ( WWE ) . It took place on May 20 , 2007 from the Scottrade Center in St. Louis , Missouri . This was the first Judgment Day event since 2003 to be an inter-brand pay-per-view , as it featured talent from the Raw , SmackDown ! , and ECW brands . The main match on the Raw brand was John Cena versus The Great Khali for the WWE Championship , which Cena won after forcing Khali to submit to the STFU . The featured match on the SmackDown ! brand was Edge versus Batista for the World Heavyweight Championship , which Edge won via pinfall with a school boy pin . The primary match on the ECW brand was a Handicap match for the ECW World Championship between Team McMahon ( champion Vince McMahon , Shane McMahon and Umaga ) and Bobby Lashley . Lashley won the match by pinning Shane McMahon ; however , he did not win the title since he d</t>
+          <t xml:space="preserve">Malliswari ( 1951 film ) = Malliswari is a 1951 Indian Telugu-language historical romance film produced and directed by Bommireddy Narasimha Reddy under his banner Vauhini Studios . N. T. Rama Rao and Bhanumathi Ramakrishna star as a couple – Nagaraju and Malliswari – who are separated by Malliswari 's greedy mother . Malliswari is sent to the king 's palace according to the custom of " Rani Vasam " , a tradition during the Vijayanagara Empire wherein young women were fetched to the palace with an offering gold and jewellery to their parents . The rest of the film focuses on the consequences faced by Nagaraju when he , against all rules , surreptitiously enters the palace to meet Malliswari . Narasimha Reddy wanted to make a film based on Krishnadevaraya 's character ever since his visit to Hampi for the filming of his debut Vandemataram ( 1939 ) . He employed Devulapalli Krishnasastri to write the film 's script and took inspiration from Buchibabu 's play " Rayalavari Karunakruthyamu </t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Survivor Series ( 2005 ) = Survivor Series ( 2005 ) was the 19th annual Survivor Series professional wrestling pay-per-view event produced by World Wrestling Entertainment ( WWE ) . It took place on November 27 , 2005 , at the Joe Louis Arena in Detroit , Michigan and consisted of six professional wrestling matches involving wrestlers from the Raw and SmackDown brands . In the first of two main event matches , WWE Champion John Cena defeated Kurt Angle to retain his title . The second main event was an interpromotional 5-on-5 Survivor Series match , in which Team SmackDown ( Batista , Rey Mysterio , John " Bradshaw " Layfield ( JBL ) , Bobby Lashley , and Randy Orton ) defeated Team Raw ( Shawn Michaels , Kane , The Big Show , Carlito , and Chris Masters ) after Orton last eliminated Michaels . In another match , Triple H defeated Ric Flair in a Last Man Standing match . = = Background = = The event 's card consisted of six professional wrestling involving wrestlers from either Raw or </t>
+          <t>Jennifer Connelly = Jennifer Lynn Connelly ( born December 12 , 1970 ) is an American film actress who began her career as a child model . She appeared in magazine , newspaper and television advertising , before she made her debut role in the 1984 crime film Once Upon a Time in America . Connelly continued modeling and acting , starring in films such as the 1986 film Labyrinth and the 1991 films Career Opportunities and The Rocketeer . She gained critical acclaim for her work in the 1998 science fiction film Dark City and for her portrayal of Marion Silver in the 2000 drama Requiem for a Dream . In 2002 , Connelly won an Academy Award , a Golden Globe Award and a BAFTA Award for her supporting role as Alicia Nash in Ron Howard 's 2001 biopic A Beautiful Mind . Her later credits include the 2003 Marvel superhero film Hulk where she played Bruce Banner 's true love Betty Ross , the 2005 horror film Dark Water , the 2006 drama Blood Diamond , the 2008 science fiction remake The Day the Ea</t>
         </is>
       </c>
     </row>
@@ -1036,32 +1036,32 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>['watershed', 'creek', 'dam', 'island', 'population', 'city', 'area', 'river', 'volcano', 'volcanic', 'flows', 'lighthouse', 'lava', 'bay', 'water']</t>
+          <t>['cambridge', 'oxford', 'boat', 'competition', 'silver', 'summer', 'competed', 'referred', 'medal', 'seconds', 'olympics', 'compete', 'athletes', 'champions', 'heat']</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Little Catawissa Creek = Little Catawissa Creek is a tributary of Catawissa Creek in Columbia County and Schuylkill County , in Pennsylvania , in the United States . It is approximately 10.8 miles ( 17.4 km ) long and flows through Conyngham Township in Columbia County and Union Township and North Union Township in Schuylkill County . The named tributaries of the creek include Stony Run and Trexler Run . The creek has some alkalinity and is slightly acidic . The main rock formations in the watershed of it are the Mauch Chunk Formation , the Pocono Formation , and the Pottsville Formation . A number of other rock formations occur in small areas of the watershed as well . The main soils in the watershed are the Leck Kill soil and the Hazleton soil . The watershed of Little Catawissa Creek has an area of 16.70 square miles ( 43.3 km2 ) . A number of bridges cross the creek . There are a number of major roads in the watershed of the creek and most of the creek is within several hundred met</t>
+          <t>The Boat Race 1956 = The 102nd Boat Race took place on 24 March 1956 . Held annually , the Boat Race is a side-by-side rowing race between crews from the Universities of Oxford and Cambridge along the River Thames . In a race umpired by former rower Kenneth Payne , Cambridge won by one-and-a-quarter lengths in a time of 18 minutes 36 seconds , the fourth quickest time in the history of the event . The victory took the overall record to 56 – 45 in their favour . = = Background = = The Boat Race is a side-by-side rowing competition between the University of Oxford ( sometimes referred to as the " Dark Blues " ) and the University of Cambridge ( sometimes referred to as the " Light Blues " ) . First held in 1829 , the race takes place on the 4.2-mile ( 6.8 km ) Championship Course on the River Thames in southwest London . The rivalry is a major point of honour between the two universities ; it is followed throughout the United Kingdom and , as of 2014 , broadcast worldwide . Cambridge wen</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Muncy Creek = Muncy Creek ( also known as Big Muncy Creek ) is a tributary of the West Branch Susquehanna River in Sullivan County and Lycoming County , in Pennsylvania , in the United States . It is approximately 34.5 miles ( 55.5 km ) long . The watershed of the creek has an area of 216 square miles ( 560 km2 ) . The creek 's discharge averages 49 cubic feet per second ( 1.4 m3 / s ) at Sonestown , but can be up to a thousand times higher at Muncy . The headwaters of the creek are on the Allegheny Plateau . Rock formations in the watershed include the Chemung Formation and the Catskill Formation . There are a number of lakes in the watershed of Muncy Creek , including Eagles Mere Lake , Highland Lake , and Beaver Lake . The creek was known as Occohpocheny to Native Americans . The area in its vicinity was settled in 1783 . Various other industries and mills were constructed in the creek 's vicinity from the late 18th century to the early 20th century . Wild trout naturally reproduce </t>
+          <t>Mauritania at the 2004 Summer Olympics = Mauritania competed at the 2004 Summer Olympics in Athens , Greece , from 13 to 29 August 2004 . The country 's participation at Athens marked its sixth appearance in the Summer Olympics since its debut in the 1984 Summer Olympics . The delegation included two track and field athletes , Youba Hmeida and Aminata Kamissoko , who were both selected by wildcards after both failed to meet either the " A " or " B " qualifying standards . Hmeida was selected as the flag bearer for the opening ceremony . Neither of the Mauritanians progressed beyond the heats . = = Background = = Mauritania participated in six Summer Olympic games between its debut in the 1984 Summer Olympics in Los Angeles , United States and the 2004 Summer Olympics in Athens . The Mauritania National Olympic Committee ( NOC ) selected two athletes via wildcards . Usually , an NOC would be able to enter up to 3 qualified athletes in each individual event as long as each athlete met th</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve">West Branch Fishing Creek = West Branch Fishing Creek is one of the northernmost major tributaries of Fishing Creek in Sullivan County , Pennsylvania and Columbia County , Pennsylvania , in the United States . It is 11.1 miles ( 17.9 km ) long and flows through Davidson Township , Sullivan County and Sugarloaf Township , Columbia County . The creek 's watershed has an area of 33.5 square miles , nearly all of which is forested land . Rock formations in the watershed of West Branch Fishing Creek include the Catskill Formation , the Huntley Mountain Formation , and the Burgoon Sandstone . North Mountain , Huckleberry Mountain , and Central Mountain are all in the creek 's vicinity . The temperature of the creek 's waters ranges from − 2 ° C ( 28 ° F ) to 23 ° C ( 73 ° F ) and its pH ranges from approximately 5.5 to just under 7.0 . The creek 's discharge ranges from nearly 0 cubic meters per second to approximately 25 cubic meters per second . Communities in the watershed of West Branch </t>
+          <t>Saint Vincent and the Grenadines at the 2008 Summer Olympics = Saint Vincent and the Grenadines sent a delegation to compete at the 2008 Summer Olympics in Beijing , China . The year 's team included two athletes engaged in track and field events ( Kineke Alexander and Jared Lewis ) , and was accompanied by the team coach , manager , and chaperone . Saint Vincent and the Grenadines ' appearance in Beijing marked its sixth consecutive Olympic appearance since its 1988 debut in Seoul , South Korea , and its smallest delegation to date . Alexander bore the flag of Saint Vincent and the Grenadines in the opening ceremony and neither athlete medaled in their events or advanced to later rounds . = = Background = = Saint Vincent and the Grenadines debuted in the Olympic Games at the 1988 Summer Olympics in Seoul , South Korea and , as of 2008 , has participated in every edition since . The Beijing Games marked the smallest Vincentian delegation in the country 's history , the size having decl</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Sulphur Creek ( California ) = Sulphur Creek is a 4.5-mile ( 7.2 km ) tributary of Aliso Creek in Orange County in the U.S. state of California . Draining about 6 square miles ( 16 km2 ) of mostly residential land in the southern San Joaquin Hills , it is Aliso Creek 's largest tributary . Geologically the Sulphur Creek watershed was once part of a large and shallow sea that covered most of southern California . As the San Joaquin Hills rose and river sediments were deposited , land gradually emerged to form the present-day Orange County coast . Sulphur Creek is located in a crumpled , hilly area in the southern part of this range , formed differently from the continuous mountain chain to the north . Historically , being south of Aliso Creek , the Sulphur Creek watershed was part of the territory of the semi-nomadic Acjachemen Indian group , conquered by Spanish conquistadors in the 17th and 18th centuries and renamed the Juaneño by them . During the 19th century , the watershed became</t>
+          <t>Haiti at the 2008 Summer Olympics = Haiti sent a delegation to compete in the 2008 Summer Olympics , held in Beijing , People 's Republic of China from August 8 to August 24 , 2008 . Its participation in Beijing marked its seventh consecutive appearance at the summer Olympics and its fourteenth appearance overall , with its first being at the 1900 Summer Olympics in Paris . The Haitian Olympic team included seven athletes ( three men and four women ) participating in track and field ( Barbara Pierre , Ginou Etienne , Nadine Faustin-Parker , and Dudley Dorival ) , boxing ( Azea Austinama ) , and judo ( Joel Brutus and Ange Jean Baptiste ) . More women participated for Haiti in 2008 than at any single Olympic games prior . Although Pierre and Dorival advanced to quarterfinals in their events , there were no Haitian medalists in Beijing . Brutus carried his countries flag at the ceremonies . = = Background = = For Haiti , the 2008 Beijing Olympics marked its fourteenth appearance at any O</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Shickshinny Creek = Shickshinny Creek ( historically known as Shickohinna ) is a tributary of the Susquehanna River in the Wyoming Valley in Luzerne County , Pennsylvania , in the United States . It is approximately 10.1 miles ( 16.3 km ) long and flows through Ross Township , Union Township , and Shickshinny . Its watershed has an area of 35.0 square miles ( 91 km2 ) and its tributaries include Culver Creek , Reyburn Creek , and Little Shickshinny Creek . The creek is designated as a Coldwater Fishery and a Migratory Fishery . A sawmill and a gristmill were built on the creek in 1802 and 1804 , respectively . Several bridges have also been constructed over it . The creek was historically polluted by culm near its mouth , but agriculture was the main industry in the watershed in the early 1900s . It was historically used as a water supply . The surficial geology near Shickshinny Creek mainly consists of urban land , fill , alluvium , alluvial terrace , alluvial fan , Wisconsinan Ice-Co</t>
+          <t>Kayla Clarke = Kayla Clarke ( born 6 August 1991 ) is an Australian swimmer who represented Australia at the 2012 Summer Paralympics in swimming , and has medalled at the 2010 Australian Disability Age Group Nationals , and 2010 International Paralympic Swimming World Championships , 2009 Queensland State Championships , 2009 Queensland Secondary School Titles , and 2009 Global Games . She competes in a number of events , including the 100m freestyle , 100m backstroke , 100m breaststroke , 100m butterfly and 200m individual medley . = = Personal = = Clarke was born in Silkstone , Queensland . She has an intellectual disability . She attended Ipswich Central High School and Bremer State High School , and was named the 2009 – 10 Ipswich News YoungStar Sports winner . = = Swimming = = Clarke started swimming competitively in 2007 , and competes in the S14 classification . She was a member of the Woogaroo Swimming Club , and was coached by Tony Keogh , who became her coach in 2008 . She ha</t>
         </is>
       </c>
     </row>
@@ -1071,32 +1071,32 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>['liz', 'dwight', 'jim', 'pam', 'michael', 'episode', 'nbc', 'jack', 'fey', 'jenna', 'andy', 'office', 'tracy', 'kenneth', 'tgs']</t>
+          <t>['album', 'music', 'songs', 'rock', 'recorded', 'recording', 'band', 'beatles', 'lyrics', 'musicians', 'george_harrison', 'sound', 'harrison', 'song', 'bands']</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Tracy Does Conan = " Tracy Does Conan " is the seventh episode of NBC 's first season of 30 Rock . It was written by the series ' creator and executive producer , Tina Fey and it was directed by one of the season 's supervising producers , Adam Bernstein . It first aired on December 7 , 2006 in the United States and November 29 , 2007 in the United Kingdom . Guest stars in the episode included Katrina Bowden , Kevin Brown , Grizz Chapman , Rachel Dratch , Dave Finkel , Steve Hollander , Johnnie May , Maulik Pancholy , Chris Parnell , Aubrey Plaza , Keith Powell , R. N. Rao and Dean Winters . Conan O 'Brien appeared as himself in this episode . The episode marks the first appearance of Chris Parnell as recurring character , Dr. Leo Spaceman . This episode revolves around Liz Lemon ( played by Tina Fey ) and Pete Hornberger ( Scott Adsit ) trying to get Tracy Jordan ( Tracy Morgan ) to make a successful appearance on Late Night with Conan O 'Brien , a late night talk show . These attempt</t>
+          <t>Psychedelic rock = Psychedelic rock is a style of rock music that is inspired or influenced by psychedelic culture and attempts to replicate and enhance the mind-altering experiences of psychedelic drugs , most notably LSD . It often uses new recording techniques and effects and sometimes draws on sources such as the ragas and drones of Indian music . It was pioneered by musicians including the Beatles , the Beach Boys , and the Byrds , emerging as a genre during the mid-1960s among folk rock and blues rock bands in the United Kingdom and United States , such as the 13th Floor Elevators , Grateful Dead , Jefferson Airplane , the Jimi Hendrix Experience , Cream , The Doors and Pink Floyd . It reached a peak in between 1967 and 1969 with the Summer of Love and Woodstock Rock Festival , respectively , becoming an international musical movement and associated with a widespread counterculture , before beginning a decline as changing attitudes , the loss of some key individuals and a back-to</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Sandwich Day = " Sandwich Day " is the fourteenth episode of the second season of 30 Rock and the thirty-fifth episode overall . It was written by one of the season 's executive producers , Robert Carlock , and one of the season 's co-executive producers , Jack Burditt . The episode was directed by one of the season 's producers , Don Scardino . The episode first aired on May 1 , 2008 on the NBC network in the United States . Guest stars in this episode included Bill Cwikowski , Brian Dennehy , Marceline Hugot , Johnnie May , Jason Sudeikis , Miriam Tolan and Rip Torn . The episode earned Tina Fey the Primetime Emmy Award for Outstanding Lead Actress in a Comedy Series . Unusually this episode begins on the 30 Rock title sequence - there is no cold open as is normally the case . This episode begins on the annual TGS with Tracy Jordan ( a fictional sketch comedy series ) Sandwich Day . Liz Lemon ( Tina Fey ) receives a phone call from her ex-boyfriend , Floyd ( Jason Sudeikis ) , asking</t>
+          <t xml:space="preserve">The Beatles ( album ) = The Beatles , also known as the White Album , is the ninth studio album by English rock group the Beatles , released on 22 November 1968 . A double album , its plain white sleeve has no graphics or text other than the band 's name embossed , and was intended as a direct contrast to the vivid cover artwork of the band 's earlier Sgt. Pepper 's Lonely Hearts Club Band . Although no singles were issued from The Beatles in Britain and the United States , the songs " Hey Jude " and " Revolution " originated from the same recording sessions and were issued on a single in August 1968 . The album 's songs range in style from British blues and ska to tracks influenced by Chuck Berry and by Karlheinz Stockhausen . Most of the songs on the album were written during March and April 1968 at a Transcendental Meditation course in Rishikesh , India . The group returned to EMI Studios in May with recording lasting through to October . During these sessions , arguments broke out </t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>A Benihana Christmas = " A Benihana Christmas " is the tenth and eleventh episode of the third season of the American comedy television series The Office , and the thirty-eighth and thirty-ninth episode overall . It was written by Jennifer Celotta and directed by Harold Ramis . The episode originally aired in the United States on December 14 , 2006 , on NBC . In the episode , Christmas time at the office leads to depression for Michael , when his girlfriend Carol ( Steve Carell 's wife , Nancy Walls ) breaks up with him . Michael , Andy , Dwight , and Jim then go to a local Benihana restaurant , where Michael and Andy find dates with two of the restaurant 's waitresses . Back at the office , after a conflict with a bossy Angela , Karen and Pam decide to create their own Christmas party . When the majority of the office decide to go to Karen and Pam 's party , Angela becomes upset , and seeing this , Karen and Pam decide to combine the parties . Soon after , Michael and Andy 's dates le</t>
+          <t>Psychedelic music = Psychedelic music ( sometimes psychedelia ) covers a range of popular music styles and genres influenced by the 1960s psychedelic culture , a subculture of people who used psychedelic drugs such as LSD , psilocybin mushrooms , mescaline and DMT to experience visual and auditory hallucinations , synesthesia and altered states of consciousness . Psychedelic music attempted to replicate the hallucinogenic experience of using these drugs or enhance the experience of using them . Psychedelic music emerged during the mid-1960s among folk rock and blues rock bands in the United States and Britain . Psychedelic bands often drew on non-Western sources such as the ragas , drones and sitars of Indian music and they used electric instruments and electronic effects – notably the lead electric guitar played with heavy distortion – and new , unorthodox recording techniques , such as playing tapes backwards or panning the music from one side to the other . Psychedelic influences sp</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Ben Franklin ( The Office ) = " Ben Franklin " is the fifteenth episode of the third season of the American comedy television series The Office , and the show 's forty-third episode overall . Written by Mindy Kaling , who also acts in the show as Kelly Kapoor , and directed by Randall Einhorn , the episode first aired in the United States on February 1 , 2007 on NBC . " Ben Franklin " received 5.0 / 13 in the ages 18 – 49 demographic of the Nielsen ratings , and was watched by an estimated audience of 10.1 million viewers , and the episode received mixed reviews among critics . In the episode , the employees from the office prepare for Phyllis 's wedding . Michael , acting under advice from Todd , instructs Dwight to hire a stripper for the men and delegates Jim to hire one for the women . While Dwight hires a stripper , Jim ends up hiring a Ben Franklin impersonator instead . = = Plot = = The office plays host to a bridal shower for Phyllis Lapin ( Phyllis Smith ) while Bob Vance 's (</t>
+          <t>Ballad of Sir Frankie Crisp ( Let It Roll ) = " Ballad of Sir Frankie Crisp ( Let It Roll ) " is a song by English musician George Harrison , released on his 1970 triple album All Things Must Pass . Harrison wrote the song as a tribute to Frank Crisp , a nineteenth-century lawyer and the original owner of Friar Park – the Victorian Gothic residence in Henley-on-Thames , Oxfordshire , that Harrison purchased in early 1970 . Commentators have likened the song to a cinematic journey through the grand house and the grounds of the estate . The recording features backing from musicians such as Pete Drake , Billy Preston , Gary Wright , Klaus Voormann and Alan White . It was co-produced by Phil Spector , whose heavy use of reverb adds to the ethereal quality of the song . AllMusic critic Scott Janovitz describes " Ballad of Sir Frankie Crisp ( Let It Roll ) " as offering " a glimpse of the true George Harrison – at once mystical , humorous , solitary , playful , and serious " . Crisp 's eccen</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>The Aftermath ( 30 Rock ) = " The Aftermath " is the second episode of the first season of the American situation comedy 30 Rock , which first aired on October 17 , 2006 on CTV in Canada . It aired on October 18 , 2006 on the NBC network in the United States , its country of origin , and October 18 , 2007 in the United Kingdom . The episode was written by Tina Fey and was directed by Adam Bernstein . Guest stars in this episode include Katrina Bowden , Tom Broecker , Teddy Coluca , Rachel Dratch , Adrienne Frost , Maulik Pancholy , Keith Powell , Lonny Ross , Kevin Scanlon and Sorab Wadia . The episode focuses on the reaction of the crew to the casting of Tracy Jordan ( Tracy Morgan ) , and the subsequent changes made to The Girlie Show . This becomes evident when Jack Donaghy ( Alec Baldwin ) changes the title of the show to TGS with Tracy Jordan , much to Jenna Maroney 's ( Jane Krakowski ) dismay . Liz Lemon ( Tina Fey ) struggles to keep the cast and crew happy , so together with T</t>
+          <t xml:space="preserve">The Notorious Byrd Brothers = The Notorious Byrd Brothers is the fifth album by the American rock band The Byrds and was released in January 1968 on Columbia Records ( see 1968 in music ) . Musically , the album represents the pinnacle of The Byrds ' psychedelic experimentation , with the band blending together elements of folk rock , psychedelic rock , country music , electronic music , baroque pop and jazz on many of the songs . Of these disparate styles , the subtle country and western influences evident on a number of tracks pointed towards the full-blown country rock direction that the band would pursue on their next album . In addition , The Notorious Byrd Brothers saw the band and record producer Gary Usher making extensive use of a number of studio effects and production techniques , including phasing , flanging , and spatial panning . The Byrds also introduced the sound of the pedal steel guitar and the Moog modular synthesizer into their music for the first time on the album </t>
         </is>
       </c>
     </row>
@@ -1106,32 +1106,32 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>['oxford', 'cambridge', 'race', 'boat', 'blues', 'rowed', 'rowing', 'lengths', 'crews', 'rower', 'thames', 'races', 'crew', 'universities', 'university_of_cambridge']</t>
+          <t>['song', 'video', 'number', 'like', 'performance', 'tour', 'music', 'madonna', 'performed', 'best', 'songs', 'stage', 'beyoncé', 'week', 'gaga']</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>The Boat Race 1873 = The 30th Boat Race took place on the 29 March 1873 . The Boat Race is an annual side-by-side rowing race between crews from the Universities of Oxford and Cambridge along the River Thames . In a race umpired by former Oxford rower Joseph William Chitty , Cambridge won by three lengths in a time of 19 minutes and 35 seconds , the fastest time in the history of the event . It was the first time that rowers raced on sliding seats . = = Background = = The Boat Race is a side-by-side rowing competition between the University of Oxford ( sometimes referred to as the " Dark Blues " ) and the University of Cambridge ( sometimes referred to as the " Light Blues " ) . The race was first held in 1829 , and since 1845 has taken place on the 4.2-mile ( 6.8 km ) Championship Course on the River Thames in southwest London . Cambridge went into the race as reigning champions , having defeated Oxford by two lengths in the previous year 's race , while Oxford led overall with sixtee</t>
+          <t>Femme Fatale Tour = The Femme Fatale Tour was the eighth concert tour by American recording artist Britney Spears . It was launched in support of her seventh studio album Femme Fatale ( 2011 ) . It was officially announced in March 2011 , with dates for North American venues revealed . The tour was initially planned as a co-headlining tour with Enrique Iglesias , but he canceled only hours after the announcement . The show is inspired by the concept of the femme fatale and femmes fatales throughout the ages . The setlist was mostly composed of songs from Femme Fatale , although Spears also performed hits from her previous albums for her fans . Fashion designer Zaldy Goco created the costumes . In July 2011 , Spears announced plans of playing a South American leg in territories she either had never been to or had not played for a long time . Spears has named the Femme Fatale Tour the best show of her career . The tour , divided in five segments , portrays a story in which Spears is a se</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve">The Boat Race 1879 = The 36th Boat Race took place on 5 April 1879 . The Boat Race is an annual side-by-side rowing race between crews from the Universities of Oxford and Cambridge along the River Thames . Each crew contained four Blues . In a race umpired by former Oxford rower Joseph William Chitty , Cambridge led all the way , and won by a margin of three lengths in a time of 21 minutes 18 seconds . The victory took the overall record to 18 – 17 in Oxford 's favour . = = Background = = The Boat Race is a side-by-side rowing competition between the University of Oxford ( sometimes referred to as the " Dark Blues " ) and the University of Cambridge ( sometimes referred to as the " Light Blues " ) . The race was first held in 1829 , and since 1845 has taken place on the 4.2-mile ( 6.8 km ) Championship Course on the River Thames in southwest London . Cambridge went into the race as reigning champions having won the previous year 's race by ten lengths . However Oxford held the overall </t>
+          <t>Dream Within a Dream Tour = The Dream Within a Dream Tour was the fourth concert tour by American recording artist Britney Spears . It was launched in support of her third studio album , Britney ( 2001 ) . The tour was promoted by Concerts West , marking the first time Spears did not tour with Clear Channel Entertainment . On September 21 , 2001 , a North American tour was announced that kicked off exactly two months later after various dates were postponed . In February 2002 , Spears announced a second leg of the tour . It was directed and choreographed by Wade Robson , who explained the main theme of the show was Spears 's coming of age and newfound independence . The stage was designed by Steve Cohen and Rob Brenner and was composed of a main stage and a B-stage , united by a runway . Inspired by Cleopatra 's barge , a flying device was developed so Spears could travel over the audience to the B-stage . The setlist was mostly composed by songs from the supporting album , as Spears f</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>The Boat Race 1882 = The 39th Boat Race took place on 1 April 1882 . The Boat Race is an annual side-by-side rowing race between crews from the Universities of Oxford and Cambridge along the River Thames . In the race , umpired by former Cambridge rower Robert Lewis-Lloyd , Oxford won by a margin of seven lengths in a time of 20 minutes 12 seconds , taking the overall record to 21 – 17 in their favour . = = Background = = The Boat Race is an annual rowing eight competition between the University of Oxford and the University of Cambridge . First held in 1829 , the competition is a 4.2-mile ( 6.8 km ) race along The Championship Course on the River Thames in southwest London . The rivalry is a major point of honour between the two universities and followed throughout the United Kingdom and worldwide . Oxford went into the race as reigning champions having won the previous year 's race by three lengths , and held the overall lead , with 20 victories to Cambridge 's 17 ( excluding the " de</t>
+          <t>The Onyx Hotel Tour = The Onyx Hotel Tour was the fifth concert tour by American recording artist Britney Spears . It showcased her fourth studio album , In the Zone ( 2003 ) and visited North America and Europe . A tour to promote the album was announced in December 2003 . Its original name was the In the Zone Tour , but Spears was sued for trademark infringement and banned from using the name . Spears felt inspired to create a show with a hotel theme which she later mixed with the concept of an onyx stone . The stage , inspired by Broadway musicals , was less elaborate than her previous tours . The setlist was composed mostly by songs from In the Zone as well as some of her past songs reworked with different elements of jazz , blues and Latin percussion . Tour promoter Clear Channel Entertainment marketed the tour to a more adult audience than her previous shows while sponsor MTV highly promoted the tour on TV shows and the network 's website . The tour was divided into seven segment</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t xml:space="preserve">The Boat Race 1889 = The 46th Boat Race took place on 30 March 1889 . The Boat Race is an annual side-by-side rowing race between crews from the Universities of Oxford and Cambridge along the River Thames . For the first time in the history of the event , all eight rowers in the Cambridge crew had rowed the previous year . Cambridge won by three lengths in a time of 20 minutes 14 seconds , their fourth consecutive victory which took the overall record in the event to 23 – 22 in Oxford 's favour . = = Background = = The Boat Race is a side-by-side rowing competition between the University of Oxford ( sometimes referred to as the " Dark Blues " ) and the University of Cambridge ( sometimes referred to as the " Light Blues " ) . First held in 1829 , the race takes place on the 4.2 miles ( 6.8 km ) Championship Course on the River Thames in southwest London . The rivalry is a major point of honour between the two universities ; it is followed throughout the United Kingdom and as of 2014 , </t>
+          <t xml:space="preserve">Ghosttown ( Madonna song ) = " Ghosttown " is a song recorded by American singer Madonna for her thirteenth studio album , Rebel Heart ( 2015 ) . It was released to radio stations on March 13 , 2015 , as the album 's second single . The song was written by Madonna , Jason Evigan , Evan Bogart , and Sean Douglas , and produced by Madonna , Billboard and Evigan . Madonna had listened to Douglas 's previous works and had requested studio time with him . Together with the other songwriters , they wrote " Ghosttown " in three days . A pop ballad , the song was inspired by the imagery of a destructed city after armageddon , and how the survivors carry on with their lives , with love being the only thing they can hold onto . Composed as an uplifting track , " Ghosttown " features instrumentation from organ and drums , with minor vocoder effects on Madonna 's vocals . " Ghosttown " was released to iTunes Store as part of the album 's pre-order in December 2014 , in response to hackers leaking </t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>The Boat Race 1872 = The 29th Boat Race took place on the 27 March 1872 . The Boat Race is an annual side-by-side rowing race between crews from the Universities of Oxford and Cambridge along the River Thames . In a race umpired by Robert Lewis-Lloyd , Cambridge won by two lengths in a time of 21 minutes 15 seconds taking the overall record to 16 – 13 in Oxford 's favour . = = Background = = The Boat Race is a side-by-side rowing competition between the University of Oxford ( sometimes referred to as the " Dark Blues " ) and the University of Cambridge ( sometimes referred to as the " Light Blues " ) . The race was first held in 1829 , and since 1845 has taken place on the 4.2-mile ( 6.8 km ) Championship Course on the River Thames in southwest London . Cambridge went into the race as reigning champions , having defeated Oxford by one length in the previous year 's race , while Oxford led overall with sixteen wins to Cambridge 's twelve . During the build-up to the race , Oxford 's boa</t>
+          <t>Scream &amp; Shout = " Scream &amp; Shout " is a song by American recording artists will.i.am and Britney Spears , taken from the former 's fourth studio album # willpower . It was released on November 20 , 2012 by Interscope Records as the second single from the album , and sent to mainstream radio in the United States on November 27 . The song was written by will.i.am , Jef Martens and Jean Baptiste and was produced by Martens under the alias Lazy Jay , with additional production by will.i.am. " Scream &amp; Shout " is an upbeat dance-pop song ; its lyrics are about having a good time on a night out . It interpolates a sample of the lyric " Britney , bitch " , which was used on Spears ' 2007 single " Gimme More " . " Scream &amp; Shout " received mixed reviews from music critics . Some critics described the song as a dark club track , but others criticized the use of Auto-Tune on the vocals . The song was a commercial success worldwide , topping the charts in over 24 countries and reached the top te</t>
         </is>
       </c>
     </row>
@@ -1141,32 +1141,32 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>['women', 'party', 'police', 'labour', 'book', 'rights', 'suffrage', 'government', 'feminist', 'political', 'feminism', 'murder', 'case', 'minister', 'trial']</t>
+          <t>['class', 'built', 'main', 'guns', 'line', 'castle', 'new', 'service', 'use', 'long', 'locomotives', 'london', 'speed', 'intended', 'locomotive']</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Free Expression Policy Project = The Free Expression Policy Project ( FEPP ) is an organization devoted to assisting researchers with assembling information related to freedom of speech , media democracy , and copyright , and advocating for these issues . Civil liberties lawyer Marjorie Heins founded the nonprofit organization in 2000 . Based in Manhattan , New York , it was initially associated with the National Coalition Against Censorship , and subsequently operated as part of the Democracy Program of the Brennan Center for Justice at New York University Law School . The FEPP conducted a survey in 2001 which revealed that online monitoring software , including Net Nanny , SurfWatch , and Cybersitter , cast too broad a net and often blocked legitimate educational websites in their attempts to censor material from youths . In 2003 , the organization assisted 33 academics in filing a friend-of-the-court brief challenging a law which restricted the sale of violent video games to minors </t>
+          <t xml:space="preserve">Rail transport in Victoria = Rail transport in Victoria , Australia , is provided by a number of railway operators who operate over the government-owned railway lines . Victorian lines use 5 ft 3 in ( 1,600 mm ) broad gauge , with the exception of a number of standard gauge 4 ft 8 1 ⁄ 2 in ( 1,435 mm ) freight and interstate lines , a few experimental 2 ft 6 in ( 762 mm ) narrow gauge lines , and various private logging , mining and industrial railways . Railways were privately owned and operated , until the State Government established the vertically integrated Victorian Railways in 1883 . This remained until corporatisation occurred in the 1980s , followed by privatisation in the 1990s . Passenger services today are operated by Metro Trains Melbourne in suburban Melbourne with electric multiple units , and V / Line in regional Victoria with diesel trains . Freight services are operated by Aurizon ( interstate ) , Pacific National and SCT Logistics ( interstate and intrastate ) , and </t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Weiquan movement = The Weiquan movement is a non-centralized group of lawyers , legal experts , and intellectuals in China who seek to protect and defend the civil rights of the citizenry through litigation and legal activism . The movement , which began in the early 2000s , has organized demonstrations , sought reform via the legal system and media , defended victims of human rights abuses , and written appeal letters , despite opposition from Communist Party authorities . Among the issues adopted by Weiquan lawyers are property and housing rights , protection for AIDS victims , environmental damage , religious freedom , freedom of speech and the press , and defending the rights of other lawyers facing disbarment or imprisonment . Individuals involved in the Weiquan movement have met with occasionally harsh reprisals from Chinese officials , including disbarment , detention , harassment , and , in extreme instances , torture . Authorities have also responded to the movement with the l</t>
+          <t>McDonnell Douglas F-4 Phantom II in UK service = The United Kingdom operated the McDonnell Douglas F-4 Phantom II as one of its principal combat aircraft from the 1960s to the early 1990s . The UK was the first export customer for the Phantom , which was ordered in the context of political and economic difficulties around indigenous British designs for the roles that it was eventually purchased to undertake . The Phantom was procured to serve in both the Fleet Air Arm and Royal Air Force in several roles including air defence , close air support , low-level strike and tactical reconnaissance . Although assembled in the United States , the UK 's Phantoms were a special batch built separately and containing a significant amount of British technology as a means of easing the pressure on the domestic aerospace industry in the wake of major project cancellations . Two individual variants were eventually built for the UK ; the F-4K variant was designed from the outset as an air defence inter</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Azimzhan Askarov = Azimzhan Askarov ( Uzbek : Azimjon Asqarov , Азимжон Асқаров ; born 1951 ) is an ethnically Uzbek Kyrgyzstani political activist who founded the group Vozduh in 2002 to investigate police brutality . During the 2010 South Kyrgyzstan ethnic clashes , which primarily targeted people of the Uzbek nationality , Askarov worked to document the violence . He was subsequently arrested and prosecuted on charges of creating mass disturbances , incitement of ethnic hatred , and complicity in murder . Following a trial protested by several international human rights groups for irregularities — including alleged torture and the courtroom intimidation of witnesses by police — Askarov was given a life sentence , which he is currently serving . In November 2010 , Askarov 's health was reported to be rapidly deteriorating as a result of his confinement . Numerous groups have advocated on his behalf , including Human Rights Watch , Reporters Without Borders , People In Need , the Comm</t>
+          <t>Anglesey Central Railway = The Anglesey Central Railway ( Welsh : Lein Amlwch , Amlwch Line ) was a 17.5 miles ( 28.2 km ) long standard-gauge railway in Anglesey , Wales , connecting the port of Amlwch and the county town of Llangefni with the North Wales Coast Line at Gaerwen . Built as an independent railway , the railway opened in portions from 1864 to 1867 . Due to financial troubles the railway was sold to the London and North Western Railway in 1876 , who invested significantly in the infrastructure . Operation continued under various companies during the 20th century , but passenger services were withdrawn in 1964 as part of the Beeching Axe . Industrial freight services continued until 1993 . The railway 's tracks have been left in situ , and local groups have demonstrated an interest in restoring services ( possibly as a heritage railway ) . The sustainable transport charity Sustrans has proposed to use the route as a cycle path . The Welsh Assembly Government , in partnershi</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>New Labour = New Labour refers to a period in the history of the British Labour Party from the mid-1990s to the early 2010s , under leaders Tony Blair and Gordon Brown . The name dates from a conference slogan first used by the party in 1994 which was later seen in a draft manifesto published in 1996 , called New Labour , New Life For Britain . It was presented as the brand of a newly reformed party that had altered Clause IV and endorsed market economics . The branding was extensively used while the party was in government , between 1997 and 2010 . New Labour won landslide election victories in 1997 and 2001 , and won again in 2005 . In 2007 , Blair resigned as the party 's leader and was succeeded by Gordon Brown . Labour lost the 2010 general election , which resulted in a hung parliament and led to the creation of a Conservative – Liberal Democrat coalition government ; Gordon Brown resigned as Prime Minister , and as Labour leader shortly thereafter . He was succeeded by Ed Miliba</t>
+          <t>Gangut-class battleship = The Gangut-class battleships , also known as the " Sevastopol class " , were the first dreadnoughts begun for the Imperial Russian Navy before World War I. They had a convoluted design history involving several British companies , evolving requirements , an international design competition , and foreign protests . Four ships were ordered in 1909 ; two were named after victorious battles of Peter the Great in the Great Northern War and the other two were named after battles in the Crimean War . Three ships of the class used names of pre-dreadnought battleships of the Petropavlovsk-class lost in the Russo-Japanese War . Construction was delayed by financing problems until the Duma formally authorized the ships in 1911 . They were delivered from December 1914 through January 1915 , although they still needed work on the turrets and fire-control systems until mid-1915 . Their role was to defend the mouth of the Gulf of Finland against the Germans , who never tried</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Feminism in India = Feminism in India is a set of movements aimed at defining , establishing , and defending equal political , economic , and social rights and equal opportunities for Indian women . It is the pursuit of women 's rights within the society of India . Like their feminist counterparts all over the world , feminists in India seek gender equality : the right to work for equal wages , the right to equal access to health and education , and equal political rights . Indian feminists also have fought against culture-specific issues within India 's patriarchal society , such as inheritance laws and the practice of widow immolation known as Sati . The history of feminism in India can be divided into three phases : the first phase , beginning in the mid-nineteenth century , initiated when male European colonists began to speak out against the social evils of Sati ; the second phase , from 1915 to Indian independence , when Gandhi incorporated women 's movements into the Quit India </t>
+          <t>Fairchild Republic A-10 Thunderbolt II = The Fairchild Republic A-10 Thunderbolt II is a single seat , twin turbofan engine , straight wing jet aircraft developed by Fairchild-Republic for the United States Air Force . Commonly referred to by its nicknames " Warthog " or " Hog " , its official name comes from the Republic P-47 Thunderbolt , a fighter particularly effective at close air support . The A-10 was designed for close-in support of ground troops , close air support ( CAS ) , providing quick-action support for troops against helicopters , vehicles , and ground troops . It entered service in 1976 and is the only production-built aircraft that has served in the USAF that was designed solely for CAS . Its secondary mission is to provide forward air controller - airborne ( FAC-A ) support , by directing other aircraft in attacks on ground targets . Aircraft used primarily in this role are designated OA-10 . The A-10 was intended to improve on the performance of the A-1 Skyraider an</t>
         </is>
       </c>
     </row>
@@ -1176,32 +1176,32 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>['officer', 'commander', 'lieutenant', 'command', 'fighter', 'promoted', 'victories', 'war', 'aircraft', 'flying', 'squadron', 'enemy', 'rank', 'medal', 'training']</t>
+          <t>['cap', 'fruit', 'color', 'shaped', 'spores', 'bodies', 'fungus', 'stem', 'mushroom', 'spore', 'taxonomy', 'yellow', 'diameter', 'collected', 'gill']</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Neville McNamara = Air Chief Marshal Sir Neville Patrick McNamara , KBE , AO , AFC , AE ( 17 April 1923 – 7 May 2014 ) was a senior commander of the Royal Australian Air Force ( RAAF ) . He served as Chief of the Air Staff ( CAS ) , the RAAF 's highest-ranking position , from 1979 until 1982 , and as Chief of the Defence Force Staff ( CDFS ) , Australia 's top military role at the time , from 1982 until 1984 . He was the second RAAF officer to hold the rank of air chief marshal . Born in Queensland , McNamara joined the RAAF during World War II and saw action in the South West Pacific , flying P-40 Kittyhawks . He also flew combat missions in Gloster Meteors during the Korean War . In 1961 , he was awarded the Air Force Cross for his leadership of No. 2 Operational Conversion Unit . He gained further operational experience heading the RAAF presence in Ubon , Thailand , in the late 1960s . Promoted to air commodore , McNamara was Commander RAAF Forces Vietnam , and Deputy Commander Aust</t>
+          <t>Mycena overholtsii = Mycena overholtsii , commonly known as the snowbank fairy helmet or fuzzy foot , is a species of fungus in the family Mycenaceae . The mushrooms produced by the fungus are relatively large for the genus Mycena , with convex grayish caps up to 5 cm ( 2.0 in ) in diameter and stems up to 15 cm ( 5.9 in ) long . The gills on the underside of the cap are whitish to pale gray , and initially closely spaced before becoming well-spaced at maturity after the cap enlarges . The mushrooms are characterized by the dense covering of white " hairs " on the base of the stem . M. overholtsii is an example of a snowbank fungus , growing on well-decayed conifer logs near snowbanks , during or just after snowmelt . Formerly known only from high-elevation areas of western North America , particularly the Rocky Mountain and Cascade regions , it was reported for the first time in Japan in 2010 . The edibility of the mushroom is unknown . M. overholtsii can be distinguished from other c</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Richard Barrons = General Sir Richard Lawson Barrons KCB , CBE , ADC Gen ( born 17 May 1959 ) is a retired British Army officer . He was Commander Joint Forces Command from April 2013 until his retirement in April 2016 . Barrons ' early career was spent in various staff and field posts in the UK , across Europe , and in the Far East . He also spent time working at the Ministry of Defence and in education . Sent to Germany in 1991 , Barrons then served his first tour of duty in the Balkans in 1993 . Returning to the UK , Barrons took up a staff position and went on to do a tour in Northern Ireland and then to become a Military Assistant , first to the High Representative for Bosnia and Herzegovina and then to the Chief of the General Staff . Between 2000 and 2003 , Barrons served again in the Balkans , in Afghanistan during the early days of International Security Assistance Force , and then in a staff position in Basra , Iraq . As a brigadier in 2003 , Barrons served his second tour in</t>
+          <t>Harrya chromapes = Harrya chromapes , commonly known as the yellowfoot bolete or the chrome-footed bolete , is species of bolete fungus in the family Boletaceae . The bolete is found in eastern North America , Costa Rica , and eastern Asia , where it grows on the ground , in a mycorrhizal association with deciduous and coniferous trees . Fruit bodies have smooth , rose-pink caps that are initially convex before flattening out . The pores on the cap undersurface are white , aging to a pale pink as the spores mature . The thick stipe has fine pink or reddish dots ( scabers ) , and is white to pinkish but with a bright yellow base . The mushrooms are edible but are popular with insects , and so they are often infested with maggots . In its taxonomic history , Harrya chromapes has been shuffled to several different genera , including Boletus , Leccinum , and Tylopilus , and is known in field guides as a member of one of these genera . In 2012 , it was transferred to the newly created genus</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>John Emilius Fauquier = Air Commodore John Emilius " Johnny " Fauquier DSO &amp; Two Bars , DFC ( March 19 , 1909 – April 3 , 1981 ) was a Canadian aviator and Second World War Bomber Command leader . He commanded No. 405 Squadron RCAF and later No. 617 Squadron RAF ( the Dambusters ) over the course of the war . A bush pilot , prior to the war , he joined the Royal Canadian Air Force as a flight instructor in 1939 . He then joined 405 Squadron in 1941 and would fly operationally for the rest of the war , taking a drop in rank on one occasion to return to active command . During his three tours of operation he participated in Operation Hydra and dozens of other sorties over Europe . = = Early years = = John Emilius " Johnny " Fauquier was born at Ottawa , Ontario on March 19 , 1909 , educated at Ashbury College and then entered the investment business at Montreal , Quebec where he joined a flying club . After earning his commercial pilot 's licence he formed Commercial Airways at Noranda ,</t>
+          <t>Lepiota babruzalka = Lepiota babruzalka is an agaric mushroom of the genus Lepiota in the order Agaricales . Described as new to science in 2009 , it is found in Kerala State , India , where it grows on the ground in litterfall around bamboo stems . Fruit bodies have caps that measure up to 1.3 cm ( 0.5 in ) in diameter , and are covered with reddish-brown scales . The cap is supported by a long and slender stem up to 4.5 cm ( 1.8 in ) long and 1.5 millimetres ( 0.1 in ) thick . One of the distinguishing microscopic features of the species is the variably shaped cystidia found on the edges of the gills . = = Taxonomy = = The species was first described by Arun Kumar Thirovoth Kottuvetta and P. Manimohan in the journal Mycotaxon in 2009 , in a survey of the genus Lepiota in Kerala State in southern India . The holotype collection was made in 2004 in Chelavur , located in the Kozhikode District ; it is now kept in the herbarium of Kew Gardens . The specific epithet babruzalka derives fro</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Jean-Marie Defrance = Jean-Marie Defrance ( 1771 – 1855 ) was a French General of the French Revolutionary Wars and the Napoleonic Wars . He was also a member of the Council of Five Hundred ( the lower house of the legislative branch of the French government under The Directory ) , and a teacher at the military school of Rebais , Champagne . Defrance had an extensive and successful military career in the French Revolutionary Wars and the Napoleonic Wars . After the First Battle of Zurich , he refused a battlefield promotion to brigadier general , asking instead for a cavalry regiment ; he received command of the 12th Regiment of Chasseurs-a-Cheval ( light cavalry ) as Chef-de-Brigade , a rank equivalent to colonel . He led this brigade in the campaigns of 1799 – 1800 in southwestern Germany and northern Italy . By 1805 , he had been promoted to brigadier general . At the Battle of Austerlitz and the Battle of Jena-Auerstadt , he commanded a cavalry brigade of carabiniers in Étienne Mar</t>
+          <t>Leucopholiota decorosa = Leucopholiota decorosa is a species of fungus in the Tricholomataceae family of mushrooms . Commonly known as the decorated Pholiota , it is distinguished by its fruit body which is covered with pointed brown , curved scales on the cap and stem , and by its white gills . Found in the eastern United States , France , and Pakistan , it is saprobic , growing on the decaying wood of hardwood trees . L. decorosa was first described by American mycologist Charles Horton Peck as Agaricus decorosus in 1873 , and the species has been transferred to several genera in its history , including Tricholoma , Tricholomopsis , Armillaria , and Floccularia . Three American mycologists considered the species unique enough to warrant its own genus , and transferred it into the new genus Leucopholiota in a 1996 publication . Lookalike species with similar colors and scaly fruit bodies include Pholiota squarrosoides , Phaeomarasmius erinaceellus , and Leucopholiota lignicola . L. de</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Humfrey Gale = Lieutenant General Sir Humfrey Myddelton Gale KBE , CB , CVO , MC ( 4 October 1890 – 8 April 1971 ) was an officer in the British Army who served in the First and Second World War , during which he was Chief Administrative Officer at Allied Forces Headquarters and later SHAEF under General of the Army Dwight Eisenhower . After the Second World War he was European Director of the United Nations Relief and Rehabilitation Administration , worked for the Anglo-Iranian Oil Company , and was chairman of the Basildon , Essex New Town Development Corporation = = Early life = = Humfrey Myddelton Gale was born in London , England on 4 October 1890 , the eldest of five children of Ernest Sewell Gale , an architect , and his wife Charlotte Sarah née Goddard . He was educated at St Paul 's School , London and studied at the Architectural School , Westminster from 1908 to 1910 . While there he served with the Artists Rifles . He decided to pursue a career in the British Indian Army an</t>
+          <t xml:space="preserve">Pholiota flammans = Pholiota flammans , commonly known as the yellow pholiota , the flaming Pholiota , or the flame scalecap , is a basidiomycete agaric mushroom of the genus Pholiota . Its fruit body is golden-yellow in color throughout , while its cap and stem are covered in sharp scales . As it is a saprobic fungus , the fruit bodies typically appear in clusters on the stumps of dead coniferous trees . P. flammans is distributed throughout Europe , North America , and Asia in boreal and temperate regions . Its edibility has not been clarified . = = Taxonomy = = This species was first recognised in 1783 by the German , August Batsch , as Agaricus flammans , and later sanctioned by Swedish mycologist Elias Magnus Fries in his Systema Mycologicum . The specific epithet flammans is a Latin adjective meaning flaming . In 1871 , with the recognition of Pholiota as an independent genus with type species Pholiota squarrosa , another German , Paul Kummer renamed the fungus Pholiota flammans </t>
         </is>
       </c>
     </row>
@@ -1211,32 +1211,32 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>['breed', 'horses', 'horse', 'breeds', 'dog', 'dogs', 'arabian', 'bred', 'breeding', 'stud', 'stallion', 'breeders', 'pony', 'registered', 'hair']</t>
+          <t>['episode', 'mulder', 'plot', 'find', 'scully', 'nielsen', 'doctor', 'files', 'scene', 'david_duchovny', 'finds', 'x-files', 'filmed', 'dana_scully', 'enterprise']</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Heck horse = The Heck horse is a horse breed that is claimed to resemble the tarpan ( Equus ferus ferus ) , an extinct wild equine . The breed was created by the German zoologist brothers Heinz Heck and Lutz Heck in an attempt to breed back the tarpan . Although unsuccessful at creating a genetic copy of the extinct species , they developed a breed with grullo coloration and primitive markings . After the Nazi invasion of Poland , they were introduced to the Białowieża Forest , where a small herd still survives . Heck horses were subsequently exported to the United States , where a breed association was created in the 1960s . = = Breed characteristics = = Heck horses are dun or grullo ( a dun variant ) in color , with no white markings . The breed has primitive markings , including a dorsal stripe and horizontal striping on the legs . Heck horses generally stand between 12.2 and 13.2 hands ( 50 and 54 inches , 127 and 137 cm ) tall . The head is large , the withers low , and the legs a</t>
+          <t>Field Trip ( The X-Files ) = " Field Trip " is the twenty-first episode of the sixth season of the science fiction television series The X-Files . It premiered on the Fox network on May 9 , 1999 in the United States and Canada , and subsequently aired in the United Kingdom on Sky1 on July 18 . The episode was written by John Shiban and Vince Gilligan , from a story by Frank Spotnitz , and was directed by Kim Manners . The episode is a " Monster-of-the-Week " story , unconnected to the series ' wider mythology . " Field Trip " earned a Nielsen household rating of 9.5 , being watched by 15.40 million people in its initial broadcast . The episode received largely positive reviews from television critics . The show centers on FBI special agents Fox Mulder ( David Duchovny ) and Dana Scully ( Gillian Anderson ) who work on cases linked to the paranormal , called X-Files . Mulder is a believer in the paranormal , while the skeptical Scully has been assigned to debunk his work . In the episod</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Florida Cracker Horse = The Florida Cracker Horse is a breed of horse from Florida in the United States . It is genetically and physically similar to many other Spanish-style horses , especially those from the Spanish Colonial Horse group . The Florida Cracker is a gaited breed known for its agility and speed . The Spanish first brought horses to Florida with their expeditions in the early 16th century ; as colonial settlement progressed , they used the horses for herding cattle . These horses developed into the Florida Cracker type seen today , and continued to be used by Florida cowboys ( known as " crackers " ) until the 1930s . At this point they were superseded by American Quarter Horses needed to work larger cattle brought to Florida during the Dust Bowl , and population numbers declined precipitously . Through the efforts of several private families and the Florida government , the breed was saved from extinction , but there is still concern about its low numbers . Both The Live</t>
+          <t>Sein und Zeit ( The X-Files ) = " Sein und Zeit " is the tenth episode of the seventh season of the science fiction television series The X-Files . It premiered on the Fox network on February 6 , 2000 , in the United States . The episode was written by Chris Carter and Frank Spotnitz , and directed by Michael Watkins . The episode helped to explore the series ' overarching mythology . " Sein und Zeit " earned a Nielsen household rating of 8.4 , being watched by 13.95 million people in its initial broadcast . It received mixed to positive reviews from critics . The show centers on FBI special agents Fox Mulder ( David Duchovny ) and Dana Scully ( Gillian Anderson ) , who work on cases linked to the paranormal , called X-Files . Mulder is a believer in the paranormal , while the skeptical Scully has been assigned to debunk his work . In this episode , Mulder becomes obsessed with a number of children who have vanished while investigating the bizarre disappearance of a young girl from her</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Colorado Ranger = The Colorado Ranger is a horse breed from the Colorado High Plains in the United States . The breed is descended from two stallions imported from Turkey to the US state of Virginia in the late 1800s . These stallions were then bred to ranch horses in Nebraska and Colorado , and in the early 1900s the two stallions who every registered Colorado Ranger traces to , Patches # 1 and Max # 2 , were foaled . The breed was championed by rancher Mike Ruby , who founded the Colorado Ranger Horse Association in 1935 . Original registry membership limits resulted in many Colorado Ranger horses being registered instead as Appaloosas , but pedigree research is ongoing to discover additional horses who trace their ancestry back to the original stallions . By 2005 , more than 6,000 Colorado Ranger horses had been registered . Colorado Rangers may be any solid color or carry leopard spotting patterns . Pinto coloration and American Paint Horse breeding are not allowed , nor are draft </t>
+          <t>The X-Files Mythology , Volume 3 – Colonization = The X-Files Mythology – Volume 3 collection is the third DVD release containing selected episodes from the fifth to the eighth seasons of the American science fiction television series The X-Files . The episodes collected in the release form the middle of the series ' mythology , and are centered on alien colonization efforts , the fall of the Syndicate , and Fox Mulder 's ( David Duchovny ) abduction . The collection contains three episodes from the fifth season , five from the sixth , six from the seventh , and two from the eighth . The episodes follow the investigations of paranormal-related cases , or X-Files , by FBI Special Agents Fox Mulder and Dana Scully ( Gillian Anderson ) . Mulder is a believer in the paranormal , while the skeptical Scully has been assigned to debunk his work . Events covered in the episodes include the discovery of alien-human hybrid Cassandra Spender ( Veronica Cartwright ) , the destruction of the Syndic</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Kentucky Mountain Saddle Horse = The Kentucky Mountain Saddle Horse is a horse breed from the US state of Kentucky . Developed as an all-around farm and riding horse in eastern Kentucky , they are related to the Tennessee Walking Horse and other gaited breeds . In 1989 the Kentucky Mountain Saddle Horse Association ( KMSHA ) was formed , and in 2002 , the subsidiary Spotted Mountain Horse Association ( SMHA ) was developed to registered Kentucky Mountain Saddle Horses with excessive white markings and pinto patterns . Conformation standards are the same for the two groups of horses , with the main difference being the color requirements . The KMSHA studbook is now closed to horses from unregistered parents , although it cross-registers with several other registries , while the SMHA studbook remains open . = = Characteristics = = Kentucky Mountain Saddle Horses must stand above 11 hands ( 44 inches , 112 cm ) high to be registered . Horses above this height are divided into two categori</t>
+          <t>Empedocles ( The X-Files ) = " Empedocles " is the seventeenth episode of the eighth season of the American science fiction television series The X-Files . It premiered on the Fox network on April 22 , 2001 . The episode was written by Greg Walker and directed by Barry K. Thomas . " Empedocles " is a " Monster-of-the-Week " story , unconnected to the series ' wider mythology . The episode received a Nielsen rating of 7.3 and was viewed by 7.46 million households and over 12.46 million viewers . Overall , the episode received mixed reviews from critics . The show centers on FBI special agents Fox Mulder ( David Duchovny ) , Dana Scully ( Gillian Anderson ) and John Doggett ( Robert Patrick ) , who work on cases linked to the paranormal , called X-Files . In this episode , Monica Reyes ( Annabeth Gish ) enlists Mulder ’ s help investigating a killer ’ s connection to the unsolved murder of Doggett ’ s son , but Mulder soon finds himself clashing with Doggett . " Empedocles " was named af</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Azteca horse = The Azteca is a horse breed from Mexico , with a subtype , called the " American Azteca " , found in the United States . They are well-muscled horses that may be of any solid color , and the American Azteca may also have pinto coloration . Aztecas are known to compete in many western riding and some English riding disciplines . The Mexican registry for the original Azteca and the United States registries for the American Azteca have registration rules that vary in several key aspects , including ancestral bloodlines and requirements for physical inspections . The Azteca was first developed in Mexico in 1972 , from a blend of Andalusian , American Quarter Horse and Mexican Criollo bloodlines . From there , they spread to the United States , where American Paint Horse blood was added . = = Breed characteristics = = The three foundation breeds of the Azteca are the Andalusian ( defined by the Mexican registry as either Pura Raza Española or Lusitano ) , American Quarter Hor</t>
+          <t>The Erlenmeyer Flask = " The Erlenmeyer Flask " is the 24th episode and the first season finale of the science fiction television series The X-Files . Written by executive producer Chris Carter , and directed by R. W. Goodwin , the episode continues with the mythology story arc which started with " Pilot " . The episode first aired in the United States on May 13 , 1994 on the Fox network . With 8.3 million households turning in during its initial broadcast , the episode was the most-viewed episode of the show 's first season . The episode received an Edgar Award nomination in the Best Episode in a TV Series category , and has , since broadcast , received positive responses from both critics and crew members . The show centers on FBI special agents Fox Mulder ( David Duchovny ) and Dana Scully ( Gillian Anderson ) who work on cases linked to the paranormal , called X-Files . In this episode , Mulder and Scully discover evidence of a secret government experimentation with alien DNA , but</t>
         </is>
       </c>
     </row>
@@ -1246,32 +1246,32 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>['british', 'french', 'militia', 'troops', 'fort', 'howe', 'battle', 'frigate', 'spanish', 'men', 'washington', 'fleet', 'expedition', 'continental_army', 'wounded']</t>
+          <t>['son', 'king', 'died', 'brother', 'death', 'daughter', 'father', 'reign', 'royal', 'kings', 'younger', 'succeeded', 'sons', 'kingdom', 'probably']</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Battle of Bonchurch = The Battle of Bonchurch took place sometime in late July 1545 at Bonchurch on the Isle of Wight . No source of information states a specific date , although it could have happened on 21 July . The battle was a part of the wider Italian War of 1542 – 1546 , and took place during the 1545 French invasion of the Isle of Wight . Several landings were made by the French during the invasion of the Isle of Wight , including the one at Bonchurch . The two combatants were the Kingdom of England and the Kingdom of France . England won the battle , and the French advance across the Isle of Wight was halted . The battle was fought between French regular soldiers , and English militiamen . The number of French soldiers involved is believed to be around 500 . The number of English militiamen is uncertain , with one source of information stating 300 , and another stating 2800 . English forces at the battle are understood to have been commanded by Captain Robert Fyssher , whilst </t>
+          <t>Ímar mac Arailt = Ímar mac Arailt ( died 1054 ) was an eleventh-century ruler of the Kingdom of Dublin and perhaps the Kingdom of the Isles . He was the son of a man named Aralt , and appears to have been a grandson of Amlaíb Cuarán , King of Northumbria and Dublin . Such a relationship would have meant that Ímar was a member of the Uí Ímair , and that he was a nephew of Amlaíb Cuarán 's son , Sitriuc mac Amlaíb , King of Dublin , a man driven from Dublin by Echmarcach mac Ragnaill in 1036 . Ímar 's reign in Dublin spanned at least eight years , from 1038 to 1046 . Although he began by seizing the kingship from Echmarcach in 1038 , he eventually lost it to him in 1046 . As king , Ímar is recorded to have overseen military operations throughout Ireland , and seems to have actively assisted the family of Iago ab Idwal ap Meurig , King of Gwynedd overseas in Wales . After Echmarcach 's final expulsion from Dublin 1052 , Ímar may well have been reinstalled as King of Dublin by Diarmait mac</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Boston campaign = The Boston campaign was the opening campaign of the American Revolutionary War , taking place primarily in the Province of Massachusetts Bay . The campaign began with the Battles of Lexington and Concord on April 19 , 1775 , in which the local colonial militias interdicted a British government attempt to seize military stores and leaders in Concord , Massachusetts . The entire British expedition suffered significant casualties during a running battle back to Charlestown against an ever-growing number of militia . Subsequently , accumulated militia forces surrounded the city of Boston , beginning the Siege of Boston . The main action during the siege , the Battle of Bunker Hill on June 17 , 1775 , was one of the bloodiest encounters of the war , an resulted in a Pyrrhic British victory . There were also numerous skirmishes near Boston and the coastal areas of Boston , resulting in loss of life , military supplies , or both . In July 1775 , George Washington took comman</t>
+          <t>Malcolm II of Scotland = Malcolm ( Gaelic : Máel Coluim ; died 25 November 1034 ) , was King of the Scots from 1005 until his death . He was a son of King Kenneth II ; the Prophecy of Berchán says that his mother was a woman of Leinster and refers to him as Forranach , " the destroyer " . To the Irish annals which recorded his death , Malcolm was ard rí Alban , High King of Scotland . In the same way that Brian Bóruma , High King of Ireland , was not the only king in Ireland , Malcolm was one of several kings within the geographical boundaries of modern Scotland : his fellow kings included the king of Strathclyde , who ruled much of the south-west , various Norse-Gael kings on the western coast and the Hebrides and , nearest and most dangerous rivals , the kings or Mormaers of Moray . To the south , in the Kingdom of England , the Earls of Bernicia and Northumbria , whose predecessors as kings of Northumbria had once ruled most of southern Scotland , still controlled large parts of the</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Meigs Raid = The Meigs Raid ( also known as the Battle of Sag Harbor ) was a military raid by American Continental Army forces , under the command of Connecticut Colonel Return Jonathan Meigs , on a British Loyalist foraging party at Sag Harbor , New York on May 24 , 1777 during the American Revolutionary War . Six Loyalists were killed and 90 captured while the Americans suffered no casualties . The raid was made in response to a successful British raid on Danbury , Connecticut in late April that was opposed by American forces in the Battle of Ridgefield . Organized in New Haven , Connecticut by Brigadier General Samuel Holden Parsons , the expedition crossed Long Island Sound from Guilford on May 23 , dragged whaleboats across the North Fork of Long Island , and raided Sag Harbor early the next morning , destroying boats and supplies . The battle marked the first American victory in the state of New York after New York City and Long Island had fallen in the British campaign for the c</t>
+          <t>Ascall mac Ragnaill = Ascall mac Ragnaill meic Torcaill ( died 1171 ) , also known as Ascall Mac Torcaill , was the last Norse-Gaelic King of Dublin . He was a member of the Meic Torcaill , a Dublin family of significance since the early twelfth century . Control of the wealthy coastal kingdom was bitterly contested during Ascall 's floruit , with members of his immediate family , as well as Islesmen and Irishmen , all securing power for brief periods of time . Throughout much of this period , however , the overlord of Dublin was Diarmait Mac Murchada , King of Leinster . In 1166 , after the death of his close ally Muirchertach Mac Lochlainn , High King of Ireland , Mac Murchada was beset by his enemies . At this critical point of his reign , Mac Murchada lost the support of the Dubliners , which contributed to his expulsion from Ireland that year . Not long afterwards , however , he made his return with significant military assistance from mercenary English adventurers . In the latter</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Battle of Kemp 's Landing = The Battle of Kemp 's Landing , also known as the Skirmish of Kempsville , was a skirmish in the American Revolutionary War that occurred on November 15 , 1775 . Militia companies from Princess Anne County in the Province of Virginia assembled at Kemp 's Landing to counter British troops under the command of Virginia 's last colonial governor , John Murray , Lord Dunmore , that had landed at nearby Great Bridge . Dunmore was investigating rumors of Patriot troop arrivals from North Carolina that turned out to be false ; he instead moved against the Princess Anne militia , defeating their attempt at an ambush and routing them . Dunmore followed up the victory with a reading of his proclamation declaring martial law and promising freedom to slaves belonging to Patriot owners if they served in the British military . This increased opposition to his activities , and he was eventually forced to leave Virginia . = = Background = = Tensions in the British Colony of</t>
+          <t>William of York = William of York ( late 11th century – 8 June 1154 ) , also known as William fitzHerbert , William I fitzHerbert and William of Thwayt , was an English priest and Archbishop of York . William has the unusual distinction of having been Archbishop of York twice , both before and after his rival Henry Murdac . He was a relative of King Stephen of England , and the king helped secure FitzHerbert 's election to York after a number of candidates had failed to secure papal confirmation . William faced opposition from the Cistercians who , after the election of the Cistercian Pope Eugene III , managed to have the archbishop deposed in favour of the Cistercian Murdac . From 1147 until 1153 , William worked to secure his restoration to York , which he finally achieved after the deaths of both Murdac and Eugene III . He did not retain the see long , as he died shortly after returning to York , allegedly having been poisoned . After William 's death miracles were reported at his t</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Mount Hope Bay raids = The Mount Hope Bay raids were a series of military raids conducted by British troops during the American Revolutionary War against communities on the shores of Mount Hope Bay on May 25 and 30 , 1778 . The towns of Bristol and Warren , Rhode Island were significantly damaged , and Freetown , Massachusetts ( present-day Fall River ) was also attacked , although its militia resisted British activities . The British destroyed military defenses in the area , including supplies that had been cached by the Continental Army in anticipation of an assault on British-occupied Newport , Rhode Island . Homes as well as municipal and religious buildings were also destroyed in the raids . On May 25 , 500 British and Hessian soldiers , under orders from General Sir Robert Pigot , the commander of the British garrison at Newport , Rhode Island , landed between Bristol and Warren , destroyed boats and other supplies , and plundered Bristol . Local resistance was minimal and ineffe</t>
+          <t xml:space="preserve">Ivan Vladislav of Bulgaria = Ivan Vladislav ( Bulgarian : Иван Владислав ) ruled as emperor ( tsar ) of Bulgaria from August or September 1015 to February 1018 . The year of his birth is unknown ; he was born at least a decade before 987 , but probably not much earlier than that . Saved from death by his cousin Gavril Radomir , the Bulgarian Emperor , in 976 , Ivan Vladislav murdered him in October 1015 and seized the Bulgarian throne . Due to the desperate situation of the country following the decades-long war with the Byzantine Empire , and in an attempt to consolidate his position , he tried to negotiate truce with the Byzantine emperor Basil II . After the failure of the negotiations he continued the resistance , attempting unsuccessfully to push the Byzantines back . During his period of rule , Ivan Vladislav tried to strengthen the Bulgarian army , reconstructed many Bulgarian fortresses and even carried out a counter-offensive , but he died at the Battle of Dyrrhachium in 1018 </t>
         </is>
       </c>
     </row>
@@ -1281,32 +1281,32 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>['lap', 'race', 'drivers', 'laps', 'pit', 'car', 'ferrari', 'prix', 'driver', 'qualifying', 'session', 'fastest', 'ahead', 'hamilton', 'points']</t>
+          <t>['text', 'notes', 'book', 'bach', 'sunday', 'published', 'setting', 'edition', 'movements', 'describes', 'publication', 'bass', 'read', 'author', 'magazine']</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2010 Showtime Southern 500 = The 2010 Showtime Southern 500 , 61st running of the event , was a NASCAR Sprint Cup Series motor race that was held on May 8 , 2010 at Darlington Raceway in Darlington , South Carolina . It was the eleventh race of the 2010 NASCAR Sprint Cup Series season . The event began at 7 : 30 p.m. EDT . It was televised live in the United States on Fox and its U.S. radio coverage was broadcast on Motor Racing Network starting at 6 p.m. EDT . The 367-lap race was won by Denny Hamlin for Joe Gibbs Racing after starting seven positions behind polesitter Jamie McMurray . McMurray finished second in a Chevrolet , and Kurt Busch finished third in a Dodge . The race had a total of 11 cautions and 22 lead changes among 11 different drivers . Kevin Harvick remained the point leader after finishing the race in the sixth position . = = Background = = Coming into the race , Richard Childress Racing driver Kevin Harvick led the Drivers ' Championship with 1,467 points , with Hen</t>
+          <t xml:space="preserve">Bereitet die Wege , bereitet die Bahn , BWV 132 = Bereitet die Wege , bereitet die Bahn ( Prepare the paths , prepare the road ) , BWV 132 , is a church cantata by Johann Sebastian Bach . He composed it in Weimar in 1715 for the fourth Sunday in Advent and led the first performance on 22 December 1715 . Bach had taken up regular cantata composition a year before when he was promoted to concertmaster at the Weimar court , writing one cantata per month to be performed in the Schlosskirche , the court chapel in the ducal Schloss . Bereitet die Wege , bereitet die Bahn was his first cantata for the fourth Sunday in Advent . The libretto by the court poet Salomo Franck is related to the day 's prescribed gospel reading , the testimony of John the Baptist . Franck derives from it thoughts about baptism as a preparation of the individual Christian who is addressed as a limb of Christ . Bach structured the music in six movements of alternating arias and recitatives , and scored it for a small </t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2013 Mudsummer Classic = The 2013 Mudsummer Classic ( formally the CarCash Mudsummer Classic presented by CNBC Prime 's The Profit ) was a NASCAR Camping World Truck Series stock car race held on July 24 , 2013 at Eldora Speedway in New Weston , Ohio . The race was the first dirt track race held by a NASCAR national touring series ( Cup , Xfinity , Trucks ) since 1970 . Contested over 150 laps , the race was the tenth of the 2013 NASCAR Camping World Truck Series season . Ken Schrader of self-owned Ken Schrader Racing won the pole position , and became the oldest pole sitter in NASCAR history at 58 years of age . Austin Dillon of Richard Childress Racing won the race , while Kyle Larson and Ryan Newman finished second and third , respectively . The qualifying procedure was unique for the race ; drivers ' qualifying times set the starting grids for five heat races to determine the feature race 's starting lineup , while the top five of a last chance qualifier ( LCQ ) advance to the feat</t>
+          <t xml:space="preserve">Christ unser Herr zum Jordan kam , BWV 7 = Christ unser Herr zum Jordan kam ( Christ our Lord came to the Jordan ) , BWV 7 , is a church cantata by Johann Sebastian Bach . He composed it in Leipzig for the Feast of St. John the Baptist and led its first performance on 24 June 1724 . It is the third cantata Bach composed for his chorale cantata cycle , the second cycle he started after being appointed Thomaskantor in 1723 . The cantata is based on the seven stanzas of Martin Luther 's hymn " Christ unser Herr zum Jordan kam " , about baptism . The first and last stanza of the chorale were used for the outer movements of the cantata , while an unknown librettist paraphrased the inner stanzas of the hymn into the text for the five other movements . The first movement , a chorale fantasia , is followed by a succession of arias alternating with recitatives , leading to a four-part closing chorale . The cantata is scored for three vocal soloists ( alto , tenor and bass ) , a four-part choir </t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2009 Ford 400 = The 2009 Ford 400 was the thirty-six and final stock car race of the 2009 NASCAR Sprint Cup Series as well as the tenth and final race of the season-ending Chase for the Sprint Cup . It was held on November 22 , 2009 at Homestead-Miami Speedway , in Homestead , Florida before a crowd of 70,000 people . The 267-lap race was won by Denny Hamlin of the Joe Gibbs Racing team after starting from thirty-eighth position . Jeff Burton finished second and his teammate Kevin Harvick came in third . Jimmie Johnson won the pole position and maintained his lead on the first lap of the race . Many Chase for the Sprint Cup participants , including Johnson , Kurt Busch and Mark Martin , were in the top ten for most of the race , although some encountered problems in the closing laps . Kyle Busch was leading the race with forty-four laps remaining , giving the lead to Hamlin who maintained it to win the race . There were seven cautions in the race , as well as eighteen lead changes amon</t>
+          <t>O ewiges Feuer , o Ursprung der Liebe , BWV 34 = O ewiges Feuer , o Ursprung der Liebe ( O eternal fire , o source of love ) , BWV 34 , is a church cantata by Johann Sebastian Bach . He composed it in Leipzig in for Pentecost Sunday , based on an earlier wedding cantata , BWV 34a , beginning with the same line . Bach led the first performance on 1 June 1727 . An unknown librettist adapted the text of three movements from the wedding cantata and added two recitatives . A central contemplative aria for alto , accompanied by two flutes and muted strings , is framed by recitatives , while the two outer movements are performed by the chorus and a festive Baroque instrumental ensemble of three trumpets , timpani , two oboes , strings and continuo . The last movement quotes the conclusion of Psalm 128 , " Friede über Israel " ( Peace upon Israel ) . The themes of eternal fire , love , dwelling together and peace suit both occasions , wedding and Pentecost . = = History and text = = Bach adapt</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2010 Price Chopper 400 = The 2010 Price Chopper 400 was a NASCAR Sprint Cup Series stock car race that was held on October 3 , 2010 at Kansas Speedway in Kansas City , Kansas . The 300 lap race was the twenty-ninth in the 2010 NASCAR Sprint Cup Series . The race was also the third event in the ten round Chase for the Sprint Cup competition , which would conclude the 2010 season . Greg Biffle , of the Roush Fenway Racing team , won the race , with Jimmie Johnson finishing second and Kevin Harvick third . Pole position driver Kasey Kahne maintained his lead on the first lap to begin the race , as Jeff Gordon , who started in the third position on the grid , remained behind him . Twenty-three laps later Jeff Gordon became the leader of the race . After the final pit stops , Paul Menard became the leader of the race , but with less than fifty laps remaining , Biffle passed him . He maintained the first position to lead a total of sixty laps , and to win his second race of the season . Ther</t>
+          <t>St John Passion structure = The structure of the St John Passion ( German : Johannes-Passion ) , BWV 245 , a sacred oratorio by Johann Sebastian Bach , is " carefully designed with a great deal of musico-theological intent " . Some main aspects of the structure are shown in tables below . The original Latin title Paßio secundum Joannem translates to " The Passion after John " . Bach 's large choral composition in two parts on German text , written to be performed in a Lutheran service on Good Friday , is based on the Passion , as told in two chapters from the Gospel of John ( John 18 and John 19 ) in the translation by Martin Luther , with two short interpolations from the Gospel of Matthew ( in Version I , one from the Gospel of Matthew and one from the Gospel of Mark ) . During the vespers service , the two parts of the work were performed before and after the sermon . Part I covers the events until Peter 's denial of Jesus , Part II concludes with the burial of Jesus . The Bible tex</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2011 Coca-Cola 600 = The 2011 Coca-Cola 600 , the 52nd running of the event , was a NASCAR Sprint Cup Series motor race held on May 29 , 2011 , at Charlotte Motor Speedway in Concord , North Carolina . Contested over 400 laps on the 1.5-mile ( 2.4 km ) asphalt quad-oval , it was the twelfth race of the 2011 Sprint Cup Series season . The race was won by Kevin Harvick for the Richard Childress Racing team . David Ragan finished second , and Joey Logano clinched third . There were 14 cautions and 38 lead changes among 19 different drivers throughout the course of the race . The result moved Harvick to the second position in the Drivers ' Championship . He remained 36 points behind first place driver Carl Edwards and one ahead of Jimmie Johnson in third . In the Manufacturers ' Championship , Chevrolet was first with 83 points , six ahead of Ford . Toyota was third with 64 points , 24 points ahead of Dodge . The race was extended to 402 laps and 603 miles ( 970 km ) , making it the longes</t>
+          <t>Oh Pray My Wings Are Gonna Fit Me Well = Oh Pray My Wings Are Gonna Fit Me Well is a book of poems by American author Maya Angelou , published by Random House in 1975 . It is Angelou 's second volume of poetry , written after her first two autobiographies and first volume of poetry were published . Angelou considers herself a poet and a playwright , but is best known for her seven autobiographies , especially her first , I Know Why the Caged Bird Sings , although her poetry has also been successful . She began , early in her writing career , alternating the publication of an autobiography and a volume of poetry . Although her poetry collections have been best-sellers , they have not received serious critical attention . Oh Pray is divided into five parts and consists of 36 poems . The volume is dedicated to " Paul " . Like many of Angelou 's poems , the poetry in the volume has been characterized as light verse . They contain identifications with ordinary objects and universal identifi</t>
         </is>
       </c>
     </row>
@@ -1316,32 +1316,32 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>['temple', 'mosque', 'han', 'dynasty', 'sanskrit', 'buddhist', 'hindu', 'chinese', 'bce', 'texts', 'monastery', 'buddhism', 'temples', 'wall', 'text']</t>
+          <t>['raaf', 'flying', 'wing', 'combat', 'unit', 'training', 'operational', 'pilot', 'officer', 'aircraft', 'flight', 'pilots', 'disbanded', 'commanding', 'squadron']</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Pundarikakshan Perumal Temple = Pundarikakshan Perumal Temple or Thiruvellarai a in Thiruvellarai , a village in the outskirts of Tiruchirappalli in the South Indian state of Tamil Nadu , is dedicated to the Hindu god Vishnu . Constructed in the Dravidian style of architecture , the temple is glorified in the Divya Prabandha , the early medieval Tamil canon of the Azhwar saints from the 6th – 9th centuries AD . It is one of the 108 Divyadesam dedicated to Vishnu , who is worshipped as Pundarikakshan and his consort Lakshmi as Pankajavalli . The temple was built by Shivi Chakravarthy , king of Ayodhya in Treta Yuga 15 lakh years ago . This temple is older than Srirangam temple.The temple has three inscriptions in its two rock-cut caves , two dating from the period of Nandivarman II ( 732 – 796 AD ) and the other to that of Dantivarman ( 796 – 847 ) . It also has Pallava sculptural depictions of Narasimha and Varaha , two of the ten avatars of Vishnu . A granite wall surrounds the temple</t>
+          <t xml:space="preserve">No. 84 Wing RAAF = No. 84 Wing is a Royal Australian Air Force ( RAAF ) transport wing . Coming under the control of Air Mobility Group ( AMG ) , it is headquartered at RAAF Base Richmond , New South Wales . The wing comprises No. 34 Squadron , operating Boeing 737 and Bombardier Challenger 604 VIP jets ; No. 37 Squadron , operating Lockheed Martin C-130J Super Hercules medium transports ; and a technical training unit , No. 285 Squadron . Formed in 1944 for army co-operation duties in the South West Pacific theatre of World War II , No. 84 Wing operated a mix of aircraft including CAC Boomerangs , CAC Wirraways , Auster AOPs and Bristol Beauforts , before disbanding in 1946 . It was re-formed in 1991 as a tactical transport wing headquartered at RAAF Base Townsville , Queensland , comprising Nos. 35 and 38 Squadrons operating de Havilland Canada DHC-4 Caribous . By 1996 , it had been augmented by No. 32 Squadron , operating Hawker Siddeley HS 748 trainer-transports . In 1998 , No. 84 </t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kandariya Mahadeva Temple = The Kandariya Mahadeva Temple ( Devanagari : कंदारिया महादेव मंदिर , Kaṇḍāriyā Mahādeva Mandir ) , meaning " the Great God of the Cave " , is the largest and most ornate Hindu temple in the medieval temple group found at Khajuraho in Madhya Pradesh , India . It is considered one of the best examples of temples preserved from the medieval period in India . = = Location = = Kaṇḍāriyā Mahādeva Temple is located in the Chhatarpur district of Madhya Pradesh in Central India . It is in the Khajuraho village , and the temple complex is spread over an area of 6 square kilometres ( 2.3 sq mi ) . It is in the western part of the village to the west of the Vishnu temple . The temple complex , in the Khajuraho village at an elevation of 282 metres ( 925 ft ) , is well connected by road , rail and air services . Khajuraho is 34 miles ( 55 km ) to the south of Mahoba , 29 miles ( 47 km ) away from the Chhatarpur city to its east , 27 miles ( 43 km ) away from Panna , 400 </t>
+          <t>Neville McNamara = Air Chief Marshal Sir Neville Patrick McNamara , KBE , AO , AFC , AE ( 17 April 1923 – 7 May 2014 ) was a senior commander of the Royal Australian Air Force ( RAAF ) . He served as Chief of the Air Staff ( CAS ) , the RAAF 's highest-ranking position , from 1979 until 1982 , and as Chief of the Defence Force Staff ( CDFS ) , Australia 's top military role at the time , from 1982 until 1984 . He was the second RAAF officer to hold the rank of air chief marshal . Born in Queensland , McNamara joined the RAAF during World War II and saw action in the South West Pacific , flying P-40 Kittyhawks . He also flew combat missions in Gloster Meteors during the Korean War . In 1961 , he was awarded the Air Force Cross for his leadership of No. 2 Operational Conversion Unit . He gained further operational experience heading the RAAF presence in Ubon , Thailand , in the late 1960s . Promoted to air commodore , McNamara was Commander RAAF Forces Vietnam , and Deputy Commander Aust</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Raghunath Temple = Raghunath Temple consists of a complex of seven Hindu shrines , each with its own Shikhara . It is one of the largest temple complexes of north India . It is located in Jammu in the Indian state of Jammu and Kashmir . The temple was built during the period 1822 – 1860 by order of Maharaja Ranjit Singh , while Jammu was under his administration by Maharaja Gulab Singh . The temple has many gods in its complex of shrines , but the presiding deity is Rama , an Avatar of Vishnu . The Mughal architectural influence is seen in all the spiral shaped towers which have gold plated spires , except the tower over the main shrine which is said to be in Sikh architectural style . The niches in the walls of the shrines are decorated with 300 well crafted images of deities . The paintings in the 15 panels of the main shrine are based on themes from Ramayana , Mahabharata , and Bhagavad Gita . The temple was also in the news during 2002 when suicide bombers Fidayeen of the Lashkar-e</t>
+          <t>John Emilius Fauquier = Air Commodore John Emilius " Johnny " Fauquier DSO &amp; Two Bars , DFC ( March 19 , 1909 – April 3 , 1981 ) was a Canadian aviator and Second World War Bomber Command leader . He commanded No. 405 Squadron RCAF and later No. 617 Squadron RAF ( the Dambusters ) over the course of the war . A bush pilot , prior to the war , he joined the Royal Canadian Air Force as a flight instructor in 1939 . He then joined 405 Squadron in 1941 and would fly operationally for the rest of the war , taking a drop in rank on one occasion to return to active command . During his three tours of operation he participated in Operation Hydra and dozens of other sorties over Europe . = = Early years = = John Emilius " Johnny " Fauquier was born at Ottawa , Ontario on March 19 , 1909 , educated at Ashbury College and then entered the investment business at Montreal , Quebec where he joined a flying club . After earning his commercial pilot 's licence he formed Commercial Airways at Noranda ,</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Zhenguo Temple = Zhenguo Temple ( Chinese : 镇国寺 ) is a Buddhist temple located 10 km from Pingyao in the village of Hadongcun , in Shanxi Province , China . The temple 's oldest hall , the Wanfo Hall , was built in 963 during the Northern Han dynasty , and is notable for featuring very large brackets that hold up the roof and flying eaves . The sculptures inside the hall are among the only examples of 10th century Buddhist sculpture in China . = = History = = The history of the temple begins in 963 , when it was recorded that Ten-Thousand Buddha Hall ( Wànfó diàn 万佛殿 ) was built . The date is written on a beam in the hall , and is also the date given by a local history of Pingyao county written in the 19th century . A stela written in 1819 also confirms this date . Wanfo Hall is the oldest building at Zhenguo temple , and is the only surviving building that dates from the short-lived Northern Han dynasty . Although little is known of the temple 's history , stelae record that it was re</t>
+          <t>Southern Area Command ( RAAF ) = Southern Area Command was one of several geographically based commands raised by the Royal Australian Air Force ( RAAF ) during World War II . It was formed in March 1940 , and initially controlled units based in Victoria , Tasmania , South Australia and southern New South Wales . Headquartered at Melbourne , Southern Area Command was primarily responsible for air defence , aerial reconnaissance and protection of the sea lanes within its boundaries . From 1942 its operational responsibilities excluded New South Wales . The area continued to operate following the end of the war , before being re-formed in October 1953 as Training Command under the RAAF 's new functional command-and-control system . = = History = = = = = World War II = = = Prior to World War II , the Royal Australian Air Force was small enough for all its elements to be directly controlled by RAAF Headquarters in Melbourne . After war broke out in September 1939 , the RAAF began to decent</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Jokhang = The Jokhang ( Tibetan : ཇོ ་ ཁང ། , Chinese : 大昭寺 ) , also known as the Qoikang Monastery , Jokang , Jokhang Temple , Jokhang Monastery and Zuglagkang ( Tibetan : གཙུག ་ ལག ་ ཁང ༌ ། , Wylie : gtsug-lag-khang , ZYPY : Zuglagkang or Tsuklakang ) , is a Buddhist temple in Barkhor Square in Lhasa , the capital city of Tibet . Tibetans , in general , consider this temple as the most sacred and important temple in Tibet . The temple is currently maintained by the Gelug school , but they accept worshipers from all sects of Buddhism . The temple 's architectural style is a mixture of Indian vihara design , Tibetan and Nepalese design . The Jokhang was founded during the reign of King Songtsen Gampo . According to tradition , the temple was built for the king 's two brides : Princess Wencheng of the Chinese Tang dynasty and Princess Bhrikuti of Nepal . Both are said to have brought important Buddhist statues and images from China and Nepal to Tibet , which were housed here , as part o</t>
+          <t>Hawker Siddeley P.1127 = The Hawker P.1127 and the Hawker Siddeley Kestrel FGA.1 were the experimental and development aircraft that led to the Hawker Siddeley Harrier , the first vertical and / or short take-off and landing ( V / STOL ) jet fighter-bomber . Kestrel development began in 1957 , taking advantage of the Bristol Engine Company 's choice to invest in the creation of the Pegasus vectored-thrust engine . Testing began in July 1960 and by the end of the year the aircraft had achieved both vertical take-off and horizontal flight . The test program also explored the possibility of use upon aircraft carriers , landing on HMS Ark Royal in 1963 . The first three aircraft crashed during testing , one at the 1963 Paris Air Show . Improvements to future development aircraft , such as swept wings and more powerful Pegasus engines , led to the development of the Kestrel . The Kestrel was evaluated by the Tri-partite Evaluation Squadron , made up of military pilots from Britain , the Uni</t>
         </is>
       </c>
     </row>
@@ -1351,32 +1351,32 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>['simpsons', 'south_park', 'homer', 'lisa', 'episode', 'episodes', 'kenny', 'jake', 'stan', 'kyle', 'finn', 'animated', 'parker', 'voice', 'voiced']</t>
+          <t>['took', 'second', 'played', 'runs', 'team', 'tour', 'england', 'australia', 'playing', 'class', 'run', 'came', 'score', 'match', 'taking']</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>SpongeBob SquarePants ( season 7 ) = The seventh season of the American animated television series SpongeBob SquarePants , created by marine biologist and animator Stephen Hillenburg , originally aired on Nickelodeon in the United States from July 19 , 2009 to June 11 , 2011 . It contained 26 episodes , beginning with the episodes " Tentacle Vision " and " I Heart Dancing " . The series chronicles the exploits and adventures of the title character and his various friends in the fictional underwater city of Bikini Bottom . The season was executive produced by series creator Hillenburg and writer Paul Tibbitt , who also acted as the showrunner . In 2011 , Legends of Bikini Bottom , an anthology series consists of five episodes from the season , was launched . A number of guest stars appeared on the season 's episodes . Several compilation DVDs that contained episodes from the season were released . The SpongeBob SquarePants : Complete Seventh Season DVD was released in Region 1 on Decemb</t>
+          <t>Alyssa Healy = Alyssa Jean Healy ( born 24 March 1990 on the Gold Coast , Queensland ) is a cricketer who plays for New South Wales and the Australian women 's team . She made her international debut in February 2010 . A right-handed batter and wicket-keeper , she is the daughter of Greg Healy , who was part of the Queensland squad , while her uncle Ian Healy was Australia 's Test wicket-keeper and held the world record for the most Test dismissals . Healy first came to prominence in late 2006 when she became the first girl to play among boys in the private schools ' competition in New South Wales . She moved up the state age group ranks and made her debut for the senior New South Wales team in the 2007 – 08 season . She played most of her first two seasons as a specialist batsman due to the presence of Leonie Coleman — a wicket-keeper for Australia — in the state side . Coleman left New South Wales at the start of the 2009 – 10 season and Healy took up the glovework on a full-time bas</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Cartman 's Mom Is a Dirty Slut = " Cartman 's Mom Is a Dirty Slut " is the first season finale of the American animated television series South Park . It originally aired on Comedy Central in the United States on February 25 , 1998 . The episode is the highest viewed episode in the entire South Park series , with 6.4 million views . It is part one of a two-episode story arc , which concluded with " Cartman 's Mom Is Still a Dirty Slut " . The episode follows Eric Cartman , one of the show 's child protagonists , becoming curious about the identity of his father . He discovers that his father is most likely a man his mother had sexual intercourse with during an annual party called " The Drunken Barn Dance " . Meanwhile , his friends Stan , Kyle and Kenny participate on America 's Stupidest Home Videos , after filming Cartman playing in his yard with plush toys . The episode was written by Trey Parker and staff writer David A. Goodman , and directed by Parker . It featured a guest appear</t>
+          <t>Robert Key ( cricketer ) = Robert William Trevor Key ( born 12 May 1979 ) is an English former cricketer . He represented Kent County Cricket Club and is a former member of the England Test match and One Day International sides . A right-handed opening batsman , Key made appearances at age-group level for Kent from the age of eleven , moving up until he made his first-class debut in 1998 . He made eight first-class and 4 List A appearances for England 's youth sides , and was a member of the side which won the 1998 Under-19 Cricket World Cup . Following a season of heavy run-scoring , Key was called up to the England A side in 1999 . Following an injury to Marcus Trescothick , Key made his Test debut against India in 2002 . He toured Australia during the 2002 – 03 Ashes series , where he justified his selection ahead of a more experienced player . His One Day International debut came in 2003 , against Zimbabwe , however he was dropped from both squads shortly after . Injury to Mark But</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>An Elephant Makes Love to a Pig = " An Elephant Makes Love to a Pig " is the fifth episode in the first season of the American animated television series South Park . It originally aired on Comedy Central in the United States on September 10 , 1997 . In the episode , the boys of South Park try to force Kyle 's pet elephant to crossbreed with Cartman 's pet pig for a class project on genetic engineering . Meanwhile , Stan tries to deal with his sister Shelley , who keeps beating him up . The episode was written by series co-creators Trey Parker and Matt Stone along with Dan Sterling . The episode served as both a parody of genetic engineering and a statement against its potential evils . The scenes of Stan getting beat up by his sister were inspired by Parker 's real-life childhood experiences with his own sister , who is also named Shelley . " An Elephant Makes Love to a Pig " was met with generally positive reviews , and has been described as one of the most popular early South Park e</t>
+          <t>Jack Fingleton = John " Jack " Henry Webb Fingleton OBE ( 28 April 1908 – 22 November 1981 ) was an Australian cricketer who was trained as a journalist and became a political and cricket commentator after the end of his playing career . A stubborn opening batsman known for his dour defensive approach , he scored five Test centuries , representing Australia in 18 Tests between 1932 and 1938 . He was also known for his involvement in several cricket diplomacy incidents in his career , accused of leaking the infamous verbal exchange between Australian captain Bill Woodfull and English manager Plum Warner during the acrimonious Bodyline series , and later of causing sectarian tension within the team by leading a group of players of Irish Catholic descent in undermining the leadership of the Protestant Don Bradman . In retirement , Fingleton became a prominent political commentator in Canberra , with links to Australian prime ministers . The author of many cricket books , he is regarded as</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Julie Kavner = Julie Deborah Kavner ( born September 7 , 1950 ) is an American film and television actress , voice actress and comedian . She first attracted notice for her role as Valerie Harper 's character 's younger sister Brenda in the sitcom Rhoda for which she won a Primetime Emmy Award for Outstanding Supporting Actress in a Comedy Series . She is best known for her voice role as Marge Simpson on the animated television series The Simpsons . She also voices other characters for the show , including Jacqueline Bouvier , and Patty and Selma Bouvier . Known for her improvisation and distinctive " honeyed gravel voice , " Kavner was cast in her first professional acting role as Brenda Morgenstern in Rhoda in 1974 . She received the Primetime Emmy Award in 1978 and three more nominations for playing the character . Following Rhoda , Kavner was cast in The Tracey Ullman Show , which debuted in 1987 . The Tracey Ullman Show included a series of animated shorts about a dysfunctional fa</t>
+          <t>Colin McCool = Colin Leslie McCool ( 9 December 1916 – 5 April 1986 ) was an Australian cricketer who played in 14 Tests from 1946 to 1950 . McCool , born in Paddington , New South Wales , was an all-rounder who bowled leg spin and googlies with a round arm action and as a lower order batsman was regarded as effective square of the wicket and against spin bowling . He made his Test début against New Zealand in 1946 , taking a wicket with his second delivery . He was part of Donald Bradman 's Invincibles team that toured England in 1948 but injury saw him miss selection in any of the Test matches . A good tour of South Africa in 1949 – 50 was followed by a lack of opportunity in the next two seasons , leading McCool to sign a contract to play professional cricket in the Lancashire League in 1953 . Three years later , Somerset County Cricket Club recruited McCool where he was a success , especially as a middle-order batsman ; he played five seasons and saw the club achieve its highest pl</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Reptar on Ice = " Reptar on Ice " is the tenth episode of the second season of the animated television series Rugrats . It is the first segment of the twenty-third episode for the entire series . The episode was written by Peter Gaffney and directed by Howard E. Baker . It was originally broadcast on November 8 , 1992 . " Reptar on Ice " followed the infant main characters , Tommy , Chuckie , Phil , and Lil going to an ice show with their parents that follows the love story of the babies ' favorite monster , Reptar . There , the babies attempt to return a lizard to the actor , assuming it is his child . " Reptar on Ice " continued Rugrats ' employment of the character Reptar , a satirical parody of Godzilla . The episode included several other cultural references ; the basic theme lampoons the commercialization of children 's media products and its plethora of merchandise tie-ins . The ice show the children see is referent to real-life ice shows , such as " Disney on Ice , " and its pl</t>
+          <t>2008 Indian Premier League Final = The 2008 Indian Premier League Final was a day / night Twenty20 cricket match played between the Rajasthan Royals and the Chennai Super Kings on 1 June 2008 at the DY Patil Stadium , Navi Mumbai to determine the winner of the 2008 Indian Premier League , a professional Twenty20 cricket league in India . It ended as the Royals defeated the Super Kings by three wickets . The Royals , captained by Shane Warne , topped the group stage table , whereas the Super Kings , led by Mahendra Singh Dhoni , stood at the third position . They had defeated the Delhi Daredevils and the Kings XI Punjab respectively in the semi-finals . Winning the toss , Royals ' captain Shane Warne opted to field first . The Super Kings scored 163 runs in 20 overs with a loss of 5 wickets . Batting at number three , Suresh Raina top scored for the Super Kings with 43 runs . Royals ' bowler Yusuf Pathan took three wickets for 22 runs . The Royals failed to build a good opening partners</t>
         </is>
       </c>
     </row>
@@ -1386,32 +1386,32 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>['formula', 'matrix', 'function', 'newton', 'linear', 'plants', 'constant', 'language', 'defined', 'theory', 'functions', 'example', 'consciousness', 'space', 'derivative']</t>
+          <t>['highway', 'north', 'road', 'east', 'route', 'lane', 'south', 'intersection', 'west', 'continues', 'interchange', 'designated', 'completed', 'state', 'passes']</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Biology = Biology is a natural science concerned with the study of life and living organisms , including their structure , function , growth , evolution , distribution , identification and taxonomy . Modern biology is a vast and eclectic field , composed of many branches and subdisciplines . However , despite the broad scope of biology , there are certain general and unifying concepts within it that govern all study and research , consolidating it into single , coherent field . In general , biology recognizes the cell as the basic unit of life , genes as the basic unit of heredity , and evolution as the engine that propels the synthesis and creation of new species . It is also understood today that all the organisms survive by consuming and transforming energy and by regulating their internal environment to maintain a stable and vital condition known as homeostasis . Sub-disciplines of biology are defined by the scale at which organisms are studied , the kinds of organisms studied , an</t>
+          <t>Maryland Route 7 = Maryland Route 7 ( MD 7 ) is a collection of state highways in the U.S. state of Maryland . Known for much of their length as Philadelphia Road , there are five disjoint mainline sections of the highway totaling 40.23 miles ( 64.74 km ) that parallel U.S. Route 40 ( US 40 ) in Baltimore , Harford , and Cecil counties in northeastern Maryland . The longest section of MD 7 begins at US 40 just east of the city of Baltimore in Rosedale and extends through eastern Baltimore County and southern Harford County to US 40 in Aberdeen . The next segment of the state highway is a C-shaped route through Havre de Grace . The third mainline section of MD 7 begins in Perryville and ends at US 40 a short distance west of the start of the fourth section , which passes through Charlestown and North East before ending at US 40 just west of Elkton . The fifth segment of the highway begins at South Street and passes through the eastern part of Elkton before reconnecting with US 40 west o</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Myco-heterotrophy = Myco-heterotrophy ( Greek : μυκός mykós , " fungus " , ἕτερος heteros = " another " , " different " and τροφή trophe = " nutrition " ) is a symbiotic relationship between certain kinds of plants and fungi , in which the plant gets all or part of its food from parasitism upon fungi rather than from photosynthesis . A myco-heterotroph is the parasitic plant partner in this relationship . Myco-heterotrophy is considered a kind of cheating relationship and myco-heterotrophs are sometimes informally referred to as " mycorrhizal cheaters " . This relationship is sometimes referred to as mycotrophy , though this term is also used for plants that engage in mutualistic mycorrhizal relationships . = = Relationship between myco-heterotrophs and host fungi = = Full ( or obligate ) myco-heterotrophy exists when a non-photosynthetic plant ( a plant largely lacking in chlorophyll or otherwise lacking a functional photosystem ) gets all of its food from the fungi that it parasitize</t>
+          <t>Maryland Route 404 = Maryland Route 404 ( MD 404 ) is a major highway on Maryland 's Eastern Shore in the United States . It runs 24.61 miles ( 39.61 km ) from MD 662 in Wye Mills on the border of Queen Anne 's and Talbot counties , southeast to the Delaware state line in Caroline County , where the road continues as Delaware Route 404 ( DE 404 ) to Nassau ( near Rehoboth Beach ) . The Maryland and Delaware state highways together cross the width of the Delmarva Peninsula and serve to connect the cities west of the Chesapeake Bay by way of the Chesapeake Bay Bridge and U.S. Route 50 ( US 50 ) with the Delaware Beaches . Along the way , MD 404 passes through mostly farmland and woodland as well as the towns of Queen Anne , Hillsboro , and Denton . The road is a two-lane undivided highway for most of its length with the exception of the bypass around Denton and a section near Hillsboro , which is a four-lane divided highway . MD 404 was designated by 1933 to run from Matapeake ( where th</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Philosophy of science = Philosophy of science is a branch of philosophy concerned with the foundations , methods , and implications of science . The central questions of this study concern what qualifies as science , the reliability of scientific theories , and the ultimate purpose of science . This discipline overlaps with metaphysics , ontology , and epistemology , for example , when it explores the relationship between science and truth . There is no consensus among philosophers about many of the central problems concerned with the philosophy of science , including whether science can reveal the truth about unobservable things and whether scientific reasoning can be justified at all . In addition to these general questions about science as a whole , philosophers of science consider problems that apply to particular sciences ( such as biology or physics ) . Some philosophers of science also use contemporary results in science to reach conclusions about philosophy itself . While philo</t>
+          <t>U.S. Route 10 in Michigan = US Highway 10 ( US 10 ) is a part of the United States Numbered Highway System that runs from West Fargo , North Dakota , to the Lower Peninsula of the US state of Michigan . The highway enters Michigan on the SS Badger , which crosses Lake Michigan between Manitowoc , Wisconsin , and Ludington . As the highway crosses the state , it is a two-lane undivided highway between Ludington and Farwell and a freeway from Farwell east to the highway 's terminus in Bay City . US 10 runs concurrently with US 127 in the Clare area along a section of freeway that includes a welcome center in the median . Outside of the Clare and Midland areas , US 10 runs through rural areas of Western and Central Michigan in a section of the Manistee National Forest as well as farm fields . As part of the original US Highway System , US 10 was first designated in Michigan in 1926 . It replaced three state trunkline highways of the day : M-20 , M-24 and M-10 , running between Ludington o</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Ecology = Ecology ( from Greek : οἶκος , " house " , or " environment " ; -λογία , " study of " ) is the scientific analysis and study of interactions among organisms and their environment . It is an interdisciplinary field that includes biology , geography , and Earth science . Ecology includes the study of interactions organisms have with each other , other organisms , and with abiotic components of their environment . Topics of interest to ecologists include the diversity , distribution , amount ( biomass ) , and number ( population ) of particular organisms , as well as cooperation and competition between organisms , both within and among ecosystems . Ecosystems are composed of dynamically interacting parts including organisms , the communities they make up , and the non-living components of their environment . Ecosystem processes , such as primary production , pedogenesis , nutrient cycling , and various niche construction activities , regulate the flux of energy and matter throug</t>
+          <t>Interstate 695 ( Maryland ) = Interstate 695 ( I-695 ) is a 51.46-mile-long ( 82.82 km ) full beltway Interstate Highway extending around Baltimore , Maryland , USA . I-695 is officially designated the McKeldin Beltway , but is colloquially referred to as either the Baltimore Beltway or 695 . The route is an auxiliary route of I-95 , intersecting that route southwest of Baltimore near Arbutus and northeast of the city near White Marsh . It also intersects other major roads radiating from the Baltimore area , including I-97 near Glen Burnie , the Baltimore – Washington Parkway ( Maryland Route 295 , MD 295 ) near Linthicum , I-70 near Woodlawn , I-795 near Pikesville , and I-83 in the Timonium area . The 19.37-mile ( 31.17 km ) portion of the Baltimore Beltway between I-95 northeast of Baltimore and I-97 south of Baltimore is officially MD 695 , and is not part of the Interstate Highway System , but is signed as I-695 . This section of the route includes the Francis Scott Key Bridge tha</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Force = In physics , a force is any interaction that , when unopposed , will change the motion of an object . In other words , a force can cause an object with mass to change its velocity ( which includes to begin moving from a state of rest ) , i.e. , to accelerate . Force can also be described by intuitive concepts such as a push or a pull . A force has both magnitude and direction , making it a vector quantity . It is measured in the SI unit of newtons and represented by the symbol F. The original form of Newton 's second law states that the net force acting upon an object is equal to the rate at which its momentum changes with time . If the mass of the object is constant , this law implies that the acceleration of an object is directly proportional to the net force acting on the object , is in the direction of the net force , and is inversely proportional to the mass of the object Related concepts to force include : thrust , which increases the velocity of an object ; drag , which </t>
+          <t xml:space="preserve">U.S. Route 60 in Oklahoma = U.S. Route 60 ( US-60 ) is a transcontinental U.S. highway extending from near Brenda , Arizona to Virginia Beach , Virginia on the Atlantic Ocean . Along the way , 352.39 miles ( 567.12 km ) of the route lies within the state of Oklahoma . The highway crosses into the state from Texas west of Arnett and serves many towns and cities in the northern part of the state , including Arnett , Seiling , Fairview , Enid , Ponca City , Pawhuska , Bartlesville , and Vinita . US-60 exits Oklahoma near Seneca , Missouri . In Oklahoma , US-60 has three business routes , serving Tonkawa , Ponca City , and Seneca . The first 60.2 miles ( 96.9 km ) of the route , from the Texas line to Seiling , is also designated as State Highway 51 ( SH-51 ) . US-60 , as originally designated , did not enter Oklahoma . Instead , it ended in Springfield , Missouri , continuing east from there . AASHO approved an extension of US-60 on May 29 , 1930 , which extended it west through Oklahoma </t>
         </is>
       </c>
     </row>
@@ -1421,32 +1421,32 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>['glee', 'kurt', 'rachel', 'meredith', 'finn', 'episode', 'grey', 'quinn', 'anatomy', 'viewers', 'sue', 'watched', 'yang', 'club', 'grace']</t>
+          <t>['game', 'team', 'play', 'season', 'second', 'defense', 'kick', 'led', 'lead', 'week', 'half', 'record', 'end', 'football', 'field']</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ballad ( Glee ) = " Ballad " is the tenth episode of the American television series Glee . The episode premiered on the Fox network on November 18 , 2009 , and was written and directed by series creator Brad Falchuk . " Ballad " sees the glee club split into pairs to sing ballads to one another . Rachel ( Lea Michele ) is paired with club director Will ( Matthew Morrison ) and develops a crush on him . Quinn 's ( Dianna Agron ) parents learn that Quinn is pregnant , and she moves in with Finn ( Cory Monteith ) and his mother when her own parents evict her . Gregg Henry and Charlotte Ross guest-star as Quinn 's parents Russell and Judy Fabray , and Sarah Drew appears as Suzy Pepper , a student with a former crush on Will . Romy Rosemont returns as Finn 's mother , Carole Hudson . The episode features covers of seven songs , including a mash-up of " Don 't Stand So Close to Me " by The Police and " Young Girl " by Gary Puckett and The Union Gap . Studio recordings of all songs performed </t>
+          <t xml:space="preserve">2007 Texas Longhorns football team = The 2007 Texas Longhorn football team ( variously " Texas " or " UT " or the " Horns " ) represented the University of Texas at Austin in the 2007 NCAA Division I FBS football season . The team was coached by Mack Brown , who received the 2005 Paul " Bear " Bryant Coach of the Year award . The Longhorns play their home games in Darrell K Royal – Texas Memorial Stadium ( DKR ) . The Longhorns entered the 2007 season ranked third on all-time college football lists in both total wins and winning percentage . A pre-season ranking by ESPN writer Mark Schlabach had the Longhorns ranked eighth , while College Football News ranked Texas third . The Longhorns came into the season ranked fourth in both the Coaches Poll and AP Poll . During the preceding summer five players had been disciplined for legal infractions , another suspended for NCAA rule violations , and a coach had undergone surgery for cancer . Additional players were suspended during the season </t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>The Rhodes Not Taken = " The Rhodes Not Taken " is the fifth episode of the American television series Glee . It premiered on the Fox network on September 30 , 2009 and was written by series co-creator Ian Brennan and directed by John Scott . The episode features glee club director Will Schuester ( Matthew Morrison ) recruiting former star April Rhodes ( Kristin Chenoweth ) , hoping to improve the club 's chances in the wake of Rachel 's ( Lea Michele ) defection to the school musical . Finn ( Cory Monteith ) flirts with Rachel in an attempt to convince her to return , and although Rachel is angry when she discovers Finn 's girlfriend is pregnant , she ultimately rejoins the club . Special guest star Kristin Chenoweth played April , and performed on three of the episode 's six musical tracks . Studio recordings of four of the songs performed in the episode were released as singles , available for digital download , and two appear on the album Glee : The Music , Volume 1 . The episode w</t>
+          <t>2012 Liberty Bowl = The 2012 AutoZone Liberty Bowl was a post-season American college football bowl game held on December 31 , 2012 at the Liberty Bowl Memorial Stadium in Memphis , Tennessee in the United States . The 54th edition of the Liberty Bowl began at 2 : 30 p.m. CST and aired on ESPN . It featured the Iowa State Cyclones from the Big 12 Conference against the Conference USA champion Tulsa Golden Hurricane and was the final game of the 2012 NCAA Division I FBS football season for both teams . The Golden Hurricane advanced to the game by virtue of winning the 2012 Conference USA Football Championship Game , while the Cyclones were also eligible for the bowl game due to their 6 – 6 regular-season record . The two teams had previously met on September 1 at the Cyclones ' home of Jack Trice Stadium in Ames , Iowa ; Iowa State won that game , 38 – 23 . The pre-game buildup was primarily focused on the rematch . A slight plurality of experts picked Tulsa over Iowa State , but most p</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Get It Right ( Glee cast song ) = " Get It Right " is a song performed by the cast of American television series Glee , taken from their sixth soundtrack album , Glee : The Music , Volume 5 . It is sung by Lea Michele who portrays the series ' lead character , Rachel Berry . The song was written by the series ' music producer Adam Anders , who created the song with his wife Nikki Hassman , and writing partner Peer Åström . Anders and company wrote the song specifically for Michele , and based the lyrics on the storyline of Rachel . The song was released with a number of Glee songs on the iTunes Store on March 15 , 2011 . Musically , " Get It Right " is a piano-driven pop ballad , with mild country influences . According to MTV 's Aly Semigran , the song has similarities to Britney Spears ' Everytime " ( 2004 ) . While critics praised Michele 's vocals in the song , they were not as receptive to the song itself with it being coined as " dull " and " boring . " The lyrics of the song rev</t>
+          <t>1917 Georgia Tech Golden Tornado football team = The 1917 Georgia Tech Golden Tornado football team represented the Georgia Institute of Technology ( commonly known as Georgia Tech ) in American football during the 1917 college football season as a member of the Southern Intercollegiate Athletic Association ( SIAA ) . The Golden Tornado , coached by John Heisman in his 14th year as head coach , compiled a 9 – 0 record ( 4 – 0 SIAA ) and outscored opponents 491 to 17 on the way to its first national championship . Heisman considered the 1917 team his best , and for many years it was considered " the greatest football team the South had ever produced " . The backfield of Albert Hill , Everett Strupper , Joe Guyon , and Judy Harlan led the Golden Tornado , and all four rushed for more than 100 yards in a 48 – 0 victory over Tulane . During the regular season Georgia Tech defeated strong opponents by large margins , and its 41 – 0 victory over eastern Penn shocked many ; Davidson , with Bu</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t xml:space="preserve">Journey to Regionals = " Journey to Regionals " is the twenty-second episode and first season finale of the American television series Glee . The episode was written and directed by series creator Brad Falchuk , and premiered on the Fox network on June 8 , 2010 . In " Journey to Regionals " , New Directions performs at Regionals in front of celebrity judges Josh Groban , Olivia Newton-John , Rod Remington ( Bill A. Jones ) and Sue Sylvester ( Jane Lynch ) . Club member Quinn ( Dianna Agron ) gives birth to her daughter , Beth , whom rival glee club coach Shelby Corcoran ( Idina Menzel ) adopts . Co-captains Finn ( Cory Monteith ) and Rachel ( Lea Michele ) reunite , and director Will Schuester ( Matthew Morrison ) professes his love for guidance counselor Emma Pillsbury ( Jayma Mays ) . Although New Directions comes in last in the competition , Sue persuades Principal Figgins ( Iqbal Theba ) not to disband the club for another year . The episode features cover versions of nine songs , </t>
+          <t xml:space="preserve">2012 New Mexico Bowl = The 2012 Gildan New Mexico Bowl was a post-season American college football bowl game that was held on December 15 , 2012 , at University Stadium on the campus of the University of New Mexico in Albuquerque , New Mexico in the United States . The seventh edition of the New Mexico Bowl began at 11 : 00 a.m. MST and aired on ESPN . It featured the Nevada Wolf Pack , who represented the Mountain West Conference in their first year as a member , against the Arizona Wildcats , who represented the Pac-12 Conference . The Wolf Pack accepted their invitation with a 7 – 4 record in their first eleven games of the season , while the Wildcats accepted their invitation after finishing the regular season at 7 – 5 . The bowl was the first of 35 played in the 2012 – 13 bowl game season . Coming into the game , both teams had sound offenses and were led by their respective running backs , sophomore Ka 'Deem Carey for Arizona and senior Stefphon Jefferson for Nevada , who ranked </t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Throwdown ( Glee ) = " Throwdown " is the seventh episode of the American television series Glee . The episode premiered on the Fox network on October 14 , 2009 . It was directed by series creator Ryan Murphy and written by Brad Falchuk . The episode includes a clash between glee club director Will Schuester ( Matthew Morrison ) and cheerleading coach Sue Sylvester ( Jane Lynch ) when she is named co-director of the glee club . As Sue tries to divide the club by turning the students against Will , his wife Terri ( Jessalyn Gilsig ) blackmails her OB / GYN into colluding with her over her fake pregnancy . The episode features covers of five songs . Studio recordings of four of the songs performed were released as singles , available for digital download , and were also included on the album Glee : The Music , Volume 1 . " Throwdown " was watched by 7.65 million US viewers and received mixed reviews from critics . The pregnancy storyline was criticized by both Ken Tucker of Entertainment</t>
+          <t>1957 NCAA Men 's Division I Basketball Championship Game = The 1957 NCAA Men 's Division I Basketball Championship Game took place on March 23 , 1957 between the North Carolina Tar Heels and Kansas Jayhawks at the Municipal Auditorium in Kansas City , Missouri . The match-up was the final one of the nineteenth consecutive NCAA Men 's Division I Basketball Championship single-elimination tournament — commonly referred to as the NCAA Tournament — organized by the National Collegiate Athletic Association ( NCAA ) and is used to crown a national champion for men 's basketball at the Division I level . After surviving numerous close games during the regular season , conference tournament , and most recently a triple overtime game against Michigan State in the national semifinal , North Carolina came into the National Championship game with an unblemished record of 31 – 0 . Led by coach Frank McGuire and Helms Foundation College Basketball Player of the Year Lennie Rosenbluth , the Tar Heels</t>
         </is>
       </c>
     </row>
@@ -1456,32 +1456,32 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>['bach', 'poem', 'poems', 'shakespeare', 'poet', 'poetry', 'movement', 'ode', 'movements', 'soprano', 'text', 'alto', 'aria', 'stanza', 'narrator']</t>
+          <t>['second', 'place', 'position', 'race', 'track', 'car', 'lead', 'fifth', 'fourth', 'sixth', 'pole', 'passed', 'championship', 'ferrari', 'stop']</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve">Der Herr ist mein getreuer Hirt , BWV 112 = Der Herr ist mein getreuer Hirt ( The Lord is my faithful Shepherd ) , BWV 112 , is a cantata by Johann Sebastian Bach , a church cantata for the second Sunday after Easter . Bach composed the chorale cantata in Leipzig and first performed it on 8 April 1731 . It is based on the hymn by Wolfgang Meuslin , a paraphrase of Psalm 23 written in 1530 , sung to a melody by Nikolaus Decius . Bach , the Thomaskantor in Leipzig from May 1723 , composed this cantata to complete his second cantata cycle of chorale cantatas , begun in 1724 . He used the lyrics of the hymn unchanged , which reflect the psalm and Jesus as the Good Shepherd . Bach structured the work in five movements . The outer choral movements are a chorale fantasia and a four-part closing chorale , both on the hymn tune . Bach set the inner stanzas as aria – recitative – aria , with music unrelated to the hymn tune . He scored the cantata for four vocal soloists , a four-part choir and </t>
+          <t xml:space="preserve">2011 Canadian Grand Prix = The 2011 Canadian Grand Prix ( formally the Formula 1 Grand Prix du Canada ) was a Formula One motor race held on 12 June 2011 at the Circuit Gilles Villeneuve , in Montreal , Canada . It was the seventh race of the 2011 Formula One season and the 48th Canadian Grand Prix . The 70-lap race was won by McLaren driver Jenson Button after starting from seventh position . Sebastian Vettel , who started from pole position , finished second in a Red Bull with teammate Mark Webber finishing third . The race began behind the safety car , and once it returned to the pits Vettel built a lead over Fernando Alonso . A second safety car deployment caused by the collision of Button and teammate Lewis Hamilton closed the time gaps between cars , but Vettel retained the lead . By lap 26 , increasingly heavy rain led to the race 's suspension , before it was restarted over two hours later . Button was involved in another collision on lap 37 , which led to Alonso 's retirement </t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Lobe den Herrn , meine Seele , BWV 143 = Lobe den Herrn , meine Seele ( Praise the Lord , my soul ) , BWV 143 , is an early cantata by Johann Sebastian Bach . It is not known if he composed the cantata for New Year 's Day in Mühlhausen or Weimar , as the date of composition is unclear . An unknown librettist drew mainly from Psalm 146 and from Jakob Ebert 's hymn " Du Friedefürst , Herr Jesu Christ " to develop seven movements , supplying only two of the movements himself . The text assembly is similar to Bach 's early cantatas . Bach 's authorship is doubted because the cantata has several features unusual for Bach 's later cantatas : it is the only Bach cantata to combine three corni da caccia with timpani . The cantata is in seven movements which combine the three major text sources : psalm , hymn and contemporary poetry . The opening chorus is based on a psalm verse , followed by the first hymn stanza and another psalm verse as a recitative . An aria on poetry is followed by a thir</t>
+          <t>2010 Irwin Tools Night Race = The 2010 Irwin Tools Night Race was a NASCAR Sprint Cup Series stock car race that was held on August 21 , 2010 at Bristol Motor Speedway in Bristol , Tennessee . Contested over 500 laps , it was the twenty-fourth race of the 2010 Sprint Cup Series season . Kyle Busch of Joe Gibbs Racing won the race , while David Reutimann finished second , and Jamie McMurray clinched third . Pole position driver Jimmie Johnson maintained his lead on the first lap to begin the race , as Carl Edwards , who started in the second position on the grid , remained behind him . Afterward , Kyle Busch became the leader , and would eventually lead to the race high of 282 laps . On lap 163 , early race leader , Johnson had collided with Juan Pablo Montoya ; when he returned to the track he was seventy-seven laps behind the leader . David Reutimann led after the final pit stops , ahead of Kyle Busch and Jamie McMurray . With seventy-one laps remaining , Kyle Busch passed Reutimann .</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Unser Mund sei voll Lachens , BWV 110 = Unser Mund sei voll Lachens ( May our mouth be full of laughter ) , BWV 110 , is a church cantata by Johann Sebastian Bach . He composed the Christmas cantata in Leipzig for Christmas Day and first performed it on 25 December 1725 . Bach composed the cantata in his third year as Thomaskantor in Leipzig . He used a text by Georg Christian Lehms , which was published already in 1711 . The text has no recitatives alternating with arias , but instead three biblical quotations , opening with verses from Psalm 26 , then a verse from the Book of Jeremiah about God 's greatness , and finally the angels ' song from the Nativity according to the Gospel of Luke . The closing chorale is taken from Caspar Füger 's " Wir Christenleut " . Bach scored the work festively for four vocal soloists , a four-part choir and a Baroque instrumental ensemble of trumpets and timpani , transverse flutes , different kinds of oboe , strings and basso continuo including bassoo</t>
+          <t>2008 Belgian Grand Prix = The 2008 Belgian Grand Prix ( formally the LXIV ING Belgian Grand Prix ) was a Formula One motor race held on 7 September 2008 at the Circuit de Spa-Francorchamps near the town of Spa , Belgium . It was the 13th race of the 2008 Formula One season . The 44-lap race was won by Felipe Massa for the Ferrari team , after the initial winner , McLaren driver Lewis Hamilton , was penalised for cutting a chicane and gaining an advantage over Ferrari 's Kimi Räikkönen . Hamilton started from pole position alongside title rival Massa . Hamilton 's McLaren teammate Heikki Kovalainen started from third next to the 2007 winner Kimi Räikkönen . Following a spin by Hamilton on the second lap , Räikkönen led most of the race , until rain fell on lap 41 and Hamilton performed the penalised pass . Räikkönen crashed on the following lap as the rain became heavier . Massa finished second on the road after Hamilton , followed by Nick Heidfeld of BMW Sauber . Hamilton received a 25</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Du Friedefürst , Herr Jesu Christ , BWV 116 = Du Friedefürst , Herr Jesu Christ ( You Prince of Peace , Lord Jesus Christ ) , BWV 116 , is a church cantata written by Johann Sebastian Bach in 1724 in Leipzig for the 25th Sunday after Trinity . He led the first performance it on 26 November 1724 , concluding the liturgical year of 1724 . The cantata is based upon Jakob Ebert 's hymn " Du Friedefürst , Herr Jesu Christ " . It matches the Sunday 's prescribed gospel reading , the Tribulation from the Gospel of Matthew , in a general way . The hymn 's first and last stanza are used unchanged in both text and tune : the former is set as a chorale fantasia , the latter as a four-part closing chorale . An unknown librettist paraphrased the inner stanzas as alternating arias and recitatives . Bach scored the cantata for four vocal soloists ( soprano , alto , tenor , bass ) , a four-part choir and a Baroque instrumental ensemble of natural horn , enforcing the soprano in the hymn tune , two obo</t>
+          <t>2007 Indy Japan 300 = The 2007 Indy Japan 300 was an IndyCar Series motor race held on April 21 , 2007 , at the Twin Ring Motegi in Motegi , Tochigi , Japan . It was the third race of the 2007 IndyCar Series season , the fifth annual edition of the Indy Japan 300 in the IndyCar Series , and the tenth anniversary running of the race ( including its five years on the Championship Auto Racing Teams ( CART ) schedule ) . Andretti Green Racing driver Tony Kanaan won the race with a 0.4828 second margin of victory over Chip Ganassi Racing 's Dan Wheldon . Dario Franchitti , Scott Dixon , and Sam Hornish , Jr. rounded out the top five . Hélio Castroneves , the defending champion of the Indy Japan 300 , won the pole position by posting the fastest lap in qualifying . In the race , Wheldon gained the lead from Castroneves on lap 44 and led for more than half of the 200 laps , but a pit stop with 14 laps remaining forced him to relinquish the top position . Kanaan took the lead because of a late</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Es ist das Heil uns kommen her , BWV 9 = Es ist das Heil uns kommen her ( It is our salvation come here to us ) , BWV 9 , is a church cantata by Johann Sebastian Bach . He composed the chorale cantata in Leipzig for the sixth Sunday after Trinity between 1732 and 1735 , based on the hymn " Es ist das Heil uns kommen her " by Paul Speratus . Bach composed the cantata to fill a gap in his cycle of chorale cantatas written for performances in Leipzig from 1724 . The cantata is structured in seven movements , framed as the earlier chorale cantatas by a chorale fantasia and a chorale four-part setting of the first and the twelfth stanza in the original words by the reformer Speratus , published in the First Lutheran Hymnal . The theme is salvation from sin by God 's grace alone . An anonymous librettist paraphrased the content of ten inner stanzas to alternating recitatives and arias . Bach scored the cantata for a chamber ensemble of four vocal parts , flauto traverso , oboe d 'amore , str</t>
+          <t>David Pearson ( racing driver ) = David Gene Pearson ( born December 22 , 1934 ) is a former American stock car racer from Spartanburg , South Carolina . Pearson began his NASCAR career in 1960 and ended his first season by winning the 1960 NASCAR Rookie of the Year award . He won three championships ( 1966 , 1968 , and 1969 ) every year he ran the full schedule in NASCAR 's Grand National Series ( now Sprint Cup Series ) . NASCAR described his 1974 season as an indication of his " consistent greatness " ; that season he finished third in the season points having competed in only 19 of 30 races . At his finalist nomination for NASCAR Hall of Fame 's inaugural 2010 class , NASCAR described Pearson as " ... the model of NASCAR efficiency during his career . With little exaggeration , when Pearson showed up at a race track , he won . " Pearson ended his career in 1986 , and currently holds the second position on NASCAR 's all-time win list with 105 victories ; as well as achieving 113 pol</t>
         </is>
       </c>
     </row>
@@ -1491,32 +1491,32 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>['wickets', 'innings', 'test', 'cricket', 'wicket', 'runs', 'matches', 'australia', 'england', 'scored', 'bowling', 'match', 'bowled', 'overs', 'miller']</t>
+          <t>['episode', 'viewers', 'glee', 'club', 'watched', 'relationship', 'finn', 'rating', 'rachel', 'character', 'tells', 'kurt', 'storyline', 'share', 'demographic']</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve">Munir Malik = Munir Malik ( Urdu : منيرملک ; 10 July 1934 – 30 November 2012 ) was a Pakistani cricketer who played three Tests for Pakistan between 1959 and 1962 . A right-arm fast-medium bowler , he took nine wickets in Test cricket at an average of 39.77 , including a five-wicket haul against England . During his first-class career , he took 197 wickets at the average of 21.75 . = = First-class career = = Malik played 49 first-class matches for Karachi , Punjab , Rawalpindi and Services teams during 1956 – 66 . During his first-class career , he achieved five or more wickets in an innings on fourteen occasions , and ten or more wickets in a match four times . Malik made his first-class debut for Punjab B during the Quaid-e-Azam Trophy , against Bahawalpur in 1956 – 57 . He finished the season taking 13 wickets at an average of 8.30 . His 5 wickets for 19 runs for Punjab B , against Punjab , was his best performance in the season . Malik played three matches during 1957 – 58 and his </t>
+          <t xml:space="preserve">The Substitute ( Glee ) = " The Substitute " is the seventh episode of the second season of the American television series Glee , and the twenty-ninth episode overall . It was written by Ian Brennan , directed by Ryan Murphy , and premiered on Fox on November 16 , 2010 . The episode guest stars Gwyneth Paltrow as Holly Holliday , a substitute teacher who takes the place of glee club director Will Schuester ( Matthew Morrison ) while he is ill . Cheerleading coach Sue Sylvester ( Jane Lynch ) becomes principal of William McKinley High School , and glee club members Mercedes Jones ( Amber Riley ) and Kurt Hummel ( Chris Colfer ) experience tension in their friendship . The episode features cover versions of six songs , which received mixed reviews from critics . While the Glee cover of Cee Lo Green 's " Forget You " and mash-up of " Singin ' in the Rain " with Rihanna 's " Umbrella " attracted critical praise and charted both on the Billboard Hot 100 and internationally , the episode 's </t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1889 – 90 Currie Cup = The 1889 – 90 Currie Cup was the inaugural edition of the Currie Cup , the premier first-class cricket tournament in South Africa . The 1889 – 90 competition involved just two teams , Transvaal and Kimberley . The two sides played a single , three-day match , which was won by Transvaal by six wickets . Both sides made low scores in their first innings ; Kimberley , who had opted to bat first , were dismissed for 98 runs , and in their reply Transvaal reached 117 , a lead of just 19 runs . In the second innings , they both fared better ; a century from Bernard Tancred helped Kimberley to a total of 235 , but Transvaal reached their total in 38 five-ball overs , helped by a century from Monty Bowden . = = Background = = First-class cricket was first played in South Africa in the previous 1888 – 89 season , when Robert Warton managed a side which toured the country , playing against representative teams from each of the provinces , and two matches against South Afri</t>
+          <t xml:space="preserve">A Night of Neglect = " A Night of Neglect " is the seventeenth episode of the second season of the American musical television series Glee , and the thirty-ninth episode overall . It was written by Ian Brennan , directed by Carol Banker , and aired on Fox in the United States on April 19 , 2011 . It features the McKinley High glee club , New Directions , fundraising for a fellow extracurricular activity group by holding a benefit concert , while cheerleading coach Sue Sylvester ( Jane Lynch ) attempts to thwart them . Thirteen guest stars appeared in the episode , including Gwyneth Paltrow in her final season two appearance . Several cast members returned after extended absences : Jessalyn Gilsig , Cheyenne Jackson and Stephen Tobolowsky as members of Sue 's anti-New Directions " League of Doom " , and Charice as student Sunshine Corazon . Four songs were covered and released as singles , and a fifth featured as a dance performance . Upon its initial airing , the episode was viewed by </t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Maurice Fernandes = Maurius Pacheco " Maurice " Fernandes , ( 12 August 1897 – 8 May 1981 ) was a West Indian Test cricketer who played first-class cricket for British Guiana between 1922 and 1932 . He made two Test appearances for the West Indies , in 1928 and 1930 . Fernandes played as a right-handed top-order batsman and occasional wicket-keeper . He scored 2,087 first-class runs in 46 appearances at an average of 28.20 . Graduating from playing at the Demerara Cricket Club as a teenager , to play for British Guiana in 1922 , Fernandes took part in tours of England in 1923 and 1928 . He made his debut Test appearance during the 1928 tour , playing in the first of the three Tests . His next , and final Test match came during the English tour of the West Indies in 1930 . At the time , the West Indies had a practice of picking their captain from the colony that the match was being played in , and Fernandes was granted the honour for the match in British Guiana . The West Indies won the</t>
+          <t>Acafellas = " Acafellas " is the third episode of the American television series Glee . The episode premiered on the Fox network on September 16 , 2009 . It was directed by John Scott and written by series creator Ryan Murphy . The episode sees glee club director Will Schuester ( Matthew Morrison ) form an all-male a cappella group , the Acafellas , neglecting the club in favor of dedicating his time to the new endeavor . New Directions struggle with choreography , and resist attempts at sabotage by members of the cheer squad . Mercedes ( Amber Riley ) harbors romantic feelings for Kurt ( Chris Colfer ) , who comes out as homosexual . Singer Josh Groban guest stars as himself , John Lloyd Young appears as wood shop teacher Henri St. Pierre , and Victor Garber and Debra Monk play Will 's parents . The episode features covers of seven songs , including the instrumental piece " La Camisa Negra " performed on guitar by Mark Salling . Studio recordings of two of the songs performed were rel</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Haseeb Ahsan = Haseeb Ahsan ( Urdu : حسيب احسن ; 15 July 1939 – 8 March 2013 ) was a Pakistani cricketer who played 12 Tests for Pakistan between 1958 and 1962 . He was born in Peshawar , Khyber Pakhtunkhwa . A right-arm off spinner , he took 27 wickets in Test cricket at an average of 49.25 , including two five-wicket hauls . During his first-class career , he played 49 matches and took 142 wickets at an average of 27.71 . Former Pakistan cricketer Waqar Hasan said about him that he " was a fighter to the core and served Pakistan cricket with honour and dignity . " Ahsan had conflicts with former Pakistan captain Javed Burki . A controversy regarding his bowling action resulted in the premature end of his international career when he was only 23 . He worked as chief selector , team manager of Pakistan , and member of the 1987 Cricket World Cup organising committee . He died in Karachi on 8 March 2013 , aged 73 . = = Cricketing career = = Ahsan played 49 first-class matches for Pakista</t>
+          <t>The Power of Madonna = " The Power of Madonna " is the fifteenth episode of the American television series Glee . The episode premiered on the Fox network on April 20 , 2010 . When cheerleading coach Sue Sylvester ( Jane Lynch ) demands that Madonna 's music be played over the school intercom system , glee club director Will Schuester ( Matthew Morrison ) sets the club a Madonna-themed assignment , hoping to empower the female club members . " The Power of Madonna " was written and directed by series creator Ryan Murphy , and serves as a musical tribute to Madonna , featuring cover versions of eight of her songs , with the singer having granted Glee the rights to her entire catalogue of music . Glee : The Music , The Power of Madonna , an album containing studio recordings of songs performed in the episode , was released on April 20 , 2010 . The episode was watched by 12.98 million American viewers , and was generally well received by critics . Tim Stack of Entertainment Weekly and Aly</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Steph Davies = Stephanie Ann Davies , commonly known as Steph Davies , ( born 21 October 1987 ) is an international cricketer who has represented the England women 's cricket team in four One Day Internationals ( ODIs ) . A right-arm medium-fast bowler and right-handed attacking batsman , she has played for Somerset women since 2001 . After making her county debut for Somerset at the age of 13 , Davies quickly progressed into the England development and youth sides . She toured Australia with England Under-19s aged 15 and after two successful European tournaments , she captained the England Under-21s to victory in the 2006 Under-21 European Championships . After more matches for the development squad , and a number of tour matches for England , she made her ODI debut during the 2007 – 08 tour of Australia and New Zealand , playing the fifth and final one-day match against Australia , and three of the five matches against New Zealand . Following this , she continued to be involved in th</t>
+          <t>New Guys = " New Guys " is the first episode of the ninth season of the American comedy television series The Office , and the show 's 177th episode overall . It originally aired on NBC on September 20 , 2012 . The episode was written and directed by series creator Greg Daniels ; this is his first writing credit for the series since the seventh season episode " Goodbye , Michael " , and his first directing credit since " PDA " . The series depicts the everyday lives of office employees in the Scranton , Pennsylvania branch of the fictional Dunder Mifflin Paper Company . In this episode , two new employees ( Clark Duke and Jake Lacy ) are hired by the Scranton branch and cause trouble for Dwight Schrute ( Rainn Wilson ) and Jim Halpert ( John Krasinski ) . Andy Bernard ( Ed Helms ) returns from manager training , hoping for revenge on Nellie Bertram ( Catherine Tate ) . Oscar Martinez ( Oscar Nunez ) considers adopting Angela Lipton 's ( Angela Kinsey ) cat . Kevin Malone ( Brian Baumga</t>
         </is>
       </c>
     </row>
@@ -1526,32 +1526,32 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>['hitler', 'holocaust', 'physics', 'jews', 'nazi', 'nuclear', 'germany', 'manhattan_project', 'atomic', 'berlin', 'jewish', 'nobel', 'german', 'munich', 'research']</t>
+          <t>['time', 'year', 'world', 'won', 'games', 'record', 'team', 'years', 'title', 'season', 'final', 'second', 'player', 'win', 'best']</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Henry DeWolf Smyth = Henry DeWolf " Harry " Smyth ( / ˈhɛnri dəˈwʊlf ˈsmaɪθ / ; May 1 , 1898 – September 11 , 1986 ) was an American physicist , diplomat , and bureaucrat . He played a number of key roles in the early development of nuclear energy , as a participant in the Manhattan Project , a member of the U.S. Atomic Energy Commission ( AEC ) , and U.S. ambassador to the International Atomic Energy Agency ( IAEA ) . Educated at Princeton University and the University of Cambridge , he was a faculty member in Princeton 's Department of Physics from 1924 to 1966 . He chaired the department from 1935 to 1949 . His early research was on the ionization of gases , but his interests shifted toward nuclear physics beginning in the mid-1930s . During World War II he was a member of the National Defense Research Committee 's Uranium Section and a consultant on the Manhattan Project . He wrote the Manhattan Project 's first public official history , which came to be known as the Smyth Report .</t>
+          <t>Milos Raonic = Milos Raonic ( / ˈmiːloʊʃ ˈraʊnɪtʃ / MEE-lohsh ROW-nich ; Serbian : Милош Раонић , Miloš Raonić [ mîloʃ râonitɕ ] ; born December 27 , 1990 ) is a Canadian professional tennis player . He reached a career-high world No. 4 singles ranking on May 11 , 2015 , as ranked by the Association of Tennis Professionals ( ATP ) . His career highlights include a Grand Slam final at the 2016 Wimbledon Championships ; two Grand Slam semifinals at the 2014 Wimbledon Championships and 2016 Australian Open ; and three ATP World Tour Masters 1000 finals at the 2013 Canadian Open , 2014 Paris Masters , and 2016 Indian Wells Masters . Raonic first gained international acclaim by reaching the fourth round of the 2011 Australian Open as a qualifier , being referred to as " the real deal " , " a new star " , part of " a new generation " , and " a future superstar " . Coupled with his first ATP World Tour title three weeks later , his world ranking rose from No. 152 to No. 37 in one month . He w</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Julius Schreck = Julius Schreck ( 13 July 1898 – 16 May 1936 ) was a senior Nazi official and close confidant of Adolf Hitler . Born on 13 July 1898 in Munich , Schreck served in World War I and shortly afterwards joined right-wing paramilitary units . He joined the Nazi Party in 1920 and developed a close friendship with Adolf Hitler . Schreck was a founding member of the Sturmabteilung ( " Storm Department " ; SA ) and was active in its development . Later in 1925 , he became the first leader of the Schutzstaffel ( " Protection Squadron " ; SS ) . He then served for a time as a chauffeur for Hitler . Schreck developed meningitis in 1936 and died on 16 May . Hitler gave him a state funeral which was attended by several members of the Nazi elite with Hitler delivering the eulogy . = = Early life = = Julius Schreck was born on 13 July 1898 in Munich , a largely Catholic city in Bavaria . He served in the German Army during World War I. After the war ended in November 1918 , he became a </t>
+          <t xml:space="preserve">César Cielo = César Cielo Filho ( Portuguese pronunciation : [ ˈsɛzɐɾ si.ˈelu ˈfiʎu ] , born 10 January 1987 ) is a Brazilian competitive swimmer who specializes in sprint events . He is the most successful Brazilian swimmer in history , having obtained three Olympic medals , winning six individual World Championship gold medals and breaking two world records . Cielo is the current world record holder in the 100-metre and 50-metre freestyle ( long course ) . His gold medal at the 2008 Summer Olympics , in the 50-metre freestyle competition , is Brazil 's only Olympic gold in swimming to date . In 2008 , he broke the NCAA record in the 50-yard ( 46 m ) freestyle ( 18.47 seconds ) and in the 100-yard ( 91 m ) freestyle ( 40.92 seconds ) . Cielo became the fastest swimmer in the world in the two distances , and was named NCAA Swimmer of the Year for the second year in a row . = = Early life = = César Cielo was born on January 10 , 1987 in Santa Bárbara d 'Oeste , São Paulo , Brazil . The </t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Robert Brode = Robert Bigham Brode ( June 12 , 1900 – February 19 , 1986 ) was an American physicist , who during World War II led the group at the Manhattan Project 's Los Alamos laboratory that developed the fuses used in the atomic bombing of Hiroshima and Nagasaki . A graduate of the California Institute of Technology , where he earned his doctorate in 1924 , Brode attended Oxford University on a Rhodes Scholarship and the University of Göttingen on a National Research Council Fellowship . During World War II , Brode worked at Applied Physics Laboratory at Johns Hopkins University , where he helped develop the proximity fuse , and then as a group leader at the Los Alamos Laboratory . In 1950 he was one of a dozen prominent scientists who petitioned President Harry S. Truman to declare that the United States would never be the first to use the hydrogen bomb . After the war , Brode returned to teaching at Berkeley . Between 1930 and 1957 he supervised 37 graduate students . In additi</t>
+          <t>Tyson Gay = Tyson Gay ( born August 9 , 1982 ) is an American track and field sprinter , who competes in the 100 and 200 meters dash . His 100 m personal best of 9.69 seconds is the American record and makes him tied for second fastest athlete ever , after Usain Bolt . His 200 m time of 19.58 makes him the sixth fastest athlete in that event . He has since received a one-year ban for doping . Gay has won numerous medals in major international competitions , including a gold medal sweep of the 100 m , 200 m and 4 × 100 m relay at the 2007 Osaka World Championships . This made him the second man to win all three events at the same World Championships , after Maurice Greene ( Usain Bolt duplicated the feat two years later ) . Gay is a four-time U.S. champion in the 100 m . At the 2008 Olympic Trials , he ran a wind assisted 9.68 seconds in the 100 m . Days after he suffered a severe hamstring injury in the 200 m trials and did not win any medals at the Beijing Olympics . His performance o</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Adolf Hitler = Adolf Hitler ( German : [ ˈadɔlf ˈhɪtlɐ ] ; 20 April 1889 – 30 April 1945 ) was a German politician who was the leader of the Nazi Party ( Nationalsozialistische Deutsche Arbeiterpartei ; NSDAP ) , Chancellor of Germany from 1933 to 1945 , and Führer ( " leader " ) of Nazi Germany from 1934 to 1945 . As dictator of Nazi Germany , he initiated World War II in Europe with the invasion of Poland in September 1939 and was a central figure of the Holocaust . Hitler was born in Austria , then part of Austria-Hungary , and raised near Linz . He moved to Germany in 1913 and was decorated during his service in the German Army in World War I. He joined the German Workers ' Party , the precursor of the NSDAP , in 1919 and became leader of the NSDAP in 1921 . In 1923 , he attempted a coup in Munich to seize power . The failed coup resulted in Hitler 's imprisonment , during which time he dictated the first volume of his autobiography and political manifesto Mein Kampf ( " My Struggl</t>
+          <t>Magnus Carlsen = Sven Magnus Øen Carlsen ( Norwegian : [ sʋɛn ˈmɑŋnʉs øːn ˈkɑːɭsn ̩ ] ; born 30 November 1990 ) is a Norwegian chess grandmaster , and the current World Chess Champion . Carlsen is a former chess prodigy . He became a Grandmaster in 2004 , at the age of 13 years , 148 days . This made him the third youngest grandmaster in history . In November 2013 Carlsen became World Champion by defeating Viswanathan Anand in the World Chess Championship 2013 . On the May 2014 FIDE rating list , Carlsen reached his peak rating of 2882 , which is the highest in history . He successfully defended his title in November 2014 , once again defeating Anand . The same year , he also won the World Rapid Championship and the World Blitz Championship , thus holding all three world championship titles . In 2015 Carlsen won the inaugural Grand Chess Tour , a series of three supertournaments featuring the 10 best chess grandmasters in the world . Carlsen was known for his attacking style as a teena</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Mujaddid Ahmed Ijaz = Mujaddid Ahmed Ijaz , Ph.D. ( Urdu : مجدد احمد اعجا ز ; June 12 , 1937 — July 9 , 1992 ) , was a Pakistani-American experimental physicist noted for his role in discovering new isotopes that expanded the neutron-deficient side of the atomic chart . Some of the isotopes he discovered enabled significant advances in medical research , particularly in the treatment of cancer , and further advanced the experimental understanding of nuclear structures . Ijaz conducted his research work at Oak Ridge National Laboratories ( ORNL ) . He and his ORNL colleagues published more than 60 papers in physics journals announcing isotope discoveries and other results of their accelerator experiments from 1968 until 1983 . Ijaz participated in the U.S. Atoms for Peace initiative during the 1970s . The program provided a number of third-world countries , including Pakistan , with civilian nuclear reactor technology to develop energy for peaceful purposes . As a tenured professor of P</t>
+          <t>Counter Logic Gaming = Counter Logic Gaming ( CLG ) is an American eSports organization headquartered in Los Angeles , California . It was founded in April 2010 by George " HotshotGG " Georgallidis and Alexander " Vodoo " Beutel as a League of Legends team , and has since branched out into other games . CLG fields the oldest League of Legends team still active , having competed in every split of the North American League of Legends Championship Series ( LCS ) since it began in Spring 2013 . CLG has won two NA LCS splits , the 2015 Summer NA LCS and 2016 Spring NA LCS . The team has also attended the 2012 and 2015 League of Legends World Championships , and was eliminated in the group stage on both occasions . The organization also fields Halo , Counter-Strike : Global Offensive ( CS : GO ) , Super Smash Bros. , and Call of Duty teams , and previously included a Dota 2 team . The organization was also one of the first in North America to implement a multi-team gaming house , and the cur</t>
         </is>
       </c>
     </row>
@@ -1561,32 +1561,32 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>['ride', 'coaster', 'roller', 'riders', 'train', 'flags', 'coasters', 'park', 'cedar', 'lift', 'attraction', 'drop', 'queue', 'trains', 'rides']</t>
+          <t>['game', 'player', 'mario', 'mega', 'gameplay', 'graphics', 'praised', 'enemies', 'players', 'ign', 'controls', 'gaming', 'sonic', 'arcade', 'console']</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Dive Coaster = The Dive Coaster is a steel roller coaster manufactured by Bolliger &amp; Mabillard where riders experience a moment of free-falling with at least one 90-degree drop . Unlike other roller coasters where the lift hill takes the train directly to the first drop , a Dive Coaster lift hill leads to a flat section of track followed by a holding brake which stops the train just as it enters the vertical drop . After a few seconds , the train is released into the drop . Development of the Dive Coaster began between 1994 and 1995 with Oblivion at Alton Towers opening on March 14 , 1998 , making it the world 's first Dive Coaster . The trains for this type of coaster are relatively short consisting of two to three cars . Bolliger &amp; Mabillard have recently begun to also use floorless trains on this model to enhance the experience . As of May 2016 , ten Dive Coasters have been built , with the newest being Valravn at Cedar Point . = = History = = According to Walter Bolliger , developm</t>
+          <t>Super Punch-Out ! ! = Super Punch-Out ! ! ( スーパーパンチアウト ！ ！ , Sūpā Panchi-Auto ! ! ) is a boxing video game developed and published by Nintendo for the SNES . It was released on September 14 , 1994 in North America and again in the same region in 1996 . It was released in Europe on January 26 , 1995 for the same console and in Japan in 1998 for the Nintendo Power flash RAM cartridge series and the Super Famicom . The game was released for the Wii 's Virtual Console in Europe on March 20 , 2009 , in North America on March 30 , 2009 , and in Japan on July 7 , 2009 . The game was also released on the New Nintendo 3ds eShop on May 5 , 2016 . It is the fourth game in the Punch-Out ! ! series , taking place after the Punch-Out ! ! game for the NES . In Super Punch-Out ! ! the player controls Little Mac , as he fights his way to become the World Video Boxing Association champion . Players , fighting from a " behind the back " perspective , must knockout their opponent in three minutes to win .</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bolliger &amp; Mabillard = Bolliger &amp; Mabillard , abbreviated B &amp; M and formally known as Bolliger &amp; Mabillard Consulting Engineers Inc . , is a roller coaster design consultancy based in Monthey , Switzerland . The company was founded in 1988 by Walter Bolliger and Claude Mabillard , with Bolliger as president and Mabillard as vice-president . Since 1988 , B &amp; M has built 100 roller coasters around the world and have pioneered several new ride technologies , most notably the inverted roller coaster . Since 1990 , all coasters designed by B &amp; M that have been built within North America have been manufactured by Clermont Steel Fabricators which is located in Batavia , Ohio , United States . B &amp; M started with four employees and has since grown ; as of 2012 it employs 37 people , mostly engineers and draftsmen . In 2016 the company completed its 100th coaster . = = History = = Walter Bolliger and Claude Mabillard starting working for Giovanola , a manufacturing company who supplied rides to </t>
+          <t>Dr. Mario = Dr. Mario ( Japanese : ドクターマリオ , Hepburn : Dokutā Mario , often stylized as D ℞ . Mario ) is a 1990 Mario arcade-style action puzzle video game designed by Gunpei Yokoi and produced by Takahiro Harada . Nintendo developed and published the game for the Nintendo Entertainment System and Game Boy consoles . The game 's soundtrack was composed by Hirokazu Tanaka . The game focuses on the player character Mario , who assumes the role of a doctor and is tasked with eradicating deadly viruses . In this falling block puzzle game , the player 's objective is to destroy the viruses populating the on-screen playing field by using colored capsules that are dropped into the field . The player manipulates the capsules as they fall so that they are aligned with viruses of matching colors , which removes them from play . The player progresses through the game by eliminating all the viruses on the screen in each level . Dr. Mario received positive reception , appearing on several " Best Ni</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t xml:space="preserve">Tatsu = Tatsu is a steel flying roller coaster designed by Bolliger &amp; Mabillard at the Six Flags Magic Mountain amusement park located in Valencia , California . Announced on November 17 , 2005 , the roller coaster opened to the public on May 13 , 2006 as the park 's seventeenth roller coaster . Tatsu reaches a height of 170 feet ( 52 m ) and speeds up to 62 miles per hour ( 100 km / h ) . The ride 's name comes from Japanese mythology and means Flying Beast in Japanese . The roller coaster is also the world 's tallest and fastest flying coaster ; is the only flying roller coaster to feature a zero-gravity roll ; and has the world 's highest pretzel loop . It was the world 's longest flying coaster until The Flying Dinosaur surpassed it . In the roller coaster 's opening year , it was named the 40th best roller coaster in the world in Amusement Today 's Golden Ticket Awards ; in Mitch Hawker 's Best Steel Roller Coaster Poll , the roller coaster placed at the 34 position . = = History </t>
+          <t>Stealth game = A stealth game is a type of video game that tasks the player with using stealth to avoid or overcome antagonists . Games in the genre typically allow the player to remain undetected by hiding , using disguises , and / or avoiding noise . Some games allow the player to choose between a stealthy approach or directly attacking antagonists , perhaps rewarding the player for greater levels of stealth . The genre has employed espionage , counter-terrorism and rogue themes , with protagonists who have been identified as special forces operatives , spies , thieves , ninjas , and assassins . Some games have also combined stealth elements with other genres , such as first-person shooters and even platformers . Some of the early games emphasizing stealth include Manbiki Shounen ( 1979 ) , Lupin III ( 1980 ) , 005 ( 1981 ) , Castle Wolfenstein ( 1981 ) , Infiltrator ( 1986 ) , Metal Gear ( 1987 ) , and Metal Gear 2 : Solid Snake ( 1990 ) . The genre became popular in 1998 , with the</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Batman : The Dark Knight ( roller coaster ) = Batman : The Dark Knight ( formerly known as Batman : The Ride ) is a steel floorless roller coaster designed by Bolliger &amp; Mabillard located in the south end of Six Flags New England . The roller coaster has 2,600 feet ( 790 m ) of track , reaches a maximum height of 117.8 feet ( 35.9 m ) , and features five inversions . The coaster was announced on February 6 , 2002 and opened to the public on April 20 , 2002 . In 2008 , the ride 's name was changed to Batman : The Ride to avoid confusion with The Dark Knight Coaster that was planned to be built at the park ; after the project was cancelled , the ride 's name reverted to its original . = = History = = Batman : The Dark Knight was announced to the public on February 6 , 2002 though construction had started in September 2001 . After construction and testing was completed by Martin &amp; Vleminckx , the ride officially opened on April 20 , 2002 . In 2007 , Six Flags announced three The Dark Knig</t>
+          <t>X-Men Legends = X-Men Legends is an action role-playing video game developed by Raven Software and published by Activision . It was released on the GameCube , PlayStation 2 and Xbox consoles in the fall of 2004 . Barking Lizards Technologies developed the N-Gage port of the game , which was released in early 2005 . Players can play as one of fifteen X-Men characters , with the ability to switch between four computer- or human-controlled characters at any time . X-Men Legends follows Alison Crestmere , a young mutant who has the ability to summon and control volcanic activity . As Alison is taught to control her powers at the X-Mansion , the X-Men are sent on several missions . Eventually the X-Men learn of Magneto 's plan to cover the Earth in darkness from his base on Asteroid M. X-Men Legends received generally positive reviews from critics . The Xbox version was the best received , garnering aggregate scores of 83 % and 82 / 100 on the review aggregating websites GameRankings and Me</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Kumba ( roller coaster ) = Kumba is a Bolliger &amp; Mabillard sit down roller coaster located at Busch Gardens Tampa Bay , in Tampa , Florida . Opened in 1993 , it stands 143 feet ( 44 m ) tall and has a top speed of 60 miles per hour ( 97 km / h ) . Kumba features a total of seven inversions across the 3-minute ride . = = History = = Kumba was officially announced in November 1992 as a record-breaking Bolliger &amp; Mabillard roller coaster set to become the park 's signature attraction . The ride officially opened to the public on April 20 , 1993 . When Kumba opened , it featured the world 's tallest vertical loop , and was also the tallest , fastest and longest roller coaster in Florida . In 1995 , Kumba conceded the title of ride with the world 's tallest vertical loop to Dragon Khan at PortAventura which features a 118-foot-tall ( 36 m ) vertical loop . In 1996 , it conceded Florida 's titles of tallest and longest roller coaster to Montu , a Bolliger &amp; Mabillard roller coaster in the Eg</t>
+          <t>The Legend of Zelda : The Minish Cap = The Legend of Zelda : The Minish Cap ( / ˈmɪnɪʃ / ) ( Japanese : ゼルダの伝説 ふしぎのぼうし , Hepburn : Zeruda no Densetsu : Fushigi no Bōshi , lit . The Legend of Zelda : The Mysterious Cap ) is an action-adventure game and the twelfth entry in the The Legend of Zelda series . Developed by Capcom , with Nintendo overseeing the development process , it was released for the Game Boy Advance handheld game console in Japan and Europe in 2004 and in North America and Australia the following year . The Minish Cap is the third Zelda game that involves the legend of the Four Sword , expanding on the story of Four Swords and Four Swords Adventures . A magical talking cap named Ezlo can shrink series protagonist Link to the size of the Minish , a bug-sized race that live in Hyrule . The game retains some common elements from previous Zelda installments , such as the presence of Gorons , while introducing Kinstones and other new gameplay features . The Minish Cap was g</t>
         </is>
       </c>
     </row>
@@ -1596,32 +1596,32 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>['chicken', 'cheese', 'fried', 'sandwich', 'wine', 'dishes', 'recipes', 'dish', 'cream', 'cuisine', 'cooking', 'food', 'ingredients', 'bacon', 'meat']</t>
+          <t>['series', 'character', 'television', 'season', 'episodes', 'episode', 'characters', 'story', 'cast', 'dvd', 'aired', 'doctor', 'viewers', 'producer', 'seasons']</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Beurre Maître d 'Hôtel = Beurre Maître d 'Hôtel , also referred to as Maître d 'Hôtel butter , is a type of compound butter ( French : " Beurre composé " ) of French origin , prepared with butter , parsley , lemon juice , salt and pepper . It is a savory butter that is used on meats such as steak ( including the chateaubriand sauce for chateaubriand steak ) , fish , vegetables and other foods . It may be used in place of a sauce , and can significantly enhance a dish 's flavor . Some variations with a sweet flavor exist . It is usually served cold as sliced disks on foods , and is sometimes served as a side condiment . = = Etymology = = The name of Beurre Maître d 'Hôtel is derived from the manner in which it was commonly prepared from scratch by a restaurant 's maître d 'hôtel at diners ' tables . It is also referred to as Maître d 'Hôtel butter . = = Preparation = = Beurre Maître d 'Hôtel is a savory butter prepared by mixing softened butter with very finely minced parsley , lemon ju</t>
+          <t>Doctor Who ( series 5 ) = The fifth series of British science fiction television programme Doctor Who began on 3 April 2010 with " The Eleventh Hour " and ended with " The Big Bang " on 26 June 2010 . The series was led by head writer and executive producer Steven Moffat , who took over after Russell T Davies , who ended his involvement with the show after The End of Time . The series comprises 13 episodes , six of which Moffat wrote . Piers Wenger and Beth Willis served with Moffat as executive producers , while Tracie Simpson and Peter Bennett served as producers . Though it is the fifth series since the show 's revival in 2005 and the thirty-first since it began in 1963 , the largely new production team led to the series production codes being reset . This is the first series to feature Matt Smith as the eleventh incarnation of the Doctor , an alien Time Lord who travels through time and space in his TARDIS , which appears to be a British police box on the outside . It also introduc</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Applesauce cake = Applesauce cake is a dessert cake prepared using apple sauce , flour and sugar as primary ingredients . Various spices are typically used , and it tends to be a moist cake . Applesauce cake prepared with chunky-style apple sauce may be less moist . Several additional ingredients may also be used in its preparation , and it is sometimes prepared and served as a coffee cake . The cake dates back to early colonial times in the United States . National Applesauce Cake Day occurs annually on June 6 in the U.S. = = History = = The preparation of applesauce cake dates back to early colonial times in the New England Colonies of the northeastern United States . From 1900 to the 1950s , recipes for applesauce cake frequently appeared in American cookbooks . In the United States , National Applesauce Cake Day occurs annually on June 6 . = = Ingredients and preparation = = Applesauce cake is a dessert cake prepared using apple sauce , flour and sugar as main ingredients . Store-b</t>
+          <t xml:space="preserve">Ninth Doctor = The Ninth Doctor is an incarnation of the Doctor , the protagonist of the BBC science fiction television programme Doctor Who . He is portrayed by Christopher Eccleston during the first series of the show 's revival in 2005 . Within the programme 's narrative , the Doctor is a time travelling , humanoid alien from a race known as the Time Lords . When the Doctor is critically injured , he can regenerate his body but in doing so gains a new physical appearance and with it , a distinct new personality . The production team 's approach to the character and Eccleston 's portrayal were highlighted as being intentionally different from his predecessors , with Eccleston stating that his character would be less eccentric . To fit in with a 21st-century audience , the Doctor was given a primary companion , Rose Tyler , who was designed to be as independent and courageous as himself . He also briefly travels with Adam Mitchell , a self-serving boy genius who acts as a foil to the </t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Avocado cake = Avocado cake is a cake prepared using avocado as a primary ingredient , together with other typical cake ingredients . The avocados may be mashed , and may be used as an ingredient in cake batter , in cake toppings and alone atop a cake . Cake variations include raw avocado cake , avocado brownies and avocado cheesecake . Raw , uncooked versions of avocado cake can be high in vitamin E and essential fatty acids , which are derived from avocado . Avocado-based cake toppings include avocado fool and avocado crazy . = = Overview = = Avocado is a main ingredient in avocado cake , along with other typical cake ingredients . Various varieties of avocados may be used . Avocado cake may have a subtle avocado flavor imbued in the dish . Mashed avocado may be used as an ingredient in the batter and in cake frostings and toppings . Sliced avocado may be used to top or garnish it , as may other ingredients such as the zest of citrus fruits . Additional ingredients used may include y</t>
+          <t>Star Trek : The Next Generation ( season 2 ) = The second season of the American science fiction television series Star Trek : The Next Generation commenced airing in broadcast syndication in the United States on November 21 , 1988 , and concluded on July 17 , 1989 , after airing 22 episodes . Set in the 24th century , the series follows the adventures of the crew of the Starfleet starship Enterprise-D. Season two featured changes to the main cast , following the departure of Gates McFadden . Diana Muldaur was cast as Dr. Katherine Pulaski for a single season before the return of McFadden in season three . Academy Award winner Whoopi Goldberg also joined the cast after pursuing a role from the producers . There were significant changes backstage to the writing team . Maurice Hurley became head writer , and following extensive re-writes to " The Royale " and " Manhunt " , Tracy Tormé left the writing team . Likewise , following the submission of a script for " Blood and Fire " , David G</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Carrot soup = Carrot soup ( referred to in French as Potage de Crécy , Potage Crécy , Potage à la Crécy , Purée à la Crécy and Crème à la Crécy ) is a soup prepared with carrot as a primary ingredient . It may be prepared as a cream- or broth-style soup . Additional vegetables , root vegetables and various other ingredients may be used in its preparation . It may be served hot or cold , and several recipes exist . Carrot soup has been described as a " classic " dish in French cuisine . The soup was eaten by King Edward VII every year on 26 August to commemorate the 1346 Battle of Crécy . = = Overview = = Carrot soup may be prepared as a cream-style soup and as a broth-style soup . Vegetable stock or chicken stock may be used as ingredients in both styles of soup . Other vegetables may be used in the dish , including root vegetables , the latter of which may include garlic onion , shallot , potato , turnip and others . Carrot juice and orange juice may be used in its preparation , and s</t>
+          <t>Sanctuary ( season 1 ) = The first season of the Canadian science fiction – fantasy television series Sanctuary premiered on the Sci Fi Channel in the United States on October 3 , 2008 , and concluded on ITV4 in the United Kingdom on January 5 , 2009 , after 13 episodes . It follows the actions of a secret organization known as the Sanctuary , who track down a series of creatures known as abnormals , and then bring them to the Sanctuary for refuge . The main story arc of the season involves the Sanctuary working against the Cabal , an organization who seek to control all abnormals for their own gain . Amanda Tapping , Robin Dunne , Emilie Ullerup , and Christopher Heyerdahl are billed in the opening credits as the main cast . Initially an eight-part web series , Sanctuary was successful enough for Sci Fi to commission a television series . Series creator and head writer Damian Kindler hired Sam Egan , and the two wrote all the episodes and composed the season-long storyline . Many epis</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Israeli cuisine = Israeli cuisine ( Hebrew : המטבח הישראלי ha-mitbach ha-yisra ’ eli ) comprises local dishes by people native to Israel and dishes brought to Israel by Jews from the Diaspora . Since before the establishment of the State of Israel in 1948 , and particularly since the late 1970s , an Israeli Jewish fusion cuisine has developed . Israeli cuisine has adopted , and continues to adapt , elements of various styles of Jewish cuisine , particularly the Mizrahi , Sephardic and Ashkenazi styles of cooking . It incorporates many foods traditionally eaten in Levantine , Middle Eastern and Mediterranean cuisines , and foods such as falafel , hummus , msabbha , shakshouka , couscous , and za 'atar are now widely popular in Israel . Other influences on the cuisine are the availability of foods common to the Mediterranean region , especially certain kinds of fruits and vegetables , dairy products and fish ; the distinctive traditional dishes prepared at holiday times ; the tradition o</t>
+          <t>Daredevil ( season 2 ) = The second season of the American web television series Daredevil , which is based on the Marvel Comics character of the same name , follows Matt Murdock / Daredevil , a blind lawyer-by-day who fights crime at night , crossing paths with the deadly Frank Castle / Punisher along with the return of an old girlfriend – Elektra Natchios . It is set in the Marvel Cinematic Universe ( MCU ) , sharing continuity with the films and other television series of the franchise . The season is produced by Marvel Television in association with ABC Studios , with Doug Petrie and Marco Ramirez serving as showrunners , and series creator Drew Goddard acting as consultant . Charlie Cox stars as Murdock , while Jon Bernthal and Élodie Yung are introduced as Castle and Natchios . Deborah Ann Woll , Elden Henson , Rosario Dawson , and Vincent D 'Onofrio also return from the first season , with Stephen Rider joining them . The season was ordered in April 2015 after the successful rel</t>
         </is>
       </c>
     </row>
@@ -1631,32 +1631,32 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>['buenos_aires', 'soviet', 'argentina', 'argentine', 'revolution', 'cuban', 'dictator', 'drug', 'government', 'soviet_union', 'mafia', 'cuba', 'spanish', 'political', 'spain']</t>
+          <t>['campaign', 'said', 'announced', 'stated', 'saying', 'support', 'election', 'media', 'party', 'political', 'criticized', 'government', 'president', 'leader', 'presidential']</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Last use of capital punishment in Spain = The last use of capital punishment in Spain took place on 27 September 1975 when two members of the armed Basque nationalist and separatist group ETA political-military and three members of the Revolutionary Antifascist Patriotic Front ( FRAP ) were shot dead by firing squads after having been convicted and sentenced to death by military tribunals for the murder of policemen and civil guards . Spain was Western Europe 's last dictatorship at this time and had been unpopular and internationally isolated in the post-war period due to its relations with Nazi Germany in the 1930s and the fact that the authoritarian Spanish leader , Francisco Franco , had come to power by overthrowing a democratically elected government . As a result , the executions resulted in substantial criticism of the Spanish government , both domestically and abroad . Reactions included street protests , attacks on Spanish embassies , international criticism of the Spanish go</t>
+          <t>Scottish Labour Party leadership election , 2014 = The 2014 Scottish Labour Party leadership election was an internal party election to choose a new leader and deputy leader of the Scottish Labour Party , following the resignations of Johann Lamont as leader and Anas Sarwar as deputy . Lamont announced her decision in an interview with the Daily Record on 24 October , saying that she was stepping down effective immediately because the UK Labour Party treated the Scottish party as a " branch office of London " . Lamont , who had won the 2011 leadership contest , thus becoming the first Scottish leader to have authority over Labour 's Scottish MPs in the House of Commons as well as in the Scottish Parliament , was the second leader of a Scottish political party to resign in the wake of the 2014 independence referendum . Before her resignation , Alex Salmond announced his intention to relinquish the role of Scottish National Party ( SNP ) leader and First Minister . Sarwar announced his o</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ricardo Arias Calderón = Ricardo Arias Calderón ( born 4 May 1933 ) is a Panamanian politician who served as First Vice President from 1989 to 1992 . A Roman Catholic who studied at Yale and the Sorbonne , Arias returned to Panama in the 1960s to work for political reform . He went on to become the president of the Christian Democratic Party of Panama and a leading opponent of the military government of Manuel Noriega . In 1984 , he ran as a candidate for Second Vice President on the ticket of three-time former president Arnulfo Arias , but they were defeated by pro-Noriega candidate Nicolás Ardito Barletta . Following an annulled 1989 election and the US invasion of Panama later in the same year , Arias Calderón was sworn in as First Vice President of Panama under President Guillermo Endara . After growing tensions in the ruling coalition , Arias resigned his position on December 17 , 1992 , stating that the government had not done enough to help Panama 's people . He continued to be </t>
+          <t xml:space="preserve">Premiership of Gordon Brown = The premiership of Gordon Brown began on 27 June 2007 when Brown accepted the Queen 's invitation to form a government , replacing Tony Blair as the Prime Minister of the United Kingdom . It ended with his resignation as Prime Minister on 11 May 2010 . While serving as Prime Minister , Brown also served as the First Lord of the Treasury , the Minister for the Civil Service and the Leader of the Labour Party . He was succeeded as Prime Minister by David Cameron Brown 's style of government differed from that of Tony Blair , who had been seen as presidential . Brown rescinded some of the policies which had been introduced or were planned by Blair 's administration . He remained committed to close ties with the United States and to the war in Iraq , although he established an inquiry into the reasons for Britain 's participation in the conflict . He proposed a " government of all the talents " which would involve co-opting leading personalities from industry </t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Adolfo Rodríguez Saá = Adolfo Rodríguez Saá ( born July 25 , 1947 ) is an Argentine Peronist politician . Born in a family that was highly influential in the history of the San Luis Province , he became governor in 1983 , after the end of the National Reorganization Process military dictatorship . He remained governor up to 2001 , being re-elected in successive elections . President Fernando de la Rúa resigned in that year , amid the December 2001 riots , and the Congress appointed Rodríguez Saá as president of Argentina . In response to the 1998 – 2002 Argentine great depression , he declared the highest sovereign default in history and resigned days later amid civil unrest . The Congress appointed a new president , Eduardo Duhalde , who completed the term of office of De la Rúa . Rodríguez Saá ran for the 2003 and 2015 presidential elections but did not win . = = Early life = = Rodríguez Saá was born to an important political family in San Luis . The Rodriguez Saá family is well know</t>
+          <t>Eugene McCarthy presidential campaign , 1968 = The Eugene McCarthy presidential campaign of 1968 was launched by Senator Eugene McCarthy of Minnesota in the latter part of 1967 to vie for 1968 Democratic Party nomination for President of the United States . The focus of his campaign was his support for a swift end to the Vietnam War through a withdrawal of American forces . The campaign appealed to youths who were tired of the establishment and dissatisfied with government . Early on , McCarthy was vocal in his intent to unseat the incumbent Democratic President Lyndon B. Johnson . Following McCarthy 's 42 % showing in New Hampshire , Senator Robert F. Kennedy ( D-N.Y. ) entered the race . Kennedy 's entrance forced President Johnson to withdraw . After Johnson 's withdrawal , Vice President Hubert H. Humphrey entered the contest but avoided the primaries . Kennedy fought it out with McCarthy in the primaries , as Humphrey used favorite son stand-ins to help him win delegates to the De</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Fidel Castro = Fidel Alejandro Castro Ruz ( American Spanish : [ fiˈðel aleˈxandɾo ˈkastɾo ˈrus ] audio ; born August 13 , 1926 ) , commonly known as Fidel Castro , is a Cuban politician and revolutionary who governed the Republic of Cuba as Prime Minister from 1959 to 1976 and then as President from 1976 to 2008 . Politically a Marxist – Leninist and Cuban nationalist , he also served as the First Secretary of the Communist Party of Cuba from 1961 until 2011 . Under his administration Cuba became a one-party communist state ; industry and business were nationalized , and state socialist reforms implemented throughout society . Born in Birán as the son of a wealthy farmer , Castro adopted leftist anti-imperialist politics while studying law at the University of Havana . After participating in rebellions against right-wing governments in the Dominican Republic and Colombia , he planned the overthrow of Cuban President Fulgencio Batista , launching a failed attack on the Moncada Barracks</t>
+          <t>White House travel office controversy = The White House travel office controversy , sometimes referred to as Travelgate , was the first major ethics controversy of the Clinton administration . It began in May 1993 , when seven employees of the White House Travel Office were fired . This action was unusual because although theoretically staff employees serve at the pleasure of the President and could be dismissed without cause , in practice , such employees usually remain in their posts for many years . The White House stated the firings were done because financial improprieties in the Travel Office operation during previous administrations had been revealed by an FBI investigation . Critics contended the firings were done to allow friends of President Bill Clinton and First Lady Hillary Rodham Clinton to take over the travel business and that the involvement of the FBI was unwarranted . Heavy media attention forced the White House to reinstate most of the employees in other jobs and re</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Regina Martínez Pérez = Regina Martínez Pérez ( 7 September 1963 – 28 April 2012 ) was a Mexican journalist and veteran crime reporter for Proceso , a center-left Mexican news magazine known for its critical reporting of the social and political establishment . Born in a small town in the state of Veracruz , Martínez Pérez left her hometown to study journalism at Universidad Veracruzana . After graduating from university , she went to work at a state-owned television company in Chiapas in the early 1980s , but she encountered various forms of censorship that convinced her to pursue a career in print media . After five years in Chiapas , Martínez Pérez relocated to Veracruz and worked for several local newspapers . In Veracruz , Martínez Pérez faced several challenges of censorship by the political establishment for her direct reporting , and particularly for being an outspoken critic of human rights violations , government corruption , abuse of authority , and for her in-depth coverage</t>
+          <t>Quebec referendum , 1995 = The 1995 Quebec referendum was the second referendum to ask voters in the Canadian province of Quebec whether Quebec should proclaim national sovereignty and become an independent country , with the condition precedent of offering a political and economic agreement to Canada . The culmination of multiple years of debate and planning after the failure of the Meech Lake and Charlottetown constitutional accords , the referendum was launched solely by the provincial Parti Québécois government of Jacques Parizeau . Despite initial predictions of a heavy sovereignist defeat , an eventful and complex campaign followed , with the " Yes " side flourishing after being taken over by charismatic Bloc Québécois leader Lucien Bouchard . The fast rise of the " Yes " campaign and apparent inability of the personalities of the " No " campaign to counter their message created an atmosphere of great uncertainty , both in the federal government and across Canada . Voting took pl</t>
         </is>
       </c>
     </row>
@@ -1666,32 +1666,32 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>['twitter', 'cylinder', 'cylinders', 'vehicle', 'watson', 'vehicles', 'toyota', 'users', 'model', 'models', 'gas', 'car', 'electric', 'engine', 'valve']</t>
+          <t>['member', 'served', 'elected', 'governor', 'committee', 'serving', 'worked', 'election', 'appointed', 'kentucky', 'married', 'resigned', 'attended', 'born', 'fellow']</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Saviem = The Société Anonyme de Véhicules Industriels et d 'Equipements Mécaniques ( French pronunciation : ​ [ sɔsjete də vɛikyl ɛ ̃ dystʁijɛl e dəkipəmɑ ̃ mekanik ] ) , commonly known by the acronym Saviem ( French pronunciation : ​ [ savjɛ ̃ ] ) , was a French manufacturer of trucks and buses / coaches part of the Renault group , headquartered in Suresnes . The company was established in 1955 by merging Renault heavy vehicle operations with Somua and Latil and disappeared in 1978 when was merged with former rival Berliet to form Renault Véhicules Industriels . The company initially had various factories for vehicle production around France ( mainly at the Paris area ) which came from its predecessors and Chausson , but it soon centred assembly on Blainville-sur-Orne ( trucks ) and Annonay ( buses and coaches ) . Saviem formed partnerships with other manufacturers , leading to technology-sharing agreements . = = History = = = = = Early years = = = At the end of 1946 , Renault abandon</t>
+          <t>Gabriel Slaughter = Gabriel Slaughter ( December 12 , 1767 – September 19 , 1830 ) was the seventh Governor of Kentucky and was the first person to ascend to that office upon the death of the sitting governor . His family moved to Kentucky from Virginia when he was very young . He became a member of the Kentucky militia , serving throughout his political career . He received a citation from the state legislature in recognition of his service at the Battle of New Orleans . After spending a decade in the state legislature , Slaughter was elected the fourth Lieutenant Governor , serving under Charles Scott . With the War of 1812 looming at the end of his tenure , Slaughter ran for governor against Isaac Shelby , the state 's first governor and a noted military leader . Shelby beat Slaughter soundly . Four years later , Slaughter was again elected as lieutenant governor , serving under George Madison . Madison died a short time into his term , whereupon Slaughter became acting governor . H</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Renault Agriculture = Renault Agriculture S.A.S. ( French pronunciation : ​ [ ʁəno aɡʁikyltyʁ ( ə ) ] ) was the agricultural machinery division of the French car manufacturer Renault established in 1918 from its armored military vehicles division . While in operation , Renault Agriculture had various partnerships with major manufacturers and focussed production on tractors . The company was sold between 2003 and 2008 to German rival Claas . Renault Agriculture was dissolved in 2008 and its facilities became part of Claas ' tractor division . Claas ' tractor division and Renault 's Auto Châssis International are Renault Agriculture successors . = = History = = After the end of World War I , the Renault company used its experience in armored tanks to devise agricultural vehicles . The Renault 's Department 14 ( responsible for the FT tank ) developed the first tractor of the company , the Type GP , which was powered by an engine similar to that of the FT ( a four-cylinder ) and had track</t>
+          <t xml:space="preserve">Cabell Breckinridge = Joseph " Cabell " Breckinridge ( July 14 , 1788 – September 1 , 1823 ) was a lawyer and politician in the U.S. state of Kentucky . From 1816 to 1819 , he was a member of the Kentucky House of Representatives , serving as speaker from 1817 to 1819 . In 1820 , he was appointed Kentucky Secretary of State by Governor John Adair . A member of the Breckinridge political family , he was the son of U.S. Attorney General John Breckinridge and the father of U.S. Vice President John C. Breckinridge . Born in Albemarle County , Virginia to John Breckinridge ( 1760-1806 ) and Mary Hopkins Cabell Breckinridge ( 1769-1858 ) , Breckinridge moved to Kentucky with his parents in 1793 . When John Breckinridge was elected to the U.S. Senate in 1801 , Cabell traveled with him to Washington , D.C. , and completed preparatory studies at New London Academy ( now Colby – Sawyer College ) . In 1806 , he enrolled in the College of New Jersey ( now Princeton University ) . His studies were </t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Renault Samsung Motors = Renault Samsung Motors ( Korean : 르노삼성자동차 , IPA : [ ɾɯnoː sʰamsʰʌŋ dʑadoŋtɕʰa ] ) , also known by the acronym RSM , is a South Korean car manufacturer headquartered in Busan where its single assembly site is also located , with additional facilities at Seoul ( administration ) and Giheung ( research and development ) . It was first established as Samsung Motors in 1994 by the chaebol Samsung , with technical assistance from Nissan . The company started selling cars in 1998 , just before South Korea was hit by the Asian financial crisis . In September 2000 , it became a subsidiary of Renault and adopted its present name , although Samsung maintained a minority ownership . RSM markets a range of cars , including electric models and crossovers . = = History = = = = = Beginnings : Samsung Group era ( 1994 – 2000 ) = = = In the early 1990s , Samsung 's Chairman Kun Hee Lee recognised the automotive industry as the culmination of several others . For the Samsung Grou</t>
+          <t>Richard O 'Connor ( politician ) = Richard Edward O 'Connor QC ( 4 August 1851 – 18 November 1912 ) was an Australian politician and judge . A barrister and later Queen 's Counsel , O 'Connor was active in the campaign for Australian Federation and was a close associate of Edmund Barton . He served as New South Wales Minister for Justice in the Dibbs ministry from 1891 to 1893 while a member of the New South Wales Legislative Council ( 1888 – 98 ) , and was a member of the constitutional committee at the Federal Convention that drafted the Australian Constitution . A member of the first federal ministry as Vice-President of the Executive Council , O 'Connor led the government in the Senate from 1901 to 1903 , playing a key role in the development of that chamber 's role in Australian politics . O 'Connor resigned from Parliament in 1903 to become one of the inaugural justices of the High Court of Australia , which he had helped to create . He had a reputation as a liberal and independe</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>NextWorth = NextWorth is an electronics trade-in and recycling service . Users of the service exchange used electronics for cash or discounts on newer models . NextWorth was founded by business students at Babson College in 2005 . It started as a commission-based service to help businesses setup online auctions for their used items , then changed its business model to focus on electronics trade-ins in 2006 . As of late 2012 , NextWorth was one of the best-known and largest electronics trade-in and recycling services in the United States , although it handles only a small percentage of total trade-in traffic . = = History = = NextWorth was founded by David Chen , Andrew Walsh and Scott Richardson while they were students at Babson College . The company was selected for Babson College 's 2005 Business Hatcheries program , which provides free resources to student-led startups . NextWorth Inc. began operations the following year . It was originally a service that helped businesses and non-</t>
+          <t>Charles A. Wickliffe = Charles Anderson Wickliffe ( June 8 , 1788 – October 31 , 1869 ) was a U.S. Representative from Kentucky . He also served as Speaker of the Kentucky House of Representatives , the 14th Governor of Kentucky , and was appointed Postmaster General by President John Tyler . Though he consistently identified with the Whig Party , he was politically independent , and often had differences of opinion with Whig founder and fellow Kentuckian Henry Clay . Wickliffe received a strong education in public school and through private tutors . He studied law and was part of a debate club that also included future U.S. Attorney General Felix Grundy and future Governor of Florida William Pope Duval . He was elected to the Kentucky House of Representatives in 1812 . A vigorous supporter of the War of 1812 , he served for a brief time as aide-de-camp to two American generals in the war . In 1823 , he was elected to the first of five consecutive terms in the U.S. House of Representat</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Lexus = Lexus ( レクサス , Rekusasu ) is the luxury vehicle division of Japanese automaker Toyota . The Lexus marque is marketed in over 70 countries and territories worldwide , has become Japan 's largest-selling make of premium cars , and has ranked among the ten largest Japanese global brands in market value . Lexus is headquartered in Nagoya , Japan . Operational centers are located in Brussels , Belgium , and the U.S. in Torrance , California . Lexus originated from a corporate project to develop a new premium sedan , code-named F1 , which began in 1983 and culminated in the launch of the Lexus LS in 1989 . Subsequently , the division added sedan , coupé , convertible , and SUV models . Until 2005 Lexus did not exist as a brand in its home market and all vehicles marketed internationally as Lexus from 1989-2005 were released in Japan under the Toyota marque and an equivalent model name . In 2005 , a hybrid version of the RX crossover debuted , and additional hybrid models later joined</t>
+          <t xml:space="preserve">Edith Rogers ( Alberta politician ) = Edith Blanche Rogers ( née Edith Blanche Cox ) ( September 20 , 1894 – July 17 , 1985 ) was a Canadian politician who served as a member of the Legislative Assembly of Alberta from 1935 until 1940 . Born in Nova Scotia , she came west to Alberta to accept a job as a teacher . She later moved to Calgary where she encountered evangelist William Aberhart and became a convert to his social credit economic theories . After advocating these theories across the province , she was elected in the 1935 provincial election as a candidate of Aberhart 's newly formed Social Credit League . Left out of cabinet despite her loyalty to Aberhart , she sided with the insurgents during the 1937 Social Credit backbenchers ' revolt , rejoining Aberhart 's followers once a settlement was reached . She was defeated in the 1940 election . After her defeat , she abandoned Social Credit for the Cooperative Commonwealth Federation , moved to Edmonton , and served for fifteen </t>
         </is>
       </c>
     </row>
@@ -1701,32 +1701,32 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>['fiction', 'gay', 'stories', 'pulp', 'lgbt', 'science', 'magazine', 'lesbian', 'comics', 'fantasy', 'issue', 'magazines', 'comic', 'hugo', 'published']</t>
+          <t>['daily', 'trunkline', 'roadway', 'national_highway_system', 'travels', 'designated', 'surveys', 'entire', 'paved', 'intersections', 'designation', 'traveling', 'terminus', 'rural', 'mdot']</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Uncanny Stories ( magazine ) = Uncanny Stories was a pulp magazine which published a single issue , dated April 1941 . It was published by Abraham and Martin Goodman , who were better known for " weird-menace " pulp magazines that included much more sex in the fiction than was usual in science fiction of that era . The Goodmans published Marvel Science Stories from 1938 to 1941 , and Uncanny Stories appeared just as Marvel Science Stories ceased publication , perhaps in order to use up the material in inventory acquired by Marvel Science Stories . The fiction was poor quality ; the lead story , Ray Cummings ' " Coming of the Giant Germs " , has been described as " one of his most appalling stories " . = = Publication history = = Although science fiction had been published before the 1920s , it did not begin to coalesce into a separately marketed genre until the appearance in 1926 of Amazing Stories , a pulp magazine published by Hugo Gernsback . After 1931 , when Miracle Science and Fa</t>
+          <t>Illinois Route 103 = Illinois Route 103 is a 9.18-mile ( 14.77 km ) state route in west-central Illinois , United States . The route , entirely in Schuyler County , runs from U.S. Route 24 near Ripley east to the intersection of U.S. Route 67 and Illinois Route 100 across the Illinois River from Beardstown . In addition to connecting Ripley and Beardstown , Route 103 also serves the community of Sugar Grove . The highway is part of both the National Highway System and the Lincoln Heritage Trail . Route 103 is maintained by the Illinois Department of Transportation . The route was established in 1924 between Ripley and its current eastern terminus ; its western terminus was moved north to its current location in 1932 . = = Route description = = Route 103 begins at a junction with U.S. Route 24 in Woodstock Township in southern Schuyler County , northeast of Ripley . The route initially runs eastward along the LaMoine River , passing through a forested area . After the river turns southw</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Dynamic Science Stories = Dynamic Science Stories was a pulp magazine which published two issues , dated February and April 1939 . A companion to Marvel Science Stories , it was edited by Robert O. Erisman and published by Western Fiction Publishing . Among the better known authors who appeared in its pages were L. Sprague de Camp and Manly Wade Wellman . = = Publication history and contents = = Although science fiction had been published before the 1920s , it did not begin to coalesce into a separately marketed genre until the appearance in 1926 of Amazing Stories , a pulp magazine published by Hugo Gernsback . By the end of the 1930s the field was booming . In 1938 Abraham and Martin Goodman , two brothers who owned a publishing company with multiple imprints , launched Marvel Science Stories , edited by Robert O. Erisman . In February of the following year they added Dynamic Science Stories as a companion magazine intended to run longer stories . The contents were typical pulp scien</t>
+          <t>M-132 ( Michigan highway ) = M-132 was the designation of a former state trunkline highway in the Lower Peninsula of the US state of Michigan near Ann Arbor . The highway , commissioned in 1929 , connected Ann Arbor and Dexter to the northwest along present-day Dexter – Ann Arbor Road . The roadway was turned back to local control around 1960 . = = Route description = = Beginning at the intersection of Main Street and Baker Road in downtown Dexter , M-132 ran southeasterly along Main Street through town . Upon reaching the city limits , the highway became Dexter – Ann Arbor Road . It ran southeast across rural Washtenaw County through fields before entering Ann Arbor where it followed Dexter Avenue and terminated at US Highway 12 ( US 12 , Huron Street / Jackson Avenue ) . = = History = = M-132 was commissioned in 1929 between Dexter and Ann Arbor ; at the time it was created , it was fully paved . It remained in the same configuration until it was removed from the state trunkline syst</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Fantastic Story Quarterly = Fantastic Story Quarterly was a pulp science fiction magazine , published from 1950 to 1955 by Best Books , a subsidiary imprint of Standard Magazines . The name was changed with the Summer 1951 issue to Fantastic Story Magazine . It was launched to reprint stories from the early years of the science fiction pulp magazines , and was initially intended to carry no new fiction , though in the end every issue contained at least one new story . It was sufficiently successful for Standard to launch Wonder Story Annual as a vehicle for more science fiction reprints , but the success did not last . In 1955 it was merged with Standard 's Startling Stories . Original fiction in Fantastic Story included Gordon R. Dickson 's first sale , " Trespass " , and stories by Walter M. Miller and Richard Matheson . = = Publication history and contents = = The first science fiction ( sf ) magazine , Amazing Stories , was launched in 1926 by Hugo Gernsback at the height of the pu</t>
+          <t>Washington State Route 220 = State Route 220 ( SR 220 ) was a 27.42-mile ( 44.13 km ) long state highway located entirely in the Yakama Indian Reservation , Yakima County , Washington , United States . The highway linked Fort Simcoe State Park in the west to White Swan and Toppenish in the east . The highway had been built sometime between 1915 and 1937 , and was renumbered from Secondary State Highway 3B during the 1964 state highway renumbering . The route was slated to be removed from the state highway system during the 1991 legislative session , and was removed April 1 , 1992 . = = Route description = = SR 220 started at Fort Simcoe State Park , headed easterly along Fort Simcoe Road until it intersected Hawk Road . At the t intersection with Hawk Road , the highway turned north and follows Hawk Road until an intersection with White Swan Road . The highway turned back east along White Swan Road , passing through downtown White Swan , before turning south along Curtis Street . The h</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ghost Stories ( magazine ) = Ghost Stories was a pulp magazine which published 64 issues between 1926 and 1932 . It was one of the earliest competitors to Weird Tales , the first magazine to specialize in the fantasy and occult fiction genre . It was a companion magazine to True Story and True Detective Stories , and focused almost entirely on stories about ghosts , with many of the stories written by staff writers but presented under pseudonyms in a " true confession " style . These were often accompanied by faked photographs to make the stories appear more believable . Ghost Stories also ran original and reprinted contributions , including works by Robert E. Howard , Carl Jacobi , and Frank Belknap Long . Among the reprints were Agatha Christie 's " The Last Seance " ( under the title " The Woman Who Stole a Ghost " ) , several stories by H.G. Wells , and Charles Dickens ' " The Signalman " . The magazine was initially successful , but began to lose readers , and in 1930 was sold to </t>
+          <t>M-24 ( Michigan highway ) = M-24 is a state trunkline highway in the U.S. state of Michigan that extends 75.691 miles ( 121.813 km ) through Southeast Michigan and The Thumb , from northeast Auburn Hills to Unionville . It starts at an interchange with Interstate 75 ( I-75 ) and ends where it merges with M-25 . While the M-24 designation is similar to that of US Highway 24 ( US 24 ) which has a northern terminus located only a few miles from the southern terminus of M-24 , M-24 was never part of US 24 . The first M-24 in Michigan was replaced by M-20 when US 10 replaced the original M-20 in 1926 . A 1936 bypass of downtown Pontiac resulted in the creation of M-24A which later became BUS M-24 in 1940 . An extension in 1997 moved the northern end of M-24 northward from Caro to Unionville , replacing a section of M-138 in the process . = = Route description = = M-24 begins a hundred feet south of an overpass that is part of a double trumpet interchange with I-75 in Auburn Hills . The inte</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Miracle Science and Fantasy Stories = Miracle Science and Fantasy Stories was a pulp science fiction magazine which published two issues in 1931 . The fiction was unremarkable , but the cover art and illustrations , by Elliott Dold , were high quality , and have made the magazine a collector 's item . The magazine ceased publication when Dold became ill and was unable to continue his duties both as editor and artist . = = Publication history = = In 1931 , Harold Hersey , who had been working in the pulp magazine field for over a decade , decided to launch a new science fiction ( sf ) and fantasy magazine . Hersey had been the editor for the first half of The Thrill Book 's run of 16 issues in 1919 , and had also worked for Clayton Magazines , where in 1928 he had proposed a sf magazine to William Clayton . Clayton turned down the idea , but the following year changed his mind and launched Astounding Stories of Super Science , with Harry Bates as editor . After Hersey left Clayton and s</t>
+          <t>Manitoba Provincial Road 280 = Provincial Road 280 ( PR 280 ) is a road in the Canadian province of Manitoba . It runs from PR 391 northwest of Thompson to local streets in Gillam . The route is 291 kilometres ( 181 mi ) long , which during its length , passes several large lakes and intersects with one provincial road , PR 290 , just north of Gillam . The route is very scenic , passing through dense forests and rural lands . The route supplies three municipalities , Thompson , Split Lake , and Gillam . From its terminus north of Thompson , Manitoba to the town Gillam , PR 280 is classified as a Class A1 Provincial Route . PR 280 was designated in 1987 as a connector from Thompson to Gillam with a spur to Sundance . = = Route description = = PR 280 begins at an intersection north of Thompson on the shores of Birch Tree Lake with PR 391 . PR 280 runs northeast from PR 391 as a two-lane gravel road through the dense woods north of Thompson Airport . As the road bends to the northeast , i</t>
         </is>
       </c>
     </row>
@@ -1736,32 +1736,32 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>['nickelodeon', 'patrick', 'dvd', 'bikini', 'episodes', 'animation', 'kenny', 'voice', 'kids', 'storyboard', 'episode', 'animated', 'lawrence', 'character', 'television']</t>
+          <t>['song', 'video', 'number', 'single', 'chart', 'performed', 'peaked', 'weeks', 'carey', 'debuted', 'rihanna', 'hot', 'background', 'week', 'girl']</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Crab dip = Crab dip , sometimes referred to as Maryland crab dip , is a thick , creamy dip that is typically prepared from cream cheese and lump crab meat . Other primary ingredients such as mayonnaise may be used . Various types of crab preparations , species and superfamilies are used , as are a variety of added ingredients . It is typically served hot , although cold versions also exist . Hot versions are typically baked or broiled . It is sometimes served as an appetizer . Accompaniments may include crackers and various breads . Some U.S. restaurants offer crab dip , commercially produced varieties exist , and some stadiums offer it as a part of their concessions . = = Ingredients = = Fresh , frozen or canned crab meat may be used in the preparation of crab dip . Different types of crab meat may be used , such as jumbo lump , lump backfin , leg and claw , among others . Various types of crab species and superfamilies are also used , such as blue crab , Dungeness crab and Alaska kin</t>
+          <t>Birthday Cake ( song ) = " Birthday Cake " is a song by Barbadian recording artist Rihanna , from her sixth studio album , Talk That Talk ( 2011 ) . After it leaked onto the internet , fans expressed interest in the track being included on Talk That Talk , but it was later revealed that the 1 : 18 ( one minute , 18 seconds ) length that leaked was in fact the final cut and was not being considered for inclusion on the album . Due to a high level of fan interest , the song was included on the album as an interlude . The full length version , also known as the official remix of the track , featuring Rihanna 's ex-boyfriend Chris Brown , was premiered online on February 20 , 2012 , to coincide with Rihanna 's 24th birthday . The song peaked in the top fifty . The lyrics to " Birthday Cake " express the desire to have spontaneous sex . Music critics were divided on " Birthday Cake " , with the majority both praising and criticising the song 's sexual lyrical content . Several critics compa</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>SpongeBob SquarePants ( season 7 ) = The seventh season of the American animated television series SpongeBob SquarePants , created by marine biologist and animator Stephen Hillenburg , originally aired on Nickelodeon in the United States from July 19 , 2009 to June 11 , 2011 . It contained 26 episodes , beginning with the episodes " Tentacle Vision " and " I Heart Dancing " . The series chronicles the exploits and adventures of the title character and his various friends in the fictional underwater city of Bikini Bottom . The season was executive produced by series creator Hillenburg and writer Paul Tibbitt , who also acted as the showrunner . In 2011 , Legends of Bikini Bottom , an anthology series consists of five episodes from the season , was launched . A number of guest stars appeared on the season 's episodes . Several compilation DVDs that contained episodes from the season were released . The SpongeBob SquarePants : Complete Seventh Season DVD was released in Region 1 on Decemb</t>
+          <t xml:space="preserve">Oh Santa ! = " Oh Santa ! " is a song by American singer and songwriter Mariah Carey from her second Christmas album / thirteenth studio album , Merry Christmas II You ( 2010 ) . Carey wrote and produced the song in collaboration with Jermaine Dupri and Bryan-Michael Cox . It was released as the lead single from the album . It is an up-tempo R &amp; B song about Carey making a plea for Santa Claus to bring back her partner in time for the Christmas holidays . Instrumentation of sleigh bells , jingle bells and hand claps . It received a positive response from music critics , with many praising its composition and style . The track set a record on the United States Billboard Adult Contemporary songs chart , debuting at number twelve and peaking at number one the following week for four weeks . It became the first song to reach the summit in two weeks . It further became Carey 's seventh number-one song on the chart . Carey filmed a 1960s style music video to accompany the songs release as a </t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>SpongeBob SquarePants ( season 6 ) = The sixth season of the American animated television series SpongeBob SquarePants , created by former marine biologist and animator Stephen Hillenburg , aired on Nickelodeon from March 3 , 2008 to July 5 , 2010 , and contained 26 episodes , beginning with the episode " Krabby Road " . The series chronicles the exploits and adventures of the title character and his various friends in the fictional underwater city of Bikini Bottom . The season was executive produced by series creator Hillenburg , who also acted as the showrunner . In 2009 , the show celebrated its tenth anniversary on television . The documentary film titled Square Roots : The Story of SpongeBob SquarePants premiered on July 17 , 2009 , and marked the anniversary . SpongeBob 's Truth or Square , a television film , and the special episode " To SquarePants or Not to SquarePants " were broadcast on Nickelodeon , as part of the celebration . The show itself received several recognition ,</t>
+          <t>Mama ( Spice Girls song ) = " Mama " is a song by British pop group Spice Girls . It was written by the Spice Girls , Matt Rowe and Richard Stannard , and produced by Rowe and Stannard for the group 's debut album Spice , released in November 1996 . " Mama " is a pop ballad that features instrumentation from keyboards , a rhythm guitar , a cello , and a violin , and its lyrics deal with the difficulties in relationships between mothers and daughters that appear during adolescence . It was released as a double A-side with " Who Do You Think You Are " , and became the official single of the 1997 Comic Relief . Its Big TV ! directed music video , featured the group singing to an audience of children and their own mothers . Despite receiving mixed reviews from music critics , " Mama " was commercially successful . Released as the album 's fourth single in March 1997 , it became their fourth consecutive number-one single in the United Kingdom , which made the Spice Girls the first act in UK</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>SpongeBob SquarePants ( season 4 ) = The fourth season of the American animated television series SpongeBob SquarePants , created by former marine biologist and animator Stephen Hillenburg , aired on Nickelodeon from May 6 , 2005 to July 24 , 2007 , and contained 20 episodes , beginning with the episodes " Fear of a Krabby Patty " and " Shell of a Man " . The series chronicles the exploits and adventures of the title character and his various friends in the fictional underwater city of Bikini Bottom . The season was executive produced by series creator Hillenburg , while writer Paul Tibbitt acted as the showrunner . The show underwent a hiatus on television as Hillenburg halted the production in 2002 to work on the film adaptation of the series , The SpongeBob SquarePants Movie . Once the film was finalized and the previous season had completed broadcast on television , Hillenburg wanted to end the show , but the success of the series led to more episodes , so Tibbitt took over Hillenb</t>
+          <t>Causing a Commotion = " Causing a Commotion " is a song by American singer Madonna from the soundtrack album to the 1987 film Who 's That Girl . It was released as the album 's second single on August 25 , 1987 by Sire Records . Its Silver Screen Single Mix later appeared on the 1991 UK compilation EP The Holiday Collection . Written and produced by Madonna and Stephen Bray , the song was inspired by Madonna 's relationship with then husband Sean Penn , and his abusive and violent nature . Containing a dance-oriented , up-tempo groove , the song begins with the chorus and is accompanied by a four-note descending bassline and staccato chords in the verse . Since its release , the song has received mixed reviews by critics . It became a top-ten hit in the United States , Australia , Canada , Ireland , Italy , New Zealand , Sweden and the United Kingdom , and topped the Billboard U.S. dance chart . Madonna performed the song on the Who 's That Girl World Tour – which was transmitted via s</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Pizza Delivery ( SpongeBob SquarePants ) = " Pizza Delivery " is the first segment of the fifth episode of the American animated television series SpongeBob SquarePants . The episode was written by Sherm Cohen , Aaron Springer , and Peter Burns , and was directed by Sean Dempsey . Cohen also functioned as storyboard director , and Springer worked as storyboard artist . It originally aired on Nickelodeon in the United States on August 14 , 1999 . In the episode , the Krusty Krab receives a call from a customer ordering a pizza , and Mr. Krabs sends SpongeBob and Squidward to deliver it . When the two employees become stranded in the middle of a desert , they get into numerous predicaments . Along the way , SpongeBob tries to show Squidward the way of the pioneers . In pitching the show to Nickelodeon , creator Stephen Hillenburg originally wanted the idea of having the characters on a road trip , inspired by the 1989 film Powwow Highway . However , he eventually gave up the idea , and r</t>
+          <t>Into the Groove = " Into the Groove " is a song by American singer Madonna from the 1985 film Desperately Seeking Susan . It was featured on the re-issue of her second studio album Like a Virgin ( 1984 ) , and released on July 23 , 1985 , by Sire Records as the album 's fourth single outside North America . The original song was included on her third greatest hits album , Celebration ( 2009 ) , while remixes of it appeared on the remix compilation You Can Dance ( 1987 ) , and her first greatest hits compilation The Immaculate Collection ( 1990 ) . Madonna 's inspiration behind the song was the dance floor , and she wrote it while watching a handsome Puerto Rican man , across her balcony . Initially written for her friend Mark Kamins , Madonna later decided to use it as the soundtrack of her film Desperately Seeking Susan . " Into the Groove " was recorded at Sigma Sound Studios . A remixed version , titled " Into the Hollywood Groove " , was created by Madonna in 2003 for a Gap commerc</t>
         </is>
       </c>
     </row>
@@ -1771,32 +1771,32 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>['scottish', 'scotland', 'painting', 'edinburgh', 'architecture', 'houses', 'century', 'churches', 'scots', 'bricks', 'portrait', 'highlands', 'glasgow', 'brick', 'portraits']</t>
+          <t>['war', 'following', 'german', 'april', 'training', 'japanese', 'division', 'attack', 'march', 'assigned', 'transferred', 'november', 'december', 'command', 'commander']</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Architecture of Scotland in the Middle Ages = The architecture of Scotland in the Middle Ages includes all building within the modern borders of Scotland , between the departure of the Romans from Northern Britain in the early fifth century and the adoption of the Renaissance in the early sixteenth century , and includes vernacular , ecclesiastical , royal , aristocratic and military constructions . The first surviving houses in Scotland go back 9500 years . There is evidence of different forms of stone and wooden houses exist and earthwork hill forts from the Iron Age . The arrival of the Romans from about led to the abandonment of many of these forts . After the departure of the Romans in the fifth century , there evidence their reoccupation and of the building of a series of smaller " nucleated " constructions sometimes utilising major geographical features , as at Dunadd and Dumbarton . In the following centuries new forms of construction emerged throughout Scotland that would come</t>
+          <t>2 / 5th Battalion ( Australia ) = The 2 / 5th Battalion was an infantry battalion of the Australian Army that operated during World War II . It was raised at Melbourne , Victoria , on 18 October 1939 as part of the Second Australian Imperial Force ( 2nd AIF ) , attached to the 17th Brigade of the 6th Division . The 2 / 5th was one of only two Australian infantry battalions to fight against all of the major Axis powers during the war , seeing action against the Germans and Italians in Egypt , Libya , Greece and Crete , and the Vichy French in Syria , before returning to Australia in 1942 to fight the Japanese following a period of garrison duties in Ceylon , where it formed part of an Australian force established to defend against a possible Japanese invasion . Following its return to Australia , the battalion was re-organised for jungle warfare and took part in two campaigns in New Guinea . The first of these campaigns came in 1942 – 43 when it was involved in the defence of Wau and th</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Architecture of Scotland = The architecture of Scotland includes all human building within the modern borders of Scotland , from the Neolithic era to the present day . The earliest surviving houses go back around 9500 years , and the first villages 6000 years : Skara Brae on the Mainland of Orkney being the earliest preserved example in Europe . Crannogs , roundhouses , each built on an artificial island , date from the Bronze Age and stone buildings called Atlantic roundhouses and larger earthwork hill forts from the Iron Age . The arrival of the Romans from about 71 AD led to the creation of forts like that at Trimontium , and a continuous fortification between the Firth of Forth and the Firth of Clyde known as the Antonine Wall , built in the second century AD . Beyond Roman influence , there is evidence of wheelhouses and underground souterrains . After the departure of the Romans there were a series of nucleated hill forts , often utilising major geographical features , as at Duna</t>
+          <t>Māori Battalion = The 28th ( Māori ) Battalion , more commonly known as the Māori Battalion , was an infantry battalion of the New Zealand Army that served during the Second World War . It was formed following pressure on the Labour government by some Māori Members of Parliament ( MPs ) and Māori organisations throughout the country which wanted a full Māori unit to be raised for service overseas . The Māori Battalion followed in the footsteps of the Māori Pioneer Battalion that served during the First World War with success , and was wanted by Māori to raise their profile , and to serve alongside their Pākehā compatriots as subjects of the British Empire . It also gave a generation of people with a well-noted military ancestry a chance to test their own warrior skills . Raised in 1940 as part of the Second New Zealand Expeditionary Force ( 2NZEF ) , the 28th ( Māori ) Battalion was attached to the 2nd New Zealand Division as an extra battalion that was moved between the division 's th</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Scottish art in the eighteenth century = Scottish art in the eighteenth century is the body of visual art made in Scotland , by Scots , or about Scottish subjects , in the eighteenth century . This period saw development of professionalisation , with art academies were established in Edinburgh and Glasgow . Art was increasingly influenced by Neoclassicism , the Enlightenment and towards the end of the century by Romanticism , with Italy becoming a major centre of Scottish art . The origins of the tradition of Scottish landscape painting are in the capriccios of Italian and Dutch landscapes undertaken by James Norie and his sons . These were further developed by Jacob More , who added a romantic sensibility to the Scottish landscape . Alexander Nasmyth helped found the Scottish landscape tradition and was highly influential as a teacher in Edinburgh on the subsequent generation of artists . John Knox linked it with the Romantic works of Walter Scott and was one of the first artists to t</t>
+          <t>1st Airlanding Brigade ( United Kingdom ) = The 1st Airlanding Brigade was an airborne infantry brigade of the British Army during the Second World War and the only glider infantry formation assigned to the 1st Airborne Division , serving alongside the 1st Parachute Brigade and 4th Parachute Brigade . The brigade was formed in late 1941 during World War II through the conversion of an existing infantry brigade previously stationed in India , the 31st Independent Infantry Brigade . Two of the initial four infantry battalions left in May 1943 to form the new 6th Airlanding Brigade of the 6th Airborne Division and were replaced by a single new battalion , thereby reducing the brigade 's strength by one quarter . The brigade only saw action on two occasions during the Second World War , in Operation Ladbroke , as part of the Allied invasion of Sicily , in July 1943 and later in Operation Market Garden in September 1944 . During the second operation , in the fighting around Arnhem , 1st Air</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Art in early modern Scotland = Art in early modern Scotland includes all forms of artistic production within the modern borders of Scotland , between the adoption of the Renaissance in the early sixteenth century to the beginnings of the Enlightenment in the mid-eighteenth century . Devotional art before the Reformation included books and images commissioned in the Netherlands . Before the Reformation in the mid-sixteenth century the interiors of Scottish churches were often elaborate and colourful , with sacrament houses and monumental effigies . Scotland 's ecclesiastical art paid a heavy toll as a result of Reformation iconoclasm , with the almost total loss of medieval stained glass , religious sculpture and paintings . In about 1500 the Scottish monarchy turned to the recording of royal likenesses in panel portraits . More impressive are the works or artists imported from the continent , particularly the Netherlands . The tradition of royal portrait painting in Scotland was probab</t>
+          <t>Australian Army during World War I = The Australian Army was the largest service in the Australian military during World War I. The First Australian Imperial Force ( AIF ) was the Army 's main expeditionary force and was formed from 15 August 1914 with an initial strength of 20,000 men , following Britain 's declaration of war on Germany . Meanwhile , the separate , hastily raised 2,000-man Australian Naval and Military Expeditionary Force ( AN &amp; MEF ) , landed near Rabaul in German New Guinea on 11 September 1914 and obtained the surrender of the German garrison after ten days ; it later provided occupation forces for the duration of the war . In addition , small military forces based on the pre-war Permanent Forces and part-time Citizen Forces were maintained in Australia to defend the country from attack . The AIF initially consisted of one infantry division and one light horse brigade . The first contingent departed Australia by ship for Egypt on 1 November 1914 , where it formed p</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Church architecture in Scotland = Church architecture in Scotland incorporates all church building within the modern borders of Scotland , from the earliest Christian structures in the sixth century until the present day . The early Christian churches for which there is evidence are basic masonry-built constructions on the west coast and islands . As Christianity spread , local churches tended to remain much simpler than their English counterparts . By the eighth century more sophisticated ashlar block-built buildings began to be constructed . From the eleventh century , there were larger and more ornate Romanesque buildings , as with Dunfermline Abbey and St Magnus Cathedral in Orkney . From the twelfth century the introduction of new monastic orders led to a boom in ecclesiastical building , often using English and Continental forms . From the thirteenth century elements of the European Gothic style began to appear in Scotland , cumulating in buildings such as Glasgow Cathedral and t</t>
+          <t>4th Parachute Brigade ( United Kingdom ) = The 4th Parachute Brigade was an airborne , specifically a parachute infantry , brigade formation of the British Army during the Second World War . Formed in late 1942 in the Mediterranean and Middle East , the brigade was composed of three parachute infantry units , the 10th , 11th and 156th Parachute Battalions . The brigade was assigned to the 1st Airborne Division , just prior to the Allied invasion of Sicily , but played no part in the invasion . Instead the brigade first saw action in September 1943 , during Operation Slapstick , an amphibious landing at the port of Taranto , as part of the early stages of the Allied invasion of Italy . Largely unopposed , the brigade captured the ports of Brindisi and Bari before being withdrawn . By the end of the year , the 4th Parachute Brigade was in England , preparing for the Allied invasion of North-West Europe . The brigade did not see action in France , being instead placed on standby for an em</t>
         </is>
       </c>
     </row>
@@ -1806,32 +1806,32 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>['hebrew', 'text', 'manuscripts', 'gospel', 'jesus', 'manuscript', 'matthew', 'john', 'biblical', 'luke', 'greek', 'printing', 'readings', 'scholars', 'letters']</t>
+          <t>['rainfall', 'meteorological', 'preparations', 'watch', 'florida', 'flooding', 'damage', 'winds', 'hurricane', 'issued', 'reported', 'rain', 'landfall', 'mexico', 'usd']</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Codex Boreelianus = Codex Boreelianus , Codex Boreelianus Rheno-Trajectinus ( full name ) , designated by Fe or 09 in the Gregory-Aland numbering and ε 86 in von Soden numbering , is a 9th ( or 10th ) century uncial manuscript of the four Gospels in Greek . The manuscript , written on parchment , is full of lacunae ( or gaps ) , many of which arose between 1751 and 1830 . The codex was named Boreelianus after Johannes Boreel ( 1577 – 1629 ) , who brought it from the East . The text of the codex represents the majority of the text ( Byzantine text-type ) , but with numerous alien readings ( non-Byzantine ) . Some of its readings do not occur in any other manuscript ( so called singular readings ) . According to the present textual critics its text is not a very important manuscript , but it is quoted in all modern editions of the Greek New Testament . The manuscript was brought from the East at the beginning of the 17th century . It was in private hands for over 100 years . Since 1830 i</t>
+          <t>Hurricane Octave ( 1989 ) = Hurricane Octave was a Category 4 hurricane which existed during the above-average 1989 Pacific hurricane season . The remnants of Atlantic Tropical Depression Nine tracked westward across the Caribbean Sea , entering the Pacific Ocean on September 3 . It slowly developed , and organized into a tropical depression on September 8 . It strengthened into a tropical storm on September 10 , thus earning the name Octave . After strengthening into a hurricane the next day , Octave started to steadily intensify en route to a peak as a Category 4 hurricane of the Saffir – Simpson Hurricane Scale . After reaching peak winds of 135 mph ( 215 km / h ) on September 13 , Octave moved into a region of cooler waters . The hurricane weakened into a tropical storm on September 14 , and degenerated further into a tropical depression the next day , before dissipating on September 16 . The remnants of the storm brought moderate rainfall to parts of California and Arizona , as we</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Novum Instrumentum omne = Novum Instrumentum omne was the first published New Testament in Greek ( 1516 ) . It was prepared by Desiderius Erasmus ( 1469 – 1536 ) and printed by Johann Froben ( 1460 – 1527 ) of Basel . Although the first printed Greek New Testament was the Complutensian Polyglot ( 1514 ) , it was the second to be published ( 1522 ) . Erasmus used several Greek manuscripts housed in Basel , but some a few verses in Revelation he translated from the Latin Vulgate . Five editions of Novum Instrumentum omne were published , though its title was changed to Novum Testamentum omne with the second edition , and the name continued . Erasmus issued editions in 1516 , 1519 , 1522 , 1527 , and 1536 . Notable amongst these are the second edition ( 1519 ) , used by Martin Luther for his translation of the New Testament into German , the so-called " September Testament , " and the third edition ( 1522 ) , which was used by Tyndale for the first English New Testament ( 1526 ) and later</t>
+          <t>Hurricane Barbara ( 2013 ) = Hurricane Barbara was the easternmost landfalling Pacific hurricane on record . As the first hurricane of the 2013 Pacific hurricane season , Barbara developed from a low-pressure area while located southeast of Mexico on May 28 . It headed slowly north-northeastward and strengthened into a tropical storm early on the following day . After recurving to the northeast , Barbara intensified into a Category 1 hurricane on May 29 and made landfall in Chiapas at peak intensity with winds of 80 mph ( 130 km / h ) and a barometric pressure estimated at 983 mbar ( hPa ; 29.03 inHg ) . When the hurricane made landfall , it was the second earliest landfalling hurricane in the basin since reliable records began in 1966 . Barbara then moved across the Isthmus of Tehuantepec and dissipated within the mountainous terrain of Sierra Madre de Chiapas on May 30 . The precursor of Hurricane Barbara brought light to moderate rainfall to El Salvador . Many homes were damaged , r</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Codex Zacynthius = Codex Zacynthius ( designated by siglum Ξ or 040 in the Gregory-Aland numbering ; A1 in von Soden ) is a Greek New Testament codex , dated paleographically to the 6th century . First thought to have been written in the 8th century , it is a palimpsest — the original ( lower ) text was washed off its vellum pages and overwritten in the 12th or 13th century . The upper text of the palimpsest contains weekday Gospel lessons ; the lower text contains portions of the Gospel of Luke , deciphered by biblical scholar and palaeographer Tregelles in 1861 . The lower text is of most interest to scholars . The manuscript came from Zakynthos , a Greek island , and has survived in a fragmentary condition . It was brought to England in 1821 and transferred to Cambridge University in 1985 . It is often cited in critical editions of the Greek New Testament . = = Description = = The lower text of the manuscript contains fragments of the chapters 1 : 1-11 : 33 of the Gospel of Luke . T</t>
+          <t>Hurricane Sergio ( 2006 ) = Hurricane Sergio was the third strongest Pacific hurricane in the month of November on record . The nineteenth named storm and eleventh hurricane of the 2006 Pacific hurricane season , Sergio developed from a tropical wave on November 13 about 460 miles ( 740 km ) south of Manzanillo , Mexico , and steadily intensified as it tracked southeastward . It reached peak winds of 110 mph ( 175 km / h ) on November 15 , and subsequently began to weaken due to increased wind shear as it turned to the north . Sergio later turned to the west , remaining well off the coast of Mexico , and dissipated on November 20 about 320 miles ( 515 km ) west-northwest of it originally formed . Sergio produced light rainfall along the coast of Mexico , though its effects were minimal . The formation of Sergio marked the 2006 season as the busiest in 12 years and the first season in which more than one tropical storm formed in November . Sergio , in addition to being the strongest hur</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Codex Alexandrinus = The Codex Alexandrinus ( London , British Library , MS Royal 1 . D. V-VIII ; Gregory-Aland no . A or 02 , Soden δ 4 ) is a fifth-century manuscript of the Greek Bible , containing the majority of the Septuagint and the New Testament . It is one of the four Great uncial codices . Along with the Codex Sinaiticus and the Vaticanus , it is one of the earliest and most complete manuscripts of the Bible . Brian Walton assigned Alexandrinus the capital Latin letter A in the Polyglot Bible of 1657 . This designation was maintained when the system was standardized by Wettstein in 1751 . Thus , Alexandrinus held the first position in the manuscript list . It derives its name from Alexandria where it resided for a number of years before it was brought by the Eastern Orthodox Patriarch Cyril Lucaris from Alexandria to Constantinople . Then it was given to Charles I of England in the 17th century . Until the later purchase of Codex Sinaiticus , it was the best manuscript of the</t>
+          <t>Hurricane Danny ( 2015 ) = Hurricane Danny in August 2015 was the first major hurricane to develop between the Lesser Antilles and Western Africa since Hurricane Julia in 2010 . The hurricane originated from a well-defined tropical wave that emerged over the Atlantic Ocean on August 14 . Traveling west , the system gradually coalesced into a tropical depression by August 18 . After becoming a tropical storm later that day , dry air slowed further development . On August 20 – 21 , dry air became removed from the system , and Danny rapidly intensified into a Category 3 on the Saffir – Simpson hurricane wind scale . Its peak was short-lived as wind shear soon increased and prompted significant weakening . Degrading to a tropical storm by August 23 , Danny approached the Lesser Antilles . It degenerated into a tropical wave as it traversed the archipelago on August 24 and was last noted over Hispaniola the following day . The hurricane prompted the issuance of several tropical storm warnin</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Gospel of John = The Gospel According to John ( Greek : Τὸ κατὰ Ἰωάννην εὐαγγέλιον , translit . To kata Iōánnēn euangélion ; also called the Gospel of John , the Fourth Gospel , or simply John ) is one of the four canonical gospels in the New Testament . It traditionally appears fourth , after the synoptic gospels of Matthew , Mark , and Luke . John begins with the witness and affirmation of John the Baptist and concludes with the death , burial , resurrection , and post-resurrection appearances of Jesus . The author is identified as " the Disciple whom Jesus loved " , whom early Christian tradition identified as John the Apostle , one of Jesus ' Twelve Apostles . The gospel is so closely related in style and content to the three surviving Johannine epistles that commentators treat the four books , along with the Book of Revelation , as a single corpus of Johannine literature , but there are some arguments made by modern scholars who believe John the Apostle was not the author of any o</t>
+          <t xml:space="preserve">Tropical Storm Nicholas ( 2003 ) = Tropical Storm Nicholas was a long-lived tropical storm in October and November of the 2003 Atlantic hurricane season . Forming from a tropical wave on October 13 in the central tropical Atlantic Ocean , Nicholas slowly developed due to moderate levels of wind shear throughout its lifetime . Deep convection slowly organized , and Nicholas attained a peak intensity of 70 mph ( 110 km / h ) on October 17 . After moving west-northwestward for much of its lifetime , it turned northward and weakened due to increasing shear . The storm again turned to the west and briefly restrengthened , but after turning again to the north Nicholas transitioned to an extratropical cyclone on October 24 . As an extratropical storm , Nicholas executed a large loop to the west , and after moving erratically for a week and organizing into a tropical low , it was absorbed by a non-tropical low . The low continued westward , crossed Florida , and ultimately dissipated over the </t>
         </is>
       </c>
     </row>
@@ -1841,32 +1841,32 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>['comics', 'story', 'belgian', 'adventures', 'snowy', 'moon', 'brussels', 'cartoonist', 'comic', 'depiction', 'belgium', 'adventure', 'sun', 'explorers', 'book']</t>
+          <t>['rating', 'office', 'jim', 'dwight', 'episode', 'aired', 'nbc', 'watching', 'nielsen', 'michael', 'pam', 'share', 'rated', 'viewed', 'ratings']</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Comics = Comics is a medium used to express ideas by images , often combined with text or other visual information . Comics frequently takes the form of juxtaposed sequences of panels of images . Often textual devices such as speech balloons , captions , and onomatopoeia indicate dialogue , narration , sound effects , or other information . Size and arrangement of panels contribute to narrative pacing . Cartooning and similar forms of illustration are the most common image-making means in comics ; fumetti is a form which uses photographic images . Common forms of comics include comic strips , editorial and gag cartoons , and comic books . Since the late 20th century , bound volumes such as graphic novels , comic albums , and tankōbon have become increasingly common , and online webcomics have proliferated in the 21st century . The history of comics has followed different paths in different cultures . Scholars have posited a pre-history as far back as the Lascaux cave paintings . By the</t>
+          <t>The Merger ( The Office ) = " The Merger " is the eighth episode of the third season of the American comedy television series The Office and the show 's 36th overall . It was written by consulting producer Brent Forrester and directed by Ken Whittingham . It first aired on November 16 , 2006 , as a special " super-sized " 40-minute ( including commercials ) episode on NBC . The series depicts the everyday lives of office employees in the Scranton and Stamford branches of the fictional Dunder Mifflin Paper Company . In this episode , the two branches are merged . Jim Halpert ( John Krasinski ) and Pam Beesley ( Jenna Fischer ) have an awkward reunion , Michael Scott ( Steve Carell ) tries to make his new employees feel welcome , and a rivalry begins between Dwight Schrute ( Rainn Wilson ) and Andy Bernard ( Ed Helms ) . The episode featured recurring guest stars Helms , Creed Bratton , Rashida Jones , Wayne Wilderson , Mike Bruner , and Ursula Burton . According to Nielsen Media Researc</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Flash Gordon Strange Adventure Magazine = Flash Gordon Strange Adventure Magazine was a pulp magazine which was launched in December 1936 . It was published by Harold Hersey , and was an attempt to cash in on the growing comics boom , and the popularity of the Flash Gordon comic strip in particular . The magazine contained a novel about Flash Gordon and three unrelated stories ; there were also eight full-page color illustrations . The quality of both the artwork and the fiction was low , and the magazine only saw a single issue . It is now extremely rare . = = Publication history and contents = = Although science fiction ( sf ) had been published before the 1920s , it did not begin to coalesce into a separately marketed genre until the appearance in 1926 of Amazing Stories , a pulp magazine published by Hugo Gernsback . After 1931 , when Miracle Science and Fantasy Stories was launched , no new science fiction magazines appeared for several years . In 1934 a science fiction comic stri</t>
+          <t>Livin ' the Dream = " Livin ' the Dream " is the twenty-first episode of the ninth season of the American comedy television series The Office and the 197th episode overall . It originally aired on NBC on May 2 , 2013 . The episode guest stars Michael Imperioli as Sensei Billy , and was initially scheduled to air in its half-hour timeslot , before being expanded to a full hour . The series — presented as if it were a real documentary — depicts the everyday lives of office employees in the Scranton , Pennsylvania , branch of the fictional Dunder Mifflin Paper Company . In the episode , Andy Bernard ( Ed Helms ) decides to pursue a career as a professional actor , and quits his job at Dunder Mifflin . Meanwhile , Dwight Schrute ( Rainn Wilson ) finally receives his black belt in karate from his new sensei ( Imperioli ) and , on the recommendation of Jim Halpert ( John Krasinski ) , is promoted to Regional Manager of the Scranton branch . Jim reconnects with Pam Halpert ( Jenna Fischer ) ,</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Canadian comics = Canadian comics refers to comics and cartooning by citizens of Canada or permanent residents of Canada regardless of residence . Canada has two official languages , and distinct comics cultures have developed in English and French Canada . The English tends to follow American trends , and the French Franco-Belgian ones , with little crossover between the two cultures . Canadian comics run the gamut of comics forms , including editorial cartooning , comic strips , comic books , graphic novels , and webcomics , and are published in newspapers , magazines , books , and online . They have received attention in international comics communities and have received support from the federal and provincial governments , including grants from the Canada Council for the Arts . There are a comics publishers throughout the country , as well as large small press , self-publishing , and minicomics communities . In English Canada many cartoonists , from Hal Foster to Todd McFarlane , h</t>
+          <t xml:space="preserve">Email Surveillance = " Email Surveillance " is the ninth episode of the second season of the American comedy television series The Office , and the show 's fifteenth episode overall . Written by Jennifer Celotta , and directed by Paul Feig , the episode first aired in the United States on November 22 , 2005 on NBC . The episode guest starred Ken Jeong and Omi Vaidya . The series depicts the everyday lives of office employees in the Scranton , Pennsylvania branch of the fictional Dunder Mifflin Paper Company . In the episode , the company tech support employee gives Michael Scott ( Steve Carell ) the ability to read his employees ' emails , causing him to find out that Jim Halpert ( John Krasinski ) is throwing a party that Michael was not invited to . Meanwhile , Pam Beesly ( Jenna Fischer ) begins to suspect that Dwight Schrute ( Rainn Wilson ) and Angela Martin ( Angela Kinsey ) might secretly be having a relationship . Ken Jeong explained that , while all the scenes were scripted , </t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>10 Story Fantasy = 10 Story Fantasy ( occasionally referred to as Ten Story Fantasy ) was a science fiction and fantasy pulp magazine which was launched in 1951 . The market for pulp magazines was already declining by that time , and the magazine only lasted a single issue . The stories were of generally good quality , and included work by many well-known writers , such as John Wyndham , A.E. van Vogt and Fritz Leiber . The most famous story it published was Arthur C. Clarke 's " Sentinel from Eternity " , which later became part of the basis of the movie 2001 : A Space Odyssey . = = Publication history = = The early 1950s saw dramatic changes in the world of U.S. science fiction ( sf ) publishing . At the start of 1949 , all but one of the major magazines in the field were in pulp format ; by the end of 1955 , almost all had either ceased publication or switched to digest format . Despite the rapid decline of the pulp market , several new science fiction magazines were launched in pul</t>
+          <t>Cocktails ( The Office ) = " Cocktails " is the eighteenth episode of the third season of the US version of The Office . It was written by actor Paul Lieberstein and directed by Lost series creator J. J. Abrams , his first such credit for The Office . NBC hired Abrams and Joss Whedon to each direct an episode during their February sweeps week . Michael Patrick McGill , Dan Cole , Owen Daniels , and Jean Villepique guest starred . In the episode , Michael , Dwight , Jim and Karen attend a cocktail party at CFO David Wallace 's house . While there , Michael and Jan make their relationship public , Karen makes Jim uncomfortable by pointing out all of her ex-boyfriends in attendance , and Dwight inspects the home . Meanwhile , the rest of the office goes to a bar and Pam tries to be more honest with Roy . The first American broadcast of " Cocktails " occurred on February 22 , 2007 to an estimated 8.3 million viewers . The episode was positively received by television critics , with one bel</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Wonder Story Annual = Wonder Story Annual was a science fiction pulp magazine which was launched in 1950 by Standard Magazines . It was created as a vehicle to reprint stories from early issues of Wonder Stories , Startling Stories , and Wonder Stories Quarterly , which were owned by the same publisher . It lasted for four issues , succumbing in 1953 to competition from the growing market for paperback science fiction . Reprinted stories included Twice in Time , by Manly Wade Wellman , and " The Brain-Stealers of Mars " , by John W. Campbell . = = Publication history and contents = = The first science fiction ( sf ) magazine , Amazing Stories , was launched in 1926 by Hugo Gernsback at the height of the pulp magazine era . It helped to form science fiction as a separately marketed genre , and by the mid-1930s several more sf magazines had appeared , including Wonder Stories , also published by Gernsback . In 1936 , Ned Pines of Beacon Publications bought Wonder Stories from Gernsback ,</t>
+          <t>Take Your Daughter to Work Day ( The Office ) = " Take Your Daughter To Work Day " is the eighteenth episode of the second season of the American comedy television series The Office , and the show 's twenty-fourth episode overall . It was written by Mindy Kaling and directed by Victor Nelli , Jr . It first aired on March 16 , 2006 on NBC . The episode guest stars Jazz Raycole as Melissa Hudson , Delaney Ruth Farrell as Sasha Flenderson , Spencer Daniels as Jake Palmer , and Jake Kalender as a young Michael Scott . The series depicts the everyday lives of office employees in the Scranton , Pennsylvania branch of the fictional Dunder Mifflin Paper Company . In this episode , Take Your Daughter to Work Day results in four children spending the day at the office — Toby Flenderson 's ( Paul Lieberstein ) daughter Sasha , Stanley Hudson 's ( Leslie David Baker ) daughter Melissa , Kevin Malone 's ( Brian Baumgartner ) fiancee 's daughter Abby , and Meredith Palmer 's ( Kate Flannery ) son Ja</t>
         </is>
       </c>
     </row>
@@ -1876,32 +1876,32 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>['spacecraft', 'apollo', 'nasa', 'lunar', 'mission', 'orbit', 'launch', 'moon', 'saturn', 'module', 'manned', 'docking', 'landing', 'flight', 'space']</t>
+          <t>['species', 'small', 'female', 'large', 'male', 'found', 'larger', 'size', 'long', 'shark', 'dorsal', 'head', 'adult', 'waters', 'body']</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Advanced Gemini = Advanced Gemini is a number of proposals that would have extended the Gemini program by the addition of various missions , including manned low Earth orbit , circumlunar and lunar landing missions . Gemini was the second manned spaceflight program operated by NASA , and consisted of a two-seat spacecraft capable of maneuvering in orbit , docking with unmanned spacecraft such as Agena Target Vehicles , and allowing the crew to perform tethered extra-vehicular activities . A range of applications were considered for Advanced Gemini missions , including military flights , space station crew and logistics delivery , and lunar flights . The Lunar proposals ranged from reusing the docking systems developed for the Agena target vehicle on more powerful upper stages such as the Centaur , which could propel the spacecraft to the Moon , to complete modifications of the Gemini to enable it to land on the Lunar surface . Its applications would have ranged from manned lunar flybys</t>
+          <t>Zebra shark = This species is sometimes called the leopard shark , a name otherwise used for Triakis semifasciata . The zebra shark ( Stegostoma fasciatum ) is a species of carpet shark and the sole member of the family Stegostomatidae . It is found throughout the tropical Indo-Pacific , frequenting coral reefs and sandy flats to a depth of 62 m ( 203 ft ) . Adult zebra sharks are distinctive in appearance , with five longitudinal ridges on a cylindrical body , a low caudal fin comprising nearly half the total length , and a pattern of dark spots on a pale background . Young zebra sharks under 50 – 90 cm ( 20 – 35 in ) long have a completely different pattern , consisting of light vertical stripes on a brown background , and lack the ridges . This species attains a length of 2.5 m ( 8.2 ft ) . Zebra sharks are nocturnal and spend most of the day resting motionless on the sea floor . At night , they actively hunt for molluscs , crustaceans , small bony fishes , and possibly sea snakes i</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Soyuz TM-30 = Soyuz TM-30 ( Russian : Союз ТМ-30 , Union TM-30 ) , also known as Mir EO-28 , was a Soyuz mission , the 39th and final human spaceflight to the Mir space station . The crew of the mission was sent by MirCorp , a privately funded company , to reactivate and repair the station . The crew also resupplied the station and boosted the station to an orbit with a low point ( perigee ) of 360 and a high point ( apogee ) of 378 kilometers ( 223 and 235 miles , respectively ) . The boost in the station 's orbit , which was done by utilizing the engines of the Progress M1-1 and M1-2 spacecraft , made transit between Mir and the International Space Station impossible , as desired by NASA . The mission was the first privately funded mission to a space station . The mission was part of an effort by MirCorp to refurbish and privatize the aging Mir space station , which was nearing the end of its operational life . Further commercially funded missions beyond Soyuz TM-30 were originally p</t>
+          <t>Australian blacktip shark = The Australian blacktip shark ( Carcharhinus tilstoni ) is a species of requiem shark , in the family Carcharhinidae , endemic to northern and eastern Australia . Favoring the upper and middle parts of the water column , it can be found from the intertidal zone to a depth of 50 m ( 160 ft ) . Appearance-wise this species is virtually identical to the common blacktip shark ( C. limbatus ) , from which it can be reliably distinguished only by its lower vertebra number and by genetic markers . Generally reaching 1.5 – 1.8 m ( 4.9 – 5.9 ft ) in length , it is a fairly stout-bodied , bronze-colored shark with a long snout and black-tipped fins . Primarily piscivorous , the Australian blacktip shark forms large groups of similar size and sex that tend to remain within a local area . It exhibits vivipary , meaning that the unborn young are provisioned through a placental connection . There is a well-defined annual reproductive cycle with mating occurring in Februar</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Apollo program = The Apollo program , also known as Project Apollo , was the third United States human spaceflight program carried out by the National Aeronautics and Space Administration ( NASA ) , which accomplished landing the first humans on the Moon from 1969 to 1972 . First conceived during Dwight D. Eisenhower 's administration as a three-man spacecraft to follow the one-man Project Mercury which put the first Americans in space , Apollo was later dedicated to President John F. Kennedy 's national goal of " landing a man on the Moon and returning him safely to the Earth " by the end of the 1960s , which he proposed in an address to Congress on May 25 , 1961 . Kennedy 's goal was accomplished on the Apollo 11 mission when astronauts Neil Armstrong and Buzz Aldrin landed their Lunar Module ( LM ) on July 20 , 1969 , and walked on the lunar surface , while Michael Collins remained in lunar orbit in the Command / Service Module ( CSM ) , and all three landed safely on Earth on July </t>
+          <t>Smalleye hammerhead = The smalleye hammerhead or golden hammerhead ( Sphyrna tudes ) , is a small species of hammerhead shark , belonging to the family Sphyrnidae . This species is common in the shallow coastal waters of the western Atlantic Ocean , from Venezuela to Uruguay . It favors muddy habitats with poor visibility , reflected by its relatively small eyes . Adult males and juveniles are schooling and generally found apart from the solitary adult females . Typically reaching 1.2 – 1.3 m ( 3.9 – 4.3 ft ) in length , this shark has a unique , bright golden color on its head , sides , and fins , which was only scientifically documented in the 1980s . As in all hammerheads , its head is flattened and laterally expanded into a hammer-shaped structure called the " cephalofoil " , which in this species is wide and long with an arched front margin bearing central and lateral indentations . The yellow-orange pigments of the smalleye hammerhead seem to have been acquired from the penaeid s</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Space Interferometry Mission = The Space Interferometry Mission , or SIM , also known as SIM Lite ( formerly known as SIM PlanetQuest ) , was a planned space telescope developed by the U.S. National Aeronautics and Space Administration ( NASA ) , in conjunction with contractor Northrop Grumman . One of the main goals of the mission was the hunt for Earth-sized planets orbiting in the habitable zones of nearby stars other than the Sun . SIM was postponed several times and finally cancelled in 2010 . In addition to hunting for extrasolar planets , SIM would have helped astronomers construct a map of the Milky Way galaxy . Other important tasks would have included collecting data to help pinpoint stellar masses for specific types of stars , assisting in the determination of the spatial distribution of dark matter in the Milky Way and in the Local Group of galaxies and using the gravitational microlensing effect to measure the mass of stars . The spacecraft would have used optical interfer</t>
+          <t xml:space="preserve">Smalltooth sand tiger = The smalltooth sand tiger or bumpytail ragged-tooth ( Odontaspis ferox ) is a species of mackerel shark in the family Odontaspididae , with a patchy but worldwide distribution in tropical and warm temperate waters . They usually inhabit deepwater rocky habitats , though they are occasionally encountered in shallow water , and have been known to return to the same location year after year . This rare species is often mistaken for the much more common grey nurse shark ( Carcharias taurus ) , from which it can be distinguished by its first dorsal fin , which is larger than the second and placed further forward . It grows to at least 4.1 m ( 13.5 ft ) in length . Very little is known of the biology and behavior of the smalltooth sand tiger . It is an active predator of benthic bony fishes , invertebrates , and cartilaginous fishes . This species is thought to be ovoviviparous with oophagous embryos like other mackerel sharks . In contrast to its formidable size and </t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>STS-8 = STS-8 was the eighth NASA Space Shuttle mission and the third flight of the Space Shuttle Challenger . It launched on August 30 , 1983 and landed on September 5 , conducting the first night launch and night landing of the Space Shuttle program . It also carried the first African-American astronaut , Guion Bluford . The mission successfully achieved all of its planned research objectives , but was marred by the subsequent discovery that a solid-fuel rocket booster had almost malfunctioned catastrophically during the launch . The mission 's primary payload was INSAT-1B , an Indian communications and weather observation satellite , which was released by the orbiter and boosted into a geostationary orbit . The secondary payload , replacing a delayed NASA communications satellite , was a four-metric-ton dummy payload , intended to test the use of the shuttle 's " Canadarm " remote manipulator system . Scientific experiments carried onboard Challenger included the environmental testi</t>
+          <t>Yellow stingray = The yellow stingray ( Urobatis jamaicensis ) is a species of stingray in the family Urotrygonidae , found in the tropical western Atlantic Ocean from North Carolina to Trinidad . This bottom-dwelling species inhabits sandy , muddy , or seagrass bottoms in shallow inshore waters , commonly near coral reefs . Reaching no more than 36 cm ( 14 in ) across , the yellow stingray has a round pectoral fin disc and a short tail with a well-developed caudal fin . It has a highly variable but distinctive dorsal color pattern consisting of either light-on-dark or dark-on-light reticulations forming spots and blotches , and can rapidly change the tonality of this coloration to improve its camouflage . Relatively sedentary during the day , the yellow stingray feeds on small invertebrates and bony fishes . When hunting it may undulate its disc to uncover buried prey , or lift the front of its disc to form a " cave " attractive to shelter-seeking organisms . This species is aplacenta</t>
         </is>
       </c>
     </row>
@@ -1911,32 +1911,32 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>['phillies', 'inning', 'yankees', 'dodgers', 'giants', 'yankee', 'breaker', 'innings', 'tie', 'pitcher', 'run', 'braves', 'game', 'runs', 'pennant']</t>
+          <t>['ride', 'train', 'coaster', 'roller', 'riders', 'station', 'steel', 'trains', 'lift', 'operate', 'hour', 'brake', 'drop', 'themed', 'officially']</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2013 American League Wild Card tie-breaker game = The 2013 American League Wild Card tie-breaker game was a one-game extension to Major League Baseball 's ( MLB ) 2013 regular season , played between the Texas Rangers and Tampa Bay Rays to determine the second participant in the 2013 American League ( AL ) Wild Card Game . It was played at the Rangers Ballpark in Arlington on September 30 , 2013 . The Rays defeated the Rangers , 5 – 2 , and advanced to the AL Wild Card Game against the Cleveland Indians at Progressive Field , which they won 4 – 0 ; the Rangers failed to qualify for the postseason . The tie-breaker game was necessary after both teams finished the season with win – loss records of 91 – 71 and thus tied for the second Wild Card position in the AL . The Rangers were awarded home field for the game , as they won the regular season series against the Rays , four-games-to-three . The game was televised on TBS . It was the fourth tie-breaker in MLB history for a Wild Card spot</t>
+          <t>Nitro ( Adlabs Imagica ) = Nitro is a steel Floorless Coaster at the Adlabs Imagica amusement park located in Khopoli , Mumbai , India . Manufactured by Bolliger &amp; Mabillard , the roller coaster reaches a maximum height of 132 feet ( 40 m ) and a maximum speed of 65.2 miles per hour ( 104.9 km / h ) . The coaster also features five inversions . Nitro opened to the public in October 2013 . = = History = = As construction progressed with the theme park in early 2013 , the owners of the park gave no details about the roller coaster other than that it would be the largest roller coaster in India . Even after the Roller Coaster Database reported that a Bolliger &amp; Mabillard Floorless Coaster would be built at the park , the owners still released no details . In April 2013 , the first pieces of the roller coaster were erected . By the end of August , all of the coaster 's track was installed . Then in the third quarter of 2013 , Adlabs Imagica released the details of Nitro . Nitro was origina</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2014 National League Wild Card Game = The 2014 National League Wild Card Game was a play-in game during Major League Baseball 's ( MLB ) 2014 postseason played between the National League 's ( NL ) two wild card teams , the San Francisco Giants and the Pittsburgh Pirates . It was held at PNC Park in Pittsburgh , Pennsylvania , on October 1 , 2014 , starting at 8 : 07 p.m. EDT . After both teams finished the regular season with identical records of 88 – 74 , the Pirates were awarded home field for the game , as they won the season series against the Giants , four games to two . Despite this advantage , the Giants won by a score of 8 – 0 and advanced to play the Washington Nationals in the NL Division Series ( NLDS ) . In addition to being the third NL Wild Card Game played , it is notable for the first postseason grand slam hit by a shortstop . The game was televised on ESPN , and was also broadcast on ESPN Radio . = = Background = = In Major League Baseball , the two teams with the bes</t>
+          <t>Hollywood Rip Ride Rockit = Hollywood Rip Ride Rockit is a steel roller coaster at Universal Studios Florida in Orlando , Florida . With a height of 167 feet ( 51 m ) , a length of 3,800 feet ( 1,200 m ) , and a top speed of 65 miles per hour ( 105 km / h ) , it is the largest X-Coaster ever built by German manufacturer Maurer Söhne . It was announced on March 19 , 2008 and officially opened on August 19 , 2009 though originally planned to open in the spring of that year . Some of the special features are that riders are recorded during the entire 1 minute and 37 second ride and can choose one of thirty songs to listen to during the experience . = = History = = During the second week of January 2008 , Universal Parks &amp; Resorts filed a Notice of Commencement with Orange County , Florida indicating that they were to construct a ride system that they had code-named " Project Rumble . " The notice also stated that the contractor was " Maurer Rides GmbH , " located in Munich , Germany . Aft</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1951 National League tie-breaker series = The 1951 National League tie-breaker series was a best-of-three playoff series at the conclusion of Major League Baseball 's ( MLB ) 1951 regular season to decide the winner of the National League ( NL ) pennant . The games were played on October 1 , 2 , and 3 , 1951 , between the New York Giants and Brooklyn Dodgers . It was necessary after both teams finished the season with identical win – loss records of 96 – 58 . It is most famous for the walk-off home run hit by Bobby Thomson of the Giants in the deciding game , which has come to be known as baseball 's " Shot Heard ' Round the World " . This was the second three-game playoff in NL history . After no tiebreakers had been needed since the American League ( AL ) became a major league in 1901 , this was the third such tie in the previous six seasons . The Dodgers had been involved in the previous one as well , losing to the St. Louis Cardinals during the 1946 season in two straight games . I</t>
+          <t xml:space="preserve">NSB Class 93 = NSB Class 93 ( Norwegian : NSB-type 93 ) is a tilting two-carriage diesel multiple unit used by Norwegian State Railways ( NSB ) for passenger trains on non-electrified stretches of the Norwegian railway network . Used on the Nordland Line , the Røros Line and the Rauma Line , they were purchased to replace the aging Di3 locomotive-hauled trains . The Class 93 was produced by Bombardier , and is part of the Talent family . Fifteen units were delivered between 2000 and 2002 . Powered by two Cummins diesel engines with a combined output of 612 kW ( 821 hp ) , the trains are capable of speeds of 140 km / h ( 87 mph ) . The trains entered service as part of the Agenda regional train concept . However , the technical problems to which the units have been prone and a cramped interior design have made them unpopular among riders . In 2007 , the units were replaced by locomotive-hauled trains on some services on the Nordland Line . = = History = = During the mid-1990s , NSB had </t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t xml:space="preserve">1999 National League Wild Card tie-breaker game = The 1999 National League wild-card tie-breaker game was a one-game extension to Major League Baseball 's ( MLB ) 1999 regular season , played between the New York Mets and Cincinnati Reds to determine the winner of the National League ( NL ) wild card . It was played at Cinergy Field in Cincinnati , on October 4 , 1999 . The Mets won the game 5 – 0 , with starting pitcher Al Leiter pitching a two-hit shutout . As a result , the Mets qualified for the postseason and the Reds did not . The game was necessary after both teams finished the season with identical win – loss records of 96 – 66 . Some described the Mets as collapsing late in the season while the race between the Reds and their division rival Houston Astros was close enough to create the possibility of a three-way tie . The Reds won a coin flip late in the season which , by rule at the time , awarded them home field for the game . Upon winning , the Mets advanced to NL Division </t>
+          <t>Trondheim Central Station = Trondheim Central Station ( Norwegian : Trondheim sentralstasjon ) or Trondheim S is the main railway station serving the city of Trondheim , Norway . Located at Brattøra in the north part of the city centre , it is the terminus of the Dovre Line , running southwards , and the Nordland Line , which runs north . The railway is electrified south of the station but not north of it , so through trains must change locomotives at the station . The Norwegian State Railways ( NSB ) serves the station with express trains to Oslo and Bodø , regional trains to Røros and Östersund in Sweden , and the Trøndelag Commuter Rail . The Trondheim Bus Station located at the station serves all long-distance buses , and some city buses . From 1913 to 1968 the station was also the terminus for two lines of the Trondheim Tramway . Trondheim 's first station , dating from 1864 , was located at Kalvskinnet . In 1877 the current station was built to serve the Meråker Line line to Swed</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t xml:space="preserve">1959 National League tie-breaker series = The 1959 National League tie-breaker series was a best-of-three playoff series at the conclusion of Major League Baseball 's ( MLB ) 1959 regular season to decide the winner of the National League ( NL ) pennant . The games were played on September 28 and 29 , 1959 , between the Los Angeles Dodgers and the Milwaukee Braves . The first game was played at Milwaukee County Stadium and the second took place at Los Angeles Memorial Coliseum . The playoff series was necessary after both teams finished the season with identical win – loss records of 86 – 68 . The Dodgers won a coin flip late in the season that gave them home field advantage for the series , although the series did not reach a third game . Following a rain-delayed start , the Dodgers won Game 1 by a close 3 – 2 score , with a home run by John Roseboro providing the margin of victory . The Dodgers then won the series and the pennant with another close victory in Game 2 ; they came back </t>
+          <t>Broadway Limited = The Broadway Limited was a passenger train operated by the Pennsylvania Railroad between New York City and Chicago . It operated from 1912 to 1995 . It was the Pennsylvania 's premier train , competing directly with the New York Central Railroad 's 20th Century Limited . The Broadway Limited continued operating after the Penn Central Transportation merger , one of the few long-distance trains to do so . Penn Central conveyed the train to Amtrak in 1971 ; Amtrak discontinued it in 1995 . The train 's name referred not to Broadway in Manhattan , but rather to the " broad way " of the Pennsylvania 's four-track right of way along a large portion of the route . = = History = = = = = Pennsylvania Railroad = = = The Pennsylvania Special was one of nine express trains the Pennsylvania operated between New York City and Chicago . On November 14 , 1912 the Pennsylvania renamed it the Broadway Limited , to avoid confusion with the similarly-named Pennsylvania Limited . The nam</t>
         </is>
       </c>
     </row>
@@ -1946,32 +1946,32 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>['amendment', 'shall', 'constitution', 'clause', 'defendant', 'states', 'rights', 'congress', 'jury', 'amendments', 'ratification', 'constitutional', 'supreme_court', 'senate', 'convention']</t>
+          <t>['building', 'church', 'stone', 'wall', 'built', 'site', 'listed', 'roof', 'windows', 'century', 'walls', 'buildings', 'tower', '19th', 'restoration']</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Crimes Act of 1790 = The Crimes Act of 1790 ( or the Federal Criminal Code of 1790 ) , formally titled An Act for the Punishment of Certain Crimes Against the United States , defined some of the first federal crimes in the United States and expanded on the criminal procedure provisions of the Judiciary Act of 1789 . The Crimes Act was a " comprehensive statute defining an impressive variety of federal crimes . " As an enactment of the First Congress , the Crimes Act is often regarded as a quasi-constitutional text . The punishment of treason , piracy , counterfeiting , as well as crimes committed on the high seas or against the law of nations , followed from relatively explicit constitutional authority . The creation of crimes within areas under exclusive federal jurisdiction followed from the plenary power of Congress over the " Seat of the Government , " federal enclaves , and federal territories . The creation of crimes involving the integrity of the judicial process derived from Co</t>
+          <t>St Eugrad 's Church , Llaneugrad = St Eugrad 's Church , Llaneugrad is an isolated church near the village of Marian-glas , in Anglesey , north Wales . A church was supposedly founded here by St Eugrad in about 605 , although the earliest parts of the present structure are the nave , chancel and chancel arch , which date from the 12th century . A side chapel was added to the north in the 16th century , and some moderate restoration work was carried out in the 19th century . It contains a 12th-century font , a 13th-century carved stone depicting the crucifixion , and a memorial to one of the officers killed when the Royal Charter sank off Anglesey in 1859 . The church is still used for worship by the Church in Wales , one of four in a combined parish ; one of the others is St Gallgo 's Church , Llanallgo , founded by Eugrad 's brother . As of 2012 , the parish does not have an incumbent priest . St Eugrad 's is a Grade II * listed building , a national designation given to " particularl</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t xml:space="preserve">United States constitutional criminal procedure = The United States Constitution contains several provisions regarding the law of criminal procedure . Petit jury and venue provisions — both traceable to enumerated complaints in the Declaration of Independence — are included in Article Three of the United States Constitution . More criminal procedure provisions are contained in the United States Bill of Rights , specifically the Fifth , Sixth , and Eighth Amendments . With the exception of the Grand Jury Clause of the Fifth Amendment , the Vicinage Clause of the Sixth Amendment , and ( maybe ) the Excessive Bail Clause of the Eighth Amendment , all of the criminal procedure provisions of the Bill of Rights have been incorporated to apply to the state governments . Several of these rights regulate pre-trial procedure : access to a non-excessive bail , the right to indictment by a grand jury , the right to an information ( charging document ) , the right to a speedy trial , and the right </t>
+          <t>St Michael 's Church , Llanfihangel Ysgeifiog = St Michael 's Church , Llanfihangel Ysgeifiog , is a former parish church in Anglesey , Wales , which is now closed and in ruins . The structure dates from the 15th century and a chapel was added to the north side in the 17th century . A replacement church ( St Michael 's , Gaerwen ) was built elsewhere in the parish in 1847 , and the old church was closed , partly demolished and abandoned . Some restoration work has taken place in the 21st century and some occasional services have been held . It is a Grade II listed building , a national designation given to " buildings of special interest , which warrant every effort being made to preserve them " , in particular because it is " an important survival , retaining unrestored original late medieval features . " = = History and location = = St Michael 's Church is set in a churchyard in the countryside of Anglesey , north Wales , about 1.4 kilometres ( 0.87 mi ) from the village of Gaerwen .</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Vicinage Clause = The Vicinage Clause is a provision in the Sixth Amendment to the United States Constitution regulating the vicinity from which a jury pool may be selected . The clause says that the accused shall be entitled to a jury " of the State and district wherein the crime shall have been committed , which district shall have been previously ascertained by law " . The Vicinage Clause limits the vicinity of criminal jury selection to both the state and the federal judicial district where the crime has been committed whereas the venue provision of Article Three of the United States Constitution regulates the location of the actual trial . The Vicinage clause has its roots in medieval English criminal procedure , the perceived abuses of criminal vicinage and venue during the colonial period and Anti-federalist objections to the United States Constitution . The clause is one of the few constitutional criminal procedure provisions that has not been incorporated to apply to proceedin</t>
+          <t>Bishop 's Palace , Wells = The Bishop 's Palace and accompanying Bishops House at Wells in the English county of Somerset , is adjacent to Wells Cathedral and has been the home of the Bishops of the Diocese of Bath and Wells for 800 years . It has been designated by English Heritage as a Grade I listed building . Building of the palace started around 1210 by Bishops Jocelin of Wells and Reginald Fitz Jocelin . The chapel and great hall were added by Bishop Robert Burnell between 1275 and 1292 . The walls , gatehouse and moat were added in the 14th century by Bishop Ralph of Shrewsbury . The Bishops House was added in the 15th century by Bishop Thomas Beckington . The great hall later fell into disrepair and was partially demolished around 1830 . The palace was originally surrounded by a medieval deer park . When the walls were built , streams were diverted to form the moat as a reservoir . In the 1820s , the grounds within the walls were planted and laid out as pleasure grounds by Bish</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Section Thirty-four of the Canadian Charter of Rights and Freedoms = Section 34 of the Canadian Charter of Rights and Freedoms is the last section of Canada 's Charter of Rights , which is entrenched in the Constitution Act , 1982 . Section 34 provides guidance for the legal citation of the Charter . The section has been interpreted by Canadian writers , who have analyzed both its intention and its meaning . Because the section affirms the name of the Charter and thus entrenches it in the Constitution Act , it came into focus in 1994 when a Member of Parliament ( MP ) proposed to change the name of the Charter . = = Text = = Under the heading " Citation , " the section reads : = = Function = = Section 34 , as part of the Constitution Act , 1982 , came into force on April 17 , 1982 . According to the government of Canada , section 34 's function " simply " relates to citation . The section clarifies that the first 34 sections of the Constitution Act , 1982 may be collectively called the</t>
+          <t>Avery Homestead = The Avery Homestead is a two-story Colonial-style home in Ledyard , Connecticut that was built circa 1696 . Evidence suggests that the house may have begun as a single-story , one-room house and later expanded to a two-story , two-room house by 1726 . The house underwent major additions and renovations by Theophilus Avery and later his grandson , Theophilus Avery . In the mid-1950s , Amos Avery began a decade-long restoration effort to return the house to its 18th-century appearance . The Avery Homestead is historically significant as a well-preserved example of an 18th-century farmhouse with fine craftsmanship . The home is also historically important because more than twelve generations of the Avery family have resided there over the course of three centuries . The Avery Homestead was listed on the National Register of Historic Places in 1992 . = = Overview = = The Avery Homestead is located on the west side of Ledyard , Connecticut and faces south on Avery Hill Roa</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Fifteenth Amendment to the United States Constitution = The Fifteenth Amendment ( Amendment XV ) to the United States Constitution prohibits the federal and state governments from denying a citizen the right to vote based on that citizen 's " race , color , or previous condition of servitude . " It was ratified on February 3 , 1870 , as the third and last of the Reconstruction Amendments . In the final years of the American Civil War and the Reconstruction Era that followed , Congress repeatedly debated the rights of the millions of black former slaves . By 1869 , amendments had been passed to abolish slavery and provide citizenship and equal protection under the laws , but the election of Ulysses S. Grant to the presidency in 1868 convinced a majority of Republicans that protecting the franchise of black voters was important for the party 's future . After rejecting more sweeping versions of a suffrage amendment , Congress proposed a compromise amendment banning franchise restrictions</t>
+          <t>College of All Saints , Maidstone = The College of All Saints was an ecclesiastical college in Maidstone , Kent , England , founded in 1395 by Archbishop Courtenay . It was part of the establishment of the nearby Archbishop 's Palace , but was closed in 1546 . The College church was the neighbouring Church of All Saints . Following its closure , the College estate was sold . The buildings and land passed through the ownership of three aristocratic families , being farmed until the late 19th century . A number of the College 's buildings survive and all are listed buildings . Additionally , the whole site of the College is protected as a scheduled monument . = = History = = The College was founded by Archbishop of Canterbury William Courtenay in 1395 . Courtenay died in 1396 and the College and church were completed by his successor , Thomas Arundel . Richard II endowed the College with land and income from the Hospital of St Peter and St Paul in Maidstone and from the parishes of Linto</t>
         </is>
       </c>
     </row>
@@ -1981,32 +1981,32 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>['singapore', 'law', 'judicial', 'parliament', 'constitution', 'article', 'courts', 'minister', 'court', 'constitutional', 'high_court', 'persons', 'public', 'tribunal', 'act']</t>
+          <t>['battle', 'men', 'army', 'troops', 'french', 'command', 'general', 'british', 'sent', 'attack', 'soldiers', 'forces', 'wounded', 'killed', 'commanded']</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Article 14 of the Constitution of Singapore = Article 14 of the Constitution of the Republic of Singapore , specifically Article 14 ( 1 ) , guarantees to Singapore citizens the rights to freedom of speech and expression , peaceful assembly without arms , and association . However , the enjoyment of these rights may be restricted by laws imposed by the Parliament of Singapore on the grounds stated in Article 14 ( 2 ) of the Constitution . There are two types of grounds . For the first type , it must be shown that restricting the rights is " necessary or expedient in the interest " of the grounds . The grounds are the security of Singapore and public order ( applicable to all three rights protected by Article 14 ( 1 ) ) , morality ( freedom of speech and freedom of association ) , and friendly relations with other countries ( freedom of speech only ) . In a 2005 judgment , the High Court expressed the view that the phrase necessary or expedient confers upon Parliament " an extremely wide</t>
+          <t>Battle of the Lippe = The Battle of the Lippe was a cavalry action fought on 2 September 1595 on the banks of the Lippe river , in Germany , between a corps of Spanish cavalry led by Juan de Córdoba and a corps of Dutch cavalry , supported by English troops , led by Philip of Nassau . The Dutch statholder Maurice of Nassau , taking advantage of the fact that the bulk of the Spanish army was busied in operations in France , besieged the town of Groenlo in Gelderland , but the elderly governor of the citadel of Antwerp , Cristóbal de Mondragón , organized a relief army and forced Maurice to lift the siege . Mondragón next moved to Wesel , positioning his troops on the southern bank of the Lippe river to cover Rheinberg from a Dutch attack . Maurice aimed then , relying on his superior army , to entice Mondragón into a pitched battle , planning to use an ambush to draw the Spanish army into a trap . However , the plan was discovered by the Spanish commander , who organized a counter-ambus</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Rule of law doctrine in Singapore = In Singapore , the rule of law doctrine has been the topic of considerable disagreement and debate , largely through differing conceptions of the doctrine . These conceptions can generally be divided into two categories developed by legal academics , the " thin " , or formal , conception and the " thick " , or substantive , conception of the rule of law . The thin conception , often associated with the legal scholars Albert Venn Dicey and Joseph Raz , advocates the view that the rule of law is fulfilled by adhering to formal procedures and requirements , such as the stipulations that all laws be prospective , clear , stable and constitutionally enacted , and that the parties to legal disputes are treated equally and without bias on the part of judges . While people subscribing to the thin conception do not dismiss the importance of the content of the law , they take the view that this is a matter of substantive justice and should not be regarded as p</t>
+          <t xml:space="preserve">Battle of Spencer 's Ordinary = The Battle of Spencer 's Ordinary was an inconclusive skirmish that took place on 26 June 1781 , late in the American Revolutionary War . British forces under Lieutenant Colonel John Graves Simcoe and American forces under Colonel Richard Butler , light detachments from the armies of General Lord Cornwallis and the Marquis de Lafayette respectively , clashed near a tavern ( the " ordinary " ) at a road intersection not far from Williamsburg , Virginia . Lafayette had been shadowing Cornwallis as he moved his army toward Williamsburg from central Virginia . Aware that Simcoe had become separated from Cornwallis , he sent Butler out in an attempt to cut Simcoe off . Both sides , concerned that the other might be reinforced by its main army , eventually broke off the battle . = = Background = = In May 1781 , Lord Charles Cornwallis arrived in Petersburg , Virginia after a lengthy campaign through North and South Carolina . In addition to his 1,400 troops , </t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Article 9 of the Constitution of Singapore = Article 9 of the Constitution of the Republic of Singapore , specifically Article 9 ( 1 ) , guarantees the right to life and the right to personal liberty . The Court of Appeal has called the right to life the most basic of human rights , but has yet to fully define the term in the Constitution . Contrary to the broad position taken in jurisdictions such as Malaysia and the United States , the High Court of Singapore has said that personal liberty only refers to freedom from unlawful incarceration or detention . Article 9 ( 1 ) states that persons may be deprived of life or personal liberty " in accordance with law " . In Ong Ah Chuan v. Public Prosecutor ( 1980 ) , an appeal to the Judicial Committee of the Privy Council from Singapore , it was held that the term law means more than just legislation validly enacted by Parliament , and includes fundamental rules of natural justice . Subsequently , in Yong Vui Kong v. Attorney-General ( 2011 </t>
+          <t>Battle of Jumonville Glen = The Battle of Jumonville Glen , also known as the Jumonville affair , was the opening battle of the French and Indian War fought on May 28 , 1754 near what is present-day Hopwood and Uniontown in Fayette County , Pennsylvania . A company of colonial militia from Virginia under the command of Lieutenant Colonel George Washington , and a small number of Mingo warriors led by Tanacharison ( also known as " Half King " ) , ambushed a force of 35 Canadiens under the command of Joseph Coulon de Villiers de Jumonville . The British colonial force had been sent to protect a fort under construction under the auspices of the Ohio Company at the location of present-day Pittsburgh , Pennsylvania . A larger Canadien force had driven off the small construction crew , and sent Jumonville to warn Washington about encroaching on French-claimed territory . Washington was alerted to Jumonville 's presence by Tanacharison , and they joined forces to surround the Canadian camp .</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Article 12 of the Constitution of Singapore = Article 12 of the Constitution of the Republic of Singapore guarantees to all persons equality before the law and equal protection of the law . The Article also identifies four forbidden classifications – religion , race , descent and place of birth – upon which Singapore citizens may not be discriminated for specific reasons . For example , discrimination on those classifications is prohibited in the appointment to any office or employment under a public authority or in the administration of any law relating to the establishing or carrying on of any trade , business , profession , vocation or employment . Persons unable to show that one of the forbidden classifications applies to them may try to argue that they are members of a group defined by a law in a way that violates the general guarantee of equality and equal protection . To succeed , they must establish that the classification used in the law fails the rational nexus test , which i</t>
+          <t>Siege of Fort St. Jean = The Siege of Fort St. Jean ( also called St. John , St. Johns , or St. John 's ) was conducted by American Brigadier General Richard Montgomery on the town and fort of Saint-Jean in the British province of Quebec during the American Revolutionary War . The siege lasted from September 17 to November 3 , 1775 . After several false starts in early September , the Continental Army established a siege around Fort St. Jean . Beset by illness , bad weather , and logistical problems , they established mortar batteries that were able to penetrate into the interior the fort , but the defenders , who were well-supplied with munitions , but not food and other supplies , persisted in their defence , believing the siege would be broken by forces from Montreal under General Guy Carleton . On October 18 , the nearby Fort Chambly fell , and on October 30 , an attempt at relief by Carleton was thwarted . When word of this made its way to St. Jean 's defenders , combined with a n</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Section 3 of the Human Rights Act 1998 = Section 3 of the Human Rights Act 1998 is a provision of the Human Rights Act 1998 that enables the Act to take effect in the United Kingdom . The section requires courts to interpret both primary and subordinate legislation so that their provisions are compatible with the articles of the European Convention of Human Rights , which are also part of the Human Rights Act 1998 . This interpretation goes far beyond normal statutory interpretation , and includes past and future legislation , therefore preventing the Human Rights act from being impliedly repealed by subsequent contradictory legislation . Courts have applied section 3 of the Act through three forms of interpretation : " reading in " – inserting words where there are none in a statute ; " reading out " where words are omitted from a statute ; and " reading down " where a particular meaning is chosen to be in compliance . They do not interpret statutes to conflict with legislative intent</t>
+          <t>Battle of Cobleskill = The Battle of Cobleskill ( also known as the Cobleskill massacre ) was an American Revolutionary War raid on the frontier settlement of Cobleskill , New York on May 30 , 1778 . The battle , having taken place in the modern-day village of Warnerville , NY near Cobleskill-Richmondville High School , marked the beginning of a phase in which Loyalists and Iroquois , encouraged and supplied by British authorities in the Province of Quebec , raided and destroyed numerous villages on what was then the United States western frontier of New York and Pennsylvania . A small party of Iroquois entered Cobleskill and drew the local defenders into a trap set by a much larger party of Iroquois and Loyalists under the command of Joseph Brant . After killing a number of the militia and driving off the remainder , Brant 's forces destroyed much of the settlement . New York 's defenders retaliated against Brant 's actions against Cobleskill and other communities by destroying Iroquo</t>
         </is>
       </c>
     </row>
@@ -2016,32 +2016,32 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>['motorway', 'croatia', 'toll', 'croatian', 'traffic', 'interchanges', 'kilometre', 'route', 'interchange', 'section', 'rest', 'kilometres', 'areas', 'tunnels', 'construction']</t>
+          <t>['championship', 'match', 'title', 'defeated', 'event', 'team', 'face', 'won', 'night', 'following', 'kane', 'attacked', 'main', 'wrestler', 'win']</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t xml:space="preserve">A5 ( Croatia ) = The A5 motorway ( Croatian : Autocesta A5 ) is a motorway in Croatia spanning 55.5 kilometres ( 34.5 mi ) . It connects Osijek , the largest city in Slavonia region , to the Croatian motorway network at the Sredanci interchange of the A3 motorway . The A5 represents a significant north – south transportation corridor in Croatia and is a part of the European route E73 . The A5 motorway route also follows Pan-European corridor Vc . In addition to Osijek , the A5 motorway also passes near Đakovo . The first section of the A5 , joining the Sredanci interchange to Đakovo , was opened in 2007 ; the route to Osijek opened in 2009 . As of September 2011 , the section south of the A3 , extending to the Sava River and border of Bosnia and Herzegovina , is under construction . Once the entire Pan-European corridor Vc is completed , motorists will recognize the A5 's importance as a transit route . When completed , the corridor shall entail the A5 itself extended to the Hungarian </t>
+          <t>Judgment Day ( 2008 ) = Judgment Day ( 2008 ) was a professional wrestling pay-per-view event produced by World Wrestling Entertainment ( WWE ) and sponsored by Lionsgate 's Rambo , which took place on May 18 , 2008 , at the Qwest Center Omaha in Omaha , Nebraska . It was the tenth annual Judgment Day event and starred wrestlers from the Raw , SmackDown , and ECW brands . The show 's seven matches showcased prominent WWE wrestlers , who acted out the franchise 's stories in and out of the ring . The main event featured Raw wrestlers in a Steel Cage match , a match in a ring surrounded by four walls of mesh metal . In this match , WWE Champion Triple H defeated Randy Orton to retain his title . In SmackDown 's main match , The Undertaker defeated Edge by countout , but did not win the vacant World Heavyweight Championship because in WWE , a championship cannot change hands via countout or disqualification . While in ECW 's prime match , WWE Tag Team Champions John Morrison and The Miz d</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>A6 ( Croatia ) = The A6 motorway ( Croatian : Autocesta A6 ) is a motorway in Croatia spanning 80.2 kilometres ( 49.8 mi ) . It connects the nation 's capital , Zagreb , via the A1 , to the seaport of Rijeka . The motorway forms a major north – south transportation corridor in Croatia and is a part of European route E65 Nagykanizsa – Zagreb – Rijeka – Zadar – Split – Dubrovnik – Podgorica . The A6 motorway route also follows Pan-European corridor Vb . The A6 motorway runs near a number of Croatian cities , provides access to Risnjak National Park and indirectly to numerous resorts , notably in the Istria and Kvarner Gulf regions . The motorway route was completed in 2008 . The motorway is nationally significant because of its positive economic impact on the cities and towns it connects , and because of its contribution to tourism in Croatia . The importance of the motorway as a transit route will be further increased upon completion of a proposed expansion of the Port of Rijeka and Rij</t>
+          <t>Shawn Michaels = Michael Shawn Hickenbottom ( born July 22 , 1965 ) , better known by his ring name Shawn Michaels , is an American professional wrestling personality , television presenter and retired professional wrestler . He has been signed to WWE , as an ambassador and occasional non-wrestling performer , since December 2010 . Michaels wrestled consistently for WWE , formerly the World Wrestling Federation ( WWF ) , from 1988 until his first retirement in 1998 . He held non-wrestling roles from 1998 to 2000 and resumed wrestling in 2002 until retiring ceremoniously in 2010 . In the WWF / E , Michaels headlined major pay-per-view events between 1989 and 2010 , closing the company 's flagship annual event , WrestleMania , five times . He was the co-founder and original leader of the successful stable , D-Generation X. He also wrestled in the American Wrestling Association ( AWA ) , where he founded The Midnight Rockers with Marty Jannetty in 1985 . After winning the AWA Tag Team Cha</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>A3 ( Croatia ) = The A3 motorway ( Croatian : Autocesta A3 ) is a major motorway in Croatia spanning 306.5 kilometres ( 190.5 mi ) . The motorway connects Zagreb , the nation 's capital , to the Slavonia region and a number of cities along the Sava River . It represents a major east – west transportation corridor in Croatia and a significant part of the Pan-European Corridor X , serving as a transit route between the European Union states and the Balkans . Apart from Zagreb , where the A3 motorway comprises a considerable part of the Zagreb bypass , the motorway runs near a number of significant Croatian cities . The motorway has a positive economic impact on the cities and towns it connects , and is an important route within Croatia . The motorway consists of two traffic lanes and an emergency lane in each driving direction , separated by a central reservation . All intersections of the A3 motorway are grade separated , and the motorway comprises several large stack and cloverleaf int</t>
+          <t>Sacrifice ( 2008 ) = Sacrifice ( 2008 ) was a professional wrestling pay-per-view ( PPV ) event produced by the Total Nonstop Action Wrestling ( TNA ) promotion that took place on May 11 , 2008 at the TNA Impact ! Zone in Orlando , Florida . It was the fourth event in the Sacrifice chronology and fifth event in the 2008 TNA PPV schedule . Ten professional wrestling matches , two for championships , were featured on the card . The main event was a Three Way match for the TNA World Heavyweight Championship between then-champion Samoa Joe and challengers Kaz and Scott Steiner . The match was initially promoted as Joe 's defense of his title against Kurt Angle and Steiner . However , Angle sustained an injury before the match that removed him from the bout ; he was replaced with Kaz . Joe won the match , retaining the championship . The Deuces Wild Tag Team Tournament for the vacant TNA World Tag Team Championship was also held at Sacrifice . The Latin American Xchange ( Hernandez and Homi</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Delaware Route 37 = Delaware Route 37 ( DE 37 ) is a state highway in New Castle County , Delaware . The route runs from Delaware Route 273 near Christiana northeast to U.S. Route 202 and Delaware Route 141 near the Wilmington Airport . The road runs through suburban neighborhoods before passing along the edge of Wilmington Airport , where it provides access to business parks . The Airport Road portion of DE 37 was originally a dirt road that was paved by 1942 . DE 37 was assigned to its current alignment by 1985 . = = Route description = = DE 37 heads to the northeast from DE 273 on the two-lane , undivided Airport Road . It passes through suburban neighborhoods and then intersects DE 58 ( Churchmans Road ) in a commercial area . Past the DE 58 intersection , the route widens into a four-lane divided highway and forms the northwestern boundary of the Wilmington Airport , with residential areas on the opposite side of the road . After the boundary with the airport , Airport Road splits</t>
+          <t>Armageddon ( 2008 ) = Armageddon ( 2008 ) was a professional-wrestling pay-per-view event produced by the World Wrestling Entertainment ( WWE ) promotion and presented by Ubisoft 's Prince of Persia . It took place on December 14 , 2008 , at the HSBC Arena in Buffalo , New York . It featured professional wrestlers and other talent from all WWE 's three brands : Raw , SmackDown and ECW . The ninth and final event within the Armageddon chronology , it featured on its card seven professional wrestling matches . During the SmackDown main event , Jeff Hardy defeated Triple H and WWE Champion Edge in a Triple Threat match to win the championship . The Raw main event featured the World Heavyweight Championship contested in a standard wrestling match , in which John Cena defeated Chris Jericho to retain the title . The undercard featured several matches , including CM Punk against Rey Mysterio in the finals of a tournament to determine the number-one contender to the WWE Intercontinental Champ</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>A9 ( Croatia ) = The A9 motorway ( Croatian : Autocesta A9 ) is a north – south motorway in Croatia , with a length of 78.3 kilometres ( 48.7 miles ) . Beginning in Pula , the largest city on the Istrian peninsula , it runs north to the Croatian motorway and expressway network at the Kanfanar interchange . Here it meets the A8 motorway , forming the Istrian Y road system . The A9 continues north from here to the Kaštel and Plovanija border crossings into Slovenia . The motorway represents a significant north – south transportation corridor in Croatia and is a part of the European route E751 . The motorway 's national significance is reflected in the positive economic impact on the cities and towns it connects , as well as its importance to tourism in Croatia . Importance of the motorway for tourism is particularly high during summer tourist seasons , when traffic volume increases by more than 80 % . The A9 motorway construction works began in 1988 with its first section opening in 1991</t>
+          <t>Kurt Angle = Kurt Steven Angle ( born December 9 , 1968 ) is an American professional wrestler , actor , former mixed martial artist and retired amateur wrestler . While at Clarion University of Pennsylvania , he won numerous accolades , including being a two-time National Collegiate Athletic Association ( NCAA ) Division I Heavyweight Wrestling Champion . After graduating college , Angle won a gold medal in freestyle wrestling at the 1995 World Wrestling Championships . He then won a freestyle wrestling gold medal at the 1996 Summer Olympics . Angle is one of only four people to complete an amateur wrestling Grand Slam ( junior nationals , NCAA , World Championships , Olympics ) . In 2006 , he was named by USA Wrestling as the greatest shoot wrestler ever and one of the top 15 college wrestlers of all time . He was inducted into the International Sports Hall of Fame in 2016 for his amateur accomplishments . Angle made his first appearance at a professional wrestling event in 1996 , wi</t>
         </is>
       </c>
     </row>
@@ -2051,32 +2051,32 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>['clark', 'superman', 'oliver', 'finale', 'season', 'comic', 'character', 'relationship', 'whitney', 'metropolis', 'believes', 'discovers', 'secret', 'martha', 'series']</t>
+          <t>['entertain', 'entertained', 'buddy', 'profanity', 'flamboyant', 'racially', 'courted', 'rampant', 'subtitles', 'bishop', 'psychologically', 'app', 'oppressed', 'horrific', 'bother']</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Batman in film = The fictional character Batman , a comic book superhero featured in DC Comics publications and created by Bob Kane and Bill Finger , has appeared in various films since his inception . The character first starred in two serial films in the 1940s , Batman and Batman and Robin . The character also appeared in the 1966 film Batman , which was a feature film adaptation of the 1960s Batman TV series starring Adam West and Burt Ward , who also starred in the film . Toward the end of the 1980s , the Warner Bros. studio began producing a series of feature films starring Batman , beginning with the 1989 film Batman , directed by Tim Burton and starring Michael Keaton . Burton and Keaton returned for the 1992 sequel Batman Returns , and in 1995 , Joel Schumacher directed Batman Forever with Val Kilmer as Batman . Schumacher also directed the 1997 sequel Batman &amp; Robin , which starred George Clooney . Batman &amp; Robin was poorly received by both critics and fans , leading to the ca</t>
+          <t>Romanus ( bishop of Rochester ) = Romanus ( died before 627 ) was the second bishop of Rochester and presumably was a member of the Gregorian mission sent to Kent to Christianize the Anglo-Saxons from their native Anglo-Saxon paganism . Romanus was consecrated bishop around 624 and died before 627 by drowning . Little is known of his life beyond these facts . = = Career = = Presumably Romanus came to England with Augustine of Canterbury 's mission to Kent , He would have arrived either in 597 with the first group of missionaries , or in 601 with the second group . He was consecrated as bishop by his predecessor Justus in 624 , after Justus became Archbishop of Canterbury . He was the second bishop at Rochester . Romanus died before 627 , probably about 625 . He drowned in the Mediterranean Sea off Italy while on a mission to Rome for Justus . Presumably this happened before Justus ' death in 627 . He was certainly dead by 633 , when Paulinus of York became bishop at Rochester after fle</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Clark Kent ( Smallville ) = Clark Kent is a fictional character on the television series Smallville . The character of Clark Kent , first created for comic books by Jerry Siegel and Joe Shuster in 1938 as the alternate identity of Superman , was adapted to television in 2001 by Alfred Gough and Miles Millar . This is the fourth time the character has been adapted to a live-action television series . Clark Kent has been played continually by Tom Welling , with various other actors portraying Clark as a child . The character has also appeared in various literature based on the Smallville series , all of which are completely independent of the television episodes . As of 2011 , Smallville 's Clark Kent has appeared in eighteen young adult novels . In the series , Clark Kent attempts to live the life of a normal human being , and struggles with keeping the secret of his alien heritage from his friends . He has an on-again , off-again relationship with Lana Lang through the first seven seas</t>
+          <t>Beurre Maître d 'Hôtel = Beurre Maître d 'Hôtel , also referred to as Maître d 'Hôtel butter , is a type of compound butter ( French : " Beurre composé " ) of French origin , prepared with butter , parsley , lemon juice , salt and pepper . It is a savory butter that is used on meats such as steak ( including the chateaubriand sauce for chateaubriand steak ) , fish , vegetables and other foods . It may be used in place of a sauce , and can significantly enhance a dish 's flavor . Some variations with a sweet flavor exist . It is usually served cold as sliced disks on foods , and is sometimes served as a side condiment . = = Etymology = = The name of Beurre Maître d 'Hôtel is derived from the manner in which it was commonly prepared from scratch by a restaurant 's maître d 'hôtel at diners ' tables . It is also referred to as Maître d 'Hôtel butter . = = Preparation = = Beurre Maître d 'Hôtel is a savory butter prepared by mixing softened butter with very finely minced parsley , lemon ju</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Justice League ( Smallville ) = The Justice League is a fictional group of superheroes on the television series , Smallville , who were adapted for television by Alfred Gough and Miles Millar . The Justice League originally included Oliver Queen , Bart Allen , Victor Stone , and Arthur Curry ; Clark Kent did not accept a role until three seasons later . As the team continued to appear in the series , new characters were introduced and subsequently joined the team . The original Justice League first appeared in the DC comic book The Brave and the Bold # 28 ( 1960 ) , and consisted of members Superman , Batman , Wonder Woman , Flash , Green Lantern , Aquaman , and the Martian Manhunter . In Smallville , the team did not make its first official appearance until the season six episode " Justice " , although each member had been previously introduced individually on various episodes since season four . In the series , the team never formalized a name for themselves , although the cast and c</t>
+          <t>BLT cocktail = A BLT cocktail is a cocktail made out of the contents of a BLT sandwich , ( bacon , lettuce and tomato ) , blended together with vodka . Variants on the drink include utilizing bacon vodka instead of traditional vodka , substituting liquor for lettuce , incorporating bacon salt , or including cucumber flavored vodka . The drink gained popularity in the United States in 2009 . Varieties of the beverage were served in regions including Colorado , Florida , Maine , Massachusetts , Missouri , Oregon , and Virginia . It has also achieved notice in Canada and the United Kingdom . Frank Bruni , the chief restaurant critic for The New York Times , gave a favorable review in 2007 to a BLT cocktail made by chef Gordon Ramsay . An Associated Press review in 2009 of the BLT cocktail made by mixologist Todd Thrasher of Alexandria , Virginia described it as " a drink full of mind-bending , taste bud-tingling turns " . Food critics have given the beverage favorable reviews in The Bosto</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Finale ( Smallville ) = " Finale " is the title of the two-episode series finale of the superhero television series Smallville . The episodes are the 21st and 22nd of the 10th season , and the 216th and 217th episodes overall . The finale originally aired on The CW in the United States on May 13 , 2011 . The first half was written by Al Septien and Turi Meyer , and directed by Kevin G. Fair , and the second half was written by Kelly Souders and Brian Peterson , and directed by Greg Beeman . The series follows the adventures of the young Clark Kent ( Tom Welling ) in the fictional town of Smallville , Kansas , before he becomes Superman . In the series finale , Tess Mercer ( Cassidy Freeman ) learns that the planet Apokolips is coming to destroy humanity , and that Oliver Queen ( Justin Hartley ) is under the possession of Darkseid . Meanwhile , a parallel universe version of Lionel Luthor ( John Glover ) attempts to bring a clone of his son Lex ( Michael Rosenbaum ) to life . Clark fin</t>
+          <t>Genes , Brain and Behavior = Genes , Brain and Behavior ( also known as G2B ) is a peer-reviewed online-only scientific journal covering research in the fields of behavioral , neural , and psychiatric genetics . It is published by Wiley-Blackwell on behalf of the International Behavioural and Neural Genetics Society . The journal was established in 2002 as a quarterly and is currently published monthly . G2B is a hybrid open access journal , but all content is available online for free two years after publication . = = Overview and history = = Genes , Brain and Behavior is published by Wiley-Blackwell on behalf of the International Behavioural and Neural Genetics Society . Volume 1 appeared in 2002 and issues appeared quarterly . As submissions increased , the journal switched in 2003 to a bimonthly schedule , in 2006 to 8-times-a-year , and in 2014 to a monthly frequency . Content is available online from the Wiley Online Library or , after a 12-month embargo , from EBSCOhost . Author</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t xml:space="preserve">The X-Files ( season 9 ) = The ninth season of the American science fiction television series The X-Files commenced airing in the United States on November 11 , 2001 , concluded on May 19 , 2002 , and consists of twenty episodes . Season nine takes place after Fox Mulder ( David Duchovny ) goes into hiding , following the events of the eighth season finale , " Existence " . As such , the main storyarc for the season follows Dana Scully ( Gillian Anderson ) , John Doggett ( Robert Patrick ) , and Monica Reyes ( Annabeth Gish ) on their hunt to reveal a government conspiracy who are creating " Super Soldiers " . For this season , former series ' leads Duchovny and Anderson scaled back their involvement with the show , with the former only starring in the two episodes that formed the season finale , " The Truth " . Doggett and Reyes became the show 's central characters , and former recurring character Walter Skinner ( Mitch Pileggi ) became a main character . Series creator Chris Carter </t>
+          <t>.bv = .bv is the Internet country code top-level domain ( ccTLD ) reserved for the uninhabited Norwegian dependent territory of Bouvet Island . The domain name registry and sponsor is Norid , but .bv is not open for registration . .bv was designated on 21 August 1997 and was placed under the .no registry Norid . Norwegian policy states that .no is sufficient for those institutions connected to Bouvet Island , and therefore the domain is not open to registration . It is Norwegian policy not to commercialize domain resources , so there are no plans to sell .bv. Should the domain later come into use , it will be under the regulation of the Norwegian Post and Telecommunications Authority and follow the same policy as .no. = = History = = Bouvet Island is an uninhabited volcanic island in the South Atlantic Ocean . It was claimed by Norway in 1927 . The domain was allocated on 21 August 1997 , at the same time .sj was allocated for Svalbard and Jan Mayen . The allocation occurred because th</t>
         </is>
       </c>
     </row>
@@ -2086,32 +2086,32 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>['euro', 'coins', 'currency', 'note', 'notes', 'denominations', 'dollar', 'value', 'stripe', 'tender', 'silver', 'puerto_rico', 'thread', 'ink', 'issued']</t>
+          <t>['production', 'system', 'crew', 'mission', 'use', 'development', 'based', 'high', 'million', 'aircraft', 'engine', 'control', 'announced', 'new', 'flight']</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Euro = The euro ( sign : € ; code : EUR ) is the official currency of the eurozone , which consists of 19 of the 28 member states of the European Union : Austria , Belgium , Cyprus , Estonia , Finland , France , Germany , Greece , Ireland , Italy , Latvia , Lithuania , Luxembourg , Malta , the Netherlands , Portugal , Slovakia , Slovenia , and Spain . The currency is also officially used by the institutions of the European Union and four other European countries , as well as unilaterally by two others , and is consequently used daily by some 337 million Europeans as of 2015 . Outside of Europe , a number of overseas territories of EU members also use the euro as their currency . Additionally , 210 million people worldwide as of 2013 use currencies pegged to the euro . The euro is the second largest reserve currency as well as the second most traded currency in the world after the United States dollar . As of August 2014 , with more than € 995,000,000,000 in circulation , the euro has t</t>
+          <t>Lockheed Martin F-22 Raptor = The Lockheed Martin F-22 Raptor is a fifth-generation , single-seat , twin-engine , all-weather stealth tactical fighter aircraft developed for the United States Air Force ( USAF ) . The result of the USAF 's Advanced Tactical Fighter program , the aircraft was designed primarily as an air superiority fighter , but also has ground attack , electronic warfare , and signals intelligence capabilities . The prime contractor , Lockheed Martin , built most of the F-22 's airframe and weapons systems and did its final assembly , while Boeing provided the wings , aft fuselage , avionics integration , and training systems . The aircraft was variously designated F-22 and F / A-22 before it formally entered service in December 2005 as the F-22A . After a protracted development and despite operational issues , the USAF considers the F-22 critical to its tactical air power , and says that the aircraft is unmatched by any known or projected fighter . The Raptor 's combi</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>500 euro note = The five hundred euro note ( € 500 ) is the highest-value euro banknote and has been used since the introduction of the euro ( in its cash form ) in 2002 . It is one of the highest value circulating banknotes in the world , worth around 551 USD , 3,677 CNY , 58,254 JPY , 543 CHF or 417 GBP . The note is used in the 23 countries which have the euro as their sole currency ( with 22 legally adopting it ) , with a population of about 338 million . It is the largest note measuring 160 × 82 mm and has a purple colour scheme . The five hundred euro banknotes depict bridges and arches / doorways in modern architecture ( around the late 20th century ) . The five hundred euro note contains several complex security features such as watermarks , invisible ink , holograms and microprinting that make counterfeiting very difficult . Initially the high denomination notes were introduced very rapidly so that in first 7 years ( by Dec 2008 ) there were 530,064,413 five hundred euro bankn</t>
+          <t>Mercury-Atlas 8 = Mercury-Atlas 8 ( MA-8 ) was the fifth United States manned space mission , part of NASA 's Mercury program . Astronaut Walter M. Schirra , Jr . , orbited the Earth six times in the Sigma 7 spacecraft on October 3 , 1962 , in a nine-hour flight focused mainly on technical evaluation rather than on scientific experimentation . This was the longest U.S. manned orbital flight yet achieved in the Space Race , though well behind the several-day record set by the Soviet Vostok 3 earlier in the year . It confirmed the Mercury spacecraft 's durability ahead of the one-day Mercury-Atlas 9 mission that followed in 1963 . Planning began for the third U.S. orbital mission in February 1962 , aiming for a six-or-seven-orbit flight to build on the previous three-orbit missions . NASA officially announced the mission on June 27 , and the flight plan was finalized in late July . The mission focused on engineering tests rather than on scientific experimentation . The mission finally la</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>50 euro note = The fifty euro note ( € 50 ) is one of the middle value euro banknotes and has been used since the introduction of the euro ( in its cash form ) in 2002 . The note is used daily by some 332 million Europeans and in the 23 countries which have the euro as their sole currency ( with 22 legally adopting it ) . It is the fourth smallest note , measuring 140 mm × 77 mm , and has an orange colour scheme . The note depicts bridges and arches / doorways in the Renaissance era ( 15th and 16th centuries ) . The € 50 note contains several complex security features such as watermarks , invisible ink , holograms and microprinting that document its authenticity . In January 2016 , there were about 8,170,123,315 fifty euro banknotes in circulation in the eurozone . It is by far the most widely circulated denomination , compromising over 44 % of the total banknotes . The full design of the Europa series € 50 banknote was revealed on 5 July 2016 ; it is due to be launched in April 2017 .</t>
+          <t>Holden Commodore = The Holden Commodore is a car manufactured since 1978 by Holden in Australia and , formerly , in New Zealand . For the original model , Holden replaced the long-serving Kingswood and Premier large cars developed in Australia , with another rear wheel drive ( RWD ) platform that was , however , based on a smaller European design by Opel , re-engineered for Australian conditions . Subsequent series became larger , culminating with the fourth generation Commodore , fully developed in Australia and based on the GM Zeta platform . Initially introduced as a single sedan body style , the range expanded in 1979 to include a station wagon . From 1984 , Holden began branding the flagship Commodore model as Holden Calais , with the Commodore Berlina introduced in 1984 gaining independent Holden Berlina nomenclature in 1988 . Long-wheelbase Statesman / Caprice derivatives and Commodore utility body variants followed in 1990 . The third generation architecture spawned the most bo</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>10 euro note = The ten euro note ( € 10 ) is the second-lowest value euro banknote and has been used since the introduction of the euro ( in its cash form ) in 2002 . The note is used in the 23 countries which have it as their sole currency ( with 22 legally adopting it ) ; with a population of about 332 million . It is the second-smallest note measuring 127x67mm with a red colour scheme . The ten euro banknotes depict bridges and arches / doorways in Romanesque architecture ( between the 11th and 12th centuries ) . The ten euro note contains several complex security features such as watermarks , invisible ink , holograms and microprinting that document its authenticity . In September 2011 , there were approximately 2,005,149,600 ten euro banknotes in circulation around the eurozone . = = History = = The euro was founded on 1 January 1999 , when it became the currency of over 300 million people in Europe . For the first three years of its existence it was an invisible currency , only u</t>
+          <t>Northrop F-20 Tigershark = The Northrop F-20 Tigershark ( initially F-5G ) was a privately financed light fighter , designed and built by Northrop . Its development began in 1975 as a further evolution of Northrop 's F-5E Tiger II , featuring a new engine that greatly improved overall performance , and a modern avionics suite including a powerful and flexible radar . Compared with the F-5E , the F-20 was much faster , gained beyond-visual-range air-to-air capability , and had a full suite of air-to-ground modes capable of firing most U.S. weapons . With these improved capabilities , the F-20 became competitive with contemporary fighter designs such as the General Dynamics F-16 Fighting Falcon , but was much less expensive to purchase and operate . Much of the F-20 's development was carried out under a US Department of Defense ( DoD ) project called " FX " . FX sought to develop fighters that would be capable in combat with the latest Soviet aircraft , but excluding sensitive front-lin</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aksumite currency = Aksumite currency was coinage produced and used within the Kingdom of Aksum ( or Axum ) centered in present-day Ethiopia and Eritrea . It was issued and circulated from the reign of King Endubis around AD 270 until it began its decline in the first half of the 7th century . During the succeeding medieval period , Mogadishu currency , minted by the Sultanate of Mogadishu , was the most widely circulated currency in the Horn of Africa . Aksum 's currency served as a vessel of propaganda demonstrating the kingdom 's wealth and promoting the national religion ( first polytheistic and later Oriental Christianity ) . It also facilitated the Red Sea trade on which it thrived . The coinage has also proved invaluable in providing a reliable chronology of Aksumite kings due to the lack of extensive archaeological work in the area . = = Origins = = = = = Pre-coinage period = = = Though the issuing of minted coins didn 't begin until around 270 , metal coins may have been used </t>
+          <t>History of the metric system = Concepts similar to those behind the metric system had been discussed in the 16th and 17th centuries . Simon Stevin had published his ideas for a decimal notation and John Wilkins had published a proposal for a decimal system of measurement based on natural units . The first practical realisation of the metric system came in 1799 , during the French Revolution , when the existing system of measure , which had fallen into disrepute , was temporarily replaced by a decimal system based on the kilogram and the metre . The work of reforming the old system of weights and measures had the support of whoever was in power , including Louis XVI . The metric system was to be , in the words of philosopher and mathematician Condorcet , " for all people for all time " . In the era of humanism , the basic units were taken from the natural world : the unit of length , the metre , was based on the dimensions of the Earth , and the unit of mass , the kilogram , was based o</t>
         </is>
       </c>
     </row>
@@ -2121,32 +2121,32 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>['painting', 'paintings', 'works', 'abstract', 'dots', 'art', 'canvas', 'okay', 'artist', 'breasts', 'portrait', 'mirror', 'girl', 'work', 'balloon']</t>
+          <t>['album', 'songs', 'number', 'band', 'release', 'single', 'music', 'track', 'copies', 'released', 'chart', 'billboard', 'tracks', 'sound', 'recording']</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Artist 's Studio — Look Mickey = Artist 's Studio — Look Mickey ( sometimes Artist 's Studio , Look Mickey , Artist 's Studio – Look Mickey or Artist 's Studio No. 1 ( Look Mickey ) ) is a 1973 painting by Roy Lichtenstein . It is one of five large-scale studio interior paintings in a series . The series is either referred to as the Artist 's Studio series or more colloquially as the Studios and sometimes is described as excluding the other 1973 painting , reducing the series to four . The series refers to a set of works by Henri Matisse , with this work specifically referring to L 'Atelier Rouge . The work incorporates several other Lichtenstein 's works and gets its name from the large portion of Lichtenstein 's Look Mickey that is included . Lichtenstein used a much more realistic representation of his own works than is standard for most artists . Elements of the work also refer to works from both Fernand Léger and Matisse . = = Background = = Lichtenstein 's studios reference what </t>
+          <t xml:space="preserve">Coming Up to Breathe = Coming Up to Breathe is the fourth studio album by Christian rock band MercyMe . Released on April 25 , 2006 , by INO Records , the album was intended by MercyMe to be edgier than their previous albums . Coming Up to Breathe sold 58,000 copies its first week , MercyMe 's biggest sales week at the time . It debuted and peaked at number one on the Billboard Christian Albums chart , number five on the Rock Albums chart , and number thirteen on the Billboard 200 . It also appeared on the Alternative Albums chart in 2007 , peaking at number thirteen . Coming Up to Breathe was certified Gold by the Recording Industry Association of America ( RIAA ) in 2007 , signifying shipments of over 500,000 copies . Coming Up to Breathe received positive reviews from critics . It was also nominated for Best Pop / Contemporary Gospel Album at the 49th Grammy Awards , and for Pop / Contemporary Album of the Year at the 38th GMA Dove Awards . The song " Bring the Rain " was nominated </t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Girl with Ball = Girl with Ball is a 1961 painting by Roy Lichtenstein . It is an oil on canvas Pop art work that is now in the collection of the Museum of Modern Art , after being owned for several decades by Philip Johnson . It is one of Lichtenstein 's earliest Pop art works and is known for its source , which is a newspaper ad that ran for several decades and which was among Lichtenstein 's earliest works sourced from pop culture . Girl with Ball was exhibited at Lichtenstein 's first solo exhibition and was displayed in Newsweek 's review of the show . This work significantly alters the original source and is considered exemplary of Lichtenstein 's works that exaggerate the mechanically produced appearance although the result of his painterly work . It is an enduring depiction of the contemporary beauty figure . = = Background = = Girl with Ball was inspired by a 1961 advertisement for the Mount Airy Lodge in the Pocono Mountains . The ad , which started running in 1955 , was wide</t>
+          <t>Dignity ( album ) = Dignity is the fourth studio album by American recording artist Hilary Duff . It was released on March 21 , 2007 , by Hollywood Records . After launching her third record Hilary Duff ( 2004 ) , she experienced an eventful personal life , including a stalking incident , her parents ' separation , and breaking up with her boyfriend . Consequently , Duff assumed an integral position in its production , co-writing almost every track with longtime collaborator Kara DioGuardi instead of her previously-limited involvement . Duff was musically inspired by indie rock band The Faint and pop singers Beyoncé and Gwen Stefani . In contrast to the pop rock themes of her prior releases , Dignity takes on more of a dance sound , which she said was not her intention while writing the album . The lyrics reference the events Duff experienced in the years leading to the album 's release , and the album 's songs contain influences of rock and roll and hip hop music . Critical response w</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Brushstrokes series = Brushstrokes series is the name for a series of paintings produced in 1965 – 66 by Roy Lichtenstein . It also refers to derivative sculptural representations of these paintings that were first made in the 1980s . In the series , the theme is art as a subject , but rather than reproduce masterpieces as he had starting in 1962 , Lichtenstein depicted the gestural expressions of the painting brushstroke itself . The works in this series are linked to those produced by artists who use the gestural painting style of abstract expressionism made famous by Jackson Pollock , but differ from them due to their mechanically produced appearance . The series is considered a satire or parody of gestural painting by both Lichtenstein and his critics . After 1966 , Lichtenstein incorporated this series into later motifs and themes of his work . = = Background = = In the early 1960s , Lichtenstein reproduced masterpieces by Cézanne , Mondrian and Picasso before embarking on the Bru</t>
+          <t xml:space="preserve">We 're New Here = We 're New Here is a remix album by American recording artist Gil Scott-Heron and English music producer Jamie xx , released on February 21 , 2011 , by Young Turks and XL Recordings . A longtime fan of Scott-Heron , Jamie xx was approached by XL label head Richard Russell to remix Scott-Heron 's 2010 studio album I 'm New Here . He worked on the album while touring with his band The xx in 2010 and occasionally communicated with Scott-Heron through letters for his approval to rework certain material . Incorporating dubstep and UK garage styles , Jamie xx applied electronic music techniques in his production to remix Scott-Heron 's vocals from the original album over his own instrumentals . Although it is structured similarly , We 're New Here eschews the original album 's stark style and lo-fi production for bass-driven , musically varied production and sonical illumination of Scott-Heron 's vocals . It has been noted by music writers for recontextualizing Scott-Heron </t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Symphony in White , No. 2 : The Little White Girl = Symphony in White , No. 2 , also known as The Little White Girl is a painting by James Abbott McNeill Whistler . The work shows a woman in three-quarter figure standing by a fireplace with a mirror over it . She is holding a fan in her hand , and wearing a white dress . The model is Joanna Hiffernan , the artist 's mistress . Though the painting was originally called The Little White Girl , Whistler later started calling it Symphony in White , No. 2 . By referring to his work in such abstract terms , he intended to emphasize his " art for art 's sake " philosophy . In this painting , Heffernan wears a ring on her ring finger , even though the two were not married . By this religious imagery , Whistler emphasizes the aesthetic philosophy behind his work . Whistler created the painting in the winter of 1864 , and it was displayed at the Royal Academy the next year . The original frame carried a poem written by Whistler 's friend Algerno</t>
+          <t>Xenogears Original Soundtrack = The Xenogears Original Soundtrack is the official soundtrack to Square 's role-playing video game Xenogears . It was composed by Yasunori Mitsuda and contains 44 tracks , including a Bulgarian choral song and two pieces performed by the Irish singer Joanne Hogg . Though the game was released in both Japan and North America , the album was published in Japan exclusively as a 2-CD set on March 1 , 1998 . The soundtrack was composed with strong traditional and Irish music influences , while the lyrics for the vocal tracks were written by the game 's director Tetsuya Takahashi and its scenario writer Masato Kato . The soundtrack reached # 55 in Japan and was generally well received by critics , though some disagreed on whether the album can be fully appreciated by non-players . Two arranged versions of the soundtrack , Creid ( 1998 ) and Myth : The Xenogears Orchestral Album ( 2011 ) , were also released by Mitsuda . The composer , along with Joanne Hogg , r</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Grrrrrrrrrrr ! ! = Grrrrrrrrrrr ! ! is a 1965 oil and Magna on canvas painting by Roy Lichtenstein . Measuring 68 in × 56.125 in ( 172.7 cm × 142.6 cm ) , it was bequeathed to the Solomon R. Guggenheim Museum collection from Lichtenstein 's estate . It depicts a head-on representation of an angry dog growling with the onomatopoeic expression " Grrrrrrrrrrr ! ! " . The work was derived from Our Fighting Forces , which also served as the source for other military dog paintwork by Lichtenstein . = = Background = = The Lichtenstein foundation notes that the inspiration for this painting is a frame of Our Fighting Forces # 66 ( February 1962 ) , which was published by National Periodical Publications ( now DC Comics ) . In that frame only a portion of the dog 's head is visible and the speech balloon says " Grrrrr ! " In addition to the painting itself , Lichtenstein produced a small 5.75 in × 4.5 in ( 14.6 cm × 11.4 cm ) graphite on paper study . The painting was bestowed to the Guggenheim</t>
+          <t xml:space="preserve">Born This Way : The Remix = Born This Way : The Remix is the second remix album by American recording artist Lady Gaga , released on November 18 , 2011 by Interscope . This album contains remixes of multiple songs off of Gaga 's second studio album , Born This Way . It was also released as part of the Born This Way : The Collection , a special edition release including the 17-track version of Gaga 's second studio album and a DVD release of the HBO concert special Lady Gaga Presents the Monster Ball Tour : At Madison Square Garden . Most of the remixes had been available in the remix EPs released alongside each single from Born This Way . Musically , the album is an electronic and dance record ; there are also influences of Europop , techno and dubstep within the composition . Critics gave mixed reviews for the album , with their general complaint being that the release was unnecessary . Most of them , however , complimented The Weeknd , Twin Shadow and Guéna LG 's remixes . It earned </t>
         </is>
       </c>
     </row>
@@ -2156,32 +2156,67 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>['ben', 'shannon', 'survivors', 'bernard', 'island', 'freighter', 'dave', 'frank', 'plane', 'jack', 'alex', 'miles', 'kate', 'crash', 'rose']</t>
+          <t>['ship', 'ships', 'torpedo', 'tons', 'guns', 'admiral', 'cruiser', 'fleet', 'submarine', 'sank', 'laid', 'sinking', 'convoy', 'german', 'destroyer']</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Shannon Rutherford = Shannon Rutherford was a fictional character played by Maggie Grace on the ABC drama television series Lost , which chronicled the lives of the survivors of a plane crash in the South Pacific . Shannon was introduced in the pilot episode as the stepsister of fellow crash survivor Boone Carlyle ( Ian Somerhalder ) . She was a series regular until her funeral in " What Kate Did " . For most of her time on the Island , she was unhelpful and spent much of her time sunbathing . She formed a relationship with another survivor from the plane crash , Sayid Jarrah ( Naveen Andrews ) . Shannon was accidentally shot by Ana Lucia Cortez who mistakes her for an Other . During the casting process , she was compared to Paris Hilton . Naveen Andrews , who played the character Sayid on the show , had the idea of encouraging the writers to write a romantic relationship between his character and Shannon into the story . Critics found her to be a largely unsympathetic character until </t>
+          <t>German destroyer Z10 Hans Lody = Z10 Hans Lody was a Type 1934A-class destroyer built for Nazi Germany 's Kriegsmarine in the mid-1930s . At the beginning of World War II on 1 September 1939 , the ship was initially deployed to blockade the Polish coast , but she was quickly transferred to the North Sea to lay defensive minefields . In late 1939 the ship laid multiple offensive minefields off the English coast that claimed nine merchant ships and she crippled a British a destroyer during one of these missions . Hans Lody was under repair for most of the Norwegian Campaign and was transferred to France in late 1940 where she participated in several engagements with British ships , crippling another destroyer . The ship returned to Germany in late 1940 for a refit and was transferred to Norway in June 1941 as part of the preparations for Operation Barbarossa , the German invasion of the Soviet Union . Hans Lody spent some time at the beginning of the campaign conducting anti-shipping pat</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Danielle Rousseau = Danielle Rousseau is a fictional character on the ABC drama television series Lost , which chronicles the lives of over forty people after their plane crashes on a remote island somewhere in the South Pacific . Croatian actress Mira Furlan plays the scientist who shipwrecks on the island sixteen years prior to the crash of Oceanic Flight 815 . After Rousseau is killed in the fourth season , the American actress Melissa Farman portrayed a younger version of the character in the fifth season . Furlan later reappears for one episode in the sixth season . Rousseau is a recurring on-island character who has appeared in nineteen episodes in seasons one through four , as well as one episode where her voice alone is heard , and her final episode in the sixth season . The character , who is commonly known as " The French Woman " among the survivors on the island , is introduced early in the first season . Sixteen years prior to the plane crash , Rousseau was a member of a Fr</t>
+          <t>Japanese battleship Hiei = Hiei ( 比叡 ) was a warship of the Imperial Japanese Navy during World War I and World War II . Designed by British naval architect George Thurston , she was the second launched of four Kongō-class battlecruisers , among the most heavily armed ships in any navy when built . Laid down in 1911 at the Yokosuka Naval Arsenal , Hiei was formally commissioned in 1914 . She patrolled off the Chinese coast on several occasions during World War I , and helped with rescue efforts following the 1923 Great Kantō earthquake . Starting in 1929 , Hiei was converted to a gunnery training ship to avoid being scrapped under the terms of the Washington Naval Treaty . She served as Emperor Hirohito 's transport in the mid-1930s . Starting in 1937 , she underwent a full-scale reconstruction that completely rebuilt her superstructure , upgraded her powerplant , and equipped her with launch catapults for floatplanes . Now fast enough to accompany Japan 's growing fleet of aircraft ca</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Tom Friendly = Tom Friendly , often referred to as Tom or Mr. Friendly , is a fictional character portrayed by M. C. Gainey on the American Broadcasting Company ( ABC ) television series Lost . The series follows the lives of around forty survivors from the crash of Oceanic Flight 815 . The survivors find themselves on a mysterious tropical island , and interact with a group known as the Others , who appear to have lived on the island since long before the crash . Tom is an influential member of the Others , and is introduced in 2005 in the season one finale " Exodus : Part 2 " , where he kidnaps one of the survivors . The character makes another fifteen appearances before being killed in the season three finale " Through the Looking Glass " . Tom appears twice in season four in the flashbacks of other characters . Gainey was initially credited as playing " bearded man " and then as " Mr. Friendly " throughout season two before the character was given a first name . In a montage of dec</t>
+          <t>German Type IXA submarine = The German Type IXA submarine was a sub-class of the German Type IX submarine built for Nazi Germany 's Kriegsmarine between 1937 and 1938 . These U-boats were designed between 1935 and 1936 and were intended to be fairly large ocean-going submarines . The inspiration for the Type IXA submarine came from the German Type IA submarine , which had a similar diving depth and identical submerged horsepower . Two of the eight Type IXA submarines ( U-37 and U-38 ) would become the 6th and 10th most successful U-boats that saw service in World War II , sinking 53 and 35 ships respectively . All of the Type IXA submarines were sunk fairly early in the war except for U-37 and U-38 , which were scuttled in May 1945 to prevent them from falling into the hands of the Allies . = = Construction = = All Type IXA submarines were ordered by the Kriegsmarine between 29 July 1936 and 21 November 1936 as part of Plan Z and the overall German plan of re-armament in violation of t</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Rose and Bernard Nadler = Rose and Bernard Nadler are fictional characters on the American Broadcasting Company ( ABC ) television series Lost , played by L. Scott Caldwell and Sam Anderson respectively . Rose and Bernard visit a faith healer on their honeymoon in Australia , in the hope of healing Rose 's cancer . When Bernard visits the restroom during the return flight , the plane splits in half , with the two halves crashing on different parts of an island in the South Pacific . The couple reunite midway through season two , and Rose reveals the Island has healed her . After time traveling in season five they separate from the remaining survivors and build a cabin near the ocean to live in . Originally , the story of a woman separated from her husband when the plane crashes was going to be used for Kate , but when Kate 's role in the series changed the producers kept that story for Rose . Much of the couple 's story prior to the plane crash was based on the events of Caldwell 's li</t>
+          <t>HMS Glorious = HMS Glorious was the second of the Courageous-class battlecruisers built for the Royal Navy during the First World War . Designed to support the Baltic Project championed by the First Sea Lord , Lord Fisher , they were very lightly armoured and armed with only a few heavy guns . Glorious was completed in late 1916 and spent the war patrolling the North Sea . She participated in the Second Battle of Heligoland Bight in November 1917 and was present when the German High Seas Fleet surrendered a year later . Glorious was paid off after the end of the war , but was rebuilt as an aircraft carrier during the late 1920s . She could carry 30 % more aircraft than her half-sister Furious which had approximately the same tonnage . After recommissioning she spent most of her career operating in the Mediterranean Sea . After the start of the Second World War , Glorious spent the rest of 1939 unsuccessfully hunting for the German cruiser Admiral Graf Spee in the Indian Ocean before re</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Ben Linus = Benjamin " Ben " Linus is a fictional character portrayed by Michael Emerson on the ABC television series Lost . Ben was the leader of a group of island natives called the Others and was initially known as Henry Gale to the survivors of Oceanic Flight 815 . He began as the main antagonist during the second and third seasons , but in subsequent seasons , becomes a morally ambiguous ally to the main characters . Other characters frequently describe him as loyal only to himself , though it is also often hinted that he may be driven by some higher purpose . As with most characters on Lost , Ben 's history is revealed through flashbacks and episodes set in other time periods which are revealed slowly as the series progresses . Sterling Beaumon first portrayed a young Ben late in season three , in the character 's first centric episode , " The Man Behind the Curtain " . Ben 's childhood is further explored in the fifth season of the series , partially set in 1977 . Fifth season e</t>
+          <t>German cruiser Emden = Emden was a light cruiser built by the Reichsmarine in the early 1920s . She was the only ship of her class and was the first large warship built in Germany after the end of World War I. She was built at the Reichsmarinewerft in Wilhelmshaven ; her keel was laid in December 1921 and her completed hull was launched in January 1925 . Emden was commissioned into the German fleet in October 1925 . Her design was heavily informed by the restrictions of the Treaty of Versailles and the dictates of the Allied disarmament commission . She was armed with a main battery of surplus 15 cm ( 5.9 in ) guns left over from World War I , mounted in single gun turrets , as mandated by the Allied powers . She had a top speed of 29 knots ( 54 km / h ; 33 mph ) . Emden spent the majority of her career as a training ship ; in the inter-war period , she conducted several world cruises to train naval cadets . At the outbreak of war , she laid minefields off the German coast and was dama</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>['government', 'war', 'military', 'led', 'political', 'country', 'party', 'support', 'polish', 'foreign', 'soviet', 'revolution', 'leader', 'russian', 'members']</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Armenian Revolutionary Federation = The Armenian Revolutionary Federation ( ARF ) ( classical Armenian : Հայ Յեղափոխական Դաշնակցութիւն , ՀՅԴ ) , also known as Dashnaktsutyun ( in a short form , " Dashnak " ) , is an Armenian nationalist and socialist political party founded in 1890 in Tiflis , Russian Empire ( now Tbilisi , Georgia ) in 1890 by Christapor Mikaelian , Stepan Zorian , and Simon Zavarian . The party operates in Armenia , Nagorno-Karabakh and in countries where the Armenian diaspora is present , notably in Lebanon , where the party is represented in the parliament as part of the March 8 alliance . The ARF has traditionally advocated democratic socialism and is a full member of the Socialist International since 2003 , which it had originally joined in 1907 . It possesses the largest number of members from the political parties present in the Armenian diaspora , having established affiliates in more than 20 countries . Compared to other Armenian parties which tend to primari</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Stanisław August Poniatowski = Stanisław II August ( also Stanisław August Poniatowski ; born Stanisław Antoni Poniatowski ; 17 January 1732 – 12 February 1798 ) was the last King and Grand Duke of the Polish – Lithuanian Commonwealth ( 1764 – 95 ) . He remains a controversial figure in Polish history . Recognized as a great patron of the arts and sciences . Initiatior and firm supporter of progressive reforms , he is also remembered as the last king of the Commonwealth whose election was marred by Russian involvement . Main criticism resonates around being the one who failed to stand against the partitions , and in the end to prevent the destruction of Poland . Arriving at the Russian imperial court in Saint Petersburg in 1755 , he became romantically involved with the twenty-six-year-old Catherine Alexeievna ( the future Empress Catherine the Great , reigned 1762 – 1796 ) , three years his senior . With her support , in 1764 he was elected king of Poland . Against expectations , he a</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Hafizullah Amin = Hafizullah Amin ( Persian : حفيظ الله امين born 1 August 1929 – 27 December 1979 ) was an Afghan politician and statesman during the Cold War . Amin was born in Paghman and educated at Kabul University , after which he started his career as a teacher . After a few years in that occupation , he went to the United States to study . He would visit the United States a second time before moving permanently to Afghanistan , and starting his career in radical politics . He ran as a candidate in the 1965 parliamentary election but failed to secure a seat . Amin was the only Khalqist elected to parliament in the 1969 parliamentary election , thus increasing his standing within the party . He was one of the leading organisers of the Saur Revolution which overthrew the government of Mohammad Daoud Khan . Amin 's short-lived presidency was marked by controversies from beginning to end . He came to power by ordering the death of his predecessor Nur Muhammad Taraki . The revolt aga</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Adolf Hitler = Adolf Hitler ( German : [ ˈadɔlf ˈhɪtlɐ ] ; 20 April 1889 – 30 April 1945 ) was a German politician who was the leader of the Nazi Party ( Nationalsozialistische Deutsche Arbeiterpartei ; NSDAP ) , Chancellor of Germany from 1933 to 1945 , and Führer ( " leader " ) of Nazi Germany from 1934 to 1945 . As dictator of Nazi Germany , he initiated World War II in Europe with the invasion of Poland in September 1939 and was a central figure of the Holocaust . Hitler was born in Austria , then part of Austria-Hungary , and raised near Linz . He moved to Germany in 1913 and was decorated during his service in the German Army in World War I. He joined the German Workers ' Party , the precursor of the NSDAP , in 1919 and became leader of the NSDAP in 1921 . In 1923 , he attempted a coup in Munich to seize power . The failed coup resulted in Hitler 's imprisonment , during which time he dictated the first volume of his autobiography and political manifesto Mein Kampf ( " My Struggl</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Klemens von Metternich = Prince Klemens Wenzel von Metternich ( German : Klemens Wenzel Nepomuk Lothar , Fürst von Metternich-Winneburg zu Beilstein , Anglicized as Clement Wenceslaus Lothair , Prince of Metternich-Winneburg-Beilstein ; 15 May 1773 – 11 June 1859 ) was a politician and statesman of Rhenish extraction and one of the most important diplomats of his era , serving as the Austrian Empire 's Foreign Minister from 1809 and Chancellor from 1821 until the liberal revolutions of 1848 forced his resignation . One of his first tasks was to engineer a détente with France that included the marriage of Napoleon to the Austrian archduchess Marie Louise . Soon after , he engineered Austria 's entry into the War of the Sixth Coalition on the Allied side , signed the Treaty of Fontainebleau that sent Napoleon into exile , and led the Austrian delegation at the Congress of Vienna that divided post-Napoleonic Europe amongst the major powers . For his service to the Austrian Empire he was g</t>
         </is>
       </c>
     </row>

</xml_diff>